<commit_message>
Remove mock data from workbooks
</commit_message>
<xml_diff>
--- a/Config.xlsx
+++ b/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mateus.cruz\Documents\GitHub\OrchestratorManager\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED1004AE-B580-43C7-BD79-D397B3EEC684}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53A92161-7664-443C-953C-B8ED07DB07C9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="3" r:id="rId1"/>
@@ -1181,13 +1181,13 @@
     <t>OK</t>
   </si>
   <si>
-    <t>https://win-bthk15upk2f/</t>
-  </si>
-  <si>
     <t>Default</t>
   </si>
   <si>
     <t>Organization Units</t>
+  </si>
+  <si>
+    <t>https://win-9d2vvsqpta7/</t>
   </si>
 </sst>
 </file>
@@ -1570,7 +1570,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D89C9C48-5454-47C4-AB1D-448E4519251A}">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -1597,7 +1597,7 @@
         <v>59</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>381</v>
+        <v>383</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>286</v>
@@ -1608,7 +1608,7 @@
         <v>219</v>
       </c>
       <c r="B3" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>287</v>
@@ -1616,7 +1616,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{DEB48CDE-C611-45AA-8916-106D46639E00}"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{B579A2F5-99A4-49E1-B807-A008372D3262}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
@@ -2105,7 +2105,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1927ABA9-1814-4487-9CEC-ABDCAF91481F}">
   <dimension ref="A1:C107"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -2198,7 +2198,7 @@
         <v>351</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>350</v>

</xml_diff>

<commit_message>
Accept Orchestrator URL, tenant name and path to workbooks via process arguments from Orchestrator
</commit_message>
<xml_diff>
--- a/Config.xlsx
+++ b/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mateus.cruz\Documents\GitHub\OrchestratorManager\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53A92161-7664-443C-953C-B8ED07DB07C9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96A6F0E7-1CF6-4E04-81D9-A29A007B7E9E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="411" uniqueCount="384">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="414" uniqueCount="387">
   <si>
     <t>Name</t>
   </si>
@@ -145,9 +145,6 @@
     <t>C</t>
   </si>
   <si>
-    <t>MachineConfigFilepath</t>
-  </si>
-  <si>
     <t>D</t>
   </si>
   <si>
@@ -187,9 +184,6 @@
     <t>ID{0}マシン取得が失敗しました。リクエストステータス：{1} / レスポンス：{2}。</t>
   </si>
   <si>
-    <t>AssetConfigFilepath</t>
-  </si>
-  <si>
     <t>UnsupportedAssetType</t>
   </si>
   <si>
@@ -211,9 +205,6 @@
     <t>DeleteAssetResultColumn</t>
   </si>
   <si>
-    <t>UserConfigFilepath</t>
-  </si>
-  <si>
     <t>OrchestratorURL</t>
   </si>
   <si>
@@ -232,9 +223,6 @@
     <t>EditUserResultColumn</t>
   </si>
   <si>
-    <t>RobotConfigFilepath</t>
-  </si>
-  <si>
     <t>ProcessedRobot</t>
   </si>
   <si>
@@ -529,9 +517,6 @@
     <t>DeleteEnvironmentResultColumn</t>
   </si>
   <si>
-    <t>EnvironmentConfigFilepath</t>
-  </si>
-  <si>
     <t>EnvironmentIDInvalidOrNotSpecified</t>
   </si>
   <si>
@@ -734,9 +719,6 @@
   </si>
   <si>
     <t>OrganizationUnitsPanelPath</t>
-  </si>
-  <si>
-    <t>ProcessConfigFilepath</t>
   </si>
   <si>
     <t>FormProcessOption</t>
@@ -1142,52 +1124,79 @@
     <t>Core\Forms\AuthenticationPanel.html</t>
   </si>
   <si>
-    <t>Workbooks\EN\Assets.xlsx</t>
-  </si>
-  <si>
-    <t>Workbooks\EN\Users.xlsx</t>
-  </si>
-  <si>
-    <t>Workbooks\EN\Robots.xlsx</t>
-  </si>
-  <si>
-    <t>Workbooks\EN\Machines.xlsx</t>
-  </si>
-  <si>
-    <t>Workbooks\EN\Environments.xlsx</t>
-  </si>
-  <si>
-    <t>Workbooks\EN\Processes.xlsx</t>
-  </si>
-  <si>
-    <t>Workbooks\JA\アセット.xlsx</t>
-  </si>
-  <si>
-    <t>Workbooks\JA\ユーザー.xlsx</t>
-  </si>
-  <si>
-    <t>Workbooks\JA\ロボット.xlsx</t>
-  </si>
-  <si>
-    <t>Workbooks\JA\マシン.xlsx</t>
-  </si>
-  <si>
-    <t>Workbooks\JA\ロボットグループ.xlsx</t>
-  </si>
-  <si>
-    <t>Workbooks\JA\プロセス.xlsx</t>
-  </si>
-  <si>
     <t>OK</t>
   </si>
   <si>
+    <t>Organization Units</t>
+  </si>
+  <si>
+    <t>EN\Assets.xlsx</t>
+  </si>
+  <si>
+    <t>EN\Users.xlsx</t>
+  </si>
+  <si>
+    <t>EN\Robots.xlsx</t>
+  </si>
+  <si>
+    <t>EN\Machines.xlsx</t>
+  </si>
+  <si>
+    <t>EN\Environments.xlsx</t>
+  </si>
+  <si>
+    <t>EN\Processes.xlsx</t>
+  </si>
+  <si>
+    <t>JA\アセット.xlsx</t>
+  </si>
+  <si>
+    <t>JA\ユーザー.xlsx</t>
+  </si>
+  <si>
+    <t>JA\ロボット.xlsx</t>
+  </si>
+  <si>
+    <t>JA\マシン.xlsx</t>
+  </si>
+  <si>
+    <t>JA\ロボットグループ.xlsx</t>
+  </si>
+  <si>
+    <t>JA\プロセス.xlsx</t>
+  </si>
+  <si>
+    <t>Path to the folder that contains entities workbooks.</t>
+  </si>
+  <si>
+    <t>AssetConfigFilePath</t>
+  </si>
+  <si>
+    <t>UserConfigFilePath</t>
+  </si>
+  <si>
+    <t>RobotConfigFilePath</t>
+  </si>
+  <si>
+    <t>MachineConfigFilePath</t>
+  </si>
+  <si>
+    <t>EnvironmentConfigFilePath</t>
+  </si>
+  <si>
+    <t>ProcessConfigFilePath</t>
+  </si>
+  <si>
+    <t>EntitiesWorkbooksFolderPath</t>
+  </si>
+  <si>
+    <t>Workbooks\</t>
+  </si>
+  <si>
+    <t>https://win-9d2vvsqpta7/</t>
+  </si>
+  <si>
     <t>Default</t>
-  </si>
-  <si>
-    <t>Organization Units</t>
-  </si>
-  <si>
-    <t>https://win-9d2vvsqpta7/</t>
   </si>
 </sst>
 </file>
@@ -1270,8 +1279,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{7F8F45FE-2B96-4F08-8C9F-E71B4ACCE2FA}" name="Table14" displayName="Table14" ref="A1:C3" totalsRowShown="0">
-  <autoFilter ref="A1:C3" xr:uid="{A7872B2C-8222-446D-9C51-8EA59078049C}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{7F8F45FE-2B96-4F08-8C9F-E71B4ACCE2FA}" name="Table14" displayName="Table14" ref="A1:C4" totalsRowShown="0">
+  <autoFilter ref="A1:C4" xr:uid="{A7872B2C-8222-446D-9C51-8EA59078049C}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{D8D5B6DE-5265-4940-BA42-B3804FA368B2}" name="Name"/>
     <tableColumn id="2" xr3:uid="{040BFB8F-6ACC-4B54-BAD6-564D9FD4EC4E}" name="Value"/>
@@ -1568,10 +1577,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D89C9C48-5454-47C4-AB1D-448E4519251A}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1594,29 +1603,40 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>383</v>
+        <v>385</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>286</v>
+        <v>280</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="B3" t="s">
-        <v>381</v>
+        <v>386</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>287</v>
+        <v>281</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>383</v>
+      </c>
+      <c r="B4" t="s">
+        <v>384</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>376</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{B579A2F5-99A4-49E1-B807-A008372D3262}"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{DFA77488-10FF-443E-B95E-CC939F36A29C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
@@ -1631,7 +1651,7 @@
   <dimension ref="A1:C41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1660,7 +1680,7 @@
         <v>200</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>293</v>
+        <v>287</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="29" x14ac:dyDescent="0.35">
@@ -1671,117 +1691,117 @@
         <v>0</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>292</v>
+        <v>286</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="B4">
         <v>500</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>288</v>
+        <v>282</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="B5">
         <v>600</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>289</v>
+        <v>283</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>355</v>
+        <v>349</v>
       </c>
       <c r="B6">
         <v>3</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>357</v>
+        <v>351</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>356</v>
+        <v>350</v>
       </c>
       <c r="B7">
         <v>5000</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>361</v>
+        <v>355</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="B8" t="s">
-        <v>362</v>
+        <v>356</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>291</v>
+        <v>285</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="B9" t="s">
-        <v>363</v>
+        <v>357</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>290</v>
+        <v>284</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
       <c r="B10" t="s">
-        <v>364</v>
+        <v>358</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>295</v>
+        <v>289</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="B11" t="s">
-        <v>365</v>
+        <v>359</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>294</v>
+        <v>288</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="B12" t="s">
-        <v>366</v>
+        <v>360</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>296</v>
+        <v>290</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="B13" t="s">
-        <v>367</v>
+        <v>361</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>297</v>
+        <v>291</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="29" x14ac:dyDescent="0.35">
@@ -1792,7 +1812,7 @@
         <v>30</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>298</v>
+        <v>292</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="29" x14ac:dyDescent="0.35">
@@ -1803,293 +1823,293 @@
         <v>35</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>300</v>
+        <v>294</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B16" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>305</v>
+        <v>299</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="B17" t="s">
         <v>35</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>304</v>
+        <v>298</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B18" t="s">
         <v>30</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>306</v>
+        <v>300</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B19" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>301</v>
+        <v>295</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>349</v>
+        <v>343</v>
       </c>
       <c r="B20" t="s">
         <v>30</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>306</v>
+        <v>300</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>345</v>
+        <v>339</v>
       </c>
       <c r="B21" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>346</v>
+        <v>340</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B22" t="s">
         <v>30</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>302</v>
+        <v>296</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>347</v>
+        <v>341</v>
       </c>
       <c r="B23" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>348</v>
+        <v>342</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B24" t="s">
         <v>30</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>299</v>
+        <v>293</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B25" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>312</v>
+        <v>306</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B26" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>303</v>
+        <v>297</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B27" t="s">
         <v>35</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>307</v>
+        <v>301</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B28" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>308</v>
+        <v>302</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="B29" t="s">
         <v>30</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>309</v>
+        <v>303</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="B30" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>324</v>
+        <v>318</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="B31" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>310</v>
+        <v>304</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="B32" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>311</v>
+        <v>305</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="B33" t="s">
         <v>35</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>317</v>
+        <v>311</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="B34" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>313</v>
+        <v>307</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="B35" t="s">
         <v>30</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>314</v>
+        <v>308</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="B36" t="s">
         <v>30</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>321</v>
+        <v>315</v>
       </c>
     </row>
     <row r="37" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>319</v>
+        <v>313</v>
       </c>
       <c r="B37" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>320</v>
+        <v>314</v>
       </c>
     </row>
     <row r="38" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>322</v>
+        <v>316</v>
       </c>
       <c r="B38" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>323</v>
+        <v>317</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>272</v>
+        <v>266</v>
       </c>
       <c r="B39" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>318</v>
+        <v>312</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>271</v>
+        <v>265</v>
       </c>
       <c r="B40" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>315</v>
+        <v>309</v>
       </c>
     </row>
     <row r="41" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="B41" t="s">
         <v>30</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>316</v>
+        <v>310</v>
       </c>
     </row>
   </sheetData>
@@ -2129,51 +2149,51 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>325</v>
+        <v>319</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>13</v>
@@ -2184,7 +2204,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>12</v>
@@ -2195,101 +2215,101 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>351</v>
+        <v>345</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>382</v>
+        <v>363</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>350</v>
+        <v>344</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="B11" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>204</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>209</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>235</v>
+        <v>229</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>236</v>
+        <v>230</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
+        <v>191</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>362</v>
+      </c>
+      <c r="C15" s="1" t="s">
         <v>196</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>380</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>201</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.35">
@@ -2298,68 +2318,68 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>50</v>
+        <v>377</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>58</v>
+        <v>378</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>369</v>
+        <v>365</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>375</v>
+        <v>371</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>65</v>
+        <v>379</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>370</v>
+        <v>366</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>376</v>
+        <v>372</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>36</v>
+        <v>380</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>377</v>
+        <v>373</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>164</v>
+        <v>381</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>378</v>
+        <v>374</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>233</v>
+        <v>382</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>379</v>
+        <v>375</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.35">
@@ -2412,68 +2432,68 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>339</v>
+        <v>333</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>341</v>
+        <v>335</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>343</v>
+        <v>337</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>340</v>
+        <v>334</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>342</v>
+        <v>336</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>344</v>
+        <v>338</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>329</v>
+        <v>323</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>327</v>
+        <v>321</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>326</v>
+        <v>320</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>328</v>
+        <v>322</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>260</v>
+        <v>254</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>261</v>
+        <v>255</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.35">
@@ -2515,134 +2535,134 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
+        <v>37</v>
+      </c>
+      <c r="B39" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B39" s="1" t="s">
+      <c r="C39" s="1" t="s">
         <v>39</v>
-      </c>
-      <c r="C39" s="1" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>352</v>
+        <v>346</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>353</v>
+        <v>347</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>354</v>
+        <v>348</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
-        <v>358</v>
+        <v>352</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>359</v>
+        <v>353</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>360</v>
+        <v>354</v>
       </c>
     </row>
     <row r="42" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
+        <v>40</v>
+      </c>
+      <c r="B42" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B42" s="1" t="s">
+      <c r="C42" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="C42" s="1" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
+        <v>43</v>
+      </c>
+      <c r="B44" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B44" s="1" t="s">
+      <c r="C44" s="1" t="s">
         <v>45</v>
-      </c>
-      <c r="C44" s="1" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.35">
@@ -2651,90 +2671,90 @@
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
+        <v>49</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C52" s="1" t="s">
         <v>51</v>
-      </c>
-      <c r="B52" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="C52" s="1" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
-        <v>330</v>
+        <v>324</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>332</v>
+        <v>326</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>331</v>
+        <v>325</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
-        <v>335</v>
+        <v>329</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>334</v>
+        <v>328</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>333</v>
+        <v>327</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
-        <v>336</v>
+        <v>330</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>337</v>
+        <v>331</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>338</v>
+        <v>332</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.35">
@@ -2743,101 +2763,101 @@
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>251</v>
+        <v>245</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
-        <v>262</v>
+        <v>256</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>263</v>
+        <v>257</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>264</v>
+        <v>258</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
-        <v>256</v>
+        <v>250</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>257</v>
+        <v>251</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>258</v>
+        <v>252</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.35">
@@ -2846,90 +2866,90 @@
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.35">
@@ -2938,189 +2958,189 @@
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
+        <v>46</v>
+      </c>
+      <c r="B81" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B81" s="1" t="s">
+      <c r="C81" s="1" t="s">
         <v>48</v>
-      </c>
-      <c r="C81" s="1" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
-        <v>253</v>
+        <v>247</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>255</v>
+        <v>249</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>244</v>
+        <v>238</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>245</v>
+        <v>239</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="B92" t="s">
-        <v>239</v>
+        <v>233</v>
       </c>
       <c r="C92" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="B93" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="C93" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="C94" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="B95" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="C95" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>252</v>
+        <v>246</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
-        <v>246</v>
+        <v>240</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>247</v>
+        <v>241</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>248</v>
+        <v>242</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.35">
@@ -3129,46 +3149,46 @@
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
-        <v>265</v>
+        <v>259</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>266</v>
+        <v>260</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>267</v>
+        <v>261</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
-        <v>276</v>
+        <v>270</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>277</v>
+        <v>271</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>278</v>
+        <v>272</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
-        <v>279</v>
+        <v>273</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>280</v>
+        <v>274</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>281</v>
+        <v>275</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
-        <v>282</v>
+        <v>276</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>283</v>
+        <v>277</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>284</v>
+        <v>278</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.35">
@@ -3177,24 +3197,24 @@
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
-        <v>268</v>
+        <v>262</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>269</v>
+        <v>263</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
-        <v>273</v>
+        <v>267</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>274</v>
+        <v>268</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>275</v>
+        <v>269</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add explanation about UiPath Cloud Platform not being supported
</commit_message>
<xml_diff>
--- a/Config.xlsx
+++ b/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mateus.cruz\Documents\GitHub\OrchestratorManager\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96A6F0E7-1CF6-4E04-81D9-A29A007B7E9E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB3316B7-08AA-402C-AFB0-60519D476816}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -877,9 +877,6 @@
     <t>DeleteProcessResultColumn</t>
   </si>
   <si>
-    <t>URL of the Orchestrator instance to be used.</t>
-  </si>
-  <si>
     <t>Name of the tenant to be used.</t>
   </si>
   <si>
@@ -1197,6 +1194,9 @@
   </si>
   <si>
     <t>Default</t>
+  </si>
+  <si>
+    <t>URL of the Orchestrator instance to be used. UiPath Cloud Platform (https://platform.uipath.com) is currently not supported.</t>
   </si>
 </sst>
 </file>
@@ -1580,7 +1580,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1601,15 +1601,15 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>56</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>280</v>
+        <v>386</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
@@ -1617,21 +1617,21 @@
         <v>214</v>
       </c>
       <c r="B3" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
+        <v>382</v>
+      </c>
+      <c r="B4" t="s">
         <v>383</v>
       </c>
-      <c r="B4" t="s">
-        <v>384</v>
-      </c>
       <c r="C4" s="1" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
   </sheetData>
@@ -1680,7 +1680,7 @@
         <v>200</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="29" x14ac:dyDescent="0.35">
@@ -1691,7 +1691,7 @@
         <v>0</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
@@ -1702,7 +1702,7 @@
         <v>500</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
@@ -1713,29 +1713,29 @@
         <v>600</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B6">
         <v>3</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B7">
         <v>5000</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
@@ -1743,10 +1743,10 @@
         <v>185</v>
       </c>
       <c r="B8" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
@@ -1754,10 +1754,10 @@
         <v>186</v>
       </c>
       <c r="B9" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="29" x14ac:dyDescent="0.35">
@@ -1765,10 +1765,10 @@
         <v>226</v>
       </c>
       <c r="B10" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
@@ -1776,10 +1776,10 @@
         <v>227</v>
       </c>
       <c r="B11" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
@@ -1787,10 +1787,10 @@
         <v>212</v>
       </c>
       <c r="B12" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
@@ -1798,10 +1798,10 @@
         <v>213</v>
       </c>
       <c r="B13" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="29" x14ac:dyDescent="0.35">
@@ -1812,7 +1812,7 @@
         <v>30</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="29" x14ac:dyDescent="0.35">
@@ -1823,7 +1823,7 @@
         <v>35</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
@@ -1834,7 +1834,7 @@
         <v>36</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.35">
@@ -1845,7 +1845,7 @@
         <v>35</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.35">
@@ -1856,7 +1856,7 @@
         <v>30</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="29" x14ac:dyDescent="0.35">
@@ -1867,29 +1867,29 @@
         <v>53</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="B20" t="s">
         <v>30</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B21" t="s">
         <v>53</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.35">
@@ -1900,18 +1900,18 @@
         <v>30</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B23" t="s">
         <v>53</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="29" x14ac:dyDescent="0.35">
@@ -1922,7 +1922,7 @@
         <v>30</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.35">
@@ -1933,7 +1933,7 @@
         <v>57</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="29" x14ac:dyDescent="0.35">
@@ -1944,7 +1944,7 @@
         <v>59</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="29" x14ac:dyDescent="0.35">
@@ -1955,7 +1955,7 @@
         <v>35</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.35">
@@ -1966,7 +1966,7 @@
         <v>223</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="29" x14ac:dyDescent="0.35">
@@ -1977,7 +1977,7 @@
         <v>30</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.35">
@@ -1988,7 +1988,7 @@
         <v>57</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="29" x14ac:dyDescent="0.35">
@@ -1999,7 +1999,7 @@
         <v>59</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.35">
@@ -2010,7 +2010,7 @@
         <v>57</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.35">
@@ -2021,7 +2021,7 @@
         <v>35</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="29" x14ac:dyDescent="0.35">
@@ -2032,7 +2032,7 @@
         <v>36</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="29" x14ac:dyDescent="0.35">
@@ -2043,7 +2043,7 @@
         <v>30</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="29" x14ac:dyDescent="0.35">
@@ -2054,29 +2054,29 @@
         <v>30</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="37" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B37" t="s">
         <v>36</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="38" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B38" t="s">
         <v>36</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.35">
@@ -2087,7 +2087,7 @@
         <v>53</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="29" x14ac:dyDescent="0.35">
@@ -2098,7 +2098,7 @@
         <v>223</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="41" spans="1:3" ht="29" x14ac:dyDescent="0.35">
@@ -2109,7 +2109,7 @@
         <v>30</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
   </sheetData>
@@ -2163,7 +2163,7 @@
         <v>221</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>222</v>
@@ -2215,13 +2215,13 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
@@ -2295,7 +2295,7 @@
         <v>191</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>196</v>
@@ -2318,68 +2318,68 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.35">
@@ -2432,29 +2432,29 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>176</v>
@@ -2465,10 +2465,10 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>253</v>
@@ -2476,7 +2476,7 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>254</v>
@@ -2546,24 +2546,24 @@
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
+        <v>345</v>
+      </c>
+      <c r="B40" s="1" t="s">
         <v>346</v>
       </c>
-      <c r="B40" s="1" t="s">
+      <c r="C40" s="1" t="s">
         <v>347</v>
-      </c>
-      <c r="C40" s="1" t="s">
-        <v>348</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
+        <v>351</v>
+      </c>
+      <c r="B41" s="1" t="s">
         <v>352</v>
       </c>
-      <c r="B41" s="1" t="s">
+      <c r="C41" s="1" t="s">
         <v>353</v>
-      </c>
-      <c r="C41" s="1" t="s">
-        <v>354</v>
       </c>
     </row>
     <row r="42" spans="1:3" ht="29" x14ac:dyDescent="0.35">
@@ -2726,35 +2726,35 @@
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
+        <v>323</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>325</v>
+      </c>
+      <c r="C57" s="1" t="s">
         <v>324</v>
-      </c>
-      <c r="B57" s="1" t="s">
-        <v>326</v>
-      </c>
-      <c r="C57" s="1" t="s">
-        <v>325</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
+        <v>329</v>
+      </c>
+      <c r="B59" s="1" t="s">
         <v>330</v>
       </c>
-      <c r="B59" s="1" t="s">
+      <c r="C59" s="1" t="s">
         <v>331</v>
-      </c>
-      <c r="C59" s="1" t="s">
-        <v>332</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Add verification for mandatory arguments
</commit_message>
<xml_diff>
--- a/Config.xlsx
+++ b/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mateus.cruz\Documents\GitHub\OrchestratorManager\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB3316B7-08AA-402C-AFB0-60519D476816}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C551DFC9-CECF-4EDF-9CCA-2AFE49D5F224}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -877,9 +877,6 @@
     <t>DeleteProcessResultColumn</t>
   </si>
   <si>
-    <t>Name of the tenant to be used.</t>
-  </si>
-  <si>
     <t>Height of the window used to show forms.</t>
   </si>
   <si>
@@ -1163,9 +1160,6 @@
     <t>JA\プロセス.xlsx</t>
   </si>
   <si>
-    <t>Path to the folder that contains entities workbooks.</t>
-  </si>
-  <si>
     <t>AssetConfigFilePath</t>
   </si>
   <si>
@@ -1187,16 +1181,26 @@
     <t>EntitiesWorkbooksFolderPath</t>
   </si>
   <si>
-    <t>Workbooks\</t>
-  </si>
-  <si>
-    <t>https://win-9d2vvsqpta7/</t>
-  </si>
-  <si>
-    <t>Default</t>
-  </si>
-  <si>
-    <t>URL of the Orchestrator instance to be used. UiPath Cloud Platform (https://platform.uipath.com) is currently not supported.</t>
+    <t>MandatoryArgumentsNotSpecified</t>
+  </si>
+  <si>
+    <t>Mandatory arguments not specified.</t>
+  </si>
+  <si>
+    <t>必須引数が指定されませんでした。</t>
+  </si>
+  <si>
+    <t>URL of the Orchestrator instance to be used. 
+Sample value: https://myOrchestratorurl.
+UiPath Cloud Platform (https://platform.uipath.com) is currently not supported.</t>
+  </si>
+  <si>
+    <t>Name of the tenant to be used. 
+Sample value: Default.</t>
+  </si>
+  <si>
+    <t>Path to the folder that contains entities workbooks. 
+Sample value: C:\Users\MyUser\Desktop\Workbooks</t>
   </si>
 </sst>
 </file>
@@ -1601,47 +1605,36 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" ht="58" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>56</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="2"/>
+      <c r="C2" s="1" t="s">
         <v>384</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>386</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    </row>
+    <row r="3" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>214</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" s="1" t="s">
         <v>385</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    </row>
+    <row r="4" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>382</v>
-      </c>
-      <c r="B4" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>375</v>
+        <v>386</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{DFA77488-10FF-443E-B95E-CC939F36A29C}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
@@ -1680,7 +1673,7 @@
         <v>200</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="29" x14ac:dyDescent="0.35">
@@ -1691,7 +1684,7 @@
         <v>0</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
@@ -1702,7 +1695,7 @@
         <v>500</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
@@ -1713,29 +1706,29 @@
         <v>600</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B6">
         <v>3</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B7">
         <v>5000</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
@@ -1743,10 +1736,10 @@
         <v>185</v>
       </c>
       <c r="B8" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
@@ -1754,10 +1747,10 @@
         <v>186</v>
       </c>
       <c r="B9" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="29" x14ac:dyDescent="0.35">
@@ -1765,10 +1758,10 @@
         <v>226</v>
       </c>
       <c r="B10" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
@@ -1776,10 +1769,10 @@
         <v>227</v>
       </c>
       <c r="B11" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
@@ -1787,10 +1780,10 @@
         <v>212</v>
       </c>
       <c r="B12" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
@@ -1798,10 +1791,10 @@
         <v>213</v>
       </c>
       <c r="B13" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="29" x14ac:dyDescent="0.35">
@@ -1812,7 +1805,7 @@
         <v>30</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="29" x14ac:dyDescent="0.35">
@@ -1823,7 +1816,7 @@
         <v>35</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
@@ -1834,7 +1827,7 @@
         <v>36</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.35">
@@ -1845,7 +1838,7 @@
         <v>35</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.35">
@@ -1856,7 +1849,7 @@
         <v>30</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="29" x14ac:dyDescent="0.35">
@@ -1867,29 +1860,29 @@
         <v>53</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="B20" t="s">
         <v>30</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B21" t="s">
         <v>53</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.35">
@@ -1900,18 +1893,18 @@
         <v>30</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="B23" t="s">
         <v>53</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="29" x14ac:dyDescent="0.35">
@@ -1922,7 +1915,7 @@
         <v>30</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.35">
@@ -1933,7 +1926,7 @@
         <v>57</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="29" x14ac:dyDescent="0.35">
@@ -1944,7 +1937,7 @@
         <v>59</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="29" x14ac:dyDescent="0.35">
@@ -1955,7 +1948,7 @@
         <v>35</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.35">
@@ -1966,7 +1959,7 @@
         <v>223</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="29" x14ac:dyDescent="0.35">
@@ -1977,7 +1970,7 @@
         <v>30</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.35">
@@ -1988,7 +1981,7 @@
         <v>57</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="29" x14ac:dyDescent="0.35">
@@ -1999,7 +1992,7 @@
         <v>59</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.35">
@@ -2010,7 +2003,7 @@
         <v>57</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.35">
@@ -2021,7 +2014,7 @@
         <v>35</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="29" x14ac:dyDescent="0.35">
@@ -2032,7 +2025,7 @@
         <v>36</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="29" x14ac:dyDescent="0.35">
@@ -2043,7 +2036,7 @@
         <v>30</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="29" x14ac:dyDescent="0.35">
@@ -2054,29 +2047,29 @@
         <v>30</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="37" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="B37" t="s">
         <v>36</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="38" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="B38" t="s">
         <v>36</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.35">
@@ -2087,7 +2080,7 @@
         <v>53</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="29" x14ac:dyDescent="0.35">
@@ -2098,7 +2091,7 @@
         <v>223</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="41" spans="1:3" ht="29" x14ac:dyDescent="0.35">
@@ -2109,7 +2102,7 @@
         <v>30</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
   </sheetData>
@@ -2163,7 +2156,7 @@
         <v>221</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>222</v>
@@ -2215,13 +2208,13 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
@@ -2295,7 +2288,7 @@
         <v>191</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>196</v>
@@ -2318,68 +2311,68 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.35">
@@ -2432,29 +2425,29 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>176</v>
@@ -2465,10 +2458,10 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>253</v>
@@ -2476,7 +2469,7 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>254</v>
@@ -2497,8 +2490,15 @@
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B35" s="1"/>
-      <c r="C35" s="1"/>
+      <c r="A35" t="s">
+        <v>381</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>382</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>383</v>
+      </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
@@ -2546,24 +2546,24 @@
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
+        <v>344</v>
+      </c>
+      <c r="B40" s="1" t="s">
         <v>345</v>
       </c>
-      <c r="B40" s="1" t="s">
+      <c r="C40" s="1" t="s">
         <v>346</v>
-      </c>
-      <c r="C40" s="1" t="s">
-        <v>347</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
+        <v>350</v>
+      </c>
+      <c r="B41" s="1" t="s">
         <v>351</v>
       </c>
-      <c r="B41" s="1" t="s">
+      <c r="C41" s="1" t="s">
         <v>352</v>
-      </c>
-      <c r="C41" s="1" t="s">
-        <v>353</v>
       </c>
     </row>
     <row r="42" spans="1:3" ht="29" x14ac:dyDescent="0.35">
@@ -2726,35 +2726,35 @@
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
+        <v>322</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="C57" s="1" t="s">
         <v>323</v>
-      </c>
-      <c r="B57" s="1" t="s">
-        <v>325</v>
-      </c>
-      <c r="C57" s="1" t="s">
-        <v>324</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
+        <v>328</v>
+      </c>
+      <c r="B59" s="1" t="s">
         <v>329</v>
       </c>
-      <c r="B59" s="1" t="s">
+      <c r="C59" s="1" t="s">
         <v>330</v>
-      </c>
-      <c r="C59" s="1" t="s">
-        <v>331</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Change AddOrRemoveRobots localization string
</commit_message>
<xml_diff>
--- a/Config.xlsx
+++ b/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mateus.cruz\Documents\GitHub\OrchestratorManager\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{290B3149-3FBE-4179-8F25-A36F9F085AAD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{183092F0-D80F-4E9F-9A3D-849A2AA8D578}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -565,9 +565,6 @@
     <t>{0}というロボットが見つかりませんでした。</t>
   </si>
   <si>
-    <t>Add Or Remove Robots</t>
-  </si>
-  <si>
     <t>SurnameNotSpecified</t>
   </si>
   <si>
@@ -797,9 +794,6 @@
   </si>
   <si>
     <t>組織単位の追加・削除</t>
-  </si>
-  <si>
-    <t>Add Or Remove Roles</t>
   </si>
   <si>
     <t>ロールの追加・削除</t>
@@ -990,9 +984,6 @@
   </si>
   <si>
     <t>Please mind that many unsuccessful login attempts can temporarily lock the account, as specified in the Security settings of the tenant.</t>
-  </si>
-  <si>
-    <t>Add Or Remove OUs</t>
   </si>
   <si>
     <t>AddRemoveUserOrganizationUnitsOperationName</t>
@@ -1201,6 +1192,15 @@
   <si>
     <t>Path to the folder that contains entities workbooks. 
 Sample value: C:\Users\MyUser\Desktop\Workbooks</t>
+  </si>
+  <si>
+    <t>Add or Remove Robots</t>
+  </si>
+  <si>
+    <t>Add or Remove OUs</t>
+  </si>
+  <si>
+    <t>Add or Remove Roles</t>
   </si>
 </sst>
 </file>
@@ -1611,23 +1611,23 @@
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="1" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
     </row>
   </sheetData>
@@ -1673,7 +1673,7 @@
         <v>200</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="29" x14ac:dyDescent="0.35">
@@ -1684,117 +1684,117 @@
         <v>0</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B4">
         <v>500</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B5">
         <v>600</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="B6">
         <v>3</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="B7">
         <v>5000</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B8" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B9" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B10" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B11" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B12" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B13" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="29" x14ac:dyDescent="0.35">
@@ -1805,7 +1805,7 @@
         <v>30</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="29" x14ac:dyDescent="0.35">
@@ -1816,7 +1816,7 @@
         <v>35</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
@@ -1827,7 +1827,7 @@
         <v>36</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.35">
@@ -1838,7 +1838,7 @@
         <v>35</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.35">
@@ -1849,7 +1849,7 @@
         <v>30</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="29" x14ac:dyDescent="0.35">
@@ -1860,29 +1860,29 @@
         <v>53</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="B20" t="s">
         <v>30</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="B21" t="s">
         <v>53</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.35">
@@ -1893,18 +1893,18 @@
         <v>30</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="B23" t="s">
         <v>53</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="29" x14ac:dyDescent="0.35">
@@ -1915,7 +1915,7 @@
         <v>30</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.35">
@@ -1926,7 +1926,7 @@
         <v>57</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="29" x14ac:dyDescent="0.35">
@@ -1937,7 +1937,7 @@
         <v>59</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="29" x14ac:dyDescent="0.35">
@@ -1948,7 +1948,7 @@
         <v>35</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.35">
@@ -1956,10 +1956,10 @@
         <v>61</v>
       </c>
       <c r="B28" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="29" x14ac:dyDescent="0.35">
@@ -1970,7 +1970,7 @@
         <v>30</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.35">
@@ -1981,7 +1981,7 @@
         <v>57</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="29" x14ac:dyDescent="0.35">
@@ -1992,7 +1992,7 @@
         <v>59</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.35">
@@ -2003,7 +2003,7 @@
         <v>57</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.35">
@@ -2014,7 +2014,7 @@
         <v>35</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="29" x14ac:dyDescent="0.35">
@@ -2025,7 +2025,7 @@
         <v>36</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="29" x14ac:dyDescent="0.35">
@@ -2036,7 +2036,7 @@
         <v>30</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="29" x14ac:dyDescent="0.35">
@@ -2047,62 +2047,62 @@
         <v>30</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
     </row>
     <row r="37" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="B37" t="s">
         <v>36</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
     </row>
     <row r="38" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="B38" t="s">
         <v>36</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="B39" t="s">
         <v>53</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B40" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
     </row>
     <row r="41" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="B41" t="s">
         <v>30</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
     </row>
   </sheetData>
@@ -2142,51 +2142,51 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
+        <v>220</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>315</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>221</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>317</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>222</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>13</v>
@@ -2197,7 +2197,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>12</v>
@@ -2208,101 +2208,101 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B9" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>201</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>202</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
+        <v>227</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>228</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="C14" s="1" t="s">
         <v>229</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>230</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
+        <v>214</v>
+      </c>
+      <c r="B16" s="1" t="s">
         <v>215</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="C16" s="1" t="s">
         <v>216</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>217</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.35">
@@ -2311,68 +2311,68 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>366</v>
+        <v>363</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.35">
@@ -2425,32 +2425,32 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>176</v>
+        <v>384</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>171</v>
@@ -2458,46 +2458,46 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>318</v>
+        <v>385</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>254</v>
+        <v>386</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
+        <v>218</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="C34" s="1" t="s">
         <v>219</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>218</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>220</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.35">
@@ -2546,24 +2546,24 @@
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
     </row>
     <row r="42" spans="1:3" ht="29" x14ac:dyDescent="0.35">
@@ -2726,35 +2726,35 @@
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.35">
@@ -2807,57 +2807,57 @@
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
+        <v>176</v>
+      </c>
+      <c r="B65" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="B65" s="1" t="s">
+      <c r="C65" s="1" t="s">
         <v>178</v>
-      </c>
-      <c r="C65" s="1" t="s">
-        <v>179</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
+        <v>179</v>
+      </c>
+      <c r="B66" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="B66" s="1" t="s">
+      <c r="C66" s="1" t="s">
         <v>181</v>
-      </c>
-      <c r="C66" s="1" t="s">
-        <v>182</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
+        <v>242</v>
+      </c>
+      <c r="B67" s="1" t="s">
         <v>243</v>
       </c>
-      <c r="B67" s="1" t="s">
+      <c r="C67" s="1" t="s">
         <v>244</v>
-      </c>
-      <c r="C67" s="1" t="s">
-        <v>245</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
+        <v>254</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="C68" s="1" t="s">
         <v>256</v>
-      </c>
-      <c r="B68" s="1" t="s">
-        <v>257</v>
-      </c>
-      <c r="C68" s="1" t="s">
-        <v>258</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
+        <v>249</v>
+      </c>
+      <c r="B69" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="B69" s="1" t="s">
+      <c r="C69" s="1" t="s">
         <v>251</v>
-      </c>
-      <c r="C69" s="1" t="s">
-        <v>252</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.35">
@@ -2991,13 +2991,13 @@
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
+        <v>246</v>
+      </c>
+      <c r="B83" s="1" t="s">
         <v>247</v>
       </c>
-      <c r="B83" s="1" t="s">
+      <c r="C83" s="1" t="s">
         <v>248</v>
-      </c>
-      <c r="C83" s="1" t="s">
-        <v>249</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.35">
@@ -3046,13 +3046,13 @@
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
+        <v>236</v>
+      </c>
+      <c r="B89" s="1" t="s">
         <v>237</v>
       </c>
-      <c r="B89" s="1" t="s">
+      <c r="C89" s="1" t="s">
         <v>238</v>
-      </c>
-      <c r="C89" s="1" t="s">
-        <v>239</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.35">
@@ -3071,7 +3071,7 @@
         <v>149</v>
       </c>
       <c r="B92" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C92" t="s">
         <v>150</v>
@@ -3112,35 +3112,35 @@
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
+        <v>223</v>
+      </c>
+      <c r="B96" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="C96" s="1" t="s">
         <v>224</v>
-      </c>
-      <c r="B96" s="1" t="s">
-        <v>246</v>
-      </c>
-      <c r="C96" s="1" t="s">
-        <v>225</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
+        <v>233</v>
+      </c>
+      <c r="B98" s="1" t="s">
         <v>234</v>
       </c>
-      <c r="B98" s="1" t="s">
+      <c r="C98" s="1" t="s">
         <v>235</v>
-      </c>
-      <c r="C98" s="1" t="s">
-        <v>236</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
+        <v>239</v>
+      </c>
+      <c r="B99" s="1" t="s">
         <v>240</v>
       </c>
-      <c r="B99" s="1" t="s">
+      <c r="C99" s="1" t="s">
         <v>241</v>
-      </c>
-      <c r="C99" s="1" t="s">
-        <v>242</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.35">
@@ -3149,46 +3149,46 @@
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
+        <v>257</v>
+      </c>
+      <c r="B101" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="C101" s="1" t="s">
         <v>259</v>
-      </c>
-      <c r="B101" s="1" t="s">
-        <v>260</v>
-      </c>
-      <c r="C101" s="1" t="s">
-        <v>261</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
+        <v>268</v>
+      </c>
+      <c r="B102" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="C102" s="1" t="s">
         <v>270</v>
-      </c>
-      <c r="B102" s="1" t="s">
-        <v>271</v>
-      </c>
-      <c r="C102" s="1" t="s">
-        <v>272</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
+        <v>271</v>
+      </c>
+      <c r="B103" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="C103" s="1" t="s">
         <v>273</v>
-      </c>
-      <c r="B103" s="1" t="s">
-        <v>274</v>
-      </c>
-      <c r="C103" s="1" t="s">
-        <v>275</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
+        <v>274</v>
+      </c>
+      <c r="B104" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="C104" s="1" t="s">
         <v>276</v>
-      </c>
-      <c r="B104" s="1" t="s">
-        <v>277</v>
-      </c>
-      <c r="C104" s="1" t="s">
-        <v>278</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.35">
@@ -3197,24 +3197,24 @@
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
+        <v>260</v>
+      </c>
+      <c r="B106" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="C106" s="1" t="s">
         <v>262</v>
-      </c>
-      <c r="B106" s="1" t="s">
-        <v>263</v>
-      </c>
-      <c r="C106" s="1" t="s">
-        <v>264</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
+        <v>265</v>
+      </c>
+      <c r="B107" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="C107" s="1" t="s">
         <v>267</v>
-      </c>
-      <c r="B107" s="1" t="s">
-        <v>268</v>
-      </c>
-      <c r="C107" s="1" t="s">
-        <v>269</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add default value to workbooks path
</commit_message>
<xml_diff>
--- a/Config.xlsx
+++ b/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mateus.cruz\Documents\GitHub\OrchestratorManager\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{183092F0-D80F-4E9F-9A3D-849A2AA8D578}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16BE9BED-DE3E-4A42-B959-BB2EF612BA5E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="414" uniqueCount="387">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="415" uniqueCount="388">
   <si>
     <t>Name</t>
   </si>
@@ -1201,6 +1201,9 @@
   </si>
   <si>
     <t>Add or Remove Roles</t>
+  </si>
+  <si>
+    <t>Workbooks</t>
   </si>
 </sst>
 </file>
@@ -1626,6 +1629,9 @@
       <c r="A4" t="s">
         <v>377</v>
       </c>
+      <c r="B4" t="s">
+        <v>387</v>
+      </c>
       <c r="C4" s="1" t="s">
         <v>383</v>
       </c>

</xml_diff>

<commit_message>
Fixed bug that would prevent retrying after a new token is retrieved
</commit_message>
<xml_diff>
--- a/Config.xlsx
+++ b/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mateus.cruz\Documents\GitHub\OrchestratorManager\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16BE9BED-DE3E-4A42-B959-BB2EF612BA5E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85A05FB8-F551-4CC7-981A-6855DA3CFF76}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="415" uniqueCount="388">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="418" uniqueCount="391">
   <si>
     <t>Name</t>
   </si>
@@ -1204,6 +1204,15 @@
   </si>
   <si>
     <t>Workbooks</t>
+  </si>
+  <si>
+    <t>TokenExpired</t>
+  </si>
+  <si>
+    <t>Authentication token expired.</t>
+  </si>
+  <si>
+    <t>認証トークンの期限が切れました。</t>
   </si>
 </sst>
 </file>
@@ -1310,8 +1319,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{F8A6BD26-C645-4175-8476-817D5672FD54}" name="Table13" displayName="Table13" ref="A1:C107" totalsRowShown="0">
-  <autoFilter ref="A1:C107" xr:uid="{A7872B2C-8222-446D-9C51-8EA59078049C}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{F8A6BD26-C645-4175-8476-817D5672FD54}" name="Table13" displayName="Table13" ref="A1:C108" totalsRowShown="0">
+  <autoFilter ref="A1:C108" xr:uid="{A7872B2C-8222-446D-9C51-8EA59078049C}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{5D541690-4DCC-4D96-9FCC-B1699146EC35}" name="Name"/>
     <tableColumn id="2" xr3:uid="{86DF2464-58F6-48AD-98C9-2D16B29FBB6F}" name="EN" dataDxfId="1"/>
@@ -2122,7 +2131,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1927ABA9-1814-4487-9CEC-ABDCAF91481F}">
-  <dimension ref="A1:C107"/>
+  <dimension ref="A1:C108"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -2552,674 +2561,685 @@
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>341</v>
+        <v>388</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>342</v>
+        <v>389</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>343</v>
+        <v>390</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
+        <v>341</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>342</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A42" t="s">
         <v>347</v>
       </c>
-      <c r="B41" s="1" t="s">
+      <c r="B42" s="1" t="s">
         <v>348</v>
       </c>
-      <c r="C41" s="1" t="s">
+      <c r="C42" s="1" t="s">
         <v>349</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="29" x14ac:dyDescent="0.35">
-      <c r="A42" t="s">
+    <row r="43" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="A43" t="s">
         <v>40</v>
       </c>
-      <c r="B42" s="1" t="s">
+      <c r="B43" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C42" s="1" t="s">
+      <c r="C43" s="1" t="s">
         <v>42</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A43" t="s">
-        <v>93</v>
-      </c>
-      <c r="B43" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="C43" s="1" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
-        <v>43</v>
+        <v>93</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>44</v>
+        <v>94</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>45</v>
+        <v>92</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
-        <v>88</v>
+        <v>43</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>87</v>
+        <v>44</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>86</v>
+        <v>45</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
-        <v>113</v>
+        <v>89</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>116</v>
+        <v>90</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>119</v>
+        <v>91</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
+        <v>115</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A51" t="s">
         <v>83</v>
       </c>
-      <c r="B50" s="1" t="s">
+      <c r="B51" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="C50" s="1" t="s">
+      <c r="C51" s="1" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B51" s="1"/>
-      <c r="C51" s="1"/>
-    </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A52" t="s">
-        <v>49</v>
-      </c>
-      <c r="B52" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="C52" s="1" t="s">
-        <v>51</v>
-      </c>
+      <c r="B52" s="1"/>
+      <c r="C52" s="1"/>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
-        <v>75</v>
+        <v>49</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>85</v>
+        <v>50</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>81</v>
+        <v>51</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
-        <v>95</v>
+        <v>75</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>97</v>
+        <v>81</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>112</v>
+        <v>102</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
-        <v>319</v>
+        <v>107</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>321</v>
+        <v>112</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>320</v>
+        <v>108</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
-        <v>324</v>
+        <v>319</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
+        <v>324</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>323</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A60" t="s">
         <v>325</v>
       </c>
-      <c r="B59" s="1" t="s">
+      <c r="B60" s="1" t="s">
         <v>326</v>
       </c>
-      <c r="C59" s="1" t="s">
+      <c r="C60" s="1" t="s">
         <v>327</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B60" s="1"/>
-      <c r="C60" s="1"/>
-    </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A61" t="s">
-        <v>124</v>
-      </c>
-      <c r="B61" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="C61" s="1" t="s">
-        <v>126</v>
-      </c>
+      <c r="B61" s="1"/>
+      <c r="C61" s="1"/>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
-        <v>176</v>
+        <v>133</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>177</v>
+        <v>134</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>178</v>
+        <v>135</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
-        <v>242</v>
+        <v>179</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>243</v>
+        <v>180</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>244</v>
+        <v>181</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
-        <v>254</v>
+        <v>242</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>255</v>
+        <v>243</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>256</v>
+        <v>244</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
+        <v>254</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A70" t="s">
         <v>249</v>
       </c>
-      <c r="B69" s="1" t="s">
+      <c r="B70" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="C69" s="1" t="s">
+      <c r="C70" s="1" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B70" s="1"/>
-      <c r="C70" s="1"/>
-    </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A71" t="s">
-        <v>62</v>
-      </c>
-      <c r="B71" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="C71" s="1" t="s">
-        <v>63</v>
-      </c>
+      <c r="B71" s="1"/>
+      <c r="C71" s="1"/>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>123</v>
+        <v>172</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>78</v>
+        <v>63</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
-        <v>136</v>
+        <v>67</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>137</v>
+        <v>123</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>138</v>
+        <v>78</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
+        <v>154</v>
+      </c>
+      <c r="B78" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="C78" s="1" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A79" t="s">
         <v>173</v>
       </c>
-      <c r="B78" s="1" t="s">
+      <c r="B79" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="C78" s="1" t="s">
+      <c r="C79" s="1" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B79" s="1"/>
-      <c r="C79" s="1"/>
-    </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A80" t="s">
-        <v>66</v>
-      </c>
-      <c r="B80" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="C80" s="1" t="s">
-        <v>79</v>
-      </c>
+      <c r="B80" s="1"/>
+      <c r="C80" s="1"/>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
-        <v>46</v>
+        <v>66</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>47</v>
+        <v>122</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>48</v>
+        <v>79</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
-        <v>142</v>
+        <v>46</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>143</v>
+        <v>47</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>144</v>
+        <v>48</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
+        <v>142</v>
+      </c>
+      <c r="B83" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="C83" s="1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A84" t="s">
         <v>246</v>
       </c>
-      <c r="B83" s="1" t="s">
+      <c r="B84" s="1" t="s">
         <v>247</v>
       </c>
-      <c r="C83" s="1" t="s">
+      <c r="C84" s="1" t="s">
         <v>248</v>
-      </c>
-    </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A85" t="s">
-        <v>68</v>
-      </c>
-      <c r="B85" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="C85" s="1" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
-        <v>98</v>
+        <v>68</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>99</v>
+        <v>76</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>100</v>
+        <v>77</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
+        <v>109</v>
+      </c>
+      <c r="B89" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="C89" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A90" t="s">
         <v>236</v>
       </c>
-      <c r="B89" s="1" t="s">
+      <c r="B90" s="1" t="s">
         <v>237</v>
       </c>
-      <c r="C89" s="1" t="s">
+      <c r="C90" s="1" t="s">
         <v>238</v>
-      </c>
-    </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A91" t="s">
-        <v>72</v>
-      </c>
-      <c r="B91" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="C91" s="1" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
-        <v>149</v>
-      </c>
-      <c r="B92" t="s">
-        <v>232</v>
-      </c>
-      <c r="C92" t="s">
-        <v>150</v>
+        <v>72</v>
+      </c>
+      <c r="B92" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="C92" s="1" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
-        <v>160</v>
+        <v>149</v>
       </c>
       <c r="B93" t="s">
-        <v>161</v>
+        <v>232</v>
       </c>
       <c r="C93" t="s">
-        <v>162</v>
+        <v>150</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
-        <v>163</v>
-      </c>
-      <c r="B94" s="1" t="s">
-        <v>164</v>
+        <v>160</v>
+      </c>
+      <c r="B94" t="s">
+        <v>161</v>
       </c>
       <c r="C94" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
-        <v>167</v>
-      </c>
-      <c r="B95" t="s">
-        <v>168</v>
+        <v>163</v>
+      </c>
+      <c r="B95" s="1" t="s">
+        <v>164</v>
       </c>
       <c r="C95" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
+        <v>167</v>
+      </c>
+      <c r="B96" t="s">
+        <v>168</v>
+      </c>
+      <c r="C96" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A97" t="s">
         <v>223</v>
       </c>
-      <c r="B96" s="1" t="s">
+      <c r="B97" s="1" t="s">
         <v>245</v>
       </c>
-      <c r="C96" s="1" t="s">
+      <c r="C97" s="1" t="s">
         <v>224</v>
-      </c>
-    </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A98" t="s">
-        <v>233</v>
-      </c>
-      <c r="B98" s="1" t="s">
-        <v>234</v>
-      </c>
-      <c r="C98" s="1" t="s">
-        <v>235</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
+        <v>233</v>
+      </c>
+      <c r="B99" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="C99" s="1" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A100" t="s">
         <v>239</v>
       </c>
-      <c r="B99" s="1" t="s">
+      <c r="B100" s="1" t="s">
         <v>240</v>
       </c>
-      <c r="C99" s="1" t="s">
+      <c r="C100" s="1" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B100" s="1"/>
-      <c r="C100" s="1"/>
-    </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A101" t="s">
-        <v>257</v>
-      </c>
-      <c r="B101" s="1" t="s">
-        <v>258</v>
-      </c>
-      <c r="C101" s="1" t="s">
-        <v>259</v>
-      </c>
+      <c r="B101" s="1"/>
+      <c r="C101" s="1"/>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
-        <v>268</v>
+        <v>257</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>269</v>
+        <v>258</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>270</v>
+        <v>259</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
+        <v>271</v>
+      </c>
+      <c r="B104" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="C104" s="1" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A105" t="s">
         <v>274</v>
       </c>
-      <c r="B104" s="1" t="s">
+      <c r="B105" s="1" t="s">
         <v>275</v>
       </c>
-      <c r="C104" s="1" t="s">
+      <c r="C105" s="1" t="s">
         <v>276</v>
       </c>
     </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B105" s="1"/>
-      <c r="C105" s="1"/>
-    </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A106" t="s">
-        <v>260</v>
-      </c>
-      <c r="B106" s="1" t="s">
-        <v>261</v>
-      </c>
-      <c r="C106" s="1" t="s">
-        <v>262</v>
-      </c>
+      <c r="B106" s="1"/>
+      <c r="C106" s="1"/>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
+        <v>260</v>
+      </c>
+      <c r="B107" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="C107" s="1" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A108" t="s">
         <v>265</v>
       </c>
-      <c r="B107" s="1" t="s">
+      <c r="B108" s="1" t="s">
         <v>266</v>
       </c>
-      <c r="C107" s="1" t="s">
+      <c r="C108" s="1" t="s">
         <v>267</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Retrieve User's type when performing Get
</commit_message>
<xml_diff>
--- a/Config.xlsx
+++ b/Config.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22624"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mateus.cruz\Documents\GitHub\OrchestratorManager\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85A05FB8-F551-4CC7-981A-6855DA3CFF76}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0473E236-96C6-45B8-84B5-0948A7422371}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>

</xml_diff>

<commit_message>
Use the same process naming convention as Orchestrator's web interface
</commit_message>
<xml_diff>
--- a/Config.xlsx
+++ b/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mateus.cruz\Documents\GitHub\OrchestratorManager\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0473E236-96C6-45B8-84B5-0948A7422371}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7EF5D41-18B7-438B-AC21-E8ADF703CDB3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2092,7 +2092,7 @@
         <v>264</v>
       </c>
       <c r="B39" t="s">
-        <v>53</v>
+        <v>30</v>
       </c>
       <c r="C39" s="1" t="s">
         <v>308</v>
@@ -2103,7 +2103,7 @@
         <v>263</v>
       </c>
       <c r="B40" t="s">
-        <v>222</v>
+        <v>53</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>305</v>

</xml_diff>

<commit_message>
Change localization strings based on review
</commit_message>
<xml_diff>
--- a/Config.xlsx
+++ b/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mateus.cruz\Documents\GitHub\OrchestratorManager\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30BF165F-116E-474B-8191-78B1D009AA22}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C130D8A-7387-453B-847A-843DCDC01A6D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="3" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="418" uniqueCount="391">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="418" uniqueCount="390">
   <si>
     <t>Name</t>
   </si>
@@ -148,9 +148,6 @@
     <t>Unable to get access token due to failed authentication.</t>
   </si>
   <si>
-    <t>API認証のためのトークンが取得できませんでした。</t>
-  </si>
-  <si>
     <t>ConfirmNumerousRequests</t>
   </si>
   <si>
@@ -280,9 +277,6 @@
     <t>Asset not found.</t>
   </si>
   <si>
-    <t>処理が失敗しました。リクエストステータス：{0} / レスポンス：{1}。</t>
-  </si>
-  <si>
     <t>Failed to process entity. Request status: {0} / Response: {1}.</t>
   </si>
   <si>
@@ -295,9 +289,6 @@
     <t>Already processed.</t>
   </si>
   <si>
-    <t>処理済。</t>
-  </si>
-  <si>
     <t>NumerousRequestsNotConfirmed</t>
   </si>
   <si>
@@ -529,9 +520,6 @@
     <t>AddRemoveEnvironmentRobotsResultColumn</t>
   </si>
   <si>
-    <t>ロボットの追加・削除</t>
-  </si>
-  <si>
     <t>Robot already processed. Robot name: {0} / ID: {1}.</t>
   </si>
   <si>
@@ -601,9 +589,6 @@
     <t>パスワード</t>
   </si>
   <si>
-    <t>送信</t>
-  </si>
-  <si>
     <t>Environment</t>
   </si>
   <si>
@@ -685,9 +670,6 @@
     <t>RobotAddedAndRemoved</t>
   </si>
   <si>
-    <t>ロボットが同時に追加・削除されています。</t>
-  </si>
-  <si>
     <t>OrganizationUnitsPanelTemplatePath</t>
   </si>
   <si>
@@ -745,9 +727,6 @@
     <t>An Organization Unit is being added and removed at the same time.</t>
   </si>
   <si>
-    <t>組織単位が同時に追加・削除されています。</t>
-  </si>
-  <si>
     <t>A Robot is being added and removed at the same time.</t>
   </si>
   <si>
@@ -769,19 +748,10 @@
     <t>{0}というユーザー名が見つかりませんでした。</t>
   </si>
   <si>
-    <t>組織単位の追加・削除</t>
-  </si>
-  <si>
-    <t>ロールの追加・削除</t>
-  </si>
-  <si>
     <t>RoleAddedAndRemoved</t>
   </si>
   <si>
     <t>A Role is being added and removed at the same time.</t>
-  </si>
-  <si>
-    <t>ロールが同時に追加・削除されています。</t>
   </si>
   <si>
     <t>ProcessNameNotSpecified</t>
@@ -1008,12 +978,6 @@
   </si>
   <si>
     <t>Edit Credential</t>
-  </si>
-  <si>
-    <t>Credential型の作成</t>
-  </si>
-  <si>
-    <t>Credential型の編集</t>
   </si>
   <si>
     <t>CreateCredentialAssetResultColumn</t>
@@ -1188,31 +1152,64 @@
     <t>認証トークンの期限が切れました。</t>
   </si>
   <si>
-    <t>ご注意ください - ログイン試行に複数回失敗した場合、テナントの設定により指定された秒数の間、アカウントがロックされることがあります。</t>
-  </si>
-  <si>
     <t>指定されたエンティティはサポートされていません。</t>
   </si>
   <si>
-    <t>指定された操作はサポートされていません。</t>
-  </si>
-  <si>
     <t>指定されたHTTPメソッドはサポートされていません。</t>
   </si>
   <si>
-    <t>この操作により、多数のHTTPリクエストが送信されます。これにより、対象となるOrchestratorのインフラに負荷を与える可能性があります。実行しますか？</t>
-  </si>
-  <si>
     <t>多数のAPIリクエストを伴う操作を、ユーザーが承認しませんでした。</t>
   </si>
   <si>
     <t>多数のAPIリクエストを伴う操作を、ユーザーが承認しました。</t>
   </si>
   <si>
-    <t>指定されたアセットタイプはサポートされていません。</t>
-  </si>
-  <si>
-    <t>指定されたステータスはサポートされていません。</t>
+    <t>ご注意ください: ログイン試行に複数回失敗した場合、テナントのセキュリティ設定で指定した秒数の間、アカウントがロックされることがあります。</t>
+  </si>
+  <si>
+    <t>Credential 型を作成</t>
+  </si>
+  <si>
+    <t>Credential 型を編集</t>
+  </si>
+  <si>
+    <t>ロボットを追加または削除</t>
+  </si>
+  <si>
+    <t>組織単位を追加または削除</t>
+  </si>
+  <si>
+    <t>ロールを追加または削除</t>
+  </si>
+  <si>
+    <t>操作はサポートされていません。</t>
+  </si>
+  <si>
+    <t>認証に失敗したため、アクセス トークンを取得できません。</t>
+  </si>
+  <si>
+    <t>選択した操作により、多数の HTTP リクエストが送信されます。これにより、対象となる Orchestrator のインフラストラクチャに負荷を与える可能性があります。処理を続行しますか?</t>
+  </si>
+  <si>
+    <t>エンティティの処理に失敗しました。リクエストの状態: {0} / レスポンス: {1}。</t>
+  </si>
+  <si>
+    <t>既に処理されています。</t>
+  </si>
+  <si>
+    <t>指定されたアセット型はサポートされていません。</t>
+  </si>
+  <si>
+    <t>ステータスはサポートされていません。</t>
+  </si>
+  <si>
+    <t>組織単位が同時に追加および削除されています。</t>
+  </si>
+  <si>
+    <t>ロールが同時に追加および削除されています。</t>
+  </si>
+  <si>
+    <t>ロボットが同時に追加および削除されています。</t>
   </si>
 </sst>
 </file>
@@ -1595,7 +1592,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D89C9C48-5454-47C4-AB1D-448E4519251A}">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -1619,30 +1616,30 @@
     </row>
     <row r="2" spans="1:3" ht="58" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="1" t="s">
-        <v>372</v>
+        <v>360</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>373</v>
+        <v>361</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>368</v>
+        <v>356</v>
       </c>
       <c r="B4" t="s">
-        <v>378</v>
+        <v>366</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>374</v>
+        <v>362</v>
       </c>
     </row>
   </sheetData>
@@ -1688,7 +1685,7 @@
         <v>200</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>275</v>
+        <v>265</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="29" x14ac:dyDescent="0.35">
@@ -1699,117 +1696,117 @@
         <v>0</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>274</v>
+        <v>264</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="B4">
         <v>500</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>270</v>
+        <v>260</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>223</v>
+        <v>217</v>
       </c>
       <c r="B5">
         <v>600</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>271</v>
+        <v>261</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>335</v>
+        <v>323</v>
       </c>
       <c r="B6">
         <v>3</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>337</v>
+        <v>325</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>336</v>
+        <v>324</v>
       </c>
       <c r="B7">
         <v>5000</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>341</v>
+        <v>329</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="B8" t="s">
-        <v>342</v>
+        <v>330</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>273</v>
+        <v>263</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="B9" t="s">
-        <v>343</v>
+        <v>331</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>272</v>
+        <v>262</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="B10" t="s">
-        <v>344</v>
+        <v>332</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>277</v>
+        <v>267</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="B11" t="s">
-        <v>345</v>
+        <v>333</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>276</v>
+        <v>266</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="B12" t="s">
-        <v>346</v>
+        <v>334</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>278</v>
+        <v>268</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="B13" t="s">
-        <v>347</v>
+        <v>335</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>279</v>
+        <v>269</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="29" x14ac:dyDescent="0.35">
@@ -1820,7 +1817,7 @@
         <v>28</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>280</v>
+        <v>270</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="29" x14ac:dyDescent="0.35">
@@ -1831,293 +1828,293 @@
         <v>33</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>282</v>
+        <v>272</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B16" t="s">
         <v>34</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>287</v>
+        <v>277</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B17" t="s">
         <v>33</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>286</v>
+        <v>276</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B18" t="s">
         <v>28</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>288</v>
+        <v>278</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
+        <v>46</v>
+      </c>
+      <c r="B19" t="s">
         <v>47</v>
       </c>
-      <c r="B19" t="s">
-        <v>48</v>
-      </c>
       <c r="C19" s="1" t="s">
-        <v>283</v>
+        <v>273</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>330</v>
+        <v>318</v>
       </c>
       <c r="B20" t="s">
         <v>28</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>288</v>
+        <v>278</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>326</v>
+        <v>314</v>
       </c>
       <c r="B21" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>327</v>
+        <v>315</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B22" t="s">
         <v>28</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>284</v>
+        <v>274</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>328</v>
+        <v>316</v>
       </c>
       <c r="B23" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>329</v>
+        <v>317</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B24" t="s">
         <v>28</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>281</v>
+        <v>271</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B25" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>294</v>
+        <v>284</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
+        <v>52</v>
+      </c>
+      <c r="B26" t="s">
         <v>53</v>
       </c>
-      <c r="B26" t="s">
-        <v>54</v>
-      </c>
       <c r="C26" s="1" t="s">
-        <v>285</v>
+        <v>275</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B27" t="s">
         <v>33</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>289</v>
+        <v>279</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B28" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>290</v>
+        <v>280</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B29" t="s">
         <v>28</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>291</v>
+        <v>281</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B30" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>306</v>
+        <v>296</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B31" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>292</v>
+        <v>282</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="B32" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>293</v>
+        <v>283</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="B33" t="s">
         <v>33</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>299</v>
+        <v>289</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="B34" t="s">
         <v>34</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>295</v>
+        <v>285</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="B35" t="s">
         <v>28</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>296</v>
+        <v>286</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="B36" t="s">
         <v>28</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>303</v>
+        <v>293</v>
       </c>
     </row>
     <row r="37" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>301</v>
+        <v>291</v>
       </c>
       <c r="B37" t="s">
         <v>34</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>302</v>
+        <v>292</v>
       </c>
     </row>
     <row r="38" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>304</v>
+        <v>294</v>
       </c>
       <c r="B38" t="s">
         <v>34</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>305</v>
+        <v>295</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>256</v>
+        <v>246</v>
       </c>
       <c r="B39" t="s">
         <v>28</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>300</v>
+        <v>290</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>255</v>
+        <v>245</v>
       </c>
       <c r="B40" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>297</v>
+        <v>287</v>
       </c>
     </row>
     <row r="41" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
-        <v>269</v>
+        <v>259</v>
       </c>
       <c r="B41" t="s">
         <v>28</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>298</v>
+        <v>288</v>
       </c>
     </row>
   </sheetData>
@@ -2133,8 +2130,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1927ABA9-1814-4487-9CEC-ABDCAF91481F}">
   <dimension ref="A1:C108"/>
   <sheetViews>
-    <sheetView topLeftCell="A54" workbookViewId="0">
-      <selection activeCell="C64" sqref="C64"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2157,51 +2154,51 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>307</v>
+        <v>297</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>382</v>
+        <v>374</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
+        <v>176</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>184</v>
-      </c>
       <c r="C4" s="1" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>13</v>
@@ -2212,7 +2209,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>12</v>
@@ -2223,101 +2220,101 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>332</v>
+        <v>320</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>349</v>
+        <v>337</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>331</v>
+        <v>319</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="B11" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>191</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>196</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>219</v>
+        <v>213</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>220</v>
+        <v>214</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>348</v>
+        <v>336</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>188</v>
+        <v>336</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.35">
@@ -2326,68 +2323,68 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>362</v>
+        <v>350</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>350</v>
+        <v>338</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>356</v>
+        <v>344</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>363</v>
+        <v>351</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>351</v>
+        <v>339</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>357</v>
+        <v>345</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>364</v>
+        <v>352</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>352</v>
+        <v>340</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>358</v>
+        <v>346</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>365</v>
+        <v>353</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>353</v>
+        <v>341</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>359</v>
+        <v>347</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>366</v>
+        <v>354</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>354</v>
+        <v>342</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>360</v>
+        <v>348</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>367</v>
+        <v>355</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>355</v>
+        <v>343</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>361</v>
+        <v>349</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.35">
@@ -2440,79 +2437,79 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>320</v>
+        <v>310</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>322</v>
+        <v>312</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>324</v>
+        <v>375</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>321</v>
+        <v>311</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>323</v>
+        <v>313</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>325</v>
+        <v>376</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>310</v>
+        <v>300</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>375</v>
+        <v>363</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>164</v>
+        <v>377</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>308</v>
+        <v>298</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>376</v>
+        <v>364</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>244</v>
+        <v>378</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>309</v>
+        <v>299</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>377</v>
+        <v>365</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>245</v>
+        <v>379</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>369</v>
+        <v>357</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>370</v>
+        <v>358</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>371</v>
+        <v>359</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.35">
@@ -2523,7 +2520,7 @@
         <v>21</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>383</v>
+        <v>370</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.35">
@@ -2534,7 +2531,7 @@
         <v>26</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>384</v>
+        <v>380</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.35">
@@ -2556,139 +2553,139 @@
         <v>36</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>37</v>
+        <v>381</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>379</v>
+        <v>367</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>380</v>
+        <v>368</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>381</v>
+        <v>369</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
-        <v>333</v>
+        <v>321</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>334</v>
+        <v>322</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>385</v>
+        <v>371</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
-        <v>338</v>
+        <v>326</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>339</v>
+        <v>327</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>340</v>
+        <v>328</v>
       </c>
     </row>
     <row r="43" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
+        <v>37</v>
+      </c>
+      <c r="B43" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B43" s="1" t="s">
-        <v>39</v>
-      </c>
       <c r="C43" s="1" t="s">
-        <v>386</v>
+        <v>382</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>387</v>
+        <v>372</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
+        <v>39</v>
+      </c>
+      <c r="B45" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B45" s="1" t="s">
-        <v>41</v>
-      </c>
       <c r="C45" s="1" t="s">
-        <v>388</v>
+        <v>373</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>81</v>
+        <v>383</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>86</v>
+        <v>384</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
+        <v>104</v>
+      </c>
+      <c r="B48" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="B48" s="1" t="s">
+      <c r="C48" s="1" t="s">
         <v>110</v>
-      </c>
-      <c r="C48" s="1" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
+        <v>105</v>
+      </c>
+      <c r="B49" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="B49" s="1" t="s">
+      <c r="C49" s="1" t="s">
         <v>111</v>
-      </c>
-      <c r="C49" s="1" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
+        <v>106</v>
+      </c>
+      <c r="B50" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="B50" s="1" t="s">
+      <c r="C50" s="1" t="s">
         <v>112</v>
-      </c>
-      <c r="C50" s="1" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
+        <v>77</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C51" s="1" t="s">
         <v>78</v>
-      </c>
-      <c r="B51" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="C51" s="1" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.35">
@@ -2697,90 +2694,90 @@
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
+        <v>44</v>
+      </c>
+      <c r="B53" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B53" s="1" t="s">
-        <v>46</v>
-      </c>
       <c r="C53" s="1" t="s">
-        <v>389</v>
+        <v>385</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
-        <v>311</v>
+        <v>301</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>313</v>
+        <v>303</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>312</v>
+        <v>302</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
-        <v>316</v>
+        <v>306</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>315</v>
+        <v>305</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>314</v>
+        <v>304</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
-        <v>317</v>
+        <v>307</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>318</v>
+        <v>308</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>319</v>
+        <v>309</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.35">
@@ -2789,101 +2786,101 @@
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>390</v>
+        <v>386</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>235</v>
+        <v>229</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>236</v>
+        <v>387</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
-        <v>246</v>
+        <v>237</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>247</v>
+        <v>238</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>248</v>
+        <v>388</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>242</v>
+        <v>235</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>243</v>
+        <v>236</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.35">
@@ -2892,90 +2889,90 @@
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
+        <v>56</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="C72" s="1" t="s">
         <v>57</v>
-      </c>
-      <c r="B72" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="C72" s="1" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.35">
@@ -2984,189 +2981,189 @@
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
+        <v>41</v>
+      </c>
+      <c r="B82" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B82" s="1" t="s">
+      <c r="C82" s="1" t="s">
         <v>43</v>
-      </c>
-      <c r="C82" s="1" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>239</v>
+        <v>232</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>240</v>
+        <v>233</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B86" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C86" s="1" t="s">
         <v>71</v>
-      </c>
-      <c r="C86" s="1" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>230</v>
+        <v>224</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="B93" t="s">
-        <v>224</v>
+        <v>218</v>
       </c>
       <c r="C93" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="B94" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="C94" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="C95" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="B96" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="C96" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>237</v>
+        <v>230</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>216</v>
+        <v>389</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
-        <v>225</v>
+        <v>219</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>226</v>
+        <v>220</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>227</v>
+        <v>221</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>232</v>
+        <v>226</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.35">
@@ -3175,46 +3172,46 @@
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
-        <v>249</v>
+        <v>239</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>250</v>
+        <v>240</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>251</v>
+        <v>241</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
-        <v>260</v>
+        <v>250</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>261</v>
+        <v>251</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>262</v>
+        <v>252</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
-        <v>263</v>
+        <v>253</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>264</v>
+        <v>254</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>265</v>
+        <v>255</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
-        <v>266</v>
+        <v>256</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>267</v>
+        <v>257</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>268</v>
+        <v>258</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.35">
@@ -3223,24 +3220,24 @@
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
-        <v>252</v>
+        <v>242</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>253</v>
+        <v>243</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>254</v>
+        <v>244</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
-        <v>257</v>
+        <v>247</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>258</v>
+        <v>248</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>259</v>
+        <v>249</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Change default sheet when opening Config.xlsx
</commit_message>
<xml_diff>
--- a/Config.xlsx
+++ b/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mateus.cruz\Documents\GitHub\OrchestratorManager\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C130D8A-7387-453B-847A-843DCDC01A6D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EC2017E-B612-4D27-8F35-E3FAD7F88193}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="3" r:id="rId1"/>
@@ -1592,7 +1592,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D89C9C48-5454-47C4-AB1D-448E4519251A}">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -2130,7 +2130,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1927ABA9-1814-4487-9CEC-ABDCAF91481F}">
   <dimension ref="A1:C108"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Add retry in case of server error
</commit_message>
<xml_diff>
--- a/Config.xlsx
+++ b/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mateus.cruz\Documents\GitHub\OrchestratorManager\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EC2017E-B612-4D27-8F35-E3FAD7F88193}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0C35FBB-E6B6-4D24-8061-FE10CCA2798A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="3" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="418" uniqueCount="390">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="421" uniqueCount="393">
   <si>
     <t>Name</t>
   </si>
@@ -1210,6 +1210,15 @@
   </si>
   <si>
     <t>ロボットが同時に追加および削除されています。</t>
+  </si>
+  <si>
+    <t>ServerErrorFailure</t>
+  </si>
+  <si>
+    <t>HTTP Request failed due to server error issues.</t>
+  </si>
+  <si>
+    <t>サーバーエラーの問題のため、リクエストが失敗しました。</t>
   </si>
 </sst>
 </file>
@@ -1316,8 +1325,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{F8A6BD26-C645-4175-8476-817D5672FD54}" name="Table13" displayName="Table13" ref="A1:C108" totalsRowShown="0">
-  <autoFilter ref="A1:C108" xr:uid="{A7872B2C-8222-446D-9C51-8EA59078049C}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{F8A6BD26-C645-4175-8476-817D5672FD54}" name="Table13" displayName="Table13" ref="A1:C109" totalsRowShown="0">
+  <autoFilter ref="A1:C109" xr:uid="{A7872B2C-8222-446D-9C51-8EA59078049C}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{5D541690-4DCC-4D96-9FCC-B1699146EC35}" name="Name"/>
     <tableColumn id="2" xr3:uid="{86DF2464-58F6-48AD-98C9-2D16B29FBB6F}" name="EN" dataDxfId="1"/>
@@ -1592,7 +1601,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D89C9C48-5454-47C4-AB1D-448E4519251A}">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -2128,9 +2137,9 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1927ABA9-1814-4487-9CEC-ABDCAF91481F}">
-  <dimension ref="A1:C108"/>
+  <dimension ref="A1:C109"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -2589,654 +2598,665 @@
         <v>328</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
+        <v>390</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>391</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="A44" t="s">
         <v>37</v>
       </c>
-      <c r="B43" s="1" t="s">
+      <c r="B44" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C43" s="1" t="s">
+      <c r="C44" s="1" t="s">
         <v>382</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A44" t="s">
-        <v>84</v>
-      </c>
-      <c r="B44" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="C44" s="1" t="s">
-        <v>372</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
-        <v>39</v>
+        <v>84</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>40</v>
+        <v>85</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
-        <v>81</v>
+        <v>39</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>80</v>
+        <v>40</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>383</v>
+        <v>373</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
-        <v>104</v>
+        <v>82</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>107</v>
+        <v>83</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>110</v>
+        <v>384</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
+        <v>106</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A52" t="s">
         <v>77</v>
       </c>
-      <c r="B51" s="1" t="s">
+      <c r="B52" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="C51" s="1" t="s">
+      <c r="C52" s="1" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B52" s="1"/>
-      <c r="C52" s="1"/>
-    </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A53" t="s">
-        <v>44</v>
-      </c>
-      <c r="B53" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C53" s="1" t="s">
-        <v>385</v>
-      </c>
+      <c r="B53" s="1"/>
+      <c r="C53" s="1"/>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
-        <v>69</v>
+        <v>44</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>79</v>
+        <v>45</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>75</v>
+        <v>385</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
-        <v>86</v>
+        <v>69</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>88</v>
+        <v>75</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>103</v>
+        <v>93</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
-        <v>301</v>
+        <v>98</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>303</v>
+        <v>103</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>302</v>
+        <v>99</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
-        <v>306</v>
+        <v>301</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
+        <v>306</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>305</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A61" t="s">
         <v>307</v>
       </c>
-      <c r="B60" s="1" t="s">
+      <c r="B61" s="1" t="s">
         <v>308</v>
       </c>
-      <c r="C60" s="1" t="s">
+      <c r="C61" s="1" t="s">
         <v>309</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B61" s="1"/>
-      <c r="C61" s="1"/>
-    </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A62" t="s">
-        <v>115</v>
-      </c>
-      <c r="B62" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="C62" s="1" t="s">
-        <v>117</v>
-      </c>
+      <c r="B62" s="1"/>
+      <c r="C62" s="1"/>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>386</v>
+        <v>117</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>122</v>
+        <v>386</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
-        <v>165</v>
+        <v>123</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>166</v>
+        <v>124</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>167</v>
+        <v>125</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
-        <v>228</v>
+        <v>168</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>229</v>
+        <v>169</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>387</v>
+        <v>170</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
-        <v>237</v>
+        <v>228</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>238</v>
+        <v>229</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
+        <v>237</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="C70" s="1" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A71" t="s">
         <v>234</v>
       </c>
-      <c r="B70" s="1" t="s">
+      <c r="B71" s="1" t="s">
         <v>235</v>
       </c>
-      <c r="C70" s="1" t="s">
+      <c r="C71" s="1" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B71" s="1"/>
-      <c r="C71" s="1"/>
-    </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A72" t="s">
-        <v>56</v>
-      </c>
-      <c r="B72" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="C72" s="1" t="s">
-        <v>57</v>
-      </c>
+      <c r="B72" s="1"/>
+      <c r="C72" s="1"/>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>114</v>
+        <v>161</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>72</v>
+        <v>57</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
-        <v>126</v>
+        <v>61</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>127</v>
+        <v>114</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>128</v>
+        <v>72</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
+        <v>144</v>
+      </c>
+      <c r="B79" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="C79" s="1" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A80" t="s">
         <v>162</v>
       </c>
-      <c r="B79" s="1" t="s">
+      <c r="B80" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="C79" s="1" t="s">
+      <c r="C80" s="1" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B80" s="1"/>
-      <c r="C80" s="1"/>
-    </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A81" t="s">
-        <v>60</v>
-      </c>
-      <c r="B81" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="C81" s="1" t="s">
-        <v>73</v>
-      </c>
+      <c r="B81" s="1"/>
+      <c r="C81" s="1"/>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
-        <v>41</v>
+        <v>60</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>42</v>
+        <v>113</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>43</v>
+        <v>73</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
-        <v>132</v>
+        <v>41</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>133</v>
+        <v>42</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>134</v>
+        <v>43</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
+        <v>132</v>
+      </c>
+      <c r="B84" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="C84" s="1" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A85" t="s">
         <v>231</v>
       </c>
-      <c r="B84" s="1" t="s">
+      <c r="B85" s="1" t="s">
         <v>232</v>
       </c>
-      <c r="C84" s="1" t="s">
+      <c r="C85" s="1" t="s">
         <v>233</v>
-      </c>
-    </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A86" t="s">
-        <v>62</v>
-      </c>
-      <c r="B86" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="C86" s="1" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
-        <v>89</v>
+        <v>62</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>90</v>
+        <v>70</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>91</v>
+        <v>71</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
+        <v>100</v>
+      </c>
+      <c r="B90" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C90" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A91" t="s">
         <v>222</v>
       </c>
-      <c r="B90" s="1" t="s">
+      <c r="B91" s="1" t="s">
         <v>223</v>
       </c>
-      <c r="C90" s="1" t="s">
+      <c r="C91" s="1" t="s">
         <v>224</v>
-      </c>
-    </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A92" t="s">
-        <v>66</v>
-      </c>
-      <c r="B92" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="C92" s="1" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
-        <v>139</v>
-      </c>
-      <c r="B93" t="s">
-        <v>218</v>
-      </c>
-      <c r="C93" t="s">
-        <v>140</v>
+        <v>66</v>
+      </c>
+      <c r="B93" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="C93" s="1" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
-        <v>150</v>
+        <v>139</v>
       </c>
       <c r="B94" t="s">
-        <v>151</v>
+        <v>218</v>
       </c>
       <c r="C94" t="s">
-        <v>152</v>
+        <v>140</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
-        <v>153</v>
-      </c>
-      <c r="B95" s="1" t="s">
-        <v>154</v>
+        <v>150</v>
+      </c>
+      <c r="B95" t="s">
+        <v>151</v>
       </c>
       <c r="C95" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
-        <v>157</v>
-      </c>
-      <c r="B96" t="s">
-        <v>158</v>
+        <v>153</v>
+      </c>
+      <c r="B96" s="1" t="s">
+        <v>154</v>
       </c>
       <c r="C96" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
+        <v>157</v>
+      </c>
+      <c r="B97" t="s">
+        <v>158</v>
+      </c>
+      <c r="C97" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A98" t="s">
         <v>210</v>
       </c>
-      <c r="B97" s="1" t="s">
+      <c r="B98" s="1" t="s">
         <v>230</v>
       </c>
-      <c r="C97" s="1" t="s">
+      <c r="C98" s="1" t="s">
         <v>389</v>
-      </c>
-    </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A99" t="s">
-        <v>219</v>
-      </c>
-      <c r="B99" s="1" t="s">
-        <v>220</v>
-      </c>
-      <c r="C99" s="1" t="s">
-        <v>221</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
+        <v>219</v>
+      </c>
+      <c r="B100" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="C100" s="1" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A101" t="s">
         <v>225</v>
       </c>
-      <c r="B100" s="1" t="s">
+      <c r="B101" s="1" t="s">
         <v>226</v>
       </c>
-      <c r="C100" s="1" t="s">
+      <c r="C101" s="1" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B101" s="1"/>
-      <c r="C101" s="1"/>
-    </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A102" t="s">
-        <v>239</v>
-      </c>
-      <c r="B102" s="1" t="s">
-        <v>240</v>
-      </c>
-      <c r="C102" s="1" t="s">
-        <v>241</v>
-      </c>
+      <c r="B102" s="1"/>
+      <c r="C102" s="1"/>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
-        <v>250</v>
+        <v>239</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>251</v>
+        <v>240</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>252</v>
+        <v>241</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
+        <v>253</v>
+      </c>
+      <c r="B105" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="C105" s="1" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A106" t="s">
         <v>256</v>
       </c>
-      <c r="B105" s="1" t="s">
+      <c r="B106" s="1" t="s">
         <v>257</v>
       </c>
-      <c r="C105" s="1" t="s">
+      <c r="C106" s="1" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B106" s="1"/>
-      <c r="C106" s="1"/>
-    </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A107" t="s">
-        <v>242</v>
-      </c>
-      <c r="B107" s="1" t="s">
-        <v>243</v>
-      </c>
-      <c r="C107" s="1" t="s">
-        <v>244</v>
-      </c>
+      <c r="B107" s="1"/>
+      <c r="C107" s="1"/>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
+        <v>242</v>
+      </c>
+      <c r="B108" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="C108" s="1" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A109" t="s">
         <v>247</v>
       </c>
-      <c r="B108" s="1" t="s">
+      <c r="B109" s="1" t="s">
         <v>248</v>
       </c>
-      <c r="C108" s="1" t="s">
+      <c r="C109" s="1" t="s">
         <v>249</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Revert "Add retry in case of server error"
This reverts commit 9df6daee840ee19fdfd9baba6db8764076d41769.
</commit_message>
<xml_diff>
--- a/Config.xlsx
+++ b/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mateus.cruz\Documents\GitHub\OrchestratorManager\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0C35FBB-E6B6-4D24-8061-FE10CCA2798A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EC2017E-B612-4D27-8F35-E3FAD7F88193}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="3" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="421" uniqueCount="393">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="418" uniqueCount="390">
   <si>
     <t>Name</t>
   </si>
@@ -1210,15 +1210,6 @@
   </si>
   <si>
     <t>ロボットが同時に追加および削除されています。</t>
-  </si>
-  <si>
-    <t>ServerErrorFailure</t>
-  </si>
-  <si>
-    <t>HTTP Request failed due to server error issues.</t>
-  </si>
-  <si>
-    <t>サーバーエラーの問題のため、リクエストが失敗しました。</t>
   </si>
 </sst>
 </file>
@@ -1325,8 +1316,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{F8A6BD26-C645-4175-8476-817D5672FD54}" name="Table13" displayName="Table13" ref="A1:C109" totalsRowShown="0">
-  <autoFilter ref="A1:C109" xr:uid="{A7872B2C-8222-446D-9C51-8EA59078049C}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{F8A6BD26-C645-4175-8476-817D5672FD54}" name="Table13" displayName="Table13" ref="A1:C108" totalsRowShown="0">
+  <autoFilter ref="A1:C108" xr:uid="{A7872B2C-8222-446D-9C51-8EA59078049C}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{5D541690-4DCC-4D96-9FCC-B1699146EC35}" name="Name"/>
     <tableColumn id="2" xr3:uid="{86DF2464-58F6-48AD-98C9-2D16B29FBB6F}" name="EN" dataDxfId="1"/>
@@ -1601,7 +1592,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D89C9C48-5454-47C4-AB1D-448E4519251A}">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -2137,9 +2128,9 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1927ABA9-1814-4487-9CEC-ABDCAF91481F}">
-  <dimension ref="A1:C109"/>
+  <dimension ref="A1:C108"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -2598,665 +2589,654 @@
         <v>328</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
-        <v>390</v>
+        <v>37</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>391</v>
+        <v>38</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>392</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
-        <v>37</v>
+        <v>84</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>38</v>
+        <v>85</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>382</v>
+        <v>372</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
-        <v>84</v>
+        <v>39</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>85</v>
+        <v>40</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
-        <v>39</v>
+        <v>81</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>40</v>
+        <v>80</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>373</v>
+        <v>383</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
-        <v>82</v>
+        <v>104</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>83</v>
+        <v>107</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>384</v>
+        <v>110</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
-        <v>106</v>
+        <v>77</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>109</v>
+        <v>76</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>112</v>
+        <v>78</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A52" t="s">
-        <v>77</v>
-      </c>
-      <c r="B52" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="C52" s="1" t="s">
-        <v>78</v>
-      </c>
+      <c r="B52" s="1"/>
+      <c r="C52" s="1"/>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B53" s="1"/>
-      <c r="C53" s="1"/>
+      <c r="A53" t="s">
+        <v>44</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>385</v>
+      </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
-        <v>44</v>
+        <v>69</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>45</v>
+        <v>79</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>385</v>
+        <v>75</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
-        <v>69</v>
+        <v>86</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>79</v>
+        <v>87</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>75</v>
+        <v>88</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>88</v>
+        <v>94</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>93</v>
+        <v>103</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>94</v>
+        <v>99</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
-        <v>98</v>
+        <v>301</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>103</v>
+        <v>303</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>99</v>
+        <v>302</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
-        <v>301</v>
+        <v>306</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>303</v>
+        <v>305</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>305</v>
+        <v>308</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>304</v>
+        <v>309</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A61" t="s">
-        <v>307</v>
-      </c>
-      <c r="B61" s="1" t="s">
-        <v>308</v>
-      </c>
-      <c r="C61" s="1" t="s">
-        <v>309</v>
-      </c>
+      <c r="B61" s="1"/>
+      <c r="C61" s="1"/>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B62" s="1"/>
-      <c r="C62" s="1"/>
+      <c r="A62" t="s">
+        <v>115</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>117</v>
+      </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>117</v>
+        <v>386</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>386</v>
+        <v>122</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
-        <v>123</v>
+        <v>165</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>124</v>
+        <v>166</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>125</v>
+        <v>167</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
-        <v>168</v>
+        <v>228</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>169</v>
+        <v>229</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>170</v>
+        <v>387</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
-        <v>228</v>
+        <v>237</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>229</v>
+        <v>238</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>388</v>
+        <v>236</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A71" t="s">
-        <v>234</v>
-      </c>
-      <c r="B71" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="C71" s="1" t="s">
-        <v>236</v>
-      </c>
+      <c r="B71" s="1"/>
+      <c r="C71" s="1"/>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B72" s="1"/>
-      <c r="C72" s="1"/>
+      <c r="A72" t="s">
+        <v>56</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="C72" s="1" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>161</v>
+        <v>114</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>57</v>
+        <v>72</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
-        <v>61</v>
+        <v>126</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>114</v>
+        <v>127</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>72</v>
+        <v>128</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
-        <v>129</v>
+        <v>135</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>130</v>
+        <v>136</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>131</v>
+        <v>137</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
-        <v>135</v>
+        <v>141</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>136</v>
+        <v>142</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>137</v>
+        <v>143</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
-        <v>144</v>
+        <v>162</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>145</v>
+        <v>163</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>146</v>
+        <v>164</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A80" t="s">
-        <v>162</v>
-      </c>
-      <c r="B80" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="C80" s="1" t="s">
-        <v>164</v>
-      </c>
+      <c r="B80" s="1"/>
+      <c r="C80" s="1"/>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B81" s="1"/>
-      <c r="C81" s="1"/>
+      <c r="A81" t="s">
+        <v>60</v>
+      </c>
+      <c r="B81" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="C81" s="1" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
-        <v>60</v>
+        <v>41</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>113</v>
+        <v>42</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>73</v>
+        <v>43</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
-        <v>41</v>
+        <v>132</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>42</v>
+        <v>133</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>43</v>
+        <v>134</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
-        <v>132</v>
+        <v>231</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>133</v>
+        <v>232</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A85" t="s">
-        <v>231</v>
-      </c>
-      <c r="B85" s="1" t="s">
-        <v>232</v>
-      </c>
-      <c r="C85" s="1" t="s">
         <v>233</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A86" t="s">
+        <v>62</v>
+      </c>
+      <c r="B86" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C86" s="1" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
-        <v>62</v>
+        <v>89</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>70</v>
+        <v>90</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>71</v>
+        <v>91</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
-        <v>89</v>
+        <v>95</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>90</v>
+        <v>96</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>91</v>
+        <v>97</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
-        <v>95</v>
+        <v>100</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>96</v>
+        <v>102</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
-        <v>100</v>
+        <v>222</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>102</v>
+        <v>223</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A91" t="s">
-        <v>222</v>
-      </c>
-      <c r="B91" s="1" t="s">
-        <v>223</v>
-      </c>
-      <c r="C91" s="1" t="s">
         <v>224</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A92" t="s">
+        <v>66</v>
+      </c>
+      <c r="B92" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="C92" s="1" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
-        <v>66</v>
-      </c>
-      <c r="B93" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="C93" s="1" t="s">
-        <v>74</v>
+        <v>139</v>
+      </c>
+      <c r="B93" t="s">
+        <v>218</v>
+      </c>
+      <c r="C93" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
-        <v>139</v>
+        <v>150</v>
       </c>
       <c r="B94" t="s">
-        <v>218</v>
+        <v>151</v>
       </c>
       <c r="C94" t="s">
-        <v>140</v>
+        <v>152</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
-        <v>150</v>
-      </c>
-      <c r="B95" t="s">
-        <v>151</v>
+        <v>153</v>
+      </c>
+      <c r="B95" s="1" t="s">
+        <v>154</v>
       </c>
       <c r="C95" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
-        <v>153</v>
-      </c>
-      <c r="B96" s="1" t="s">
-        <v>154</v>
+        <v>157</v>
+      </c>
+      <c r="B96" t="s">
+        <v>158</v>
       </c>
       <c r="C96" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
-        <v>157</v>
-      </c>
-      <c r="B97" t="s">
-        <v>158</v>
-      </c>
-      <c r="C97" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A98" t="s">
         <v>210</v>
       </c>
-      <c r="B98" s="1" t="s">
+      <c r="B97" s="1" t="s">
         <v>230</v>
       </c>
-      <c r="C98" s="1" t="s">
+      <c r="C97" s="1" t="s">
         <v>389</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A99" t="s">
+        <v>219</v>
+      </c>
+      <c r="B99" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="C99" s="1" t="s">
+        <v>221</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
-        <v>219</v>
+        <v>225</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>220</v>
+        <v>226</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>221</v>
+        <v>227</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A101" t="s">
-        <v>225</v>
-      </c>
-      <c r="B101" s="1" t="s">
-        <v>226</v>
-      </c>
-      <c r="C101" s="1" t="s">
-        <v>227</v>
-      </c>
+      <c r="B101" s="1"/>
+      <c r="C101" s="1"/>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B102" s="1"/>
-      <c r="C102" s="1"/>
+      <c r="A102" t="s">
+        <v>239</v>
+      </c>
+      <c r="B102" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="C102" s="1" t="s">
+        <v>241</v>
+      </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
-        <v>239</v>
+        <v>250</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>240</v>
+        <v>251</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>241</v>
+        <v>252</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
-        <v>250</v>
+        <v>253</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>251</v>
+        <v>254</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>252</v>
+        <v>255</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
-        <v>253</v>
+        <v>256</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>254</v>
+        <v>257</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>255</v>
+        <v>258</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A106" t="s">
-        <v>256</v>
-      </c>
-      <c r="B106" s="1" t="s">
-        <v>257</v>
-      </c>
-      <c r="C106" s="1" t="s">
-        <v>258</v>
-      </c>
+      <c r="B106" s="1"/>
+      <c r="C106" s="1"/>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B107" s="1"/>
-      <c r="C107" s="1"/>
+      <c r="A107" t="s">
+        <v>242</v>
+      </c>
+      <c r="B107" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="C107" s="1" t="s">
+        <v>244</v>
+      </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
-        <v>242</v>
+        <v>247</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>243</v>
+        <v>248</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A109" t="s">
-        <v>247</v>
-      </c>
-      <c r="B109" s="1" t="s">
-        <v>248</v>
-      </c>
-      <c r="C109" s="1" t="s">
         <v>249</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Revert "Revert "Add retry in case of server error""
This reverts commit bf45e0ad00fd70eb61158db26c0d062f0113c5c8.
</commit_message>
<xml_diff>
--- a/Config.xlsx
+++ b/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mateus.cruz\Documents\GitHub\OrchestratorManager\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EC2017E-B612-4D27-8F35-E3FAD7F88193}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0C35FBB-E6B6-4D24-8061-FE10CCA2798A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="3" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="418" uniqueCount="390">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="421" uniqueCount="393">
   <si>
     <t>Name</t>
   </si>
@@ -1210,6 +1210,15 @@
   </si>
   <si>
     <t>ロボットが同時に追加および削除されています。</t>
+  </si>
+  <si>
+    <t>ServerErrorFailure</t>
+  </si>
+  <si>
+    <t>HTTP Request failed due to server error issues.</t>
+  </si>
+  <si>
+    <t>サーバーエラーの問題のため、リクエストが失敗しました。</t>
   </si>
 </sst>
 </file>
@@ -1316,8 +1325,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{F8A6BD26-C645-4175-8476-817D5672FD54}" name="Table13" displayName="Table13" ref="A1:C108" totalsRowShown="0">
-  <autoFilter ref="A1:C108" xr:uid="{A7872B2C-8222-446D-9C51-8EA59078049C}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{F8A6BD26-C645-4175-8476-817D5672FD54}" name="Table13" displayName="Table13" ref="A1:C109" totalsRowShown="0">
+  <autoFilter ref="A1:C109" xr:uid="{A7872B2C-8222-446D-9C51-8EA59078049C}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{5D541690-4DCC-4D96-9FCC-B1699146EC35}" name="Name"/>
     <tableColumn id="2" xr3:uid="{86DF2464-58F6-48AD-98C9-2D16B29FBB6F}" name="EN" dataDxfId="1"/>
@@ -1592,7 +1601,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D89C9C48-5454-47C4-AB1D-448E4519251A}">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -2128,9 +2137,9 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1927ABA9-1814-4487-9CEC-ABDCAF91481F}">
-  <dimension ref="A1:C108"/>
+  <dimension ref="A1:C109"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -2589,654 +2598,665 @@
         <v>328</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
+        <v>390</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>391</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="A44" t="s">
         <v>37</v>
       </c>
-      <c r="B43" s="1" t="s">
+      <c r="B44" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C43" s="1" t="s">
+      <c r="C44" s="1" t="s">
         <v>382</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A44" t="s">
-        <v>84</v>
-      </c>
-      <c r="B44" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="C44" s="1" t="s">
-        <v>372</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
-        <v>39</v>
+        <v>84</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>40</v>
+        <v>85</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
-        <v>81</v>
+        <v>39</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>80</v>
+        <v>40</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>383</v>
+        <v>373</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
-        <v>104</v>
+        <v>82</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>107</v>
+        <v>83</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>110</v>
+        <v>384</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
+        <v>106</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A52" t="s">
         <v>77</v>
       </c>
-      <c r="B51" s="1" t="s">
+      <c r="B52" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="C51" s="1" t="s">
+      <c r="C52" s="1" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B52" s="1"/>
-      <c r="C52" s="1"/>
-    </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A53" t="s">
-        <v>44</v>
-      </c>
-      <c r="B53" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C53" s="1" t="s">
-        <v>385</v>
-      </c>
+      <c r="B53" s="1"/>
+      <c r="C53" s="1"/>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
-        <v>69</v>
+        <v>44</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>79</v>
+        <v>45</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>75</v>
+        <v>385</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
-        <v>86</v>
+        <v>69</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>88</v>
+        <v>75</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>103</v>
+        <v>93</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
-        <v>301</v>
+        <v>98</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>303</v>
+        <v>103</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>302</v>
+        <v>99</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
-        <v>306</v>
+        <v>301</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
+        <v>306</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>305</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A61" t="s">
         <v>307</v>
       </c>
-      <c r="B60" s="1" t="s">
+      <c r="B61" s="1" t="s">
         <v>308</v>
       </c>
-      <c r="C60" s="1" t="s">
+      <c r="C61" s="1" t="s">
         <v>309</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B61" s="1"/>
-      <c r="C61" s="1"/>
-    </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A62" t="s">
-        <v>115</v>
-      </c>
-      <c r="B62" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="C62" s="1" t="s">
-        <v>117</v>
-      </c>
+      <c r="B62" s="1"/>
+      <c r="C62" s="1"/>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>386</v>
+        <v>117</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>122</v>
+        <v>386</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
-        <v>165</v>
+        <v>123</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>166</v>
+        <v>124</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>167</v>
+        <v>125</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
-        <v>228</v>
+        <v>168</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>229</v>
+        <v>169</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>387</v>
+        <v>170</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
-        <v>237</v>
+        <v>228</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>238</v>
+        <v>229</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
+        <v>237</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="C70" s="1" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A71" t="s">
         <v>234</v>
       </c>
-      <c r="B70" s="1" t="s">
+      <c r="B71" s="1" t="s">
         <v>235</v>
       </c>
-      <c r="C70" s="1" t="s">
+      <c r="C71" s="1" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B71" s="1"/>
-      <c r="C71" s="1"/>
-    </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A72" t="s">
-        <v>56</v>
-      </c>
-      <c r="B72" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="C72" s="1" t="s">
-        <v>57</v>
-      </c>
+      <c r="B72" s="1"/>
+      <c r="C72" s="1"/>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>114</v>
+        <v>161</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>72</v>
+        <v>57</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
-        <v>126</v>
+        <v>61</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>127</v>
+        <v>114</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>128</v>
+        <v>72</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
+        <v>144</v>
+      </c>
+      <c r="B79" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="C79" s="1" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A80" t="s">
         <v>162</v>
       </c>
-      <c r="B79" s="1" t="s">
+      <c r="B80" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="C79" s="1" t="s">
+      <c r="C80" s="1" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B80" s="1"/>
-      <c r="C80" s="1"/>
-    </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A81" t="s">
-        <v>60</v>
-      </c>
-      <c r="B81" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="C81" s="1" t="s">
-        <v>73</v>
-      </c>
+      <c r="B81" s="1"/>
+      <c r="C81" s="1"/>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
-        <v>41</v>
+        <v>60</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>42</v>
+        <v>113</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>43</v>
+        <v>73</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
-        <v>132</v>
+        <v>41</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>133</v>
+        <v>42</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>134</v>
+        <v>43</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
+        <v>132</v>
+      </c>
+      <c r="B84" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="C84" s="1" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A85" t="s">
         <v>231</v>
       </c>
-      <c r="B84" s="1" t="s">
+      <c r="B85" s="1" t="s">
         <v>232</v>
       </c>
-      <c r="C84" s="1" t="s">
+      <c r="C85" s="1" t="s">
         <v>233</v>
-      </c>
-    </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A86" t="s">
-        <v>62</v>
-      </c>
-      <c r="B86" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="C86" s="1" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
-        <v>89</v>
+        <v>62</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>90</v>
+        <v>70</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>91</v>
+        <v>71</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
+        <v>100</v>
+      </c>
+      <c r="B90" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C90" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A91" t="s">
         <v>222</v>
       </c>
-      <c r="B90" s="1" t="s">
+      <c r="B91" s="1" t="s">
         <v>223</v>
       </c>
-      <c r="C90" s="1" t="s">
+      <c r="C91" s="1" t="s">
         <v>224</v>
-      </c>
-    </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A92" t="s">
-        <v>66</v>
-      </c>
-      <c r="B92" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="C92" s="1" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
-        <v>139</v>
-      </c>
-      <c r="B93" t="s">
-        <v>218</v>
-      </c>
-      <c r="C93" t="s">
-        <v>140</v>
+        <v>66</v>
+      </c>
+      <c r="B93" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="C93" s="1" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
-        <v>150</v>
+        <v>139</v>
       </c>
       <c r="B94" t="s">
-        <v>151</v>
+        <v>218</v>
       </c>
       <c r="C94" t="s">
-        <v>152</v>
+        <v>140</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
-        <v>153</v>
-      </c>
-      <c r="B95" s="1" t="s">
-        <v>154</v>
+        <v>150</v>
+      </c>
+      <c r="B95" t="s">
+        <v>151</v>
       </c>
       <c r="C95" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
-        <v>157</v>
-      </c>
-      <c r="B96" t="s">
-        <v>158</v>
+        <v>153</v>
+      </c>
+      <c r="B96" s="1" t="s">
+        <v>154</v>
       </c>
       <c r="C96" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
+        <v>157</v>
+      </c>
+      <c r="B97" t="s">
+        <v>158</v>
+      </c>
+      <c r="C97" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A98" t="s">
         <v>210</v>
       </c>
-      <c r="B97" s="1" t="s">
+      <c r="B98" s="1" t="s">
         <v>230</v>
       </c>
-      <c r="C97" s="1" t="s">
+      <c r="C98" s="1" t="s">
         <v>389</v>
-      </c>
-    </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A99" t="s">
-        <v>219</v>
-      </c>
-      <c r="B99" s="1" t="s">
-        <v>220</v>
-      </c>
-      <c r="C99" s="1" t="s">
-        <v>221</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
+        <v>219</v>
+      </c>
+      <c r="B100" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="C100" s="1" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A101" t="s">
         <v>225</v>
       </c>
-      <c r="B100" s="1" t="s">
+      <c r="B101" s="1" t="s">
         <v>226</v>
       </c>
-      <c r="C100" s="1" t="s">
+      <c r="C101" s="1" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B101" s="1"/>
-      <c r="C101" s="1"/>
-    </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A102" t="s">
-        <v>239</v>
-      </c>
-      <c r="B102" s="1" t="s">
-        <v>240</v>
-      </c>
-      <c r="C102" s="1" t="s">
-        <v>241</v>
-      </c>
+      <c r="B102" s="1"/>
+      <c r="C102" s="1"/>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
-        <v>250</v>
+        <v>239</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>251</v>
+        <v>240</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>252</v>
+        <v>241</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
+        <v>253</v>
+      </c>
+      <c r="B105" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="C105" s="1" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A106" t="s">
         <v>256</v>
       </c>
-      <c r="B105" s="1" t="s">
+      <c r="B106" s="1" t="s">
         <v>257</v>
       </c>
-      <c r="C105" s="1" t="s">
+      <c r="C106" s="1" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B106" s="1"/>
-      <c r="C106" s="1"/>
-    </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A107" t="s">
-        <v>242</v>
-      </c>
-      <c r="B107" s="1" t="s">
-        <v>243</v>
-      </c>
-      <c r="C107" s="1" t="s">
-        <v>244</v>
-      </c>
+      <c r="B107" s="1"/>
+      <c r="C107" s="1"/>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
+        <v>242</v>
+      </c>
+      <c r="B108" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="C108" s="1" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A109" t="s">
         <v>247</v>
       </c>
-      <c r="B108" s="1" t="s">
+      <c r="B109" s="1" t="s">
         <v>248</v>
       </c>
-      <c r="C108" s="1" t="s">
+      <c r="C109" s="1" t="s">
         <v>249</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Implement UpdateProcessToLatestPackageVersion and RollbackProcessToPreviousPackageVersion
</commit_message>
<xml_diff>
--- a/Config.xlsx
+++ b/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mateus.cruz\Documents\GitHub\OrchestratorManager\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0C35FBB-E6B6-4D24-8061-FE10CCA2798A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46F1C01E-9050-41B2-B073-BA65218451DE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="3" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="421" uniqueCount="393">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="436" uniqueCount="406">
   <si>
     <t>Name</t>
   </si>
@@ -1219,6 +1219,45 @@
   </si>
   <si>
     <t>サーバーエラーの問題のため、リクエストが失敗しました。</t>
+  </si>
+  <si>
+    <t>UpdateProcessToLatestPackageVersionOperationName</t>
+  </si>
+  <si>
+    <t>Rollback to Previous Package</t>
+  </si>
+  <si>
+    <t>Update to Latest Package</t>
+  </si>
+  <si>
+    <t>最新のパッケージ バージョンに更新</t>
+  </si>
+  <si>
+    <t>以前使用していたバージョンに戻す</t>
+  </si>
+  <si>
+    <t>NamedProcessNotFound</t>
+  </si>
+  <si>
+    <t>Process named {0} not found.</t>
+  </si>
+  <si>
+    <t>{0}というプロセスが見つかりませんでした。</t>
+  </si>
+  <si>
+    <t>RollbackProcessToPreviousPackageVersionOperationName</t>
+  </si>
+  <si>
+    <t>UpdateProcessToLatestPackageVersionResultColumn</t>
+  </si>
+  <si>
+    <t>Column to which the result of the Update Process to Latest Package Version operation should be written.</t>
+  </si>
+  <si>
+    <t>RollbackProcessToPreviousPackageVersionResultColumn</t>
+  </si>
+  <si>
+    <t>Column to which the result of the Rollback Process to Previous Package Version operation should be written.</t>
   </si>
 </sst>
 </file>
@@ -1313,8 +1352,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E8BA34AD-7169-40BC-A1CB-84FE2C4A09B4}" name="Table1" displayName="Table1" ref="A1:C41" totalsRowShown="0">
-  <autoFilter ref="A1:C41" xr:uid="{A7872B2C-8222-446D-9C51-8EA59078049C}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E8BA34AD-7169-40BC-A1CB-84FE2C4A09B4}" name="Table1" displayName="Table1" ref="A1:C43" totalsRowShown="0">
+  <autoFilter ref="A1:C43" xr:uid="{A7872B2C-8222-446D-9C51-8EA59078049C}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{E8DD1BD3-BDF1-4CD9-9C4F-5DF2DD0162DA}" name="Name"/>
     <tableColumn id="2" xr3:uid="{2B35EEA3-E0F7-4524-A794-0928233E506B}" name="Value"/>
@@ -1325,8 +1364,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{F8A6BD26-C645-4175-8476-817D5672FD54}" name="Table13" displayName="Table13" ref="A1:C109" totalsRowShown="0">
-  <autoFilter ref="A1:C109" xr:uid="{A7872B2C-8222-446D-9C51-8EA59078049C}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{F8A6BD26-C645-4175-8476-817D5672FD54}" name="Table13" displayName="Table13" ref="A1:C112" totalsRowShown="0">
+  <autoFilter ref="A1:C112" xr:uid="{A7872B2C-8222-446D-9C51-8EA59078049C}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{5D541690-4DCC-4D96-9FCC-B1699146EC35}" name="Name"/>
     <tableColumn id="2" xr3:uid="{86DF2464-58F6-48AD-98C9-2D16B29FBB6F}" name="EN" dataDxfId="1"/>
@@ -1601,7 +1640,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D89C9C48-5454-47C4-AB1D-448E4519251A}">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -1662,7 +1701,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C41"/>
+  <dimension ref="A1:C43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -1670,7 +1709,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="39.6328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="48.453125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="57.7265625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="63.90625" customWidth="1"/>
   </cols>
@@ -2124,6 +2163,28 @@
       </c>
       <c r="C41" s="1" t="s">
         <v>288</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="A42" t="s">
+        <v>402</v>
+      </c>
+      <c r="B42" t="s">
+        <v>33</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="A43" t="s">
+        <v>404</v>
+      </c>
+      <c r="B43" t="s">
+        <v>33</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>405</v>
       </c>
     </row>
   </sheetData>
@@ -2137,15 +2198,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1927ABA9-1814-4487-9CEC-ABDCAF91481F}">
-  <dimension ref="A1:C109"/>
+  <dimension ref="A1:C112"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="43.7265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="50.36328125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="79" customWidth="1"/>
     <col min="3" max="3" width="114.26953125" bestFit="1" customWidth="1"/>
   </cols>
@@ -2501,762 +2562,795 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>206</v>
+        <v>393</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>205</v>
+        <v>395</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>207</v>
+        <v>396</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>357</v>
+        <v>401</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>358</v>
+        <v>394</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>359</v>
+        <v>397</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>20</v>
+        <v>206</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>21</v>
+        <v>205</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>370</v>
+        <v>207</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>25</v>
+        <v>357</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>26</v>
+        <v>358</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>380</v>
+        <v>359</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>31</v>
+        <v>370</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>367</v>
+        <v>29</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>368</v>
+        <v>30</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>369</v>
+        <v>31</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
-        <v>321</v>
+        <v>35</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>322</v>
+        <v>36</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>371</v>
+        <v>381</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
-        <v>326</v>
+        <v>367</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>327</v>
+        <v>368</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>328</v>
+        <v>369</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
-        <v>390</v>
+        <v>321</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>391</v>
+        <v>322</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>392</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
-        <v>37</v>
+        <v>326</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>38</v>
+        <v>327</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>382</v>
+        <v>328</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
-        <v>84</v>
+        <v>390</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>85</v>
+        <v>391</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>372</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>373</v>
+        <v>382</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>383</v>
+        <v>372</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
-        <v>82</v>
+        <v>39</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>83</v>
+        <v>40</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>384</v>
+        <v>373</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
-        <v>104</v>
+        <v>81</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>107</v>
+        <v>80</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>110</v>
+        <v>383</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
-        <v>105</v>
+        <v>82</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>108</v>
+        <v>83</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>111</v>
+        <v>384</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
-        <v>77</v>
+        <v>105</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>76</v>
+        <v>108</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>78</v>
+        <v>111</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B53" s="1"/>
-      <c r="C53" s="1"/>
+      <c r="A53" t="s">
+        <v>106</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
-        <v>44</v>
+        <v>77</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>45</v>
+        <v>76</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>385</v>
+        <v>78</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A55" t="s">
-        <v>69</v>
-      </c>
-      <c r="B55" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="C55" s="1" t="s">
-        <v>75</v>
-      </c>
+      <c r="B55" s="1"/>
+      <c r="C55" s="1"/>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
-        <v>86</v>
+        <v>44</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>87</v>
+        <v>45</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>88</v>
+        <v>385</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
-        <v>92</v>
+        <v>69</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>93</v>
+        <v>79</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>94</v>
+        <v>75</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
-        <v>98</v>
+        <v>86</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>103</v>
+        <v>87</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>99</v>
+        <v>88</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
-        <v>301</v>
+        <v>92</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>303</v>
+        <v>93</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>302</v>
+        <v>94</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
-        <v>306</v>
+        <v>98</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>305</v>
+        <v>103</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>304</v>
+        <v>99</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
-        <v>307</v>
+        <v>301</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>308</v>
+        <v>303</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>309</v>
+        <v>302</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B62" s="1"/>
-      <c r="C62" s="1"/>
+      <c r="A62" t="s">
+        <v>306</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>305</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>304</v>
+      </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
-        <v>115</v>
+        <v>307</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>116</v>
+        <v>308</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>117</v>
+        <v>309</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A64" t="s">
-        <v>118</v>
-      </c>
-      <c r="B64" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="C64" s="1" t="s">
-        <v>386</v>
-      </c>
+      <c r="B64" s="1"/>
+      <c r="C64" s="1"/>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>125</v>
+        <v>386</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
-        <v>165</v>
+        <v>120</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>166</v>
+        <v>121</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>167</v>
+        <v>122</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
-        <v>168</v>
+        <v>123</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>169</v>
+        <v>124</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>170</v>
+        <v>125</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
-        <v>228</v>
+        <v>165</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>229</v>
+        <v>166</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>387</v>
+        <v>167</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
-        <v>237</v>
+        <v>168</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>238</v>
+        <v>169</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>388</v>
+        <v>170</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>235</v>
+        <v>229</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>236</v>
+        <v>387</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B72" s="1"/>
-      <c r="C72" s="1"/>
+      <c r="A72" t="s">
+        <v>237</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="C72" s="1" t="s">
+        <v>388</v>
+      </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
-        <v>56</v>
+        <v>234</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>161</v>
+        <v>235</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>57</v>
+        <v>236</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A74" t="s">
-        <v>61</v>
-      </c>
-      <c r="B74" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="C74" s="1" t="s">
-        <v>72</v>
-      </c>
+      <c r="B74" s="1"/>
+      <c r="C74" s="1"/>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
-        <v>126</v>
+        <v>56</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>127</v>
+        <v>161</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>128</v>
+        <v>57</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
-        <v>129</v>
+        <v>61</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>130</v>
+        <v>114</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>131</v>
+        <v>72</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
-        <v>135</v>
+        <v>126</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>136</v>
+        <v>127</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
-        <v>141</v>
+        <v>129</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>142</v>
+        <v>130</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>143</v>
+        <v>131</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
-        <v>162</v>
+        <v>141</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>163</v>
+        <v>142</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>164</v>
+        <v>143</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B81" s="1"/>
-      <c r="C81" s="1"/>
+      <c r="A81" t="s">
+        <v>144</v>
+      </c>
+      <c r="B81" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="C81" s="1" t="s">
+        <v>146</v>
+      </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
-        <v>60</v>
+        <v>162</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>113</v>
+        <v>163</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>73</v>
+        <v>164</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A83" t="s">
-        <v>41</v>
-      </c>
-      <c r="B83" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="C83" s="1" t="s">
-        <v>43</v>
-      </c>
+      <c r="B83" s="1"/>
+      <c r="C83" s="1"/>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
-        <v>132</v>
+        <v>60</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>133</v>
+        <v>113</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>134</v>
+        <v>73</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
-        <v>231</v>
+        <v>41</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>232</v>
+        <v>42</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>233</v>
+        <v>43</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A86" t="s">
+        <v>132</v>
+      </c>
+      <c r="B86" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="C86" s="1" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
-        <v>62</v>
+        <v>231</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>70</v>
+        <v>232</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A88" t="s">
-        <v>89</v>
-      </c>
-      <c r="B88" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="C88" s="1" t="s">
-        <v>91</v>
+        <v>233</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
-        <v>95</v>
+        <v>62</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>96</v>
+        <v>70</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>97</v>
+        <v>71</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
-        <v>100</v>
+        <v>89</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>102</v>
+        <v>90</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>101</v>
+        <v>91</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
-        <v>222</v>
+        <v>95</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>223</v>
+        <v>96</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>224</v>
+        <v>97</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A92" t="s">
+        <v>100</v>
+      </c>
+      <c r="B92" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C92" s="1" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
-        <v>66</v>
+        <v>222</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>138</v>
+        <v>223</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A94" t="s">
-        <v>139</v>
-      </c>
-      <c r="B94" t="s">
-        <v>218</v>
-      </c>
-      <c r="C94" t="s">
-        <v>140</v>
+        <v>224</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
-        <v>150</v>
-      </c>
-      <c r="B95" t="s">
-        <v>151</v>
-      </c>
-      <c r="C95" t="s">
-        <v>152</v>
+        <v>66</v>
+      </c>
+      <c r="B95" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="C95" s="1" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
-        <v>153</v>
-      </c>
-      <c r="B96" s="1" t="s">
-        <v>154</v>
+        <v>139</v>
+      </c>
+      <c r="B96" t="s">
+        <v>218</v>
       </c>
       <c r="C96" t="s">
-        <v>155</v>
+        <v>140</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="B97" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="C97" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
-        <v>210</v>
+        <v>153</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>230</v>
-      </c>
-      <c r="C98" s="1" t="s">
-        <v>389</v>
+        <v>154</v>
+      </c>
+      <c r="C98" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A99" t="s">
+        <v>157</v>
+      </c>
+      <c r="B99" t="s">
+        <v>158</v>
+      </c>
+      <c r="C99" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
+        <v>210</v>
+      </c>
+      <c r="B100" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="C100" s="1" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A102" t="s">
         <v>219</v>
       </c>
-      <c r="B100" s="1" t="s">
+      <c r="B102" s="1" t="s">
         <v>220</v>
       </c>
-      <c r="C100" s="1" t="s">
+      <c r="C102" s="1" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A101" t="s">
-        <v>225</v>
-      </c>
-      <c r="B101" s="1" t="s">
-        <v>226</v>
-      </c>
-      <c r="C101" s="1" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B102" s="1"/>
-      <c r="C102" s="1"/>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
-        <v>239</v>
+        <v>225</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>240</v>
+        <v>226</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>241</v>
+        <v>227</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A104" t="s">
-        <v>250</v>
-      </c>
-      <c r="B104" s="1" t="s">
-        <v>251</v>
-      </c>
-      <c r="C104" s="1" t="s">
-        <v>252</v>
-      </c>
+      <c r="B104" s="1"/>
+      <c r="C104" s="1"/>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
-        <v>253</v>
+        <v>239</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>254</v>
+        <v>240</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>255</v>
+        <v>241</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
-        <v>256</v>
+        <v>250</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>257</v>
+        <v>251</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>258</v>
+        <v>252</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B107" s="1"/>
-      <c r="C107" s="1"/>
+      <c r="A107" t="s">
+        <v>253</v>
+      </c>
+      <c r="B107" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="C107" s="1" t="s">
+        <v>255</v>
+      </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
-        <v>242</v>
+        <v>256</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>243</v>
+        <v>257</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>244</v>
+        <v>258</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
+        <v>398</v>
+      </c>
+      <c r="B109" s="1" t="s">
+        <v>399</v>
+      </c>
+      <c r="C109" s="1" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B110" s="1"/>
+      <c r="C110" s="1"/>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A111" t="s">
+        <v>242</v>
+      </c>
+      <c r="B111" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="C111" s="1" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A112" t="s">
         <v>247</v>
       </c>
-      <c r="B109" s="1" t="s">
+      <c r="B112" s="1" t="s">
         <v>248</v>
       </c>
-      <c r="C109" s="1" t="s">
+      <c r="C112" s="1" t="s">
         <v>249</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Ask user for entities workbooks path
Use the stored value as form default in subsequent runs
</commit_message>
<xml_diff>
--- a/Config.xlsx
+++ b/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mateus.cruz\Documents\GitHub\OrchestratorManager\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADB5CFF0-2518-4C5E-AF66-A205B6320440}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D16476D5-E3A2-43E1-9B4F-F3BD8CBF6BF9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="445" uniqueCount="414">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="450" uniqueCount="419">
   <si>
     <t>Name</t>
   </si>
@@ -50,11 +50,14 @@
   </si>
   <si>
     <t>URL of the Orchestrator instance to be used. 
-Sample value: https://myOrchestratorurl.
+Sample value: https://myOrchestratorURL.
 UiPath Cloud Platform (https://platform.uipath.com) is currently not supported.</t>
   </si>
   <si>
     <t>OrchestratorTenant</t>
+  </si>
+  <si>
+    <t>Default</t>
   </si>
   <si>
     <t>Name of the tenant to be used. 
@@ -64,9 +67,6 @@
     <t>EntitiesWorkbooksFolderPath</t>
   </si>
   <si>
-    <t>Workbooks</t>
-  </si>
-  <si>
     <t>Path to the folder that contains entities workbooks. 
 Sample value: C:\Users\MyUser\Desktop\Workbooks</t>
   </si>
@@ -396,6 +396,15 @@
     <t>テナント名</t>
   </si>
   <si>
+    <t>FormWorkbooksFolderPathLabel</t>
+  </si>
+  <si>
+    <t>Workbooks Path</t>
+  </si>
+  <si>
+    <t>ワークボックスパス</t>
+  </si>
+  <si>
     <t>FormUsernameLabel</t>
   </si>
   <si>
@@ -1282,6 +1291,12 @@
   </si>
   <si>
     <t>パッケージバージョンが指定されませんでした。</t>
+  </si>
+  <si>
+    <t>Workbooks</t>
+  </si>
+  <si>
+    <t>https://myOrchestratorURL</t>
   </si>
 </sst>
 </file>
@@ -1322,18 +1337,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1374,8 +1391,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table13" displayName="Table13" ref="A1:C115" totalsRowShown="0">
-  <autoFilter ref="A1:C115" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table13" displayName="Table13" ref="A1:C116" totalsRowShown="0">
+  <autoFilter ref="A1:C116" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Name"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="EN"/>
@@ -1676,8 +1693,10 @@
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="3" t="s">
+      <c r="B2" s="3" t="s">
+        <v>418</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1685,26 +1704,32 @@
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="B3" s="1" t="s">
         <v>6</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="3" t="s">
+        <v>417</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>9</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
@@ -1742,7 +1767,7 @@
       <c r="B2" s="1">
         <v>200</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>11</v>
       </c>
     </row>
@@ -1753,7 +1778,7 @@
       <c r="B3" s="1">
         <v>0</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="2" t="s">
         <v>13</v>
       </c>
     </row>
@@ -1764,7 +1789,7 @@
       <c r="B4" s="1">
         <v>500</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="2" t="s">
         <v>15</v>
       </c>
     </row>
@@ -1775,7 +1800,7 @@
       <c r="B5" s="1">
         <v>600</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="2" t="s">
         <v>17</v>
       </c>
     </row>
@@ -1786,7 +1811,7 @@
       <c r="B6" s="1">
         <v>3</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="2" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1797,7 +1822,7 @@
       <c r="B7" s="1">
         <v>5000</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="2" t="s">
         <v>21</v>
       </c>
     </row>
@@ -1808,7 +1833,7 @@
       <c r="B8" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="2" t="s">
         <v>24</v>
       </c>
     </row>
@@ -1819,7 +1844,7 @@
       <c r="B9" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C9" s="2" t="s">
         <v>27</v>
       </c>
     </row>
@@ -1830,7 +1855,7 @@
       <c r="B10" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C10" s="2" t="s">
         <v>30</v>
       </c>
     </row>
@@ -1841,7 +1866,7 @@
       <c r="B11" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C11" s="2" t="s">
         <v>33</v>
       </c>
     </row>
@@ -1852,7 +1877,7 @@
       <c r="B12" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C12" s="2" t="s">
         <v>36</v>
       </c>
     </row>
@@ -1863,7 +1888,7 @@
       <c r="B13" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C13" s="2" t="s">
         <v>39</v>
       </c>
     </row>
@@ -1874,7 +1899,7 @@
       <c r="B14" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="C14" s="2" t="s">
         <v>42</v>
       </c>
     </row>
@@ -1885,7 +1910,7 @@
       <c r="B15" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="C15" s="2" t="s">
         <v>45</v>
       </c>
     </row>
@@ -1896,7 +1921,7 @@
       <c r="B16" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="C16" s="2" t="s">
         <v>48</v>
       </c>
     </row>
@@ -1907,7 +1932,7 @@
       <c r="B17" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="C17" s="3" t="s">
+      <c r="C17" s="2" t="s">
         <v>50</v>
       </c>
     </row>
@@ -1918,7 +1943,7 @@
       <c r="B18" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C18" s="3" t="s">
+      <c r="C18" s="2" t="s">
         <v>52</v>
       </c>
     </row>
@@ -1929,7 +1954,7 @@
       <c r="B19" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="C19" s="3" t="s">
+      <c r="C19" s="2" t="s">
         <v>55</v>
       </c>
     </row>
@@ -1940,7 +1965,7 @@
       <c r="B20" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C20" s="3" t="s">
+      <c r="C20" s="2" t="s">
         <v>52</v>
       </c>
     </row>
@@ -1951,7 +1976,7 @@
       <c r="B21" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="C21" s="3" t="s">
+      <c r="C21" s="2" t="s">
         <v>58</v>
       </c>
     </row>
@@ -1962,7 +1987,7 @@
       <c r="B22" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C22" s="3" t="s">
+      <c r="C22" s="2" t="s">
         <v>60</v>
       </c>
     </row>
@@ -1973,7 +1998,7 @@
       <c r="B23" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="C23" s="3" t="s">
+      <c r="C23" s="2" t="s">
         <v>62</v>
       </c>
     </row>
@@ -1984,7 +2009,7 @@
       <c r="B24" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C24" s="3" t="s">
+      <c r="C24" s="2" t="s">
         <v>64</v>
       </c>
     </row>
@@ -1995,7 +2020,7 @@
       <c r="B25" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="C25" s="3" t="s">
+      <c r="C25" s="2" t="s">
         <v>67</v>
       </c>
     </row>
@@ -2006,7 +2031,7 @@
       <c r="B26" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="C26" s="3" t="s">
+      <c r="C26" s="2" t="s">
         <v>70</v>
       </c>
     </row>
@@ -2017,7 +2042,7 @@
       <c r="B27" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="C27" s="3" t="s">
+      <c r="C27" s="2" t="s">
         <v>72</v>
       </c>
     </row>
@@ -2028,7 +2053,7 @@
       <c r="B28" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="C28" s="3" t="s">
+      <c r="C28" s="2" t="s">
         <v>75</v>
       </c>
     </row>
@@ -2039,7 +2064,7 @@
       <c r="B29" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C29" s="3" t="s">
+      <c r="C29" s="2" t="s">
         <v>77</v>
       </c>
     </row>
@@ -2050,7 +2075,7 @@
       <c r="B30" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="C30" s="3" t="s">
+      <c r="C30" s="2" t="s">
         <v>79</v>
       </c>
     </row>
@@ -2061,7 +2086,7 @@
       <c r="B31" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="C31" s="3" t="s">
+      <c r="C31" s="2" t="s">
         <v>81</v>
       </c>
     </row>
@@ -2072,7 +2097,7 @@
       <c r="B32" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="C32" s="3" t="s">
+      <c r="C32" s="2" t="s">
         <v>83</v>
       </c>
     </row>
@@ -2083,7 +2108,7 @@
       <c r="B33" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="C33" s="3" t="s">
+      <c r="C33" s="2" t="s">
         <v>85</v>
       </c>
     </row>
@@ -2094,7 +2119,7 @@
       <c r="B34" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="C34" s="3" t="s">
+      <c r="C34" s="2" t="s">
         <v>87</v>
       </c>
     </row>
@@ -2105,7 +2130,7 @@
       <c r="B35" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C35" s="3" t="s">
+      <c r="C35" s="2" t="s">
         <v>89</v>
       </c>
     </row>
@@ -2116,7 +2141,7 @@
       <c r="B36" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C36" s="3" t="s">
+      <c r="C36" s="2" t="s">
         <v>91</v>
       </c>
     </row>
@@ -2127,7 +2152,7 @@
       <c r="B37" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="C37" s="3" t="s">
+      <c r="C37" s="2" t="s">
         <v>93</v>
       </c>
     </row>
@@ -2138,7 +2163,7 @@
       <c r="B38" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="C38" s="3" t="s">
+      <c r="C38" s="2" t="s">
         <v>95</v>
       </c>
     </row>
@@ -2149,7 +2174,7 @@
       <c r="B39" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C39" s="3" t="s">
+      <c r="C39" s="2" t="s">
         <v>97</v>
       </c>
     </row>
@@ -2160,7 +2185,7 @@
       <c r="B40" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="C40" s="3" t="s">
+      <c r="C40" s="2" t="s">
         <v>99</v>
       </c>
     </row>
@@ -2171,7 +2196,7 @@
       <c r="B41" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C41" s="3" t="s">
+      <c r="C41" s="2" t="s">
         <v>101</v>
       </c>
     </row>
@@ -2182,7 +2207,7 @@
       <c r="B42" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="C42" s="3" t="s">
+      <c r="C42" s="2" t="s">
         <v>103</v>
       </c>
     </row>
@@ -2193,7 +2218,7 @@
       <c r="B43" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="C43" s="3" t="s">
+      <c r="C43" s="2" t="s">
         <v>105</v>
       </c>
     </row>
@@ -2208,7 +2233,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1927ABA9-1814-4487-9CEC-ABDCAF91481F}">
-  <dimension ref="A1:C115"/>
+  <dimension ref="A1:C116"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -2236,10 +2261,10 @@
       <c r="A2" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>109</v>
       </c>
     </row>
@@ -2247,10 +2272,10 @@
       <c r="A3" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="2" t="s">
         <v>112</v>
       </c>
     </row>
@@ -2258,10 +2283,10 @@
       <c r="A4" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="2" t="s">
         <v>114</v>
       </c>
     </row>
@@ -2269,10 +2294,10 @@
       <c r="A5" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="2" t="s">
         <v>117</v>
       </c>
     </row>
@@ -2280,10 +2305,10 @@
       <c r="A6" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="2" t="s">
         <v>120</v>
       </c>
     </row>
@@ -2291,10 +2316,10 @@
       <c r="A7" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="2" t="s">
         <v>123</v>
       </c>
     </row>
@@ -2302,10 +2327,10 @@
       <c r="A8" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="2" t="s">
         <v>126</v>
       </c>
     </row>
@@ -2313,10 +2338,10 @@
       <c r="A9" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C9" s="2" t="s">
         <v>129</v>
       </c>
     </row>
@@ -2324,10 +2349,10 @@
       <c r="A10" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C10" s="2" t="s">
         <v>132</v>
       </c>
     </row>
@@ -2335,10 +2360,10 @@
       <c r="A11" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C11" s="2" t="s">
         <v>135</v>
       </c>
     </row>
@@ -2346,10 +2371,10 @@
       <c r="A12" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B12" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C12" s="2" t="s">
         <v>138</v>
       </c>
     </row>
@@ -2357,10 +2382,10 @@
       <c r="A13" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B13" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C13" s="2" t="s">
         <v>141</v>
       </c>
     </row>
@@ -2368,10 +2393,10 @@
       <c r="A14" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="B14" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="C14" s="2" t="s">
         <v>144</v>
       </c>
     </row>
@@ -2379,10 +2404,10 @@
       <c r="A15" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="B15" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="C15" s="2" t="s">
         <v>147</v>
       </c>
     </row>
@@ -2390,10 +2415,10 @@
       <c r="A16" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="B16" s="3" t="s">
+      <c r="B16" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="C16" s="2" t="s">
         <v>150</v>
       </c>
     </row>
@@ -2401,47 +2426,47 @@
       <c r="A17" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="B17" s="3" t="s">
+      <c r="B17" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="C17" s="3" t="s">
-        <v>152</v>
+      <c r="C17" s="2" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="B18" s="3" t="s">
         <v>154</v>
       </c>
-      <c r="C18" s="3" t="s">
+      <c r="B18" s="2" t="s">
         <v>155</v>
       </c>
+      <c r="C18" s="2" t="s">
+        <v>155</v>
+      </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B19" s="3"/>
-      <c r="C19" s="3"/>
+      <c r="A19" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>158</v>
+      </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A20" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>157</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>158</v>
-      </c>
+      <c r="B20" s="2"/>
+      <c r="C20" s="2"/>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="B21" s="3" t="s">
+      <c r="B21" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="C21" s="3" t="s">
+      <c r="C21" s="2" t="s">
         <v>161</v>
       </c>
     </row>
@@ -2449,10 +2474,10 @@
       <c r="A22" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="B22" s="3" t="s">
+      <c r="B22" s="2" t="s">
         <v>163</v>
       </c>
-      <c r="C22" s="3" t="s">
+      <c r="C22" s="2" t="s">
         <v>164</v>
       </c>
     </row>
@@ -2460,10 +2485,10 @@
       <c r="A23" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="B23" s="3" t="s">
+      <c r="B23" s="2" t="s">
         <v>166</v>
       </c>
-      <c r="C23" s="3" t="s">
+      <c r="C23" s="2" t="s">
         <v>167</v>
       </c>
     </row>
@@ -2471,10 +2496,10 @@
       <c r="A24" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="B24" s="3" t="s">
+      <c r="B24" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="C24" s="3" t="s">
+      <c r="C24" s="2" t="s">
         <v>170</v>
       </c>
     </row>
@@ -2482,36 +2507,36 @@
       <c r="A25" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="B25" s="3" t="s">
+      <c r="B25" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="C25" s="3" t="s">
+      <c r="C25" s="2" t="s">
         <v>173</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B26" s="3"/>
-      <c r="C26" s="3"/>
+      <c r="A26" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>176</v>
+      </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A27" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="B27" s="3" t="s">
-        <v>175</v>
-      </c>
-      <c r="C27" s="3" t="s">
-        <v>176</v>
-      </c>
+      <c r="B27" s="2"/>
+      <c r="C27" s="2"/>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="B28" s="3" t="s">
+      <c r="B28" s="2" t="s">
         <v>178</v>
       </c>
-      <c r="C28" s="3" t="s">
+      <c r="C28" s="2" t="s">
         <v>179</v>
       </c>
     </row>
@@ -2519,10 +2544,10 @@
       <c r="A29" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="B29" s="3" t="s">
+      <c r="B29" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="C29" s="3" t="s">
+      <c r="C29" s="2" t="s">
         <v>182</v>
       </c>
     </row>
@@ -2530,10 +2555,10 @@
       <c r="A30" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="B30" s="3" t="s">
+      <c r="B30" s="2" t="s">
         <v>184</v>
       </c>
-      <c r="C30" s="3" t="s">
+      <c r="C30" s="2" t="s">
         <v>185</v>
       </c>
     </row>
@@ -2541,10 +2566,10 @@
       <c r="A31" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="B31" s="3" t="s">
+      <c r="B31" s="2" t="s">
         <v>187</v>
       </c>
-      <c r="C31" s="3" t="s">
+      <c r="C31" s="2" t="s">
         <v>188</v>
       </c>
     </row>
@@ -2552,10 +2577,10 @@
       <c r="A32" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="B32" s="3" t="s">
+      <c r="B32" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="C32" s="3" t="s">
+      <c r="C32" s="2" t="s">
         <v>191</v>
       </c>
     </row>
@@ -2563,10 +2588,10 @@
       <c r="A33" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="B33" s="3" t="s">
+      <c r="B33" s="2" t="s">
         <v>193</v>
       </c>
-      <c r="C33" s="3" t="s">
+      <c r="C33" s="2" t="s">
         <v>194</v>
       </c>
     </row>
@@ -2574,10 +2599,10 @@
       <c r="A34" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="B34" s="3" t="s">
+      <c r="B34" s="2" t="s">
         <v>196</v>
       </c>
-      <c r="C34" s="3" t="s">
+      <c r="C34" s="2" t="s">
         <v>197</v>
       </c>
     </row>
@@ -2585,10 +2610,10 @@
       <c r="A35" s="1" t="s">
         <v>198</v>
       </c>
-      <c r="B35" s="3" t="s">
+      <c r="B35" s="2" t="s">
         <v>199</v>
       </c>
-      <c r="C35" s="3" t="s">
+      <c r="C35" s="2" t="s">
         <v>200</v>
       </c>
     </row>
@@ -2596,10 +2621,10 @@
       <c r="A36" s="1" t="s">
         <v>201</v>
       </c>
-      <c r="B36" s="3" t="s">
+      <c r="B36" s="2" t="s">
         <v>202</v>
       </c>
-      <c r="C36" s="3" t="s">
+      <c r="C36" s="2" t="s">
         <v>203</v>
       </c>
     </row>
@@ -2607,10 +2632,10 @@
       <c r="A37" s="1" t="s">
         <v>204</v>
       </c>
-      <c r="B37" s="3" t="s">
+      <c r="B37" s="2" t="s">
         <v>205</v>
       </c>
-      <c r="C37" s="3" t="s">
+      <c r="C37" s="2" t="s">
         <v>206</v>
       </c>
     </row>
@@ -2618,10 +2643,10 @@
       <c r="A38" s="1" t="s">
         <v>207</v>
       </c>
-      <c r="B38" s="3" t="s">
+      <c r="B38" s="2" t="s">
         <v>208</v>
       </c>
-      <c r="C38" s="3" t="s">
+      <c r="C38" s="2" t="s">
         <v>209</v>
       </c>
     </row>
@@ -2629,10 +2654,10 @@
       <c r="A39" s="1" t="s">
         <v>210</v>
       </c>
-      <c r="B39" s="3" t="s">
+      <c r="B39" s="2" t="s">
         <v>211</v>
       </c>
-      <c r="C39" s="3" t="s">
+      <c r="C39" s="2" t="s">
         <v>212</v>
       </c>
     </row>
@@ -2640,10 +2665,10 @@
       <c r="A40" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="B40" s="3" t="s">
+      <c r="B40" s="2" t="s">
         <v>214</v>
       </c>
-      <c r="C40" s="3" t="s">
+      <c r="C40" s="2" t="s">
         <v>215</v>
       </c>
     </row>
@@ -2651,10 +2676,10 @@
       <c r="A41" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="B41" s="3" t="s">
+      <c r="B41" s="2" t="s">
         <v>217</v>
       </c>
-      <c r="C41" s="3" t="s">
+      <c r="C41" s="2" t="s">
         <v>218</v>
       </c>
     </row>
@@ -2662,10 +2687,10 @@
       <c r="A42" s="1" t="s">
         <v>219</v>
       </c>
-      <c r="B42" s="3" t="s">
+      <c r="B42" s="2" t="s">
         <v>220</v>
       </c>
-      <c r="C42" s="3" t="s">
+      <c r="C42" s="2" t="s">
         <v>221</v>
       </c>
     </row>
@@ -2673,10 +2698,10 @@
       <c r="A43" s="1" t="s">
         <v>222</v>
       </c>
-      <c r="B43" s="3" t="s">
+      <c r="B43" s="2" t="s">
         <v>223</v>
       </c>
-      <c r="C43" s="3" t="s">
+      <c r="C43" s="2" t="s">
         <v>224</v>
       </c>
     </row>
@@ -2684,10 +2709,10 @@
       <c r="A44" s="1" t="s">
         <v>225</v>
       </c>
-      <c r="B44" s="3" t="s">
+      <c r="B44" s="2" t="s">
         <v>226</v>
       </c>
-      <c r="C44" s="3" t="s">
+      <c r="C44" s="2" t="s">
         <v>227</v>
       </c>
     </row>
@@ -2695,10 +2720,10 @@
       <c r="A45" s="1" t="s">
         <v>228</v>
       </c>
-      <c r="B45" s="3" t="s">
+      <c r="B45" s="2" t="s">
         <v>229</v>
       </c>
-      <c r="C45" s="3" t="s">
+      <c r="C45" s="2" t="s">
         <v>230</v>
       </c>
     </row>
@@ -2706,10 +2731,10 @@
       <c r="A46" s="1" t="s">
         <v>231</v>
       </c>
-      <c r="B46" s="3" t="s">
+      <c r="B46" s="2" t="s">
         <v>232</v>
       </c>
-      <c r="C46" s="3" t="s">
+      <c r="C46" s="2" t="s">
         <v>233</v>
       </c>
     </row>
@@ -2717,10 +2742,10 @@
       <c r="A47" s="1" t="s">
         <v>234</v>
       </c>
-      <c r="B47" s="3" t="s">
+      <c r="B47" s="2" t="s">
         <v>235</v>
       </c>
-      <c r="C47" s="3" t="s">
+      <c r="C47" s="2" t="s">
         <v>236</v>
       </c>
     </row>
@@ -2728,32 +2753,32 @@
       <c r="A48" s="1" t="s">
         <v>237</v>
       </c>
-      <c r="B48" s="3" t="s">
+      <c r="B48" s="2" t="s">
         <v>238</v>
       </c>
-      <c r="C48" s="3" t="s">
+      <c r="C48" s="2" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="49" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A49" s="1" t="s">
         <v>240</v>
       </c>
-      <c r="B49" s="3" t="s">
+      <c r="B49" s="2" t="s">
         <v>241</v>
       </c>
-      <c r="C49" s="3" t="s">
+      <c r="C49" s="2" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A50" s="1" t="s">
         <v>243</v>
       </c>
-      <c r="B50" s="3" t="s">
+      <c r="B50" s="2" t="s">
         <v>244</v>
       </c>
-      <c r="C50" s="3" t="s">
+      <c r="C50" s="2" t="s">
         <v>245</v>
       </c>
     </row>
@@ -2761,10 +2786,10 @@
       <c r="A51" s="1" t="s">
         <v>246</v>
       </c>
-      <c r="B51" s="3" t="s">
+      <c r="B51" s="2" t="s">
         <v>247</v>
       </c>
-      <c r="C51" s="3" t="s">
+      <c r="C51" s="2" t="s">
         <v>248</v>
       </c>
     </row>
@@ -2772,10 +2797,10 @@
       <c r="A52" s="1" t="s">
         <v>249</v>
       </c>
-      <c r="B52" s="3" t="s">
+      <c r="B52" s="2" t="s">
         <v>250</v>
       </c>
-      <c r="C52" s="3" t="s">
+      <c r="C52" s="2" t="s">
         <v>251</v>
       </c>
     </row>
@@ -2783,10 +2808,10 @@
       <c r="A53" s="1" t="s">
         <v>252</v>
       </c>
-      <c r="B53" s="3" t="s">
+      <c r="B53" s="2" t="s">
         <v>253</v>
       </c>
-      <c r="C53" s="3" t="s">
+      <c r="C53" s="2" t="s">
         <v>254</v>
       </c>
     </row>
@@ -2794,10 +2819,10 @@
       <c r="A54" s="1" t="s">
         <v>255</v>
       </c>
-      <c r="B54" s="3" t="s">
+      <c r="B54" s="2" t="s">
         <v>256</v>
       </c>
-      <c r="C54" s="3" t="s">
+      <c r="C54" s="2" t="s">
         <v>257</v>
       </c>
     </row>
@@ -2805,10 +2830,10 @@
       <c r="A55" s="1" t="s">
         <v>258</v>
       </c>
-      <c r="B55" s="3" t="s">
+      <c r="B55" s="2" t="s">
         <v>259</v>
       </c>
-      <c r="C55" s="3" t="s">
+      <c r="C55" s="2" t="s">
         <v>260</v>
       </c>
     </row>
@@ -2816,10 +2841,10 @@
       <c r="A56" s="1" t="s">
         <v>261</v>
       </c>
-      <c r="B56" s="3" t="s">
+      <c r="B56" s="2" t="s">
         <v>262</v>
       </c>
-      <c r="C56" s="3" t="s">
+      <c r="C56" s="2" t="s">
         <v>263</v>
       </c>
     </row>
@@ -2827,36 +2852,36 @@
       <c r="A57" s="1" t="s">
         <v>264</v>
       </c>
-      <c r="B57" s="3" t="s">
+      <c r="B57" s="2" t="s">
         <v>265</v>
       </c>
-      <c r="C57" s="3" t="s">
+      <c r="C57" s="2" t="s">
         <v>266</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B58" s="3"/>
-      <c r="C58" s="3"/>
+      <c r="A58" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>268</v>
+      </c>
+      <c r="C58" s="2" t="s">
+        <v>269</v>
+      </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A59" s="1" t="s">
-        <v>267</v>
-      </c>
-      <c r="B59" s="3" t="s">
-        <v>268</v>
-      </c>
-      <c r="C59" s="3" t="s">
-        <v>269</v>
-      </c>
+      <c r="B59" s="2"/>
+      <c r="C59" s="2"/>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A60" s="1" t="s">
         <v>270</v>
       </c>
-      <c r="B60" s="3" t="s">
+      <c r="B60" s="2" t="s">
         <v>271</v>
       </c>
-      <c r="C60" s="3" t="s">
+      <c r="C60" s="2" t="s">
         <v>272</v>
       </c>
     </row>
@@ -2864,10 +2889,10 @@
       <c r="A61" s="1" t="s">
         <v>273</v>
       </c>
-      <c r="B61" s="3" t="s">
+      <c r="B61" s="2" t="s">
         <v>274</v>
       </c>
-      <c r="C61" s="3" t="s">
+      <c r="C61" s="2" t="s">
         <v>275</v>
       </c>
     </row>
@@ -2875,10 +2900,10 @@
       <c r="A62" s="1" t="s">
         <v>276</v>
       </c>
-      <c r="B62" s="3" t="s">
+      <c r="B62" s="2" t="s">
         <v>277</v>
       </c>
-      <c r="C62" s="3" t="s">
+      <c r="C62" s="2" t="s">
         <v>278</v>
       </c>
     </row>
@@ -2886,10 +2911,10 @@
       <c r="A63" s="1" t="s">
         <v>279</v>
       </c>
-      <c r="B63" s="3" t="s">
+      <c r="B63" s="2" t="s">
         <v>280</v>
       </c>
-      <c r="C63" s="3" t="s">
+      <c r="C63" s="2" t="s">
         <v>281</v>
       </c>
     </row>
@@ -2897,10 +2922,10 @@
       <c r="A64" s="1" t="s">
         <v>282</v>
       </c>
-      <c r="B64" s="3" t="s">
+      <c r="B64" s="2" t="s">
         <v>283</v>
       </c>
-      <c r="C64" s="3" t="s">
+      <c r="C64" s="2" t="s">
         <v>284</v>
       </c>
     </row>
@@ -2908,10 +2933,10 @@
       <c r="A65" s="1" t="s">
         <v>285</v>
       </c>
-      <c r="B65" s="3" t="s">
+      <c r="B65" s="2" t="s">
         <v>286</v>
       </c>
-      <c r="C65" s="3" t="s">
+      <c r="C65" s="2" t="s">
         <v>287</v>
       </c>
     </row>
@@ -2919,36 +2944,36 @@
       <c r="A66" s="1" t="s">
         <v>288</v>
       </c>
-      <c r="B66" s="3" t="s">
+      <c r="B66" s="2" t="s">
         <v>289</v>
       </c>
-      <c r="C66" s="3" t="s">
+      <c r="C66" s="2" t="s">
         <v>290</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B67" s="3"/>
-      <c r="C67" s="3"/>
+      <c r="A67" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="B67" s="2" t="s">
+        <v>292</v>
+      </c>
+      <c r="C67" s="2" t="s">
+        <v>293</v>
+      </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A68" s="1" t="s">
-        <v>291</v>
-      </c>
-      <c r="B68" s="3" t="s">
-        <v>292</v>
-      </c>
-      <c r="C68" s="3" t="s">
-        <v>293</v>
-      </c>
+      <c r="B68" s="2"/>
+      <c r="C68" s="2"/>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A69" s="1" t="s">
         <v>294</v>
       </c>
-      <c r="B69" s="3" t="s">
+      <c r="B69" s="2" t="s">
         <v>295</v>
       </c>
-      <c r="C69" s="3" t="s">
+      <c r="C69" s="2" t="s">
         <v>296</v>
       </c>
     </row>
@@ -2956,10 +2981,10 @@
       <c r="A70" s="1" t="s">
         <v>297</v>
       </c>
-      <c r="B70" s="3" t="s">
+      <c r="B70" s="2" t="s">
         <v>298</v>
       </c>
-      <c r="C70" s="3" t="s">
+      <c r="C70" s="2" t="s">
         <v>299</v>
       </c>
     </row>
@@ -2967,10 +2992,10 @@
       <c r="A71" s="1" t="s">
         <v>300</v>
       </c>
-      <c r="B71" s="3" t="s">
+      <c r="B71" s="2" t="s">
         <v>301</v>
       </c>
-      <c r="C71" s="3" t="s">
+      <c r="C71" s="2" t="s">
         <v>302</v>
       </c>
     </row>
@@ -2978,10 +3003,10 @@
       <c r="A72" s="1" t="s">
         <v>303</v>
       </c>
-      <c r="B72" s="3" t="s">
+      <c r="B72" s="2" t="s">
         <v>304</v>
       </c>
-      <c r="C72" s="3" t="s">
+      <c r="C72" s="2" t="s">
         <v>305</v>
       </c>
     </row>
@@ -2989,10 +3014,10 @@
       <c r="A73" s="1" t="s">
         <v>306</v>
       </c>
-      <c r="B73" s="3" t="s">
+      <c r="B73" s="2" t="s">
         <v>307</v>
       </c>
-      <c r="C73" s="3" t="s">
+      <c r="C73" s="2" t="s">
         <v>308</v>
       </c>
     </row>
@@ -3000,10 +3025,10 @@
       <c r="A74" s="1" t="s">
         <v>309</v>
       </c>
-      <c r="B74" s="3" t="s">
+      <c r="B74" s="2" t="s">
         <v>310</v>
       </c>
-      <c r="C74" s="3" t="s">
+      <c r="C74" s="2" t="s">
         <v>311</v>
       </c>
     </row>
@@ -3011,10 +3036,10 @@
       <c r="A75" s="1" t="s">
         <v>312</v>
       </c>
-      <c r="B75" s="3" t="s">
+      <c r="B75" s="2" t="s">
         <v>313</v>
       </c>
-      <c r="C75" s="3" t="s">
+      <c r="C75" s="2" t="s">
         <v>314</v>
       </c>
     </row>
@@ -3022,36 +3047,36 @@
       <c r="A76" s="1" t="s">
         <v>315</v>
       </c>
-      <c r="B76" s="3" t="s">
+      <c r="B76" s="2" t="s">
         <v>316</v>
       </c>
-      <c r="C76" s="3" t="s">
+      <c r="C76" s="2" t="s">
         <v>317</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B77" s="3"/>
-      <c r="C77" s="3"/>
+      <c r="A77" s="1" t="s">
+        <v>318</v>
+      </c>
+      <c r="B77" s="2" t="s">
+        <v>319</v>
+      </c>
+      <c r="C77" s="2" t="s">
+        <v>320</v>
+      </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A78" s="1" t="s">
-        <v>318</v>
-      </c>
-      <c r="B78" s="3" t="s">
-        <v>319</v>
-      </c>
-      <c r="C78" s="3" t="s">
-        <v>320</v>
-      </c>
+      <c r="B78" s="2"/>
+      <c r="C78" s="2"/>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A79" s="1" t="s">
         <v>321</v>
       </c>
-      <c r="B79" s="3" t="s">
+      <c r="B79" s="2" t="s">
         <v>322</v>
       </c>
-      <c r="C79" s="3" t="s">
+      <c r="C79" s="2" t="s">
         <v>323</v>
       </c>
     </row>
@@ -3059,10 +3084,10 @@
       <c r="A80" s="1" t="s">
         <v>324</v>
       </c>
-      <c r="B80" s="3" t="s">
+      <c r="B80" s="2" t="s">
         <v>325</v>
       </c>
-      <c r="C80" s="3" t="s">
+      <c r="C80" s="2" t="s">
         <v>326</v>
       </c>
     </row>
@@ -3070,10 +3095,10 @@
       <c r="A81" s="1" t="s">
         <v>327</v>
       </c>
-      <c r="B81" s="3" t="s">
+      <c r="B81" s="2" t="s">
         <v>328</v>
       </c>
-      <c r="C81" s="3" t="s">
+      <c r="C81" s="2" t="s">
         <v>329</v>
       </c>
     </row>
@@ -3081,10 +3106,10 @@
       <c r="A82" s="1" t="s">
         <v>330</v>
       </c>
-      <c r="B82" s="3" t="s">
+      <c r="B82" s="2" t="s">
         <v>331</v>
       </c>
-      <c r="C82" s="3" t="s">
+      <c r="C82" s="2" t="s">
         <v>332</v>
       </c>
     </row>
@@ -3092,10 +3117,10 @@
       <c r="A83" s="1" t="s">
         <v>333</v>
       </c>
-      <c r="B83" s="3" t="s">
+      <c r="B83" s="2" t="s">
         <v>334</v>
       </c>
-      <c r="C83" s="3" t="s">
+      <c r="C83" s="2" t="s">
         <v>335</v>
       </c>
     </row>
@@ -3103,10 +3128,10 @@
       <c r="A84" s="1" t="s">
         <v>336</v>
       </c>
-      <c r="B84" s="3" t="s">
+      <c r="B84" s="2" t="s">
         <v>337</v>
       </c>
-      <c r="C84" s="3" t="s">
+      <c r="C84" s="2" t="s">
         <v>338</v>
       </c>
     </row>
@@ -3114,36 +3139,36 @@
       <c r="A85" s="1" t="s">
         <v>339</v>
       </c>
-      <c r="B85" s="3" t="s">
+      <c r="B85" s="2" t="s">
         <v>340</v>
       </c>
-      <c r="C85" s="3" t="s">
+      <c r="C85" s="2" t="s">
         <v>341</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B86" s="3"/>
-      <c r="C86" s="3"/>
+      <c r="A86" s="1" t="s">
+        <v>342</v>
+      </c>
+      <c r="B86" s="2" t="s">
+        <v>343</v>
+      </c>
+      <c r="C86" s="2" t="s">
+        <v>344</v>
+      </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A87" s="1" t="s">
-        <v>342</v>
-      </c>
-      <c r="B87" s="3" t="s">
-        <v>343</v>
-      </c>
-      <c r="C87" s="3" t="s">
-        <v>344</v>
-      </c>
+      <c r="B87" s="2"/>
+      <c r="C87" s="2"/>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A88" s="1" t="s">
         <v>345</v>
       </c>
-      <c r="B88" s="3" t="s">
+      <c r="B88" s="2" t="s">
         <v>346</v>
       </c>
-      <c r="C88" s="3" t="s">
+      <c r="C88" s="2" t="s">
         <v>347</v>
       </c>
     </row>
@@ -3151,10 +3176,10 @@
       <c r="A89" s="1" t="s">
         <v>348</v>
       </c>
-      <c r="B89" s="3" t="s">
+      <c r="B89" s="2" t="s">
         <v>349</v>
       </c>
-      <c r="C89" s="3" t="s">
+      <c r="C89" s="2" t="s">
         <v>350</v>
       </c>
     </row>
@@ -3162,21 +3187,21 @@
       <c r="A90" s="1" t="s">
         <v>351</v>
       </c>
-      <c r="B90" s="3" t="s">
+      <c r="B90" s="2" t="s">
         <v>352</v>
       </c>
-      <c r="C90" s="3" t="s">
+      <c r="C90" s="2" t="s">
         <v>353</v>
       </c>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A92" s="1" t="s">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A91" s="1" t="s">
         <v>354</v>
       </c>
-      <c r="B92" s="3" t="s">
+      <c r="B91" s="2" t="s">
         <v>355</v>
       </c>
-      <c r="C92" s="3" t="s">
+      <c r="C91" s="2" t="s">
         <v>356</v>
       </c>
     </row>
@@ -3184,10 +3209,10 @@
       <c r="A93" s="1" t="s">
         <v>357</v>
       </c>
-      <c r="B93" s="3" t="s">
+      <c r="B93" s="2" t="s">
         <v>358</v>
       </c>
-      <c r="C93" s="3" t="s">
+      <c r="C93" s="2" t="s">
         <v>359</v>
       </c>
     </row>
@@ -3195,10 +3220,10 @@
       <c r="A94" s="1" t="s">
         <v>360</v>
       </c>
-      <c r="B94" s="3" t="s">
+      <c r="B94" s="2" t="s">
         <v>361</v>
       </c>
-      <c r="C94" s="3" t="s">
+      <c r="C94" s="2" t="s">
         <v>362</v>
       </c>
     </row>
@@ -3206,10 +3231,10 @@
       <c r="A95" s="1" t="s">
         <v>363</v>
       </c>
-      <c r="B95" s="3" t="s">
+      <c r="B95" s="2" t="s">
         <v>364</v>
       </c>
-      <c r="C95" s="3" t="s">
+      <c r="C95" s="2" t="s">
         <v>365</v>
       </c>
     </row>
@@ -3217,21 +3242,21 @@
       <c r="A96" s="1" t="s">
         <v>366</v>
       </c>
-      <c r="B96" s="3" t="s">
+      <c r="B96" s="2" t="s">
         <v>367</v>
       </c>
-      <c r="C96" s="3" t="s">
+      <c r="C96" s="2" t="s">
         <v>368</v>
       </c>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A98" s="1" t="s">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A97" s="1" t="s">
         <v>369</v>
       </c>
-      <c r="B98" s="3" t="s">
+      <c r="B97" s="2" t="s">
         <v>370</v>
       </c>
-      <c r="C98" s="3" t="s">
+      <c r="C97" s="2" t="s">
         <v>371</v>
       </c>
     </row>
@@ -3239,10 +3264,10 @@
       <c r="A99" s="1" t="s">
         <v>372</v>
       </c>
-      <c r="B99" s="1" t="s">
+      <c r="B99" s="2" t="s">
         <v>373</v>
       </c>
-      <c r="C99" s="1" t="s">
+      <c r="C99" s="2" t="s">
         <v>374</v>
       </c>
     </row>
@@ -3261,7 +3286,7 @@
       <c r="A101" s="1" t="s">
         <v>378</v>
       </c>
-      <c r="B101" s="3" t="s">
+      <c r="B101" s="1" t="s">
         <v>379</v>
       </c>
       <c r="C101" s="1" t="s">
@@ -3272,7 +3297,7 @@
       <c r="A102" s="1" t="s">
         <v>381</v>
       </c>
-      <c r="B102" s="1" t="s">
+      <c r="B102" s="2" t="s">
         <v>382</v>
       </c>
       <c r="C102" s="1" t="s">
@@ -3283,21 +3308,21 @@
       <c r="A103" s="1" t="s">
         <v>384</v>
       </c>
-      <c r="B103" s="3" t="s">
+      <c r="B103" s="1" t="s">
         <v>385</v>
       </c>
-      <c r="C103" s="3" t="s">
+      <c r="C103" s="1" t="s">
         <v>386</v>
       </c>
     </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A105" s="1" t="s">
+    <row r="104" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A104" s="1" t="s">
         <v>387</v>
       </c>
-      <c r="B105" s="3" t="s">
+      <c r="B104" s="2" t="s">
         <v>388</v>
       </c>
-      <c r="C105" s="3" t="s">
+      <c r="C104" s="2" t="s">
         <v>389</v>
       </c>
     </row>
@@ -3305,36 +3330,36 @@
       <c r="A106" s="1" t="s">
         <v>390</v>
       </c>
-      <c r="B106" s="3" t="s">
+      <c r="B106" s="2" t="s">
         <v>391</v>
       </c>
-      <c r="C106" s="3" t="s">
+      <c r="C106" s="2" t="s">
         <v>392</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B107" s="3"/>
-      <c r="C107" s="3"/>
+      <c r="A107" s="1" t="s">
+        <v>393</v>
+      </c>
+      <c r="B107" s="2" t="s">
+        <v>394</v>
+      </c>
+      <c r="C107" s="2" t="s">
+        <v>395</v>
+      </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A108" s="1" t="s">
-        <v>393</v>
-      </c>
-      <c r="B108" s="3" t="s">
-        <v>394</v>
-      </c>
-      <c r="C108" s="3" t="s">
-        <v>395</v>
-      </c>
+      <c r="B108" s="2"/>
+      <c r="C108" s="2"/>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A109" s="1" t="s">
         <v>396</v>
       </c>
-      <c r="B109" s="3" t="s">
+      <c r="B109" s="2" t="s">
         <v>397</v>
       </c>
-      <c r="C109" s="3" t="s">
+      <c r="C109" s="2" t="s">
         <v>398</v>
       </c>
     </row>
@@ -3342,10 +3367,10 @@
       <c r="A110" s="1" t="s">
         <v>399</v>
       </c>
-      <c r="B110" s="3" t="s">
+      <c r="B110" s="2" t="s">
         <v>400</v>
       </c>
-      <c r="C110" s="3" t="s">
+      <c r="C110" s="2" t="s">
         <v>401</v>
       </c>
     </row>
@@ -3353,10 +3378,10 @@
       <c r="A111" s="1" t="s">
         <v>402</v>
       </c>
-      <c r="B111" s="3" t="s">
+      <c r="B111" s="2" t="s">
         <v>403</v>
       </c>
-      <c r="C111" s="3" t="s">
+      <c r="C111" s="2" t="s">
         <v>404</v>
       </c>
     </row>
@@ -3364,37 +3389,48 @@
       <c r="A112" s="1" t="s">
         <v>405</v>
       </c>
-      <c r="B112" s="3" t="s">
+      <c r="B112" s="2" t="s">
         <v>406</v>
       </c>
-      <c r="C112" s="3" t="s">
+      <c r="C112" s="2" t="s">
         <v>407</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B113" s="3"/>
-      <c r="C113" s="3"/>
+      <c r="A113" s="1" t="s">
+        <v>408</v>
+      </c>
+      <c r="B113" s="2" t="s">
+        <v>409</v>
+      </c>
+      <c r="C113" s="2" t="s">
+        <v>410</v>
+      </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A114" s="1" t="s">
-        <v>408</v>
-      </c>
-      <c r="B114" s="3" t="s">
-        <v>409</v>
-      </c>
-      <c r="C114" s="3" t="s">
-        <v>410</v>
-      </c>
+      <c r="B114" s="2"/>
+      <c r="C114" s="2"/>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A115" s="1" t="s">
         <v>411</v>
       </c>
-      <c r="B115" s="3" t="s">
+      <c r="B115" s="2" t="s">
         <v>412</v>
       </c>
-      <c r="C115" s="3" t="s">
+      <c r="C115" s="2" t="s">
         <v>413</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A116" s="1" t="s">
+        <v>414</v>
+      </c>
+      <c r="B116" s="2" t="s">
+        <v>415</v>
+      </c>
+      <c r="C116" s="2" t="s">
+        <v>416</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add support to UiPath Cloud Platform
Authentication using ClientID/UserKey and disabling Users manipulation in case of Cloud Platform Orchestrator
</commit_message>
<xml_diff>
--- a/Config.xlsx
+++ b/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mateus.cruz\Documents\GitHub\OrchestratorManager\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D16476D5-E3A2-43E1-9B4F-F3BD8CBF6BF9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{391BC970-942E-4B9F-8E9B-4F6B66FF839F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="450" uniqueCount="419">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="474" uniqueCount="443">
   <si>
     <t>Name</t>
   </si>
@@ -50,21 +50,29 @@
   </si>
   <si>
     <t>URL of the Orchestrator instance to be used. 
-Sample value: https://myOrchestratorURL.
-UiPath Cloud Platform (https://platform.uipath.com) is currently not supported.</t>
-  </si>
-  <si>
-    <t>OrchestratorTenant</t>
-  </si>
-  <si>
-    <t>Default</t>
+This parameter is exclusive to on-premises Orchestrator instances.
+Sample value: https://myOrchestratorURL.</t>
+  </si>
+  <si>
+    <t>TenantName</t>
   </si>
   <si>
     <t>Name of the tenant to be used. 
 Sample value: Default.</t>
   </si>
   <si>
+    <t>AccountName</t>
+  </si>
+  <si>
+    <t>Unique site URL for Cloud Platform organization.
+This parameter is exclusive to Cloud Platform Orchestrator instances.
+Sample value: MyAccount (assuming the organization account URL is https://platform.uipath.com/MyAccount).</t>
+  </si>
+  <si>
     <t>EntitiesWorkbooksFolderPath</t>
+  </si>
+  <si>
+    <t>Workbooks</t>
   </si>
   <si>
     <t>Path to the folder that contains entities workbooks. 
@@ -108,6 +116,24 @@
     <t>Interval (in milliseconds) between retries of making a HTTP request.</t>
   </si>
   <si>
+    <t>CloudPlatformAuthenticationURL</t>
+  </si>
+  <si>
+    <t>https://account.uipath.com/oauth/token</t>
+  </si>
+  <si>
+    <t>URL used to authenticate to UiPath Cloud Platform.</t>
+  </si>
+  <si>
+    <t>CloudPlatformURL</t>
+  </si>
+  <si>
+    <t>https://platform.uipath.com/</t>
+  </si>
+  <si>
+    <t>URL of UiPath Cloud Platform.</t>
+  </si>
+  <si>
     <t>ControlPanelTemplatePath</t>
   </si>
   <si>
@@ -387,7 +413,52 @@
     <t>Orchestrator URL</t>
   </si>
   <si>
-    <t>FormOrchestratorTenantLabel</t>
+    <t>FormOnPremisesOrchestratorLabel</t>
+  </si>
+  <si>
+    <t>On-Premises</t>
+  </si>
+  <si>
+    <t>オンプレミス</t>
+  </si>
+  <si>
+    <t>FormCloudOrchestratorLabel</t>
+  </si>
+  <si>
+    <t>Cloud</t>
+  </si>
+  <si>
+    <t>クラウド</t>
+  </si>
+  <si>
+    <t>FormUserKeyLabel</t>
+  </si>
+  <si>
+    <t>User Key</t>
+  </si>
+  <si>
+    <t>ユーザー キー</t>
+  </si>
+  <si>
+    <t>FormAccountNameLabel</t>
+  </si>
+  <si>
+    <t>Account Name</t>
+  </si>
+  <si>
+    <t>アカウントの論理名</t>
+  </si>
+  <si>
+    <t>FormClientIDLabel</t>
+  </si>
+  <si>
+    <t>Client Id</t>
+  </si>
+  <si>
+    <t>クライアント ID</t>
+  </si>
+  <si>
+    <t>FormTenantNameLabel</t>
   </si>
   <si>
     <t>Tenant Name</t>
@@ -1293,10 +1364,13 @@
     <t>パッケージバージョンが指定されませんでした。</t>
   </si>
   <si>
-    <t>Workbooks</t>
-  </si>
-  <si>
     <t>https://myOrchestratorURL</t>
+  </si>
+  <si>
+    <t>Default</t>
+  </si>
+  <si>
+    <t>MyAccount</t>
   </si>
 </sst>
 </file>
@@ -1341,9 +1415,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1367,8 +1442,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table14" displayName="Table14" ref="A1:C4" totalsRowShown="0">
-  <autoFilter ref="A1:C4" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table14" displayName="Table14" ref="A1:C5" totalsRowShown="0">
+  <autoFilter ref="A1:C5" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Name"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Value"/>
@@ -1379,8 +1454,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table1" displayName="Table1" ref="A1:C43" totalsRowShown="0">
-  <autoFilter ref="A1:C43" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table1" displayName="Table1" ref="A1:C45" totalsRowShown="0">
+  <autoFilter ref="A1:C45" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Name"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Value"/>
@@ -1391,8 +1466,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table13" displayName="Table13" ref="A1:C116" totalsRowShown="0">
-  <autoFilter ref="A1:C116" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table13" displayName="Table13" ref="A1:C121" totalsRowShown="0">
+  <autoFilter ref="A1:C121" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Name"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="EN"/>
@@ -1665,7 +1740,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D89C9C48-5454-47C4-AB1D-448E4519251A}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -1693,33 +1768,44 @@
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>418</v>
-      </c>
-      <c r="C2" s="2" t="s">
+      <c r="B2" s="4" t="s">
+        <v>440</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" ht="43.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>441</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="2" t="s">
+    </row>
+    <row r="4" spans="1:3" ht="72.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="1" t="s">
+      <c r="B4" s="1" t="s">
+        <v>442</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>417</v>
-      </c>
-      <c r="C4" s="2" t="s">
+    </row>
+    <row r="5" spans="1:3" ht="43.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="1" t="s">
         <v>9</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -1736,7 +1822,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C43"/>
+  <dimension ref="A1:C45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -1762,478 +1848,504 @@
     </row>
     <row r="2" spans="1:3" ht="101.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B2" s="1">
         <v>200</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>11</v>
+      <c r="C2" s="3" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B3" s="1">
         <v>0</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>13</v>
+      <c r="C3" s="3" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B4" s="1">
         <v>500</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>15</v>
+      <c r="C4" s="3" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B5" s="1">
         <v>600</v>
       </c>
-      <c r="C5" s="2" t="s">
-        <v>17</v>
+      <c r="C5" s="3" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B6" s="1">
         <v>3</v>
       </c>
-      <c r="C6" s="2" t="s">
-        <v>19</v>
+      <c r="C6" s="3" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B7" s="1">
         <v>5000</v>
       </c>
-      <c r="C7" s="2" t="s">
-        <v>21</v>
+      <c r="C7" s="3" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C8" s="2" t="s">
         <v>24</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C9" s="2" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B9" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+        <v>34</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
+        <v>40</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
+        <v>43</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+        <v>46</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+        <v>49</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>50</v>
+        <v>52</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C18" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A19" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B19" s="1" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>55</v>
+      <c r="C19" s="3" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>52</v>
+        <v>49</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>58</v>
+        <v>62</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C22" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C22" s="3" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="C23" s="2" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C23" s="3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
+        <v>49</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>67</v>
+        <v>62</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
+        <v>49</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
+        <v>74</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>75</v>
+        <v>77</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>77</v>
+        <v>52</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A30" s="1" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>79</v>
+        <v>82</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" s="1" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>81</v>
+        <v>49</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A32" s="1" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="C32" s="2" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
+        <v>74</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" s="1" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="C33" s="2" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
+        <v>77</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A34" s="1" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="C34" s="2" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
+        <v>74</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A35" s="1" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C35" s="2" t="s">
-        <v>89</v>
+        <v>52</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A36" s="1" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C36" s="2" t="s">
-        <v>91</v>
+        <v>55</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="37" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A37" s="1" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="C37" s="2" t="s">
-        <v>93</v>
+        <v>49</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="38" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A38" s="1" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="C38" s="2" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
+        <v>49</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A39" s="1" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C39" s="2" t="s">
-        <v>97</v>
+        <v>55</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A40" s="1" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="C40" s="2" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
+        <v>55</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A41" s="1" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C41" s="2" t="s">
-        <v>101</v>
+        <v>49</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="42" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A42" s="1" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="C42" s="2" t="s">
-        <v>103</v>
+        <v>62</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="43" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A43" s="1" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="C43" s="2" t="s">
-        <v>105</v>
+        <v>49</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A44" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C44" s="3" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A45" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C45" s="3" t="s">
+        <v>113</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B8" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="B9" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId4"/>
   </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1927ABA9-1814-4487-9CEC-ABDCAF91481F}">
-  <dimension ref="A1:C116"/>
+  <dimension ref="A1:C121"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -2251,1186 +2363,1241 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>106</v>
+        <v>114</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>107</v>
+        <v>115</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>109</v>
+        <v>116</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="43.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>112</v>
+        <v>118</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>114</v>
+        <v>121</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>117</v>
+        <v>123</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>120</v>
+        <v>126</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>123</v>
+        <v>129</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>126</v>
+        <v>132</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>129</v>
+        <v>135</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>132</v>
+        <v>138</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>135</v>
+        <v>141</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>138</v>
+        <v>144</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>141</v>
+        <v>147</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>149</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>144</v>
+        <v>150</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>147</v>
+        <v>153</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>155</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>150</v>
+        <v>156</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>153</v>
+        <v>159</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>161</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>155</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>155</v>
+        <v>162</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>158</v>
+        <v>165</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>167</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
+      <c r="A20" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>170</v>
+      </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>161</v>
+        <v>171</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>173</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>163</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>164</v>
+        <v>174</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>176</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>166</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>167</v>
+        <v>177</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>178</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>169</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>170</v>
+        <v>179</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>181</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A25" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>172</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>173</v>
-      </c>
+      <c r="B25" s="3"/>
+      <c r="C25" s="3"/>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>176</v>
+        <v>182</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>184</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B27" s="2"/>
-      <c r="C27" s="2"/>
+      <c r="A27" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>187</v>
+      </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="s">
-        <v>177</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>178</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>179</v>
+        <v>188</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>190</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="s">
-        <v>180</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>181</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>182</v>
+        <v>191</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>193</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A30" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>184</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>185</v>
+        <v>194</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>196</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A31" s="1" t="s">
-        <v>186</v>
-      </c>
-      <c r="B31" s="2" t="s">
-        <v>187</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>188</v>
+        <v>197</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>199</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A32" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="B32" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="C32" s="2" t="s">
-        <v>191</v>
-      </c>
+      <c r="B32" s="3"/>
+      <c r="C32" s="3"/>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A33" s="1" t="s">
-        <v>192</v>
-      </c>
-      <c r="B33" s="2" t="s">
-        <v>193</v>
-      </c>
-      <c r="C33" s="2" t="s">
-        <v>194</v>
+        <v>200</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>202</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A34" s="1" t="s">
-        <v>195</v>
-      </c>
-      <c r="B34" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="C34" s="2" t="s">
-        <v>197</v>
+        <v>203</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>204</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>205</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A35" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="B35" s="2" t="s">
-        <v>199</v>
-      </c>
-      <c r="C35" s="2" t="s">
-        <v>200</v>
+        <v>206</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>208</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A36" s="1" t="s">
-        <v>201</v>
-      </c>
-      <c r="B36" s="2" t="s">
-        <v>202</v>
-      </c>
-      <c r="C36" s="2" t="s">
-        <v>203</v>
+        <v>209</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>211</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A37" s="1" t="s">
-        <v>204</v>
-      </c>
-      <c r="B37" s="2" t="s">
-        <v>205</v>
-      </c>
-      <c r="C37" s="2" t="s">
-        <v>206</v>
+        <v>212</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>213</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>214</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A38" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="B38" s="2" t="s">
-        <v>208</v>
-      </c>
-      <c r="C38" s="2" t="s">
-        <v>209</v>
+        <v>215</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>217</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A39" s="1" t="s">
-        <v>210</v>
-      </c>
-      <c r="B39" s="2" t="s">
-        <v>211</v>
-      </c>
-      <c r="C39" s="2" t="s">
-        <v>212</v>
+        <v>218</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>220</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A40" s="1" t="s">
-        <v>213</v>
-      </c>
-      <c r="B40" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="C40" s="2" t="s">
-        <v>215</v>
+        <v>221</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>222</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>223</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A41" s="1" t="s">
-        <v>216</v>
-      </c>
-      <c r="B41" s="2" t="s">
-        <v>217</v>
-      </c>
-      <c r="C41" s="2" t="s">
-        <v>218</v>
+        <v>224</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>225</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>226</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A42" s="1" t="s">
-        <v>219</v>
-      </c>
-      <c r="B42" s="2" t="s">
-        <v>220</v>
-      </c>
-      <c r="C42" s="2" t="s">
-        <v>221</v>
+        <v>227</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>228</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>229</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A43" s="1" t="s">
-        <v>222</v>
-      </c>
-      <c r="B43" s="2" t="s">
-        <v>223</v>
-      </c>
-      <c r="C43" s="2" t="s">
-        <v>224</v>
+        <v>230</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>231</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>232</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A44" s="1" t="s">
-        <v>225</v>
-      </c>
-      <c r="B44" s="2" t="s">
-        <v>226</v>
-      </c>
-      <c r="C44" s="2" t="s">
-        <v>227</v>
+        <v>233</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>234</v>
+      </c>
+      <c r="C44" s="3" t="s">
+        <v>235</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A45" s="1" t="s">
-        <v>228</v>
-      </c>
-      <c r="B45" s="2" t="s">
-        <v>229</v>
-      </c>
-      <c r="C45" s="2" t="s">
-        <v>230</v>
+        <v>236</v>
+      </c>
+      <c r="B45" s="3" t="s">
+        <v>237</v>
+      </c>
+      <c r="C45" s="3" t="s">
+        <v>238</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A46" s="1" t="s">
-        <v>231</v>
-      </c>
-      <c r="B46" s="2" t="s">
-        <v>232</v>
-      </c>
-      <c r="C46" s="2" t="s">
-        <v>233</v>
+        <v>239</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>240</v>
+      </c>
+      <c r="C46" s="3" t="s">
+        <v>241</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A47" s="1" t="s">
-        <v>234</v>
-      </c>
-      <c r="B47" s="2" t="s">
-        <v>235</v>
-      </c>
-      <c r="C47" s="2" t="s">
-        <v>236</v>
+        <v>242</v>
+      </c>
+      <c r="B47" s="3" t="s">
+        <v>243</v>
+      </c>
+      <c r="C47" s="3" t="s">
+        <v>244</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A48" s="1" t="s">
-        <v>237</v>
-      </c>
-      <c r="B48" s="2" t="s">
-        <v>238</v>
-      </c>
-      <c r="C48" s="2" t="s">
-        <v>239</v>
+        <v>245</v>
+      </c>
+      <c r="B48" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="C48" s="3" t="s">
+        <v>247</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A49" s="1" t="s">
-        <v>240</v>
-      </c>
-      <c r="B49" s="2" t="s">
-        <v>241</v>
-      </c>
-      <c r="C49" s="2" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
+        <v>248</v>
+      </c>
+      <c r="B49" s="3" t="s">
+        <v>249</v>
+      </c>
+      <c r="C49" s="3" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A50" s="1" t="s">
-        <v>243</v>
-      </c>
-      <c r="B50" s="2" t="s">
-        <v>244</v>
-      </c>
-      <c r="C50" s="2" t="s">
-        <v>245</v>
+        <v>251</v>
+      </c>
+      <c r="B50" s="3" t="s">
+        <v>252</v>
+      </c>
+      <c r="C50" s="3" t="s">
+        <v>253</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A51" s="1" t="s">
-        <v>246</v>
-      </c>
-      <c r="B51" s="2" t="s">
-        <v>247</v>
-      </c>
-      <c r="C51" s="2" t="s">
-        <v>248</v>
+        <v>254</v>
+      </c>
+      <c r="B51" s="3" t="s">
+        <v>255</v>
+      </c>
+      <c r="C51" s="3" t="s">
+        <v>256</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A52" s="1" t="s">
-        <v>249</v>
-      </c>
-      <c r="B52" s="2" t="s">
-        <v>250</v>
-      </c>
-      <c r="C52" s="2" t="s">
-        <v>251</v>
+        <v>257</v>
+      </c>
+      <c r="B52" s="3" t="s">
+        <v>258</v>
+      </c>
+      <c r="C52" s="3" t="s">
+        <v>259</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A53" s="1" t="s">
-        <v>252</v>
-      </c>
-      <c r="B53" s="2" t="s">
-        <v>253</v>
-      </c>
-      <c r="C53" s="2" t="s">
-        <v>254</v>
+        <v>260</v>
+      </c>
+      <c r="B53" s="3" t="s">
+        <v>261</v>
+      </c>
+      <c r="C53" s="3" t="s">
+        <v>262</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A54" s="1" t="s">
-        <v>255</v>
-      </c>
-      <c r="B54" s="2" t="s">
-        <v>256</v>
-      </c>
-      <c r="C54" s="2" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.35">
+        <v>263</v>
+      </c>
+      <c r="B54" s="3" t="s">
+        <v>264</v>
+      </c>
+      <c r="C54" s="3" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A55" s="1" t="s">
-        <v>258</v>
-      </c>
-      <c r="B55" s="2" t="s">
-        <v>259</v>
-      </c>
-      <c r="C55" s="2" t="s">
-        <v>260</v>
+        <v>266</v>
+      </c>
+      <c r="B55" s="3" t="s">
+        <v>267</v>
+      </c>
+      <c r="C55" s="3" t="s">
+        <v>268</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A56" s="1" t="s">
-        <v>261</v>
-      </c>
-      <c r="B56" s="2" t="s">
-        <v>262</v>
-      </c>
-      <c r="C56" s="2" t="s">
-        <v>263</v>
+        <v>269</v>
+      </c>
+      <c r="B56" s="3" t="s">
+        <v>270</v>
+      </c>
+      <c r="C56" s="3" t="s">
+        <v>271</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A57" s="1" t="s">
-        <v>264</v>
-      </c>
-      <c r="B57" s="2" t="s">
-        <v>265</v>
-      </c>
-      <c r="C57" s="2" t="s">
-        <v>266</v>
+        <v>272</v>
+      </c>
+      <c r="B57" s="3" t="s">
+        <v>273</v>
+      </c>
+      <c r="C57" s="3" t="s">
+        <v>274</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A58" s="1" t="s">
-        <v>267</v>
-      </c>
-      <c r="B58" s="2" t="s">
-        <v>268</v>
-      </c>
-      <c r="C58" s="2" t="s">
-        <v>269</v>
+        <v>275</v>
+      </c>
+      <c r="B58" s="3" t="s">
+        <v>276</v>
+      </c>
+      <c r="C58" s="3" t="s">
+        <v>277</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B59" s="2"/>
-      <c r="C59" s="2"/>
+      <c r="A59" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="B59" s="3" t="s">
+        <v>279</v>
+      </c>
+      <c r="C59" s="3" t="s">
+        <v>280</v>
+      </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A60" s="1" t="s">
-        <v>270</v>
-      </c>
-      <c r="B60" s="2" t="s">
-        <v>271</v>
-      </c>
-      <c r="C60" s="2" t="s">
-        <v>272</v>
+        <v>281</v>
+      </c>
+      <c r="B60" s="3" t="s">
+        <v>282</v>
+      </c>
+      <c r="C60" s="3" t="s">
+        <v>283</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A61" s="1" t="s">
-        <v>273</v>
-      </c>
-      <c r="B61" s="2" t="s">
-        <v>274</v>
-      </c>
-      <c r="C61" s="2" t="s">
-        <v>275</v>
+        <v>284</v>
+      </c>
+      <c r="B61" s="3" t="s">
+        <v>285</v>
+      </c>
+      <c r="C61" s="3" t="s">
+        <v>286</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A62" s="1" t="s">
-        <v>276</v>
-      </c>
-      <c r="B62" s="2" t="s">
-        <v>277</v>
-      </c>
-      <c r="C62" s="2" t="s">
-        <v>278</v>
+        <v>287</v>
+      </c>
+      <c r="B62" s="3" t="s">
+        <v>288</v>
+      </c>
+      <c r="C62" s="3" t="s">
+        <v>289</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A63" s="1" t="s">
-        <v>279</v>
-      </c>
-      <c r="B63" s="2" t="s">
-        <v>280</v>
-      </c>
-      <c r="C63" s="2" t="s">
-        <v>281</v>
+        <v>290</v>
+      </c>
+      <c r="B63" s="3" t="s">
+        <v>291</v>
+      </c>
+      <c r="C63" s="3" t="s">
+        <v>292</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A64" s="1" t="s">
-        <v>282</v>
-      </c>
-      <c r="B64" s="2" t="s">
-        <v>283</v>
-      </c>
-      <c r="C64" s="2" t="s">
-        <v>284</v>
-      </c>
+      <c r="B64" s="3"/>
+      <c r="C64" s="3"/>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A65" s="1" t="s">
-        <v>285</v>
-      </c>
-      <c r="B65" s="2" t="s">
-        <v>286</v>
-      </c>
-      <c r="C65" s="2" t="s">
-        <v>287</v>
+        <v>293</v>
+      </c>
+      <c r="B65" s="3" t="s">
+        <v>294</v>
+      </c>
+      <c r="C65" s="3" t="s">
+        <v>295</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A66" s="1" t="s">
-        <v>288</v>
-      </c>
-      <c r="B66" s="2" t="s">
-        <v>289</v>
-      </c>
-      <c r="C66" s="2" t="s">
-        <v>290</v>
+        <v>296</v>
+      </c>
+      <c r="B66" s="3" t="s">
+        <v>297</v>
+      </c>
+      <c r="C66" s="3" t="s">
+        <v>298</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A67" s="1" t="s">
-        <v>291</v>
-      </c>
-      <c r="B67" s="2" t="s">
-        <v>292</v>
-      </c>
-      <c r="C67" s="2" t="s">
-        <v>293</v>
+        <v>299</v>
+      </c>
+      <c r="B67" s="3" t="s">
+        <v>300</v>
+      </c>
+      <c r="C67" s="3" t="s">
+        <v>301</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B68" s="2"/>
-      <c r="C68" s="2"/>
+      <c r="A68" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="B68" s="3" t="s">
+        <v>303</v>
+      </c>
+      <c r="C68" s="3" t="s">
+        <v>304</v>
+      </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A69" s="1" t="s">
-        <v>294</v>
-      </c>
-      <c r="B69" s="2" t="s">
-        <v>295</v>
-      </c>
-      <c r="C69" s="2" t="s">
-        <v>296</v>
+        <v>305</v>
+      </c>
+      <c r="B69" s="3" t="s">
+        <v>306</v>
+      </c>
+      <c r="C69" s="3" t="s">
+        <v>307</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A70" s="1" t="s">
-        <v>297</v>
-      </c>
-      <c r="B70" s="2" t="s">
-        <v>298</v>
-      </c>
-      <c r="C70" s="2" t="s">
-        <v>299</v>
+        <v>308</v>
+      </c>
+      <c r="B70" s="3" t="s">
+        <v>309</v>
+      </c>
+      <c r="C70" s="3" t="s">
+        <v>310</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A71" s="1" t="s">
-        <v>300</v>
-      </c>
-      <c r="B71" s="2" t="s">
-        <v>301</v>
-      </c>
-      <c r="C71" s="2" t="s">
-        <v>302</v>
+        <v>311</v>
+      </c>
+      <c r="B71" s="3" t="s">
+        <v>312</v>
+      </c>
+      <c r="C71" s="3" t="s">
+        <v>313</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A72" s="1" t="s">
-        <v>303</v>
-      </c>
-      <c r="B72" s="2" t="s">
-        <v>304</v>
-      </c>
-      <c r="C72" s="2" t="s">
-        <v>305</v>
+        <v>314</v>
+      </c>
+      <c r="B72" s="3" t="s">
+        <v>315</v>
+      </c>
+      <c r="C72" s="3" t="s">
+        <v>316</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A73" s="1" t="s">
-        <v>306</v>
-      </c>
-      <c r="B73" s="2" t="s">
-        <v>307</v>
-      </c>
-      <c r="C73" s="2" t="s">
-        <v>308</v>
-      </c>
+      <c r="B73" s="3"/>
+      <c r="C73" s="3"/>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A74" s="1" t="s">
-        <v>309</v>
-      </c>
-      <c r="B74" s="2" t="s">
-        <v>310</v>
-      </c>
-      <c r="C74" s="2" t="s">
-        <v>311</v>
+        <v>317</v>
+      </c>
+      <c r="B74" s="3" t="s">
+        <v>318</v>
+      </c>
+      <c r="C74" s="3" t="s">
+        <v>319</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A75" s="1" t="s">
-        <v>312</v>
-      </c>
-      <c r="B75" s="2" t="s">
-        <v>313</v>
-      </c>
-      <c r="C75" s="2" t="s">
-        <v>314</v>
+        <v>320</v>
+      </c>
+      <c r="B75" s="3" t="s">
+        <v>321</v>
+      </c>
+      <c r="C75" s="3" t="s">
+        <v>322</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A76" s="1" t="s">
-        <v>315</v>
-      </c>
-      <c r="B76" s="2" t="s">
-        <v>316</v>
-      </c>
-      <c r="C76" s="2" t="s">
-        <v>317</v>
+        <v>323</v>
+      </c>
+      <c r="B76" s="3" t="s">
+        <v>324</v>
+      </c>
+      <c r="C76" s="3" t="s">
+        <v>325</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A77" s="1" t="s">
-        <v>318</v>
-      </c>
-      <c r="B77" s="2" t="s">
-        <v>319</v>
-      </c>
-      <c r="C77" s="2" t="s">
-        <v>320</v>
+        <v>326</v>
+      </c>
+      <c r="B77" s="3" t="s">
+        <v>327</v>
+      </c>
+      <c r="C77" s="3" t="s">
+        <v>328</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B78" s="2"/>
-      <c r="C78" s="2"/>
+      <c r="A78" s="1" t="s">
+        <v>329</v>
+      </c>
+      <c r="B78" s="3" t="s">
+        <v>330</v>
+      </c>
+      <c r="C78" s="3" t="s">
+        <v>331</v>
+      </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A79" s="1" t="s">
-        <v>321</v>
-      </c>
-      <c r="B79" s="2" t="s">
-        <v>322</v>
-      </c>
-      <c r="C79" s="2" t="s">
-        <v>323</v>
+        <v>332</v>
+      </c>
+      <c r="B79" s="3" t="s">
+        <v>333</v>
+      </c>
+      <c r="C79" s="3" t="s">
+        <v>334</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A80" s="1" t="s">
-        <v>324</v>
-      </c>
-      <c r="B80" s="2" t="s">
-        <v>325</v>
-      </c>
-      <c r="C80" s="2" t="s">
-        <v>326</v>
+        <v>335</v>
+      </c>
+      <c r="B80" s="3" t="s">
+        <v>336</v>
+      </c>
+      <c r="C80" s="3" t="s">
+        <v>337</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A81" s="1" t="s">
-        <v>327</v>
-      </c>
-      <c r="B81" s="2" t="s">
-        <v>328</v>
-      </c>
-      <c r="C81" s="2" t="s">
-        <v>329</v>
+        <v>338</v>
+      </c>
+      <c r="B81" s="3" t="s">
+        <v>339</v>
+      </c>
+      <c r="C81" s="3" t="s">
+        <v>340</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A82" s="1" t="s">
-        <v>330</v>
-      </c>
-      <c r="B82" s="2" t="s">
-        <v>331</v>
-      </c>
-      <c r="C82" s="2" t="s">
-        <v>332</v>
+        <v>341</v>
+      </c>
+      <c r="B82" s="3" t="s">
+        <v>342</v>
+      </c>
+      <c r="C82" s="3" t="s">
+        <v>343</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A83" s="1" t="s">
-        <v>333</v>
-      </c>
-      <c r="B83" s="2" t="s">
-        <v>334</v>
-      </c>
-      <c r="C83" s="2" t="s">
-        <v>335</v>
-      </c>
+      <c r="B83" s="3"/>
+      <c r="C83" s="3"/>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A84" s="1" t="s">
-        <v>336</v>
-      </c>
-      <c r="B84" s="2" t="s">
-        <v>337</v>
-      </c>
-      <c r="C84" s="2" t="s">
-        <v>338</v>
+        <v>344</v>
+      </c>
+      <c r="B84" s="3" t="s">
+        <v>345</v>
+      </c>
+      <c r="C84" s="3" t="s">
+        <v>346</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A85" s="1" t="s">
-        <v>339</v>
-      </c>
-      <c r="B85" s="2" t="s">
-        <v>340</v>
-      </c>
-      <c r="C85" s="2" t="s">
-        <v>341</v>
+        <v>347</v>
+      </c>
+      <c r="B85" s="3" t="s">
+        <v>348</v>
+      </c>
+      <c r="C85" s="3" t="s">
+        <v>349</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A86" s="1" t="s">
-        <v>342</v>
-      </c>
-      <c r="B86" s="2" t="s">
-        <v>343</v>
-      </c>
-      <c r="C86" s="2" t="s">
-        <v>344</v>
+        <v>350</v>
+      </c>
+      <c r="B86" s="3" t="s">
+        <v>351</v>
+      </c>
+      <c r="C86" s="3" t="s">
+        <v>352</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B87" s="2"/>
-      <c r="C87" s="2"/>
+      <c r="A87" s="1" t="s">
+        <v>353</v>
+      </c>
+      <c r="B87" s="3" t="s">
+        <v>354</v>
+      </c>
+      <c r="C87" s="3" t="s">
+        <v>355</v>
+      </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A88" s="1" t="s">
-        <v>345</v>
-      </c>
-      <c r="B88" s="2" t="s">
-        <v>346</v>
-      </c>
-      <c r="C88" s="2" t="s">
-        <v>347</v>
+        <v>356</v>
+      </c>
+      <c r="B88" s="3" t="s">
+        <v>357</v>
+      </c>
+      <c r="C88" s="3" t="s">
+        <v>358</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A89" s="1" t="s">
-        <v>348</v>
-      </c>
-      <c r="B89" s="2" t="s">
-        <v>349</v>
-      </c>
-      <c r="C89" s="2" t="s">
-        <v>350</v>
+        <v>359</v>
+      </c>
+      <c r="B89" s="3" t="s">
+        <v>360</v>
+      </c>
+      <c r="C89" s="3" t="s">
+        <v>361</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A90" s="1" t="s">
-        <v>351</v>
-      </c>
-      <c r="B90" s="2" t="s">
-        <v>352</v>
-      </c>
-      <c r="C90" s="2" t="s">
-        <v>353</v>
+        <v>362</v>
+      </c>
+      <c r="B90" s="3" t="s">
+        <v>363</v>
+      </c>
+      <c r="C90" s="3" t="s">
+        <v>364</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A91" s="1" t="s">
-        <v>354</v>
-      </c>
-      <c r="B91" s="2" t="s">
-        <v>355</v>
-      </c>
-      <c r="C91" s="2" t="s">
-        <v>356</v>
-      </c>
+        <v>365</v>
+      </c>
+      <c r="B91" s="3" t="s">
+        <v>366</v>
+      </c>
+      <c r="C91" s="3" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B92" s="3"/>
+      <c r="C92" s="3"/>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A93" s="1" t="s">
-        <v>357</v>
-      </c>
-      <c r="B93" s="2" t="s">
-        <v>358</v>
-      </c>
-      <c r="C93" s="2" t="s">
-        <v>359</v>
+        <v>368</v>
+      </c>
+      <c r="B93" s="3" t="s">
+        <v>369</v>
+      </c>
+      <c r="C93" s="3" t="s">
+        <v>370</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A94" s="1" t="s">
-        <v>360</v>
-      </c>
-      <c r="B94" s="2" t="s">
-        <v>361</v>
-      </c>
-      <c r="C94" s="2" t="s">
-        <v>362</v>
+        <v>371</v>
+      </c>
+      <c r="B94" s="3" t="s">
+        <v>372</v>
+      </c>
+      <c r="C94" s="3" t="s">
+        <v>373</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A95" s="1" t="s">
-        <v>363</v>
-      </c>
-      <c r="B95" s="2" t="s">
-        <v>364</v>
-      </c>
-      <c r="C95" s="2" t="s">
-        <v>365</v>
+        <v>374</v>
+      </c>
+      <c r="B95" s="3" t="s">
+        <v>375</v>
+      </c>
+      <c r="C95" s="3" t="s">
+        <v>376</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A96" s="1" t="s">
-        <v>366</v>
-      </c>
-      <c r="B96" s="2" t="s">
-        <v>367</v>
-      </c>
-      <c r="C96" s="2" t="s">
-        <v>368</v>
-      </c>
-    </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A97" s="1" t="s">
-        <v>369</v>
-      </c>
-      <c r="B97" s="2" t="s">
-        <v>370</v>
-      </c>
-      <c r="C97" s="2" t="s">
-        <v>371</v>
+        <v>377</v>
+      </c>
+      <c r="B96" s="3" t="s">
+        <v>378</v>
+      </c>
+      <c r="C96" s="3" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A98" s="1" t="s">
+        <v>380</v>
+      </c>
+      <c r="B98" s="3" t="s">
+        <v>381</v>
+      </c>
+      <c r="C98" s="3" t="s">
+        <v>382</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A99" s="1" t="s">
-        <v>372</v>
-      </c>
-      <c r="B99" s="2" t="s">
-        <v>373</v>
-      </c>
-      <c r="C99" s="2" t="s">
-        <v>374</v>
+        <v>383</v>
+      </c>
+      <c r="B99" s="3" t="s">
+        <v>384</v>
+      </c>
+      <c r="C99" s="3" t="s">
+        <v>385</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A100" s="1" t="s">
-        <v>375</v>
-      </c>
-      <c r="B100" s="1" t="s">
-        <v>376</v>
-      </c>
-      <c r="C100" s="1" t="s">
-        <v>377</v>
+        <v>386</v>
+      </c>
+      <c r="B100" s="3" t="s">
+        <v>387</v>
+      </c>
+      <c r="C100" s="3" t="s">
+        <v>388</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A101" s="1" t="s">
-        <v>378</v>
-      </c>
-      <c r="B101" s="1" t="s">
-        <v>379</v>
-      </c>
-      <c r="C101" s="1" t="s">
-        <v>380</v>
+        <v>389</v>
+      </c>
+      <c r="B101" s="3" t="s">
+        <v>390</v>
+      </c>
+      <c r="C101" s="3" t="s">
+        <v>391</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A102" s="1" t="s">
-        <v>381</v>
-      </c>
-      <c r="B102" s="2" t="s">
-        <v>382</v>
-      </c>
-      <c r="C102" s="1" t="s">
-        <v>383</v>
-      </c>
-    </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A103" s="1" t="s">
-        <v>384</v>
-      </c>
-      <c r="B103" s="1" t="s">
-        <v>385</v>
-      </c>
-      <c r="C103" s="1" t="s">
-        <v>386</v>
+        <v>392</v>
+      </c>
+      <c r="B102" s="3" t="s">
+        <v>393</v>
+      </c>
+      <c r="C102" s="3" t="s">
+        <v>394</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A104" s="1" t="s">
-        <v>387</v>
-      </c>
-      <c r="B104" s="2" t="s">
-        <v>388</v>
-      </c>
-      <c r="C104" s="2" t="s">
-        <v>389</v>
+        <v>395</v>
+      </c>
+      <c r="B104" s="3" t="s">
+        <v>396</v>
+      </c>
+      <c r="C104" s="3" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A105" s="1" t="s">
+        <v>398</v>
+      </c>
+      <c r="B105" s="1" t="s">
+        <v>399</v>
+      </c>
+      <c r="C105" s="1" t="s">
+        <v>400</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A106" s="1" t="s">
-        <v>390</v>
-      </c>
-      <c r="B106" s="2" t="s">
-        <v>391</v>
-      </c>
-      <c r="C106" s="2" t="s">
-        <v>392</v>
+        <v>401</v>
+      </c>
+      <c r="B106" s="1" t="s">
+        <v>402</v>
+      </c>
+      <c r="C106" s="1" t="s">
+        <v>403</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A107" s="1" t="s">
-        <v>393</v>
-      </c>
-      <c r="B107" s="2" t="s">
-        <v>394</v>
-      </c>
-      <c r="C107" s="2" t="s">
-        <v>395</v>
+        <v>404</v>
+      </c>
+      <c r="B107" s="3" t="s">
+        <v>405</v>
+      </c>
+      <c r="C107" s="1" t="s">
+        <v>406</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B108" s="2"/>
-      <c r="C108" s="2"/>
+      <c r="A108" s="1" t="s">
+        <v>407</v>
+      </c>
+      <c r="B108" s="1" t="s">
+        <v>408</v>
+      </c>
+      <c r="C108" s="1" t="s">
+        <v>409</v>
+      </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A109" s="1" t="s">
-        <v>396</v>
-      </c>
-      <c r="B109" s="2" t="s">
-        <v>397</v>
-      </c>
-      <c r="C109" s="2" t="s">
-        <v>398</v>
-      </c>
-    </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A110" s="1" t="s">
-        <v>399</v>
-      </c>
-      <c r="B110" s="2" t="s">
-        <v>400</v>
-      </c>
-      <c r="C110" s="2" t="s">
-        <v>401</v>
+        <v>410</v>
+      </c>
+      <c r="B109" s="3" t="s">
+        <v>411</v>
+      </c>
+      <c r="C109" s="3" t="s">
+        <v>412</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A111" s="1" t="s">
-        <v>402</v>
-      </c>
-      <c r="B111" s="2" t="s">
-        <v>403</v>
-      </c>
-      <c r="C111" s="2" t="s">
-        <v>404</v>
+        <v>413</v>
+      </c>
+      <c r="B111" s="3" t="s">
+        <v>414</v>
+      </c>
+      <c r="C111" s="3" t="s">
+        <v>415</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A112" s="1" t="s">
-        <v>405</v>
-      </c>
-      <c r="B112" s="2" t="s">
-        <v>406</v>
-      </c>
-      <c r="C112" s="2" t="s">
-        <v>407</v>
+        <v>416</v>
+      </c>
+      <c r="B112" s="3" t="s">
+        <v>417</v>
+      </c>
+      <c r="C112" s="3" t="s">
+        <v>418</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A113" s="1" t="s">
-        <v>408</v>
-      </c>
-      <c r="B113" s="2" t="s">
-        <v>409</v>
-      </c>
-      <c r="C113" s="2" t="s">
-        <v>410</v>
-      </c>
+      <c r="B113" s="3"/>
+      <c r="C113" s="3"/>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B114" s="2"/>
-      <c r="C114" s="2"/>
+      <c r="A114" s="1" t="s">
+        <v>419</v>
+      </c>
+      <c r="B114" s="3" t="s">
+        <v>420</v>
+      </c>
+      <c r="C114" s="3" t="s">
+        <v>421</v>
+      </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A115" s="1" t="s">
-        <v>411</v>
-      </c>
-      <c r="B115" s="2" t="s">
-        <v>412</v>
-      </c>
-      <c r="C115" s="2" t="s">
-        <v>413</v>
+        <v>422</v>
+      </c>
+      <c r="B115" s="3" t="s">
+        <v>423</v>
+      </c>
+      <c r="C115" s="3" t="s">
+        <v>424</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A116" s="1" t="s">
-        <v>414</v>
-      </c>
-      <c r="B116" s="2" t="s">
-        <v>415</v>
-      </c>
-      <c r="C116" s="2" t="s">
-        <v>416</v>
+        <v>425</v>
+      </c>
+      <c r="B116" s="3" t="s">
+        <v>426</v>
+      </c>
+      <c r="C116" s="3" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A117" s="1" t="s">
+        <v>428</v>
+      </c>
+      <c r="B117" s="3" t="s">
+        <v>429</v>
+      </c>
+      <c r="C117" s="3" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A118" s="1" t="s">
+        <v>431</v>
+      </c>
+      <c r="B118" s="3" t="s">
+        <v>432</v>
+      </c>
+      <c r="C118" s="3" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B119" s="3"/>
+      <c r="C119" s="3"/>
+    </row>
+    <row r="120" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A120" s="1" t="s">
+        <v>434</v>
+      </c>
+      <c r="B120" s="3" t="s">
+        <v>435</v>
+      </c>
+      <c r="C120" s="3" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A121" s="1" t="s">
+        <v>437</v>
+      </c>
+      <c r="B121" s="3" t="s">
+        <v>438</v>
+      </c>
+      <c r="C121" s="3" t="s">
+        <v>439</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Implement manipulation of Organization Units
</commit_message>
<xml_diff>
--- a/Config.xlsx
+++ b/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mateus.cruz\Documents\GitHub\OrchestratorManager\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{391BC970-942E-4B9F-8E9B-4F6B66FF839F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7B0C459-3890-4A03-AD44-C48021E1C725}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="474" uniqueCount="443">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="489" uniqueCount="454">
   <si>
     <t>Name</t>
   </si>
@@ -57,6 +57,9 @@
     <t>TenantName</t>
   </si>
   <si>
+    <t>Default</t>
+  </si>
+  <si>
     <t>Name of the tenant to be used. 
 Sample value: Default.</t>
   </si>
@@ -72,9 +75,6 @@
     <t>EntitiesWorkbooksFolderPath</t>
   </si>
   <si>
-    <t>Workbooks</t>
-  </si>
-  <si>
     <t>Path to the folder that contains entities workbooks. 
 Sample value: C:\Users\MyUser\Desktop\Workbooks</t>
   </si>
@@ -386,6 +386,24 @@
     <t>Column to which the result of the Rollback Process to Previous Package Version operation should be written.</t>
   </si>
   <si>
+    <t>CreateOrganizationUnitIDColumn</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>CreateOrganizationUnitResultColumn</t>
+  </si>
+  <si>
+    <t>Column to which the result of the Create Organization Unit operation should be written.</t>
+  </si>
+  <si>
+    <t>DeleteOrganizationUnitResultColumn</t>
+  </si>
+  <si>
+    <t>Column to which the result of the Delete Organization Unit operation should be written.</t>
+  </si>
+  <si>
     <t>EN</t>
   </si>
   <si>
@@ -575,6 +593,12 @@
     <t>プロセス</t>
   </si>
   <si>
+    <t>FormOrganizationUnitOption</t>
+  </si>
+  <si>
+    <t>Organiztion Unit</t>
+  </si>
+  <si>
     <t>FormSubmitButton</t>
   </si>
   <si>
@@ -644,6 +668,15 @@
     <t>JA\プロセス.xlsx</t>
   </si>
   <si>
+    <t>OrganizationUnitConfigFilePath</t>
+  </si>
+  <si>
+    <t>EN\OrganizationUnits.xlsx</t>
+  </si>
+  <si>
+    <t>JA\組織単位.xlsx</t>
+  </si>
+  <si>
     <t>GetOperationName</t>
   </si>
   <si>
@@ -1367,10 +1400,10 @@
     <t>https://myOrchestratorURL</t>
   </si>
   <si>
-    <t>Default</t>
-  </si>
-  <si>
     <t>MyAccount</t>
+  </si>
+  <si>
+    <t>Workbooks</t>
   </si>
 </sst>
 </file>
@@ -1454,8 +1487,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table1" displayName="Table1" ref="A1:C45" totalsRowShown="0">
-  <autoFilter ref="A1:C45" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table1" displayName="Table1" ref="A1:C48" totalsRowShown="0">
+  <autoFilter ref="A1:C48" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Name"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Value"/>
@@ -1466,8 +1499,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table13" displayName="Table13" ref="A1:C121" totalsRowShown="0">
-  <autoFilter ref="A1:C121" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table13" displayName="Table13" ref="A1:C123" totalsRowShown="0">
+  <autoFilter ref="A1:C123" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Name"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="EN"/>
@@ -1769,7 +1802,7 @@
         <v>3</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>440</v>
+        <v>451</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>4</v>
@@ -1780,29 +1813,29 @@
         <v>5</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>441</v>
+        <v>6</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="72.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>442</v>
+        <v>452</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="43.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>10</v>
+        <v>453</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>11</v>
@@ -1822,7 +1855,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C45"/>
+  <dimension ref="A1:C48"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -2330,6 +2363,39 @@
         <v>113</v>
       </c>
     </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A46" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="C46" s="3" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A47" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C47" s="3" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A48" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C48" s="3" t="s">
+        <v>119</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B8" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
@@ -2345,7 +2411,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1927ABA9-1814-4487-9CEC-ABDCAF91481F}">
-  <dimension ref="A1:C121"/>
+  <dimension ref="A1:C123"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -2363,1241 +2429,1263 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>114</v>
+        <v>120</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>115</v>
+        <v>121</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>116</v>
+        <v>122</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>117</v>
+        <v>123</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>117</v>
+        <v>123</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="43.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>118</v>
+        <v>124</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>119</v>
+        <v>125</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>120</v>
+        <v>126</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>121</v>
+        <v>127</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>122</v>
+        <v>128</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>122</v>
+        <v>128</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>123</v>
+        <v>129</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>124</v>
+        <v>130</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>125</v>
+        <v>131</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
-        <v>126</v>
+        <v>132</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>127</v>
+        <v>133</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>128</v>
+        <v>134</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
-        <v>129</v>
+        <v>135</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>130</v>
+        <v>136</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>131</v>
+        <v>137</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
-        <v>132</v>
+        <v>138</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>133</v>
+        <v>139</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>134</v>
+        <v>140</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
-        <v>135</v>
+        <v>141</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>136</v>
+        <v>142</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>137</v>
+        <v>143</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
-        <v>138</v>
+        <v>144</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>139</v>
+        <v>145</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>140</v>
+        <v>146</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
-        <v>141</v>
+        <v>147</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>142</v>
+        <v>148</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>143</v>
+        <v>149</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
-        <v>144</v>
+        <v>150</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>145</v>
+        <v>151</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>146</v>
+        <v>152</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
-        <v>147</v>
+        <v>153</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>148</v>
+        <v>154</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>149</v>
+        <v>155</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
-        <v>150</v>
+        <v>156</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>151</v>
+        <v>157</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>152</v>
+        <v>158</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
-        <v>153</v>
+        <v>159</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>154</v>
+        <v>160</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>155</v>
+        <v>161</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
-        <v>156</v>
+        <v>162</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>157</v>
+        <v>163</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>158</v>
+        <v>164</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
-        <v>159</v>
+        <v>165</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>160</v>
+        <v>166</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>161</v>
+        <v>167</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
-        <v>162</v>
+        <v>168</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>163</v>
+        <v>169</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>164</v>
+        <v>170</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
-        <v>165</v>
+        <v>171</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>166</v>
+        <v>172</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>167</v>
+        <v>173</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
-        <v>168</v>
+        <v>174</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>169</v>
+        <v>175</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>170</v>
+        <v>176</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
-        <v>171</v>
+        <v>177</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>172</v>
+        <v>178</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>173</v>
+        <v>179</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>175</v>
+        <v>181</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>176</v>
+        <v>182</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
-        <v>177</v>
+        <v>183</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>178</v>
+        <v>184</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>178</v>
+        <v>164</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
-        <v>179</v>
+        <v>185</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>180</v>
+        <v>186</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>181</v>
+        <v>186</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B25" s="3"/>
-      <c r="C25" s="3"/>
+      <c r="A25" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>189</v>
+      </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A26" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="B26" s="3" t="s">
-        <v>183</v>
-      </c>
-      <c r="C26" s="3" t="s">
-        <v>184</v>
-      </c>
+      <c r="B26" s="3"/>
+      <c r="C26" s="3"/>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
-        <v>185</v>
+        <v>190</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>186</v>
+        <v>191</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>187</v>
+        <v>192</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="s">
-        <v>188</v>
+        <v>193</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>189</v>
+        <v>194</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>190</v>
+        <v>195</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="s">
-        <v>191</v>
+        <v>196</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>192</v>
+        <v>197</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>193</v>
+        <v>198</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A30" s="1" t="s">
-        <v>194</v>
+        <v>199</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>195</v>
+        <v>200</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>196</v>
+        <v>201</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A31" s="1" t="s">
-        <v>197</v>
+        <v>202</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>198</v>
+        <v>203</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>199</v>
+        <v>204</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B32" s="3"/>
-      <c r="C32" s="3"/>
+      <c r="A32" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>207</v>
+      </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A33" s="1" t="s">
-        <v>200</v>
+        <v>208</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>201</v>
+        <v>209</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>202</v>
+        <v>210</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A34" s="1" t="s">
-        <v>203</v>
-      </c>
-      <c r="B34" s="3" t="s">
-        <v>204</v>
-      </c>
-      <c r="C34" s="3" t="s">
-        <v>205</v>
-      </c>
+      <c r="B34" s="3"/>
+      <c r="C34" s="3"/>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A35" s="1" t="s">
-        <v>206</v>
+        <v>211</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>207</v>
+        <v>212</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>208</v>
+        <v>213</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A36" s="1" t="s">
-        <v>209</v>
+        <v>214</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>210</v>
+        <v>215</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A37" s="1" t="s">
-        <v>212</v>
+        <v>217</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>213</v>
+        <v>218</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>214</v>
+        <v>219</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A38" s="1" t="s">
-        <v>215</v>
+        <v>220</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>216</v>
+        <v>221</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>217</v>
+        <v>222</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A39" s="1" t="s">
-        <v>218</v>
+        <v>223</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>219</v>
+        <v>224</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>220</v>
+        <v>225</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A40" s="1" t="s">
-        <v>221</v>
+        <v>226</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>222</v>
+        <v>227</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>223</v>
+        <v>228</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A41" s="1" t="s">
-        <v>224</v>
+        <v>229</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>225</v>
+        <v>230</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>226</v>
+        <v>231</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A42" s="1" t="s">
-        <v>227</v>
+        <v>232</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>228</v>
+        <v>233</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>229</v>
+        <v>234</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A43" s="1" t="s">
-        <v>230</v>
+        <v>235</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>231</v>
+        <v>236</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>232</v>
+        <v>237</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A44" s="1" t="s">
-        <v>233</v>
+        <v>238</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>234</v>
+        <v>239</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>235</v>
+        <v>240</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A45" s="1" t="s">
-        <v>236</v>
+        <v>241</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>237</v>
+        <v>242</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>238</v>
+        <v>243</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A46" s="1" t="s">
-        <v>239</v>
+        <v>244</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>240</v>
+        <v>245</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>241</v>
+        <v>246</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A47" s="1" t="s">
-        <v>242</v>
+        <v>247</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>243</v>
+        <v>248</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>244</v>
+        <v>249</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A48" s="1" t="s">
-        <v>245</v>
+        <v>250</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>246</v>
+        <v>251</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>247</v>
+        <v>252</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A49" s="1" t="s">
-        <v>248</v>
+        <v>253</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>249</v>
+        <v>254</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>250</v>
+        <v>255</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A50" s="1" t="s">
-        <v>251</v>
+        <v>256</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>252</v>
+        <v>257</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>253</v>
+        <v>258</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A51" s="1" t="s">
-        <v>254</v>
+        <v>259</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>255</v>
+        <v>260</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>256</v>
+        <v>261</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A52" s="1" t="s">
-        <v>257</v>
+        <v>262</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>258</v>
+        <v>263</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>259</v>
+        <v>264</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A53" s="1" t="s">
-        <v>260</v>
+        <v>265</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>261</v>
+        <v>266</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>262</v>
+        <v>267</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A54" s="1" t="s">
-        <v>263</v>
+        <v>268</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>264</v>
+        <v>269</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A55" s="1" t="s">
-        <v>266</v>
+        <v>271</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>267</v>
+        <v>272</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>268</v>
+        <v>273</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A56" s="1" t="s">
-        <v>269</v>
+        <v>274</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>270</v>
+        <v>275</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.35">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A57" s="1" t="s">
-        <v>272</v>
+        <v>277</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>273</v>
+        <v>278</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>274</v>
+        <v>279</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A58" s="1" t="s">
-        <v>275</v>
+        <v>280</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>276</v>
+        <v>281</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>277</v>
+        <v>282</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A59" s="1" t="s">
-        <v>278</v>
+        <v>283</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>279</v>
+        <v>284</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>280</v>
+        <v>285</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A60" s="1" t="s">
-        <v>281</v>
+        <v>286</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>282</v>
+        <v>287</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>283</v>
+        <v>288</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A61" s="1" t="s">
-        <v>284</v>
+        <v>289</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>285</v>
+        <v>290</v>
       </c>
       <c r="C61" s="3" t="s">
-        <v>286</v>
+        <v>291</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A62" s="1" t="s">
-        <v>287</v>
+        <v>292</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>288</v>
+        <v>293</v>
       </c>
       <c r="C62" s="3" t="s">
-        <v>289</v>
+        <v>294</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A63" s="1" t="s">
-        <v>290</v>
+        <v>295</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>291</v>
+        <v>296</v>
       </c>
       <c r="C63" s="3" t="s">
-        <v>292</v>
+        <v>297</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B64" s="3"/>
-      <c r="C64" s="3"/>
+      <c r="A64" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="B64" s="3" t="s">
+        <v>299</v>
+      </c>
+      <c r="C64" s="3" t="s">
+        <v>300</v>
+      </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A65" s="1" t="s">
-        <v>293</v>
+        <v>301</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>294</v>
+        <v>302</v>
       </c>
       <c r="C65" s="3" t="s">
-        <v>295</v>
+        <v>303</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A66" s="1" t="s">
-        <v>296</v>
-      </c>
-      <c r="B66" s="3" t="s">
-        <v>297</v>
-      </c>
-      <c r="C66" s="3" t="s">
-        <v>298</v>
-      </c>
+      <c r="B66" s="3"/>
+      <c r="C66" s="3"/>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A67" s="1" t="s">
-        <v>299</v>
+        <v>304</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>300</v>
+        <v>305</v>
       </c>
       <c r="C67" s="3" t="s">
-        <v>301</v>
+        <v>306</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A68" s="1" t="s">
-        <v>302</v>
+        <v>307</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>303</v>
+        <v>308</v>
       </c>
       <c r="C68" s="3" t="s">
-        <v>304</v>
+        <v>309</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A69" s="1" t="s">
-        <v>305</v>
+        <v>310</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>306</v>
+        <v>311</v>
       </c>
       <c r="C69" s="3" t="s">
-        <v>307</v>
+        <v>312</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A70" s="1" t="s">
-        <v>308</v>
+        <v>313</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>309</v>
+        <v>314</v>
       </c>
       <c r="C70" s="3" t="s">
-        <v>310</v>
+        <v>315</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A71" s="1" t="s">
-        <v>311</v>
+        <v>316</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>312</v>
+        <v>317</v>
       </c>
       <c r="C71" s="3" t="s">
-        <v>313</v>
+        <v>318</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A72" s="1" t="s">
-        <v>314</v>
+        <v>319</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>315</v>
+        <v>320</v>
       </c>
       <c r="C72" s="3" t="s">
-        <v>316</v>
+        <v>321</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B73" s="3"/>
-      <c r="C73" s="3"/>
+      <c r="A73" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="B73" s="3" t="s">
+        <v>323</v>
+      </c>
+      <c r="C73" s="3" t="s">
+        <v>324</v>
+      </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A74" s="1" t="s">
-        <v>317</v>
+        <v>325</v>
       </c>
       <c r="B74" s="3" t="s">
-        <v>318</v>
+        <v>326</v>
       </c>
       <c r="C74" s="3" t="s">
-        <v>319</v>
+        <v>327</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A75" s="1" t="s">
-        <v>320</v>
-      </c>
-      <c r="B75" s="3" t="s">
-        <v>321</v>
-      </c>
-      <c r="C75" s="3" t="s">
-        <v>322</v>
-      </c>
+      <c r="B75" s="3"/>
+      <c r="C75" s="3"/>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A76" s="1" t="s">
-        <v>323</v>
+        <v>328</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>324</v>
+        <v>329</v>
       </c>
       <c r="C76" s="3" t="s">
-        <v>325</v>
+        <v>330</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A77" s="1" t="s">
-        <v>326</v>
+        <v>331</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>327</v>
+        <v>332</v>
       </c>
       <c r="C77" s="3" t="s">
-        <v>328</v>
+        <v>333</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A78" s="1" t="s">
-        <v>329</v>
+        <v>334</v>
       </c>
       <c r="B78" s="3" t="s">
-        <v>330</v>
+        <v>335</v>
       </c>
       <c r="C78" s="3" t="s">
-        <v>331</v>
+        <v>336</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A79" s="1" t="s">
-        <v>332</v>
+        <v>337</v>
       </c>
       <c r="B79" s="3" t="s">
-        <v>333</v>
+        <v>338</v>
       </c>
       <c r="C79" s="3" t="s">
-        <v>334</v>
+        <v>339</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A80" s="1" t="s">
-        <v>335</v>
+        <v>340</v>
       </c>
       <c r="B80" s="3" t="s">
-        <v>336</v>
+        <v>341</v>
       </c>
       <c r="C80" s="3" t="s">
-        <v>337</v>
+        <v>342</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A81" s="1" t="s">
-        <v>338</v>
+        <v>343</v>
       </c>
       <c r="B81" s="3" t="s">
-        <v>339</v>
+        <v>344</v>
       </c>
       <c r="C81" s="3" t="s">
-        <v>340</v>
+        <v>345</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A82" s="1" t="s">
-        <v>341</v>
+        <v>346</v>
       </c>
       <c r="B82" s="3" t="s">
-        <v>342</v>
+        <v>347</v>
       </c>
       <c r="C82" s="3" t="s">
-        <v>343</v>
+        <v>348</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B83" s="3"/>
-      <c r="C83" s="3"/>
+      <c r="A83" s="1" t="s">
+        <v>349</v>
+      </c>
+      <c r="B83" s="3" t="s">
+        <v>350</v>
+      </c>
+      <c r="C83" s="3" t="s">
+        <v>351</v>
+      </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A84" s="1" t="s">
-        <v>344</v>
+        <v>352</v>
       </c>
       <c r="B84" s="3" t="s">
-        <v>345</v>
+        <v>353</v>
       </c>
       <c r="C84" s="3" t="s">
-        <v>346</v>
+        <v>354</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A85" s="1" t="s">
-        <v>347</v>
-      </c>
-      <c r="B85" s="3" t="s">
-        <v>348</v>
-      </c>
-      <c r="C85" s="3" t="s">
-        <v>349</v>
-      </c>
+      <c r="B85" s="3"/>
+      <c r="C85" s="3"/>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A86" s="1" t="s">
-        <v>350</v>
+        <v>355</v>
       </c>
       <c r="B86" s="3" t="s">
-        <v>351</v>
+        <v>356</v>
       </c>
       <c r="C86" s="3" t="s">
-        <v>352</v>
+        <v>357</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A87" s="1" t="s">
-        <v>353</v>
+        <v>358</v>
       </c>
       <c r="B87" s="3" t="s">
-        <v>354</v>
+        <v>359</v>
       </c>
       <c r="C87" s="3" t="s">
-        <v>355</v>
+        <v>360</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A88" s="1" t="s">
-        <v>356</v>
+        <v>361</v>
       </c>
       <c r="B88" s="3" t="s">
-        <v>357</v>
+        <v>362</v>
       </c>
       <c r="C88" s="3" t="s">
-        <v>358</v>
+        <v>363</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A89" s="1" t="s">
-        <v>359</v>
+        <v>364</v>
       </c>
       <c r="B89" s="3" t="s">
-        <v>360</v>
+        <v>365</v>
       </c>
       <c r="C89" s="3" t="s">
-        <v>361</v>
+        <v>366</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A90" s="1" t="s">
-        <v>362</v>
+        <v>367</v>
       </c>
       <c r="B90" s="3" t="s">
-        <v>363</v>
+        <v>368</v>
       </c>
       <c r="C90" s="3" t="s">
-        <v>364</v>
+        <v>369</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A91" s="1" t="s">
-        <v>365</v>
+        <v>370</v>
       </c>
       <c r="B91" s="3" t="s">
-        <v>366</v>
+        <v>371</v>
       </c>
       <c r="C91" s="3" t="s">
-        <v>367</v>
+        <v>372</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B92" s="3"/>
-      <c r="C92" s="3"/>
+      <c r="A92" s="1" t="s">
+        <v>373</v>
+      </c>
+      <c r="B92" s="3" t="s">
+        <v>374</v>
+      </c>
+      <c r="C92" s="3" t="s">
+        <v>375</v>
+      </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A93" s="1" t="s">
-        <v>368</v>
+        <v>376</v>
       </c>
       <c r="B93" s="3" t="s">
-        <v>369</v>
+        <v>377</v>
       </c>
       <c r="C93" s="3" t="s">
-        <v>370</v>
+        <v>378</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A94" s="1" t="s">
-        <v>371</v>
-      </c>
-      <c r="B94" s="3" t="s">
-        <v>372</v>
-      </c>
-      <c r="C94" s="3" t="s">
-        <v>373</v>
-      </c>
+      <c r="B94" s="3"/>
+      <c r="C94" s="3"/>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A95" s="1" t="s">
-        <v>374</v>
+        <v>379</v>
       </c>
       <c r="B95" s="3" t="s">
-        <v>375</v>
+        <v>380</v>
       </c>
       <c r="C95" s="3" t="s">
-        <v>376</v>
+        <v>381</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A96" s="1" t="s">
-        <v>377</v>
+        <v>382</v>
       </c>
       <c r="B96" s="3" t="s">
-        <v>378</v>
+        <v>383</v>
       </c>
       <c r="C96" s="3" t="s">
-        <v>379</v>
+        <v>384</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A97" s="1" t="s">
+        <v>385</v>
+      </c>
+      <c r="B97" s="3" t="s">
+        <v>386</v>
+      </c>
+      <c r="C97" s="3" t="s">
+        <v>387</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A98" s="1" t="s">
-        <v>380</v>
+        <v>388</v>
       </c>
       <c r="B98" s="3" t="s">
-        <v>381</v>
+        <v>389</v>
       </c>
       <c r="C98" s="3" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A99" s="1" t="s">
-        <v>383</v>
-      </c>
-      <c r="B99" s="3" t="s">
-        <v>384</v>
-      </c>
-      <c r="C99" s="3" t="s">
-        <v>385</v>
+        <v>390</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A100" s="1" t="s">
-        <v>386</v>
+        <v>391</v>
       </c>
       <c r="B100" s="3" t="s">
-        <v>387</v>
+        <v>392</v>
       </c>
       <c r="C100" s="3" t="s">
-        <v>388</v>
+        <v>393</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A101" s="1" t="s">
-        <v>389</v>
+        <v>394</v>
       </c>
       <c r="B101" s="3" t="s">
-        <v>390</v>
+        <v>395</v>
       </c>
       <c r="C101" s="3" t="s">
-        <v>391</v>
+        <v>396</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A102" s="1" t="s">
-        <v>392</v>
+        <v>397</v>
       </c>
       <c r="B102" s="3" t="s">
-        <v>393</v>
+        <v>398</v>
       </c>
       <c r="C102" s="3" t="s">
-        <v>394</v>
+        <v>399</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A103" s="1" t="s">
+        <v>400</v>
+      </c>
+      <c r="B103" s="3" t="s">
+        <v>401</v>
+      </c>
+      <c r="C103" s="3" t="s">
+        <v>402</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A104" s="1" t="s">
-        <v>395</v>
+        <v>403</v>
       </c>
       <c r="B104" s="3" t="s">
-        <v>396</v>
+        <v>404</v>
       </c>
       <c r="C104" s="3" t="s">
-        <v>397</v>
-      </c>
-    </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A105" s="1" t="s">
-        <v>398</v>
-      </c>
-      <c r="B105" s="1" t="s">
-        <v>399</v>
-      </c>
-      <c r="C105" s="1" t="s">
-        <v>400</v>
+        <v>405</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A106" s="1" t="s">
-        <v>401</v>
-      </c>
-      <c r="B106" s="1" t="s">
-        <v>402</v>
-      </c>
-      <c r="C106" s="1" t="s">
-        <v>403</v>
+        <v>406</v>
+      </c>
+      <c r="B106" s="3" t="s">
+        <v>407</v>
+      </c>
+      <c r="C106" s="3" t="s">
+        <v>408</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A107" s="1" t="s">
-        <v>404</v>
-      </c>
-      <c r="B107" s="3" t="s">
-        <v>405</v>
+        <v>409</v>
+      </c>
+      <c r="B107" s="1" t="s">
+        <v>410</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>406</v>
+        <v>411</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A108" s="1" t="s">
-        <v>407</v>
+        <v>412</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>408</v>
+        <v>413</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>409</v>
+        <v>414</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A109" s="1" t="s">
-        <v>410</v>
+        <v>415</v>
       </c>
       <c r="B109" s="3" t="s">
-        <v>411</v>
-      </c>
-      <c r="C109" s="3" t="s">
-        <v>412</v>
+        <v>416</v>
+      </c>
+      <c r="C109" s="1" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A110" s="1" t="s">
+        <v>418</v>
+      </c>
+      <c r="B110" s="1" t="s">
+        <v>419</v>
+      </c>
+      <c r="C110" s="1" t="s">
+        <v>420</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A111" s="1" t="s">
-        <v>413</v>
+        <v>421</v>
       </c>
       <c r="B111" s="3" t="s">
-        <v>414</v>
+        <v>422</v>
       </c>
       <c r="C111" s="3" t="s">
-        <v>415</v>
-      </c>
-    </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A112" s="1" t="s">
-        <v>416</v>
-      </c>
-      <c r="B112" s="3" t="s">
-        <v>417</v>
-      </c>
-      <c r="C112" s="3" t="s">
-        <v>418</v>
+        <v>423</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B113" s="3"/>
-      <c r="C113" s="3"/>
+      <c r="A113" s="1" t="s">
+        <v>424</v>
+      </c>
+      <c r="B113" s="3" t="s">
+        <v>425</v>
+      </c>
+      <c r="C113" s="3" t="s">
+        <v>426</v>
+      </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A114" s="1" t="s">
-        <v>419</v>
+        <v>427</v>
       </c>
       <c r="B114" s="3" t="s">
-        <v>420</v>
+        <v>428</v>
       </c>
       <c r="C114" s="3" t="s">
-        <v>421</v>
+        <v>429</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A115" s="1" t="s">
-        <v>422</v>
-      </c>
-      <c r="B115" s="3" t="s">
-        <v>423</v>
-      </c>
-      <c r="C115" s="3" t="s">
-        <v>424</v>
-      </c>
+      <c r="B115" s="3"/>
+      <c r="C115" s="3"/>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A116" s="1" t="s">
-        <v>425</v>
+        <v>430</v>
       </c>
       <c r="B116" s="3" t="s">
-        <v>426</v>
+        <v>431</v>
       </c>
       <c r="C116" s="3" t="s">
-        <v>427</v>
+        <v>432</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A117" s="1" t="s">
-        <v>428</v>
+        <v>433</v>
       </c>
       <c r="B117" s="3" t="s">
-        <v>429</v>
+        <v>434</v>
       </c>
       <c r="C117" s="3" t="s">
-        <v>430</v>
+        <v>435</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A118" s="1" t="s">
-        <v>431</v>
+        <v>436</v>
       </c>
       <c r="B118" s="3" t="s">
-        <v>432</v>
+        <v>437</v>
       </c>
       <c r="C118" s="3" t="s">
-        <v>433</v>
+        <v>438</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B119" s="3"/>
-      <c r="C119" s="3"/>
+      <c r="A119" s="1" t="s">
+        <v>439</v>
+      </c>
+      <c r="B119" s="3" t="s">
+        <v>440</v>
+      </c>
+      <c r="C119" s="3" t="s">
+        <v>441</v>
+      </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A120" s="1" t="s">
-        <v>434</v>
+        <v>442</v>
       </c>
       <c r="B120" s="3" t="s">
-        <v>435</v>
+        <v>443</v>
       </c>
       <c r="C120" s="3" t="s">
-        <v>436</v>
+        <v>444</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A121" s="1" t="s">
-        <v>437</v>
-      </c>
-      <c r="B121" s="3" t="s">
-        <v>438</v>
-      </c>
-      <c r="C121" s="3" t="s">
-        <v>439</v>
+      <c r="B121" s="3"/>
+      <c r="C121" s="3"/>
+    </row>
+    <row r="122" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A122" s="1" t="s">
+        <v>445</v>
+      </c>
+      <c r="B122" s="3" t="s">
+        <v>446</v>
+      </c>
+      <c r="C122" s="3" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A123" s="1" t="s">
+        <v>448</v>
+      </c>
+      <c r="B123" s="3" t="s">
+        <v>449</v>
+      </c>
+      <c r="C123" s="3" t="s">
+        <v>450</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Allow saving credential using Windows Credential Manager
</commit_message>
<xml_diff>
--- a/Config.xlsx
+++ b/Config.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22730"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mateus.cruz\Documents\GitHub\OrchestratorManager\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7B0C459-3890-4A03-AD44-C48021E1C725}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5348853-B757-4368-A72D-BFDF157A5872}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="489" uniqueCount="454">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="501" uniqueCount="466">
   <si>
     <t>Name</t>
   </si>
@@ -57,9 +57,6 @@
     <t>TenantName</t>
   </si>
   <si>
-    <t>Default</t>
-  </si>
-  <si>
     <t>Name of the tenant to be used. 
 Sample value: Default.</t>
   </si>
@@ -188,6 +185,24 @@
     <t>Path to the file to be used as Authentication Panel form.</t>
   </si>
   <si>
+    <t>CloudCredentialName</t>
+  </si>
+  <si>
+    <t>OrchestratorManager_CloudCredential</t>
+  </si>
+  <si>
+    <t>Name of credential in Windows Credential Manager to store Cloud Platform Orchestrator administrator's credential (ClientID and UserKey).</t>
+  </si>
+  <si>
+    <t>OnPremisesCredentialName</t>
+  </si>
+  <si>
+    <t>OrchestratorManager_OnPremisesCredential</t>
+  </si>
+  <si>
+    <t>Name of credential in Windows Credential Manager to store on-premises Orchestrator administrator's credential (Username and Password).</t>
+  </si>
+  <si>
     <t>CreateMachineResultColumn</t>
   </si>
   <si>
@@ -539,6 +554,24 @@
     <t>組織単位</t>
   </si>
   <si>
+    <t>FormUseSavedCredentialLabel</t>
+  </si>
+  <si>
+    <t>Use credential stored in Windows's Credential Manager.</t>
+  </si>
+  <si>
+    <t>Windowsの資格情報マネージャーにある認証情報を使用します。</t>
+  </si>
+  <si>
+    <t>FormSaveCredentialLabel</t>
+  </si>
+  <si>
+    <t>Save credential in Windows's Credential Manager.</t>
+  </si>
+  <si>
+    <t>Windowsの資格情報マネージャーに認証情報を保存します。</t>
+  </si>
+  <si>
     <t>FormAssetOption</t>
   </si>
   <si>
@@ -596,7 +629,7 @@
     <t>FormOrganizationUnitOption</t>
   </si>
   <si>
-    <t>Organiztion Unit</t>
+    <t>Organization Unit</t>
   </si>
   <si>
     <t>FormSubmitButton</t>
@@ -1400,7 +1433,10 @@
     <t>https://myOrchestratorURL</t>
   </si>
   <si>
-    <t>MyAccount</t>
+    <t>Default</t>
+  </si>
+  <si>
+    <t>https://platform.uipath.com/MyAccount</t>
   </si>
   <si>
     <t>Workbooks</t>
@@ -1444,21 +1480,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1487,8 +1520,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table1" displayName="Table1" ref="A1:C48" totalsRowShown="0">
-  <autoFilter ref="A1:C48" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table1" displayName="Table1" ref="A1:C50" totalsRowShown="0">
+  <autoFilter ref="A1:C50" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Name"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Value"/>
@@ -1499,8 +1532,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table13" displayName="Table13" ref="A1:C123" totalsRowShown="0">
-  <autoFilter ref="A1:C123" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table13" displayName="Table13" ref="A1:C125" totalsRowShown="0">
+  <autoFilter ref="A1:C125" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Name"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="EN"/>
@@ -1801,8 +1834,8 @@
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="4" t="s">
-        <v>451</v>
+      <c r="B2" s="2" t="s">
+        <v>462</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>4</v>
@@ -1813,51 +1846,48 @@
         <v>5</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>463</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>6</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="72.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>464</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>8</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>452</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="43.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>465</v>
+      </c>
+      <c r="C5" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>453</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>11</v>
-      </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C48"/>
+  <dimension ref="A1:C50"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -1881,197 +1911,197 @@
     </row>
     <row r="2" spans="1:3" ht="101.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B2" s="1">
         <v>200</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B3" s="1">
         <v>0</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="1">
+        <v>550</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>16</v>
-      </c>
-      <c r="B4" s="1">
-        <v>500</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="1">
+        <v>650</v>
+      </c>
+      <c r="C5" s="3" t="s">
         <v>18</v>
-      </c>
-      <c r="B5" s="1">
-        <v>600</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B6" s="1">
         <v>3</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B7" s="1">
         <v>5000</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="C8" s="3" t="s">
         <v>25</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="C9" s="3" t="s">
         <v>28</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="C10" s="3" t="s">
         <v>31</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="C11" s="3" t="s">
         <v>34</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="C12" s="3" t="s">
         <v>37</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="C13" s="3" t="s">
         <v>40</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="C14" s="3" t="s">
         <v>43</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B15" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="C15" s="3" t="s">
         <v>46</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B16" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="C16" s="3" t="s">
         <v>49</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B17" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="C17" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="C17" s="3" t="s">
+    </row>
+    <row r="18" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="1" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A18" s="1" t="s">
+      <c r="B18" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="C18" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="C18" s="3" t="s">
+    </row>
+    <row r="19" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="1" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A19" s="1" t="s">
+      <c r="B19" s="1" t="s">
         <v>57</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>52</v>
       </c>
       <c r="C19" s="3" t="s">
         <v>58</v>
@@ -2082,18 +2112,18 @@
         <v>59</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>49</v>
+        <v>60</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="C21" s="3" t="s">
         <v>63</v>
@@ -2104,62 +2134,62 @@
         <v>64</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="C27" s="3" t="s">
         <v>75</v>
@@ -2170,24 +2200,24 @@
         <v>76</v>
       </c>
       <c r="B28" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C28" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="C28" s="3" t="s">
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A29" s="1" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="1" t="s">
+      <c r="B29" s="1" t="s">
         <v>79</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>52</v>
       </c>
       <c r="C29" s="3" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="1" t="s">
         <v>81</v>
       </c>
@@ -2203,7 +2233,7 @@
         <v>84</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="C31" s="3" t="s">
         <v>85</v>
@@ -2214,186 +2244,208 @@
         <v>86</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>74</v>
+        <v>87</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" s="1" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>77</v>
+        <v>54</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A34" s="1" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A35" s="1" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>52</v>
+        <v>82</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A36" s="1" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>55</v>
+        <v>79</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A37" s="1" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row r="38" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A38" s="1" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>49</v>
+        <v>60</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A39" s="1" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A40" s="1" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A41" s="1" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>49</v>
+        <v>60</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
     </row>
     <row r="42" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A42" s="1" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A43" s="1" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row r="44" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A44" s="1" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>52</v>
+        <v>67</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
     </row>
     <row r="45" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A45" s="1" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A46" s="1" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>115</v>
+        <v>57</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>105</v>
+        <v>116</v>
       </c>
     </row>
     <row r="47" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A47" s="1" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A48" s="1" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>52</v>
+        <v>120</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>119</v>
+        <v>110</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A49" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C49" s="3" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A50" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C50" s="3" t="s">
+        <v>124</v>
       </c>
     </row>
   </sheetData>
@@ -2411,7 +2463,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1927ABA9-1814-4487-9CEC-ABDCAF91481F}">
-  <dimension ref="A1:C123"/>
+  <dimension ref="A1:C125"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -2429,1263 +2481,1285 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>121</v>
+        <v>126</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>122</v>
+        <v>127</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="43.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>124</v>
+        <v>129</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>126</v>
+        <v>131</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>127</v>
+        <v>132</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>128</v>
+        <v>133</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>128</v>
+        <v>133</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>129</v>
+        <v>134</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>130</v>
+        <v>135</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>131</v>
+        <v>136</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
-        <v>132</v>
+        <v>137</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>133</v>
+        <v>138</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>134</v>
+        <v>139</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
-        <v>138</v>
+        <v>143</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>139</v>
+        <v>144</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>140</v>
+        <v>145</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>142</v>
+        <v>147</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>143</v>
+        <v>148</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
-        <v>144</v>
+        <v>149</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>145</v>
+        <v>150</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>146</v>
+        <v>151</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
-        <v>147</v>
+        <v>152</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>148</v>
+        <v>153</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>149</v>
+        <v>154</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
-        <v>150</v>
+        <v>155</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>151</v>
+        <v>156</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>152</v>
+        <v>157</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
-        <v>153</v>
+        <v>158</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>154</v>
+        <v>159</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>155</v>
+        <v>160</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
-        <v>156</v>
+        <v>161</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>157</v>
+        <v>162</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>158</v>
+        <v>163</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
-        <v>159</v>
+        <v>164</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>160</v>
+        <v>165</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>161</v>
+        <v>166</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
-        <v>162</v>
+        <v>167</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>163</v>
+        <v>168</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>164</v>
+        <v>169</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
-        <v>165</v>
+        <v>170</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>166</v>
+        <v>171</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>167</v>
+        <v>172</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
-        <v>168</v>
+        <v>173</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>169</v>
+        <v>174</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>170</v>
+        <v>175</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
-        <v>171</v>
+        <v>176</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>172</v>
+        <v>177</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>173</v>
+        <v>178</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
-        <v>174</v>
+        <v>179</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>175</v>
+        <v>180</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>176</v>
+        <v>181</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
-        <v>177</v>
+        <v>182</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>178</v>
+        <v>183</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>179</v>
+        <v>184</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
-        <v>180</v>
+        <v>185</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>181</v>
+        <v>186</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>182</v>
+        <v>187</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
-        <v>183</v>
+        <v>188</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>184</v>
+        <v>189</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>164</v>
+        <v>190</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
-        <v>185</v>
+        <v>191</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>186</v>
+        <v>192</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>186</v>
+        <v>193</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
-        <v>187</v>
+        <v>194</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>188</v>
+        <v>195</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>189</v>
+        <v>169</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B26" s="3"/>
-      <c r="C26" s="3"/>
+      <c r="A26" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>197</v>
+      </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
-        <v>190</v>
+        <v>198</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>191</v>
+        <v>199</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>192</v>
+        <v>200</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A28" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="B28" s="3" t="s">
-        <v>194</v>
-      </c>
-      <c r="C28" s="3" t="s">
-        <v>195</v>
-      </c>
+      <c r="B28" s="3"/>
+      <c r="C28" s="3"/>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="s">
-        <v>196</v>
+        <v>201</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>197</v>
+        <v>202</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>198</v>
+        <v>203</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A30" s="1" t="s">
-        <v>199</v>
+        <v>204</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>200</v>
+        <v>205</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>201</v>
+        <v>206</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A31" s="1" t="s">
-        <v>202</v>
+        <v>207</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>203</v>
+        <v>208</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>204</v>
+        <v>209</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A32" s="1" t="s">
-        <v>205</v>
+        <v>210</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>206</v>
+        <v>211</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>207</v>
+        <v>212</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A33" s="1" t="s">
-        <v>208</v>
+        <v>213</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>209</v>
+        <v>214</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>210</v>
+        <v>215</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B34" s="3"/>
-      <c r="C34" s="3"/>
+      <c r="A34" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>218</v>
+      </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A35" s="1" t="s">
-        <v>211</v>
+        <v>219</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>212</v>
+        <v>220</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>213</v>
+        <v>221</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A36" s="1" t="s">
-        <v>214</v>
-      </c>
-      <c r="B36" s="3" t="s">
-        <v>215</v>
-      </c>
-      <c r="C36" s="3" t="s">
-        <v>216</v>
-      </c>
+      <c r="B36" s="3"/>
+      <c r="C36" s="3"/>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A37" s="1" t="s">
-        <v>217</v>
+        <v>222</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>218</v>
+        <v>223</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>219</v>
+        <v>224</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A38" s="1" t="s">
-        <v>220</v>
+        <v>225</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>221</v>
+        <v>226</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>222</v>
+        <v>227</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A39" s="1" t="s">
-        <v>223</v>
+        <v>228</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>224</v>
+        <v>229</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>225</v>
+        <v>230</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A40" s="1" t="s">
-        <v>226</v>
+        <v>231</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>227</v>
+        <v>232</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>228</v>
+        <v>233</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A41" s="1" t="s">
-        <v>229</v>
+        <v>234</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>230</v>
+        <v>235</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>231</v>
+        <v>236</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A42" s="1" t="s">
-        <v>232</v>
+        <v>237</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>233</v>
+        <v>238</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>234</v>
+        <v>239</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A43" s="1" t="s">
-        <v>235</v>
+        <v>240</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>236</v>
+        <v>241</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>237</v>
+        <v>242</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A44" s="1" t="s">
-        <v>238</v>
+        <v>243</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>239</v>
+        <v>244</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>240</v>
+        <v>245</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A45" s="1" t="s">
-        <v>241</v>
+        <v>246</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>242</v>
+        <v>247</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>243</v>
+        <v>248</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A46" s="1" t="s">
-        <v>244</v>
+        <v>249</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>245</v>
+        <v>250</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>246</v>
+        <v>251</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A47" s="1" t="s">
-        <v>247</v>
+        <v>252</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>248</v>
+        <v>253</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>249</v>
+        <v>254</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A48" s="1" t="s">
-        <v>250</v>
+        <v>255</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>251</v>
+        <v>256</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>252</v>
+        <v>257</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A49" s="1" t="s">
-        <v>253</v>
+        <v>258</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>254</v>
+        <v>259</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>255</v>
+        <v>260</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A50" s="1" t="s">
-        <v>256</v>
+        <v>261</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>257</v>
+        <v>262</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>258</v>
+        <v>263</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A51" s="1" t="s">
-        <v>259</v>
+        <v>264</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>260</v>
+        <v>265</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>261</v>
+        <v>266</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A52" s="1" t="s">
-        <v>262</v>
+        <v>267</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>263</v>
+        <v>268</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>264</v>
+        <v>269</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A53" s="1" t="s">
-        <v>265</v>
+        <v>270</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>266</v>
+        <v>271</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>267</v>
+        <v>272</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A54" s="1" t="s">
-        <v>268</v>
+        <v>273</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>269</v>
+        <v>274</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>270</v>
+        <v>275</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A55" s="1" t="s">
-        <v>271</v>
+        <v>276</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>272</v>
+        <v>277</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>273</v>
+        <v>278</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A56" s="1" t="s">
-        <v>274</v>
+        <v>279</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>275</v>
+        <v>280</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A57" s="1" t="s">
-        <v>277</v>
+        <v>282</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>278</v>
+        <v>283</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>279</v>
+        <v>284</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A58" s="1" t="s">
-        <v>280</v>
+        <v>285</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>281</v>
+        <v>286</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.35">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A59" s="1" t="s">
-        <v>283</v>
+        <v>288</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>284</v>
+        <v>289</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>285</v>
+        <v>290</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A60" s="1" t="s">
-        <v>286</v>
+        <v>291</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>287</v>
+        <v>292</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>288</v>
+        <v>293</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A61" s="1" t="s">
-        <v>289</v>
+        <v>294</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>290</v>
+        <v>295</v>
       </c>
       <c r="C61" s="3" t="s">
-        <v>291</v>
+        <v>296</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A62" s="1" t="s">
-        <v>292</v>
+        <v>297</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>293</v>
+        <v>298</v>
       </c>
       <c r="C62" s="3" t="s">
-        <v>294</v>
+        <v>299</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A63" s="1" t="s">
-        <v>295</v>
+        <v>300</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>296</v>
+        <v>301</v>
       </c>
       <c r="C63" s="3" t="s">
-        <v>297</v>
+        <v>302</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A64" s="1" t="s">
-        <v>298</v>
+        <v>303</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>299</v>
+        <v>304</v>
       </c>
       <c r="C64" s="3" t="s">
-        <v>300</v>
+        <v>305</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A65" s="1" t="s">
-        <v>301</v>
+        <v>306</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>302</v>
+        <v>307</v>
       </c>
       <c r="C65" s="3" t="s">
-        <v>303</v>
+        <v>308</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B66" s="3"/>
-      <c r="C66" s="3"/>
+      <c r="A66" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="B66" s="3" t="s">
+        <v>310</v>
+      </c>
+      <c r="C66" s="3" t="s">
+        <v>311</v>
+      </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A67" s="1" t="s">
-        <v>304</v>
+        <v>312</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>305</v>
+        <v>313</v>
       </c>
       <c r="C67" s="3" t="s">
-        <v>306</v>
+        <v>314</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A68" s="1" t="s">
-        <v>307</v>
-      </c>
-      <c r="B68" s="3" t="s">
-        <v>308</v>
-      </c>
-      <c r="C68" s="3" t="s">
-        <v>309</v>
-      </c>
+      <c r="B68" s="3"/>
+      <c r="C68" s="3"/>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A69" s="1" t="s">
-        <v>310</v>
+        <v>315</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>311</v>
+        <v>316</v>
       </c>
       <c r="C69" s="3" t="s">
-        <v>312</v>
+        <v>317</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A70" s="1" t="s">
-        <v>313</v>
+        <v>318</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>314</v>
+        <v>319</v>
       </c>
       <c r="C70" s="3" t="s">
-        <v>315</v>
+        <v>320</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A71" s="1" t="s">
-        <v>316</v>
+        <v>321</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>317</v>
+        <v>322</v>
       </c>
       <c r="C71" s="3" t="s">
-        <v>318</v>
+        <v>323</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A72" s="1" t="s">
-        <v>319</v>
+        <v>324</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>320</v>
+        <v>325</v>
       </c>
       <c r="C72" s="3" t="s">
-        <v>321</v>
+        <v>326</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A73" s="1" t="s">
-        <v>322</v>
+        <v>327</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>323</v>
+        <v>328</v>
       </c>
       <c r="C73" s="3" t="s">
-        <v>324</v>
+        <v>329</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A74" s="1" t="s">
-        <v>325</v>
+        <v>330</v>
       </c>
       <c r="B74" s="3" t="s">
-        <v>326</v>
+        <v>331</v>
       </c>
       <c r="C74" s="3" t="s">
-        <v>327</v>
+        <v>332</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B75" s="3"/>
-      <c r="C75" s="3"/>
+      <c r="A75" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="B75" s="3" t="s">
+        <v>334</v>
+      </c>
+      <c r="C75" s="3" t="s">
+        <v>335</v>
+      </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A76" s="1" t="s">
-        <v>328</v>
+        <v>336</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>329</v>
+        <v>337</v>
       </c>
       <c r="C76" s="3" t="s">
-        <v>330</v>
+        <v>338</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A77" s="1" t="s">
-        <v>331</v>
-      </c>
-      <c r="B77" s="3" t="s">
-        <v>332</v>
-      </c>
-      <c r="C77" s="3" t="s">
-        <v>333</v>
-      </c>
+      <c r="B77" s="3"/>
+      <c r="C77" s="3"/>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A78" s="1" t="s">
-        <v>334</v>
+        <v>339</v>
       </c>
       <c r="B78" s="3" t="s">
-        <v>335</v>
+        <v>340</v>
       </c>
       <c r="C78" s="3" t="s">
-        <v>336</v>
+        <v>341</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A79" s="1" t="s">
-        <v>337</v>
+        <v>342</v>
       </c>
       <c r="B79" s="3" t="s">
-        <v>338</v>
+        <v>343</v>
       </c>
       <c r="C79" s="3" t="s">
-        <v>339</v>
+        <v>344</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A80" s="1" t="s">
-        <v>340</v>
+        <v>345</v>
       </c>
       <c r="B80" s="3" t="s">
-        <v>341</v>
+        <v>346</v>
       </c>
       <c r="C80" s="3" t="s">
-        <v>342</v>
+        <v>347</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A81" s="1" t="s">
-        <v>343</v>
+        <v>348</v>
       </c>
       <c r="B81" s="3" t="s">
-        <v>344</v>
+        <v>349</v>
       </c>
       <c r="C81" s="3" t="s">
-        <v>345</v>
+        <v>350</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A82" s="1" t="s">
-        <v>346</v>
+        <v>351</v>
       </c>
       <c r="B82" s="3" t="s">
-        <v>347</v>
+        <v>352</v>
       </c>
       <c r="C82" s="3" t="s">
-        <v>348</v>
+        <v>353</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A83" s="1" t="s">
-        <v>349</v>
+        <v>354</v>
       </c>
       <c r="B83" s="3" t="s">
-        <v>350</v>
+        <v>355</v>
       </c>
       <c r="C83" s="3" t="s">
-        <v>351</v>
+        <v>356</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A84" s="1" t="s">
-        <v>352</v>
+        <v>357</v>
       </c>
       <c r="B84" s="3" t="s">
-        <v>353</v>
+        <v>358</v>
       </c>
       <c r="C84" s="3" t="s">
-        <v>354</v>
+        <v>359</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B85" s="3"/>
-      <c r="C85" s="3"/>
+      <c r="A85" s="1" t="s">
+        <v>360</v>
+      </c>
+      <c r="B85" s="3" t="s">
+        <v>361</v>
+      </c>
+      <c r="C85" s="3" t="s">
+        <v>362</v>
+      </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A86" s="1" t="s">
-        <v>355</v>
+        <v>363</v>
       </c>
       <c r="B86" s="3" t="s">
-        <v>356</v>
+        <v>364</v>
       </c>
       <c r="C86" s="3" t="s">
-        <v>357</v>
+        <v>365</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A87" s="1" t="s">
-        <v>358</v>
-      </c>
-      <c r="B87" s="3" t="s">
-        <v>359</v>
-      </c>
-      <c r="C87" s="3" t="s">
-        <v>360</v>
-      </c>
+      <c r="B87" s="3"/>
+      <c r="C87" s="3"/>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A88" s="1" t="s">
-        <v>361</v>
+        <v>366</v>
       </c>
       <c r="B88" s="3" t="s">
-        <v>362</v>
+        <v>367</v>
       </c>
       <c r="C88" s="3" t="s">
-        <v>363</v>
+        <v>368</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A89" s="1" t="s">
-        <v>364</v>
+        <v>369</v>
       </c>
       <c r="B89" s="3" t="s">
-        <v>365</v>
+        <v>370</v>
       </c>
       <c r="C89" s="3" t="s">
-        <v>366</v>
+        <v>371</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A90" s="1" t="s">
-        <v>367</v>
+        <v>372</v>
       </c>
       <c r="B90" s="3" t="s">
-        <v>368</v>
+        <v>373</v>
       </c>
       <c r="C90" s="3" t="s">
-        <v>369</v>
+        <v>374</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A91" s="1" t="s">
-        <v>370</v>
+        <v>375</v>
       </c>
       <c r="B91" s="3" t="s">
-        <v>371</v>
+        <v>376</v>
       </c>
       <c r="C91" s="3" t="s">
-        <v>372</v>
+        <v>377</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A92" s="1" t="s">
-        <v>373</v>
+        <v>378</v>
       </c>
       <c r="B92" s="3" t="s">
-        <v>374</v>
+        <v>379</v>
       </c>
       <c r="C92" s="3" t="s">
-        <v>375</v>
+        <v>380</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A93" s="1" t="s">
-        <v>376</v>
+        <v>381</v>
       </c>
       <c r="B93" s="3" t="s">
-        <v>377</v>
+        <v>382</v>
       </c>
       <c r="C93" s="3" t="s">
-        <v>378</v>
+        <v>383</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B94" s="3"/>
-      <c r="C94" s="3"/>
+      <c r="A94" s="1" t="s">
+        <v>384</v>
+      </c>
+      <c r="B94" s="3" t="s">
+        <v>385</v>
+      </c>
+      <c r="C94" s="3" t="s">
+        <v>386</v>
+      </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A95" s="1" t="s">
-        <v>379</v>
+        <v>387</v>
       </c>
       <c r="B95" s="3" t="s">
-        <v>380</v>
+        <v>388</v>
       </c>
       <c r="C95" s="3" t="s">
-        <v>381</v>
+        <v>389</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A96" s="1" t="s">
-        <v>382</v>
-      </c>
-      <c r="B96" s="3" t="s">
-        <v>383</v>
-      </c>
-      <c r="C96" s="3" t="s">
-        <v>384</v>
-      </c>
+      <c r="B96" s="3"/>
+      <c r="C96" s="3"/>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A97" s="1" t="s">
-        <v>385</v>
+        <v>390</v>
       </c>
       <c r="B97" s="3" t="s">
-        <v>386</v>
+        <v>391</v>
       </c>
       <c r="C97" s="3" t="s">
-        <v>387</v>
+        <v>392</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A98" s="1" t="s">
-        <v>388</v>
+        <v>393</v>
       </c>
       <c r="B98" s="3" t="s">
-        <v>389</v>
+        <v>394</v>
       </c>
       <c r="C98" s="3" t="s">
-        <v>390</v>
+        <v>395</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A99" s="1" t="s">
+        <v>396</v>
+      </c>
+      <c r="B99" s="3" t="s">
+        <v>397</v>
+      </c>
+      <c r="C99" s="3" t="s">
+        <v>398</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A100" s="1" t="s">
-        <v>391</v>
+        <v>399</v>
       </c>
       <c r="B100" s="3" t="s">
-        <v>392</v>
+        <v>400</v>
       </c>
       <c r="C100" s="3" t="s">
-        <v>393</v>
-      </c>
-    </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A101" s="1" t="s">
-        <v>394</v>
-      </c>
-      <c r="B101" s="3" t="s">
-        <v>395</v>
-      </c>
-      <c r="C101" s="3" t="s">
-        <v>396</v>
+        <v>401</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A102" s="1" t="s">
-        <v>397</v>
+        <v>402</v>
       </c>
       <c r="B102" s="3" t="s">
-        <v>398</v>
+        <v>403</v>
       </c>
       <c r="C102" s="3" t="s">
-        <v>399</v>
+        <v>404</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A103" s="1" t="s">
-        <v>400</v>
+        <v>405</v>
       </c>
       <c r="B103" s="3" t="s">
-        <v>401</v>
+        <v>406</v>
       </c>
       <c r="C103" s="3" t="s">
-        <v>402</v>
+        <v>407</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A104" s="1" t="s">
-        <v>403</v>
+        <v>408</v>
       </c>
       <c r="B104" s="3" t="s">
-        <v>404</v>
+        <v>409</v>
       </c>
       <c r="C104" s="3" t="s">
-        <v>405</v>
+        <v>410</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A105" s="1" t="s">
+        <v>411</v>
+      </c>
+      <c r="B105" s="3" t="s">
+        <v>412</v>
+      </c>
+      <c r="C105" s="3" t="s">
+        <v>413</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A106" s="1" t="s">
-        <v>406</v>
+        <v>414</v>
       </c>
       <c r="B106" s="3" t="s">
-        <v>407</v>
+        <v>415</v>
       </c>
       <c r="C106" s="3" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A107" s="1" t="s">
-        <v>409</v>
-      </c>
-      <c r="B107" s="1" t="s">
-        <v>410</v>
-      </c>
-      <c r="C107" s="1" t="s">
-        <v>411</v>
+        <v>416</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A108" s="1" t="s">
-        <v>412</v>
-      </c>
-      <c r="B108" s="1" t="s">
-        <v>413</v>
-      </c>
-      <c r="C108" s="1" t="s">
-        <v>414</v>
+        <v>417</v>
+      </c>
+      <c r="B108" s="3" t="s">
+        <v>418</v>
+      </c>
+      <c r="C108" s="3" t="s">
+        <v>419</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A109" s="1" t="s">
-        <v>415</v>
-      </c>
-      <c r="B109" s="3" t="s">
-        <v>416</v>
+        <v>420</v>
+      </c>
+      <c r="B109" s="1" t="s">
+        <v>421</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>417</v>
+        <v>422</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A110" s="1" t="s">
-        <v>418</v>
+        <v>423</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>419</v>
+        <v>424</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>420</v>
+        <v>425</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A111" s="1" t="s">
-        <v>421</v>
+        <v>426</v>
       </c>
       <c r="B111" s="3" t="s">
-        <v>422</v>
-      </c>
-      <c r="C111" s="3" t="s">
-        <v>423</v>
+        <v>427</v>
+      </c>
+      <c r="C111" s="1" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A112" s="1" t="s">
+        <v>429</v>
+      </c>
+      <c r="B112" s="1" t="s">
+        <v>430</v>
+      </c>
+      <c r="C112" s="1" t="s">
+        <v>431</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A113" s="1" t="s">
-        <v>424</v>
+        <v>432</v>
       </c>
       <c r="B113" s="3" t="s">
-        <v>425</v>
+        <v>433</v>
       </c>
       <c r="C113" s="3" t="s">
-        <v>426</v>
-      </c>
-    </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A114" s="1" t="s">
-        <v>427</v>
-      </c>
-      <c r="B114" s="3" t="s">
-        <v>428</v>
-      </c>
-      <c r="C114" s="3" t="s">
-        <v>429</v>
+        <v>434</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B115" s="3"/>
-      <c r="C115" s="3"/>
+      <c r="A115" s="1" t="s">
+        <v>435</v>
+      </c>
+      <c r="B115" s="3" t="s">
+        <v>436</v>
+      </c>
+      <c r="C115" s="3" t="s">
+        <v>437</v>
+      </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A116" s="1" t="s">
-        <v>430</v>
+        <v>438</v>
       </c>
       <c r="B116" s="3" t="s">
-        <v>431</v>
+        <v>439</v>
       </c>
       <c r="C116" s="3" t="s">
-        <v>432</v>
+        <v>440</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A117" s="1" t="s">
-        <v>433</v>
-      </c>
-      <c r="B117" s="3" t="s">
-        <v>434</v>
-      </c>
-      <c r="C117" s="3" t="s">
-        <v>435</v>
-      </c>
+      <c r="B117" s="3"/>
+      <c r="C117" s="3"/>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A118" s="1" t="s">
-        <v>436</v>
+        <v>441</v>
       </c>
       <c r="B118" s="3" t="s">
-        <v>437</v>
+        <v>442</v>
       </c>
       <c r="C118" s="3" t="s">
-        <v>438</v>
+        <v>443</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A119" s="1" t="s">
-        <v>439</v>
+        <v>444</v>
       </c>
       <c r="B119" s="3" t="s">
-        <v>440</v>
+        <v>445</v>
       </c>
       <c r="C119" s="3" t="s">
-        <v>441</v>
+        <v>446</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A120" s="1" t="s">
-        <v>442</v>
+        <v>447</v>
       </c>
       <c r="B120" s="3" t="s">
-        <v>443</v>
+        <v>448</v>
       </c>
       <c r="C120" s="3" t="s">
-        <v>444</v>
+        <v>449</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B121" s="3"/>
-      <c r="C121" s="3"/>
+      <c r="A121" s="1" t="s">
+        <v>450</v>
+      </c>
+      <c r="B121" s="3" t="s">
+        <v>451</v>
+      </c>
+      <c r="C121" s="3" t="s">
+        <v>452</v>
+      </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A122" s="1" t="s">
-        <v>445</v>
+        <v>453</v>
       </c>
       <c r="B122" s="3" t="s">
-        <v>446</v>
+        <v>454</v>
       </c>
       <c r="C122" s="3" t="s">
-        <v>447</v>
+        <v>455</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A123" s="1" t="s">
-        <v>448</v>
-      </c>
-      <c r="B123" s="3" t="s">
-        <v>449</v>
-      </c>
-      <c r="C123" s="3" t="s">
-        <v>450</v>
+      <c r="B123" s="3"/>
+      <c r="C123" s="3"/>
+    </row>
+    <row r="124" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A124" s="1" t="s">
+        <v>456</v>
+      </c>
+      <c r="B124" s="3" t="s">
+        <v>457</v>
+      </c>
+      <c r="C124" s="3" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A125" s="1" t="s">
+        <v>459</v>
+      </c>
+      <c r="B125" s="3" t="s">
+        <v>460</v>
+      </c>
+      <c r="C125" s="3" t="s">
+        <v>461</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Allow users to choose on-premises Orchestrator version when authenticating
The version can be used to filter entities that are shown in the control panel.
</commit_message>
<xml_diff>
--- a/Config.xlsx
+++ b/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mateus.cruz\Documents\GitHub\OrchestratorManager\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5348853-B757-4368-A72D-BFDF157A5872}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77989E0F-5668-40CA-861F-0F36CA5FEFF3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="501" uniqueCount="466">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="509" uniqueCount="474">
   <si>
     <t>Name</t>
   </si>
@@ -46,34 +46,46 @@
     <t>Explanation</t>
   </si>
   <si>
-    <t>OrchestratorURL</t>
+    <t>EntitiesWorkbooksFolderPath</t>
+  </si>
+  <si>
+    <t>Path to the folder that contains entities workbooks. 
+Sample value: C:\Users\MyUser\Desktop\Workbooks</t>
+  </si>
+  <si>
+    <t>TenantName</t>
+  </si>
+  <si>
+    <t>Default</t>
+  </si>
+  <si>
+    <t>Name of the tenant to be used. 
+Sample value: Default.</t>
+  </si>
+  <si>
+    <t>OnPremisesOrchestratorURL</t>
   </si>
   <si>
     <t>URL of the Orchestrator instance to be used. 
 This parameter is exclusive to on-premises Orchestrator instances.
-Sample value: https://myOrchestratorURL.</t>
-  </si>
-  <si>
-    <t>TenantName</t>
-  </si>
-  <si>
-    <t>Name of the tenant to be used. 
-Sample value: Default.</t>
-  </si>
-  <si>
-    <t>AccountName</t>
-  </si>
-  <si>
-    <t>Unique site URL for Cloud Platform organization.
-This parameter is exclusive to Cloud Platform Orchestrator instances.
+Sample value: https://myOrchestratorURL</t>
+  </si>
+  <si>
+    <t>OnPremisesOrchestratorVersion</t>
+  </si>
+  <si>
+    <t>Version of the Orchestrator instance to be used. 
+This parameter is exclusive to on-premises Orchestrator instances.
+The specified value must be in the form YYYYMM, where YYYY is the 4-digit representation of an year and MM is the 2-digit representation of a month.
+Sample values: 201804, 201904, 201910</t>
+  </si>
+  <si>
+    <t>CloudAccountName</t>
+  </si>
+  <si>
+    <t>Unique site URL for Automation Cloud oganization.
+This parameter is exclusive to Automation Cloud Orchestrator instances.
 Sample value: MyAccount (assuming the organization account URL is https://platform.uipath.com/MyAccount).</t>
-  </si>
-  <si>
-    <t>EntitiesWorkbooksFolderPath</t>
-  </si>
-  <si>
-    <t>Path to the folder that contains entities workbooks. 
-Sample value: C:\Users\MyUser\Desktop\Workbooks</t>
   </si>
   <si>
     <t>MaximumRequestsThreshold</t>
@@ -440,6 +452,15 @@
     <t>ご注意ください: ログイン試行に複数回失敗した場合、テナントのセキュリティ設定で指定した秒数の間、アカウントがロックされることがあります。</t>
   </si>
   <si>
+    <t>FormOrchestratorVersionLabel</t>
+  </si>
+  <si>
+    <t>Version</t>
+  </si>
+  <si>
+    <t>バージョン</t>
+  </si>
+  <si>
     <t>FormOrchestratorURLLabel</t>
   </si>
   <si>
@@ -854,13 +875,22 @@
     <t>成功</t>
   </si>
   <si>
+    <t>OnPremisesOrchestratorVersionNotSupported</t>
+  </si>
+  <si>
+    <t>The specified Orchestrator version is not supported.</t>
+  </si>
+  <si>
+    <t>指定されたOrchestratorバージョンはサポートされていません。</t>
+  </si>
+  <si>
     <t>TokenNotRetrieved</t>
   </si>
   <si>
-    <t>Unable to get access token due to failed authentication.</t>
-  </si>
-  <si>
-    <t>認証に失敗したため、アクセス トークンを取得できません。</t>
+    <t>Unable to get access token due to failed authentication. Server response: {0}</t>
+  </si>
+  <si>
+    <t>認証に失敗したため、アクセス トークンを取得できません。サーバーレスポンス：{0}</t>
   </si>
   <si>
     <t>TokenExpired</t>
@@ -1430,16 +1460,13 @@
     <t>パッケージバージョンが指定されませんでした。</t>
   </si>
   <si>
+    <t>Workbooks</t>
+  </si>
+  <si>
     <t>https://myOrchestratorURL</t>
   </si>
   <si>
-    <t>Default</t>
-  </si>
-  <si>
-    <t>https://platform.uipath.com/MyAccount</t>
-  </si>
-  <si>
-    <t>Workbooks</t>
+    <t>MyAccount</t>
   </si>
 </sst>
 </file>
@@ -1486,10 +1513,10 @@
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1508,14 +1535,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table14" displayName="Table14" ref="A1:C5" totalsRowShown="0">
-  <autoFilter ref="A1:C5" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table14" displayName="Table14" ref="A1:C8" totalsRowShown="0">
+  <autoFilter ref="A1:C8" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Name"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Value"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Explanation"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -1527,19 +1554,19 @@
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Value"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Explanation"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table13" displayName="Table13" ref="A1:C125" totalsRowShown="0">
-  <autoFilter ref="A1:C125" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table13" displayName="Table13" ref="A1:C127" totalsRowShown="0">
+  <autoFilter ref="A1:C127" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Name"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="EN"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="JA"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -1806,7 +1833,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D89C9C48-5454-47C4-AB1D-448E4519251A}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -1830,14 +1857,14 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="58" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" ht="43.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>462</v>
-      </c>
-      <c r="C2" s="3" t="s">
+      <c r="B2" s="1" t="s">
+        <v>471</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1846,32 +1873,43 @@
         <v>5</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>463</v>
-      </c>
-      <c r="C3" s="3" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" ht="72.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="1" t="s">
+      <c r="C3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>464</v>
-      </c>
-      <c r="C4" s="3" t="s">
+    </row>
+    <row r="5" spans="1:3" ht="58" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" ht="43.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="1" t="s">
+      <c r="B5" s="3" t="s">
+        <v>472</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>465</v>
-      </c>
-      <c r="C5" s="3" t="s">
+    </row>
+    <row r="6" spans="1:3" ht="101.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="1" t="s">
         <v>10</v>
+      </c>
+      <c r="B6" s="1">
+        <v>201910</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="72.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>473</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -1887,8 +1925,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C50"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2 A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1911,541 +1949,541 @@
     </row>
     <row r="2" spans="1:3" ht="101.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B2" s="1">
         <v>200</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>12</v>
+      <c r="C2" s="2" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B3" s="1">
         <v>0</v>
       </c>
-      <c r="C3" s="3" t="s">
-        <v>14</v>
+      <c r="C3" s="2" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B4" s="1">
         <v>550</v>
       </c>
-      <c r="C4" s="3" t="s">
-        <v>16</v>
+      <c r="C4" s="2" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B5" s="1">
         <v>650</v>
       </c>
-      <c r="C5" s="3" t="s">
-        <v>18</v>
+      <c r="C5" s="2" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B6" s="1">
         <v>3</v>
       </c>
-      <c r="C6" s="3" t="s">
-        <v>20</v>
+      <c r="C6" s="2" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="B7" s="1">
         <v>5000</v>
       </c>
-      <c r="C7" s="3" t="s">
-        <v>22</v>
+      <c r="C7" s="2" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>25</v>
+        <v>26</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>28</v>
+        <v>29</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>31</v>
+        <v>33</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>34</v>
+        <v>36</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>37</v>
+        <v>39</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>40</v>
+        <v>42</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>43</v>
+        <v>45</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>46</v>
+        <v>48</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>49</v>
+        <v>51</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>52</v>
+        <v>54</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>55</v>
+        <v>57</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>58</v>
+        <v>60</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>61</v>
+        <v>63</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>63</v>
+        <v>60</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>65</v>
+        <v>57</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="C23" s="3" t="s">
-        <v>68</v>
+        <v>70</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="C24" s="3" t="s">
-        <v>65</v>
+        <v>57</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B25" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="B25" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="C25" s="3" t="s">
-        <v>71</v>
+      <c r="C25" s="2" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="C26" s="3" t="s">
-        <v>73</v>
+        <v>57</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="C27" s="3" t="s">
-        <v>75</v>
+        <v>70</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="C28" s="3" t="s">
-        <v>77</v>
+        <v>57</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="C29" s="3" t="s">
-        <v>80</v>
+        <v>82</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="1" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="C30" s="3" t="s">
-        <v>83</v>
+        <v>85</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" s="1" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="C31" s="3" t="s">
-        <v>85</v>
+        <v>60</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A32" s="1" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="C32" s="3" t="s">
-        <v>88</v>
+        <v>90</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" s="1" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="C33" s="3" t="s">
-        <v>90</v>
+        <v>57</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A34" s="1" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="C34" s="3" t="s">
-        <v>92</v>
+        <v>82</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A35" s="1" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="C35" s="3" t="s">
-        <v>94</v>
+        <v>85</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A36" s="1" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="C36" s="3" t="s">
-        <v>96</v>
+        <v>82</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A37" s="1" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="C37" s="3" t="s">
-        <v>98</v>
+        <v>60</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="38" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A38" s="1" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="C38" s="3" t="s">
-        <v>100</v>
+        <v>63</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A39" s="1" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="C39" s="3" t="s">
-        <v>102</v>
+        <v>57</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A40" s="1" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="C40" s="3" t="s">
-        <v>104</v>
+        <v>57</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="41" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A41" s="1" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="C41" s="3" t="s">
-        <v>106</v>
+        <v>63</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="42" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A42" s="1" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="C42" s="3" t="s">
-        <v>108</v>
+        <v>63</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A43" s="1" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="C43" s="3" t="s">
-        <v>110</v>
+        <v>57</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="44" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A44" s="1" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="C44" s="3" t="s">
-        <v>112</v>
+        <v>70</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="45" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A45" s="1" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="C45" s="3" t="s">
-        <v>114</v>
+        <v>57</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="46" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A46" s="1" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="C46" s="3" t="s">
-        <v>116</v>
+        <v>60</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="47" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A47" s="1" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="C47" s="3" t="s">
-        <v>118</v>
+        <v>60</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A48" s="1" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="C48" s="3" t="s">
-        <v>110</v>
+        <v>123</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="49" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A49" s="1" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="C49" s="3" t="s">
-        <v>122</v>
+        <v>60</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="50" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A50" s="1" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="C50" s="3" t="s">
-        <v>124</v>
+        <v>60</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>127</v>
       </c>
     </row>
   </sheetData>
@@ -2463,10 +2501,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1927ABA9-1814-4487-9CEC-ABDCAF91481F}">
-  <dimension ref="A1:C125"/>
+  <dimension ref="A1:C127"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A2" sqref="A2 A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2481,1285 +2519,1307 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>128</v>
+        <v>130</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="43.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>131</v>
+        <v>132</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>133</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>133</v>
+        <v>135</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>135</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>136</v>
+        <v>138</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>139</v>
+        <v>140</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>141</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>142</v>
+        <v>143</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>145</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>144</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>145</v>
+        <v>146</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>147</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>148</v>
+        <v>149</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>151</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>150</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>151</v>
+        <v>152</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>153</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>154</v>
+        <v>155</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>157</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>156</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>157</v>
+        <v>158</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>159</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>160</v>
+        <v>161</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>163</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>162</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>163</v>
+        <v>164</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>166</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>165</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>166</v>
+        <v>167</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>169</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>168</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>169</v>
+        <v>170</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>172</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>171</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>172</v>
+        <v>173</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>175</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>174</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>175</v>
+        <v>176</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>178</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>177</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>178</v>
+        <v>179</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>181</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
-        <v>179</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>180</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>181</v>
+        <v>182</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>184</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="B21" s="3" t="s">
-        <v>183</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>184</v>
+        <v>185</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>187</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
-        <v>185</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>186</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>187</v>
+        <v>188</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>190</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>189</v>
-      </c>
-      <c r="C23" s="3" t="s">
-        <v>190</v>
+        <v>191</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>193</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="B24" s="3" t="s">
-        <v>192</v>
-      </c>
-      <c r="C24" s="3" t="s">
-        <v>193</v>
+        <v>194</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>196</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
-        <v>194</v>
-      </c>
-      <c r="B25" s="3" t="s">
-        <v>195</v>
-      </c>
-      <c r="C25" s="3" t="s">
-        <v>169</v>
+        <v>197</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>199</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
-        <v>196</v>
-      </c>
-      <c r="B26" s="3" t="s">
-        <v>197</v>
-      </c>
-      <c r="C26" s="3" t="s">
-        <v>197</v>
+        <v>200</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>175</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="B27" s="3" t="s">
-        <v>199</v>
-      </c>
-      <c r="C27" s="3" t="s">
-        <v>200</v>
+        <v>202</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>203</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B28" s="3"/>
-      <c r="C28" s="3"/>
+      <c r="A28" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>206</v>
+      </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A29" s="1" t="s">
-        <v>201</v>
-      </c>
-      <c r="B29" s="3" t="s">
-        <v>202</v>
-      </c>
-      <c r="C29" s="3" t="s">
-        <v>203</v>
-      </c>
+      <c r="B29" s="2"/>
+      <c r="C29" s="2"/>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A30" s="1" t="s">
-        <v>204</v>
-      </c>
-      <c r="B30" s="3" t="s">
-        <v>205</v>
-      </c>
-      <c r="C30" s="3" t="s">
-        <v>206</v>
+        <v>207</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>209</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A31" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="B31" s="3" t="s">
-        <v>208</v>
-      </c>
-      <c r="C31" s="3" t="s">
-        <v>209</v>
+        <v>210</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>212</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A32" s="1" t="s">
-        <v>210</v>
-      </c>
-      <c r="B32" s="3" t="s">
-        <v>211</v>
-      </c>
-      <c r="C32" s="3" t="s">
-        <v>212</v>
+        <v>213</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>215</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A33" s="1" t="s">
-        <v>213</v>
-      </c>
-      <c r="B33" s="3" t="s">
-        <v>214</v>
-      </c>
-      <c r="C33" s="3" t="s">
-        <v>215</v>
+        <v>216</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>218</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A34" s="1" t="s">
-        <v>216</v>
-      </c>
-      <c r="B34" s="3" t="s">
-        <v>217</v>
-      </c>
-      <c r="C34" s="3" t="s">
-        <v>218</v>
+        <v>219</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>221</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A35" s="1" t="s">
-        <v>219</v>
-      </c>
-      <c r="B35" s="3" t="s">
-        <v>220</v>
-      </c>
-      <c r="C35" s="3" t="s">
-        <v>221</v>
+        <v>222</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>224</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B36" s="3"/>
-      <c r="C36" s="3"/>
+      <c r="A36" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>227</v>
+      </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A37" s="1" t="s">
-        <v>222</v>
-      </c>
-      <c r="B37" s="3" t="s">
-        <v>223</v>
-      </c>
-      <c r="C37" s="3" t="s">
-        <v>224</v>
-      </c>
+      <c r="B37" s="2"/>
+      <c r="C37" s="2"/>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A38" s="1" t="s">
-        <v>225</v>
-      </c>
-      <c r="B38" s="3" t="s">
-        <v>226</v>
-      </c>
-      <c r="C38" s="3" t="s">
-        <v>227</v>
+        <v>228</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>230</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A39" s="1" t="s">
-        <v>228</v>
-      </c>
-      <c r="B39" s="3" t="s">
-        <v>229</v>
-      </c>
-      <c r="C39" s="3" t="s">
-        <v>230</v>
+        <v>231</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>233</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A40" s="1" t="s">
-        <v>231</v>
-      </c>
-      <c r="B40" s="3" t="s">
-        <v>232</v>
-      </c>
-      <c r="C40" s="3" t="s">
-        <v>233</v>
+        <v>234</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>236</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A41" s="1" t="s">
-        <v>234</v>
-      </c>
-      <c r="B41" s="3" t="s">
-        <v>235</v>
-      </c>
-      <c r="C41" s="3" t="s">
-        <v>236</v>
+        <v>237</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>239</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A42" s="1" t="s">
-        <v>237</v>
-      </c>
-      <c r="B42" s="3" t="s">
-        <v>238</v>
-      </c>
-      <c r="C42" s="3" t="s">
-        <v>239</v>
+        <v>240</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>242</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A43" s="1" t="s">
-        <v>240</v>
-      </c>
-      <c r="B43" s="3" t="s">
-        <v>241</v>
-      </c>
-      <c r="C43" s="3" t="s">
-        <v>242</v>
+        <v>243</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>244</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>245</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A44" s="1" t="s">
-        <v>243</v>
-      </c>
-      <c r="B44" s="3" t="s">
-        <v>244</v>
-      </c>
-      <c r="C44" s="3" t="s">
-        <v>245</v>
+        <v>246</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>248</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A45" s="1" t="s">
-        <v>246</v>
-      </c>
-      <c r="B45" s="3" t="s">
-        <v>247</v>
-      </c>
-      <c r="C45" s="3" t="s">
-        <v>248</v>
+        <v>249</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>251</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A46" s="1" t="s">
-        <v>249</v>
-      </c>
-      <c r="B46" s="3" t="s">
-        <v>250</v>
-      </c>
-      <c r="C46" s="3" t="s">
-        <v>251</v>
+        <v>252</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>254</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A47" s="1" t="s">
-        <v>252</v>
-      </c>
-      <c r="B47" s="3" t="s">
-        <v>253</v>
-      </c>
-      <c r="C47" s="3" t="s">
-        <v>254</v>
+        <v>255</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>256</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>257</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A48" s="1" t="s">
-        <v>255</v>
-      </c>
-      <c r="B48" s="3" t="s">
-        <v>256</v>
-      </c>
-      <c r="C48" s="3" t="s">
-        <v>257</v>
+        <v>258</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>260</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A49" s="1" t="s">
-        <v>258</v>
-      </c>
-      <c r="B49" s="3" t="s">
-        <v>259</v>
-      </c>
-      <c r="C49" s="3" t="s">
-        <v>260</v>
+        <v>261</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>263</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A50" s="1" t="s">
-        <v>261</v>
-      </c>
-      <c r="B50" s="3" t="s">
-        <v>262</v>
-      </c>
-      <c r="C50" s="3" t="s">
-        <v>263</v>
+        <v>264</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>265</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>266</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A51" s="1" t="s">
-        <v>264</v>
-      </c>
-      <c r="B51" s="3" t="s">
-        <v>265</v>
-      </c>
-      <c r="C51" s="3" t="s">
-        <v>266</v>
+        <v>267</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>268</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>269</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A52" s="1" t="s">
-        <v>267</v>
-      </c>
-      <c r="B52" s="3" t="s">
-        <v>268</v>
-      </c>
-      <c r="C52" s="3" t="s">
-        <v>269</v>
+        <v>270</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>272</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A53" s="1" t="s">
-        <v>270</v>
-      </c>
-      <c r="B53" s="3" t="s">
-        <v>271</v>
-      </c>
-      <c r="C53" s="3" t="s">
-        <v>272</v>
+        <v>273</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>274</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>275</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A54" s="1" t="s">
-        <v>273</v>
-      </c>
-      <c r="B54" s="3" t="s">
-        <v>274</v>
-      </c>
-      <c r="C54" s="3" t="s">
-        <v>275</v>
+        <v>276</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>277</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>278</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A55" s="1" t="s">
-        <v>276</v>
-      </c>
-      <c r="B55" s="3" t="s">
-        <v>277</v>
-      </c>
-      <c r="C55" s="3" t="s">
-        <v>278</v>
+        <v>279</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>280</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>281</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A56" s="1" t="s">
-        <v>279</v>
-      </c>
-      <c r="B56" s="3" t="s">
-        <v>280</v>
-      </c>
-      <c r="C56" s="3" t="s">
-        <v>281</v>
+        <v>282</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>283</v>
+      </c>
+      <c r="C56" s="2" t="s">
+        <v>284</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A57" s="1" t="s">
-        <v>282</v>
-      </c>
-      <c r="B57" s="3" t="s">
-        <v>283</v>
-      </c>
-      <c r="C57" s="3" t="s">
-        <v>284</v>
+        <v>285</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>286</v>
+      </c>
+      <c r="C57" s="2" t="s">
+        <v>287</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A58" s="1" t="s">
-        <v>285</v>
-      </c>
-      <c r="B58" s="3" t="s">
-        <v>286</v>
-      </c>
-      <c r="C58" s="3" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
+        <v>288</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>289</v>
+      </c>
+      <c r="C58" s="2" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A59" s="1" t="s">
-        <v>288</v>
-      </c>
-      <c r="B59" s="3" t="s">
-        <v>289</v>
-      </c>
-      <c r="C59" s="3" t="s">
-        <v>290</v>
+        <v>291</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>292</v>
+      </c>
+      <c r="C59" s="2" t="s">
+        <v>293</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A60" s="1" t="s">
-        <v>291</v>
-      </c>
-      <c r="B60" s="3" t="s">
-        <v>292</v>
-      </c>
-      <c r="C60" s="3" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.35">
+        <v>294</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>295</v>
+      </c>
+      <c r="C60" s="2" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A61" s="1" t="s">
-        <v>294</v>
-      </c>
-      <c r="B61" s="3" t="s">
-        <v>295</v>
-      </c>
-      <c r="C61" s="3" t="s">
-        <v>296</v>
+        <v>297</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="C61" s="2" t="s">
+        <v>299</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A62" s="1" t="s">
-        <v>297</v>
-      </c>
-      <c r="B62" s="3" t="s">
-        <v>298</v>
-      </c>
-      <c r="C62" s="3" t="s">
-        <v>299</v>
+        <v>300</v>
+      </c>
+      <c r="B62" s="2" t="s">
+        <v>301</v>
+      </c>
+      <c r="C62" s="2" t="s">
+        <v>302</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A63" s="1" t="s">
-        <v>300</v>
-      </c>
-      <c r="B63" s="3" t="s">
-        <v>301</v>
-      </c>
-      <c r="C63" s="3" t="s">
-        <v>302</v>
+        <v>303</v>
+      </c>
+      <c r="B63" s="2" t="s">
+        <v>304</v>
+      </c>
+      <c r="C63" s="2" t="s">
+        <v>305</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A64" s="1" t="s">
-        <v>303</v>
-      </c>
-      <c r="B64" s="3" t="s">
-        <v>304</v>
-      </c>
-      <c r="C64" s="3" t="s">
-        <v>305</v>
+        <v>306</v>
+      </c>
+      <c r="B64" s="2" t="s">
+        <v>307</v>
+      </c>
+      <c r="C64" s="2" t="s">
+        <v>308</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A65" s="1" t="s">
-        <v>306</v>
-      </c>
-      <c r="B65" s="3" t="s">
-        <v>307</v>
-      </c>
-      <c r="C65" s="3" t="s">
-        <v>308</v>
+        <v>309</v>
+      </c>
+      <c r="B65" s="2" t="s">
+        <v>310</v>
+      </c>
+      <c r="C65" s="2" t="s">
+        <v>311</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A66" s="1" t="s">
-        <v>309</v>
-      </c>
-      <c r="B66" s="3" t="s">
-        <v>310</v>
-      </c>
-      <c r="C66" s="3" t="s">
-        <v>311</v>
+        <v>312</v>
+      </c>
+      <c r="B66" s="2" t="s">
+        <v>313</v>
+      </c>
+      <c r="C66" s="2" t="s">
+        <v>314</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A67" s="1" t="s">
-        <v>312</v>
-      </c>
-      <c r="B67" s="3" t="s">
-        <v>313</v>
-      </c>
-      <c r="C67" s="3" t="s">
-        <v>314</v>
+        <v>315</v>
+      </c>
+      <c r="B67" s="2" t="s">
+        <v>316</v>
+      </c>
+      <c r="C67" s="2" t="s">
+        <v>317</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B68" s="3"/>
-      <c r="C68" s="3"/>
+      <c r="A68" s="1" t="s">
+        <v>318</v>
+      </c>
+      <c r="B68" s="2" t="s">
+        <v>319</v>
+      </c>
+      <c r="C68" s="2" t="s">
+        <v>320</v>
+      </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A69" s="1" t="s">
-        <v>315</v>
-      </c>
-      <c r="B69" s="3" t="s">
-        <v>316</v>
-      </c>
-      <c r="C69" s="3" t="s">
-        <v>317</v>
+        <v>321</v>
+      </c>
+      <c r="B69" s="2" t="s">
+        <v>322</v>
+      </c>
+      <c r="C69" s="2" t="s">
+        <v>323</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A70" s="1" t="s">
-        <v>318</v>
-      </c>
-      <c r="B70" s="3" t="s">
-        <v>319</v>
-      </c>
-      <c r="C70" s="3" t="s">
-        <v>320</v>
-      </c>
+      <c r="B70" s="2"/>
+      <c r="C70" s="2"/>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A71" s="1" t="s">
-        <v>321</v>
-      </c>
-      <c r="B71" s="3" t="s">
-        <v>322</v>
-      </c>
-      <c r="C71" s="3" t="s">
-        <v>323</v>
+        <v>324</v>
+      </c>
+      <c r="B71" s="2" t="s">
+        <v>325</v>
+      </c>
+      <c r="C71" s="2" t="s">
+        <v>326</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A72" s="1" t="s">
-        <v>324</v>
-      </c>
-      <c r="B72" s="3" t="s">
-        <v>325</v>
-      </c>
-      <c r="C72" s="3" t="s">
-        <v>326</v>
+        <v>327</v>
+      </c>
+      <c r="B72" s="2" t="s">
+        <v>328</v>
+      </c>
+      <c r="C72" s="2" t="s">
+        <v>329</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A73" s="1" t="s">
-        <v>327</v>
-      </c>
-      <c r="B73" s="3" t="s">
-        <v>328</v>
-      </c>
-      <c r="C73" s="3" t="s">
-        <v>329</v>
+        <v>330</v>
+      </c>
+      <c r="B73" s="2" t="s">
+        <v>331</v>
+      </c>
+      <c r="C73" s="2" t="s">
+        <v>332</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A74" s="1" t="s">
-        <v>330</v>
-      </c>
-      <c r="B74" s="3" t="s">
-        <v>331</v>
-      </c>
-      <c r="C74" s="3" t="s">
-        <v>332</v>
+        <v>333</v>
+      </c>
+      <c r="B74" s="2" t="s">
+        <v>334</v>
+      </c>
+      <c r="C74" s="2" t="s">
+        <v>335</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A75" s="1" t="s">
-        <v>333</v>
-      </c>
-      <c r="B75" s="3" t="s">
-        <v>334</v>
-      </c>
-      <c r="C75" s="3" t="s">
-        <v>335</v>
+        <v>336</v>
+      </c>
+      <c r="B75" s="2" t="s">
+        <v>337</v>
+      </c>
+      <c r="C75" s="2" t="s">
+        <v>338</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A76" s="1" t="s">
-        <v>336</v>
-      </c>
-      <c r="B76" s="3" t="s">
-        <v>337</v>
-      </c>
-      <c r="C76" s="3" t="s">
-        <v>338</v>
+        <v>339</v>
+      </c>
+      <c r="B76" s="2" t="s">
+        <v>340</v>
+      </c>
+      <c r="C76" s="2" t="s">
+        <v>341</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B77" s="3"/>
-      <c r="C77" s="3"/>
+      <c r="A77" s="1" t="s">
+        <v>342</v>
+      </c>
+      <c r="B77" s="2" t="s">
+        <v>343</v>
+      </c>
+      <c r="C77" s="2" t="s">
+        <v>344</v>
+      </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A78" s="1" t="s">
-        <v>339</v>
-      </c>
-      <c r="B78" s="3" t="s">
-        <v>340</v>
-      </c>
-      <c r="C78" s="3" t="s">
-        <v>341</v>
+        <v>345</v>
+      </c>
+      <c r="B78" s="2" t="s">
+        <v>346</v>
+      </c>
+      <c r="C78" s="2" t="s">
+        <v>347</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A79" s="1" t="s">
-        <v>342</v>
-      </c>
-      <c r="B79" s="3" t="s">
-        <v>343</v>
-      </c>
-      <c r="C79" s="3" t="s">
-        <v>344</v>
-      </c>
+      <c r="B79" s="2"/>
+      <c r="C79" s="2"/>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A80" s="1" t="s">
-        <v>345</v>
-      </c>
-      <c r="B80" s="3" t="s">
-        <v>346</v>
-      </c>
-      <c r="C80" s="3" t="s">
-        <v>347</v>
+        <v>348</v>
+      </c>
+      <c r="B80" s="2" t="s">
+        <v>349</v>
+      </c>
+      <c r="C80" s="2" t="s">
+        <v>350</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A81" s="1" t="s">
-        <v>348</v>
-      </c>
-      <c r="B81" s="3" t="s">
-        <v>349</v>
-      </c>
-      <c r="C81" s="3" t="s">
-        <v>350</v>
+        <v>351</v>
+      </c>
+      <c r="B81" s="2" t="s">
+        <v>352</v>
+      </c>
+      <c r="C81" s="2" t="s">
+        <v>353</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A82" s="1" t="s">
-        <v>351</v>
-      </c>
-      <c r="B82" s="3" t="s">
-        <v>352</v>
-      </c>
-      <c r="C82" s="3" t="s">
-        <v>353</v>
+        <v>354</v>
+      </c>
+      <c r="B82" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="C82" s="2" t="s">
+        <v>356</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A83" s="1" t="s">
-        <v>354</v>
-      </c>
-      <c r="B83" s="3" t="s">
-        <v>355</v>
-      </c>
-      <c r="C83" s="3" t="s">
-        <v>356</v>
+        <v>357</v>
+      </c>
+      <c r="B83" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="C83" s="2" t="s">
+        <v>359</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A84" s="1" t="s">
-        <v>357</v>
-      </c>
-      <c r="B84" s="3" t="s">
-        <v>358</v>
-      </c>
-      <c r="C84" s="3" t="s">
-        <v>359</v>
+        <v>360</v>
+      </c>
+      <c r="B84" s="2" t="s">
+        <v>361</v>
+      </c>
+      <c r="C84" s="2" t="s">
+        <v>362</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A85" s="1" t="s">
-        <v>360</v>
-      </c>
-      <c r="B85" s="3" t="s">
-        <v>361</v>
-      </c>
-      <c r="C85" s="3" t="s">
-        <v>362</v>
+        <v>363</v>
+      </c>
+      <c r="B85" s="2" t="s">
+        <v>364</v>
+      </c>
+      <c r="C85" s="2" t="s">
+        <v>365</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A86" s="1" t="s">
-        <v>363</v>
-      </c>
-      <c r="B86" s="3" t="s">
-        <v>364</v>
-      </c>
-      <c r="C86" s="3" t="s">
-        <v>365</v>
+        <v>366</v>
+      </c>
+      <c r="B86" s="2" t="s">
+        <v>367</v>
+      </c>
+      <c r="C86" s="2" t="s">
+        <v>368</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B87" s="3"/>
-      <c r="C87" s="3"/>
+      <c r="A87" s="1" t="s">
+        <v>369</v>
+      </c>
+      <c r="B87" s="2" t="s">
+        <v>370</v>
+      </c>
+      <c r="C87" s="2" t="s">
+        <v>371</v>
+      </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A88" s="1" t="s">
-        <v>366</v>
-      </c>
-      <c r="B88" s="3" t="s">
-        <v>367</v>
-      </c>
-      <c r="C88" s="3" t="s">
-        <v>368</v>
+        <v>372</v>
+      </c>
+      <c r="B88" s="2" t="s">
+        <v>373</v>
+      </c>
+      <c r="C88" s="2" t="s">
+        <v>374</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A89" s="1" t="s">
-        <v>369</v>
-      </c>
-      <c r="B89" s="3" t="s">
-        <v>370</v>
-      </c>
-      <c r="C89" s="3" t="s">
-        <v>371</v>
-      </c>
+      <c r="B89" s="2"/>
+      <c r="C89" s="2"/>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A90" s="1" t="s">
-        <v>372</v>
-      </c>
-      <c r="B90" s="3" t="s">
-        <v>373</v>
-      </c>
-      <c r="C90" s="3" t="s">
-        <v>374</v>
+        <v>375</v>
+      </c>
+      <c r="B90" s="2" t="s">
+        <v>376</v>
+      </c>
+      <c r="C90" s="2" t="s">
+        <v>377</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A91" s="1" t="s">
-        <v>375</v>
-      </c>
-      <c r="B91" s="3" t="s">
-        <v>376</v>
-      </c>
-      <c r="C91" s="3" t="s">
-        <v>377</v>
+        <v>378</v>
+      </c>
+      <c r="B91" s="2" t="s">
+        <v>379</v>
+      </c>
+      <c r="C91" s="2" t="s">
+        <v>380</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A92" s="1" t="s">
-        <v>378</v>
-      </c>
-      <c r="B92" s="3" t="s">
-        <v>379</v>
-      </c>
-      <c r="C92" s="3" t="s">
-        <v>380</v>
+        <v>381</v>
+      </c>
+      <c r="B92" s="2" t="s">
+        <v>382</v>
+      </c>
+      <c r="C92" s="2" t="s">
+        <v>383</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A93" s="1" t="s">
-        <v>381</v>
-      </c>
-      <c r="B93" s="3" t="s">
-        <v>382</v>
-      </c>
-      <c r="C93" s="3" t="s">
-        <v>383</v>
+        <v>384</v>
+      </c>
+      <c r="B93" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="C93" s="2" t="s">
+        <v>386</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A94" s="1" t="s">
-        <v>384</v>
-      </c>
-      <c r="B94" s="3" t="s">
-        <v>385</v>
-      </c>
-      <c r="C94" s="3" t="s">
-        <v>386</v>
+        <v>387</v>
+      </c>
+      <c r="B94" s="2" t="s">
+        <v>388</v>
+      </c>
+      <c r="C94" s="2" t="s">
+        <v>389</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A95" s="1" t="s">
-        <v>387</v>
-      </c>
-      <c r="B95" s="3" t="s">
-        <v>388</v>
-      </c>
-      <c r="C95" s="3" t="s">
-        <v>389</v>
+        <v>390</v>
+      </c>
+      <c r="B95" s="2" t="s">
+        <v>391</v>
+      </c>
+      <c r="C95" s="2" t="s">
+        <v>392</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B96" s="3"/>
-      <c r="C96" s="3"/>
+      <c r="A96" s="1" t="s">
+        <v>393</v>
+      </c>
+      <c r="B96" s="2" t="s">
+        <v>394</v>
+      </c>
+      <c r="C96" s="2" t="s">
+        <v>395</v>
+      </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A97" s="1" t="s">
-        <v>390</v>
-      </c>
-      <c r="B97" s="3" t="s">
-        <v>391</v>
-      </c>
-      <c r="C97" s="3" t="s">
-        <v>392</v>
+        <v>396</v>
+      </c>
+      <c r="B97" s="2" t="s">
+        <v>397</v>
+      </c>
+      <c r="C97" s="2" t="s">
+        <v>398</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A98" s="1" t="s">
-        <v>393</v>
-      </c>
-      <c r="B98" s="3" t="s">
-        <v>394</v>
-      </c>
-      <c r="C98" s="3" t="s">
-        <v>395</v>
-      </c>
+      <c r="B98" s="2"/>
+      <c r="C98" s="2"/>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A99" s="1" t="s">
-        <v>396</v>
-      </c>
-      <c r="B99" s="3" t="s">
-        <v>397</v>
-      </c>
-      <c r="C99" s="3" t="s">
-        <v>398</v>
+        <v>399</v>
+      </c>
+      <c r="B99" s="2" t="s">
+        <v>400</v>
+      </c>
+      <c r="C99" s="2" t="s">
+        <v>401</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A100" s="1" t="s">
-        <v>399</v>
-      </c>
-      <c r="B100" s="3" t="s">
-        <v>400</v>
-      </c>
-      <c r="C100" s="3" t="s">
-        <v>401</v>
+        <v>402</v>
+      </c>
+      <c r="B100" s="2" t="s">
+        <v>403</v>
+      </c>
+      <c r="C100" s="2" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A101" s="1" t="s">
+        <v>405</v>
+      </c>
+      <c r="B101" s="2" t="s">
+        <v>406</v>
+      </c>
+      <c r="C101" s="2" t="s">
+        <v>407</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A102" s="1" t="s">
-        <v>402</v>
-      </c>
-      <c r="B102" s="3" t="s">
-        <v>403</v>
-      </c>
-      <c r="C102" s="3" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A103" s="1" t="s">
-        <v>405</v>
-      </c>
-      <c r="B103" s="3" t="s">
-        <v>406</v>
-      </c>
-      <c r="C103" s="3" t="s">
-        <v>407</v>
+        <v>408</v>
+      </c>
+      <c r="B102" s="2" t="s">
+        <v>409</v>
+      </c>
+      <c r="C102" s="2" t="s">
+        <v>410</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A104" s="1" t="s">
-        <v>408</v>
-      </c>
-      <c r="B104" s="3" t="s">
-        <v>409</v>
-      </c>
-      <c r="C104" s="3" t="s">
-        <v>410</v>
+        <v>411</v>
+      </c>
+      <c r="B104" s="2" t="s">
+        <v>412</v>
+      </c>
+      <c r="C104" s="2" t="s">
+        <v>413</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A105" s="1" t="s">
-        <v>411</v>
-      </c>
-      <c r="B105" s="3" t="s">
-        <v>412</v>
-      </c>
-      <c r="C105" s="3" t="s">
-        <v>413</v>
+        <v>414</v>
+      </c>
+      <c r="B105" s="2" t="s">
+        <v>415</v>
+      </c>
+      <c r="C105" s="2" t="s">
+        <v>416</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A106" s="1" t="s">
-        <v>414</v>
-      </c>
-      <c r="B106" s="3" t="s">
-        <v>415</v>
-      </c>
-      <c r="C106" s="3" t="s">
-        <v>416</v>
+        <v>417</v>
+      </c>
+      <c r="B106" s="2" t="s">
+        <v>418</v>
+      </c>
+      <c r="C106" s="2" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A107" s="1" t="s">
+        <v>420</v>
+      </c>
+      <c r="B107" s="2" t="s">
+        <v>421</v>
+      </c>
+      <c r="C107" s="2" t="s">
+        <v>422</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A108" s="1" t="s">
-        <v>417</v>
-      </c>
-      <c r="B108" s="3" t="s">
-        <v>418</v>
-      </c>
-      <c r="C108" s="3" t="s">
-        <v>419</v>
-      </c>
-    </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A109" s="1" t="s">
-        <v>420</v>
-      </c>
-      <c r="B109" s="1" t="s">
-        <v>421</v>
-      </c>
-      <c r="C109" s="1" t="s">
-        <v>422</v>
+        <v>423</v>
+      </c>
+      <c r="B108" s="2" t="s">
+        <v>424</v>
+      </c>
+      <c r="C108" s="2" t="s">
+        <v>425</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A110" s="1" t="s">
-        <v>423</v>
-      </c>
-      <c r="B110" s="1" t="s">
-        <v>424</v>
-      </c>
-      <c r="C110" s="1" t="s">
-        <v>425</v>
+        <v>426</v>
+      </c>
+      <c r="B110" s="2" t="s">
+        <v>427</v>
+      </c>
+      <c r="C110" s="2" t="s">
+        <v>428</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A111" s="1" t="s">
-        <v>426</v>
-      </c>
-      <c r="B111" s="3" t="s">
-        <v>427</v>
+        <v>429</v>
+      </c>
+      <c r="B111" s="1" t="s">
+        <v>430</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>428</v>
+        <v>431</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A112" s="1" t="s">
-        <v>429</v>
+        <v>432</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>430</v>
+        <v>433</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>431</v>
+        <v>434</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A113" s="1" t="s">
-        <v>432</v>
-      </c>
-      <c r="B113" s="3" t="s">
-        <v>433</v>
-      </c>
-      <c r="C113" s="3" t="s">
-        <v>434</v>
+        <v>435</v>
+      </c>
+      <c r="B113" s="2" t="s">
+        <v>436</v>
+      </c>
+      <c r="C113" s="1" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A114" s="1" t="s">
+        <v>438</v>
+      </c>
+      <c r="B114" s="1" t="s">
+        <v>439</v>
+      </c>
+      <c r="C114" s="1" t="s">
+        <v>440</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A115" s="1" t="s">
-        <v>435</v>
-      </c>
-      <c r="B115" s="3" t="s">
-        <v>436</v>
-      </c>
-      <c r="C115" s="3" t="s">
-        <v>437</v>
-      </c>
-    </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A116" s="1" t="s">
-        <v>438</v>
-      </c>
-      <c r="B116" s="3" t="s">
-        <v>439</v>
-      </c>
-      <c r="C116" s="3" t="s">
-        <v>440</v>
+        <v>441</v>
+      </c>
+      <c r="B115" s="2" t="s">
+        <v>442</v>
+      </c>
+      <c r="C115" s="2" t="s">
+        <v>443</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B117" s="3"/>
-      <c r="C117" s="3"/>
+      <c r="A117" s="1" t="s">
+        <v>444</v>
+      </c>
+      <c r="B117" s="2" t="s">
+        <v>445</v>
+      </c>
+      <c r="C117" s="2" t="s">
+        <v>446</v>
+      </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A118" s="1" t="s">
-        <v>441</v>
-      </c>
-      <c r="B118" s="3" t="s">
-        <v>442</v>
-      </c>
-      <c r="C118" s="3" t="s">
-        <v>443</v>
+        <v>447</v>
+      </c>
+      <c r="B118" s="2" t="s">
+        <v>448</v>
+      </c>
+      <c r="C118" s="2" t="s">
+        <v>449</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A119" s="1" t="s">
-        <v>444</v>
-      </c>
-      <c r="B119" s="3" t="s">
-        <v>445</v>
-      </c>
-      <c r="C119" s="3" t="s">
-        <v>446</v>
-      </c>
+      <c r="B119" s="2"/>
+      <c r="C119" s="2"/>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A120" s="1" t="s">
-        <v>447</v>
-      </c>
-      <c r="B120" s="3" t="s">
-        <v>448</v>
-      </c>
-      <c r="C120" s="3" t="s">
-        <v>449</v>
+        <v>450</v>
+      </c>
+      <c r="B120" s="2" t="s">
+        <v>451</v>
+      </c>
+      <c r="C120" s="2" t="s">
+        <v>452</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A121" s="1" t="s">
-        <v>450</v>
-      </c>
-      <c r="B121" s="3" t="s">
-        <v>451</v>
-      </c>
-      <c r="C121" s="3" t="s">
-        <v>452</v>
+        <v>453</v>
+      </c>
+      <c r="B121" s="2" t="s">
+        <v>454</v>
+      </c>
+      <c r="C121" s="2" t="s">
+        <v>455</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A122" s="1" t="s">
-        <v>453</v>
-      </c>
-      <c r="B122" s="3" t="s">
-        <v>454</v>
-      </c>
-      <c r="C122" s="3" t="s">
-        <v>455</v>
+        <v>456</v>
+      </c>
+      <c r="B122" s="2" t="s">
+        <v>457</v>
+      </c>
+      <c r="C122" s="2" t="s">
+        <v>458</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B123" s="3"/>
-      <c r="C123" s="3"/>
+      <c r="A123" s="1" t="s">
+        <v>459</v>
+      </c>
+      <c r="B123" s="2" t="s">
+        <v>460</v>
+      </c>
+      <c r="C123" s="2" t="s">
+        <v>461</v>
+      </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A124" s="1" t="s">
-        <v>456</v>
-      </c>
-      <c r="B124" s="3" t="s">
-        <v>457</v>
-      </c>
-      <c r="C124" s="3" t="s">
-        <v>458</v>
+        <v>462</v>
+      </c>
+      <c r="B124" s="2" t="s">
+        <v>463</v>
+      </c>
+      <c r="C124" s="2" t="s">
+        <v>464</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A125" s="1" t="s">
-        <v>459</v>
-      </c>
-      <c r="B125" s="3" t="s">
-        <v>460</v>
-      </c>
-      <c r="C125" s="3" t="s">
-        <v>461</v>
+      <c r="B125" s="2"/>
+      <c r="C125" s="2"/>
+    </row>
+    <row r="126" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A126" s="1" t="s">
+        <v>465</v>
+      </c>
+      <c r="B126" s="2" t="s">
+        <v>466</v>
+      </c>
+      <c r="C126" s="2" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A127" s="1" t="s">
+        <v>468</v>
+      </c>
+      <c r="B127" s="2" t="s">
+        <v>469</v>
+      </c>
+      <c r="C127" s="2" t="s">
+        <v>470</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Support manipulation of Folders
</commit_message>
<xml_diff>
--- a/Config.xlsx
+++ b/Config.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22827"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mateus.cruz\Documents\GitHub\OrchestratorManager\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77989E0F-5668-40CA-861F-0F36CA5FEFF3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FD507EB-60A6-4843-8EC4-65AECFC624A1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="509" uniqueCount="474">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="552" uniqueCount="514">
   <si>
     <t>Name</t>
   </si>
@@ -54,9 +54,6 @@
   </si>
   <si>
     <t>TenantName</t>
-  </si>
-  <si>
-    <t>Default</t>
   </si>
   <si>
     <t>Name of the tenant to be used. 
@@ -72,6 +69,9 @@
   </si>
   <si>
     <t>OnPremisesOrchestratorVersion</t>
+  </si>
+  <si>
+    <t>202004</t>
   </si>
   <si>
     <t>Version of the Orchestrator instance to be used. 
@@ -419,6 +419,9 @@
     <t>B</t>
   </si>
   <si>
+    <t>Column to which the ID of the created Orgnization Unit should be written.</t>
+  </si>
+  <si>
     <t>CreateOrganizationUnitResultColumn</t>
   </si>
   <si>
@@ -431,6 +434,24 @@
     <t>Column to which the result of the Delete Organization Unit operation should be written.</t>
   </si>
   <si>
+    <t>CreateFolderIDColumn</t>
+  </si>
+  <si>
+    <t>Column to which the ID of the created Folder should be written.</t>
+  </si>
+  <si>
+    <t>CreateFolderResultColumn</t>
+  </si>
+  <si>
+    <t>Column to which the result of the Create Folder operation should be written.</t>
+  </si>
+  <si>
+    <t>DeleteFolderResultColumn</t>
+  </si>
+  <si>
+    <t>Column to which the result of the Delete Folder operation should be written.</t>
+  </si>
+  <si>
     <t>EN</t>
   </si>
   <si>
@@ -575,6 +596,15 @@
     <t>組織単位</t>
   </si>
   <si>
+    <t>FormFolderLabel</t>
+  </si>
+  <si>
+    <t>Folders</t>
+  </si>
+  <si>
+    <t>フォルダー</t>
+  </si>
+  <si>
     <t>FormUseSavedCredentialLabel</t>
   </si>
   <si>
@@ -653,6 +683,12 @@
     <t>Organization Unit</t>
   </si>
   <si>
+    <t>FormFolderOption</t>
+  </si>
+  <si>
+    <t>Folder</t>
+  </si>
+  <si>
     <t>FormSubmitButton</t>
   </si>
   <si>
@@ -731,6 +767,15 @@
     <t>JA\組織単位.xlsx</t>
   </si>
   <si>
+    <t>FolderConfigFilePath</t>
+  </si>
+  <si>
+    <t>EN\Folders.xlsx</t>
+  </si>
+  <si>
+    <t>JA\フォルダー.xlsx</t>
+  </si>
+  <si>
     <t>GetOperationName</t>
   </si>
   <si>
@@ -1016,7 +1061,16 @@
     <t>Type not specified.</t>
   </si>
   <si>
-    <t>タイプが指定されませんでした。</t>
+    <t>タイプ（種類）が指定されませんでした。</t>
+  </si>
+  <si>
+    <t>TypeNotSupported</t>
+  </si>
+  <si>
+    <t>The specified type is not supported.</t>
+  </si>
+  <si>
+    <t>指定されたタイプ（種類）はサポートされていません。</t>
   </si>
   <si>
     <t>UnsupportedAssetType</t>
@@ -1280,6 +1334,69 @@
     <t>{0}というマシンが見つかりませんでした。</t>
   </si>
   <si>
+    <t>FolderNotFound</t>
+  </si>
+  <si>
+    <t>No Folder found.</t>
+  </si>
+  <si>
+    <t>フォルダーが見つかりませんでした。</t>
+  </si>
+  <si>
+    <t>FolderIDInvalidOrNotSpecified</t>
+  </si>
+  <si>
+    <t>Folder ID invalid or not specified.</t>
+  </si>
+  <si>
+    <t>フォルダーIDが無効か指定されませんでした。</t>
+  </si>
+  <si>
+    <t>FolderNameNotSpecified</t>
+  </si>
+  <si>
+    <t>Folder name not specified.</t>
+  </si>
+  <si>
+    <t>フォルダー名が指定されませんでした。</t>
+  </si>
+  <si>
+    <t>FolderIDAndNameDoNotMatch</t>
+  </si>
+  <si>
+    <t>The specified Folder ID and Folder name do not match.</t>
+  </si>
+  <si>
+    <t>指定されたフォルダー名とフォルダーIDが一致しません。</t>
+  </si>
+  <si>
+    <t>NamedFolderNotFound</t>
+  </si>
+  <si>
+    <t>Folder named {0} not found.</t>
+  </si>
+  <si>
+    <t>{0}というフォルダーが見つかりませんでした。</t>
+  </si>
+  <si>
+    <t>RoleAssignmentModelNotSpecified</t>
+  </si>
+  <si>
+    <t>Role Assignment Model not specified.</t>
+  </si>
+  <si>
+    <t>ロール割り当てモデルが指定されませんでした。</t>
+  </si>
+  <si>
+    <t>RoleAssignmentModelNotSupported</t>
+  </si>
+  <si>
+    <t>The specified Role Assignment Model is not supported.</t>
+  </si>
+  <si>
+    <t>指定されたロール割り当てモデルはサポートされていません。</t>
+  </si>
+  <si>
     <t>OUNotFound</t>
   </si>
   <si>
@@ -1461,6 +1578,9 @@
   </si>
   <si>
     <t>Workbooks</t>
+  </si>
+  <si>
+    <t>Default</t>
   </si>
   <si>
     <t>https://myOrchestratorURL</t>
@@ -1507,18 +1627,21 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1547,8 +1670,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table1" displayName="Table1" ref="A1:C50" totalsRowShown="0">
-  <autoFilter ref="A1:C50" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table1" displayName="Table1" ref="A1:C53" totalsRowShown="0">
+  <autoFilter ref="A1:C53" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Name"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Value"/>
@@ -1559,8 +1682,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table13" displayName="Table13" ref="A1:C127" totalsRowShown="0">
-  <autoFilter ref="A1:C127" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table13" displayName="Table13" ref="A1:C139" totalsRowShown="0">
+  <autoFilter ref="A1:C139" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Name"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="EN"/>
@@ -1862,7 +1985,7 @@
         <v>3</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>471</v>
+        <v>510</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>4</v>
@@ -1873,29 +1996,29 @@
         <v>5</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>511</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>6</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="58" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>512</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>8</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>472</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="101.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>10</v>
-      </c>
-      <c r="B6" s="1">
-        <v>201910</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>11</v>
@@ -1906,24 +2029,27 @@
         <v>12</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>473</v>
+        <v>513</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>13</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B5" r:id="rId1" xr:uid="{74E87DF3-3663-4772-9B1C-21DEA2FCAA51}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C50"/>
+  <dimension ref="A1:C53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2 A2"/>
@@ -2461,29 +2587,62 @@
         <v>123</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>113</v>
+        <v>124</v>
       </c>
     </row>
     <row r="49" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A49" s="1" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B49" s="1" t="s">
         <v>60</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
     </row>
     <row r="50" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A50" s="1" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B50" s="1" t="s">
         <v>60</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>127</v>
+        <v>128</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A51" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A52" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A53" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>134</v>
       </c>
     </row>
   </sheetData>
@@ -2501,7 +2660,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1927ABA9-1814-4487-9CEC-ABDCAF91481F}">
-  <dimension ref="A1:C127"/>
+  <dimension ref="A1:C139"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2 A2"/>
@@ -2519,1307 +2678,1428 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>128</v>
+        <v>135</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>129</v>
+        <v>136</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>130</v>
+        <v>137</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>131</v>
+        <v>138</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>131</v>
+        <v>138</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="43.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>132</v>
+        <v>139</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>133</v>
+        <v>140</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>134</v>
+        <v>141</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>135</v>
+        <v>142</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>136</v>
+        <v>143</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>137</v>
+        <v>144</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>138</v>
+        <v>145</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>139</v>
+        <v>146</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>139</v>
+        <v>146</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
-        <v>140</v>
+        <v>147</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>141</v>
+        <v>148</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>142</v>
+        <v>149</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
-        <v>143</v>
+        <v>150</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>144</v>
+        <v>151</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>145</v>
+        <v>152</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
-        <v>146</v>
+        <v>153</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>147</v>
+        <v>154</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>148</v>
+        <v>155</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
-        <v>149</v>
+        <v>156</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>150</v>
+        <v>157</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>151</v>
+        <v>158</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
-        <v>152</v>
+        <v>159</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>153</v>
+        <v>160</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>154</v>
+        <v>161</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
-        <v>155</v>
+        <v>162</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>156</v>
+        <v>163</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>157</v>
+        <v>164</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
-        <v>158</v>
+        <v>165</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>159</v>
+        <v>166</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>160</v>
+        <v>167</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
-        <v>161</v>
+        <v>168</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>162</v>
+        <v>169</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>163</v>
+        <v>170</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
-        <v>164</v>
+        <v>171</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>165</v>
+        <v>172</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>166</v>
+        <v>173</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
-        <v>167</v>
+        <v>174</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>168</v>
+        <v>175</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>169</v>
+        <v>176</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
-        <v>170</v>
+        <v>177</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>171</v>
+        <v>178</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>172</v>
+        <v>179</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
-        <v>173</v>
+        <v>180</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>174</v>
+        <v>181</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>175</v>
+        <v>182</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
-        <v>176</v>
+        <v>183</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>177</v>
+        <v>184</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>178</v>
+        <v>185</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
-        <v>179</v>
+        <v>186</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>180</v>
+        <v>187</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>181</v>
+        <v>188</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
-        <v>182</v>
+        <v>189</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>183</v>
+        <v>190</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>184</v>
+        <v>191</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
-        <v>185</v>
+        <v>192</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>186</v>
+        <v>193</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>187</v>
+        <v>194</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
-        <v>188</v>
+        <v>195</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>189</v>
+        <v>196</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>190</v>
+        <v>197</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
-        <v>191</v>
+        <v>198</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>192</v>
+        <v>199</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>193</v>
+        <v>200</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
-        <v>194</v>
+        <v>201</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>195</v>
+        <v>202</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>196</v>
+        <v>203</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
-        <v>197</v>
+        <v>204</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>198</v>
+        <v>205</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>199</v>
+        <v>206</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
-        <v>200</v>
+        <v>207</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>201</v>
+        <v>208</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>175</v>
+        <v>209</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
-        <v>202</v>
+        <v>210</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>203</v>
+        <v>211</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>203</v>
+        <v>182</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="s">
-        <v>204</v>
+        <v>212</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>205</v>
+        <v>213</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>206</v>
+        <v>185</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B29" s="2"/>
-      <c r="C29" s="2"/>
+      <c r="A29" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>215</v>
+      </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A30" s="1" t="s">
-        <v>207</v>
+        <v>216</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>208</v>
+        <v>217</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>209</v>
+        <v>218</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A31" s="1" t="s">
-        <v>210</v>
-      </c>
-      <c r="B31" s="2" t="s">
-        <v>211</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>212</v>
-      </c>
+      <c r="B31" s="2"/>
+      <c r="C31" s="2"/>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A32" s="1" t="s">
-        <v>213</v>
+        <v>219</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>214</v>
+        <v>220</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>215</v>
+        <v>221</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A33" s="1" t="s">
-        <v>216</v>
+        <v>222</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>217</v>
+        <v>223</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>218</v>
+        <v>224</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A34" s="1" t="s">
-        <v>219</v>
+        <v>225</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>220</v>
+        <v>226</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>221</v>
+        <v>227</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A35" s="1" t="s">
-        <v>222</v>
+        <v>228</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>223</v>
+        <v>229</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>224</v>
+        <v>230</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A36" s="1" t="s">
-        <v>225</v>
+        <v>231</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>226</v>
+        <v>232</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>227</v>
+        <v>233</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B37" s="2"/>
-      <c r="C37" s="2"/>
+      <c r="A37" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>236</v>
+      </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A38" s="1" t="s">
-        <v>228</v>
+        <v>237</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>229</v>
+        <v>238</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>230</v>
+        <v>239</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A39" s="1" t="s">
-        <v>231</v>
+        <v>240</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>232</v>
+        <v>241</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>233</v>
+        <v>242</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A40" s="1" t="s">
-        <v>234</v>
-      </c>
-      <c r="B40" s="2" t="s">
-        <v>235</v>
-      </c>
-      <c r="C40" s="2" t="s">
-        <v>236</v>
-      </c>
+      <c r="B40" s="2"/>
+      <c r="C40" s="2"/>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A41" s="1" t="s">
-        <v>237</v>
+        <v>243</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>238</v>
+        <v>244</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>239</v>
+        <v>245</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A42" s="1" t="s">
-        <v>240</v>
+        <v>246</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>241</v>
+        <v>247</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>242</v>
+        <v>248</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A43" s="1" t="s">
-        <v>243</v>
+        <v>249</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>244</v>
+        <v>250</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>245</v>
+        <v>251</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A44" s="1" t="s">
-        <v>246</v>
+        <v>252</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>247</v>
+        <v>253</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>248</v>
+        <v>254</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A45" s="1" t="s">
-        <v>249</v>
+        <v>255</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>250</v>
+        <v>256</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>251</v>
+        <v>257</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A46" s="1" t="s">
-        <v>252</v>
+        <v>258</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>253</v>
+        <v>259</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>254</v>
+        <v>260</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A47" s="1" t="s">
-        <v>255</v>
+        <v>261</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>256</v>
+        <v>262</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>257</v>
+        <v>263</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A48" s="1" t="s">
-        <v>258</v>
+        <v>264</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>259</v>
+        <v>265</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>260</v>
+        <v>266</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A49" s="1" t="s">
-        <v>261</v>
+        <v>267</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>262</v>
+        <v>268</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>263</v>
+        <v>269</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A50" s="1" t="s">
-        <v>264</v>
+        <v>270</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>265</v>
+        <v>271</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>266</v>
+        <v>272</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A51" s="1" t="s">
-        <v>267</v>
+        <v>273</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>268</v>
+        <v>274</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>269</v>
+        <v>275</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A52" s="1" t="s">
-        <v>270</v>
+        <v>276</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>271</v>
+        <v>277</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>272</v>
+        <v>278</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A53" s="1" t="s">
-        <v>273</v>
+        <v>279</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>274</v>
+        <v>280</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>275</v>
+        <v>281</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A54" s="1" t="s">
-        <v>276</v>
+        <v>282</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>277</v>
+        <v>283</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>278</v>
+        <v>284</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A55" s="1" t="s">
-        <v>279</v>
+        <v>285</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>280</v>
+        <v>286</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>281</v>
+        <v>287</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A56" s="1" t="s">
-        <v>282</v>
+        <v>288</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>283</v>
+        <v>289</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>284</v>
+        <v>290</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A57" s="1" t="s">
-        <v>285</v>
+        <v>291</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>286</v>
+        <v>292</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>287</v>
+        <v>293</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A58" s="1" t="s">
-        <v>288</v>
+        <v>294</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>289</v>
+        <v>295</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>290</v>
+        <v>296</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A59" s="1" t="s">
-        <v>291</v>
+        <v>297</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>292</v>
+        <v>298</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>293</v>
+        <v>299</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A60" s="1" t="s">
-        <v>294</v>
+        <v>300</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>295</v>
+        <v>301</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A61" s="1" t="s">
-        <v>297</v>
+        <v>303</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>298</v>
+        <v>304</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>299</v>
+        <v>305</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A62" s="1" t="s">
-        <v>300</v>
+        <v>306</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>301</v>
+        <v>307</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>302</v>
+        <v>308</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A63" s="1" t="s">
-        <v>303</v>
+        <v>309</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>304</v>
+        <v>310</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.35">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A64" s="1" t="s">
-        <v>306</v>
+        <v>312</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>307</v>
+        <v>313</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>308</v>
+        <v>314</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A65" s="1" t="s">
-        <v>309</v>
+        <v>315</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>310</v>
+        <v>316</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>311</v>
+        <v>317</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A66" s="1" t="s">
-        <v>312</v>
+        <v>318</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>313</v>
+        <v>319</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>314</v>
+        <v>320</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A67" s="1" t="s">
-        <v>315</v>
+        <v>321</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>316</v>
+        <v>322</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>317</v>
+        <v>323</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A68" s="1" t="s">
-        <v>318</v>
+        <v>324</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>319</v>
+        <v>325</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>320</v>
+        <v>326</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A69" s="1" t="s">
-        <v>321</v>
+        <v>327</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>322</v>
+        <v>328</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>323</v>
+        <v>329</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B70" s="2"/>
-      <c r="C70" s="2"/>
+      <c r="A70" s="1" t="s">
+        <v>330</v>
+      </c>
+      <c r="B70" s="2" t="s">
+        <v>331</v>
+      </c>
+      <c r="C70" s="2" t="s">
+        <v>332</v>
+      </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A71" s="1" t="s">
-        <v>324</v>
+        <v>333</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>325</v>
+        <v>334</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>326</v>
+        <v>335</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A72" s="1" t="s">
-        <v>327</v>
+        <v>336</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>328</v>
+        <v>337</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>329</v>
+        <v>338</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A73" s="1" t="s">
-        <v>330</v>
+        <v>339</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>331</v>
+        <v>340</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>332</v>
+        <v>341</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A74" s="1" t="s">
-        <v>333</v>
-      </c>
-      <c r="B74" s="2" t="s">
-        <v>334</v>
-      </c>
-      <c r="C74" s="2" t="s">
-        <v>335</v>
-      </c>
+      <c r="B74" s="2"/>
+      <c r="C74" s="2"/>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A75" s="1" t="s">
-        <v>336</v>
+        <v>342</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>337</v>
+        <v>343</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>338</v>
+        <v>344</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A76" s="1" t="s">
-        <v>339</v>
+        <v>345</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>340</v>
+        <v>346</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>341</v>
+        <v>347</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A77" s="1" t="s">
-        <v>342</v>
+        <v>348</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>343</v>
+        <v>349</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>344</v>
+        <v>350</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A78" s="1" t="s">
-        <v>345</v>
+        <v>351</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>346</v>
+        <v>352</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>347</v>
+        <v>353</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B79" s="2"/>
-      <c r="C79" s="2"/>
+      <c r="A79" s="1" t="s">
+        <v>354</v>
+      </c>
+      <c r="B79" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="C79" s="2" t="s">
+        <v>356</v>
+      </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A80" s="1" t="s">
-        <v>348</v>
+        <v>357</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>349</v>
+        <v>358</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>350</v>
+        <v>359</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A81" s="1" t="s">
-        <v>351</v>
+        <v>360</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>352</v>
+        <v>361</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>353</v>
+        <v>362</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A82" s="1" t="s">
-        <v>354</v>
+        <v>363</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>355</v>
+        <v>364</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>356</v>
+        <v>365</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A83" s="1" t="s">
-        <v>357</v>
-      </c>
-      <c r="B83" s="2" t="s">
-        <v>358</v>
-      </c>
-      <c r="C83" s="2" t="s">
-        <v>359</v>
-      </c>
+      <c r="B83" s="2"/>
+      <c r="C83" s="2"/>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A84" s="1" t="s">
-        <v>360</v>
+        <v>366</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>361</v>
+        <v>367</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>362</v>
+        <v>368</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A85" s="1" t="s">
-        <v>363</v>
+        <v>369</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>364</v>
+        <v>370</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>365</v>
+        <v>371</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A86" s="1" t="s">
-        <v>366</v>
+        <v>372</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>367</v>
+        <v>373</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>368</v>
+        <v>374</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A87" s="1" t="s">
-        <v>369</v>
+        <v>375</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>370</v>
+        <v>376</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>371</v>
+        <v>377</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A88" s="1" t="s">
-        <v>372</v>
+        <v>378</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>373</v>
+        <v>379</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>374</v>
+        <v>380</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B89" s="2"/>
-      <c r="C89" s="2"/>
+      <c r="A89" s="1" t="s">
+        <v>381</v>
+      </c>
+      <c r="B89" s="2" t="s">
+        <v>382</v>
+      </c>
+      <c r="C89" s="2" t="s">
+        <v>383</v>
+      </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A90" s="1" t="s">
-        <v>375</v>
+        <v>384</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>376</v>
+        <v>385</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>377</v>
+        <v>386</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A91" s="1" t="s">
-        <v>378</v>
+        <v>387</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>379</v>
+        <v>388</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>380</v>
+        <v>389</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A92" s="1" t="s">
-        <v>381</v>
+        <v>390</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>382</v>
+        <v>391</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>383</v>
+        <v>392</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A93" s="1" t="s">
-        <v>384</v>
-      </c>
-      <c r="B93" s="2" t="s">
-        <v>385</v>
-      </c>
-      <c r="C93" s="2" t="s">
-        <v>386</v>
-      </c>
+      <c r="B93" s="2"/>
+      <c r="C93" s="2"/>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A94" s="1" t="s">
-        <v>387</v>
+        <v>393</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>388</v>
+        <v>394</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>389</v>
+        <v>395</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A95" s="1" t="s">
-        <v>390</v>
+        <v>396</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>391</v>
+        <v>397</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>392</v>
+        <v>398</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A96" s="1" t="s">
-        <v>393</v>
+        <v>399</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>394</v>
+        <v>400</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>395</v>
+        <v>401</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A97" s="1" t="s">
-        <v>396</v>
+        <v>402</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>397</v>
+        <v>403</v>
       </c>
       <c r="C97" s="2" t="s">
-        <v>398</v>
+        <v>404</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B98" s="2"/>
-      <c r="C98" s="2"/>
+      <c r="A98" s="1" t="s">
+        <v>405</v>
+      </c>
+      <c r="B98" s="2" t="s">
+        <v>406</v>
+      </c>
+      <c r="C98" s="2" t="s">
+        <v>407</v>
+      </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A99" s="1" t="s">
-        <v>399</v>
+        <v>408</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>400</v>
+        <v>409</v>
       </c>
       <c r="C99" s="2" t="s">
-        <v>401</v>
+        <v>410</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A100" s="1" t="s">
-        <v>402</v>
+        <v>411</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>403</v>
+        <v>412</v>
       </c>
       <c r="C100" s="2" t="s">
-        <v>404</v>
+        <v>413</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A101" s="1" t="s">
-        <v>405</v>
+        <v>414</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>406</v>
+        <v>415</v>
       </c>
       <c r="C101" s="2" t="s">
-        <v>407</v>
+        <v>416</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A102" s="1" t="s">
-        <v>408</v>
-      </c>
-      <c r="B102" s="2" t="s">
-        <v>409</v>
-      </c>
-      <c r="C102" s="2" t="s">
-        <v>410</v>
+      <c r="B102" s="2"/>
+      <c r="C102" s="2"/>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A103" s="1" t="s">
+        <v>417</v>
+      </c>
+      <c r="B103" s="2" t="s">
+        <v>418</v>
+      </c>
+      <c r="C103" s="2" t="s">
+        <v>419</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A104" s="1" t="s">
-        <v>411</v>
+        <v>420</v>
       </c>
       <c r="B104" s="2" t="s">
-        <v>412</v>
+        <v>421</v>
       </c>
       <c r="C104" s="2" t="s">
-        <v>413</v>
+        <v>422</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A105" s="1" t="s">
-        <v>414</v>
+        <v>423</v>
       </c>
       <c r="B105" s="2" t="s">
-        <v>415</v>
+        <v>424</v>
       </c>
       <c r="C105" s="2" t="s">
-        <v>416</v>
+        <v>425</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A106" s="1" t="s">
-        <v>417</v>
+        <v>426</v>
       </c>
       <c r="B106" s="2" t="s">
-        <v>418</v>
+        <v>427</v>
       </c>
       <c r="C106" s="2" t="s">
-        <v>419</v>
-      </c>
-    </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A107" s="1" t="s">
-        <v>420</v>
-      </c>
-      <c r="B107" s="2" t="s">
-        <v>421</v>
-      </c>
-      <c r="C107" s="2" t="s">
-        <v>422</v>
+        <v>428</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A108" s="1" t="s">
-        <v>423</v>
+        <v>429</v>
       </c>
       <c r="B108" s="2" t="s">
-        <v>424</v>
+        <v>430</v>
       </c>
       <c r="C108" s="2" t="s">
-        <v>425</v>
+        <v>431</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A109" s="1" t="s">
+        <v>432</v>
+      </c>
+      <c r="B109" s="2" t="s">
+        <v>433</v>
+      </c>
+      <c r="C109" s="2" t="s">
+        <v>434</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A110" s="1" t="s">
-        <v>426</v>
+        <v>435</v>
       </c>
       <c r="B110" s="2" t="s">
-        <v>427</v>
+        <v>436</v>
       </c>
       <c r="C110" s="2" t="s">
-        <v>428</v>
+        <v>437</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A111" s="1" t="s">
-        <v>429</v>
-      </c>
-      <c r="B111" s="1" t="s">
-        <v>430</v>
-      </c>
-      <c r="C111" s="1" t="s">
-        <v>431</v>
+        <v>438</v>
+      </c>
+      <c r="B111" s="2" t="s">
+        <v>439</v>
+      </c>
+      <c r="C111" s="2" t="s">
+        <v>440</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A112" s="1" t="s">
-        <v>432</v>
-      </c>
-      <c r="B112" s="1" t="s">
-        <v>433</v>
-      </c>
-      <c r="C112" s="1" t="s">
-        <v>434</v>
+        <v>441</v>
+      </c>
+      <c r="B112" s="2" t="s">
+        <v>442</v>
+      </c>
+      <c r="C112" s="2" t="s">
+        <v>443</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A113" s="1" t="s">
-        <v>435</v>
+        <v>444</v>
       </c>
       <c r="B113" s="2" t="s">
-        <v>436</v>
-      </c>
-      <c r="C113" s="1" t="s">
-        <v>437</v>
+        <v>445</v>
+      </c>
+      <c r="C113" s="2" t="s">
+        <v>446</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A114" s="1" t="s">
-        <v>438</v>
-      </c>
-      <c r="B114" s="1" t="s">
-        <v>439</v>
-      </c>
-      <c r="C114" s="1" t="s">
-        <v>440</v>
-      </c>
-    </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A115" s="1" t="s">
-        <v>441</v>
-      </c>
-      <c r="B115" s="2" t="s">
-        <v>442</v>
-      </c>
-      <c r="C115" s="2" t="s">
-        <v>443</v>
+        <v>447</v>
+      </c>
+      <c r="B114" s="2" t="s">
+        <v>448</v>
+      </c>
+      <c r="C114" s="2" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A116" s="1" t="s">
+        <v>450</v>
+      </c>
+      <c r="B116" s="2" t="s">
+        <v>451</v>
+      </c>
+      <c r="C116" s="2" t="s">
+        <v>452</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A117" s="1" t="s">
-        <v>444</v>
+        <v>453</v>
       </c>
       <c r="B117" s="2" t="s">
-        <v>445</v>
+        <v>454</v>
       </c>
       <c r="C117" s="2" t="s">
-        <v>446</v>
+        <v>455</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A118" s="1" t="s">
-        <v>447</v>
+        <v>456</v>
       </c>
       <c r="B118" s="2" t="s">
-        <v>448</v>
+        <v>457</v>
       </c>
       <c r="C118" s="2" t="s">
-        <v>449</v>
+        <v>458</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B119" s="2"/>
-      <c r="C119" s="2"/>
+      <c r="A119" s="1" t="s">
+        <v>459</v>
+      </c>
+      <c r="B119" s="2" t="s">
+        <v>460</v>
+      </c>
+      <c r="C119" s="2" t="s">
+        <v>461</v>
+      </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A120" s="1" t="s">
-        <v>450</v>
+        <v>462</v>
       </c>
       <c r="B120" s="2" t="s">
-        <v>451</v>
+        <v>463</v>
       </c>
       <c r="C120" s="2" t="s">
-        <v>452</v>
-      </c>
-    </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A121" s="1" t="s">
-        <v>453</v>
-      </c>
-      <c r="B121" s="2" t="s">
-        <v>454</v>
-      </c>
-      <c r="C121" s="2" t="s">
-        <v>455</v>
+        <v>464</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A122" s="1" t="s">
-        <v>456</v>
+        <v>465</v>
       </c>
       <c r="B122" s="2" t="s">
-        <v>457</v>
+        <v>466</v>
       </c>
       <c r="C122" s="2" t="s">
-        <v>458</v>
+        <v>467</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A123" s="1" t="s">
-        <v>459</v>
-      </c>
-      <c r="B123" s="2" t="s">
-        <v>460</v>
-      </c>
-      <c r="C123" s="2" t="s">
-        <v>461</v>
+        <v>468</v>
+      </c>
+      <c r="B123" s="1" t="s">
+        <v>469</v>
+      </c>
+      <c r="C123" s="1" t="s">
+        <v>470</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A124" s="1" t="s">
-        <v>462</v>
-      </c>
-      <c r="B124" s="2" t="s">
-        <v>463</v>
-      </c>
-      <c r="C124" s="2" t="s">
-        <v>464</v>
+        <v>471</v>
+      </c>
+      <c r="B124" s="1" t="s">
+        <v>472</v>
+      </c>
+      <c r="C124" s="1" t="s">
+        <v>473</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B125" s="2"/>
-      <c r="C125" s="2"/>
+      <c r="A125" s="1" t="s">
+        <v>474</v>
+      </c>
+      <c r="B125" s="2" t="s">
+        <v>475</v>
+      </c>
+      <c r="C125" s="1" t="s">
+        <v>476</v>
+      </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A126" s="1" t="s">
-        <v>465</v>
-      </c>
-      <c r="B126" s="2" t="s">
-        <v>466</v>
-      </c>
-      <c r="C126" s="2" t="s">
-        <v>467</v>
+        <v>477</v>
+      </c>
+      <c r="B126" s="1" t="s">
+        <v>478</v>
+      </c>
+      <c r="C126" s="1" t="s">
+        <v>479</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A127" s="1" t="s">
-        <v>468</v>
+        <v>480</v>
       </c>
       <c r="B127" s="2" t="s">
-        <v>469</v>
+        <v>481</v>
       </c>
       <c r="C127" s="2" t="s">
-        <v>470</v>
+        <v>482</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A129" s="1" t="s">
+        <v>483</v>
+      </c>
+      <c r="B129" s="2" t="s">
+        <v>484</v>
+      </c>
+      <c r="C129" s="2" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A130" s="1" t="s">
+        <v>486</v>
+      </c>
+      <c r="B130" s="2" t="s">
+        <v>487</v>
+      </c>
+      <c r="C130" s="2" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B131" s="2"/>
+      <c r="C131" s="2"/>
+    </row>
+    <row r="132" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A132" s="1" t="s">
+        <v>489</v>
+      </c>
+      <c r="B132" s="2" t="s">
+        <v>490</v>
+      </c>
+      <c r="C132" s="2" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A133" s="1" t="s">
+        <v>492</v>
+      </c>
+      <c r="B133" s="2" t="s">
+        <v>493</v>
+      </c>
+      <c r="C133" s="2" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A134" s="1" t="s">
+        <v>495</v>
+      </c>
+      <c r="B134" s="2" t="s">
+        <v>496</v>
+      </c>
+      <c r="C134" s="2" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A135" s="1" t="s">
+        <v>498</v>
+      </c>
+      <c r="B135" s="2" t="s">
+        <v>499</v>
+      </c>
+      <c r="C135" s="2" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A136" s="1" t="s">
+        <v>501</v>
+      </c>
+      <c r="B136" s="2" t="s">
+        <v>502</v>
+      </c>
+      <c r="C136" s="2" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B137" s="2"/>
+      <c r="C137" s="2"/>
+    </row>
+    <row r="138" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A138" s="1" t="s">
+        <v>504</v>
+      </c>
+      <c r="B138" s="2" t="s">
+        <v>505</v>
+      </c>
+      <c r="C138" s="2" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A139" s="1" t="s">
+        <v>507</v>
+      </c>
+      <c r="B139" s="2" t="s">
+        <v>508</v>
+      </c>
+      <c r="C139" s="2" t="s">
+        <v>509</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Support manipulation of Queues
</commit_message>
<xml_diff>
--- a/Config.xlsx
+++ b/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mateus.cruz\Documents\GitHub\OrchestratorManager\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FD507EB-60A6-4843-8EC4-65AECFC624A1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A32F4B75-C6B2-479D-BD52-3A52A700A6E8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="552" uniqueCount="514">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="585" uniqueCount="544">
   <si>
     <t>Name</t>
   </si>
@@ -61,6 +61,9 @@
   </si>
   <si>
     <t>OnPremisesOrchestratorURL</t>
+  </si>
+  <si>
+    <t>https://myOrchestratorURL</t>
   </si>
   <si>
     <t>URL of the Orchestrator instance to be used. 
@@ -452,6 +455,24 @@
     <t>Column to which the result of the Delete Folder operation should be written.</t>
   </si>
   <si>
+    <t>CreateQueueIDColumn</t>
+  </si>
+  <si>
+    <t>Column to which the ID of the created Queue should be written.</t>
+  </si>
+  <si>
+    <t>CreateQueueResultColumn</t>
+  </si>
+  <si>
+    <t>Column to which the result of the Create Queue operation should be written.</t>
+  </si>
+  <si>
+    <t>DeleteQueueResultColumn</t>
+  </si>
+  <si>
+    <t>Column to which the result of the Delete Queue operation should be written.</t>
+  </si>
+  <si>
     <t>EN</t>
   </si>
   <si>
@@ -689,6 +710,15 @@
     <t>Folder</t>
   </si>
   <si>
+    <t>FormQueueOption</t>
+  </si>
+  <si>
+    <t>Queue</t>
+  </si>
+  <si>
+    <t>キュー</t>
+  </si>
+  <si>
     <t>FormSubmitButton</t>
   </si>
   <si>
@@ -776,6 +806,12 @@
     <t>JA\フォルダー.xlsx</t>
   </si>
   <si>
+    <t>QueueConfigFilePath</t>
+  </si>
+  <si>
+    <t>EN\Queues.xlsx</t>
+  </si>
+  <si>
     <t>GetOperationName</t>
   </si>
   <si>
@@ -1577,13 +1613,67 @@
     <t>パッケージバージョンが指定されませんでした。</t>
   </si>
   <si>
+    <t>UniqueReferenceInvalidOrNotSpecified</t>
+  </si>
+  <si>
+    <t>Unique Reference invalid or not specified.</t>
+  </si>
+  <si>
+    <t>一意の参照が無効か指定されませんでした。</t>
+  </si>
+  <si>
+    <t>AutoRetryInvalidOrNotSpecified</t>
+  </si>
+  <si>
+    <t>Auto Retry invalid or not specified.</t>
+  </si>
+  <si>
+    <t>自動リトライが無効か指定されませんでした。</t>
+  </si>
+  <si>
+    <t>MaxNumberOfRetriesInvalidOrNotSpecified</t>
+  </si>
+  <si>
+    <t>Max Number of Retries invalid or not specified.</t>
+  </si>
+  <si>
+    <t>最大リトライ回数が無効か指定されませんでした。</t>
+  </si>
+  <si>
+    <t>QueueNotFound</t>
+  </si>
+  <si>
+    <t>Queue not found.</t>
+  </si>
+  <si>
+    <t>キューが見つかりませんでした。</t>
+  </si>
+  <si>
+    <t>NamedQueueNotFound</t>
+  </si>
+  <si>
+    <t>Queue named {0} not found.</t>
+  </si>
+  <si>
+    <t>{0}というキューが見つかりませんでした。</t>
+  </si>
+  <si>
+    <t>JA\キュー.xlsx</t>
+  </si>
+  <si>
+    <t>QueueNameNotSpecified</t>
+  </si>
+  <si>
+    <t>Queue name not specified.</t>
+  </si>
+  <si>
+    <t>キュー名が指定されませんでした。</t>
+  </si>
+  <si>
     <t>Workbooks</t>
   </si>
   <si>
     <t>Default</t>
-  </si>
-  <si>
-    <t>https://myOrchestratorURL</t>
   </si>
   <si>
     <t>MyAccount</t>
@@ -1627,21 +1717,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1670,8 +1757,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table1" displayName="Table1" ref="A1:C53" totalsRowShown="0">
-  <autoFilter ref="A1:C53" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table1" displayName="Table1" ref="A1:C56" totalsRowShown="0">
+  <autoFilter ref="A1:C56" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Name"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Value"/>
@@ -1682,8 +1769,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table13" displayName="Table13" ref="A1:C139" totalsRowShown="0">
-  <autoFilter ref="A1:C139" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table13" displayName="Table13" ref="A1:C148" totalsRowShown="0">
+  <autoFilter ref="A1:C148" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Name"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="EN"/>
@@ -1985,7 +2072,7 @@
         <v>3</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>510</v>
+        <v>541</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>4</v>
@@ -1996,7 +2083,7 @@
         <v>5</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>511</v>
+        <v>542</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>6</v>
@@ -2006,53 +2093,53 @@
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="4" t="s">
-        <v>512</v>
+      <c r="B5" s="3" t="s">
+        <v>8</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="101.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="72.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>513</v>
+        <v>543</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B5" r:id="rId1" xr:uid="{74E87DF3-3663-4772-9B1C-21DEA2FCAA51}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <ignoredErrors>
+    <ignoredError sqref="B6" numberStoredAsText="1"/>
+  </ignoredErrors>
   <tableParts count="1">
-    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C53"/>
+  <dimension ref="A1:C56"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2 A2"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="A55" sqref="A55 A55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2075,574 +2162,607 @@
     </row>
     <row r="2" spans="1:3" ht="101.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B2" s="1">
         <v>200</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B3" s="1">
         <v>0</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B4" s="1">
         <v>550</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B5" s="1">
         <v>650</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B6" s="1">
         <v>3</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B7" s="1">
         <v>5000</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A32" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" s="1" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A34" s="1" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A35" s="1" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A36" s="1" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A37" s="1" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="38" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A38" s="1" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A39" s="1" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A40" s="1" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
     <row r="41" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A41" s="1" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row r="42" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A42" s="1" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A43" s="1" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="44" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A44" s="1" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="45" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A45" s="1" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
     </row>
     <row r="46" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A46" s="1" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
     </row>
     <row r="47" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A47" s="1" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A48" s="1" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
     </row>
     <row r="49" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A49" s="1" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="50" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A50" s="1" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A51" s="1" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
     </row>
     <row r="52" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A52" s="1" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
     </row>
     <row r="53" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A53" s="1" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>134</v>
+        <v>135</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A54" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A55" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A56" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C56" s="2" t="s">
+        <v>141</v>
       </c>
     </row>
   </sheetData>
@@ -2660,10 +2780,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1927ABA9-1814-4487-9CEC-ABDCAF91481F}">
-  <dimension ref="A1:C139"/>
+  <dimension ref="A1:C148"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2 A2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2678,1428 +2798,1516 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>135</v>
+        <v>142</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>136</v>
+        <v>143</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>137</v>
+        <v>144</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>138</v>
+        <v>145</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>138</v>
+        <v>145</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="43.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>139</v>
+        <v>146</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>140</v>
+        <v>147</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>141</v>
+        <v>148</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>142</v>
+        <v>149</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>143</v>
+        <v>150</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>144</v>
+        <v>151</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>145</v>
+        <v>152</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>146</v>
+        <v>153</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>146</v>
+        <v>153</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
-        <v>147</v>
+        <v>154</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>148</v>
+        <v>155</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>149</v>
+        <v>156</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
-        <v>150</v>
+        <v>157</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>151</v>
+        <v>158</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>152</v>
+        <v>159</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
-        <v>153</v>
+        <v>160</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>154</v>
+        <v>161</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>155</v>
+        <v>162</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
-        <v>156</v>
+        <v>163</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>157</v>
+        <v>164</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>158</v>
+        <v>165</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
-        <v>159</v>
+        <v>166</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>160</v>
+        <v>167</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>161</v>
+        <v>168</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
-        <v>162</v>
+        <v>169</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>163</v>
+        <v>170</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>164</v>
+        <v>171</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
-        <v>165</v>
+        <v>172</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>166</v>
+        <v>173</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>167</v>
+        <v>174</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
-        <v>168</v>
+        <v>175</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>169</v>
+        <v>176</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>170</v>
+        <v>177</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
-        <v>171</v>
+        <v>178</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>172</v>
+        <v>179</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>173</v>
+        <v>180</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
-        <v>174</v>
+        <v>181</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>175</v>
+        <v>182</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>176</v>
+        <v>183</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
-        <v>177</v>
+        <v>184</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>178</v>
+        <v>185</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>179</v>
+        <v>186</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
-        <v>180</v>
+        <v>187</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>181</v>
+        <v>188</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>182</v>
+        <v>189</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
-        <v>183</v>
+        <v>190</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>184</v>
+        <v>191</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>185</v>
+        <v>192</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
-        <v>186</v>
+        <v>193</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>187</v>
+        <v>194</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>188</v>
+        <v>195</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
-        <v>189</v>
+        <v>196</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>190</v>
+        <v>197</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>191</v>
+        <v>198</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
-        <v>192</v>
+        <v>199</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>193</v>
+        <v>200</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>194</v>
+        <v>201</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
-        <v>195</v>
+        <v>202</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>196</v>
+        <v>203</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>197</v>
+        <v>204</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
-        <v>198</v>
+        <v>205</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>199</v>
+        <v>206</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>200</v>
+        <v>207</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
-        <v>201</v>
+        <v>208</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>203</v>
+        <v>210</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
-        <v>204</v>
+        <v>211</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>205</v>
+        <v>212</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>206</v>
+        <v>213</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
-        <v>207</v>
+        <v>214</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>208</v>
+        <v>215</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>209</v>
+        <v>216</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
-        <v>210</v>
+        <v>217</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>182</v>
+        <v>189</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="s">
-        <v>212</v>
+        <v>219</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>213</v>
+        <v>220</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>185</v>
+        <v>192</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="s">
-        <v>214</v>
+        <v>221</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>215</v>
+        <v>222</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A30" s="1" t="s">
-        <v>216</v>
+        <v>224</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>217</v>
+        <v>225</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>218</v>
+        <v>225</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B31" s="2"/>
-      <c r="C31" s="2"/>
+      <c r="A31" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>228</v>
+      </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A32" s="1" t="s">
-        <v>219</v>
-      </c>
-      <c r="B32" s="2" t="s">
-        <v>220</v>
-      </c>
-      <c r="C32" s="2" t="s">
-        <v>221</v>
-      </c>
+      <c r="B32" s="2"/>
+      <c r="C32" s="2"/>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A33" s="1" t="s">
-        <v>222</v>
+        <v>229</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>223</v>
+        <v>230</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>224</v>
+        <v>231</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A34" s="1" t="s">
-        <v>225</v>
+        <v>232</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>226</v>
+        <v>233</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>227</v>
+        <v>234</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A35" s="1" t="s">
-        <v>228</v>
+        <v>235</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>229</v>
+        <v>236</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>230</v>
+        <v>237</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A36" s="1" t="s">
-        <v>231</v>
+        <v>238</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>232</v>
+        <v>239</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A37" s="1" t="s">
-        <v>234</v>
+        <v>241</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>235</v>
+        <v>242</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>236</v>
+        <v>243</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A38" s="1" t="s">
-        <v>237</v>
+        <v>244</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>238</v>
+        <v>245</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>239</v>
+        <v>246</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A39" s="1" t="s">
-        <v>240</v>
+        <v>247</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>241</v>
+        <v>248</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>242</v>
+        <v>249</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B40" s="2"/>
-      <c r="C40" s="2"/>
+      <c r="A40" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>251</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>252</v>
+      </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A41" s="1" t="s">
-        <v>243</v>
+        <v>253</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>244</v>
+        <v>254</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>245</v>
+        <v>537</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A42" s="1" t="s">
-        <v>246</v>
-      </c>
-      <c r="B42" s="2" t="s">
-        <v>247</v>
-      </c>
-      <c r="C42" s="2" t="s">
-        <v>248</v>
-      </c>
+      <c r="B42" s="2"/>
+      <c r="C42" s="2"/>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A43" s="1" t="s">
-        <v>249</v>
+        <v>255</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>250</v>
+        <v>256</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>251</v>
+        <v>257</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A44" s="1" t="s">
-        <v>252</v>
+        <v>258</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>253</v>
+        <v>259</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>254</v>
+        <v>260</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A45" s="1" t="s">
-        <v>255</v>
+        <v>261</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>256</v>
+        <v>262</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>257</v>
+        <v>263</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A46" s="1" t="s">
-        <v>258</v>
+        <v>264</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>259</v>
+        <v>265</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>260</v>
+        <v>266</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A47" s="1" t="s">
-        <v>261</v>
+        <v>267</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>262</v>
+        <v>268</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>263</v>
+        <v>269</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A48" s="1" t="s">
-        <v>264</v>
+        <v>270</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>265</v>
+        <v>271</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>266</v>
+        <v>272</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A49" s="1" t="s">
-        <v>267</v>
+        <v>273</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>268</v>
+        <v>274</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>269</v>
+        <v>275</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A50" s="1" t="s">
-        <v>270</v>
+        <v>276</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>271</v>
+        <v>277</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>272</v>
+        <v>278</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A51" s="1" t="s">
-        <v>273</v>
+        <v>279</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>274</v>
+        <v>280</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>275</v>
+        <v>281</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A52" s="1" t="s">
-        <v>276</v>
+        <v>282</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>277</v>
+        <v>283</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>278</v>
+        <v>284</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A53" s="1" t="s">
-        <v>279</v>
+        <v>285</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>280</v>
+        <v>286</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>281</v>
+        <v>287</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A54" s="1" t="s">
-        <v>282</v>
+        <v>288</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>283</v>
+        <v>289</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>284</v>
+        <v>290</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A55" s="1" t="s">
-        <v>285</v>
+        <v>291</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>286</v>
+        <v>292</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>287</v>
+        <v>293</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A56" s="1" t="s">
-        <v>288</v>
+        <v>294</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>289</v>
+        <v>295</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>290</v>
+        <v>296</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A57" s="1" t="s">
-        <v>291</v>
+        <v>297</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>292</v>
+        <v>298</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>293</v>
+        <v>299</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A58" s="1" t="s">
-        <v>294</v>
+        <v>300</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>295</v>
+        <v>301</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>296</v>
+        <v>302</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A59" s="1" t="s">
-        <v>297</v>
+        <v>303</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>298</v>
+        <v>304</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>299</v>
+        <v>305</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A60" s="1" t="s">
-        <v>300</v>
+        <v>306</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>301</v>
+        <v>307</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>302</v>
+        <v>308</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A61" s="1" t="s">
-        <v>303</v>
+        <v>309</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>304</v>
+        <v>310</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>305</v>
+        <v>311</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A62" s="1" t="s">
-        <v>306</v>
+        <v>312</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>307</v>
+        <v>313</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>308</v>
+        <v>314</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A63" s="1" t="s">
-        <v>309</v>
+        <v>315</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>310</v>
+        <v>316</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A64" s="1" t="s">
-        <v>312</v>
+        <v>318</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>313</v>
+        <v>319</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>314</v>
+        <v>320</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A65" s="1" t="s">
-        <v>315</v>
+        <v>321</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>316</v>
+        <v>322</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.35">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A66" s="1" t="s">
-        <v>318</v>
+        <v>324</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>319</v>
+        <v>325</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>320</v>
+        <v>326</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A67" s="1" t="s">
-        <v>321</v>
+        <v>327</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>322</v>
+        <v>328</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>323</v>
+        <v>329</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A68" s="1" t="s">
-        <v>324</v>
+        <v>330</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>325</v>
+        <v>331</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>326</v>
+        <v>332</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A69" s="1" t="s">
-        <v>327</v>
+        <v>333</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>328</v>
+        <v>334</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>329</v>
+        <v>335</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A70" s="1" t="s">
-        <v>330</v>
+        <v>336</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>331</v>
+        <v>337</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>332</v>
+        <v>338</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A71" s="1" t="s">
-        <v>333</v>
+        <v>339</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>334</v>
+        <v>340</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>335</v>
+        <v>341</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A72" s="1" t="s">
-        <v>336</v>
+        <v>342</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>337</v>
+        <v>343</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>338</v>
+        <v>344</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A73" s="1" t="s">
-        <v>339</v>
+        <v>345</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>340</v>
+        <v>346</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>341</v>
+        <v>347</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B74" s="2"/>
-      <c r="C74" s="2"/>
+      <c r="A74" s="1" t="s">
+        <v>348</v>
+      </c>
+      <c r="B74" s="2" t="s">
+        <v>349</v>
+      </c>
+      <c r="C74" s="2" t="s">
+        <v>350</v>
+      </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A75" s="1" t="s">
-        <v>342</v>
+        <v>351</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>343</v>
+        <v>352</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>344</v>
+        <v>353</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A76" s="1" t="s">
-        <v>345</v>
-      </c>
-      <c r="B76" s="2" t="s">
-        <v>346</v>
-      </c>
-      <c r="C76" s="2" t="s">
-        <v>347</v>
-      </c>
+      <c r="B76" s="2"/>
+      <c r="C76" s="2"/>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A77" s="1" t="s">
-        <v>348</v>
+        <v>354</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>349</v>
+        <v>355</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>350</v>
+        <v>356</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A78" s="1" t="s">
-        <v>351</v>
+        <v>357</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>352</v>
+        <v>358</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>353</v>
+        <v>359</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A79" s="1" t="s">
-        <v>354</v>
+        <v>360</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>355</v>
+        <v>361</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>356</v>
+        <v>362</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A80" s="1" t="s">
-        <v>357</v>
+        <v>363</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>358</v>
+        <v>364</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>359</v>
+        <v>365</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A81" s="1" t="s">
-        <v>360</v>
+        <v>366</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>361</v>
+        <v>367</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>362</v>
+        <v>368</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A82" s="1" t="s">
-        <v>363</v>
+        <v>369</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>364</v>
+        <v>370</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>365</v>
+        <v>371</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B83" s="2"/>
-      <c r="C83" s="2"/>
+      <c r="A83" s="1" t="s">
+        <v>372</v>
+      </c>
+      <c r="B83" s="2" t="s">
+        <v>373</v>
+      </c>
+      <c r="C83" s="2" t="s">
+        <v>374</v>
+      </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A84" s="1" t="s">
-        <v>366</v>
+        <v>375</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>367</v>
+        <v>376</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>368</v>
+        <v>377</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A85" s="1" t="s">
-        <v>369</v>
-      </c>
-      <c r="B85" s="2" t="s">
-        <v>370</v>
-      </c>
-      <c r="C85" s="2" t="s">
-        <v>371</v>
-      </c>
+      <c r="B85" s="2"/>
+      <c r="C85" s="2"/>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A86" s="1" t="s">
-        <v>372</v>
+        <v>378</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>373</v>
+        <v>379</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>374</v>
+        <v>380</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A87" s="1" t="s">
-        <v>375</v>
+        <v>381</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>376</v>
+        <v>382</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>377</v>
+        <v>383</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A88" s="1" t="s">
-        <v>378</v>
+        <v>384</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>379</v>
+        <v>385</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>380</v>
+        <v>386</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A89" s="1" t="s">
-        <v>381</v>
+        <v>387</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>382</v>
+        <v>388</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>383</v>
+        <v>389</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A90" s="1" t="s">
-        <v>384</v>
+        <v>390</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>385</v>
+        <v>391</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>386</v>
+        <v>392</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A91" s="1" t="s">
-        <v>387</v>
+        <v>393</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>388</v>
+        <v>394</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>389</v>
+        <v>395</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A92" s="1" t="s">
-        <v>390</v>
+        <v>396</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>391</v>
+        <v>397</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>392</v>
+        <v>398</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B93" s="2"/>
-      <c r="C93" s="2"/>
+      <c r="A93" s="1" t="s">
+        <v>399</v>
+      </c>
+      <c r="B93" s="2" t="s">
+        <v>400</v>
+      </c>
+      <c r="C93" s="2" t="s">
+        <v>401</v>
+      </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A94" s="1" t="s">
-        <v>393</v>
+        <v>402</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>394</v>
+        <v>403</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>395</v>
+        <v>404</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A95" s="1" t="s">
-        <v>396</v>
-      </c>
-      <c r="B95" s="2" t="s">
-        <v>397</v>
-      </c>
-      <c r="C95" s="2" t="s">
-        <v>398</v>
-      </c>
+      <c r="B95" s="2"/>
+      <c r="C95" s="2"/>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A96" s="1" t="s">
-        <v>399</v>
+        <v>405</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>400</v>
+        <v>406</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>401</v>
+        <v>407</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A97" s="1" t="s">
-        <v>402</v>
+        <v>408</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>403</v>
+        <v>409</v>
       </c>
       <c r="C97" s="2" t="s">
-        <v>404</v>
+        <v>410</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A98" s="1" t="s">
-        <v>405</v>
+        <v>411</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>406</v>
+        <v>412</v>
       </c>
       <c r="C98" s="2" t="s">
-        <v>407</v>
+        <v>413</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A99" s="1" t="s">
-        <v>408</v>
+        <v>414</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>409</v>
+        <v>415</v>
       </c>
       <c r="C99" s="2" t="s">
-        <v>410</v>
+        <v>416</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A100" s="1" t="s">
-        <v>411</v>
+        <v>417</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>412</v>
+        <v>418</v>
       </c>
       <c r="C100" s="2" t="s">
-        <v>413</v>
+        <v>419</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A101" s="1" t="s">
-        <v>414</v>
+        <v>420</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>415</v>
+        <v>421</v>
       </c>
       <c r="C101" s="2" t="s">
-        <v>416</v>
+        <v>422</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B102" s="2"/>
-      <c r="C102" s="2"/>
+      <c r="A102" s="1" t="s">
+        <v>423</v>
+      </c>
+      <c r="B102" s="2" t="s">
+        <v>424</v>
+      </c>
+      <c r="C102" s="2" t="s">
+        <v>425</v>
+      </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A103" s="1" t="s">
-        <v>417</v>
+        <v>426</v>
       </c>
       <c r="B103" s="2" t="s">
-        <v>418</v>
+        <v>427</v>
       </c>
       <c r="C103" s="2" t="s">
-        <v>419</v>
+        <v>428</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A104" s="1" t="s">
-        <v>420</v>
-      </c>
-      <c r="B104" s="2" t="s">
-        <v>421</v>
-      </c>
-      <c r="C104" s="2" t="s">
-        <v>422</v>
-      </c>
+      <c r="B104" s="2"/>
+      <c r="C104" s="2"/>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A105" s="1" t="s">
-        <v>423</v>
+        <v>429</v>
       </c>
       <c r="B105" s="2" t="s">
-        <v>424</v>
+        <v>430</v>
       </c>
       <c r="C105" s="2" t="s">
-        <v>425</v>
+        <v>431</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A106" s="1" t="s">
-        <v>426</v>
+        <v>432</v>
       </c>
       <c r="B106" s="2" t="s">
-        <v>427</v>
+        <v>433</v>
       </c>
       <c r="C106" s="2" t="s">
-        <v>428</v>
+        <v>434</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A107" s="1" t="s">
+        <v>435</v>
+      </c>
+      <c r="B107" s="2" t="s">
+        <v>436</v>
+      </c>
+      <c r="C107" s="2" t="s">
+        <v>437</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A108" s="1" t="s">
-        <v>429</v>
+        <v>438</v>
       </c>
       <c r="B108" s="2" t="s">
-        <v>430</v>
+        <v>439</v>
       </c>
       <c r="C108" s="2" t="s">
-        <v>431</v>
-      </c>
-    </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A109" s="1" t="s">
-        <v>432</v>
-      </c>
-      <c r="B109" s="2" t="s">
-        <v>433</v>
-      </c>
-      <c r="C109" s="2" t="s">
-        <v>434</v>
+        <v>440</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A110" s="1" t="s">
-        <v>435</v>
+        <v>441</v>
       </c>
       <c r="B110" s="2" t="s">
-        <v>436</v>
+        <v>442</v>
       </c>
       <c r="C110" s="2" t="s">
-        <v>437</v>
+        <v>443</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A111" s="1" t="s">
-        <v>438</v>
+        <v>444</v>
       </c>
       <c r="B111" s="2" t="s">
-        <v>439</v>
+        <v>445</v>
       </c>
       <c r="C111" s="2" t="s">
-        <v>440</v>
+        <v>446</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A112" s="1" t="s">
-        <v>441</v>
+        <v>447</v>
       </c>
       <c r="B112" s="2" t="s">
-        <v>442</v>
+        <v>448</v>
       </c>
       <c r="C112" s="2" t="s">
-        <v>443</v>
+        <v>449</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A113" s="1" t="s">
-        <v>444</v>
+        <v>450</v>
       </c>
       <c r="B113" s="2" t="s">
-        <v>445</v>
+        <v>451</v>
       </c>
       <c r="C113" s="2" t="s">
-        <v>446</v>
+        <v>452</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A114" s="1" t="s">
-        <v>447</v>
+        <v>453</v>
       </c>
       <c r="B114" s="2" t="s">
-        <v>448</v>
+        <v>454</v>
       </c>
       <c r="C114" s="2" t="s">
-        <v>449</v>
+        <v>455</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A115" s="1" t="s">
+        <v>456</v>
+      </c>
+      <c r="B115" s="2" t="s">
+        <v>457</v>
+      </c>
+      <c r="C115" s="2" t="s">
+        <v>458</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A116" s="1" t="s">
-        <v>450</v>
+        <v>459</v>
       </c>
       <c r="B116" s="2" t="s">
-        <v>451</v>
+        <v>460</v>
       </c>
       <c r="C116" s="2" t="s">
-        <v>452</v>
-      </c>
-    </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A117" s="1" t="s">
-        <v>453</v>
-      </c>
-      <c r="B117" s="2" t="s">
-        <v>454</v>
-      </c>
-      <c r="C117" s="2" t="s">
-        <v>455</v>
+        <v>461</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A118" s="1" t="s">
-        <v>456</v>
+        <v>462</v>
       </c>
       <c r="B118" s="2" t="s">
-        <v>457</v>
+        <v>463</v>
       </c>
       <c r="C118" s="2" t="s">
-        <v>458</v>
+        <v>464</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A119" s="1" t="s">
-        <v>459</v>
+        <v>465</v>
       </c>
       <c r="B119" s="2" t="s">
-        <v>460</v>
+        <v>466</v>
       </c>
       <c r="C119" s="2" t="s">
-        <v>461</v>
+        <v>467</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A120" s="1" t="s">
-        <v>462</v>
+        <v>468</v>
       </c>
       <c r="B120" s="2" t="s">
-        <v>463</v>
+        <v>469</v>
       </c>
       <c r="C120" s="2" t="s">
-        <v>464</v>
+        <v>470</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A121" s="1" t="s">
+        <v>471</v>
+      </c>
+      <c r="B121" s="2" t="s">
+        <v>472</v>
+      </c>
+      <c r="C121" s="2" t="s">
+        <v>473</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A122" s="1" t="s">
-        <v>465</v>
+        <v>474</v>
       </c>
       <c r="B122" s="2" t="s">
-        <v>466</v>
+        <v>475</v>
       </c>
       <c r="C122" s="2" t="s">
-        <v>467</v>
-      </c>
-    </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A123" s="1" t="s">
-        <v>468</v>
-      </c>
-      <c r="B123" s="1" t="s">
-        <v>469</v>
-      </c>
-      <c r="C123" s="1" t="s">
-        <v>470</v>
+        <v>476</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A124" s="1" t="s">
-        <v>471</v>
-      </c>
-      <c r="B124" s="1" t="s">
-        <v>472</v>
-      </c>
-      <c r="C124" s="1" t="s">
-        <v>473</v>
+        <v>477</v>
+      </c>
+      <c r="B124" s="2" t="s">
+        <v>478</v>
+      </c>
+      <c r="C124" s="2" t="s">
+        <v>479</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A125" s="1" t="s">
-        <v>474</v>
-      </c>
-      <c r="B125" s="2" t="s">
-        <v>475</v>
+        <v>480</v>
+      </c>
+      <c r="B125" s="1" t="s">
+        <v>481</v>
       </c>
       <c r="C125" s="1" t="s">
-        <v>476</v>
+        <v>482</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A126" s="1" t="s">
-        <v>477</v>
+        <v>483</v>
       </c>
       <c r="B126" s="1" t="s">
-        <v>478</v>
+        <v>484</v>
       </c>
       <c r="C126" s="1" t="s">
-        <v>479</v>
+        <v>485</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A127" s="1" t="s">
-        <v>480</v>
+        <v>486</v>
       </c>
       <c r="B127" s="2" t="s">
-        <v>481</v>
-      </c>
-      <c r="C127" s="2" t="s">
-        <v>482</v>
+        <v>487</v>
+      </c>
+      <c r="C127" s="1" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A128" s="1" t="s">
+        <v>489</v>
+      </c>
+      <c r="B128" s="1" t="s">
+        <v>490</v>
+      </c>
+      <c r="C128" s="1" t="s">
+        <v>491</v>
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A129" s="1" t="s">
-        <v>483</v>
+        <v>492</v>
       </c>
       <c r="B129" s="2" t="s">
-        <v>484</v>
+        <v>493</v>
       </c>
       <c r="C129" s="2" t="s">
-        <v>485</v>
-      </c>
-    </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A130" s="1" t="s">
-        <v>486</v>
-      </c>
-      <c r="B130" s="2" t="s">
-        <v>487</v>
-      </c>
-      <c r="C130" s="2" t="s">
-        <v>488</v>
+        <v>494</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B131" s="2"/>
-      <c r="C131" s="2"/>
+      <c r="A131" s="1" t="s">
+        <v>495</v>
+      </c>
+      <c r="B131" s="2" t="s">
+        <v>496</v>
+      </c>
+      <c r="C131" s="2" t="s">
+        <v>497</v>
+      </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A132" s="1" t="s">
-        <v>489</v>
+        <v>498</v>
       </c>
       <c r="B132" s="2" t="s">
-        <v>490</v>
+        <v>499</v>
       </c>
       <c r="C132" s="2" t="s">
-        <v>491</v>
+        <v>500</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A133" s="1" t="s">
-        <v>492</v>
-      </c>
-      <c r="B133" s="2" t="s">
-        <v>493</v>
-      </c>
-      <c r="C133" s="2" t="s">
-        <v>494</v>
-      </c>
+      <c r="B133" s="2"/>
+      <c r="C133" s="2"/>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A134" s="1" t="s">
-        <v>495</v>
+        <v>501</v>
       </c>
       <c r="B134" s="2" t="s">
-        <v>496</v>
+        <v>502</v>
       </c>
       <c r="C134" s="2" t="s">
-        <v>497</v>
+        <v>503</v>
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A135" s="1" t="s">
-        <v>498</v>
+        <v>504</v>
       </c>
       <c r="B135" s="2" t="s">
-        <v>499</v>
+        <v>505</v>
       </c>
       <c r="C135" s="2" t="s">
-        <v>500</v>
+        <v>506</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A136" s="1" t="s">
-        <v>501</v>
+        <v>507</v>
       </c>
       <c r="B136" s="2" t="s">
-        <v>502</v>
+        <v>508</v>
       </c>
       <c r="C136" s="2" t="s">
-        <v>503</v>
+        <v>509</v>
       </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B137" s="2"/>
-      <c r="C137" s="2"/>
+      <c r="A137" s="1" t="s">
+        <v>510</v>
+      </c>
+      <c r="B137" s="2" t="s">
+        <v>511</v>
+      </c>
+      <c r="C137" s="2" t="s">
+        <v>512</v>
+      </c>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A138" s="1" t="s">
-        <v>504</v>
+        <v>513</v>
       </c>
       <c r="B138" s="2" t="s">
-        <v>505</v>
+        <v>514</v>
       </c>
       <c r="C138" s="2" t="s">
-        <v>506</v>
+        <v>515</v>
       </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A139" s="1" t="s">
-        <v>507</v>
-      </c>
-      <c r="B139" s="2" t="s">
-        <v>508</v>
-      </c>
-      <c r="C139" s="2" t="s">
-        <v>509</v>
+      <c r="B139" s="2"/>
+      <c r="C139" s="2"/>
+    </row>
+    <row r="140" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A140" s="1" t="s">
+        <v>516</v>
+      </c>
+      <c r="B140" s="2" t="s">
+        <v>517</v>
+      </c>
+      <c r="C140" s="2" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A141" s="1" t="s">
+        <v>519</v>
+      </c>
+      <c r="B141" s="2" t="s">
+        <v>520</v>
+      </c>
+      <c r="C141" s="2" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A143" s="1" t="s">
+        <v>522</v>
+      </c>
+      <c r="B143" s="1" t="s">
+        <v>523</v>
+      </c>
+      <c r="C143" s="1" t="s">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="144" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A144" s="1" t="s">
+        <v>525</v>
+      </c>
+      <c r="B144" s="1" t="s">
+        <v>526</v>
+      </c>
+      <c r="C144" s="1" t="s">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="145" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A145" s="1" t="s">
+        <v>528</v>
+      </c>
+      <c r="B145" s="1" t="s">
+        <v>529</v>
+      </c>
+      <c r="C145" s="1" t="s">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="146" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A146" s="1" t="s">
+        <v>531</v>
+      </c>
+      <c r="B146" s="1" t="s">
+        <v>532</v>
+      </c>
+      <c r="C146" s="1" t="s">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="147" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A147" s="1" t="s">
+        <v>534</v>
+      </c>
+      <c r="B147" s="2" t="s">
+        <v>535</v>
+      </c>
+      <c r="C147" s="2" t="s">
+        <v>536</v>
+      </c>
+    </row>
+    <row r="148" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A148" s="1" t="s">
+        <v>538</v>
+      </c>
+      <c r="B148" s="1" t="s">
+        <v>539</v>
+      </c>
+      <c r="C148" s="1" t="s">
+        <v>540</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Inform users with message boxes in case of errors or warnings
</commit_message>
<xml_diff>
--- a/Config.xlsx
+++ b/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mateus.cruz\Documents\GitHub\OrchestratorManager\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A338AB0-E3C7-4056-B1B2-E3FBECE2563F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A734B059-D77E-493A-89B8-4C4A43A745C4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="600" uniqueCount="557">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="615" uniqueCount="572">
   <si>
     <t>Name</t>
   </si>
@@ -1052,9 +1052,6 @@
     <t>ConfirmNumerousRequests</t>
   </si>
   <si>
-    <t>The selected operation will make a large number of HTTP requests and might have a negative impact on infrastructure. Continue the processing?</t>
-  </si>
-  <si>
     <t>選択した操作により、多数の HTTP リクエストが送信されます。これにより、対象となる Orchestrator のインフラストラクチャに負荷を与える可能性があります。処理を続行しますか?</t>
   </si>
   <si>
@@ -1376,9 +1373,6 @@
     <t>GetSingleMachineFailure</t>
   </si>
   <si>
-    <t>Failed to get machine with Id: {0}. Request status: {1} / Response: {2}.</t>
-  </si>
-  <si>
     <t>ID{0}マシン取得が失敗しました。リクエストステータス：{1} / レスポンス：{2}。</t>
   </si>
   <si>
@@ -1716,6 +1710,57 @@
   </si>
   <si>
     <t>MyAccount</t>
+  </si>
+  <si>
+    <t>CredentialNotFound</t>
+  </si>
+  <si>
+    <t>The specified credential was not found.</t>
+  </si>
+  <si>
+    <t>指定された資格情報が見つかりませんでした。</t>
+  </si>
+  <si>
+    <t>The selected operation will make a large number of HTTP requests that might impact on Orchestrator's infrastructure. Continue the processing?</t>
+  </si>
+  <si>
+    <t>ユーザーが操作をキャンセルしました。</t>
+  </si>
+  <si>
+    <t>OperationCanceledByUser</t>
+  </si>
+  <si>
+    <t>Operation canceled by user.</t>
+  </si>
+  <si>
+    <t>AuthenticationFailed</t>
+  </si>
+  <si>
+    <t>Authentication failed. Please check logs for more details.</t>
+  </si>
+  <si>
+    <t>認証に失敗しました。詳細はログを確認してください。</t>
+  </si>
+  <si>
+    <t>ErrorDuringExecution</t>
+  </si>
+  <si>
+    <t>There was an execution error. Please check logs for more details.</t>
+  </si>
+  <si>
+    <t>実行中にエラーが発生しました。詳細はログを確認してください。</t>
+  </si>
+  <si>
+    <t>Failed to get machine with ID: {0}. Request status: {1} / Response: {2}.</t>
+  </si>
+  <si>
+    <t>There was an execution error: {0} at {1}.</t>
+  </si>
+  <si>
+    <t>実行中にエラーが発生しました：{1}で{0}。</t>
+  </si>
+  <si>
+    <t>ErrorDuringExecutionLog</t>
   </si>
 </sst>
 </file>
@@ -1808,8 +1853,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table13" displayName="Table13" ref="A1:C151" totalsRowShown="0">
-  <autoFilter ref="A1:C151" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table13" displayName="Table13" ref="A1:C156" totalsRowShown="0">
+  <autoFilter ref="A1:C156" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Name"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="EN"/>
@@ -2111,7 +2156,7 @@
         <v>3</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>4</v>
@@ -2122,7 +2167,7 @@
         <v>5</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>6</v>
@@ -2133,7 +2178,7 @@
         <v>7</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>8</v>
@@ -2155,7 +2200,7 @@
         <v>12</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>13</v>
@@ -2175,7 +2220,7 @@
   <dimension ref="A1:C58"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2 A2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2838,10 +2883,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1927ABA9-1814-4487-9CEC-ABDCAF91481F}">
-  <dimension ref="A1:C151"/>
+  <dimension ref="A1:C156"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2 A2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3521,884 +3566,939 @@
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A63" s="1" t="s">
-        <v>319</v>
+        <v>562</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>320</v>
+        <v>563</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>321</v>
+        <v>564</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A64" s="1" t="s">
-        <v>322</v>
+        <v>571</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>323</v>
+        <v>569</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>324</v>
+        <v>570</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A65" s="1" t="s">
-        <v>325</v>
+        <v>565</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>326</v>
+        <v>566</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>327</v>
+        <v>567</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A66" s="1" t="s">
-        <v>328</v>
+        <v>319</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>329</v>
+        <v>320</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>330</v>
+        <v>321</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A67" s="1" t="s">
-        <v>331</v>
+        <v>322</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>332</v>
+        <v>323</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>333</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A68" s="1" t="s">
-        <v>334</v>
+        <v>325</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>335</v>
+        <v>326</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>336</v>
+        <v>327</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A69" s="1" t="s">
-        <v>337</v>
+        <v>328</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>338</v>
+        <v>329</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>339</v>
+        <v>330</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A70" s="1" t="s">
-        <v>340</v>
+        <v>331</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>341</v>
+        <v>332</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.35">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A71" s="1" t="s">
-        <v>343</v>
+        <v>334</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>344</v>
+        <v>558</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>345</v>
+        <v>335</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A72" s="1" t="s">
-        <v>346</v>
+        <v>336</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>347</v>
+        <v>337</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>348</v>
+        <v>338</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A73" s="1" t="s">
-        <v>349</v>
+        <v>339</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>350</v>
+        <v>340</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>351</v>
+        <v>341</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A74" s="1" t="s">
-        <v>352</v>
+        <v>342</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>353</v>
+        <v>343</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>354</v>
+        <v>344</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A75" s="1" t="s">
-        <v>355</v>
+        <v>345</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>356</v>
+        <v>346</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>357</v>
+        <v>347</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A76" s="1" t="s">
-        <v>358</v>
+        <v>348</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>359</v>
+        <v>349</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>360</v>
+        <v>350</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A77" s="1" t="s">
-        <v>361</v>
+        <v>351</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>362</v>
+        <v>352</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>363</v>
+        <v>353</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B78" s="2"/>
-      <c r="C78" s="2"/>
+      <c r="A78" s="1" t="s">
+        <v>354</v>
+      </c>
+      <c r="B78" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="C78" s="2" t="s">
+        <v>356</v>
+      </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A79" s="1" t="s">
-        <v>364</v>
+        <v>357</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>365</v>
+        <v>358</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>366</v>
+        <v>359</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A80" s="1" t="s">
-        <v>367</v>
+        <v>360</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>368</v>
+        <v>361</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>369</v>
+        <v>362</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A81" s="1" t="s">
-        <v>370</v>
+        <v>555</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>371</v>
+        <v>556</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>372</v>
+        <v>557</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A82" s="1" t="s">
-        <v>373</v>
+        <v>560</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>374</v>
+        <v>561</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>375</v>
+        <v>559</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A83" s="1" t="s">
-        <v>376</v>
-      </c>
-      <c r="B83" s="2" t="s">
-        <v>377</v>
-      </c>
-      <c r="C83" s="2" t="s">
-        <v>378</v>
-      </c>
+      <c r="B83" s="2"/>
+      <c r="C83" s="2"/>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A84" s="1" t="s">
-        <v>379</v>
+        <v>363</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>380</v>
+        <v>364</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>381</v>
+        <v>365</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A85" s="1" t="s">
-        <v>382</v>
+        <v>366</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>383</v>
+        <v>367</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>384</v>
+        <v>368</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A86" s="1" t="s">
-        <v>385</v>
+        <v>369</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>386</v>
+        <v>370</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>387</v>
+        <v>371</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B87" s="2"/>
-      <c r="C87" s="2"/>
+      <c r="A87" s="1" t="s">
+        <v>372</v>
+      </c>
+      <c r="B87" s="2" t="s">
+        <v>373</v>
+      </c>
+      <c r="C87" s="2" t="s">
+        <v>374</v>
+      </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A88" s="1" t="s">
-        <v>388</v>
+        <v>375</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>389</v>
+        <v>376</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>390</v>
+        <v>377</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A89" s="1" t="s">
-        <v>391</v>
+        <v>378</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>392</v>
+        <v>379</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>393</v>
+        <v>380</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A90" s="1" t="s">
-        <v>394</v>
+        <v>381</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>395</v>
+        <v>382</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>396</v>
+        <v>383</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A91" s="1" t="s">
-        <v>397</v>
+        <v>384</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>398</v>
+        <v>385</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>399</v>
+        <v>386</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A92" s="1" t="s">
-        <v>400</v>
-      </c>
-      <c r="B92" s="2" t="s">
-        <v>401</v>
-      </c>
-      <c r="C92" s="2" t="s">
-        <v>402</v>
-      </c>
+      <c r="B92" s="2"/>
+      <c r="C92" s="2"/>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A93" s="1" t="s">
-        <v>403</v>
+        <v>387</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>404</v>
+        <v>388</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A94" s="1" t="s">
-        <v>406</v>
+        <v>390</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>407</v>
+        <v>391</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>408</v>
+        <v>392</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A95" s="1" t="s">
-        <v>409</v>
+        <v>393</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>410</v>
+        <v>394</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>411</v>
+        <v>395</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A96" s="1" t="s">
-        <v>412</v>
+        <v>396</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>413</v>
+        <v>397</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>414</v>
+        <v>398</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B97" s="2"/>
-      <c r="C97" s="2"/>
+      <c r="A97" s="1" t="s">
+        <v>399</v>
+      </c>
+      <c r="B97" s="2" t="s">
+        <v>400</v>
+      </c>
+      <c r="C97" s="2" t="s">
+        <v>401</v>
+      </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A98" s="1" t="s">
-        <v>415</v>
+        <v>402</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>416</v>
+        <v>403</v>
       </c>
       <c r="C98" s="2" t="s">
-        <v>417</v>
+        <v>404</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A99" s="1" t="s">
-        <v>418</v>
+        <v>405</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>419</v>
+        <v>406</v>
       </c>
       <c r="C99" s="2" t="s">
-        <v>420</v>
+        <v>407</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A100" s="1" t="s">
-        <v>421</v>
+        <v>408</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>422</v>
+        <v>409</v>
       </c>
       <c r="C100" s="2" t="s">
-        <v>423</v>
+        <v>410</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A101" s="1" t="s">
-        <v>424</v>
+        <v>411</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>425</v>
+        <v>412</v>
       </c>
       <c r="C101" s="2" t="s">
-        <v>426</v>
+        <v>413</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A102" s="1" t="s">
-        <v>427</v>
-      </c>
-      <c r="B102" s="2" t="s">
-        <v>428</v>
-      </c>
-      <c r="C102" s="2" t="s">
-        <v>429</v>
-      </c>
+      <c r="B102" s="2"/>
+      <c r="C102" s="2"/>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A103" s="1" t="s">
-        <v>430</v>
+        <v>414</v>
       </c>
       <c r="B103" s="2" t="s">
-        <v>431</v>
+        <v>415</v>
       </c>
       <c r="C103" s="2" t="s">
-        <v>432</v>
+        <v>416</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A104" s="1" t="s">
-        <v>433</v>
+        <v>417</v>
       </c>
       <c r="B104" s="2" t="s">
-        <v>434</v>
+        <v>418</v>
       </c>
       <c r="C104" s="2" t="s">
-        <v>435</v>
+        <v>419</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A105" s="1" t="s">
-        <v>436</v>
+        <v>420</v>
       </c>
       <c r="B105" s="2" t="s">
-        <v>437</v>
+        <v>421</v>
       </c>
       <c r="C105" s="2" t="s">
-        <v>438</v>
+        <v>422</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B106" s="2"/>
-      <c r="C106" s="2"/>
+      <c r="A106" s="1" t="s">
+        <v>423</v>
+      </c>
+      <c r="B106" s="2" t="s">
+        <v>424</v>
+      </c>
+      <c r="C106" s="2" t="s">
+        <v>425</v>
+      </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A107" s="1" t="s">
-        <v>439</v>
+        <v>426</v>
       </c>
       <c r="B107" s="2" t="s">
-        <v>440</v>
+        <v>427</v>
       </c>
       <c r="C107" s="2" t="s">
-        <v>441</v>
+        <v>428</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A108" s="1" t="s">
-        <v>442</v>
+        <v>429</v>
       </c>
       <c r="B108" s="2" t="s">
-        <v>443</v>
+        <v>430</v>
       </c>
       <c r="C108" s="2" t="s">
-        <v>444</v>
+        <v>431</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A109" s="1" t="s">
-        <v>445</v>
+        <v>432</v>
       </c>
       <c r="B109" s="2" t="s">
-        <v>446</v>
+        <v>433</v>
       </c>
       <c r="C109" s="2" t="s">
-        <v>447</v>
+        <v>434</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A110" s="1" t="s">
-        <v>448</v>
+        <v>435</v>
       </c>
       <c r="B110" s="2" t="s">
-        <v>449</v>
+        <v>436</v>
       </c>
       <c r="C110" s="2" t="s">
-        <v>450</v>
-      </c>
+        <v>437</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B111" s="2"/>
+      <c r="C111" s="2"/>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A112" s="1" t="s">
-        <v>451</v>
+        <v>438</v>
       </c>
       <c r="B112" s="2" t="s">
-        <v>452</v>
+        <v>439</v>
       </c>
       <c r="C112" s="2" t="s">
-        <v>453</v>
+        <v>440</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A113" s="1" t="s">
-        <v>454</v>
+        <v>441</v>
       </c>
       <c r="B113" s="2" t="s">
-        <v>455</v>
+        <v>568</v>
       </c>
       <c r="C113" s="2" t="s">
-        <v>456</v>
+        <v>442</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A114" s="1" t="s">
-        <v>457</v>
+        <v>443</v>
       </c>
       <c r="B114" s="2" t="s">
-        <v>458</v>
+        <v>444</v>
       </c>
       <c r="C114" s="2" t="s">
-        <v>459</v>
+        <v>445</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A115" s="1" t="s">
-        <v>460</v>
+        <v>446</v>
       </c>
       <c r="B115" s="2" t="s">
-        <v>461</v>
+        <v>447</v>
       </c>
       <c r="C115" s="2" t="s">
-        <v>462</v>
-      </c>
-    </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A116" s="1" t="s">
-        <v>463</v>
-      </c>
-      <c r="B116" s="2" t="s">
-        <v>464</v>
-      </c>
-      <c r="C116" s="2" t="s">
-        <v>465</v>
+        <v>448</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A117" s="1" t="s">
-        <v>466</v>
+        <v>449</v>
       </c>
       <c r="B117" s="2" t="s">
-        <v>467</v>
+        <v>450</v>
       </c>
       <c r="C117" s="2" t="s">
-        <v>468</v>
+        <v>451</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A118" s="1" t="s">
-        <v>469</v>
+        <v>452</v>
       </c>
       <c r="B118" s="2" t="s">
-        <v>470</v>
+        <v>453</v>
       </c>
       <c r="C118" s="2" t="s">
-        <v>471</v>
+        <v>454</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A119" s="1" t="s">
+        <v>455</v>
+      </c>
+      <c r="B119" s="2" t="s">
+        <v>456</v>
+      </c>
+      <c r="C119" s="2" t="s">
+        <v>457</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A120" s="1" t="s">
-        <v>472</v>
+        <v>458</v>
       </c>
       <c r="B120" s="2" t="s">
-        <v>473</v>
+        <v>459</v>
       </c>
       <c r="C120" s="2" t="s">
-        <v>474</v>
+        <v>460</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A121" s="1" t="s">
-        <v>475</v>
+        <v>461</v>
       </c>
       <c r="B121" s="2" t="s">
-        <v>476</v>
+        <v>462</v>
       </c>
       <c r="C121" s="2" t="s">
-        <v>477</v>
+        <v>463</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A122" s="1" t="s">
-        <v>478</v>
+        <v>464</v>
       </c>
       <c r="B122" s="2" t="s">
-        <v>479</v>
+        <v>465</v>
       </c>
       <c r="C122" s="2" t="s">
-        <v>480</v>
+        <v>466</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A123" s="1" t="s">
-        <v>481</v>
+        <v>467</v>
       </c>
       <c r="B123" s="2" t="s">
-        <v>482</v>
+        <v>468</v>
       </c>
       <c r="C123" s="2" t="s">
-        <v>483</v>
-      </c>
-    </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A124" s="1" t="s">
-        <v>484</v>
-      </c>
-      <c r="B124" s="2" t="s">
-        <v>485</v>
-      </c>
-      <c r="C124" s="2" t="s">
-        <v>486</v>
+        <v>469</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A125" s="1" t="s">
+        <v>470</v>
+      </c>
+      <c r="B125" s="2" t="s">
+        <v>471</v>
+      </c>
+      <c r="C125" s="2" t="s">
+        <v>472</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A126" s="1" t="s">
-        <v>487</v>
+        <v>473</v>
       </c>
       <c r="B126" s="2" t="s">
-        <v>488</v>
+        <v>474</v>
       </c>
       <c r="C126" s="2" t="s">
-        <v>489</v>
+        <v>475</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A127" s="1" t="s">
-        <v>490</v>
-      </c>
-      <c r="B127" s="1" t="s">
-        <v>491</v>
-      </c>
-      <c r="C127" s="1" t="s">
-        <v>492</v>
+        <v>476</v>
+      </c>
+      <c r="B127" s="2" t="s">
+        <v>477</v>
+      </c>
+      <c r="C127" s="2" t="s">
+        <v>478</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A128" s="1" t="s">
-        <v>493</v>
-      </c>
-      <c r="B128" s="1" t="s">
-        <v>494</v>
-      </c>
-      <c r="C128" s="1" t="s">
-        <v>495</v>
+        <v>479</v>
+      </c>
+      <c r="B128" s="2" t="s">
+        <v>480</v>
+      </c>
+      <c r="C128" s="2" t="s">
+        <v>481</v>
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A129" s="1" t="s">
-        <v>496</v>
+        <v>482</v>
       </c>
       <c r="B129" s="2" t="s">
-        <v>497</v>
-      </c>
-      <c r="C129" s="1" t="s">
-        <v>498</v>
-      </c>
-    </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A130" s="1" t="s">
-        <v>499</v>
-      </c>
-      <c r="B130" s="1" t="s">
-        <v>500</v>
-      </c>
-      <c r="C130" s="1" t="s">
-        <v>501</v>
+        <v>483</v>
+      </c>
+      <c r="C129" s="2" t="s">
+        <v>484</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A131" s="1" t="s">
-        <v>502</v>
+        <v>485</v>
       </c>
       <c r="B131" s="2" t="s">
-        <v>503</v>
+        <v>486</v>
       </c>
       <c r="C131" s="2" t="s">
-        <v>504</v>
+        <v>487</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A132" s="1" t="s">
+        <v>488</v>
+      </c>
+      <c r="B132" s="1" t="s">
+        <v>489</v>
+      </c>
+      <c r="C132" s="1" t="s">
+        <v>490</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A133" s="1" t="s">
-        <v>505</v>
-      </c>
-      <c r="B133" s="2" t="s">
-        <v>506</v>
-      </c>
-      <c r="C133" s="2" t="s">
-        <v>507</v>
+        <v>491</v>
+      </c>
+      <c r="B133" s="1" t="s">
+        <v>492</v>
+      </c>
+      <c r="C133" s="1" t="s">
+        <v>493</v>
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A134" s="1" t="s">
-        <v>508</v>
+        <v>494</v>
       </c>
       <c r="B134" s="2" t="s">
-        <v>509</v>
-      </c>
-      <c r="C134" s="2" t="s">
-        <v>510</v>
+        <v>495</v>
+      </c>
+      <c r="C134" s="1" t="s">
+        <v>496</v>
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B135" s="2"/>
-      <c r="C135" s="2"/>
+      <c r="A135" s="1" t="s">
+        <v>497</v>
+      </c>
+      <c r="B135" s="1" t="s">
+        <v>498</v>
+      </c>
+      <c r="C135" s="1" t="s">
+        <v>499</v>
+      </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A136" s="1" t="s">
-        <v>511</v>
+        <v>500</v>
       </c>
       <c r="B136" s="2" t="s">
-        <v>512</v>
+        <v>501</v>
       </c>
       <c r="C136" s="2" t="s">
-        <v>513</v>
-      </c>
-    </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A137" s="1" t="s">
-        <v>514</v>
-      </c>
-      <c r="B137" s="2" t="s">
-        <v>515</v>
-      </c>
-      <c r="C137" s="2" t="s">
-        <v>516</v>
+        <v>502</v>
       </c>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A138" s="1" t="s">
-        <v>517</v>
+        <v>503</v>
       </c>
       <c r="B138" s="2" t="s">
-        <v>518</v>
+        <v>504</v>
       </c>
       <c r="C138" s="2" t="s">
-        <v>519</v>
+        <v>505</v>
       </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A139" s="1" t="s">
-        <v>520</v>
+        <v>506</v>
       </c>
       <c r="B139" s="2" t="s">
-        <v>521</v>
+        <v>507</v>
       </c>
       <c r="C139" s="2" t="s">
-        <v>522</v>
+        <v>508</v>
       </c>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A140" s="1" t="s">
-        <v>523</v>
-      </c>
-      <c r="B140" s="2" t="s">
-        <v>524</v>
-      </c>
-      <c r="C140" s="2" t="s">
-        <v>525</v>
-      </c>
+      <c r="B140" s="2"/>
+      <c r="C140" s="2"/>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B141" s="2"/>
-      <c r="C141" s="2"/>
+      <c r="A141" s="1" t="s">
+        <v>509</v>
+      </c>
+      <c r="B141" s="2" t="s">
+        <v>510</v>
+      </c>
+      <c r="C141" s="2" t="s">
+        <v>511</v>
+      </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A142" s="1" t="s">
-        <v>526</v>
+        <v>512</v>
       </c>
       <c r="B142" s="2" t="s">
-        <v>527</v>
+        <v>513</v>
       </c>
       <c r="C142" s="2" t="s">
-        <v>528</v>
+        <v>514</v>
       </c>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A143" s="1" t="s">
-        <v>529</v>
+        <v>515</v>
       </c>
       <c r="B143" s="2" t="s">
-        <v>530</v>
+        <v>516</v>
       </c>
       <c r="C143" s="2" t="s">
-        <v>531</v>
+        <v>517</v>
+      </c>
+    </row>
+    <row r="144" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A144" s="1" t="s">
+        <v>518</v>
+      </c>
+      <c r="B144" s="2" t="s">
+        <v>519</v>
+      </c>
+      <c r="C144" s="2" t="s">
+        <v>520</v>
       </c>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A145" s="1" t="s">
-        <v>532</v>
-      </c>
-      <c r="B145" s="1" t="s">
-        <v>533</v>
-      </c>
-      <c r="C145" s="1" t="s">
-        <v>534</v>
+        <v>521</v>
+      </c>
+      <c r="B145" s="2" t="s">
+        <v>522</v>
+      </c>
+      <c r="C145" s="2" t="s">
+        <v>523</v>
       </c>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A146" s="1" t="s">
-        <v>535</v>
-      </c>
-      <c r="B146" s="1" t="s">
-        <v>536</v>
-      </c>
-      <c r="C146" s="1" t="s">
-        <v>537</v>
-      </c>
+      <c r="B146" s="2"/>
+      <c r="C146" s="2"/>
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A147" s="1" t="s">
-        <v>538</v>
-      </c>
-      <c r="B147" s="1" t="s">
-        <v>539</v>
-      </c>
-      <c r="C147" s="1" t="s">
-        <v>540</v>
+        <v>524</v>
+      </c>
+      <c r="B147" s="2" t="s">
+        <v>525</v>
+      </c>
+      <c r="C147" s="2" t="s">
+        <v>526</v>
       </c>
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A148" s="1" t="s">
-        <v>541</v>
-      </c>
-      <c r="B148" s="1" t="s">
-        <v>542</v>
-      </c>
-      <c r="C148" s="1" t="s">
-        <v>543</v>
-      </c>
-    </row>
-    <row r="149" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A149" s="1" t="s">
-        <v>544</v>
-      </c>
-      <c r="B149" s="2" t="s">
-        <v>545</v>
-      </c>
-      <c r="C149" s="2" t="s">
-        <v>546</v>
+        <v>527</v>
+      </c>
+      <c r="B148" s="2" t="s">
+        <v>528</v>
+      </c>
+      <c r="C148" s="2" t="s">
+        <v>529</v>
       </c>
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A150" s="1" t="s">
-        <v>547</v>
+        <v>530</v>
       </c>
       <c r="B150" s="1" t="s">
-        <v>548</v>
+        <v>531</v>
       </c>
       <c r="C150" s="1" t="s">
-        <v>549</v>
+        <v>532</v>
       </c>
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A151" s="1" t="s">
+        <v>533</v>
+      </c>
+      <c r="B151" s="1" t="s">
+        <v>534</v>
+      </c>
+      <c r="C151" s="1" t="s">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="152" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A152" s="1" t="s">
+        <v>536</v>
+      </c>
+      <c r="B152" s="1" t="s">
+        <v>537</v>
+      </c>
+      <c r="C152" s="1" t="s">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="153" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A153" s="1" t="s">
+        <v>539</v>
+      </c>
+      <c r="B153" s="1" t="s">
+        <v>540</v>
+      </c>
+      <c r="C153" s="1" t="s">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="154" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A154" s="1" t="s">
+        <v>542</v>
+      </c>
+      <c r="B154" s="2" t="s">
+        <v>543</v>
+      </c>
+      <c r="C154" s="2" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="155" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A155" s="1" t="s">
+        <v>545</v>
+      </c>
+      <c r="B155" s="1" t="s">
+        <v>546</v>
+      </c>
+      <c r="C155" s="1" t="s">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="156" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A156" s="1" t="s">
+        <v>548</v>
+      </c>
+      <c r="B156" s="1" t="s">
+        <v>549</v>
+      </c>
+      <c r="C156" s="1" t="s">
         <v>550</v>
-      </c>
-      <c r="B151" s="1" t="s">
-        <v>551</v>
-      </c>
-      <c r="C151" s="1" t="s">
-        <v>552</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update variable/argument naming to consider Folders
</commit_message>
<xml_diff>
--- a/Config.xlsx
+++ b/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mateus.cruz\Documents\GitHub\OrchestratorManager\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A734B059-D77E-493A-89B8-4C4A43A745C4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96A0A7B2-2386-4D2C-8682-C2F043A4B870}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="615" uniqueCount="572">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="624" uniqueCount="581">
   <si>
     <t>Name</t>
   </si>
@@ -161,21 +161,9 @@
     <t>Path to the file to be used as Control Panel form.</t>
   </si>
   <si>
-    <t>OrganizationUnitsPanelTemplatePath</t>
-  </si>
-  <si>
-    <t>Core\Forms\OrganizationUnitsPanelTemplate.html</t>
-  </si>
-  <si>
     <t>Path to the template file used to generate the Organization Units Panel form.</t>
   </si>
   <si>
-    <t>OrganizationUnitsPanelPath</t>
-  </si>
-  <si>
-    <t>Core\Forms\OrganizationUnitsPanel.html</t>
-  </si>
-  <si>
     <t>Path to the file to be used as Organization Units Panel form.</t>
   </si>
   <si>
@@ -1761,6 +1749,45 @@
   </si>
   <si>
     <t>ErrorDuringExecutionLog</t>
+  </si>
+  <si>
+    <t>OUFolderNameNotSpecified</t>
+  </si>
+  <si>
+    <t>Folder (Organization Unit) name not specified.</t>
+  </si>
+  <si>
+    <t>フォルダー名（組織単位名）が指定されませんでした。</t>
+  </si>
+  <si>
+    <t>OUFolderNotFound</t>
+  </si>
+  <si>
+    <t>No Folder (Organization Unit) found.</t>
+  </si>
+  <si>
+    <t>フォルダー（組織単位）が見つかりませんでした。</t>
+  </si>
+  <si>
+    <t>OUFolderIDInvalidOrNotSpecified</t>
+  </si>
+  <si>
+    <t>Folder (Organization Unit) ID invalid or not specified.</t>
+  </si>
+  <si>
+    <t>フォルダー（組織単位）IDが無効か指定されませんでした。</t>
+  </si>
+  <si>
+    <t>OUFoldersPanelTemplatePath</t>
+  </si>
+  <si>
+    <t>OUFoldersPanelPath</t>
+  </si>
+  <si>
+    <t>Core\Forms\OUFoldersPanelTemplate.html</t>
+  </si>
+  <si>
+    <t>Core\Forms\OUFoldersPanel.html</t>
   </si>
 </sst>
 </file>
@@ -1853,8 +1880,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table13" displayName="Table13" ref="A1:C156" totalsRowShown="0">
-  <autoFilter ref="A1:C156" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table13" displayName="Table13" ref="A1:C159" totalsRowShown="0">
+  <autoFilter ref="A1:C159" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Name"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="EN"/>
@@ -2156,7 +2183,7 @@
         <v>3</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>4</v>
@@ -2167,7 +2194,7 @@
         <v>5</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>552</v>
+        <v>548</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>6</v>
@@ -2178,7 +2205,7 @@
         <v>7</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>553</v>
+        <v>549</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>8</v>
@@ -2200,7 +2227,7 @@
         <v>12</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>554</v>
+        <v>550</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>13</v>
@@ -2353,519 +2380,519 @@
     </row>
     <row r="12" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
+        <v>577</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>579</v>
+      </c>
+      <c r="C12" s="2" t="s">
         <v>38</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
-        <v>41</v>
+        <v>578</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>42</v>
+        <v>580</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="B25" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C25" s="2" t="s">
         <v>70</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="1" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" s="1" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A32" s="1" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" s="1" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A34" s="1" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A35" s="1" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A36" s="1" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A37" s="1" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
     </row>
     <row r="38" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A38" s="1" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A39" s="1" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A40" s="1" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
     </row>
     <row r="41" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A41" s="1" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
     </row>
     <row r="42" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A42" s="1" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A43" s="1" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
     </row>
     <row r="44" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A44" s="1" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
     </row>
     <row r="45" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A45" s="1" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
     </row>
     <row r="46" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A46" s="1" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
     </row>
     <row r="47" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A47" s="1" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A48" s="1" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="49" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A49" s="1" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
     </row>
     <row r="50" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A50" s="1" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A51" s="1" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
     </row>
     <row r="52" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A52" s="1" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
     </row>
     <row r="53" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A53" s="1" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A54" s="1" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
     </row>
     <row r="55" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A55" s="1" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
     </row>
     <row r="56" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A56" s="1" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
     </row>
     <row r="57" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A57" s="1" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
     </row>
     <row r="58" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A58" s="1" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
     </row>
   </sheetData>
@@ -2883,7 +2910,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1927ABA9-1814-4487-9CEC-ABDCAF91481F}">
-  <dimension ref="A1:C156"/>
+  <dimension ref="A1:C159"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -2901,340 +2928,340 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="43.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A30" s="1" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A31" s="1" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.35">
@@ -3243,101 +3270,101 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A33" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A34" s="1" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A35" s="1" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A36" s="1" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A37" s="1" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A38" s="1" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A39" s="1" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A40" s="1" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A41" s="1" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.35">
@@ -3346,1159 +3373,1192 @@
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A43" s="1" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A44" s="1" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A45" s="1" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A46" s="1" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A47" s="1" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A48" s="1" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A49" s="1" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A50" s="1" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A51" s="1" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A52" s="1" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A53" s="1" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A54" s="1" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A55" s="1" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A56" s="1" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A57" s="1" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A58" s="1" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A59" s="1" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A60" s="1" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A61" s="1" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A62" s="1" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A63" s="1" t="s">
-        <v>562</v>
+        <v>558</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>563</v>
+        <v>559</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>564</v>
+        <v>560</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A64" s="1" t="s">
-        <v>571</v>
+        <v>567</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>569</v>
+        <v>565</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>570</v>
+        <v>566</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A65" s="1" t="s">
-        <v>565</v>
+        <v>561</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>566</v>
+        <v>562</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>567</v>
+        <v>563</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A66" s="1" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A67" s="1" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A68" s="1" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A69" s="1" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A70" s="1" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
     </row>
     <row r="71" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A71" s="1" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>558</v>
+        <v>554</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A72" s="1" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A73" s="1" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A74" s="1" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A75" s="1" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A76" s="1" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>349</v>
+        <v>345</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>350</v>
+        <v>346</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A77" s="1" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>352</v>
+        <v>348</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A78" s="1" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>356</v>
+        <v>352</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A79" s="1" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A80" s="1" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A81" s="1" t="s">
-        <v>555</v>
+        <v>551</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>556</v>
+        <v>552</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>557</v>
+        <v>553</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A82" s="1" t="s">
-        <v>560</v>
+        <v>556</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>561</v>
+        <v>557</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>559</v>
+        <v>555</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B83" s="2"/>
-      <c r="C83" s="2"/>
+      <c r="A83" s="1" t="s">
+        <v>568</v>
+      </c>
+      <c r="B83" s="2" t="s">
+        <v>569</v>
+      </c>
+      <c r="C83" s="2" t="s">
+        <v>570</v>
+      </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A84" s="1" t="s">
-        <v>363</v>
+        <v>571</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>364</v>
+        <v>572</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>365</v>
+        <v>573</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A85" s="1" t="s">
-        <v>366</v>
+        <v>574</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>367</v>
+        <v>575</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>368</v>
+        <v>576</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A86" s="1" t="s">
-        <v>369</v>
-      </c>
-      <c r="B86" s="2" t="s">
-        <v>370</v>
-      </c>
-      <c r="C86" s="2" t="s">
-        <v>371</v>
-      </c>
+      <c r="B86" s="2"/>
+      <c r="C86" s="2"/>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A87" s="1" t="s">
-        <v>372</v>
+        <v>359</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>373</v>
+        <v>360</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>374</v>
+        <v>361</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A88" s="1" t="s">
-        <v>375</v>
+        <v>362</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>376</v>
+        <v>363</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>377</v>
+        <v>364</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A89" s="1" t="s">
-        <v>378</v>
+        <v>365</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>379</v>
+        <v>366</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>380</v>
+        <v>367</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A90" s="1" t="s">
-        <v>381</v>
+        <v>368</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>382</v>
+        <v>369</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>383</v>
+        <v>370</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A91" s="1" t="s">
-        <v>384</v>
+        <v>371</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>385</v>
+        <v>372</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>386</v>
+        <v>373</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B92" s="2"/>
-      <c r="C92" s="2"/>
+      <c r="A92" s="1" t="s">
+        <v>374</v>
+      </c>
+      <c r="B92" s="2" t="s">
+        <v>375</v>
+      </c>
+      <c r="C92" s="2" t="s">
+        <v>376</v>
+      </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A93" s="1" t="s">
-        <v>387</v>
+        <v>377</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>388</v>
+        <v>378</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>389</v>
+        <v>379</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A94" s="1" t="s">
-        <v>390</v>
+        <v>380</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>391</v>
+        <v>381</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>392</v>
+        <v>382</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A95" s="1" t="s">
-        <v>393</v>
-      </c>
-      <c r="B95" s="2" t="s">
-        <v>394</v>
-      </c>
-      <c r="C95" s="2" t="s">
-        <v>395</v>
-      </c>
+      <c r="B95" s="2"/>
+      <c r="C95" s="2"/>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A96" s="1" t="s">
-        <v>396</v>
+        <v>383</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>397</v>
+        <v>384</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>398</v>
+        <v>385</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A97" s="1" t="s">
-        <v>399</v>
+        <v>386</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>400</v>
+        <v>387</v>
       </c>
       <c r="C97" s="2" t="s">
-        <v>401</v>
+        <v>388</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A98" s="1" t="s">
-        <v>402</v>
+        <v>389</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>403</v>
+        <v>390</v>
       </c>
       <c r="C98" s="2" t="s">
-        <v>404</v>
+        <v>391</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A99" s="1" t="s">
-        <v>405</v>
+        <v>392</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>406</v>
+        <v>393</v>
       </c>
       <c r="C99" s="2" t="s">
-        <v>407</v>
+        <v>394</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A100" s="1" t="s">
-        <v>408</v>
+        <v>395</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>409</v>
+        <v>396</v>
       </c>
       <c r="C100" s="2" t="s">
-        <v>410</v>
+        <v>397</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A101" s="1" t="s">
-        <v>411</v>
+        <v>398</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>412</v>
+        <v>399</v>
       </c>
       <c r="C101" s="2" t="s">
-        <v>413</v>
+        <v>400</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B102" s="2"/>
-      <c r="C102" s="2"/>
+      <c r="A102" s="1" t="s">
+        <v>401</v>
+      </c>
+      <c r="B102" s="2" t="s">
+        <v>402</v>
+      </c>
+      <c r="C102" s="2" t="s">
+        <v>403</v>
+      </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A103" s="1" t="s">
-        <v>414</v>
+        <v>404</v>
       </c>
       <c r="B103" s="2" t="s">
-        <v>415</v>
+        <v>405</v>
       </c>
       <c r="C103" s="2" t="s">
-        <v>416</v>
+        <v>406</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A104" s="1" t="s">
-        <v>417</v>
+        <v>407</v>
       </c>
       <c r="B104" s="2" t="s">
-        <v>418</v>
+        <v>408</v>
       </c>
       <c r="C104" s="2" t="s">
-        <v>419</v>
+        <v>409</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A105" s="1" t="s">
-        <v>420</v>
-      </c>
-      <c r="B105" s="2" t="s">
-        <v>421</v>
-      </c>
-      <c r="C105" s="2" t="s">
-        <v>422</v>
-      </c>
+      <c r="B105" s="2"/>
+      <c r="C105" s="2"/>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A106" s="1" t="s">
-        <v>423</v>
+        <v>410</v>
       </c>
       <c r="B106" s="2" t="s">
-        <v>424</v>
+        <v>411</v>
       </c>
       <c r="C106" s="2" t="s">
-        <v>425</v>
+        <v>412</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A107" s="1" t="s">
-        <v>426</v>
+        <v>413</v>
       </c>
       <c r="B107" s="2" t="s">
-        <v>427</v>
+        <v>414</v>
       </c>
       <c r="C107" s="2" t="s">
-        <v>428</v>
+        <v>415</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A108" s="1" t="s">
-        <v>429</v>
+        <v>416</v>
       </c>
       <c r="B108" s="2" t="s">
-        <v>430</v>
+        <v>417</v>
       </c>
       <c r="C108" s="2" t="s">
-        <v>431</v>
+        <v>418</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A109" s="1" t="s">
-        <v>432</v>
+        <v>419</v>
       </c>
       <c r="B109" s="2" t="s">
-        <v>433</v>
+        <v>420</v>
       </c>
       <c r="C109" s="2" t="s">
-        <v>434</v>
+        <v>421</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A110" s="1" t="s">
-        <v>435</v>
+        <v>422</v>
       </c>
       <c r="B110" s="2" t="s">
-        <v>436</v>
+        <v>423</v>
       </c>
       <c r="C110" s="2" t="s">
-        <v>437</v>
+        <v>424</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B111" s="2"/>
-      <c r="C111" s="2"/>
+      <c r="A111" s="1" t="s">
+        <v>425</v>
+      </c>
+      <c r="B111" s="2" t="s">
+        <v>426</v>
+      </c>
+      <c r="C111" s="2" t="s">
+        <v>427</v>
+      </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A112" s="1" t="s">
-        <v>438</v>
+        <v>428</v>
       </c>
       <c r="B112" s="2" t="s">
-        <v>439</v>
+        <v>429</v>
       </c>
       <c r="C112" s="2" t="s">
-        <v>440</v>
+        <v>430</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A113" s="1" t="s">
-        <v>441</v>
+        <v>431</v>
       </c>
       <c r="B113" s="2" t="s">
-        <v>568</v>
+        <v>432</v>
       </c>
       <c r="C113" s="2" t="s">
-        <v>442</v>
+        <v>433</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A114" s="1" t="s">
-        <v>443</v>
-      </c>
-      <c r="B114" s="2" t="s">
-        <v>444</v>
-      </c>
-      <c r="C114" s="2" t="s">
-        <v>445</v>
-      </c>
+      <c r="B114" s="2"/>
+      <c r="C114" s="2"/>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A115" s="1" t="s">
-        <v>446</v>
+        <v>434</v>
       </c>
       <c r="B115" s="2" t="s">
-        <v>447</v>
+        <v>435</v>
       </c>
       <c r="C115" s="2" t="s">
-        <v>448</v>
+        <v>436</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A116" s="1" t="s">
+        <v>437</v>
+      </c>
+      <c r="B116" s="2" t="s">
+        <v>564</v>
+      </c>
+      <c r="C116" s="2" t="s">
+        <v>438</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A117" s="1" t="s">
-        <v>449</v>
+        <v>439</v>
       </c>
       <c r="B117" s="2" t="s">
-        <v>450</v>
+        <v>440</v>
       </c>
       <c r="C117" s="2" t="s">
-        <v>451</v>
+        <v>441</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A118" s="1" t="s">
-        <v>452</v>
+        <v>442</v>
       </c>
       <c r="B118" s="2" t="s">
-        <v>453</v>
+        <v>443</v>
       </c>
       <c r="C118" s="2" t="s">
-        <v>454</v>
-      </c>
-    </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A119" s="1" t="s">
-        <v>455</v>
-      </c>
-      <c r="B119" s="2" t="s">
-        <v>456</v>
-      </c>
-      <c r="C119" s="2" t="s">
-        <v>457</v>
+        <v>444</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A120" s="1" t="s">
-        <v>458</v>
+        <v>445</v>
       </c>
       <c r="B120" s="2" t="s">
-        <v>459</v>
+        <v>446</v>
       </c>
       <c r="C120" s="2" t="s">
-        <v>460</v>
+        <v>447</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A121" s="1" t="s">
-        <v>461</v>
+        <v>448</v>
       </c>
       <c r="B121" s="2" t="s">
-        <v>462</v>
+        <v>449</v>
       </c>
       <c r="C121" s="2" t="s">
-        <v>463</v>
+        <v>450</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A122" s="1" t="s">
-        <v>464</v>
+        <v>451</v>
       </c>
       <c r="B122" s="2" t="s">
-        <v>465</v>
+        <v>452</v>
       </c>
       <c r="C122" s="2" t="s">
-        <v>466</v>
+        <v>453</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A123" s="1" t="s">
-        <v>467</v>
+        <v>454</v>
       </c>
       <c r="B123" s="2" t="s">
-        <v>468</v>
+        <v>455</v>
       </c>
       <c r="C123" s="2" t="s">
-        <v>469</v>
+        <v>456</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A124" s="1" t="s">
+        <v>457</v>
+      </c>
+      <c r="B124" s="2" t="s">
+        <v>458</v>
+      </c>
+      <c r="C124" s="2" t="s">
+        <v>459</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A125" s="1" t="s">
-        <v>470</v>
+        <v>460</v>
       </c>
       <c r="B125" s="2" t="s">
-        <v>471</v>
+        <v>461</v>
       </c>
       <c r="C125" s="2" t="s">
-        <v>472</v>
+        <v>462</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A126" s="1" t="s">
-        <v>473</v>
+        <v>463</v>
       </c>
       <c r="B126" s="2" t="s">
-        <v>474</v>
+        <v>464</v>
       </c>
       <c r="C126" s="2" t="s">
-        <v>475</v>
-      </c>
-    </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A127" s="1" t="s">
-        <v>476</v>
-      </c>
-      <c r="B127" s="2" t="s">
-        <v>477</v>
-      </c>
-      <c r="C127" s="2" t="s">
-        <v>478</v>
+        <v>465</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A128" s="1" t="s">
-        <v>479</v>
+        <v>466</v>
       </c>
       <c r="B128" s="2" t="s">
-        <v>480</v>
+        <v>467</v>
       </c>
       <c r="C128" s="2" t="s">
-        <v>481</v>
+        <v>468</v>
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A129" s="1" t="s">
-        <v>482</v>
+        <v>469</v>
       </c>
       <c r="B129" s="2" t="s">
-        <v>483</v>
+        <v>470</v>
       </c>
       <c r="C129" s="2" t="s">
-        <v>484</v>
+        <v>471</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A130" s="1" t="s">
+        <v>472</v>
+      </c>
+      <c r="B130" s="2" t="s">
+        <v>473</v>
+      </c>
+      <c r="C130" s="2" t="s">
+        <v>474</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A131" s="1" t="s">
-        <v>485</v>
+        <v>475</v>
       </c>
       <c r="B131" s="2" t="s">
-        <v>486</v>
+        <v>476</v>
       </c>
       <c r="C131" s="2" t="s">
-        <v>487</v>
+        <v>477</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A132" s="1" t="s">
-        <v>488</v>
-      </c>
-      <c r="B132" s="1" t="s">
-        <v>489</v>
-      </c>
-      <c r="C132" s="1" t="s">
-        <v>490</v>
-      </c>
-    </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A133" s="1" t="s">
-        <v>491</v>
-      </c>
-      <c r="B133" s="1" t="s">
-        <v>492</v>
-      </c>
-      <c r="C133" s="1" t="s">
-        <v>493</v>
+        <v>478</v>
+      </c>
+      <c r="B132" s="2" t="s">
+        <v>479</v>
+      </c>
+      <c r="C132" s="2" t="s">
+        <v>480</v>
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A134" s="1" t="s">
-        <v>494</v>
+        <v>481</v>
       </c>
       <c r="B134" s="2" t="s">
-        <v>495</v>
-      </c>
-      <c r="C134" s="1" t="s">
-        <v>496</v>
+        <v>482</v>
+      </c>
+      <c r="C134" s="2" t="s">
+        <v>483</v>
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A135" s="1" t="s">
-        <v>497</v>
+        <v>484</v>
       </c>
       <c r="B135" s="1" t="s">
-        <v>498</v>
+        <v>485</v>
       </c>
       <c r="C135" s="1" t="s">
-        <v>499</v>
+        <v>486</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A136" s="1" t="s">
-        <v>500</v>
-      </c>
-      <c r="B136" s="2" t="s">
-        <v>501</v>
-      </c>
-      <c r="C136" s="2" t="s">
-        <v>502</v>
+        <v>487</v>
+      </c>
+      <c r="B136" s="1" t="s">
+        <v>488</v>
+      </c>
+      <c r="C136" s="1" t="s">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A137" s="1" t="s">
+        <v>490</v>
+      </c>
+      <c r="B137" s="2" t="s">
+        <v>491</v>
+      </c>
+      <c r="C137" s="1" t="s">
+        <v>492</v>
       </c>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A138" s="1" t="s">
-        <v>503</v>
-      </c>
-      <c r="B138" s="2" t="s">
-        <v>504</v>
-      </c>
-      <c r="C138" s="2" t="s">
-        <v>505</v>
+        <v>493</v>
+      </c>
+      <c r="B138" s="1" t="s">
+        <v>494</v>
+      </c>
+      <c r="C138" s="1" t="s">
+        <v>495</v>
       </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A139" s="1" t="s">
-        <v>506</v>
+        <v>496</v>
       </c>
       <c r="B139" s="2" t="s">
-        <v>507</v>
+        <v>497</v>
       </c>
       <c r="C139" s="2" t="s">
-        <v>508</v>
-      </c>
-    </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B140" s="2"/>
-      <c r="C140" s="2"/>
+        <v>498</v>
+      </c>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A141" s="1" t="s">
-        <v>509</v>
+        <v>499</v>
       </c>
       <c r="B141" s="2" t="s">
-        <v>510</v>
+        <v>500</v>
       </c>
       <c r="C141" s="2" t="s">
-        <v>511</v>
+        <v>501</v>
       </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A142" s="1" t="s">
-        <v>512</v>
+        <v>502</v>
       </c>
       <c r="B142" s="2" t="s">
-        <v>513</v>
+        <v>503</v>
       </c>
       <c r="C142" s="2" t="s">
-        <v>514</v>
+        <v>504</v>
       </c>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A143" s="1" t="s">
-        <v>515</v>
-      </c>
-      <c r="B143" s="2" t="s">
-        <v>516</v>
-      </c>
-      <c r="C143" s="2" t="s">
-        <v>517</v>
-      </c>
+      <c r="B143" s="2"/>
+      <c r="C143" s="2"/>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A144" s="1" t="s">
-        <v>518</v>
+        <v>505</v>
       </c>
       <c r="B144" s="2" t="s">
-        <v>519</v>
+        <v>506</v>
       </c>
       <c r="C144" s="2" t="s">
-        <v>520</v>
+        <v>507</v>
       </c>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A145" s="1" t="s">
-        <v>521</v>
+        <v>508</v>
       </c>
       <c r="B145" s="2" t="s">
-        <v>522</v>
+        <v>509</v>
       </c>
       <c r="C145" s="2" t="s">
-        <v>523</v>
+        <v>510</v>
       </c>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B146" s="2"/>
-      <c r="C146" s="2"/>
+      <c r="A146" s="1" t="s">
+        <v>511</v>
+      </c>
+      <c r="B146" s="2" t="s">
+        <v>512</v>
+      </c>
+      <c r="C146" s="2" t="s">
+        <v>513</v>
+      </c>
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A147" s="1" t="s">
-        <v>524</v>
+        <v>514</v>
       </c>
       <c r="B147" s="2" t="s">
-        <v>525</v>
+        <v>515</v>
       </c>
       <c r="C147" s="2" t="s">
-        <v>526</v>
+        <v>516</v>
       </c>
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A148" s="1" t="s">
-        <v>527</v>
+        <v>517</v>
       </c>
       <c r="B148" s="2" t="s">
-        <v>528</v>
+        <v>518</v>
       </c>
       <c r="C148" s="2" t="s">
-        <v>529</v>
-      </c>
+        <v>519</v>
+      </c>
+    </row>
+    <row r="149" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B149" s="2"/>
+      <c r="C149" s="2"/>
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A150" s="1" t="s">
-        <v>530</v>
-      </c>
-      <c r="B150" s="1" t="s">
-        <v>531</v>
-      </c>
-      <c r="C150" s="1" t="s">
-        <v>532</v>
+        <v>520</v>
+      </c>
+      <c r="B150" s="2" t="s">
+        <v>521</v>
+      </c>
+      <c r="C150" s="2" t="s">
+        <v>522</v>
       </c>
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A151" s="1" t="s">
-        <v>533</v>
-      </c>
-      <c r="B151" s="1" t="s">
-        <v>534</v>
-      </c>
-      <c r="C151" s="1" t="s">
-        <v>535</v>
-      </c>
-    </row>
-    <row r="152" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A152" s="1" t="s">
-        <v>536</v>
-      </c>
-      <c r="B152" s="1" t="s">
-        <v>537</v>
-      </c>
-      <c r="C152" s="1" t="s">
-        <v>538</v>
+        <v>523</v>
+      </c>
+      <c r="B151" s="2" t="s">
+        <v>524</v>
+      </c>
+      <c r="C151" s="2" t="s">
+        <v>525</v>
       </c>
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A153" s="1" t="s">
-        <v>539</v>
+        <v>526</v>
       </c>
       <c r="B153" s="1" t="s">
-        <v>540</v>
+        <v>527</v>
       </c>
       <c r="C153" s="1" t="s">
-        <v>541</v>
+        <v>528</v>
       </c>
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A154" s="1" t="s">
-        <v>542</v>
-      </c>
-      <c r="B154" s="2" t="s">
-        <v>543</v>
-      </c>
-      <c r="C154" s="2" t="s">
-        <v>544</v>
+        <v>529</v>
+      </c>
+      <c r="B154" s="1" t="s">
+        <v>530</v>
+      </c>
+      <c r="C154" s="1" t="s">
+        <v>531</v>
       </c>
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A155" s="1" t="s">
-        <v>545</v>
+        <v>532</v>
       </c>
       <c r="B155" s="1" t="s">
-        <v>546</v>
+        <v>533</v>
       </c>
       <c r="C155" s="1" t="s">
-        <v>547</v>
+        <v>534</v>
       </c>
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A156" s="1" t="s">
-        <v>548</v>
+        <v>535</v>
       </c>
       <c r="B156" s="1" t="s">
-        <v>549</v>
+        <v>536</v>
       </c>
       <c r="C156" s="1" t="s">
-        <v>550</v>
+        <v>537</v>
+      </c>
+    </row>
+    <row r="157" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A157" s="1" t="s">
+        <v>538</v>
+      </c>
+      <c r="B157" s="2" t="s">
+        <v>539</v>
+      </c>
+      <c r="C157" s="2" t="s">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="158" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A158" s="1" t="s">
+        <v>541</v>
+      </c>
+      <c r="B158" s="1" t="s">
+        <v>542</v>
+      </c>
+      <c r="C158" s="1" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="159" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A159" s="1" t="s">
+        <v>544</v>
+      </c>
+      <c r="B159" s="1" t="s">
+        <v>545</v>
+      </c>
+      <c r="C159" s="1" t="s">
+        <v>546</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add data validation to workbooks
</commit_message>
<xml_diff>
--- a/Config.xlsx
+++ b/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mateus.cruz\Documents\GitHub\OrchestratorManager\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96A0A7B2-2386-4D2C-8682-C2F043A4B870}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9E1EE63-DDB4-4F3D-AD09-751345F7DB40}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2156,7 +2156,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D89C9C48-5454-47C4-AB1D-448E4519251A}">
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Automatically create a working copy of entities workbooks
</commit_message>
<xml_diff>
--- a/Config.xlsx
+++ b/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mateus.cruz\Documents\GitHub\OrchestratorManager\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9E1EE63-DDB4-4F3D-AD09-751345F7DB40}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{824B9220-6F42-42BD-A7AE-CCFB824A1962}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="624" uniqueCount="581">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="628" uniqueCount="585">
   <si>
     <t>Name</t>
   </si>
@@ -61,6 +61,9 @@
   </si>
   <si>
     <t>OnPremisesOrchestratorURL</t>
+  </si>
+  <si>
+    <t>https://myOrchestratorURL</t>
   </si>
   <si>
     <t>URL of the Orchestrator instance to be used. 
@@ -71,13 +74,14 @@
     <t>OnPremisesOrchestratorVersion</t>
   </si>
   <si>
-    <t>202004</t>
-  </si>
-  <si>
     <t>Version of the Orchestrator instance to be used. 
 This parameter is exclusive to on-premises Orchestrator instances.
 The specified value must be in the form YYYYMM, where YYYY is the 4-digit representation of an year and MM is the 2-digit representation of a month.
-Sample values: 201804, 201904, 201910, 202004</t>
+Supported values: 
+201804
+201904
+201910
+202004</t>
   </si>
   <si>
     <t>CloudAccountName</t>
@@ -161,9 +165,21 @@
     <t>Path to the file to be used as Control Panel form.</t>
   </si>
   <si>
+    <t>OUFoldersPanelTemplatePath</t>
+  </si>
+  <si>
+    <t>Core\Forms\OUFoldersPanelTemplate.html</t>
+  </si>
+  <si>
     <t>Path to the template file used to generate the Organization Units Panel form.</t>
   </si>
   <si>
+    <t>OUFoldersPanelPath</t>
+  </si>
+  <si>
+    <t>Core\Forms\OUFoldersPanel.html</t>
+  </si>
+  <si>
     <t>Path to the file to be used as Organization Units Panel form.</t>
   </si>
   <si>
@@ -185,6 +201,24 @@
     <t>Path to the file to be used as Authentication Panel form.</t>
   </si>
   <si>
+    <t>WorkbooksUsingOUsPath</t>
+  </si>
+  <si>
+    <t>Workbooks\UsingOUs</t>
+  </si>
+  <si>
+    <t>Path to the folder containing templates of entities workbooks that use Organization Units.</t>
+  </si>
+  <si>
+    <t>WorkbooksUsingFoldersPath</t>
+  </si>
+  <si>
+    <t>Workbooks\UsingFolders</t>
+  </si>
+  <si>
+    <t>Path to the folder containing templates of entities workbooks that use Folders.</t>
+  </si>
+  <si>
     <t>CloudCredentialName</t>
   </si>
   <si>
@@ -734,82 +768,82 @@
     <t>AssetConfigFilePath</t>
   </si>
   <si>
-    <t>EN\Assets.xlsx</t>
-  </si>
-  <si>
-    <t>JA\アセット.xlsx</t>
+    <t>Assets.xlsx</t>
+  </si>
+  <si>
+    <t>アセット.xlsx</t>
   </si>
   <si>
     <t>UserConfigFilePath</t>
   </si>
   <si>
-    <t>EN\Users.xlsx</t>
-  </si>
-  <si>
-    <t>JA\ユーザー.xlsx</t>
+    <t>Users.xlsx</t>
+  </si>
+  <si>
+    <t>ユーザー.xlsx</t>
   </si>
   <si>
     <t>RobotConfigFilePath</t>
   </si>
   <si>
-    <t>EN\Robots.xlsx</t>
-  </si>
-  <si>
-    <t>JA\ロボット.xlsx</t>
+    <t>Robots.xlsx</t>
+  </si>
+  <si>
+    <t>ロボット.xlsx</t>
   </si>
   <si>
     <t>MachineConfigFilePath</t>
   </si>
   <si>
-    <t>EN\Machines.xlsx</t>
-  </si>
-  <si>
-    <t>JA\マシン.xlsx</t>
+    <t>Machines.xlsx</t>
+  </si>
+  <si>
+    <t>マシン.xlsx</t>
   </si>
   <si>
     <t>EnvironmentConfigFilePath</t>
   </si>
   <si>
-    <t>EN\Environments.xlsx</t>
-  </si>
-  <si>
-    <t>JA\ロボットグループ.xlsx</t>
+    <t>Environments.xlsx</t>
+  </si>
+  <si>
+    <t>ロボットグループ.xlsx</t>
   </si>
   <si>
     <t>ProcessConfigFilePath</t>
   </si>
   <si>
-    <t>EN\Processes.xlsx</t>
-  </si>
-  <si>
-    <t>JA\プロセス.xlsx</t>
+    <t>Processes.xlsx</t>
+  </si>
+  <si>
+    <t>プロセス.xlsx</t>
   </si>
   <si>
     <t>OrganizationUnitConfigFilePath</t>
   </si>
   <si>
-    <t>EN\OrganizationUnits.xlsx</t>
-  </si>
-  <si>
-    <t>JA\組織単位.xlsx</t>
+    <t>OrganizationUnits.xlsx</t>
+  </si>
+  <si>
+    <t>組織単位.xlsx</t>
   </si>
   <si>
     <t>FolderConfigFilePath</t>
   </si>
   <si>
-    <t>EN\Folders.xlsx</t>
-  </si>
-  <si>
-    <t>JA\フォルダー.xlsx</t>
+    <t>Folders.xlsx</t>
+  </si>
+  <si>
+    <t>フォルダー.xlsx</t>
   </si>
   <si>
     <t>QueueConfigFilePath</t>
   </si>
   <si>
-    <t>EN\Queues.xlsx</t>
-  </si>
-  <si>
-    <t>JA\キュー.xlsx</t>
+    <t>Queues.xlsx</t>
+  </si>
+  <si>
+    <t>キュー.xlsx</t>
   </si>
   <si>
     <t>GetOperationName</t>
@@ -992,6 +1026,33 @@
     <t>認証に失敗したため、アクセス トークンを取得できません。サーバーレスポンス：{0}</t>
   </si>
   <si>
+    <t>AuthenticationFailed</t>
+  </si>
+  <si>
+    <t>Authentication failed. Please check logs for more details.</t>
+  </si>
+  <si>
+    <t>認証に失敗しました。詳細はログを確認してください。</t>
+  </si>
+  <si>
+    <t>ErrorDuringExecutionLog</t>
+  </si>
+  <si>
+    <t>There was an execution error: {0} at {1}.</t>
+  </si>
+  <si>
+    <t>実行中にエラーが発生しました：{1}で{0}。</t>
+  </si>
+  <si>
+    <t>ErrorDuringExecution</t>
+  </si>
+  <si>
+    <t>There was an execution error. Please check logs for more details.</t>
+  </si>
+  <si>
+    <t>実行中にエラーが発生しました。詳細はログを確認してください。</t>
+  </si>
+  <si>
     <t>TokenExpired</t>
   </si>
   <si>
@@ -1040,6 +1101,9 @@
     <t>ConfirmNumerousRequests</t>
   </si>
   <si>
+    <t>The selected operation will make a large number of HTTP requests that might impact on Orchestrator's infrastructure. Continue the processing?</t>
+  </si>
+  <si>
     <t>選択した操作により、多数の HTTP リクエストが送信されます。これにより、対象となる Orchestrator のインフラストラクチャに負荷を与える可能性があります。処理を続行しますか?</t>
   </si>
   <si>
@@ -1124,6 +1188,51 @@
     <t>指定されたタイプ（種類）はサポートされていません。</t>
   </si>
   <si>
+    <t>CredentialNotFound</t>
+  </si>
+  <si>
+    <t>The specified credential was not found.</t>
+  </si>
+  <si>
+    <t>指定された資格情報が見つかりませんでした。</t>
+  </si>
+  <si>
+    <t>OperationCanceledByUser</t>
+  </si>
+  <si>
+    <t>Operation canceled by user.</t>
+  </si>
+  <si>
+    <t>ユーザーが操作をキャンセルしました。</t>
+  </si>
+  <si>
+    <t>OUFolderNameNotSpecified</t>
+  </si>
+  <si>
+    <t>Folder (Organization Unit) name not specified.</t>
+  </si>
+  <si>
+    <t>フォルダー名（組織単位名）が指定されませんでした。</t>
+  </si>
+  <si>
+    <t>OUFolderNotFound</t>
+  </si>
+  <si>
+    <t>No Folder (Organization Unit) found.</t>
+  </si>
+  <si>
+    <t>フォルダー（組織単位）が見つかりませんでした。</t>
+  </si>
+  <si>
+    <t>OUFolderIDInvalidOrNotSpecified</t>
+  </si>
+  <si>
+    <t>Folder (Organization Unit) ID invalid or not specified.</t>
+  </si>
+  <si>
+    <t>フォルダー（組織単位）IDが無効か指定されませんでした。</t>
+  </si>
+  <si>
     <t>UnsupportedAssetType</t>
   </si>
   <si>
@@ -1361,6 +1470,9 @@
     <t>GetSingleMachineFailure</t>
   </si>
   <si>
+    <t>Failed to get machine with ID: {0}. Request status: {1} / Response: {2}.</t>
+  </si>
+  <si>
     <t>ID{0}マシン取得が失敗しました。リクエストステータス：{1} / レスポンス：{2}。</t>
   </si>
   <si>
@@ -1688,106 +1800,10 @@
     <t>キューアイテム一覧のファイルが見つかりませんでした。</t>
   </si>
   <si>
-    <t>Workbooks</t>
-  </si>
-  <si>
     <t>Default</t>
   </si>
   <si>
-    <t>https://myOrchestratorURL</t>
-  </si>
-  <si>
     <t>MyAccount</t>
-  </si>
-  <si>
-    <t>CredentialNotFound</t>
-  </si>
-  <si>
-    <t>The specified credential was not found.</t>
-  </si>
-  <si>
-    <t>指定された資格情報が見つかりませんでした。</t>
-  </si>
-  <si>
-    <t>The selected operation will make a large number of HTTP requests that might impact on Orchestrator's infrastructure. Continue the processing?</t>
-  </si>
-  <si>
-    <t>ユーザーが操作をキャンセルしました。</t>
-  </si>
-  <si>
-    <t>OperationCanceledByUser</t>
-  </si>
-  <si>
-    <t>Operation canceled by user.</t>
-  </si>
-  <si>
-    <t>AuthenticationFailed</t>
-  </si>
-  <si>
-    <t>Authentication failed. Please check logs for more details.</t>
-  </si>
-  <si>
-    <t>認証に失敗しました。詳細はログを確認してください。</t>
-  </si>
-  <si>
-    <t>ErrorDuringExecution</t>
-  </si>
-  <si>
-    <t>There was an execution error. Please check logs for more details.</t>
-  </si>
-  <si>
-    <t>実行中にエラーが発生しました。詳細はログを確認してください。</t>
-  </si>
-  <si>
-    <t>Failed to get machine with ID: {0}. Request status: {1} / Response: {2}.</t>
-  </si>
-  <si>
-    <t>There was an execution error: {0} at {1}.</t>
-  </si>
-  <si>
-    <t>実行中にエラーが発生しました：{1}で{0}。</t>
-  </si>
-  <si>
-    <t>ErrorDuringExecutionLog</t>
-  </si>
-  <si>
-    <t>OUFolderNameNotSpecified</t>
-  </si>
-  <si>
-    <t>Folder (Organization Unit) name not specified.</t>
-  </si>
-  <si>
-    <t>フォルダー名（組織単位名）が指定されませんでした。</t>
-  </si>
-  <si>
-    <t>OUFolderNotFound</t>
-  </si>
-  <si>
-    <t>No Folder (Organization Unit) found.</t>
-  </si>
-  <si>
-    <t>フォルダー（組織単位）が見つかりませんでした。</t>
-  </si>
-  <si>
-    <t>OUFolderIDInvalidOrNotSpecified</t>
-  </si>
-  <si>
-    <t>Folder (Organization Unit) ID invalid or not specified.</t>
-  </si>
-  <si>
-    <t>フォルダー（組織単位）IDが無効か指定されませんでした。</t>
-  </si>
-  <si>
-    <t>OUFoldersPanelTemplatePath</t>
-  </si>
-  <si>
-    <t>OUFoldersPanelPath</t>
-  </si>
-  <si>
-    <t>Core\Forms\OUFoldersPanelTemplate.html</t>
-  </si>
-  <si>
-    <t>Core\Forms\OUFoldersPanel.html</t>
   </si>
 </sst>
 </file>
@@ -1868,8 +1884,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table1" displayName="Table1" ref="A1:C58" totalsRowShown="0">
-  <autoFilter ref="A1:C58" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table1" displayName="Table1" ref="A1:C60" totalsRowShown="0">
+  <autoFilter ref="A1:C60" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Name"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Value"/>
@@ -2156,7 +2172,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D89C9C48-5454-47C4-AB1D-448E4519251A}">
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -2182,9 +2198,6 @@
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>547</v>
-      </c>
       <c r="C2" s="2" t="s">
         <v>4</v>
       </c>
@@ -2194,7 +2207,7 @@
         <v>5</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>548</v>
+        <v>583</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>6</v>
@@ -2205,18 +2218,18 @@
         <v>7</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>549</v>
+        <v>8</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="101.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="159.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" s="1" t="s">
         <v>10</v>
+      </c>
+      <c r="B6" s="1">
+        <v>202004</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>11</v>
@@ -2227,7 +2240,7 @@
         <v>12</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>550</v>
+        <v>584</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>13</v>
@@ -2244,7 +2257,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C58"/>
+  <dimension ref="A1:C60"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -2253,7 +2266,7 @@
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="48.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="57.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="43.1796875" style="1" customWidth="1"/>
     <col min="3" max="3" width="63.90625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2380,519 +2393,541 @@
     </row>
     <row r="12" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
-        <v>577</v>
+        <v>38</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>579</v>
+        <v>39</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
-        <v>578</v>
+        <v>41</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>580</v>
+        <v>42</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>56</v>
+        <v>66</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>53</v>
+        <v>69</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>66</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>53</v>
+        <v>63</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>64</v>
+        <v>74</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>66</v>
+        <v>76</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>70</v>
+        <v>77</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
-        <v>71</v>
+        <v>78</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>53</v>
+        <v>63</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>66</v>
+        <v>76</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>53</v>
+        <v>63</v>
       </c>
       <c r="C28" s="2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B29" s="1" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A29" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>78</v>
-      </c>
       <c r="C29" s="2" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="1" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>81</v>
+        <v>63</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A31" s="1" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>56</v>
+        <v>88</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="1" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" s="1" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>53</v>
+        <v>66</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A34" s="1" t="s">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>78</v>
+        <v>96</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>91</v>
+        <v>97</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A35" s="1" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>81</v>
+        <v>63</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>93</v>
+        <v>99</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A36" s="1" t="s">
-        <v>94</v>
+        <v>100</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>78</v>
+        <v>88</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A37" s="1" t="s">
-        <v>96</v>
+        <v>102</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>56</v>
+        <v>91</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A38" s="1" t="s">
-        <v>98</v>
+        <v>104</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>59</v>
+        <v>88</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A39" s="1" t="s">
-        <v>100</v>
+        <v>106</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>53</v>
+        <v>66</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>101</v>
+        <v>107</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A40" s="1" t="s">
-        <v>102</v>
+        <v>108</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>53</v>
+        <v>69</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>103</v>
+        <v>109</v>
       </c>
     </row>
     <row r="41" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A41" s="1" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>105</v>
+        <v>111</v>
       </c>
     </row>
     <row r="42" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A42" s="1" t="s">
-        <v>106</v>
+        <v>112</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A43" s="1" t="s">
-        <v>108</v>
+        <v>114</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>53</v>
+        <v>69</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>109</v>
+        <v>115</v>
       </c>
     </row>
     <row r="44" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A44" s="1" t="s">
-        <v>110</v>
+        <v>116</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A45" s="1" t="s">
-        <v>112</v>
+        <v>118</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>53</v>
+        <v>63</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>113</v>
+        <v>119</v>
       </c>
     </row>
     <row r="46" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A46" s="1" t="s">
-        <v>114</v>
+        <v>120</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>56</v>
+        <v>76</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>115</v>
+        <v>121</v>
       </c>
     </row>
     <row r="47" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A47" s="1" t="s">
-        <v>116</v>
+        <v>122</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>56</v>
+        <v>63</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A48" s="1" t="s">
-        <v>118</v>
+        <v>124</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>119</v>
+        <v>66</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
     </row>
     <row r="49" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A49" s="1" t="s">
-        <v>121</v>
+        <v>126</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>56</v>
+        <v>66</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A50" s="1" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>56</v>
+        <v>129</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.35">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A51" s="1" t="s">
-        <v>125</v>
+        <v>131</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>53</v>
+        <v>66</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>126</v>
+        <v>132</v>
       </c>
     </row>
     <row r="52" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A52" s="1" t="s">
-        <v>127</v>
+        <v>133</v>
       </c>
       <c r="B52" s="1" t="s">
         <v>66</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A53" s="1" t="s">
-        <v>129</v>
+        <v>135</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>56</v>
+        <v>63</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.35">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A54" s="1" t="s">
-        <v>131</v>
+        <v>137</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>132</v>
+        <v>138</v>
       </c>
     </row>
     <row r="55" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A55" s="1" t="s">
-        <v>133</v>
+        <v>139</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A56" s="1" t="s">
-        <v>135</v>
+        <v>141</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>53</v>
+        <v>96</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>136</v>
+        <v>142</v>
       </c>
     </row>
     <row r="57" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A57" s="1" t="s">
-        <v>137</v>
+        <v>143</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>59</v>
+        <v>88</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>138</v>
+        <v>144</v>
       </c>
     </row>
     <row r="58" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A58" s="1" t="s">
-        <v>139</v>
+        <v>145</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>53</v>
+        <v>63</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>140</v>
+        <v>146</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A59" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C59" s="2" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A60" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C60" s="2" t="s">
+        <v>150</v>
       </c>
     </row>
   </sheetData>
@@ -2912,14 +2947,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1927ABA9-1814-4487-9CEC-ABDCAF91481F}">
   <dimension ref="A1:C159"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView topLeftCell="A148" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2 A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="50.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="79" style="1" customWidth="1"/>
+    <col min="2" max="2" width="61.90625" style="1" customWidth="1"/>
     <col min="3" max="3" width="114.26953125" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2928,340 +2963,340 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>141</v>
+        <v>151</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>142</v>
+        <v>152</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>143</v>
+        <v>153</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>144</v>
+        <v>154</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>144</v>
+        <v>154</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="43.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>145</v>
+        <v>155</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>146</v>
+        <v>156</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>147</v>
+        <v>157</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>148</v>
+        <v>158</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>149</v>
+        <v>159</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>150</v>
+        <v>160</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>151</v>
+        <v>161</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>152</v>
+        <v>162</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>152</v>
+        <v>162</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
-        <v>153</v>
+        <v>163</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>154</v>
+        <v>164</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>155</v>
+        <v>165</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
-        <v>156</v>
+        <v>166</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>157</v>
+        <v>167</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>158</v>
+        <v>168</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
-        <v>159</v>
+        <v>169</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>160</v>
+        <v>170</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>161</v>
+        <v>171</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
-        <v>162</v>
+        <v>172</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>163</v>
+        <v>173</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>164</v>
+        <v>174</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
-        <v>165</v>
+        <v>175</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>166</v>
+        <v>176</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>167</v>
+        <v>177</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
-        <v>168</v>
+        <v>178</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>169</v>
+        <v>179</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>170</v>
+        <v>180</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
-        <v>171</v>
+        <v>181</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>172</v>
+        <v>182</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>173</v>
+        <v>183</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
-        <v>174</v>
+        <v>184</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>175</v>
+        <v>185</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>176</v>
+        <v>186</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
-        <v>177</v>
+        <v>187</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>178</v>
+        <v>188</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>179</v>
+        <v>189</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
-        <v>180</v>
+        <v>190</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>181</v>
+        <v>191</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>182</v>
+        <v>192</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
-        <v>183</v>
+        <v>193</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>184</v>
+        <v>194</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>185</v>
+        <v>195</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
-        <v>186</v>
+        <v>196</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>187</v>
+        <v>197</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>188</v>
+        <v>198</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
-        <v>189</v>
+        <v>199</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>190</v>
+        <v>200</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>191</v>
+        <v>201</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
-        <v>192</v>
+        <v>202</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>193</v>
+        <v>203</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>194</v>
+        <v>204</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
-        <v>195</v>
+        <v>205</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>196</v>
+        <v>206</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>197</v>
+        <v>207</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
-        <v>198</v>
+        <v>208</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>199</v>
+        <v>209</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>200</v>
+        <v>210</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
-        <v>201</v>
+        <v>211</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>202</v>
+        <v>212</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>203</v>
+        <v>213</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
-        <v>204</v>
+        <v>214</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>206</v>
+        <v>216</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
-        <v>207</v>
+        <v>217</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>208</v>
+        <v>218</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>209</v>
+        <v>219</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
-        <v>210</v>
+        <v>220</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>211</v>
+        <v>221</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>212</v>
+        <v>222</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
-        <v>213</v>
+        <v>223</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>214</v>
+        <v>224</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>215</v>
+        <v>225</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
-        <v>216</v>
+        <v>226</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>217</v>
+        <v>227</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>188</v>
+        <v>198</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="s">
-        <v>218</v>
+        <v>228</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>219</v>
+        <v>229</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>191</v>
+        <v>201</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="s">
-        <v>220</v>
+        <v>230</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>221</v>
+        <v>231</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>222</v>
+        <v>232</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A30" s="1" t="s">
-        <v>223</v>
+        <v>233</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>224</v>
+        <v>234</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>224</v>
+        <v>234</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A31" s="1" t="s">
-        <v>225</v>
+        <v>235</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>226</v>
+        <v>236</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>227</v>
+        <v>237</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.35">
@@ -3270,101 +3305,101 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A33" s="1" t="s">
-        <v>228</v>
+        <v>238</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>229</v>
+        <v>239</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>230</v>
+        <v>240</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A34" s="1" t="s">
-        <v>231</v>
+        <v>241</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>232</v>
+        <v>242</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>233</v>
+        <v>243</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A35" s="1" t="s">
-        <v>234</v>
+        <v>244</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>235</v>
+        <v>245</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>236</v>
+        <v>246</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A36" s="1" t="s">
-        <v>237</v>
+        <v>247</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>238</v>
+        <v>248</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>239</v>
+        <v>249</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A37" s="1" t="s">
-        <v>240</v>
+        <v>250</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>241</v>
+        <v>251</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>242</v>
+        <v>252</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A38" s="1" t="s">
-        <v>243</v>
+        <v>253</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>244</v>
+        <v>254</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>245</v>
+        <v>255</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A39" s="1" t="s">
-        <v>246</v>
+        <v>256</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>247</v>
+        <v>257</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>248</v>
+        <v>258</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A40" s="1" t="s">
-        <v>249</v>
+        <v>259</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>250</v>
+        <v>260</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>251</v>
+        <v>261</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A41" s="1" t="s">
-        <v>252</v>
+        <v>262</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>253</v>
+        <v>263</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>254</v>
+        <v>264</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.35">
@@ -3373,475 +3408,475 @@
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A43" s="1" t="s">
-        <v>255</v>
+        <v>265</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>256</v>
+        <v>266</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>257</v>
+        <v>267</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A44" s="1" t="s">
-        <v>258</v>
+        <v>268</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>259</v>
+        <v>269</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>260</v>
+        <v>270</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A45" s="1" t="s">
-        <v>261</v>
+        <v>271</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>262</v>
+        <v>272</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>263</v>
+        <v>273</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A46" s="1" t="s">
-        <v>264</v>
+        <v>274</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>265</v>
+        <v>275</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>266</v>
+        <v>276</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A47" s="1" t="s">
-        <v>267</v>
+        <v>277</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>268</v>
+        <v>278</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>269</v>
+        <v>279</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A48" s="1" t="s">
-        <v>270</v>
+        <v>280</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>271</v>
+        <v>281</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>272</v>
+        <v>282</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A49" s="1" t="s">
-        <v>273</v>
+        <v>283</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>274</v>
+        <v>284</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>275</v>
+        <v>285</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A50" s="1" t="s">
-        <v>276</v>
+        <v>286</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>277</v>
+        <v>287</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>278</v>
+        <v>288</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A51" s="1" t="s">
-        <v>279</v>
+        <v>289</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>280</v>
+        <v>290</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>281</v>
+        <v>291</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A52" s="1" t="s">
-        <v>282</v>
+        <v>292</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>283</v>
+        <v>293</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>284</v>
+        <v>294</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A53" s="1" t="s">
-        <v>285</v>
+        <v>295</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>286</v>
+        <v>296</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>287</v>
+        <v>297</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A54" s="1" t="s">
-        <v>288</v>
+        <v>298</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>289</v>
+        <v>299</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>290</v>
+        <v>300</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A55" s="1" t="s">
-        <v>291</v>
+        <v>301</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>292</v>
+        <v>302</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>293</v>
+        <v>303</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A56" s="1" t="s">
-        <v>294</v>
+        <v>304</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>295</v>
+        <v>305</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>296</v>
+        <v>306</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A57" s="1" t="s">
-        <v>297</v>
+        <v>307</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>298</v>
+        <v>308</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>299</v>
+        <v>309</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A58" s="1" t="s">
-        <v>300</v>
+        <v>310</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>301</v>
+        <v>311</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>302</v>
+        <v>312</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A59" s="1" t="s">
-        <v>303</v>
+        <v>313</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>304</v>
+        <v>314</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>305</v>
+        <v>315</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A60" s="1" t="s">
-        <v>306</v>
+        <v>316</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>307</v>
+        <v>317</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>308</v>
+        <v>318</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A61" s="1" t="s">
-        <v>309</v>
+        <v>319</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>310</v>
+        <v>320</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>311</v>
+        <v>321</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A62" s="1" t="s">
-        <v>312</v>
+        <v>322</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>313</v>
+        <v>323</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>314</v>
+        <v>324</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A63" s="1" t="s">
-        <v>558</v>
+        <v>325</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>559</v>
+        <v>326</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>560</v>
+        <v>327</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A64" s="1" t="s">
-        <v>567</v>
+        <v>328</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>565</v>
+        <v>329</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>566</v>
+        <v>330</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A65" s="1" t="s">
-        <v>561</v>
+        <v>331</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>562</v>
+        <v>332</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>563</v>
+        <v>333</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A66" s="1" t="s">
-        <v>315</v>
+        <v>334</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>316</v>
+        <v>335</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>317</v>
+        <v>336</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A67" s="1" t="s">
-        <v>318</v>
+        <v>337</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>319</v>
+        <v>338</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>320</v>
+        <v>339</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A68" s="1" t="s">
-        <v>321</v>
+        <v>340</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>322</v>
+        <v>341</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>323</v>
+        <v>342</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A69" s="1" t="s">
-        <v>324</v>
+        <v>343</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>325</v>
+        <v>344</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>326</v>
+        <v>345</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A70" s="1" t="s">
-        <v>327</v>
+        <v>346</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>328</v>
+        <v>347</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>329</v>
+        <v>348</v>
       </c>
     </row>
     <row r="71" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A71" s="1" t="s">
-        <v>330</v>
+        <v>349</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>554</v>
+        <v>350</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>331</v>
+        <v>351</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A72" s="1" t="s">
-        <v>332</v>
+        <v>352</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>333</v>
+        <v>353</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>334</v>
+        <v>354</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A73" s="1" t="s">
-        <v>335</v>
+        <v>355</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>336</v>
+        <v>356</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>337</v>
+        <v>357</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A74" s="1" t="s">
-        <v>338</v>
+        <v>358</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>339</v>
+        <v>359</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>340</v>
+        <v>360</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A75" s="1" t="s">
-        <v>341</v>
+        <v>361</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>342</v>
+        <v>362</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>343</v>
+        <v>363</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A76" s="1" t="s">
-        <v>344</v>
+        <v>364</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>345</v>
+        <v>365</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>346</v>
+        <v>366</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A77" s="1" t="s">
-        <v>347</v>
+        <v>367</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>348</v>
+        <v>368</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>349</v>
+        <v>369</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A78" s="1" t="s">
-        <v>350</v>
+        <v>370</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>351</v>
+        <v>371</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>352</v>
+        <v>372</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A79" s="1" t="s">
-        <v>353</v>
+        <v>373</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>354</v>
+        <v>374</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>355</v>
+        <v>375</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A80" s="1" t="s">
-        <v>356</v>
+        <v>376</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>357</v>
+        <v>377</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>358</v>
+        <v>378</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A81" s="1" t="s">
-        <v>551</v>
+        <v>379</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>552</v>
+        <v>380</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>553</v>
+        <v>381</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A82" s="1" t="s">
-        <v>556</v>
+        <v>382</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>557</v>
+        <v>383</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>555</v>
+        <v>384</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A83" s="1" t="s">
-        <v>568</v>
+        <v>385</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>569</v>
+        <v>386</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>570</v>
+        <v>387</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A84" s="1" t="s">
-        <v>571</v>
+        <v>388</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>572</v>
+        <v>389</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>573</v>
+        <v>390</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A85" s="1" t="s">
-        <v>574</v>
+        <v>391</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>575</v>
+        <v>392</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>576</v>
+        <v>393</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.35">
@@ -3850,90 +3885,90 @@
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A87" s="1" t="s">
-        <v>359</v>
+        <v>394</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>360</v>
+        <v>395</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>361</v>
+        <v>396</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A88" s="1" t="s">
-        <v>362</v>
+        <v>397</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>363</v>
+        <v>398</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>364</v>
+        <v>399</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A89" s="1" t="s">
-        <v>365</v>
+        <v>400</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>366</v>
+        <v>401</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>367</v>
+        <v>402</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A90" s="1" t="s">
-        <v>368</v>
+        <v>403</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>369</v>
+        <v>404</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>370</v>
+        <v>405</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A91" s="1" t="s">
-        <v>371</v>
+        <v>406</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>372</v>
+        <v>407</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>373</v>
+        <v>408</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A92" s="1" t="s">
-        <v>374</v>
+        <v>409</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>375</v>
+        <v>410</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>376</v>
+        <v>411</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A93" s="1" t="s">
-        <v>377</v>
+        <v>412</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>378</v>
+        <v>413</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>379</v>
+        <v>414</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A94" s="1" t="s">
-        <v>380</v>
+        <v>415</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>381</v>
+        <v>416</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>382</v>
+        <v>417</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.35">
@@ -3942,101 +3977,101 @@
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A96" s="1" t="s">
-        <v>383</v>
+        <v>418</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>384</v>
+        <v>419</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>385</v>
+        <v>420</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A97" s="1" t="s">
-        <v>386</v>
+        <v>421</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>387</v>
+        <v>422</v>
       </c>
       <c r="C97" s="2" t="s">
-        <v>388</v>
+        <v>423</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A98" s="1" t="s">
-        <v>389</v>
+        <v>424</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>390</v>
+        <v>425</v>
       </c>
       <c r="C98" s="2" t="s">
-        <v>391</v>
+        <v>426</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A99" s="1" t="s">
-        <v>392</v>
+        <v>427</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>393</v>
+        <v>428</v>
       </c>
       <c r="C99" s="2" t="s">
-        <v>394</v>
+        <v>429</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A100" s="1" t="s">
-        <v>395</v>
+        <v>430</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>396</v>
+        <v>431</v>
       </c>
       <c r="C100" s="2" t="s">
-        <v>397</v>
+        <v>432</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A101" s="1" t="s">
-        <v>398</v>
+        <v>433</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>399</v>
+        <v>434</v>
       </c>
       <c r="C101" s="2" t="s">
-        <v>400</v>
+        <v>435</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A102" s="1" t="s">
-        <v>401</v>
+        <v>436</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>402</v>
+        <v>437</v>
       </c>
       <c r="C102" s="2" t="s">
-        <v>403</v>
+        <v>438</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A103" s="1" t="s">
-        <v>404</v>
+        <v>439</v>
       </c>
       <c r="B103" s="2" t="s">
-        <v>405</v>
+        <v>440</v>
       </c>
       <c r="C103" s="2" t="s">
-        <v>406</v>
+        <v>441</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A104" s="1" t="s">
-        <v>407</v>
+        <v>442</v>
       </c>
       <c r="B104" s="2" t="s">
-        <v>408</v>
+        <v>443</v>
       </c>
       <c r="C104" s="2" t="s">
-        <v>409</v>
+        <v>444</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.35">
@@ -4045,90 +4080,90 @@
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A106" s="1" t="s">
-        <v>410</v>
+        <v>445</v>
       </c>
       <c r="B106" s="2" t="s">
-        <v>411</v>
+        <v>446</v>
       </c>
       <c r="C106" s="2" t="s">
-        <v>412</v>
+        <v>447</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A107" s="1" t="s">
-        <v>413</v>
+        <v>448</v>
       </c>
       <c r="B107" s="2" t="s">
-        <v>414</v>
+        <v>449</v>
       </c>
       <c r="C107" s="2" t="s">
-        <v>415</v>
+        <v>450</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A108" s="1" t="s">
-        <v>416</v>
+        <v>451</v>
       </c>
       <c r="B108" s="2" t="s">
-        <v>417</v>
+        <v>452</v>
       </c>
       <c r="C108" s="2" t="s">
-        <v>418</v>
+        <v>453</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A109" s="1" t="s">
-        <v>419</v>
+        <v>454</v>
       </c>
       <c r="B109" s="2" t="s">
-        <v>420</v>
+        <v>455</v>
       </c>
       <c r="C109" s="2" t="s">
-        <v>421</v>
+        <v>456</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A110" s="1" t="s">
-        <v>422</v>
+        <v>457</v>
       </c>
       <c r="B110" s="2" t="s">
-        <v>423</v>
+        <v>458</v>
       </c>
       <c r="C110" s="2" t="s">
-        <v>424</v>
+        <v>459</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A111" s="1" t="s">
-        <v>425</v>
+        <v>460</v>
       </c>
       <c r="B111" s="2" t="s">
-        <v>426</v>
+        <v>461</v>
       </c>
       <c r="C111" s="2" t="s">
-        <v>427</v>
+        <v>462</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A112" s="1" t="s">
-        <v>428</v>
+        <v>463</v>
       </c>
       <c r="B112" s="2" t="s">
-        <v>429</v>
+        <v>464</v>
       </c>
       <c r="C112" s="2" t="s">
-        <v>430</v>
+        <v>465</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A113" s="1" t="s">
-        <v>431</v>
+        <v>466</v>
       </c>
       <c r="B113" s="2" t="s">
-        <v>432</v>
+        <v>467</v>
       </c>
       <c r="C113" s="2" t="s">
-        <v>433</v>
+        <v>468</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.35">
@@ -4137,266 +4172,266 @@
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A115" s="1" t="s">
-        <v>434</v>
+        <v>469</v>
       </c>
       <c r="B115" s="2" t="s">
-        <v>435</v>
+        <v>470</v>
       </c>
       <c r="C115" s="2" t="s">
-        <v>436</v>
+        <v>471</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A116" s="1" t="s">
-        <v>437</v>
+        <v>472</v>
       </c>
       <c r="B116" s="2" t="s">
-        <v>564</v>
+        <v>473</v>
       </c>
       <c r="C116" s="2" t="s">
-        <v>438</v>
+        <v>474</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A117" s="1" t="s">
-        <v>439</v>
+        <v>475</v>
       </c>
       <c r="B117" s="2" t="s">
-        <v>440</v>
+        <v>476</v>
       </c>
       <c r="C117" s="2" t="s">
-        <v>441</v>
+        <v>477</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A118" s="1" t="s">
-        <v>442</v>
+        <v>478</v>
       </c>
       <c r="B118" s="2" t="s">
-        <v>443</v>
+        <v>479</v>
       </c>
       <c r="C118" s="2" t="s">
-        <v>444</v>
+        <v>480</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A120" s="1" t="s">
-        <v>445</v>
+        <v>481</v>
       </c>
       <c r="B120" s="2" t="s">
-        <v>446</v>
+        <v>482</v>
       </c>
       <c r="C120" s="2" t="s">
-        <v>447</v>
+        <v>483</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A121" s="1" t="s">
-        <v>448</v>
+        <v>484</v>
       </c>
       <c r="B121" s="2" t="s">
-        <v>449</v>
+        <v>485</v>
       </c>
       <c r="C121" s="2" t="s">
-        <v>450</v>
+        <v>486</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A122" s="1" t="s">
-        <v>451</v>
+        <v>487</v>
       </c>
       <c r="B122" s="2" t="s">
-        <v>452</v>
+        <v>488</v>
       </c>
       <c r="C122" s="2" t="s">
-        <v>453</v>
+        <v>489</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A123" s="1" t="s">
-        <v>454</v>
+        <v>490</v>
       </c>
       <c r="B123" s="2" t="s">
-        <v>455</v>
+        <v>491</v>
       </c>
       <c r="C123" s="2" t="s">
-        <v>456</v>
+        <v>492</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A124" s="1" t="s">
-        <v>457</v>
+        <v>493</v>
       </c>
       <c r="B124" s="2" t="s">
-        <v>458</v>
+        <v>494</v>
       </c>
       <c r="C124" s="2" t="s">
-        <v>459</v>
+        <v>495</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A125" s="1" t="s">
-        <v>460</v>
+        <v>496</v>
       </c>
       <c r="B125" s="2" t="s">
-        <v>461</v>
+        <v>497</v>
       </c>
       <c r="C125" s="2" t="s">
-        <v>462</v>
+        <v>498</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A126" s="1" t="s">
-        <v>463</v>
+        <v>499</v>
       </c>
       <c r="B126" s="2" t="s">
-        <v>464</v>
+        <v>500</v>
       </c>
       <c r="C126" s="2" t="s">
-        <v>465</v>
+        <v>501</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A128" s="1" t="s">
-        <v>466</v>
+        <v>502</v>
       </c>
       <c r="B128" s="2" t="s">
-        <v>467</v>
+        <v>503</v>
       </c>
       <c r="C128" s="2" t="s">
-        <v>468</v>
+        <v>504</v>
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A129" s="1" t="s">
-        <v>469</v>
+        <v>505</v>
       </c>
       <c r="B129" s="2" t="s">
-        <v>470</v>
+        <v>506</v>
       </c>
       <c r="C129" s="2" t="s">
-        <v>471</v>
+        <v>507</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A130" s="1" t="s">
-        <v>472</v>
+        <v>508</v>
       </c>
       <c r="B130" s="2" t="s">
-        <v>473</v>
+        <v>509</v>
       </c>
       <c r="C130" s="2" t="s">
-        <v>474</v>
+        <v>510</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A131" s="1" t="s">
-        <v>475</v>
+        <v>511</v>
       </c>
       <c r="B131" s="2" t="s">
-        <v>476</v>
+        <v>512</v>
       </c>
       <c r="C131" s="2" t="s">
-        <v>477</v>
+        <v>513</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A132" s="1" t="s">
-        <v>478</v>
+        <v>514</v>
       </c>
       <c r="B132" s="2" t="s">
-        <v>479</v>
+        <v>515</v>
       </c>
       <c r="C132" s="2" t="s">
-        <v>480</v>
+        <v>516</v>
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A134" s="1" t="s">
-        <v>481</v>
+        <v>517</v>
       </c>
       <c r="B134" s="2" t="s">
-        <v>482</v>
+        <v>518</v>
       </c>
       <c r="C134" s="2" t="s">
-        <v>483</v>
+        <v>519</v>
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A135" s="1" t="s">
-        <v>484</v>
+        <v>520</v>
       </c>
       <c r="B135" s="1" t="s">
-        <v>485</v>
+        <v>521</v>
       </c>
       <c r="C135" s="1" t="s">
-        <v>486</v>
+        <v>522</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A136" s="1" t="s">
-        <v>487</v>
+        <v>523</v>
       </c>
       <c r="B136" s="1" t="s">
-        <v>488</v>
+        <v>524</v>
       </c>
       <c r="C136" s="1" t="s">
-        <v>489</v>
+        <v>525</v>
       </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A137" s="1" t="s">
-        <v>490</v>
+        <v>526</v>
       </c>
       <c r="B137" s="2" t="s">
-        <v>491</v>
+        <v>527</v>
       </c>
       <c r="C137" s="1" t="s">
-        <v>492</v>
+        <v>528</v>
       </c>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A138" s="1" t="s">
-        <v>493</v>
+        <v>529</v>
       </c>
       <c r="B138" s="1" t="s">
-        <v>494</v>
+        <v>530</v>
       </c>
       <c r="C138" s="1" t="s">
-        <v>495</v>
+        <v>531</v>
       </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A139" s="1" t="s">
-        <v>496</v>
+        <v>532</v>
       </c>
       <c r="B139" s="2" t="s">
-        <v>497</v>
+        <v>533</v>
       </c>
       <c r="C139" s="2" t="s">
-        <v>498</v>
+        <v>534</v>
       </c>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A141" s="1" t="s">
-        <v>499</v>
+        <v>535</v>
       </c>
       <c r="B141" s="2" t="s">
-        <v>500</v>
+        <v>536</v>
       </c>
       <c r="C141" s="2" t="s">
-        <v>501</v>
+        <v>537</v>
       </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A142" s="1" t="s">
-        <v>502</v>
+        <v>538</v>
       </c>
       <c r="B142" s="2" t="s">
-        <v>503</v>
+        <v>539</v>
       </c>
       <c r="C142" s="2" t="s">
-        <v>504</v>
+        <v>540</v>
       </c>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.35">
@@ -4405,57 +4440,57 @@
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A144" s="1" t="s">
-        <v>505</v>
+        <v>541</v>
       </c>
       <c r="B144" s="2" t="s">
-        <v>506</v>
+        <v>542</v>
       </c>
       <c r="C144" s="2" t="s">
-        <v>507</v>
+        <v>543</v>
       </c>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A145" s="1" t="s">
-        <v>508</v>
+        <v>544</v>
       </c>
       <c r="B145" s="2" t="s">
-        <v>509</v>
+        <v>545</v>
       </c>
       <c r="C145" s="2" t="s">
-        <v>510</v>
+        <v>546</v>
       </c>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A146" s="1" t="s">
-        <v>511</v>
+        <v>547</v>
       </c>
       <c r="B146" s="2" t="s">
-        <v>512</v>
+        <v>548</v>
       </c>
       <c r="C146" s="2" t="s">
-        <v>513</v>
+        <v>549</v>
       </c>
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A147" s="1" t="s">
-        <v>514</v>
+        <v>550</v>
       </c>
       <c r="B147" s="2" t="s">
-        <v>515</v>
+        <v>551</v>
       </c>
       <c r="C147" s="2" t="s">
-        <v>516</v>
+        <v>552</v>
       </c>
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A148" s="1" t="s">
-        <v>517</v>
+        <v>553</v>
       </c>
       <c r="B148" s="2" t="s">
-        <v>518</v>
+        <v>554</v>
       </c>
       <c r="C148" s="2" t="s">
-        <v>519</v>
+        <v>555</v>
       </c>
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.35">
@@ -4464,101 +4499,101 @@
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A150" s="1" t="s">
-        <v>520</v>
+        <v>556</v>
       </c>
       <c r="B150" s="2" t="s">
-        <v>521</v>
+        <v>557</v>
       </c>
       <c r="C150" s="2" t="s">
-        <v>522</v>
+        <v>558</v>
       </c>
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A151" s="1" t="s">
-        <v>523</v>
+        <v>559</v>
       </c>
       <c r="B151" s="2" t="s">
-        <v>524</v>
+        <v>560</v>
       </c>
       <c r="C151" s="2" t="s">
-        <v>525</v>
+        <v>561</v>
       </c>
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A153" s="1" t="s">
-        <v>526</v>
+        <v>562</v>
       </c>
       <c r="B153" s="1" t="s">
-        <v>527</v>
+        <v>563</v>
       </c>
       <c r="C153" s="1" t="s">
-        <v>528</v>
+        <v>564</v>
       </c>
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A154" s="1" t="s">
-        <v>529</v>
+        <v>565</v>
       </c>
       <c r="B154" s="1" t="s">
-        <v>530</v>
+        <v>566</v>
       </c>
       <c r="C154" s="1" t="s">
-        <v>531</v>
+        <v>567</v>
       </c>
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A155" s="1" t="s">
-        <v>532</v>
+        <v>568</v>
       </c>
       <c r="B155" s="1" t="s">
-        <v>533</v>
+        <v>569</v>
       </c>
       <c r="C155" s="1" t="s">
-        <v>534</v>
+        <v>570</v>
       </c>
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A156" s="1" t="s">
-        <v>535</v>
+        <v>571</v>
       </c>
       <c r="B156" s="1" t="s">
-        <v>536</v>
+        <v>572</v>
       </c>
       <c r="C156" s="1" t="s">
-        <v>537</v>
+        <v>573</v>
       </c>
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A157" s="1" t="s">
-        <v>538</v>
+        <v>574</v>
       </c>
       <c r="B157" s="2" t="s">
-        <v>539</v>
+        <v>575</v>
       </c>
       <c r="C157" s="2" t="s">
-        <v>540</v>
+        <v>576</v>
       </c>
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A158" s="1" t="s">
-        <v>541</v>
+        <v>577</v>
       </c>
       <c r="B158" s="1" t="s">
-        <v>542</v>
+        <v>578</v>
       </c>
       <c r="C158" s="1" t="s">
-        <v>543</v>
+        <v>579</v>
       </c>
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A159" s="1" t="s">
-        <v>544</v>
+        <v>580</v>
       </c>
       <c r="B159" s="1" t="s">
-        <v>545</v>
+        <v>581</v>
       </c>
       <c r="C159" s="1" t="s">
-        <v>546</v>
+        <v>582</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Refactor main execution flow
Fix bug that happened when user canceled the authentication form
</commit_message>
<xml_diff>
--- a/Config.xlsx
+++ b/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mateus.cruz\Documents\GitHub\OrchestratorManager\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{824B9220-6F42-42BD-A7AE-CCFB824A1962}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67A15CFC-4DE1-4E14-8C3C-253741915440}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2260,7 +2260,7 @@
   <dimension ref="A1:C60"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A2" sqref="A2 A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2947,7 +2947,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1927ABA9-1814-4487-9CEC-ABDCAF91481F}">
   <dimension ref="A1:C159"/>
   <sheetViews>
-    <sheetView topLeftCell="A148" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2 A2"/>
     </sheetView>
   </sheetViews>
@@ -3615,7 +3615,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A62" s="1" t="s">
         <v>322</v>
       </c>
@@ -4324,7 +4324,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A131" s="1" t="s">
         <v>511</v>
       </c>

</xml_diff>

<commit_message>
Fix crash when invalid base Orchestrator URLs were used
</commit_message>
<xml_diff>
--- a/Config.xlsx
+++ b/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mateus.cruz\Documents\GitHub\OrchestratorManager\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67A15CFC-4DE1-4E14-8C3C-253741915440}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E14931CF-35BC-4B7A-92F8-8CA9A0C05D07}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -56,14 +56,14 @@
     <t>TenantName</t>
   </si>
   <si>
+    <t>Default</t>
+  </si>
+  <si>
     <t>Name of the tenant to be used. 
 Sample value: Default.</t>
   </si>
   <si>
     <t>OnPremisesOrchestratorURL</t>
-  </si>
-  <si>
-    <t>https://myOrchestratorURL</t>
   </si>
   <si>
     <t>URL of the Orchestrator instance to be used. 
@@ -87,6 +87,9 @@
     <t>CloudAccountName</t>
   </si>
   <si>
+    <t>MyAccount</t>
+  </si>
+  <si>
     <t>Unique site URL for Automation Cloud oganization.
 This parameter is exclusive to Automation Cloud Orchestrator instances.
 Sample value: MyAccount (assuming the organization account URL is https://platform.uipath.com/MyAccount).</t>
@@ -1800,10 +1803,7 @@
     <t>キューアイテム一覧のファイルが見つかりませんでした。</t>
   </si>
   <si>
-    <t>Default</t>
-  </si>
-  <si>
-    <t>MyAccount</t>
+    <t>https://myOrchestratorURL</t>
   </si>
 </sst>
 </file>
@@ -2207,18 +2207,18 @@
         <v>5</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>583</v>
+        <v>6</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="58" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>8</v>
+        <v>584</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>9</v>
@@ -2240,10 +2240,10 @@
         <v>12</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>584</v>
+        <v>13</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -2283,651 +2283,651 @@
     </row>
     <row r="2" spans="1:3" ht="101.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B2" s="1">
         <v>200</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B3" s="1">
         <v>0</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B4" s="1">
         <v>550</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B5" s="1">
         <v>650</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B6" s="1">
         <v>3</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B7" s="1">
         <v>5000</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A31" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="1" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" s="1" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A34" s="1" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A35" s="1" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A36" s="1" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="37" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A37" s="1" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A38" s="1" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A39" s="1" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A40" s="1" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row r="41" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A41" s="1" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
     </row>
     <row r="42" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A42" s="1" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="43" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A43" s="1" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="44" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A44" s="1" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A45" s="1" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
     </row>
     <row r="46" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A46" s="1" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
     <row r="47" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A47" s="1" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
     </row>
     <row r="48" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A48" s="1" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
     </row>
     <row r="49" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A49" s="1" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A50" s="1" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
     </row>
     <row r="51" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A51" s="1" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
     </row>
     <row r="52" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A52" s="1" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A53" s="1" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
     </row>
     <row r="54" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A54" s="1" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
     </row>
     <row r="55" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A55" s="1" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A56" s="1" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
     </row>
     <row r="57" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A57" s="1" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
     </row>
     <row r="58" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A58" s="1" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
     </row>
     <row r="59" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A59" s="1" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="60" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A60" s="1" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
     </row>
   </sheetData>
@@ -2963,340 +2963,340 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="43.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A30" s="1" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A31" s="1" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.35">
@@ -3305,101 +3305,101 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A33" s="1" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A34" s="1" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A35" s="1" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A36" s="1" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A37" s="1" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A38" s="1" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A39" s="1" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A40" s="1" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A41" s="1" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.35">
@@ -3408,475 +3408,475 @@
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A43" s="1" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A44" s="1" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A45" s="1" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A46" s="1" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A47" s="1" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A48" s="1" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A49" s="1" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A50" s="1" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A51" s="1" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A52" s="1" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A53" s="1" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A54" s="1" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A55" s="1" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A56" s="1" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A57" s="1" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A58" s="1" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A59" s="1" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A60" s="1" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A61" s="1" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
     </row>
     <row r="62" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A62" s="1" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A63" s="1" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A64" s="1" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A65" s="1" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A66" s="1" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A67" s="1" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A68" s="1" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A69" s="1" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A70" s="1" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
     </row>
     <row r="71" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A71" s="1" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A72" s="1" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A73" s="1" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A74" s="1" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A75" s="1" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A76" s="1" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A77" s="1" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A78" s="1" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A79" s="1" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A80" s="1" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A81" s="1" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A82" s="1" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A83" s="1" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A84" s="1" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A85" s="1" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.35">
@@ -3885,90 +3885,90 @@
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A87" s="1" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A88" s="1" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A89" s="1" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A90" s="1" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A91" s="1" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A92" s="1" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A93" s="1" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A94" s="1" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.35">
@@ -3977,101 +3977,101 @@
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A96" s="1" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A97" s="1" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
       <c r="C97" s="2" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A98" s="1" t="s">
-        <v>424</v>
+        <v>425</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
       <c r="C98" s="2" t="s">
-        <v>426</v>
+        <v>427</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A99" s="1" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="C99" s="2" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A100" s="1" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>431</v>
+        <v>432</v>
       </c>
       <c r="C100" s="2" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A101" s="1" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="C101" s="2" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A102" s="1" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="C102" s="2" t="s">
-        <v>438</v>
+        <v>439</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A103" s="1" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="B103" s="2" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="C103" s="2" t="s">
-        <v>441</v>
+        <v>442</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A104" s="1" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="B104" s="2" t="s">
-        <v>443</v>
+        <v>444</v>
       </c>
       <c r="C104" s="2" t="s">
-        <v>444</v>
+        <v>445</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.35">
@@ -4080,90 +4080,90 @@
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A106" s="1" t="s">
-        <v>445</v>
+        <v>446</v>
       </c>
       <c r="B106" s="2" t="s">
-        <v>446</v>
+        <v>447</v>
       </c>
       <c r="C106" s="2" t="s">
-        <v>447</v>
+        <v>448</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A107" s="1" t="s">
-        <v>448</v>
+        <v>449</v>
       </c>
       <c r="B107" s="2" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
       <c r="C107" s="2" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A108" s="1" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="B108" s="2" t="s">
-        <v>452</v>
+        <v>453</v>
       </c>
       <c r="C108" s="2" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A109" s="1" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="B109" s="2" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
       <c r="C109" s="2" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A110" s="1" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
       <c r="B110" s="2" t="s">
-        <v>458</v>
+        <v>459</v>
       </c>
       <c r="C110" s="2" t="s">
-        <v>459</v>
+        <v>460</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A111" s="1" t="s">
-        <v>460</v>
+        <v>461</v>
       </c>
       <c r="B111" s="2" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="C111" s="2" t="s">
-        <v>462</v>
+        <v>463</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A112" s="1" t="s">
-        <v>463</v>
+        <v>464</v>
       </c>
       <c r="B112" s="2" t="s">
-        <v>464</v>
+        <v>465</v>
       </c>
       <c r="C112" s="2" t="s">
-        <v>465</v>
+        <v>466</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A113" s="1" t="s">
-        <v>466</v>
+        <v>467</v>
       </c>
       <c r="B113" s="2" t="s">
-        <v>467</v>
+        <v>468</v>
       </c>
       <c r="C113" s="2" t="s">
-        <v>468</v>
+        <v>469</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.35">
@@ -4172,266 +4172,266 @@
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A115" s="1" t="s">
-        <v>469</v>
+        <v>470</v>
       </c>
       <c r="B115" s="2" t="s">
-        <v>470</v>
+        <v>471</v>
       </c>
       <c r="C115" s="2" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A116" s="1" t="s">
-        <v>472</v>
+        <v>473</v>
       </c>
       <c r="B116" s="2" t="s">
-        <v>473</v>
+        <v>474</v>
       </c>
       <c r="C116" s="2" t="s">
-        <v>474</v>
+        <v>475</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A117" s="1" t="s">
-        <v>475</v>
+        <v>476</v>
       </c>
       <c r="B117" s="2" t="s">
-        <v>476</v>
+        <v>477</v>
       </c>
       <c r="C117" s="2" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A118" s="1" t="s">
-        <v>478</v>
+        <v>479</v>
       </c>
       <c r="B118" s="2" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="C118" s="2" t="s">
-        <v>480</v>
+        <v>481</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A120" s="1" t="s">
-        <v>481</v>
+        <v>482</v>
       </c>
       <c r="B120" s="2" t="s">
-        <v>482</v>
+        <v>483</v>
       </c>
       <c r="C120" s="2" t="s">
-        <v>483</v>
+        <v>484</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A121" s="1" t="s">
-        <v>484</v>
+        <v>485</v>
       </c>
       <c r="B121" s="2" t="s">
-        <v>485</v>
+        <v>486</v>
       </c>
       <c r="C121" s="2" t="s">
-        <v>486</v>
+        <v>487</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A122" s="1" t="s">
-        <v>487</v>
+        <v>488</v>
       </c>
       <c r="B122" s="2" t="s">
-        <v>488</v>
+        <v>489</v>
       </c>
       <c r="C122" s="2" t="s">
-        <v>489</v>
+        <v>490</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A123" s="1" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
       <c r="B123" s="2" t="s">
-        <v>491</v>
+        <v>492</v>
       </c>
       <c r="C123" s="2" t="s">
-        <v>492</v>
+        <v>493</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A124" s="1" t="s">
-        <v>493</v>
+        <v>494</v>
       </c>
       <c r="B124" s="2" t="s">
-        <v>494</v>
+        <v>495</v>
       </c>
       <c r="C124" s="2" t="s">
-        <v>495</v>
+        <v>496</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A125" s="1" t="s">
-        <v>496</v>
+        <v>497</v>
       </c>
       <c r="B125" s="2" t="s">
-        <v>497</v>
+        <v>498</v>
       </c>
       <c r="C125" s="2" t="s">
-        <v>498</v>
+        <v>499</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A126" s="1" t="s">
-        <v>499</v>
+        <v>500</v>
       </c>
       <c r="B126" s="2" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="C126" s="2" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A128" s="1" t="s">
-        <v>502</v>
+        <v>503</v>
       </c>
       <c r="B128" s="2" t="s">
-        <v>503</v>
+        <v>504</v>
       </c>
       <c r="C128" s="2" t="s">
-        <v>504</v>
+        <v>505</v>
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A129" s="1" t="s">
-        <v>505</v>
+        <v>506</v>
       </c>
       <c r="B129" s="2" t="s">
-        <v>506</v>
+        <v>507</v>
       </c>
       <c r="C129" s="2" t="s">
-        <v>507</v>
+        <v>508</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A130" s="1" t="s">
-        <v>508</v>
+        <v>509</v>
       </c>
       <c r="B130" s="2" t="s">
-        <v>509</v>
+        <v>510</v>
       </c>
       <c r="C130" s="2" t="s">
-        <v>510</v>
+        <v>511</v>
       </c>
     </row>
     <row r="131" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A131" s="1" t="s">
-        <v>511</v>
+        <v>512</v>
       </c>
       <c r="B131" s="2" t="s">
-        <v>512</v>
+        <v>513</v>
       </c>
       <c r="C131" s="2" t="s">
-        <v>513</v>
+        <v>514</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A132" s="1" t="s">
-        <v>514</v>
+        <v>515</v>
       </c>
       <c r="B132" s="2" t="s">
-        <v>515</v>
+        <v>516</v>
       </c>
       <c r="C132" s="2" t="s">
-        <v>516</v>
+        <v>517</v>
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A134" s="1" t="s">
-        <v>517</v>
+        <v>518</v>
       </c>
       <c r="B134" s="2" t="s">
-        <v>518</v>
+        <v>519</v>
       </c>
       <c r="C134" s="2" t="s">
-        <v>519</v>
+        <v>520</v>
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A135" s="1" t="s">
-        <v>520</v>
+        <v>521</v>
       </c>
       <c r="B135" s="1" t="s">
-        <v>521</v>
+        <v>522</v>
       </c>
       <c r="C135" s="1" t="s">
-        <v>522</v>
+        <v>523</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A136" s="1" t="s">
-        <v>523</v>
+        <v>524</v>
       </c>
       <c r="B136" s="1" t="s">
-        <v>524</v>
+        <v>525</v>
       </c>
       <c r="C136" s="1" t="s">
-        <v>525</v>
+        <v>526</v>
       </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A137" s="1" t="s">
-        <v>526</v>
+        <v>527</v>
       </c>
       <c r="B137" s="2" t="s">
-        <v>527</v>
+        <v>528</v>
       </c>
       <c r="C137" s="1" t="s">
-        <v>528</v>
+        <v>529</v>
       </c>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A138" s="1" t="s">
-        <v>529</v>
+        <v>530</v>
       </c>
       <c r="B138" s="1" t="s">
-        <v>530</v>
+        <v>531</v>
       </c>
       <c r="C138" s="1" t="s">
-        <v>531</v>
+        <v>532</v>
       </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A139" s="1" t="s">
-        <v>532</v>
+        <v>533</v>
       </c>
       <c r="B139" s="2" t="s">
-        <v>533</v>
+        <v>534</v>
       </c>
       <c r="C139" s="2" t="s">
-        <v>534</v>
+        <v>535</v>
       </c>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A141" s="1" t="s">
-        <v>535</v>
+        <v>536</v>
       </c>
       <c r="B141" s="2" t="s">
-        <v>536</v>
+        <v>537</v>
       </c>
       <c r="C141" s="2" t="s">
-        <v>537</v>
+        <v>538</v>
       </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A142" s="1" t="s">
-        <v>538</v>
+        <v>539</v>
       </c>
       <c r="B142" s="2" t="s">
-        <v>539</v>
+        <v>540</v>
       </c>
       <c r="C142" s="2" t="s">
-        <v>540</v>
+        <v>541</v>
       </c>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.35">
@@ -4440,57 +4440,57 @@
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A144" s="1" t="s">
-        <v>541</v>
+        <v>542</v>
       </c>
       <c r="B144" s="2" t="s">
-        <v>542</v>
+        <v>543</v>
       </c>
       <c r="C144" s="2" t="s">
-        <v>543</v>
+        <v>544</v>
       </c>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A145" s="1" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="B145" s="2" t="s">
-        <v>545</v>
+        <v>546</v>
       </c>
       <c r="C145" s="2" t="s">
-        <v>546</v>
+        <v>547</v>
       </c>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A146" s="1" t="s">
-        <v>547</v>
+        <v>548</v>
       </c>
       <c r="B146" s="2" t="s">
-        <v>548</v>
+        <v>549</v>
       </c>
       <c r="C146" s="2" t="s">
-        <v>549</v>
+        <v>550</v>
       </c>
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A147" s="1" t="s">
-        <v>550</v>
+        <v>551</v>
       </c>
       <c r="B147" s="2" t="s">
-        <v>551</v>
+        <v>552</v>
       </c>
       <c r="C147" s="2" t="s">
-        <v>552</v>
+        <v>553</v>
       </c>
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A148" s="1" t="s">
-        <v>553</v>
+        <v>554</v>
       </c>
       <c r="B148" s="2" t="s">
-        <v>554</v>
+        <v>555</v>
       </c>
       <c r="C148" s="2" t="s">
-        <v>555</v>
+        <v>556</v>
       </c>
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.35">
@@ -4499,101 +4499,101 @@
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A150" s="1" t="s">
-        <v>556</v>
+        <v>557</v>
       </c>
       <c r="B150" s="2" t="s">
-        <v>557</v>
+        <v>558</v>
       </c>
       <c r="C150" s="2" t="s">
-        <v>558</v>
+        <v>559</v>
       </c>
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A151" s="1" t="s">
-        <v>559</v>
+        <v>560</v>
       </c>
       <c r="B151" s="2" t="s">
-        <v>560</v>
+        <v>561</v>
       </c>
       <c r="C151" s="2" t="s">
-        <v>561</v>
+        <v>562</v>
       </c>
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A153" s="1" t="s">
-        <v>562</v>
+        <v>563</v>
       </c>
       <c r="B153" s="1" t="s">
-        <v>563</v>
+        <v>564</v>
       </c>
       <c r="C153" s="1" t="s">
-        <v>564</v>
+        <v>565</v>
       </c>
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A154" s="1" t="s">
-        <v>565</v>
+        <v>566</v>
       </c>
       <c r="B154" s="1" t="s">
-        <v>566</v>
+        <v>567</v>
       </c>
       <c r="C154" s="1" t="s">
-        <v>567</v>
+        <v>568</v>
       </c>
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A155" s="1" t="s">
-        <v>568</v>
+        <v>569</v>
       </c>
       <c r="B155" s="1" t="s">
-        <v>569</v>
+        <v>570</v>
       </c>
       <c r="C155" s="1" t="s">
-        <v>570</v>
+        <v>571</v>
       </c>
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A156" s="1" t="s">
-        <v>571</v>
+        <v>572</v>
       </c>
       <c r="B156" s="1" t="s">
-        <v>572</v>
+        <v>573</v>
       </c>
       <c r="C156" s="1" t="s">
-        <v>573</v>
+        <v>574</v>
       </c>
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A157" s="1" t="s">
-        <v>574</v>
+        <v>575</v>
       </c>
       <c r="B157" s="2" t="s">
-        <v>575</v>
+        <v>576</v>
       </c>
       <c r="C157" s="2" t="s">
-        <v>576</v>
+        <v>577</v>
       </c>
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A158" s="1" t="s">
-        <v>577</v>
+        <v>578</v>
       </c>
       <c r="B158" s="1" t="s">
-        <v>578</v>
+        <v>579</v>
       </c>
       <c r="C158" s="1" t="s">
-        <v>579</v>
+        <v>580</v>
       </c>
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A159" s="1" t="s">
-        <v>580</v>
+        <v>581</v>
       </c>
       <c r="B159" s="1" t="s">
-        <v>581</v>
+        <v>582</v>
       </c>
       <c r="C159" s="1" t="s">
-        <v>582</v>
+        <v>583</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Implement exception handling at when getting data from single OU/Folder
Avoid crashing failed operation when the user does not have access to some OU/Folders and just get data from the ones that access is granted
</commit_message>
<xml_diff>
--- a/Config.xlsx
+++ b/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mateus.cruz\Documents\GitHub\OrchestratorManager\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E14931CF-35BC-4B7A-92F8-8CA9A0C05D07}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47D13A51-079A-4898-97A3-3BEB0DDC9E94}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="628" uniqueCount="585">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="631" uniqueCount="588">
   <si>
     <t>Name</t>
   </si>
@@ -1234,6 +1234,15 @@
   </si>
   <si>
     <t>フォルダー（組織単位）IDが無効か指定されませんでした。</t>
+  </si>
+  <si>
+    <t>FailedToGetDataFromOUFolder</t>
+  </si>
+  <si>
+    <t>Failed to get data from Folder (Organization Unit) named {0}.</t>
+  </si>
+  <si>
+    <t>{0}というフォルダー（組織単位）からデータを取得することができませんでした。</t>
   </si>
   <si>
     <t>UnsupportedAssetType</t>
@@ -1896,8 +1905,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table13" displayName="Table13" ref="A1:C159" totalsRowShown="0">
-  <autoFilter ref="A1:C159" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table13" displayName="Table13" ref="A1:C160" totalsRowShown="0">
+  <autoFilter ref="A1:C160" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Name"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="EN"/>
@@ -2218,7 +2227,7 @@
         <v>8</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>584</v>
+        <v>587</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>9</v>
@@ -2260,7 +2269,7 @@
   <dimension ref="A1:C60"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2 A2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2945,10 +2954,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1927ABA9-1814-4487-9CEC-ABDCAF91481F}">
-  <dimension ref="A1:C159"/>
+  <dimension ref="A1:C160"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2 A2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3880,19 +3889,19 @@
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B86" s="2"/>
-      <c r="C86" s="2"/>
+      <c r="A86" s="1" t="s">
+        <v>395</v>
+      </c>
+      <c r="B86" s="2" t="s">
+        <v>396</v>
+      </c>
+      <c r="C86" s="2" t="s">
+        <v>397</v>
+      </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A87" s="1" t="s">
-        <v>395</v>
-      </c>
-      <c r="B87" s="2" t="s">
-        <v>396</v>
-      </c>
-      <c r="C87" s="2" t="s">
-        <v>397</v>
-      </c>
+      <c r="B87" s="2"/>
+      <c r="C87" s="2"/>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A88" s="1" t="s">
@@ -3972,19 +3981,19 @@
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B95" s="2"/>
-      <c r="C95" s="2"/>
+      <c r="A95" s="1" t="s">
+        <v>419</v>
+      </c>
+      <c r="B95" s="2" t="s">
+        <v>420</v>
+      </c>
+      <c r="C95" s="2" t="s">
+        <v>421</v>
+      </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A96" s="1" t="s">
-        <v>419</v>
-      </c>
-      <c r="B96" s="2" t="s">
-        <v>420</v>
-      </c>
-      <c r="C96" s="2" t="s">
-        <v>421</v>
-      </c>
+      <c r="B96" s="2"/>
+      <c r="C96" s="2"/>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A97" s="1" t="s">
@@ -4075,19 +4084,19 @@
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B105" s="2"/>
-      <c r="C105" s="2"/>
+      <c r="A105" s="1" t="s">
+        <v>446</v>
+      </c>
+      <c r="B105" s="2" t="s">
+        <v>447</v>
+      </c>
+      <c r="C105" s="2" t="s">
+        <v>448</v>
+      </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A106" s="1" t="s">
-        <v>446</v>
-      </c>
-      <c r="B106" s="2" t="s">
-        <v>447</v>
-      </c>
-      <c r="C106" s="2" t="s">
-        <v>448</v>
-      </c>
+      <c r="B106" s="2"/>
+      <c r="C106" s="2"/>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A107" s="1" t="s">
@@ -4167,19 +4176,19 @@
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B114" s="2"/>
-      <c r="C114" s="2"/>
+      <c r="A114" s="1" t="s">
+        <v>470</v>
+      </c>
+      <c r="B114" s="2" t="s">
+        <v>471</v>
+      </c>
+      <c r="C114" s="2" t="s">
+        <v>472</v>
+      </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A115" s="1" t="s">
-        <v>470</v>
-      </c>
-      <c r="B115" s="2" t="s">
-        <v>471</v>
-      </c>
-      <c r="C115" s="2" t="s">
-        <v>472</v>
-      </c>
+      <c r="B115" s="2"/>
+      <c r="C115" s="2"/>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A116" s="1" t="s">
@@ -4214,14 +4223,14 @@
         <v>481</v>
       </c>
     </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A120" s="1" t="s">
+    <row r="119" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A119" s="1" t="s">
         <v>482</v>
       </c>
-      <c r="B120" s="2" t="s">
+      <c r="B119" s="2" t="s">
         <v>483</v>
       </c>
-      <c r="C120" s="2" t="s">
+      <c r="C119" s="2" t="s">
         <v>484</v>
       </c>
     </row>
@@ -4291,14 +4300,14 @@
         <v>502</v>
       </c>
     </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A128" s="1" t="s">
+    <row r="127" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A127" s="1" t="s">
         <v>503</v>
       </c>
-      <c r="B128" s="2" t="s">
+      <c r="B127" s="2" t="s">
         <v>504</v>
       </c>
-      <c r="C128" s="2" t="s">
+      <c r="C127" s="2" t="s">
         <v>505</v>
       </c>
     </row>
@@ -4324,7 +4333,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="131" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A131" s="1" t="s">
         <v>512</v>
       </c>
@@ -4335,7 +4344,7 @@
         <v>514</v>
       </c>
     </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A132" s="1" t="s">
         <v>515</v>
       </c>
@@ -4346,14 +4355,14 @@
         <v>517</v>
       </c>
     </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A134" s="1" t="s">
+    <row r="133" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A133" s="1" t="s">
         <v>518</v>
       </c>
-      <c r="B134" s="2" t="s">
+      <c r="B133" s="2" t="s">
         <v>519</v>
       </c>
-      <c r="C134" s="2" t="s">
+      <c r="C133" s="2" t="s">
         <v>520</v>
       </c>
     </row>
@@ -4361,10 +4370,10 @@
       <c r="A135" s="1" t="s">
         <v>521</v>
       </c>
-      <c r="B135" s="1" t="s">
+      <c r="B135" s="2" t="s">
         <v>522</v>
       </c>
-      <c r="C135" s="1" t="s">
+      <c r="C135" s="2" t="s">
         <v>523</v>
       </c>
     </row>
@@ -4383,7 +4392,7 @@
       <c r="A137" s="1" t="s">
         <v>527</v>
       </c>
-      <c r="B137" s="2" t="s">
+      <c r="B137" s="1" t="s">
         <v>528</v>
       </c>
       <c r="C137" s="1" t="s">
@@ -4394,7 +4403,7 @@
       <c r="A138" s="1" t="s">
         <v>530</v>
       </c>
-      <c r="B138" s="1" t="s">
+      <c r="B138" s="2" t="s">
         <v>531</v>
       </c>
       <c r="C138" s="1" t="s">
@@ -4405,21 +4414,21 @@
       <c r="A139" s="1" t="s">
         <v>533</v>
       </c>
-      <c r="B139" s="2" t="s">
+      <c r="B139" s="1" t="s">
         <v>534</v>
       </c>
-      <c r="C139" s="2" t="s">
+      <c r="C139" s="1" t="s">
         <v>535</v>
       </c>
     </row>
-    <row r="141" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A141" s="1" t="s">
+    <row r="140" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A140" s="1" t="s">
         <v>536</v>
       </c>
-      <c r="B141" s="2" t="s">
+      <c r="B140" s="2" t="s">
         <v>537</v>
       </c>
-      <c r="C141" s="2" t="s">
+      <c r="C140" s="2" t="s">
         <v>538</v>
       </c>
     </row>
@@ -4435,19 +4444,19 @@
       </c>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B143" s="2"/>
-      <c r="C143" s="2"/>
+      <c r="A143" s="1" t="s">
+        <v>542</v>
+      </c>
+      <c r="B143" s="2" t="s">
+        <v>543</v>
+      </c>
+      <c r="C143" s="2" t="s">
+        <v>544</v>
+      </c>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A144" s="1" t="s">
-        <v>542</v>
-      </c>
-      <c r="B144" s="2" t="s">
-        <v>543</v>
-      </c>
-      <c r="C144" s="2" t="s">
-        <v>544</v>
-      </c>
+      <c r="B144" s="2"/>
+      <c r="C144" s="2"/>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A145" s="1" t="s">
@@ -4494,19 +4503,19 @@
       </c>
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B149" s="2"/>
-      <c r="C149" s="2"/>
+      <c r="A149" s="1" t="s">
+        <v>557</v>
+      </c>
+      <c r="B149" s="2" t="s">
+        <v>558</v>
+      </c>
+      <c r="C149" s="2" t="s">
+        <v>559</v>
+      </c>
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A150" s="1" t="s">
-        <v>557</v>
-      </c>
-      <c r="B150" s="2" t="s">
-        <v>558</v>
-      </c>
-      <c r="C150" s="2" t="s">
-        <v>559</v>
-      </c>
+      <c r="B150" s="2"/>
+      <c r="C150" s="2"/>
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A151" s="1" t="s">
@@ -4519,14 +4528,14 @@
         <v>562</v>
       </c>
     </row>
-    <row r="153" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A153" s="1" t="s">
+    <row r="152" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A152" s="1" t="s">
         <v>563</v>
       </c>
-      <c r="B153" s="1" t="s">
+      <c r="B152" s="2" t="s">
         <v>564</v>
       </c>
-      <c r="C153" s="1" t="s">
+      <c r="C152" s="2" t="s">
         <v>565</v>
       </c>
     </row>
@@ -4567,10 +4576,10 @@
       <c r="A157" s="1" t="s">
         <v>575</v>
       </c>
-      <c r="B157" s="2" t="s">
+      <c r="B157" s="1" t="s">
         <v>576</v>
       </c>
-      <c r="C157" s="2" t="s">
+      <c r="C157" s="1" t="s">
         <v>577</v>
       </c>
     </row>
@@ -4578,10 +4587,10 @@
       <c r="A158" s="1" t="s">
         <v>578</v>
       </c>
-      <c r="B158" s="1" t="s">
+      <c r="B158" s="2" t="s">
         <v>579</v>
       </c>
-      <c r="C158" s="1" t="s">
+      <c r="C158" s="2" t="s">
         <v>580</v>
       </c>
     </row>
@@ -4594,6 +4603,17 @@
       </c>
       <c r="C159" s="1" t="s">
         <v>583</v>
+      </c>
+    </row>
+    <row r="160" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A160" s="1" t="s">
+        <v>584</v>
+      </c>
+      <c r="B160" s="1" t="s">
+        <v>585</v>
+      </c>
+      <c r="C160" s="1" t="s">
+        <v>586</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Handle invalid HTTP results in false positive successful requests
</commit_message>
<xml_diff>
--- a/Config.xlsx
+++ b/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mateus.cruz\Documents\GitHub\OrchestratorManager\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47D13A51-079A-4898-97A3-3BEB0DDC9E94}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D8A74E2-A916-4B5D-A51C-BDC320C5E33A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="631" uniqueCount="588">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="634" uniqueCount="591">
   <si>
     <t>Name</t>
   </si>
@@ -1099,6 +1099,15 @@
   </si>
   <si>
     <t>サーバーエラーの問題のため、リクエストが失敗しました。</t>
+  </si>
+  <si>
+    <t>InvalidResponseErrorFailure</t>
+  </si>
+  <si>
+    <t>HTTP Request failed due to invalid response. Please confirm the specified Orchestrator URL and version.</t>
+  </si>
+  <si>
+    <t>レスポンスが無効なため、リクエストが失敗しました。指定されたOrchestratorのURLやバージョンなどを確認してください。</t>
   </si>
   <si>
     <t>ConfirmNumerousRequests</t>
@@ -1905,8 +1914,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table13" displayName="Table13" ref="A1:C160" totalsRowShown="0">
-  <autoFilter ref="A1:C160" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table13" displayName="Table13" ref="A1:C161" totalsRowShown="0">
+  <autoFilter ref="A1:C161" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Name"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="EN"/>
@@ -2227,7 +2236,7 @@
         <v>8</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>587</v>
+        <v>590</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>9</v>
@@ -2269,7 +2278,7 @@
   <dimension ref="A1:C60"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A2" sqref="A2 A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2954,10 +2963,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1927ABA9-1814-4487-9CEC-ABDCAF91481F}">
-  <dimension ref="A1:C160"/>
+  <dimension ref="A1:C161"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A2" sqref="A2 A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3734,7 +3743,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A72" s="1" t="s">
         <v>353</v>
       </c>
@@ -3900,19 +3909,19 @@
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B87" s="2"/>
-      <c r="C87" s="2"/>
+      <c r="A87" s="1" t="s">
+        <v>398</v>
+      </c>
+      <c r="B87" s="2" t="s">
+        <v>399</v>
+      </c>
+      <c r="C87" s="2" t="s">
+        <v>400</v>
+      </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A88" s="1" t="s">
-        <v>398</v>
-      </c>
-      <c r="B88" s="2" t="s">
-        <v>399</v>
-      </c>
-      <c r="C88" s="2" t="s">
-        <v>400</v>
-      </c>
+      <c r="B88" s="2"/>
+      <c r="C88" s="2"/>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A89" s="1" t="s">
@@ -3992,19 +4001,19 @@
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B96" s="2"/>
-      <c r="C96" s="2"/>
+      <c r="A96" s="1" t="s">
+        <v>422</v>
+      </c>
+      <c r="B96" s="2" t="s">
+        <v>423</v>
+      </c>
+      <c r="C96" s="2" t="s">
+        <v>424</v>
+      </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A97" s="1" t="s">
-        <v>422</v>
-      </c>
-      <c r="B97" s="2" t="s">
-        <v>423</v>
-      </c>
-      <c r="C97" s="2" t="s">
-        <v>424</v>
-      </c>
+      <c r="B97" s="2"/>
+      <c r="C97" s="2"/>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A98" s="1" t="s">
@@ -4095,19 +4104,19 @@
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B106" s="2"/>
-      <c r="C106" s="2"/>
+      <c r="A106" s="1" t="s">
+        <v>449</v>
+      </c>
+      <c r="B106" s="2" t="s">
+        <v>450</v>
+      </c>
+      <c r="C106" s="2" t="s">
+        <v>451</v>
+      </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A107" s="1" t="s">
-        <v>449</v>
-      </c>
-      <c r="B107" s="2" t="s">
-        <v>450</v>
-      </c>
-      <c r="C107" s="2" t="s">
-        <v>451</v>
-      </c>
+      <c r="B107" s="2"/>
+      <c r="C107" s="2"/>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A108" s="1" t="s">
@@ -4187,19 +4196,19 @@
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B115" s="2"/>
-      <c r="C115" s="2"/>
+      <c r="A115" s="1" t="s">
+        <v>473</v>
+      </c>
+      <c r="B115" s="2" t="s">
+        <v>474</v>
+      </c>
+      <c r="C115" s="2" t="s">
+        <v>475</v>
+      </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A116" s="1" t="s">
-        <v>473</v>
-      </c>
-      <c r="B116" s="2" t="s">
-        <v>474</v>
-      </c>
-      <c r="C116" s="2" t="s">
-        <v>475</v>
-      </c>
+      <c r="B116" s="2"/>
+      <c r="C116" s="2"/>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A117" s="1" t="s">
@@ -4234,14 +4243,14 @@
         <v>484</v>
       </c>
     </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A121" s="1" t="s">
+    <row r="120" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A120" s="1" t="s">
         <v>485</v>
       </c>
-      <c r="B121" s="2" t="s">
+      <c r="B120" s="2" t="s">
         <v>486</v>
       </c>
-      <c r="C121" s="2" t="s">
+      <c r="C120" s="2" t="s">
         <v>487</v>
       </c>
     </row>
@@ -4311,14 +4320,14 @@
         <v>505</v>
       </c>
     </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A129" s="1" t="s">
+    <row r="128" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A128" s="1" t="s">
         <v>506</v>
       </c>
-      <c r="B129" s="2" t="s">
+      <c r="B128" s="2" t="s">
         <v>507</v>
       </c>
-      <c r="C129" s="2" t="s">
+      <c r="C128" s="2" t="s">
         <v>508</v>
       </c>
     </row>
@@ -4344,7 +4353,7 @@
         <v>514</v>
       </c>
     </row>
-    <row r="132" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A132" s="1" t="s">
         <v>515</v>
       </c>
@@ -4355,7 +4364,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A133" s="1" t="s">
         <v>518</v>
       </c>
@@ -4366,14 +4375,14 @@
         <v>520</v>
       </c>
     </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A135" s="1" t="s">
+    <row r="134" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A134" s="1" t="s">
         <v>521</v>
       </c>
-      <c r="B135" s="2" t="s">
+      <c r="B134" s="2" t="s">
         <v>522</v>
       </c>
-      <c r="C135" s="2" t="s">
+      <c r="C134" s="2" t="s">
         <v>523</v>
       </c>
     </row>
@@ -4381,10 +4390,10 @@
       <c r="A136" s="1" t="s">
         <v>524</v>
       </c>
-      <c r="B136" s="1" t="s">
+      <c r="B136" s="2" t="s">
         <v>525</v>
       </c>
-      <c r="C136" s="1" t="s">
+      <c r="C136" s="2" t="s">
         <v>526</v>
       </c>
     </row>
@@ -4403,7 +4412,7 @@
       <c r="A138" s="1" t="s">
         <v>530</v>
       </c>
-      <c r="B138" s="2" t="s">
+      <c r="B138" s="1" t="s">
         <v>531</v>
       </c>
       <c r="C138" s="1" t="s">
@@ -4414,7 +4423,7 @@
       <c r="A139" s="1" t="s">
         <v>533</v>
       </c>
-      <c r="B139" s="1" t="s">
+      <c r="B139" s="2" t="s">
         <v>534</v>
       </c>
       <c r="C139" s="1" t="s">
@@ -4425,21 +4434,21 @@
       <c r="A140" s="1" t="s">
         <v>536</v>
       </c>
-      <c r="B140" s="2" t="s">
+      <c r="B140" s="1" t="s">
         <v>537</v>
       </c>
-      <c r="C140" s="2" t="s">
+      <c r="C140" s="1" t="s">
         <v>538</v>
       </c>
     </row>
-    <row r="142" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A142" s="1" t="s">
+    <row r="141" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A141" s="1" t="s">
         <v>539</v>
       </c>
-      <c r="B142" s="2" t="s">
+      <c r="B141" s="2" t="s">
         <v>540</v>
       </c>
-      <c r="C142" s="2" t="s">
+      <c r="C141" s="2" t="s">
         <v>541</v>
       </c>
     </row>
@@ -4455,19 +4464,19 @@
       </c>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B144" s="2"/>
-      <c r="C144" s="2"/>
+      <c r="A144" s="1" t="s">
+        <v>545</v>
+      </c>
+      <c r="B144" s="2" t="s">
+        <v>546</v>
+      </c>
+      <c r="C144" s="2" t="s">
+        <v>547</v>
+      </c>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A145" s="1" t="s">
-        <v>545</v>
-      </c>
-      <c r="B145" s="2" t="s">
-        <v>546</v>
-      </c>
-      <c r="C145" s="2" t="s">
-        <v>547</v>
-      </c>
+      <c r="B145" s="2"/>
+      <c r="C145" s="2"/>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A146" s="1" t="s">
@@ -4514,19 +4523,19 @@
       </c>
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B150" s="2"/>
-      <c r="C150" s="2"/>
+      <c r="A150" s="1" t="s">
+        <v>560</v>
+      </c>
+      <c r="B150" s="2" t="s">
+        <v>561</v>
+      </c>
+      <c r="C150" s="2" t="s">
+        <v>562</v>
+      </c>
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A151" s="1" t="s">
-        <v>560</v>
-      </c>
-      <c r="B151" s="2" t="s">
-        <v>561</v>
-      </c>
-      <c r="C151" s="2" t="s">
-        <v>562</v>
-      </c>
+      <c r="B151" s="2"/>
+      <c r="C151" s="2"/>
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A152" s="1" t="s">
@@ -4539,14 +4548,14 @@
         <v>565</v>
       </c>
     </row>
-    <row r="154" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A154" s="1" t="s">
+    <row r="153" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A153" s="1" t="s">
         <v>566</v>
       </c>
-      <c r="B154" s="1" t="s">
+      <c r="B153" s="2" t="s">
         <v>567</v>
       </c>
-      <c r="C154" s="1" t="s">
+      <c r="C153" s="2" t="s">
         <v>568</v>
       </c>
     </row>
@@ -4587,10 +4596,10 @@
       <c r="A158" s="1" t="s">
         <v>578</v>
       </c>
-      <c r="B158" s="2" t="s">
+      <c r="B158" s="1" t="s">
         <v>579</v>
       </c>
-      <c r="C158" s="2" t="s">
+      <c r="C158" s="1" t="s">
         <v>580</v>
       </c>
     </row>
@@ -4598,10 +4607,10 @@
       <c r="A159" s="1" t="s">
         <v>581</v>
       </c>
-      <c r="B159" s="1" t="s">
+      <c r="B159" s="2" t="s">
         <v>582</v>
       </c>
-      <c r="C159" s="1" t="s">
+      <c r="C159" s="2" t="s">
         <v>583</v>
       </c>
     </row>
@@ -4614,6 +4623,17 @@
       </c>
       <c r="C160" s="1" t="s">
         <v>586</v>
+      </c>
+    </row>
+    <row r="161" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A161" s="1" t="s">
+        <v>587</v>
+      </c>
+      <c r="B161" s="1" t="s">
+        <v>588</v>
+      </c>
+      <c r="C161" s="1" t="s">
+        <v>589</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Cache OU/Folder data to avoid individual requests for each entity to be created
</commit_message>
<xml_diff>
--- a/Config.xlsx
+++ b/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mateus.cruz\Documents\GitHub\OrchestratorManager\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D8A74E2-A916-4B5D-A51C-BDC320C5E33A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DE23B65-8D72-4D9B-B07F-1D4CF63777E3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -56,14 +56,14 @@
     <t>TenantName</t>
   </si>
   <si>
-    <t>Default</t>
-  </si>
-  <si>
     <t>Name of the tenant to be used. 
 Sample value: Default.</t>
   </si>
   <si>
     <t>OnPremisesOrchestratorURL</t>
+  </si>
+  <si>
+    <t>https://myOrchestratorURL</t>
   </si>
   <si>
     <t>URL of the Orchestrator instance to be used. 
@@ -87,9 +87,6 @@
     <t>CloudAccountName</t>
   </si>
   <si>
-    <t>MyAccount</t>
-  </si>
-  <si>
     <t>Unique site URL for Automation Cloud oganization.
 This parameter is exclusive to Automation Cloud Orchestrator instances.
 Sample value: MyAccount (assuming the organization account URL is https://platform.uipath.com/MyAccount).</t>
@@ -1821,7 +1818,10 @@
     <t>キューアイテム一覧のファイルが見つかりませんでした。</t>
   </si>
   <si>
-    <t>https://myOrchestratorURL</t>
+    <t>Default</t>
+  </si>
+  <si>
+    <t>MyAccount</t>
   </si>
 </sst>
 </file>
@@ -2225,18 +2225,18 @@
         <v>5</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>589</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>6</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="58" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>8</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>590</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>9</v>
@@ -2258,10 +2258,10 @@
         <v>12</v>
       </c>
       <c r="B8" s="1" t="s">
+        <v>590</v>
+      </c>
+      <c r="C8" s="2" t="s">
         <v>13</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -2278,7 +2278,7 @@
   <dimension ref="A1:C60"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2 A2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2301,651 +2301,651 @@
     </row>
     <row r="2" spans="1:3" ht="101.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B2" s="1">
         <v>200</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B3" s="1">
         <v>0</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B4" s="1">
         <v>550</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B5" s="1">
         <v>650</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B6" s="1">
         <v>3</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B7" s="1">
         <v>5000</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="C8" s="2" t="s">
         <v>28</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B9" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="C9" s="2" t="s">
         <v>31</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="C10" s="2" t="s">
         <v>34</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="C11" s="2" t="s">
         <v>37</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="C12" s="2" t="s">
         <v>40</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="C13" s="2" t="s">
         <v>43</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="C14" s="2" t="s">
         <v>46</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B15" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="C15" s="2" t="s">
         <v>49</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B16" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="C16" s="2" t="s">
         <v>52</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B17" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="C17" s="2" t="s">
         <v>55</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B18" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="C18" s="2" t="s">
         <v>58</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B19" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="C19" s="2" t="s">
         <v>61</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B20" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="C20" s="2" t="s">
         <v>64</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B21" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="C21" s="2" t="s">
         <v>67</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B22" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="C22" s="2" t="s">
         <v>70</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C23" s="2" t="s">
         <v>72</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C24" s="2" t="s">
         <v>74</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B25" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="B25" s="1" t="s">
+      <c r="C25" s="2" t="s">
         <v>77</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C27" s="2" t="s">
         <v>80</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C28" s="2" t="s">
         <v>82</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C29" s="2" t="s">
         <v>84</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C30" s="2" t="s">
         <v>86</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A31" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B31" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="B31" s="1" t="s">
+      <c r="C31" s="2" t="s">
         <v>89</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B32" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="B32" s="1" t="s">
+      <c r="C32" s="2" t="s">
         <v>92</v>
-      </c>
-      <c r="C32" s="2" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C33" s="2" t="s">
         <v>94</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="C33" s="2" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A34" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B34" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="B34" s="1" t="s">
+      <c r="C34" s="2" t="s">
         <v>97</v>
-      </c>
-      <c r="C34" s="2" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A35" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C35" s="2" t="s">
         <v>99</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="C35" s="2" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A36" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C36" s="2" t="s">
         <v>101</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="C36" s="2" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="37" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A37" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C37" s="2" t="s">
         <v>103</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="C37" s="2" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A38" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C38" s="2" t="s">
         <v>105</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="C38" s="2" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A39" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C39" s="2" t="s">
         <v>107</v>
-      </c>
-      <c r="B39" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="C39" s="2" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A40" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C40" s="2" t="s">
         <v>109</v>
-      </c>
-      <c r="B40" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="C40" s="2" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="41" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A41" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C41" s="2" t="s">
         <v>111</v>
-      </c>
-      <c r="B41" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="C41" s="2" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="42" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A42" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C42" s="2" t="s">
         <v>113</v>
-      </c>
-      <c r="B42" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="C42" s="2" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="43" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A43" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C43" s="2" t="s">
         <v>115</v>
-      </c>
-      <c r="B43" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="C43" s="2" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="44" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A44" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C44" s="2" t="s">
         <v>117</v>
-      </c>
-      <c r="B44" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="C44" s="2" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A45" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C45" s="2" t="s">
         <v>119</v>
-      </c>
-      <c r="B45" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="C45" s="2" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="46" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A46" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C46" s="2" t="s">
         <v>121</v>
-      </c>
-      <c r="B46" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="C46" s="2" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="47" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A47" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C47" s="2" t="s">
         <v>123</v>
-      </c>
-      <c r="B47" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="C47" s="2" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="48" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A48" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C48" s="2" t="s">
         <v>125</v>
-      </c>
-      <c r="B48" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="C48" s="2" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="49" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A49" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C49" s="2" t="s">
         <v>127</v>
-      </c>
-      <c r="B49" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="C49" s="2" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A50" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="B50" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="B50" s="1" t="s">
+      <c r="C50" s="2" t="s">
         <v>130</v>
-      </c>
-      <c r="C50" s="2" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="51" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A51" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C51" s="2" t="s">
         <v>132</v>
-      </c>
-      <c r="B51" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="C51" s="2" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="52" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A52" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C52" s="2" t="s">
         <v>134</v>
-      </c>
-      <c r="B52" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="C52" s="2" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A53" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C53" s="2" t="s">
         <v>136</v>
-      </c>
-      <c r="B53" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="C53" s="2" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="54" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A54" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C54" s="2" t="s">
         <v>138</v>
-      </c>
-      <c r="B54" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="C54" s="2" t="s">
-        <v>139</v>
       </c>
     </row>
     <row r="55" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A55" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C55" s="2" t="s">
         <v>140</v>
-      </c>
-      <c r="B55" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="C55" s="2" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A56" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C56" s="2" t="s">
         <v>142</v>
-      </c>
-      <c r="B56" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="C56" s="2" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="57" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A57" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C57" s="2" t="s">
         <v>144</v>
-      </c>
-      <c r="B57" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="C57" s="2" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="58" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A58" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C58" s="2" t="s">
         <v>146</v>
-      </c>
-      <c r="B58" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="C58" s="2" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="59" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A59" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C59" s="2" t="s">
         <v>148</v>
-      </c>
-      <c r="B59" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="C59" s="2" t="s">
-        <v>149</v>
       </c>
     </row>
     <row r="60" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A60" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C60" s="2" t="s">
         <v>150</v>
-      </c>
-      <c r="B60" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="C60" s="2" t="s">
-        <v>151</v>
       </c>
     </row>
   </sheetData>
@@ -2966,7 +2966,7 @@
   <dimension ref="A1:C161"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2 A2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2981,340 +2981,340 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>152</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>155</v>
-      </c>
       <c r="C2" s="2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="43.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="C3" s="2" t="s">
         <v>157</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="C4" s="2" t="s">
         <v>160</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>161</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>163</v>
-      </c>
       <c r="C5" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="C6" s="2" t="s">
         <v>165</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="C7" s="2" t="s">
         <v>168</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>169</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="C8" s="2" t="s">
         <v>171</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>172</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="C9" s="2" t="s">
         <v>174</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>175</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>176</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="C10" s="2" t="s">
         <v>177</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>178</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="C11" s="2" t="s">
         <v>180</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="B12" s="2" t="s">
         <v>182</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="C12" s="2" t="s">
         <v>183</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="B13" s="2" t="s">
         <v>185</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="C13" s="2" t="s">
         <v>186</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>187</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="B14" s="2" t="s">
         <v>188</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="C14" s="2" t="s">
         <v>189</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>190</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="B15" s="2" t="s">
         <v>191</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="C15" s="2" t="s">
         <v>192</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>193</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="B16" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="C16" s="2" t="s">
         <v>195</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>196</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="B17" s="2" t="s">
         <v>197</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="C17" s="2" t="s">
         <v>198</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>199</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="B18" s="2" t="s">
         <v>200</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="C18" s="2" t="s">
         <v>201</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>202</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="B19" s="2" t="s">
         <v>203</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="C19" s="2" t="s">
         <v>204</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>205</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="B20" s="2" t="s">
         <v>206</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="C20" s="2" t="s">
         <v>207</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>208</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="B21" s="2" t="s">
         <v>209</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="C21" s="2" t="s">
         <v>210</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>211</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="B22" s="2" t="s">
         <v>212</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="C22" s="2" t="s">
         <v>213</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>214</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="B23" s="2" t="s">
         <v>215</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="C23" s="2" t="s">
         <v>216</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>217</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="B24" s="2" t="s">
         <v>218</v>
       </c>
-      <c r="B24" s="2" t="s">
+      <c r="C24" s="2" t="s">
         <v>219</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>220</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="B25" s="2" t="s">
         <v>221</v>
       </c>
-      <c r="B25" s="2" t="s">
+      <c r="C25" s="2" t="s">
         <v>222</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>223</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="B26" s="2" t="s">
         <v>224</v>
       </c>
-      <c r="B26" s="2" t="s">
+      <c r="C26" s="2" t="s">
         <v>225</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>226</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="B27" s="2" t="s">
         <v>227</v>
       </c>
-      <c r="B27" s="2" t="s">
-        <v>228</v>
-      </c>
       <c r="C27" s="2" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="B28" s="2" t="s">
         <v>229</v>
       </c>
-      <c r="B28" s="2" t="s">
-        <v>230</v>
-      </c>
       <c r="C28" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="B29" s="2" t="s">
         <v>231</v>
       </c>
-      <c r="B29" s="2" t="s">
+      <c r="C29" s="2" t="s">
         <v>232</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>233</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A30" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="B30" s="2" t="s">
         <v>234</v>
       </c>
-      <c r="B30" s="2" t="s">
-        <v>235</v>
-      </c>
       <c r="C30" s="2" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A31" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="B31" s="2" t="s">
         <v>236</v>
       </c>
-      <c r="B31" s="2" t="s">
+      <c r="C31" s="2" t="s">
         <v>237</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>238</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.35">
@@ -3323,101 +3323,101 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A33" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="B33" s="2" t="s">
         <v>239</v>
       </c>
-      <c r="B33" s="2" t="s">
+      <c r="C33" s="2" t="s">
         <v>240</v>
-      </c>
-      <c r="C33" s="2" t="s">
-        <v>241</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A34" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="B34" s="2" t="s">
         <v>242</v>
       </c>
-      <c r="B34" s="2" t="s">
+      <c r="C34" s="2" t="s">
         <v>243</v>
-      </c>
-      <c r="C34" s="2" t="s">
-        <v>244</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A35" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="B35" s="2" t="s">
         <v>245</v>
       </c>
-      <c r="B35" s="2" t="s">
+      <c r="C35" s="2" t="s">
         <v>246</v>
-      </c>
-      <c r="C35" s="2" t="s">
-        <v>247</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A36" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="B36" s="2" t="s">
         <v>248</v>
       </c>
-      <c r="B36" s="2" t="s">
+      <c r="C36" s="2" t="s">
         <v>249</v>
-      </c>
-      <c r="C36" s="2" t="s">
-        <v>250</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A37" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="B37" s="2" t="s">
         <v>251</v>
       </c>
-      <c r="B37" s="2" t="s">
+      <c r="C37" s="2" t="s">
         <v>252</v>
-      </c>
-      <c r="C37" s="2" t="s">
-        <v>253</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A38" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="B38" s="2" t="s">
         <v>254</v>
       </c>
-      <c r="B38" s="2" t="s">
+      <c r="C38" s="2" t="s">
         <v>255</v>
-      </c>
-      <c r="C38" s="2" t="s">
-        <v>256</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A39" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="B39" s="2" t="s">
         <v>257</v>
       </c>
-      <c r="B39" s="2" t="s">
+      <c r="C39" s="2" t="s">
         <v>258</v>
-      </c>
-      <c r="C39" s="2" t="s">
-        <v>259</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A40" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="B40" s="2" t="s">
         <v>260</v>
       </c>
-      <c r="B40" s="2" t="s">
+      <c r="C40" s="2" t="s">
         <v>261</v>
-      </c>
-      <c r="C40" s="2" t="s">
-        <v>262</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A41" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="B41" s="2" t="s">
         <v>263</v>
       </c>
-      <c r="B41" s="2" t="s">
+      <c r="C41" s="2" t="s">
         <v>264</v>
-      </c>
-      <c r="C41" s="2" t="s">
-        <v>265</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.35">
@@ -3426,497 +3426,497 @@
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A43" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="B43" s="2" t="s">
         <v>266</v>
       </c>
-      <c r="B43" s="2" t="s">
+      <c r="C43" s="2" t="s">
         <v>267</v>
-      </c>
-      <c r="C43" s="2" t="s">
-        <v>268</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A44" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="B44" s="2" t="s">
         <v>269</v>
       </c>
-      <c r="B44" s="2" t="s">
+      <c r="C44" s="2" t="s">
         <v>270</v>
-      </c>
-      <c r="C44" s="2" t="s">
-        <v>271</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A45" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="B45" s="2" t="s">
         <v>272</v>
       </c>
-      <c r="B45" s="2" t="s">
+      <c r="C45" s="2" t="s">
         <v>273</v>
-      </c>
-      <c r="C45" s="2" t="s">
-        <v>274</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A46" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="B46" s="2" t="s">
         <v>275</v>
       </c>
-      <c r="B46" s="2" t="s">
+      <c r="C46" s="2" t="s">
         <v>276</v>
-      </c>
-      <c r="C46" s="2" t="s">
-        <v>277</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A47" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="B47" s="2" t="s">
         <v>278</v>
       </c>
-      <c r="B47" s="2" t="s">
+      <c r="C47" s="2" t="s">
         <v>279</v>
-      </c>
-      <c r="C47" s="2" t="s">
-        <v>280</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A48" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="B48" s="2" t="s">
         <v>281</v>
       </c>
-      <c r="B48" s="2" t="s">
+      <c r="C48" s="2" t="s">
         <v>282</v>
-      </c>
-      <c r="C48" s="2" t="s">
-        <v>283</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A49" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="B49" s="2" t="s">
         <v>284</v>
       </c>
-      <c r="B49" s="2" t="s">
+      <c r="C49" s="2" t="s">
         <v>285</v>
-      </c>
-      <c r="C49" s="2" t="s">
-        <v>286</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A50" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="B50" s="2" t="s">
         <v>287</v>
       </c>
-      <c r="B50" s="2" t="s">
+      <c r="C50" s="2" t="s">
         <v>288</v>
-      </c>
-      <c r="C50" s="2" t="s">
-        <v>289</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A51" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="B51" s="2" t="s">
         <v>290</v>
       </c>
-      <c r="B51" s="2" t="s">
+      <c r="C51" s="2" t="s">
         <v>291</v>
-      </c>
-      <c r="C51" s="2" t="s">
-        <v>292</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A52" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="B52" s="2" t="s">
         <v>293</v>
       </c>
-      <c r="B52" s="2" t="s">
+      <c r="C52" s="2" t="s">
         <v>294</v>
-      </c>
-      <c r="C52" s="2" t="s">
-        <v>295</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A53" s="1" t="s">
+        <v>295</v>
+      </c>
+      <c r="B53" s="2" t="s">
         <v>296</v>
       </c>
-      <c r="B53" s="2" t="s">
+      <c r="C53" s="2" t="s">
         <v>297</v>
-      </c>
-      <c r="C53" s="2" t="s">
-        <v>298</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A54" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="B54" s="2" t="s">
         <v>299</v>
       </c>
-      <c r="B54" s="2" t="s">
+      <c r="C54" s="2" t="s">
         <v>300</v>
-      </c>
-      <c r="C54" s="2" t="s">
-        <v>301</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A55" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="B55" s="2" t="s">
         <v>302</v>
       </c>
-      <c r="B55" s="2" t="s">
+      <c r="C55" s="2" t="s">
         <v>303</v>
-      </c>
-      <c r="C55" s="2" t="s">
-        <v>304</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A56" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="B56" s="2" t="s">
         <v>305</v>
       </c>
-      <c r="B56" s="2" t="s">
+      <c r="C56" s="2" t="s">
         <v>306</v>
-      </c>
-      <c r="C56" s="2" t="s">
-        <v>307</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A57" s="1" t="s">
+        <v>307</v>
+      </c>
+      <c r="B57" s="2" t="s">
         <v>308</v>
       </c>
-      <c r="B57" s="2" t="s">
+      <c r="C57" s="2" t="s">
         <v>309</v>
-      </c>
-      <c r="C57" s="2" t="s">
-        <v>310</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A58" s="1" t="s">
+        <v>310</v>
+      </c>
+      <c r="B58" s="2" t="s">
         <v>311</v>
       </c>
-      <c r="B58" s="2" t="s">
+      <c r="C58" s="2" t="s">
         <v>312</v>
-      </c>
-      <c r="C58" s="2" t="s">
-        <v>313</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A59" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="B59" s="2" t="s">
         <v>314</v>
       </c>
-      <c r="B59" s="2" t="s">
+      <c r="C59" s="2" t="s">
         <v>315</v>
-      </c>
-      <c r="C59" s="2" t="s">
-        <v>316</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A60" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="B60" s="2" t="s">
         <v>317</v>
       </c>
-      <c r="B60" s="2" t="s">
+      <c r="C60" s="2" t="s">
         <v>318</v>
-      </c>
-      <c r="C60" s="2" t="s">
-        <v>319</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A61" s="1" t="s">
+        <v>319</v>
+      </c>
+      <c r="B61" s="2" t="s">
         <v>320</v>
       </c>
-      <c r="B61" s="2" t="s">
+      <c r="C61" s="2" t="s">
         <v>321</v>
-      </c>
-      <c r="C61" s="2" t="s">
-        <v>322</v>
       </c>
     </row>
     <row r="62" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A62" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="B62" s="2" t="s">
         <v>323</v>
       </c>
-      <c r="B62" s="2" t="s">
+      <c r="C62" s="2" t="s">
         <v>324</v>
-      </c>
-      <c r="C62" s="2" t="s">
-        <v>325</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A63" s="1" t="s">
+        <v>325</v>
+      </c>
+      <c r="B63" s="2" t="s">
         <v>326</v>
       </c>
-      <c r="B63" s="2" t="s">
+      <c r="C63" s="2" t="s">
         <v>327</v>
-      </c>
-      <c r="C63" s="2" t="s">
-        <v>328</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A64" s="1" t="s">
+        <v>328</v>
+      </c>
+      <c r="B64" s="2" t="s">
         <v>329</v>
       </c>
-      <c r="B64" s="2" t="s">
+      <c r="C64" s="2" t="s">
         <v>330</v>
-      </c>
-      <c r="C64" s="2" t="s">
-        <v>331</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A65" s="1" t="s">
+        <v>331</v>
+      </c>
+      <c r="B65" s="2" t="s">
         <v>332</v>
       </c>
-      <c r="B65" s="2" t="s">
+      <c r="C65" s="2" t="s">
         <v>333</v>
-      </c>
-      <c r="C65" s="2" t="s">
-        <v>334</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A66" s="1" t="s">
+        <v>334</v>
+      </c>
+      <c r="B66" s="2" t="s">
         <v>335</v>
       </c>
-      <c r="B66" s="2" t="s">
+      <c r="C66" s="2" t="s">
         <v>336</v>
-      </c>
-      <c r="C66" s="2" t="s">
-        <v>337</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A67" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="B67" s="2" t="s">
         <v>338</v>
       </c>
-      <c r="B67" s="2" t="s">
+      <c r="C67" s="2" t="s">
         <v>339</v>
-      </c>
-      <c r="C67" s="2" t="s">
-        <v>340</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A68" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="B68" s="2" t="s">
         <v>341</v>
       </c>
-      <c r="B68" s="2" t="s">
+      <c r="C68" s="2" t="s">
         <v>342</v>
-      </c>
-      <c r="C68" s="2" t="s">
-        <v>343</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A69" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="B69" s="2" t="s">
         <v>344</v>
       </c>
-      <c r="B69" s="2" t="s">
+      <c r="C69" s="2" t="s">
         <v>345</v>
-      </c>
-      <c r="C69" s="2" t="s">
-        <v>346</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A70" s="1" t="s">
+        <v>346</v>
+      </c>
+      <c r="B70" s="2" t="s">
         <v>347</v>
       </c>
-      <c r="B70" s="2" t="s">
+      <c r="C70" s="2" t="s">
         <v>348</v>
-      </c>
-      <c r="C70" s="2" t="s">
-        <v>349</v>
       </c>
     </row>
     <row r="71" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A71" s="1" t="s">
+        <v>349</v>
+      </c>
+      <c r="B71" s="2" t="s">
         <v>350</v>
       </c>
-      <c r="B71" s="2" t="s">
+      <c r="C71" s="2" t="s">
         <v>351</v>
-      </c>
-      <c r="C71" s="2" t="s">
-        <v>352</v>
       </c>
     </row>
     <row r="72" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A72" s="1" t="s">
+        <v>352</v>
+      </c>
+      <c r="B72" s="2" t="s">
         <v>353</v>
       </c>
-      <c r="B72" s="2" t="s">
+      <c r="C72" s="2" t="s">
         <v>354</v>
-      </c>
-      <c r="C72" s="2" t="s">
-        <v>355</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A73" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="B73" s="2" t="s">
         <v>356</v>
       </c>
-      <c r="B73" s="2" t="s">
+      <c r="C73" s="2" t="s">
         <v>357</v>
-      </c>
-      <c r="C73" s="2" t="s">
-        <v>358</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A74" s="1" t="s">
+        <v>358</v>
+      </c>
+      <c r="B74" s="2" t="s">
         <v>359</v>
       </c>
-      <c r="B74" s="2" t="s">
+      <c r="C74" s="2" t="s">
         <v>360</v>
-      </c>
-      <c r="C74" s="2" t="s">
-        <v>361</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A75" s="1" t="s">
+        <v>361</v>
+      </c>
+      <c r="B75" s="2" t="s">
         <v>362</v>
       </c>
-      <c r="B75" s="2" t="s">
+      <c r="C75" s="2" t="s">
         <v>363</v>
-      </c>
-      <c r="C75" s="2" t="s">
-        <v>364</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A76" s="1" t="s">
+        <v>364</v>
+      </c>
+      <c r="B76" s="2" t="s">
         <v>365</v>
       </c>
-      <c r="B76" s="2" t="s">
+      <c r="C76" s="2" t="s">
         <v>366</v>
-      </c>
-      <c r="C76" s="2" t="s">
-        <v>367</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A77" s="1" t="s">
+        <v>367</v>
+      </c>
+      <c r="B77" s="2" t="s">
         <v>368</v>
       </c>
-      <c r="B77" s="2" t="s">
+      <c r="C77" s="2" t="s">
         <v>369</v>
-      </c>
-      <c r="C77" s="2" t="s">
-        <v>370</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A78" s="1" t="s">
+        <v>370</v>
+      </c>
+      <c r="B78" s="2" t="s">
         <v>371</v>
       </c>
-      <c r="B78" s="2" t="s">
+      <c r="C78" s="2" t="s">
         <v>372</v>
-      </c>
-      <c r="C78" s="2" t="s">
-        <v>373</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A79" s="1" t="s">
+        <v>373</v>
+      </c>
+      <c r="B79" s="2" t="s">
         <v>374</v>
       </c>
-      <c r="B79" s="2" t="s">
+      <c r="C79" s="2" t="s">
         <v>375</v>
-      </c>
-      <c r="C79" s="2" t="s">
-        <v>376</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A80" s="1" t="s">
+        <v>376</v>
+      </c>
+      <c r="B80" s="2" t="s">
         <v>377</v>
       </c>
-      <c r="B80" s="2" t="s">
+      <c r="C80" s="2" t="s">
         <v>378</v>
-      </c>
-      <c r="C80" s="2" t="s">
-        <v>379</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A81" s="1" t="s">
+        <v>379</v>
+      </c>
+      <c r="B81" s="2" t="s">
         <v>380</v>
       </c>
-      <c r="B81" s="2" t="s">
+      <c r="C81" s="2" t="s">
         <v>381</v>
-      </c>
-      <c r="C81" s="2" t="s">
-        <v>382</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A82" s="1" t="s">
+        <v>382</v>
+      </c>
+      <c r="B82" s="2" t="s">
         <v>383</v>
       </c>
-      <c r="B82" s="2" t="s">
+      <c r="C82" s="2" t="s">
         <v>384</v>
-      </c>
-      <c r="C82" s="2" t="s">
-        <v>385</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A83" s="1" t="s">
+        <v>385</v>
+      </c>
+      <c r="B83" s="2" t="s">
         <v>386</v>
       </c>
-      <c r="B83" s="2" t="s">
+      <c r="C83" s="2" t="s">
         <v>387</v>
-      </c>
-      <c r="C83" s="2" t="s">
-        <v>388</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A84" s="1" t="s">
+        <v>388</v>
+      </c>
+      <c r="B84" s="2" t="s">
         <v>389</v>
       </c>
-      <c r="B84" s="2" t="s">
+      <c r="C84" s="2" t="s">
         <v>390</v>
-      </c>
-      <c r="C84" s="2" t="s">
-        <v>391</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A85" s="1" t="s">
+        <v>391</v>
+      </c>
+      <c r="B85" s="2" t="s">
         <v>392</v>
       </c>
-      <c r="B85" s="2" t="s">
+      <c r="C85" s="2" t="s">
         <v>393</v>
-      </c>
-      <c r="C85" s="2" t="s">
-        <v>394</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A86" s="1" t="s">
+        <v>394</v>
+      </c>
+      <c r="B86" s="2" t="s">
         <v>395</v>
       </c>
-      <c r="B86" s="2" t="s">
+      <c r="C86" s="2" t="s">
         <v>396</v>
-      </c>
-      <c r="C86" s="2" t="s">
-        <v>397</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A87" s="1" t="s">
+        <v>397</v>
+      </c>
+      <c r="B87" s="2" t="s">
         <v>398</v>
       </c>
-      <c r="B87" s="2" t="s">
+      <c r="C87" s="2" t="s">
         <v>399</v>
-      </c>
-      <c r="C87" s="2" t="s">
-        <v>400</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.35">
@@ -3925,90 +3925,90 @@
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A89" s="1" t="s">
+        <v>400</v>
+      </c>
+      <c r="B89" s="2" t="s">
         <v>401</v>
       </c>
-      <c r="B89" s="2" t="s">
+      <c r="C89" s="2" t="s">
         <v>402</v>
-      </c>
-      <c r="C89" s="2" t="s">
-        <v>403</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A90" s="1" t="s">
+        <v>403</v>
+      </c>
+      <c r="B90" s="2" t="s">
         <v>404</v>
       </c>
-      <c r="B90" s="2" t="s">
+      <c r="C90" s="2" t="s">
         <v>405</v>
-      </c>
-      <c r="C90" s="2" t="s">
-        <v>406</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A91" s="1" t="s">
+        <v>406</v>
+      </c>
+      <c r="B91" s="2" t="s">
         <v>407</v>
       </c>
-      <c r="B91" s="2" t="s">
+      <c r="C91" s="2" t="s">
         <v>408</v>
-      </c>
-      <c r="C91" s="2" t="s">
-        <v>409</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A92" s="1" t="s">
+        <v>409</v>
+      </c>
+      <c r="B92" s="2" t="s">
         <v>410</v>
       </c>
-      <c r="B92" s="2" t="s">
+      <c r="C92" s="2" t="s">
         <v>411</v>
-      </c>
-      <c r="C92" s="2" t="s">
-        <v>412</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A93" s="1" t="s">
+        <v>412</v>
+      </c>
+      <c r="B93" s="2" t="s">
         <v>413</v>
       </c>
-      <c r="B93" s="2" t="s">
+      <c r="C93" s="2" t="s">
         <v>414</v>
-      </c>
-      <c r="C93" s="2" t="s">
-        <v>415</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A94" s="1" t="s">
+        <v>415</v>
+      </c>
+      <c r="B94" s="2" t="s">
         <v>416</v>
       </c>
-      <c r="B94" s="2" t="s">
+      <c r="C94" s="2" t="s">
         <v>417</v>
-      </c>
-      <c r="C94" s="2" t="s">
-        <v>418</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A95" s="1" t="s">
+        <v>418</v>
+      </c>
+      <c r="B95" s="2" t="s">
         <v>419</v>
       </c>
-      <c r="B95" s="2" t="s">
+      <c r="C95" s="2" t="s">
         <v>420</v>
-      </c>
-      <c r="C95" s="2" t="s">
-        <v>421</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A96" s="1" t="s">
+        <v>421</v>
+      </c>
+      <c r="B96" s="2" t="s">
         <v>422</v>
       </c>
-      <c r="B96" s="2" t="s">
+      <c r="C96" s="2" t="s">
         <v>423</v>
-      </c>
-      <c r="C96" s="2" t="s">
-        <v>424</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.35">
@@ -4017,101 +4017,101 @@
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A98" s="1" t="s">
+        <v>424</v>
+      </c>
+      <c r="B98" s="2" t="s">
         <v>425</v>
       </c>
-      <c r="B98" s="2" t="s">
+      <c r="C98" s="2" t="s">
         <v>426</v>
-      </c>
-      <c r="C98" s="2" t="s">
-        <v>427</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A99" s="1" t="s">
+        <v>427</v>
+      </c>
+      <c r="B99" s="2" t="s">
         <v>428</v>
       </c>
-      <c r="B99" s="2" t="s">
+      <c r="C99" s="2" t="s">
         <v>429</v>
-      </c>
-      <c r="C99" s="2" t="s">
-        <v>430</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A100" s="1" t="s">
+        <v>430</v>
+      </c>
+      <c r="B100" s="2" t="s">
         <v>431</v>
       </c>
-      <c r="B100" s="2" t="s">
+      <c r="C100" s="2" t="s">
         <v>432</v>
-      </c>
-      <c r="C100" s="2" t="s">
-        <v>433</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A101" s="1" t="s">
+        <v>433</v>
+      </c>
+      <c r="B101" s="2" t="s">
         <v>434</v>
       </c>
-      <c r="B101" s="2" t="s">
+      <c r="C101" s="2" t="s">
         <v>435</v>
-      </c>
-      <c r="C101" s="2" t="s">
-        <v>436</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A102" s="1" t="s">
+        <v>436</v>
+      </c>
+      <c r="B102" s="2" t="s">
         <v>437</v>
       </c>
-      <c r="B102" s="2" t="s">
+      <c r="C102" s="2" t="s">
         <v>438</v>
-      </c>
-      <c r="C102" s="2" t="s">
-        <v>439</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A103" s="1" t="s">
+        <v>439</v>
+      </c>
+      <c r="B103" s="2" t="s">
         <v>440</v>
       </c>
-      <c r="B103" s="2" t="s">
+      <c r="C103" s="2" t="s">
         <v>441</v>
-      </c>
-      <c r="C103" s="2" t="s">
-        <v>442</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A104" s="1" t="s">
+        <v>442</v>
+      </c>
+      <c r="B104" s="2" t="s">
         <v>443</v>
       </c>
-      <c r="B104" s="2" t="s">
+      <c r="C104" s="2" t="s">
         <v>444</v>
-      </c>
-      <c r="C104" s="2" t="s">
-        <v>445</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A105" s="1" t="s">
+        <v>445</v>
+      </c>
+      <c r="B105" s="2" t="s">
         <v>446</v>
       </c>
-      <c r="B105" s="2" t="s">
+      <c r="C105" s="2" t="s">
         <v>447</v>
-      </c>
-      <c r="C105" s="2" t="s">
-        <v>448</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A106" s="1" t="s">
+        <v>448</v>
+      </c>
+      <c r="B106" s="2" t="s">
         <v>449</v>
       </c>
-      <c r="B106" s="2" t="s">
+      <c r="C106" s="2" t="s">
         <v>450</v>
-      </c>
-      <c r="C106" s="2" t="s">
-        <v>451</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.35">
@@ -4120,90 +4120,90 @@
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A108" s="1" t="s">
+        <v>451</v>
+      </c>
+      <c r="B108" s="2" t="s">
         <v>452</v>
       </c>
-      <c r="B108" s="2" t="s">
+      <c r="C108" s="2" t="s">
         <v>453</v>
-      </c>
-      <c r="C108" s="2" t="s">
-        <v>454</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A109" s="1" t="s">
+        <v>454</v>
+      </c>
+      <c r="B109" s="2" t="s">
         <v>455</v>
       </c>
-      <c r="B109" s="2" t="s">
+      <c r="C109" s="2" t="s">
         <v>456</v>
-      </c>
-      <c r="C109" s="2" t="s">
-        <v>457</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A110" s="1" t="s">
+        <v>457</v>
+      </c>
+      <c r="B110" s="2" t="s">
         <v>458</v>
       </c>
-      <c r="B110" s="2" t="s">
+      <c r="C110" s="2" t="s">
         <v>459</v>
-      </c>
-      <c r="C110" s="2" t="s">
-        <v>460</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A111" s="1" t="s">
+        <v>460</v>
+      </c>
+      <c r="B111" s="2" t="s">
         <v>461</v>
       </c>
-      <c r="B111" s="2" t="s">
+      <c r="C111" s="2" t="s">
         <v>462</v>
-      </c>
-      <c r="C111" s="2" t="s">
-        <v>463</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A112" s="1" t="s">
+        <v>463</v>
+      </c>
+      <c r="B112" s="2" t="s">
         <v>464</v>
       </c>
-      <c r="B112" s="2" t="s">
+      <c r="C112" s="2" t="s">
         <v>465</v>
-      </c>
-      <c r="C112" s="2" t="s">
-        <v>466</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A113" s="1" t="s">
+        <v>466</v>
+      </c>
+      <c r="B113" s="2" t="s">
         <v>467</v>
       </c>
-      <c r="B113" s="2" t="s">
+      <c r="C113" s="2" t="s">
         <v>468</v>
-      </c>
-      <c r="C113" s="2" t="s">
-        <v>469</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A114" s="1" t="s">
+        <v>469</v>
+      </c>
+      <c r="B114" s="2" t="s">
         <v>470</v>
       </c>
-      <c r="B114" s="2" t="s">
+      <c r="C114" s="2" t="s">
         <v>471</v>
-      </c>
-      <c r="C114" s="2" t="s">
-        <v>472</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A115" s="1" t="s">
+        <v>472</v>
+      </c>
+      <c r="B115" s="2" t="s">
         <v>473</v>
       </c>
-      <c r="B115" s="2" t="s">
+      <c r="C115" s="2" t="s">
         <v>474</v>
-      </c>
-      <c r="C115" s="2" t="s">
-        <v>475</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.35">
@@ -4212,266 +4212,266 @@
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A117" s="1" t="s">
+        <v>475</v>
+      </c>
+      <c r="B117" s="2" t="s">
         <v>476</v>
       </c>
-      <c r="B117" s="2" t="s">
+      <c r="C117" s="2" t="s">
         <v>477</v>
-      </c>
-      <c r="C117" s="2" t="s">
-        <v>478</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A118" s="1" t="s">
+        <v>478</v>
+      </c>
+      <c r="B118" s="2" t="s">
         <v>479</v>
       </c>
-      <c r="B118" s="2" t="s">
+      <c r="C118" s="2" t="s">
         <v>480</v>
-      </c>
-      <c r="C118" s="2" t="s">
-        <v>481</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A119" s="1" t="s">
+        <v>481</v>
+      </c>
+      <c r="B119" s="2" t="s">
         <v>482</v>
       </c>
-      <c r="B119" s="2" t="s">
+      <c r="C119" s="2" t="s">
         <v>483</v>
-      </c>
-      <c r="C119" s="2" t="s">
-        <v>484</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A120" s="1" t="s">
+        <v>484</v>
+      </c>
+      <c r="B120" s="2" t="s">
         <v>485</v>
       </c>
-      <c r="B120" s="2" t="s">
+      <c r="C120" s="2" t="s">
         <v>486</v>
-      </c>
-      <c r="C120" s="2" t="s">
-        <v>487</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A122" s="1" t="s">
+        <v>487</v>
+      </c>
+      <c r="B122" s="2" t="s">
         <v>488</v>
       </c>
-      <c r="B122" s="2" t="s">
+      <c r="C122" s="2" t="s">
         <v>489</v>
-      </c>
-      <c r="C122" s="2" t="s">
-        <v>490</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A123" s="1" t="s">
+        <v>490</v>
+      </c>
+      <c r="B123" s="2" t="s">
         <v>491</v>
       </c>
-      <c r="B123" s="2" t="s">
+      <c r="C123" s="2" t="s">
         <v>492</v>
-      </c>
-      <c r="C123" s="2" t="s">
-        <v>493</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A124" s="1" t="s">
+        <v>493</v>
+      </c>
+      <c r="B124" s="2" t="s">
         <v>494</v>
       </c>
-      <c r="B124" s="2" t="s">
+      <c r="C124" s="2" t="s">
         <v>495</v>
-      </c>
-      <c r="C124" s="2" t="s">
-        <v>496</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A125" s="1" t="s">
+        <v>496</v>
+      </c>
+      <c r="B125" s="2" t="s">
         <v>497</v>
       </c>
-      <c r="B125" s="2" t="s">
+      <c r="C125" s="2" t="s">
         <v>498</v>
-      </c>
-      <c r="C125" s="2" t="s">
-        <v>499</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A126" s="1" t="s">
+        <v>499</v>
+      </c>
+      <c r="B126" s="2" t="s">
         <v>500</v>
       </c>
-      <c r="B126" s="2" t="s">
+      <c r="C126" s="2" t="s">
         <v>501</v>
-      </c>
-      <c r="C126" s="2" t="s">
-        <v>502</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A127" s="1" t="s">
+        <v>502</v>
+      </c>
+      <c r="B127" s="2" t="s">
         <v>503</v>
       </c>
-      <c r="B127" s="2" t="s">
+      <c r="C127" s="2" t="s">
         <v>504</v>
-      </c>
-      <c r="C127" s="2" t="s">
-        <v>505</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A128" s="1" t="s">
+        <v>505</v>
+      </c>
+      <c r="B128" s="2" t="s">
         <v>506</v>
       </c>
-      <c r="B128" s="2" t="s">
+      <c r="C128" s="2" t="s">
         <v>507</v>
-      </c>
-      <c r="C128" s="2" t="s">
-        <v>508</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A130" s="1" t="s">
+        <v>508</v>
+      </c>
+      <c r="B130" s="2" t="s">
         <v>509</v>
       </c>
-      <c r="B130" s="2" t="s">
+      <c r="C130" s="2" t="s">
         <v>510</v>
-      </c>
-      <c r="C130" s="2" t="s">
-        <v>511</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A131" s="1" t="s">
+        <v>511</v>
+      </c>
+      <c r="B131" s="2" t="s">
         <v>512</v>
       </c>
-      <c r="B131" s="2" t="s">
+      <c r="C131" s="2" t="s">
         <v>513</v>
-      </c>
-      <c r="C131" s="2" t="s">
-        <v>514</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A132" s="1" t="s">
+        <v>514</v>
+      </c>
+      <c r="B132" s="2" t="s">
         <v>515</v>
       </c>
-      <c r="B132" s="2" t="s">
+      <c r="C132" s="2" t="s">
         <v>516</v>
-      </c>
-      <c r="C132" s="2" t="s">
-        <v>517</v>
       </c>
     </row>
     <row r="133" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A133" s="1" t="s">
+        <v>517</v>
+      </c>
+      <c r="B133" s="2" t="s">
         <v>518</v>
       </c>
-      <c r="B133" s="2" t="s">
+      <c r="C133" s="2" t="s">
         <v>519</v>
-      </c>
-      <c r="C133" s="2" t="s">
-        <v>520</v>
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A134" s="1" t="s">
+        <v>520</v>
+      </c>
+      <c r="B134" s="2" t="s">
         <v>521</v>
       </c>
-      <c r="B134" s="2" t="s">
+      <c r="C134" s="2" t="s">
         <v>522</v>
-      </c>
-      <c r="C134" s="2" t="s">
-        <v>523</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A136" s="1" t="s">
+        <v>523</v>
+      </c>
+      <c r="B136" s="2" t="s">
         <v>524</v>
       </c>
-      <c r="B136" s="2" t="s">
+      <c r="C136" s="2" t="s">
         <v>525</v>
-      </c>
-      <c r="C136" s="2" t="s">
-        <v>526</v>
       </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A137" s="1" t="s">
+        <v>526</v>
+      </c>
+      <c r="B137" s="1" t="s">
         <v>527</v>
       </c>
-      <c r="B137" s="1" t="s">
+      <c r="C137" s="1" t="s">
         <v>528</v>
-      </c>
-      <c r="C137" s="1" t="s">
-        <v>529</v>
       </c>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A138" s="1" t="s">
+        <v>529</v>
+      </c>
+      <c r="B138" s="1" t="s">
         <v>530</v>
       </c>
-      <c r="B138" s="1" t="s">
+      <c r="C138" s="1" t="s">
         <v>531</v>
-      </c>
-      <c r="C138" s="1" t="s">
-        <v>532</v>
       </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A139" s="1" t="s">
+        <v>532</v>
+      </c>
+      <c r="B139" s="2" t="s">
         <v>533</v>
       </c>
-      <c r="B139" s="2" t="s">
+      <c r="C139" s="1" t="s">
         <v>534</v>
-      </c>
-      <c r="C139" s="1" t="s">
-        <v>535</v>
       </c>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A140" s="1" t="s">
+        <v>535</v>
+      </c>
+      <c r="B140" s="1" t="s">
         <v>536</v>
       </c>
-      <c r="B140" s="1" t="s">
+      <c r="C140" s="1" t="s">
         <v>537</v>
-      </c>
-      <c r="C140" s="1" t="s">
-        <v>538</v>
       </c>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A141" s="1" t="s">
+        <v>538</v>
+      </c>
+      <c r="B141" s="2" t="s">
         <v>539</v>
       </c>
-      <c r="B141" s="2" t="s">
+      <c r="C141" s="2" t="s">
         <v>540</v>
-      </c>
-      <c r="C141" s="2" t="s">
-        <v>541</v>
       </c>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A143" s="1" t="s">
+        <v>541</v>
+      </c>
+      <c r="B143" s="2" t="s">
         <v>542</v>
       </c>
-      <c r="B143" s="2" t="s">
+      <c r="C143" s="2" t="s">
         <v>543</v>
-      </c>
-      <c r="C143" s="2" t="s">
-        <v>544</v>
       </c>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A144" s="1" t="s">
+        <v>544</v>
+      </c>
+      <c r="B144" s="2" t="s">
         <v>545</v>
       </c>
-      <c r="B144" s="2" t="s">
+      <c r="C144" s="2" t="s">
         <v>546</v>
-      </c>
-      <c r="C144" s="2" t="s">
-        <v>547</v>
       </c>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.35">
@@ -4480,57 +4480,57 @@
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A146" s="1" t="s">
+        <v>547</v>
+      </c>
+      <c r="B146" s="2" t="s">
         <v>548</v>
       </c>
-      <c r="B146" s="2" t="s">
+      <c r="C146" s="2" t="s">
         <v>549</v>
-      </c>
-      <c r="C146" s="2" t="s">
-        <v>550</v>
       </c>
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A147" s="1" t="s">
+        <v>550</v>
+      </c>
+      <c r="B147" s="2" t="s">
         <v>551</v>
       </c>
-      <c r="B147" s="2" t="s">
+      <c r="C147" s="2" t="s">
         <v>552</v>
-      </c>
-      <c r="C147" s="2" t="s">
-        <v>553</v>
       </c>
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A148" s="1" t="s">
+        <v>553</v>
+      </c>
+      <c r="B148" s="2" t="s">
         <v>554</v>
       </c>
-      <c r="B148" s="2" t="s">
+      <c r="C148" s="2" t="s">
         <v>555</v>
-      </c>
-      <c r="C148" s="2" t="s">
-        <v>556</v>
       </c>
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A149" s="1" t="s">
+        <v>556</v>
+      </c>
+      <c r="B149" s="2" t="s">
         <v>557</v>
       </c>
-      <c r="B149" s="2" t="s">
+      <c r="C149" s="2" t="s">
         <v>558</v>
-      </c>
-      <c r="C149" s="2" t="s">
-        <v>559</v>
       </c>
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A150" s="1" t="s">
+        <v>559</v>
+      </c>
+      <c r="B150" s="2" t="s">
         <v>560</v>
       </c>
-      <c r="B150" s="2" t="s">
+      <c r="C150" s="2" t="s">
         <v>561</v>
-      </c>
-      <c r="C150" s="2" t="s">
-        <v>562</v>
       </c>
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.35">
@@ -4539,101 +4539,101 @@
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A152" s="1" t="s">
+        <v>562</v>
+      </c>
+      <c r="B152" s="2" t="s">
         <v>563</v>
       </c>
-      <c r="B152" s="2" t="s">
+      <c r="C152" s="2" t="s">
         <v>564</v>
-      </c>
-      <c r="C152" s="2" t="s">
-        <v>565</v>
       </c>
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A153" s="1" t="s">
+        <v>565</v>
+      </c>
+      <c r="B153" s="2" t="s">
         <v>566</v>
       </c>
-      <c r="B153" s="2" t="s">
+      <c r="C153" s="2" t="s">
         <v>567</v>
-      </c>
-      <c r="C153" s="2" t="s">
-        <v>568</v>
       </c>
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A155" s="1" t="s">
+        <v>568</v>
+      </c>
+      <c r="B155" s="1" t="s">
         <v>569</v>
       </c>
-      <c r="B155" s="1" t="s">
+      <c r="C155" s="1" t="s">
         <v>570</v>
-      </c>
-      <c r="C155" s="1" t="s">
-        <v>571</v>
       </c>
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A156" s="1" t="s">
+        <v>571</v>
+      </c>
+      <c r="B156" s="1" t="s">
         <v>572</v>
       </c>
-      <c r="B156" s="1" t="s">
+      <c r="C156" s="1" t="s">
         <v>573</v>
-      </c>
-      <c r="C156" s="1" t="s">
-        <v>574</v>
       </c>
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A157" s="1" t="s">
+        <v>574</v>
+      </c>
+      <c r="B157" s="1" t="s">
         <v>575</v>
       </c>
-      <c r="B157" s="1" t="s">
+      <c r="C157" s="1" t="s">
         <v>576</v>
-      </c>
-      <c r="C157" s="1" t="s">
-        <v>577</v>
       </c>
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A158" s="1" t="s">
+        <v>577</v>
+      </c>
+      <c r="B158" s="1" t="s">
         <v>578</v>
       </c>
-      <c r="B158" s="1" t="s">
+      <c r="C158" s="1" t="s">
         <v>579</v>
-      </c>
-      <c r="C158" s="1" t="s">
-        <v>580</v>
       </c>
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A159" s="1" t="s">
+        <v>580</v>
+      </c>
+      <c r="B159" s="2" t="s">
         <v>581</v>
       </c>
-      <c r="B159" s="2" t="s">
+      <c r="C159" s="2" t="s">
         <v>582</v>
-      </c>
-      <c r="C159" s="2" t="s">
-        <v>583</v>
       </c>
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A160" s="1" t="s">
+        <v>583</v>
+      </c>
+      <c r="B160" s="1" t="s">
         <v>584</v>
       </c>
-      <c r="B160" s="1" t="s">
+      <c r="C160" s="1" t="s">
         <v>585</v>
-      </c>
-      <c r="C160" s="1" t="s">
-        <v>586</v>
       </c>
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A161" s="1" t="s">
+        <v>586</v>
+      </c>
+      <c r="B161" s="1" t="s">
         <v>587</v>
       </c>
-      <c r="B161" s="1" t="s">
+      <c r="C161" s="1" t="s">
         <v>588</v>
-      </c>
-      <c r="C161" s="1" t="s">
-        <v>589</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Implement manipulation of Packages
</commit_message>
<xml_diff>
--- a/Config.xlsx
+++ b/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mateus.cruz\Documents\GitHub\OrchestratorManager\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DE23B65-8D72-4D9B-B07F-1D4CF63777E3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{355826F9-84D0-4DDC-9A9E-AD3954D006AA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="634" uniqueCount="591">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="673" uniqueCount="626">
   <si>
     <t>Name</t>
   </si>
@@ -56,14 +56,14 @@
     <t>TenantName</t>
   </si>
   <si>
+    <t>Default</t>
+  </si>
+  <si>
     <t>Name of the tenant to be used. 
 Sample value: Default.</t>
   </si>
   <si>
     <t>OnPremisesOrchestratorURL</t>
-  </si>
-  <si>
-    <t>https://myOrchestratorURL</t>
   </si>
   <si>
     <t>URL of the Orchestrator instance to be used. 
@@ -171,7 +171,7 @@
     <t>Core\Forms\OUFoldersPanelTemplate.html</t>
   </si>
   <si>
-    <t>Path to the template file used to generate the Organization Units Panel form.</t>
+    <t>Path to the template file used to generate the Organization Units/Folders Panel form.</t>
   </si>
   <si>
     <t>OUFoldersPanelPath</t>
@@ -180,7 +180,7 @@
     <t>Core\Forms\OUFoldersPanel.html</t>
   </si>
   <si>
-    <t>Path to the file to be used as Organization Units Panel form.</t>
+    <t>Path to the file to be used as Organization Units/Folders Panel form.</t>
   </si>
   <si>
     <t>AuthenticationPanelTemplatePath</t>
@@ -504,6 +504,30 @@
     <t>Column to which the result of the Upload Queue Items operation should be written.</t>
   </si>
   <si>
+    <t>DeletePackageResultColumn</t>
+  </si>
+  <si>
+    <t>Column to which the result of the Delete Package operation should be written.</t>
+  </si>
+  <si>
+    <t>DownloadPackageFilePathColumn</t>
+  </si>
+  <si>
+    <t>Column to which the path to the downloaded Package should be written.</t>
+  </si>
+  <si>
+    <t>DownloadPackageResultColumn</t>
+  </si>
+  <si>
+    <t>Column to which the result of the Download Package operation should be written.</t>
+  </si>
+  <si>
+    <t>UploadPackageResultColumn</t>
+  </si>
+  <si>
+    <t>Column to which the result of the Upload Package operation should be written.</t>
+  </si>
+  <si>
     <t>EN</t>
   </si>
   <si>
@@ -750,6 +774,15 @@
     <t>キュー</t>
   </si>
   <si>
+    <t>FormPackageOption</t>
+  </si>
+  <si>
+    <t>Package</t>
+  </si>
+  <si>
+    <t>パッケージ</t>
+  </si>
+  <si>
     <t>FormSubmitButton</t>
   </si>
   <si>
@@ -846,6 +879,15 @@
     <t>キュー.xlsx</t>
   </si>
   <si>
+    <t>PackageConfigFilePath</t>
+  </si>
+  <si>
+    <t>Packages.xlsx</t>
+  </si>
+  <si>
+    <t>パッケージ.xlsx</t>
+  </si>
+  <si>
     <t>GetOperationName</t>
   </si>
   <si>
@@ -963,6 +1005,24 @@
     <t>キューアイテムをアップロード</t>
   </si>
   <si>
+    <t>DownloadPackageOperationName</t>
+  </si>
+  <si>
+    <t>Dowload</t>
+  </si>
+  <si>
+    <t>ダウンロード</t>
+  </si>
+  <si>
+    <t>UploadPackageOperationName</t>
+  </si>
+  <si>
+    <t>Upload</t>
+  </si>
+  <si>
+    <t>アップロード</t>
+  </si>
+  <si>
     <t>StoppedExecution</t>
   </si>
   <si>
@@ -1170,6 +1230,15 @@
     <t>名前が指定されませんでした。</t>
   </si>
   <si>
+    <t>VersionNotSpecified</t>
+  </si>
+  <si>
+    <t>Version not specified.</t>
+  </si>
+  <si>
+    <t>バージョンが指定されませんでした。</t>
+  </si>
+  <si>
     <t>IDAndNameDoNotMatch</t>
   </si>
   <si>
@@ -1749,12 +1818,48 @@
     <t>PackageVersionNotSpecified</t>
   </si>
   <si>
-    <t>Package version not specified</t>
+    <t>Package version not specified.</t>
   </si>
   <si>
     <t>パッケージバージョンが指定されませんでした。</t>
   </si>
   <si>
+    <t>PackageFileNotFound</t>
+  </si>
+  <si>
+    <t>Package file not found.</t>
+  </si>
+  <si>
+    <t>パッケージファイルが見つかりませんでした。</t>
+  </si>
+  <si>
+    <t>PackageNotFound</t>
+  </si>
+  <si>
+    <t>Package not found.</t>
+  </si>
+  <si>
+    <t>パッケージが見つかりませんでした。</t>
+  </si>
+  <si>
+    <t>PackageVersionNotFound</t>
+  </si>
+  <si>
+    <t>The specified Package version was not found.</t>
+  </si>
+  <si>
+    <t>指定されたパッケージバージョンが見つかりませんでした。</t>
+  </si>
+  <si>
+    <t>PackageNameVersionKeyDoNotMatch</t>
+  </si>
+  <si>
+    <t>The specified Package name, version and key do not match.</t>
+  </si>
+  <si>
+    <t>指定されたパッケージ名とバージョンとキーが一致しません。</t>
+  </si>
+  <si>
     <t>UniqueReferenceInvalidOrNotSpecified</t>
   </si>
   <si>
@@ -1818,7 +1923,7 @@
     <t>キューアイテム一覧のファイルが見つかりませんでした。</t>
   </si>
   <si>
-    <t>Default</t>
+    <t>https://myOrchestratorURL</t>
   </si>
   <si>
     <t>MyAccount</t>
@@ -1902,8 +2007,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table1" displayName="Table1" ref="A1:C60" totalsRowShown="0">
-  <autoFilter ref="A1:C60" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table1" displayName="Table1" ref="A1:C64" totalsRowShown="0">
+  <autoFilter ref="A1:C64" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Name"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Value"/>
@@ -1914,8 +2019,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table13" displayName="Table13" ref="A1:C161" totalsRowShown="0">
-  <autoFilter ref="A1:C161" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table13" displayName="Table13" ref="A1:C170" totalsRowShown="0">
+  <autoFilter ref="A1:C170" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Name"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="EN"/>
@@ -2225,18 +2330,18 @@
         <v>5</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>589</v>
+        <v>6</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="58" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>8</v>
+        <v>624</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>9</v>
@@ -2258,7 +2363,7 @@
         <v>12</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>590</v>
+        <v>625</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>13</v>
@@ -2275,7 +2380,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C60"/>
+  <dimension ref="A1:C64"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -2948,6 +3053,50 @@
         <v>150</v>
       </c>
     </row>
+    <row r="61" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A61" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C61" s="2" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A62" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C62" s="2" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A63" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C63" s="2" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A64" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="C64" s="2" t="s">
+        <v>158</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B8" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
@@ -2963,7 +3112,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1927ABA9-1814-4487-9CEC-ABDCAF91481F}">
-  <dimension ref="A1:C161"/>
+  <dimension ref="A1:C170"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -2981,1659 +3130,1758 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>152</v>
+        <v>160</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>153</v>
+        <v>161</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>154</v>
+        <v>162</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>154</v>
+        <v>162</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="43.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>155</v>
+        <v>163</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>156</v>
+        <v>164</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>157</v>
+        <v>165</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>158</v>
+        <v>166</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>159</v>
+        <v>167</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>160</v>
+        <v>168</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>161</v>
+        <v>169</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>162</v>
+        <v>170</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>162</v>
+        <v>170</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
-        <v>163</v>
+        <v>171</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>164</v>
+        <v>172</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>165</v>
+        <v>173</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
-        <v>166</v>
+        <v>174</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>167</v>
+        <v>175</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>168</v>
+        <v>176</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
-        <v>169</v>
+        <v>177</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>170</v>
+        <v>178</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>171</v>
+        <v>179</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
-        <v>172</v>
+        <v>180</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>173</v>
+        <v>181</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>174</v>
+        <v>182</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
-        <v>175</v>
+        <v>183</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>176</v>
+        <v>184</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>177</v>
+        <v>185</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
-        <v>178</v>
+        <v>186</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>179</v>
+        <v>187</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>180</v>
+        <v>188</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
-        <v>181</v>
+        <v>189</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>182</v>
+        <v>190</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>183</v>
+        <v>191</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
-        <v>184</v>
+        <v>192</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>185</v>
+        <v>193</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>186</v>
+        <v>194</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
-        <v>187</v>
+        <v>195</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>188</v>
+        <v>196</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>189</v>
+        <v>197</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
-        <v>190</v>
+        <v>198</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>191</v>
+        <v>199</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>192</v>
+        <v>200</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
-        <v>193</v>
+        <v>201</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>194</v>
+        <v>202</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>195</v>
+        <v>203</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
-        <v>196</v>
+        <v>204</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>197</v>
+        <v>205</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>198</v>
+        <v>206</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
-        <v>199</v>
+        <v>207</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>200</v>
+        <v>208</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>201</v>
+        <v>209</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
-        <v>202</v>
+        <v>210</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>203</v>
+        <v>211</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>204</v>
+        <v>212</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
-        <v>205</v>
+        <v>213</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>206</v>
+        <v>214</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>207</v>
+        <v>215</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>210</v>
+        <v>218</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
-        <v>211</v>
+        <v>219</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>212</v>
+        <v>220</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>213</v>
+        <v>221</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
-        <v>214</v>
+        <v>222</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>216</v>
+        <v>224</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
-        <v>217</v>
+        <v>225</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>218</v>
+        <v>226</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>219</v>
+        <v>227</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
-        <v>220</v>
+        <v>228</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>221</v>
+        <v>229</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>222</v>
+        <v>230</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
-        <v>223</v>
+        <v>231</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>225</v>
+        <v>233</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
-        <v>226</v>
+        <v>234</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>227</v>
+        <v>235</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>198</v>
+        <v>206</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="s">
-        <v>228</v>
+        <v>236</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>229</v>
+        <v>237</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>201</v>
+        <v>209</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="s">
-        <v>230</v>
+        <v>238</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>231</v>
+        <v>239</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>232</v>
+        <v>240</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A30" s="1" t="s">
-        <v>233</v>
+        <v>241</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>234</v>
+        <v>242</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>234</v>
+        <v>243</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A31" s="1" t="s">
-        <v>235</v>
+        <v>244</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>236</v>
+        <v>245</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>237</v>
+        <v>245</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B32" s="2"/>
-      <c r="C32" s="2"/>
+      <c r="A32" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>248</v>
+      </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A33" s="1" t="s">
-        <v>238</v>
-      </c>
-      <c r="B33" s="2" t="s">
-        <v>239</v>
-      </c>
-      <c r="C33" s="2" t="s">
-        <v>240</v>
-      </c>
+      <c r="B33" s="2"/>
+      <c r="C33" s="2"/>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A34" s="1" t="s">
-        <v>241</v>
+        <v>249</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>242</v>
+        <v>250</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>243</v>
+        <v>251</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A35" s="1" t="s">
-        <v>244</v>
+        <v>252</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>245</v>
+        <v>253</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>246</v>
+        <v>254</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A36" s="1" t="s">
-        <v>247</v>
+        <v>255</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>248</v>
+        <v>256</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>249</v>
+        <v>257</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A37" s="1" t="s">
-        <v>250</v>
+        <v>258</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>251</v>
+        <v>259</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>252</v>
+        <v>260</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A38" s="1" t="s">
-        <v>253</v>
+        <v>261</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>254</v>
+        <v>262</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>255</v>
+        <v>263</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A39" s="1" t="s">
-        <v>256</v>
+        <v>264</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>257</v>
+        <v>265</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>258</v>
+        <v>266</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A40" s="1" t="s">
-        <v>259</v>
+        <v>267</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>260</v>
+        <v>268</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>261</v>
+        <v>269</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A41" s="1" t="s">
-        <v>262</v>
+        <v>270</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>263</v>
+        <v>271</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>264</v>
+        <v>272</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B42" s="2"/>
-      <c r="C42" s="2"/>
+      <c r="A42" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>274</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>275</v>
+      </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A43" s="1" t="s">
-        <v>265</v>
+        <v>276</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>266</v>
+        <v>277</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>267</v>
+        <v>278</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A44" s="1" t="s">
-        <v>268</v>
-      </c>
-      <c r="B44" s="2" t="s">
-        <v>269</v>
-      </c>
-      <c r="C44" s="2" t="s">
-        <v>270</v>
-      </c>
+      <c r="B44" s="2"/>
+      <c r="C44" s="2"/>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A45" s="1" t="s">
-        <v>271</v>
+        <v>279</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>272</v>
+        <v>280</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>273</v>
+        <v>281</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A46" s="1" t="s">
-        <v>274</v>
+        <v>282</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>275</v>
+        <v>283</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>276</v>
+        <v>284</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A47" s="1" t="s">
-        <v>277</v>
+        <v>285</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>278</v>
+        <v>286</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>279</v>
+        <v>287</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A48" s="1" t="s">
-        <v>280</v>
+        <v>288</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>281</v>
+        <v>289</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>282</v>
+        <v>290</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A49" s="1" t="s">
-        <v>283</v>
+        <v>291</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>284</v>
+        <v>292</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>285</v>
+        <v>293</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A50" s="1" t="s">
-        <v>286</v>
+        <v>294</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>287</v>
+        <v>295</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>288</v>
+        <v>296</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A51" s="1" t="s">
-        <v>289</v>
+        <v>297</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>290</v>
+        <v>298</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>291</v>
+        <v>299</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A52" s="1" t="s">
-        <v>292</v>
+        <v>300</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>293</v>
+        <v>301</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>294</v>
+        <v>302</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A53" s="1" t="s">
-        <v>295</v>
+        <v>303</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>296</v>
+        <v>304</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>297</v>
+        <v>305</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A54" s="1" t="s">
-        <v>298</v>
+        <v>306</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>299</v>
+        <v>307</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>300</v>
+        <v>308</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A55" s="1" t="s">
-        <v>301</v>
+        <v>309</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>302</v>
+        <v>310</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>303</v>
+        <v>311</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A56" s="1" t="s">
-        <v>304</v>
+        <v>312</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>305</v>
+        <v>313</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>306</v>
+        <v>314</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A57" s="1" t="s">
-        <v>307</v>
+        <v>315</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>308</v>
+        <v>316</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>309</v>
+        <v>317</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A58" s="1" t="s">
-        <v>310</v>
+        <v>318</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>311</v>
+        <v>319</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>312</v>
+        <v>320</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A59" s="1" t="s">
-        <v>313</v>
+        <v>321</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>314</v>
+        <v>322</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>315</v>
+        <v>323</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A60" s="1" t="s">
-        <v>316</v>
+        <v>324</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>317</v>
+        <v>325</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>318</v>
+        <v>326</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A61" s="1" t="s">
-        <v>319</v>
+        <v>327</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>320</v>
+        <v>328</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A62" s="1" t="s">
-        <v>322</v>
+        <v>330</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>323</v>
+        <v>331</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>324</v>
+        <v>332</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A63" s="1" t="s">
-        <v>325</v>
+        <v>333</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>326</v>
+        <v>334</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>327</v>
+        <v>335</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A64" s="1" t="s">
-        <v>328</v>
+        <v>336</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>329</v>
+        <v>337</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>330</v>
+        <v>338</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A65" s="1" t="s">
-        <v>331</v>
+        <v>339</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>332</v>
+        <v>340</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>333</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.35">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A66" s="1" t="s">
-        <v>334</v>
+        <v>342</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>335</v>
+        <v>343</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>336</v>
+        <v>344</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A67" s="1" t="s">
-        <v>337</v>
+        <v>345</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>338</v>
+        <v>346</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>339</v>
+        <v>347</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A68" s="1" t="s">
-        <v>340</v>
+        <v>348</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>341</v>
+        <v>349</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>342</v>
+        <v>350</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A69" s="1" t="s">
-        <v>343</v>
+        <v>351</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>344</v>
+        <v>352</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>345</v>
+        <v>353</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A70" s="1" t="s">
-        <v>346</v>
+        <v>354</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>347</v>
+        <v>355</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A71" s="1" t="s">
-        <v>349</v>
+        <v>357</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>350</v>
+        <v>358</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>351</v>
-      </c>
-    </row>
-    <row r="72" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A72" s="1" t="s">
-        <v>352</v>
+        <v>360</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>353</v>
+        <v>361</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>354</v>
+        <v>362</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A73" s="1" t="s">
-        <v>355</v>
+        <v>363</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>356</v>
+        <v>364</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>357</v>
+        <v>365</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A74" s="1" t="s">
-        <v>358</v>
+        <v>366</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>359</v>
+        <v>367</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.35">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A75" s="1" t="s">
-        <v>361</v>
+        <v>369</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>362</v>
+        <v>370</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.35">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A76" s="1" t="s">
-        <v>364</v>
+        <v>372</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>365</v>
+        <v>373</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>366</v>
+        <v>374</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A77" s="1" t="s">
-        <v>367</v>
+        <v>375</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>368</v>
+        <v>376</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>369</v>
+        <v>377</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A78" s="1" t="s">
-        <v>370</v>
+        <v>378</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>371</v>
+        <v>379</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>372</v>
+        <v>380</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A79" s="1" t="s">
-        <v>373</v>
+        <v>381</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>374</v>
+        <v>382</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>375</v>
+        <v>383</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A80" s="1" t="s">
-        <v>376</v>
+        <v>384</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>377</v>
+        <v>385</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>378</v>
+        <v>386</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A81" s="1" t="s">
-        <v>379</v>
+        <v>387</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>380</v>
+        <v>388</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>381</v>
+        <v>389</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A82" s="1" t="s">
-        <v>382</v>
+        <v>390</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>383</v>
+        <v>391</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>384</v>
+        <v>392</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A83" s="1" t="s">
-        <v>385</v>
+        <v>393</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>386</v>
+        <v>394</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>387</v>
+        <v>395</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A84" s="1" t="s">
-        <v>388</v>
+        <v>396</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>389</v>
+        <v>397</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>390</v>
+        <v>398</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A85" s="1" t="s">
-        <v>391</v>
+        <v>399</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>392</v>
+        <v>400</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>393</v>
+        <v>401</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A86" s="1" t="s">
-        <v>394</v>
+        <v>402</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>395</v>
+        <v>403</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>396</v>
+        <v>404</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A87" s="1" t="s">
-        <v>397</v>
+        <v>405</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>398</v>
+        <v>406</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>399</v>
+        <v>407</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B88" s="2"/>
-      <c r="C88" s="2"/>
+      <c r="A88" s="1" t="s">
+        <v>408</v>
+      </c>
+      <c r="B88" s="2" t="s">
+        <v>409</v>
+      </c>
+      <c r="C88" s="2" t="s">
+        <v>410</v>
+      </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A89" s="1" t="s">
-        <v>400</v>
+        <v>411</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>401</v>
+        <v>412</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>402</v>
+        <v>413</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A90" s="1" t="s">
-        <v>403</v>
+        <v>414</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>404</v>
+        <v>415</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>405</v>
+        <v>416</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A91" s="1" t="s">
-        <v>406</v>
+        <v>417</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>407</v>
+        <v>418</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>408</v>
+        <v>419</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A92" s="1" t="s">
-        <v>409</v>
+        <v>420</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>410</v>
+        <v>421</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>411</v>
+        <v>422</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A93" s="1" t="s">
-        <v>412</v>
-      </c>
-      <c r="B93" s="2" t="s">
-        <v>413</v>
-      </c>
-      <c r="C93" s="2" t="s">
-        <v>414</v>
-      </c>
+      <c r="B93" s="2"/>
+      <c r="C93" s="2"/>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A94" s="1" t="s">
-        <v>415</v>
+        <v>423</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>416</v>
+        <v>424</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>417</v>
+        <v>425</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A95" s="1" t="s">
-        <v>418</v>
+        <v>426</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>419</v>
+        <v>427</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>420</v>
+        <v>428</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A96" s="1" t="s">
-        <v>421</v>
+        <v>429</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>422</v>
+        <v>430</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>423</v>
+        <v>431</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B97" s="2"/>
-      <c r="C97" s="2"/>
+      <c r="A97" s="1" t="s">
+        <v>432</v>
+      </c>
+      <c r="B97" s="2" t="s">
+        <v>433</v>
+      </c>
+      <c r="C97" s="2" t="s">
+        <v>434</v>
+      </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A98" s="1" t="s">
-        <v>424</v>
+        <v>435</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>425</v>
+        <v>436</v>
       </c>
       <c r="C98" s="2" t="s">
-        <v>426</v>
+        <v>437</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A99" s="1" t="s">
-        <v>427</v>
+        <v>438</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>428</v>
+        <v>439</v>
       </c>
       <c r="C99" s="2" t="s">
-        <v>429</v>
+        <v>440</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A100" s="1" t="s">
-        <v>430</v>
+        <v>441</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>431</v>
+        <v>442</v>
       </c>
       <c r="C100" s="2" t="s">
-        <v>432</v>
+        <v>443</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A101" s="1" t="s">
-        <v>433</v>
+        <v>444</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>434</v>
+        <v>445</v>
       </c>
       <c r="C101" s="2" t="s">
-        <v>435</v>
+        <v>446</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A102" s="1" t="s">
-        <v>436</v>
-      </c>
-      <c r="B102" s="2" t="s">
-        <v>437</v>
-      </c>
-      <c r="C102" s="2" t="s">
-        <v>438</v>
-      </c>
+      <c r="B102" s="2"/>
+      <c r="C102" s="2"/>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A103" s="1" t="s">
-        <v>439</v>
+        <v>447</v>
       </c>
       <c r="B103" s="2" t="s">
-        <v>440</v>
+        <v>448</v>
       </c>
       <c r="C103" s="2" t="s">
-        <v>441</v>
+        <v>449</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A104" s="1" t="s">
-        <v>442</v>
+        <v>450</v>
       </c>
       <c r="B104" s="2" t="s">
-        <v>443</v>
+        <v>451</v>
       </c>
       <c r="C104" s="2" t="s">
-        <v>444</v>
+        <v>452</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A105" s="1" t="s">
-        <v>445</v>
+        <v>453</v>
       </c>
       <c r="B105" s="2" t="s">
-        <v>446</v>
+        <v>454</v>
       </c>
       <c r="C105" s="2" t="s">
-        <v>447</v>
+        <v>455</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A106" s="1" t="s">
-        <v>448</v>
+        <v>456</v>
       </c>
       <c r="B106" s="2" t="s">
-        <v>449</v>
+        <v>457</v>
       </c>
       <c r="C106" s="2" t="s">
-        <v>450</v>
+        <v>458</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B107" s="2"/>
-      <c r="C107" s="2"/>
+      <c r="A107" s="1" t="s">
+        <v>459</v>
+      </c>
+      <c r="B107" s="2" t="s">
+        <v>460</v>
+      </c>
+      <c r="C107" s="2" t="s">
+        <v>461</v>
+      </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A108" s="1" t="s">
-        <v>451</v>
+        <v>462</v>
       </c>
       <c r="B108" s="2" t="s">
-        <v>452</v>
+        <v>463</v>
       </c>
       <c r="C108" s="2" t="s">
-        <v>453</v>
+        <v>464</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A109" s="1" t="s">
-        <v>454</v>
+        <v>465</v>
       </c>
       <c r="B109" s="2" t="s">
-        <v>455</v>
+        <v>466</v>
       </c>
       <c r="C109" s="2" t="s">
-        <v>456</v>
+        <v>467</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A110" s="1" t="s">
-        <v>457</v>
+        <v>468</v>
       </c>
       <c r="B110" s="2" t="s">
-        <v>458</v>
+        <v>469</v>
       </c>
       <c r="C110" s="2" t="s">
-        <v>459</v>
+        <v>470</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A111" s="1" t="s">
-        <v>460</v>
+        <v>471</v>
       </c>
       <c r="B111" s="2" t="s">
-        <v>461</v>
+        <v>472</v>
       </c>
       <c r="C111" s="2" t="s">
-        <v>462</v>
+        <v>473</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A112" s="1" t="s">
-        <v>463</v>
-      </c>
-      <c r="B112" s="2" t="s">
-        <v>464</v>
-      </c>
-      <c r="C112" s="2" t="s">
-        <v>465</v>
-      </c>
+      <c r="B112" s="2"/>
+      <c r="C112" s="2"/>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A113" s="1" t="s">
-        <v>466</v>
+        <v>474</v>
       </c>
       <c r="B113" s="2" t="s">
-        <v>467</v>
+        <v>475</v>
       </c>
       <c r="C113" s="2" t="s">
-        <v>468</v>
+        <v>476</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A114" s="1" t="s">
-        <v>469</v>
+        <v>477</v>
       </c>
       <c r="B114" s="2" t="s">
-        <v>470</v>
+        <v>478</v>
       </c>
       <c r="C114" s="2" t="s">
-        <v>471</v>
+        <v>479</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A115" s="1" t="s">
-        <v>472</v>
+        <v>480</v>
       </c>
       <c r="B115" s="2" t="s">
-        <v>473</v>
+        <v>481</v>
       </c>
       <c r="C115" s="2" t="s">
-        <v>474</v>
+        <v>482</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B116" s="2"/>
-      <c r="C116" s="2"/>
+      <c r="A116" s="1" t="s">
+        <v>483</v>
+      </c>
+      <c r="B116" s="2" t="s">
+        <v>484</v>
+      </c>
+      <c r="C116" s="2" t="s">
+        <v>485</v>
+      </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A117" s="1" t="s">
-        <v>475</v>
+        <v>486</v>
       </c>
       <c r="B117" s="2" t="s">
-        <v>476</v>
+        <v>487</v>
       </c>
       <c r="C117" s="2" t="s">
-        <v>477</v>
+        <v>488</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A118" s="1" t="s">
-        <v>478</v>
+        <v>489</v>
       </c>
       <c r="B118" s="2" t="s">
-        <v>479</v>
+        <v>490</v>
       </c>
       <c r="C118" s="2" t="s">
-        <v>480</v>
+        <v>491</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A119" s="1" t="s">
-        <v>481</v>
+        <v>492</v>
       </c>
       <c r="B119" s="2" t="s">
-        <v>482</v>
+        <v>493</v>
       </c>
       <c r="C119" s="2" t="s">
-        <v>483</v>
+        <v>494</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A120" s="1" t="s">
-        <v>484</v>
+        <v>495</v>
       </c>
       <c r="B120" s="2" t="s">
-        <v>485</v>
+        <v>496</v>
       </c>
       <c r="C120" s="2" t="s">
-        <v>486</v>
-      </c>
+        <v>497</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B121" s="2"/>
+      <c r="C121" s="2"/>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A122" s="1" t="s">
-        <v>487</v>
+        <v>498</v>
       </c>
       <c r="B122" s="2" t="s">
-        <v>488</v>
+        <v>499</v>
       </c>
       <c r="C122" s="2" t="s">
-        <v>489</v>
+        <v>500</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A123" s="1" t="s">
-        <v>490</v>
+        <v>501</v>
       </c>
       <c r="B123" s="2" t="s">
-        <v>491</v>
+        <v>502</v>
       </c>
       <c r="C123" s="2" t="s">
-        <v>492</v>
+        <v>503</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A124" s="1" t="s">
-        <v>493</v>
+        <v>504</v>
       </c>
       <c r="B124" s="2" t="s">
-        <v>494</v>
+        <v>505</v>
       </c>
       <c r="C124" s="2" t="s">
-        <v>495</v>
+        <v>506</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A125" s="1" t="s">
-        <v>496</v>
+        <v>507</v>
       </c>
       <c r="B125" s="2" t="s">
-        <v>497</v>
+        <v>508</v>
       </c>
       <c r="C125" s="2" t="s">
-        <v>498</v>
-      </c>
-    </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A126" s="1" t="s">
-        <v>499</v>
-      </c>
-      <c r="B126" s="2" t="s">
-        <v>500</v>
-      </c>
-      <c r="C126" s="2" t="s">
-        <v>501</v>
+        <v>509</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A127" s="1" t="s">
-        <v>502</v>
+        <v>510</v>
       </c>
       <c r="B127" s="2" t="s">
-        <v>503</v>
+        <v>511</v>
       </c>
       <c r="C127" s="2" t="s">
-        <v>504</v>
+        <v>512</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A128" s="1" t="s">
-        <v>505</v>
+        <v>513</v>
       </c>
       <c r="B128" s="2" t="s">
-        <v>506</v>
+        <v>514</v>
       </c>
       <c r="C128" s="2" t="s">
-        <v>507</v>
+        <v>515</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A129" s="1" t="s">
+        <v>516</v>
+      </c>
+      <c r="B129" s="2" t="s">
+        <v>517</v>
+      </c>
+      <c r="C129" s="2" t="s">
+        <v>518</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A130" s="1" t="s">
-        <v>508</v>
+        <v>519</v>
       </c>
       <c r="B130" s="2" t="s">
-        <v>509</v>
+        <v>520</v>
       </c>
       <c r="C130" s="2" t="s">
-        <v>510</v>
+        <v>521</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A131" s="1" t="s">
-        <v>511</v>
+        <v>522</v>
       </c>
       <c r="B131" s="2" t="s">
-        <v>512</v>
+        <v>523</v>
       </c>
       <c r="C131" s="2" t="s">
-        <v>513</v>
+        <v>524</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A132" s="1" t="s">
-        <v>514</v>
+        <v>525</v>
       </c>
       <c r="B132" s="2" t="s">
-        <v>515</v>
+        <v>526</v>
       </c>
       <c r="C132" s="2" t="s">
-        <v>516</v>
-      </c>
-    </row>
-    <row r="133" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A133" s="1" t="s">
-        <v>517</v>
+        <v>528</v>
       </c>
       <c r="B133" s="2" t="s">
-        <v>518</v>
+        <v>529</v>
       </c>
       <c r="C133" s="2" t="s">
-        <v>519</v>
-      </c>
-    </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A134" s="1" t="s">
-        <v>520</v>
-      </c>
-      <c r="B134" s="2" t="s">
-        <v>521</v>
-      </c>
-      <c r="C134" s="2" t="s">
-        <v>522</v>
+        <v>530</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A135" s="1" t="s">
+        <v>531</v>
+      </c>
+      <c r="B135" s="2" t="s">
+        <v>532</v>
+      </c>
+      <c r="C135" s="2" t="s">
+        <v>533</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A136" s="1" t="s">
-        <v>523</v>
+        <v>534</v>
       </c>
       <c r="B136" s="2" t="s">
-        <v>524</v>
+        <v>535</v>
       </c>
       <c r="C136" s="2" t="s">
-        <v>525</v>
+        <v>536</v>
       </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A137" s="1" t="s">
-        <v>526</v>
-      </c>
-      <c r="B137" s="1" t="s">
-        <v>527</v>
-      </c>
-      <c r="C137" s="1" t="s">
-        <v>528</v>
-      </c>
-    </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.35">
+        <v>537</v>
+      </c>
+      <c r="B137" s="2" t="s">
+        <v>538</v>
+      </c>
+      <c r="C137" s="2" t="s">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A138" s="1" t="s">
-        <v>529</v>
-      </c>
-      <c r="B138" s="1" t="s">
-        <v>530</v>
-      </c>
-      <c r="C138" s="1" t="s">
-        <v>531</v>
+        <v>540</v>
+      </c>
+      <c r="B138" s="2" t="s">
+        <v>541</v>
+      </c>
+      <c r="C138" s="2" t="s">
+        <v>542</v>
       </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A139" s="1" t="s">
-        <v>532</v>
+        <v>543</v>
       </c>
       <c r="B139" s="2" t="s">
-        <v>533</v>
-      </c>
-      <c r="C139" s="1" t="s">
-        <v>534</v>
-      </c>
-    </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A140" s="1" t="s">
-        <v>535</v>
-      </c>
-      <c r="B140" s="1" t="s">
-        <v>536</v>
-      </c>
-      <c r="C140" s="1" t="s">
-        <v>537</v>
+        <v>544</v>
+      </c>
+      <c r="C139" s="2" t="s">
+        <v>545</v>
       </c>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A141" s="1" t="s">
-        <v>538</v>
+        <v>546</v>
       </c>
       <c r="B141" s="2" t="s">
-        <v>539</v>
+        <v>547</v>
       </c>
       <c r="C141" s="2" t="s">
-        <v>540</v>
+        <v>548</v>
+      </c>
+    </row>
+    <row r="142" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A142" s="1" t="s">
+        <v>549</v>
+      </c>
+      <c r="B142" s="1" t="s">
+        <v>550</v>
+      </c>
+      <c r="C142" s="1" t="s">
+        <v>551</v>
       </c>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A143" s="1" t="s">
-        <v>541</v>
-      </c>
-      <c r="B143" s="2" t="s">
-        <v>542</v>
-      </c>
-      <c r="C143" s="2" t="s">
-        <v>543</v>
+        <v>552</v>
+      </c>
+      <c r="B143" s="1" t="s">
+        <v>553</v>
+      </c>
+      <c r="C143" s="1" t="s">
+        <v>554</v>
       </c>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A144" s="1" t="s">
-        <v>544</v>
+        <v>555</v>
       </c>
       <c r="B144" s="2" t="s">
-        <v>545</v>
-      </c>
-      <c r="C144" s="2" t="s">
-        <v>546</v>
+        <v>556</v>
+      </c>
+      <c r="C144" s="1" t="s">
+        <v>557</v>
       </c>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B145" s="2"/>
-      <c r="C145" s="2"/>
+      <c r="A145" s="1" t="s">
+        <v>558</v>
+      </c>
+      <c r="B145" s="1" t="s">
+        <v>559</v>
+      </c>
+      <c r="C145" s="1" t="s">
+        <v>560</v>
+      </c>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A146" s="1" t="s">
-        <v>547</v>
+        <v>561</v>
       </c>
       <c r="B146" s="2" t="s">
-        <v>548</v>
+        <v>562</v>
       </c>
       <c r="C146" s="2" t="s">
-        <v>549</v>
-      </c>
-    </row>
-    <row r="147" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A147" s="1" t="s">
-        <v>550</v>
-      </c>
-      <c r="B147" s="2" t="s">
-        <v>551</v>
-      </c>
-      <c r="C147" s="2" t="s">
-        <v>552</v>
+        <v>563</v>
       </c>
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A148" s="1" t="s">
-        <v>553</v>
+        <v>564</v>
       </c>
       <c r="B148" s="2" t="s">
-        <v>554</v>
+        <v>565</v>
       </c>
       <c r="C148" s="2" t="s">
-        <v>555</v>
+        <v>566</v>
       </c>
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A149" s="1" t="s">
-        <v>556</v>
+        <v>567</v>
       </c>
       <c r="B149" s="2" t="s">
-        <v>557</v>
+        <v>568</v>
       </c>
       <c r="C149" s="2" t="s">
-        <v>558</v>
+        <v>569</v>
       </c>
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A150" s="1" t="s">
-        <v>559</v>
-      </c>
-      <c r="B150" s="2" t="s">
-        <v>560</v>
-      </c>
-      <c r="C150" s="2" t="s">
-        <v>561</v>
-      </c>
+      <c r="B150" s="2"/>
+      <c r="C150" s="2"/>
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B151" s="2"/>
-      <c r="C151" s="2"/>
+      <c r="A151" s="1" t="s">
+        <v>570</v>
+      </c>
+      <c r="B151" s="2" t="s">
+        <v>571</v>
+      </c>
+      <c r="C151" s="2" t="s">
+        <v>572</v>
+      </c>
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A152" s="1" t="s">
-        <v>562</v>
+        <v>573</v>
       </c>
       <c r="B152" s="2" t="s">
-        <v>563</v>
+        <v>574</v>
       </c>
       <c r="C152" s="2" t="s">
-        <v>564</v>
+        <v>575</v>
       </c>
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A153" s="1" t="s">
-        <v>565</v>
+        <v>576</v>
       </c>
       <c r="B153" s="2" t="s">
-        <v>566</v>
+        <v>577</v>
       </c>
       <c r="C153" s="2" t="s">
-        <v>567</v>
+        <v>578</v>
+      </c>
+    </row>
+    <row r="154" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A154" s="1" t="s">
+        <v>579</v>
+      </c>
+      <c r="B154" s="2" t="s">
+        <v>580</v>
+      </c>
+      <c r="C154" s="2" t="s">
+        <v>581</v>
       </c>
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A155" s="1" t="s">
-        <v>568</v>
-      </c>
-      <c r="B155" s="1" t="s">
-        <v>569</v>
-      </c>
-      <c r="C155" s="1" t="s">
-        <v>570</v>
+        <v>582</v>
+      </c>
+      <c r="B155" s="2" t="s">
+        <v>583</v>
+      </c>
+      <c r="C155" s="2" t="s">
+        <v>584</v>
       </c>
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A156" s="1" t="s">
-        <v>571</v>
-      </c>
-      <c r="B156" s="1" t="s">
-        <v>572</v>
-      </c>
-      <c r="C156" s="1" t="s">
-        <v>573</v>
-      </c>
+      <c r="B156" s="2"/>
+      <c r="C156" s="2"/>
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A157" s="1" t="s">
-        <v>574</v>
-      </c>
-      <c r="B157" s="1" t="s">
-        <v>575</v>
-      </c>
-      <c r="C157" s="1" t="s">
-        <v>576</v>
+        <v>585</v>
+      </c>
+      <c r="B157" s="2" t="s">
+        <v>586</v>
+      </c>
+      <c r="C157" s="2" t="s">
+        <v>587</v>
       </c>
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A158" s="1" t="s">
-        <v>577</v>
-      </c>
-      <c r="B158" s="1" t="s">
-        <v>578</v>
-      </c>
-      <c r="C158" s="1" t="s">
-        <v>579</v>
+        <v>588</v>
+      </c>
+      <c r="B158" s="2" t="s">
+        <v>589</v>
+      </c>
+      <c r="C158" s="2" t="s">
+        <v>590</v>
       </c>
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A159" s="1" t="s">
-        <v>580</v>
+        <v>591</v>
       </c>
       <c r="B159" s="2" t="s">
-        <v>581</v>
+        <v>592</v>
       </c>
       <c r="C159" s="2" t="s">
-        <v>582</v>
+        <v>593</v>
       </c>
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A160" s="1" t="s">
-        <v>583</v>
-      </c>
-      <c r="B160" s="1" t="s">
-        <v>584</v>
-      </c>
-      <c r="C160" s="1" t="s">
-        <v>585</v>
+        <v>594</v>
+      </c>
+      <c r="B160" s="2" t="s">
+        <v>595</v>
+      </c>
+      <c r="C160" s="2" t="s">
+        <v>596</v>
       </c>
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A161" s="1" t="s">
-        <v>586</v>
-      </c>
-      <c r="B161" s="1" t="s">
-        <v>587</v>
-      </c>
-      <c r="C161" s="1" t="s">
-        <v>588</v>
+        <v>597</v>
+      </c>
+      <c r="B161" s="2" t="s">
+        <v>598</v>
+      </c>
+      <c r="C161" s="2" t="s">
+        <v>599</v>
+      </c>
+    </row>
+    <row r="162" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A162" s="1" t="s">
+        <v>600</v>
+      </c>
+      <c r="B162" s="2" t="s">
+        <v>601</v>
+      </c>
+      <c r="C162" s="2" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="164" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A164" s="1" t="s">
+        <v>603</v>
+      </c>
+      <c r="B164" s="1" t="s">
+        <v>604</v>
+      </c>
+      <c r="C164" s="1" t="s">
+        <v>605</v>
+      </c>
+    </row>
+    <row r="165" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A165" s="1" t="s">
+        <v>606</v>
+      </c>
+      <c r="B165" s="1" t="s">
+        <v>607</v>
+      </c>
+      <c r="C165" s="1" t="s">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="166" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A166" s="1" t="s">
+        <v>609</v>
+      </c>
+      <c r="B166" s="1" t="s">
+        <v>610</v>
+      </c>
+      <c r="C166" s="1" t="s">
+        <v>611</v>
+      </c>
+    </row>
+    <row r="167" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A167" s="1" t="s">
+        <v>612</v>
+      </c>
+      <c r="B167" s="1" t="s">
+        <v>613</v>
+      </c>
+      <c r="C167" s="1" t="s">
+        <v>614</v>
+      </c>
+    </row>
+    <row r="168" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A168" s="1" t="s">
+        <v>615</v>
+      </c>
+      <c r="B168" s="2" t="s">
+        <v>616</v>
+      </c>
+      <c r="C168" s="2" t="s">
+        <v>617</v>
+      </c>
+    </row>
+    <row r="169" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A169" s="1" t="s">
+        <v>618</v>
+      </c>
+      <c r="B169" s="1" t="s">
+        <v>619</v>
+      </c>
+      <c r="C169" s="1" t="s">
+        <v>620</v>
+      </c>
+    </row>
+    <row r="170" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A170" s="1" t="s">
+        <v>621</v>
+      </c>
+      <c r="B170" s="1" t="s">
+        <v>622</v>
+      </c>
+      <c r="C170" s="1" t="s">
+        <v>623</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Unify workbooks using OUs and using Folders
</commit_message>
<xml_diff>
--- a/Config.xlsx
+++ b/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mateus.cruz\Documents\GitHub\OrchestratorManager\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{355826F9-84D0-4DDC-9A9E-AD3954D006AA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{126847A3-A5C0-4FB7-B26E-74DBB35C1CC5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="673" uniqueCount="626">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="670" uniqueCount="623">
   <si>
     <t>Name</t>
   </si>
@@ -201,22 +201,13 @@
     <t>Path to the file to be used as Authentication Panel form.</t>
   </si>
   <si>
-    <t>WorkbooksUsingOUsPath</t>
-  </si>
-  <si>
-    <t>Workbooks\UsingOUs</t>
-  </si>
-  <si>
-    <t>Path to the folder containing templates of entities workbooks that use Organization Units.</t>
-  </si>
-  <si>
-    <t>WorkbooksUsingFoldersPath</t>
-  </si>
-  <si>
-    <t>Workbooks\UsingFolders</t>
-  </si>
-  <si>
-    <t>Path to the folder containing templates of entities workbooks that use Folders.</t>
+    <t>WorkbooksTemplatesPath</t>
+  </si>
+  <si>
+    <t>Workbooks</t>
+  </si>
+  <si>
+    <t>Path to the folder containing templates of entities workbooks.</t>
   </si>
   <si>
     <t>CloudCredentialName</t>
@@ -2007,8 +1998,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table1" displayName="Table1" ref="A1:C64" totalsRowShown="0">
-  <autoFilter ref="A1:C64" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table1" displayName="Table1" ref="A1:C63" totalsRowShown="0">
+  <autoFilter ref="A1:C63" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Name"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Value"/>
@@ -2341,7 +2332,7 @@
         <v>8</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>624</v>
+        <v>621</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>9</v>
@@ -2363,7 +2354,7 @@
         <v>12</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>625</v>
+        <v>622</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>13</v>
@@ -2380,10 +2371,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C64"/>
+  <dimension ref="A1:C63"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A2" sqref="A2 A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2558,7 +2549,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>50</v>
       </c>
@@ -2613,7 +2604,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
         <v>65</v>
       </c>
@@ -2629,101 +2620,101 @@
         <v>68</v>
       </c>
       <c r="B22" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C22" s="2" t="s">
         <v>69</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C23" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="B23" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="C23" s="2" t="s">
+    </row>
+    <row r="24" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="1" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A24" s="1" t="s">
+      <c r="B24" s="1" t="s">
         <v>73</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>63</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
         <v>75</v>
       </c>
       <c r="B25" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="C25" s="2" t="s">
+      <c r="B26" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C26" s="2" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A26" s="1" t="s">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A27" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="B26" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="1" t="s">
+      <c r="B27" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C27" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="B27" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="C27" s="2" t="s">
+    </row>
+    <row r="28" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="1" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A28" s="1" t="s">
+      <c r="B28" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C28" s="2" t="s">
         <v>81</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C29" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="B29" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="C29" s="2" t="s">
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A30" s="1" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="1" t="s">
+      <c r="B30" s="1" t="s">
         <v>85</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>63</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" s="1" t="s">
         <v>87</v>
       </c>
@@ -2739,362 +2730,351 @@
         <v>90</v>
       </c>
       <c r="B32" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C32" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="C32" s="2" t="s">
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A33" s="1" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="1" t="s">
+      <c r="B33" s="1" t="s">
         <v>93</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>66</v>
       </c>
       <c r="C33" s="2" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A34" s="1" t="s">
         <v>95</v>
       </c>
       <c r="B34" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C34" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="C34" s="2" t="s">
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A35" s="1" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="1" t="s">
+      <c r="B35" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C35" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="B35" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="C35" s="2" t="s">
+    </row>
+    <row r="36" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A36" s="1" t="s">
         <v>99</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A36" s="1" t="s">
-        <v>100</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>88</v>
       </c>
       <c r="C36" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A37" s="1" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="1" t="s">
+      <c r="B37" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C37" s="2" t="s">
         <v>102</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="C37" s="2" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A38" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C38" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="B38" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="C38" s="2" t="s">
+    </row>
+    <row r="39" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A39" s="1" t="s">
         <v>105</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A39" s="1" t="s">
-        <v>106</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>66</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A40" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C40" s="2" t="s">
         <v>108</v>
-      </c>
-      <c r="B40" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="C40" s="2" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="41" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A41" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C41" s="2" t="s">
         <v>110</v>
-      </c>
-      <c r="B41" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="C41" s="2" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="42" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A42" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C42" s="2" t="s">
         <v>112</v>
-      </c>
-      <c r="B42" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="C42" s="2" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="43" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A43" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C43" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="B43" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="C43" s="2" t="s">
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A44" s="1" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="44" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A44" s="1" t="s">
+      <c r="B44" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C44" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="B44" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="C44" s="2" t="s">
+    </row>
+    <row r="45" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A45" s="1" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A45" s="1" t="s">
+      <c r="B45" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C45" s="2" t="s">
         <v>118</v>
-      </c>
-      <c r="B45" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="C45" s="2" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="46" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A46" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C46" s="2" t="s">
         <v>120</v>
-      </c>
-      <c r="B46" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="C46" s="2" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="47" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A47" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B47" s="1" t="s">
         <v>63</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="48" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A48" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C48" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="B48" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="C48" s="2" t="s">
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A49" s="1" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="49" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A49" s="1" t="s">
+      <c r="B49" s="1" t="s">
         <v>126</v>
-      </c>
-      <c r="B49" s="1" t="s">
-        <v>66</v>
       </c>
       <c r="C49" s="2" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A50" s="1" t="s">
         <v>128</v>
       </c>
       <c r="B50" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C50" s="2" t="s">
         <v>129</v>
-      </c>
-      <c r="C50" s="2" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="51" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A51" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C51" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="B51" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="C51" s="2" t="s">
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A52" s="1" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="52" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A52" s="1" t="s">
+      <c r="B52" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C52" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="B52" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="C52" s="2" t="s">
+    </row>
+    <row r="53" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A53" s="1" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A53" s="1" t="s">
+      <c r="B53" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C53" s="2" t="s">
         <v>135</v>
-      </c>
-      <c r="B53" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="C53" s="2" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="54" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A54" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C54" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="B54" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="C54" s="2" t="s">
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A55" s="1" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="55" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A55" s="1" t="s">
+      <c r="B55" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C55" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="B55" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="C55" s="2" t="s">
+    </row>
+    <row r="56" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A56" s="1" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A56" s="1" t="s">
+      <c r="B56" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C56" s="2" t="s">
         <v>141</v>
-      </c>
-      <c r="B56" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="C56" s="2" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="57" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A57" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C57" s="2" t="s">
         <v>143</v>
-      </c>
-      <c r="B57" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="C57" s="2" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="58" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A58" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C58" s="2" t="s">
         <v>145</v>
-      </c>
-      <c r="B58" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="C58" s="2" t="s">
-        <v>146</v>
       </c>
     </row>
     <row r="59" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A59" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C59" s="2" t="s">
         <v>147</v>
-      </c>
-      <c r="B59" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="C59" s="2" t="s">
-        <v>148</v>
       </c>
     </row>
     <row r="60" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A60" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C60" s="2" t="s">
         <v>149</v>
-      </c>
-      <c r="B60" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="C60" s="2" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="61" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A61" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C61" s="2" t="s">
         <v>151</v>
-      </c>
-      <c r="B61" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="C61" s="2" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="62" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A62" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C62" s="2" t="s">
         <v>153</v>
-      </c>
-      <c r="B62" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="C62" s="2" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="63" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A63" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="C63" s="2" t="s">
         <v>155</v>
-      </c>
-      <c r="B63" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="C63" s="2" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A64" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="B64" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="C64" s="2" t="s">
-        <v>158</v>
       </c>
     </row>
   </sheetData>
@@ -3115,7 +3095,7 @@
   <dimension ref="A1:C170"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A2" sqref="A2 A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3130,351 +3110,351 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="43.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A30" s="1" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A31" s="1" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A32" s="1" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.35">
@@ -3483,112 +3463,112 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A34" s="1" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A35" s="1" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A36" s="1" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A37" s="1" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A38" s="1" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A39" s="1" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A40" s="1" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A41" s="1" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A42" s="1" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A43" s="1" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.35">
@@ -3597,530 +3577,530 @@
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A45" s="1" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A46" s="1" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A47" s="1" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A48" s="1" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A49" s="1" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A50" s="1" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A51" s="1" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A52" s="1" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A53" s="1" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A54" s="1" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A55" s="1" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A56" s="1" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A57" s="1" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A58" s="1" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A59" s="1" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A60" s="1" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A61" s="1" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A62" s="1" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A63" s="1" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A64" s="1" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A65" s="1" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
     </row>
     <row r="66" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A66" s="1" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A67" s="1" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A68" s="1" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A69" s="1" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A70" s="1" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A71" s="1" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A72" s="1" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A73" s="1" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A74" s="1" t="s">
-        <v>366</v>
+        <v>363</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
     </row>
     <row r="75" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A75" s="1" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
     </row>
     <row r="76" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A76" s="1" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A77" s="1" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A78" s="1" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A79" s="1" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A80" s="1" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A81" s="1" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A82" s="1" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A83" s="1" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A84" s="1" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>397</v>
+        <v>394</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A85" s="1" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>401</v>
+        <v>398</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A86" s="1" t="s">
-        <v>402</v>
+        <v>399</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A87" s="1" t="s">
-        <v>405</v>
+        <v>402</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A88" s="1" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>409</v>
+        <v>406</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A89" s="1" t="s">
-        <v>411</v>
+        <v>408</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>412</v>
+        <v>409</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>413</v>
+        <v>410</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A90" s="1" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>416</v>
+        <v>413</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A91" s="1" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A92" s="1" t="s">
-        <v>420</v>
+        <v>417</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>421</v>
+        <v>418</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>422</v>
+        <v>419</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.35">
@@ -4129,90 +4109,90 @@
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A94" s="1" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>424</v>
+        <v>421</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>425</v>
+        <v>422</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A95" s="1" t="s">
-        <v>426</v>
+        <v>423</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>427</v>
+        <v>424</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>428</v>
+        <v>425</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A96" s="1" t="s">
-        <v>429</v>
+        <v>426</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>430</v>
+        <v>427</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>431</v>
+        <v>428</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A97" s="1" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="C97" s="2" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A98" s="1" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="C98" s="2" t="s">
-        <v>437</v>
+        <v>434</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A99" s="1" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>439</v>
+        <v>436</v>
       </c>
       <c r="C99" s="2" t="s">
-        <v>440</v>
+        <v>437</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A100" s="1" t="s">
-        <v>441</v>
+        <v>438</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>442</v>
+        <v>439</v>
       </c>
       <c r="C100" s="2" t="s">
-        <v>443</v>
+        <v>440</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A101" s="1" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>445</v>
+        <v>442</v>
       </c>
       <c r="C101" s="2" t="s">
-        <v>446</v>
+        <v>443</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.35">
@@ -4221,101 +4201,101 @@
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A103" s="1" t="s">
-        <v>447</v>
+        <v>444</v>
       </c>
       <c r="B103" s="2" t="s">
-        <v>448</v>
+        <v>445</v>
       </c>
       <c r="C103" s="2" t="s">
-        <v>449</v>
+        <v>446</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A104" s="1" t="s">
-        <v>450</v>
+        <v>447</v>
       </c>
       <c r="B104" s="2" t="s">
-        <v>451</v>
+        <v>448</v>
       </c>
       <c r="C104" s="2" t="s">
-        <v>452</v>
+        <v>449</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A105" s="1" t="s">
-        <v>453</v>
+        <v>450</v>
       </c>
       <c r="B105" s="2" t="s">
-        <v>454</v>
+        <v>451</v>
       </c>
       <c r="C105" s="2" t="s">
-        <v>455</v>
+        <v>452</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A106" s="1" t="s">
-        <v>456</v>
+        <v>453</v>
       </c>
       <c r="B106" s="2" t="s">
-        <v>457</v>
+        <v>454</v>
       </c>
       <c r="C106" s="2" t="s">
-        <v>458</v>
+        <v>455</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A107" s="1" t="s">
-        <v>459</v>
+        <v>456</v>
       </c>
       <c r="B107" s="2" t="s">
-        <v>460</v>
+        <v>457</v>
       </c>
       <c r="C107" s="2" t="s">
-        <v>461</v>
+        <v>458</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A108" s="1" t="s">
-        <v>462</v>
+        <v>459</v>
       </c>
       <c r="B108" s="2" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="C108" s="2" t="s">
-        <v>464</v>
+        <v>461</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A109" s="1" t="s">
-        <v>465</v>
+        <v>462</v>
       </c>
       <c r="B109" s="2" t="s">
-        <v>466</v>
+        <v>463</v>
       </c>
       <c r="C109" s="2" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A110" s="1" t="s">
-        <v>468</v>
+        <v>465</v>
       </c>
       <c r="B110" s="2" t="s">
-        <v>469</v>
+        <v>466</v>
       </c>
       <c r="C110" s="2" t="s">
-        <v>470</v>
+        <v>467</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A111" s="1" t="s">
-        <v>471</v>
+        <v>468</v>
       </c>
       <c r="B111" s="2" t="s">
-        <v>472</v>
+        <v>469</v>
       </c>
       <c r="C111" s="2" t="s">
-        <v>473</v>
+        <v>470</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.35">
@@ -4324,90 +4304,90 @@
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A113" s="1" t="s">
-        <v>474</v>
+        <v>471</v>
       </c>
       <c r="B113" s="2" t="s">
-        <v>475</v>
+        <v>472</v>
       </c>
       <c r="C113" s="2" t="s">
-        <v>476</v>
+        <v>473</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A114" s="1" t="s">
-        <v>477</v>
+        <v>474</v>
       </c>
       <c r="B114" s="2" t="s">
-        <v>478</v>
+        <v>475</v>
       </c>
       <c r="C114" s="2" t="s">
-        <v>479</v>
+        <v>476</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A115" s="1" t="s">
-        <v>480</v>
+        <v>477</v>
       </c>
       <c r="B115" s="2" t="s">
-        <v>481</v>
+        <v>478</v>
       </c>
       <c r="C115" s="2" t="s">
-        <v>482</v>
+        <v>479</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A116" s="1" t="s">
-        <v>483</v>
+        <v>480</v>
       </c>
       <c r="B116" s="2" t="s">
-        <v>484</v>
+        <v>481</v>
       </c>
       <c r="C116" s="2" t="s">
-        <v>485</v>
+        <v>482</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A117" s="1" t="s">
-        <v>486</v>
+        <v>483</v>
       </c>
       <c r="B117" s="2" t="s">
-        <v>487</v>
+        <v>484</v>
       </c>
       <c r="C117" s="2" t="s">
-        <v>488</v>
+        <v>485</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A118" s="1" t="s">
-        <v>489</v>
+        <v>486</v>
       </c>
       <c r="B118" s="2" t="s">
-        <v>490</v>
+        <v>487</v>
       </c>
       <c r="C118" s="2" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A119" s="1" t="s">
-        <v>492</v>
+        <v>489</v>
       </c>
       <c r="B119" s="2" t="s">
-        <v>493</v>
+        <v>490</v>
       </c>
       <c r="C119" s="2" t="s">
-        <v>494</v>
+        <v>491</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A120" s="1" t="s">
-        <v>495</v>
+        <v>492</v>
       </c>
       <c r="B120" s="2" t="s">
-        <v>496</v>
+        <v>493</v>
       </c>
       <c r="C120" s="2" t="s">
-        <v>497</v>
+        <v>494</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.35">
@@ -4416,266 +4396,266 @@
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A122" s="1" t="s">
-        <v>498</v>
+        <v>495</v>
       </c>
       <c r="B122" s="2" t="s">
-        <v>499</v>
+        <v>496</v>
       </c>
       <c r="C122" s="2" t="s">
-        <v>500</v>
+        <v>497</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A123" s="1" t="s">
-        <v>501</v>
+        <v>498</v>
       </c>
       <c r="B123" s="2" t="s">
-        <v>502</v>
+        <v>499</v>
       </c>
       <c r="C123" s="2" t="s">
-        <v>503</v>
+        <v>500</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A124" s="1" t="s">
-        <v>504</v>
+        <v>501</v>
       </c>
       <c r="B124" s="2" t="s">
-        <v>505</v>
+        <v>502</v>
       </c>
       <c r="C124" s="2" t="s">
-        <v>506</v>
+        <v>503</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A125" s="1" t="s">
-        <v>507</v>
+        <v>504</v>
       </c>
       <c r="B125" s="2" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
       <c r="C125" s="2" t="s">
-        <v>509</v>
+        <v>506</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A127" s="1" t="s">
-        <v>510</v>
+        <v>507</v>
       </c>
       <c r="B127" s="2" t="s">
-        <v>511</v>
+        <v>508</v>
       </c>
       <c r="C127" s="2" t="s">
-        <v>512</v>
+        <v>509</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A128" s="1" t="s">
-        <v>513</v>
+        <v>510</v>
       </c>
       <c r="B128" s="2" t="s">
-        <v>514</v>
+        <v>511</v>
       </c>
       <c r="C128" s="2" t="s">
-        <v>515</v>
+        <v>512</v>
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A129" s="1" t="s">
-        <v>516</v>
+        <v>513</v>
       </c>
       <c r="B129" s="2" t="s">
-        <v>517</v>
+        <v>514</v>
       </c>
       <c r="C129" s="2" t="s">
-        <v>518</v>
+        <v>515</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A130" s="1" t="s">
-        <v>519</v>
+        <v>516</v>
       </c>
       <c r="B130" s="2" t="s">
-        <v>520</v>
+        <v>517</v>
       </c>
       <c r="C130" s="2" t="s">
-        <v>521</v>
+        <v>518</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A131" s="1" t="s">
-        <v>522</v>
+        <v>519</v>
       </c>
       <c r="B131" s="2" t="s">
-        <v>523</v>
+        <v>520</v>
       </c>
       <c r="C131" s="2" t="s">
-        <v>524</v>
+        <v>521</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A132" s="1" t="s">
-        <v>525</v>
+        <v>522</v>
       </c>
       <c r="B132" s="2" t="s">
-        <v>526</v>
+        <v>523</v>
       </c>
       <c r="C132" s="2" t="s">
-        <v>527</v>
+        <v>524</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A133" s="1" t="s">
-        <v>528</v>
+        <v>525</v>
       </c>
       <c r="B133" s="2" t="s">
-        <v>529</v>
+        <v>526</v>
       </c>
       <c r="C133" s="2" t="s">
-        <v>530</v>
+        <v>527</v>
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A135" s="1" t="s">
-        <v>531</v>
+        <v>528</v>
       </c>
       <c r="B135" s="2" t="s">
-        <v>532</v>
+        <v>529</v>
       </c>
       <c r="C135" s="2" t="s">
-        <v>533</v>
+        <v>530</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A136" s="1" t="s">
-        <v>534</v>
+        <v>531</v>
       </c>
       <c r="B136" s="2" t="s">
-        <v>535</v>
+        <v>532</v>
       </c>
       <c r="C136" s="2" t="s">
-        <v>536</v>
+        <v>533</v>
       </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A137" s="1" t="s">
-        <v>537</v>
+        <v>534</v>
       </c>
       <c r="B137" s="2" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
       <c r="C137" s="2" t="s">
-        <v>539</v>
+        <v>536</v>
       </c>
     </row>
     <row r="138" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A138" s="1" t="s">
-        <v>540</v>
+        <v>537</v>
       </c>
       <c r="B138" s="2" t="s">
-        <v>541</v>
+        <v>538</v>
       </c>
       <c r="C138" s="2" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A139" s="1" t="s">
-        <v>543</v>
+        <v>540</v>
       </c>
       <c r="B139" s="2" t="s">
-        <v>544</v>
+        <v>541</v>
       </c>
       <c r="C139" s="2" t="s">
-        <v>545</v>
+        <v>542</v>
       </c>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A141" s="1" t="s">
-        <v>546</v>
+        <v>543</v>
       </c>
       <c r="B141" s="2" t="s">
-        <v>547</v>
+        <v>544</v>
       </c>
       <c r="C141" s="2" t="s">
-        <v>548</v>
+        <v>545</v>
       </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A142" s="1" t="s">
-        <v>549</v>
+        <v>546</v>
       </c>
       <c r="B142" s="1" t="s">
-        <v>550</v>
+        <v>547</v>
       </c>
       <c r="C142" s="1" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A143" s="1" t="s">
-        <v>552</v>
+        <v>549</v>
       </c>
       <c r="B143" s="1" t="s">
-        <v>553</v>
+        <v>550</v>
       </c>
       <c r="C143" s="1" t="s">
-        <v>554</v>
+        <v>551</v>
       </c>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A144" s="1" t="s">
-        <v>555</v>
+        <v>552</v>
       </c>
       <c r="B144" s="2" t="s">
-        <v>556</v>
+        <v>553</v>
       </c>
       <c r="C144" s="1" t="s">
-        <v>557</v>
+        <v>554</v>
       </c>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A145" s="1" t="s">
-        <v>558</v>
+        <v>555</v>
       </c>
       <c r="B145" s="1" t="s">
-        <v>559</v>
+        <v>556</v>
       </c>
       <c r="C145" s="1" t="s">
-        <v>560</v>
+        <v>557</v>
       </c>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A146" s="1" t="s">
-        <v>561</v>
+        <v>558</v>
       </c>
       <c r="B146" s="2" t="s">
-        <v>562</v>
+        <v>559</v>
       </c>
       <c r="C146" s="2" t="s">
-        <v>563</v>
+        <v>560</v>
       </c>
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A148" s="1" t="s">
-        <v>564</v>
+        <v>561</v>
       </c>
       <c r="B148" s="2" t="s">
-        <v>565</v>
+        <v>562</v>
       </c>
       <c r="C148" s="2" t="s">
-        <v>566</v>
+        <v>563</v>
       </c>
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A149" s="1" t="s">
-        <v>567</v>
+        <v>564</v>
       </c>
       <c r="B149" s="2" t="s">
-        <v>568</v>
+        <v>565</v>
       </c>
       <c r="C149" s="2" t="s">
-        <v>569</v>
+        <v>566</v>
       </c>
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.35">
@@ -4684,57 +4664,57 @@
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A151" s="1" t="s">
-        <v>570</v>
+        <v>567</v>
       </c>
       <c r="B151" s="2" t="s">
-        <v>571</v>
+        <v>568</v>
       </c>
       <c r="C151" s="2" t="s">
-        <v>572</v>
+        <v>569</v>
       </c>
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A152" s="1" t="s">
-        <v>573</v>
+        <v>570</v>
       </c>
       <c r="B152" s="2" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="C152" s="2" t="s">
-        <v>575</v>
+        <v>572</v>
       </c>
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A153" s="1" t="s">
-        <v>576</v>
+        <v>573</v>
       </c>
       <c r="B153" s="2" t="s">
-        <v>577</v>
+        <v>574</v>
       </c>
       <c r="C153" s="2" t="s">
-        <v>578</v>
+        <v>575</v>
       </c>
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A154" s="1" t="s">
-        <v>579</v>
+        <v>576</v>
       </c>
       <c r="B154" s="2" t="s">
-        <v>580</v>
+        <v>577</v>
       </c>
       <c r="C154" s="2" t="s">
-        <v>581</v>
+        <v>578</v>
       </c>
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A155" s="1" t="s">
-        <v>582</v>
+        <v>579</v>
       </c>
       <c r="B155" s="2" t="s">
-        <v>583</v>
+        <v>580</v>
       </c>
       <c r="C155" s="2" t="s">
-        <v>584</v>
+        <v>581</v>
       </c>
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.35">
@@ -4743,145 +4723,145 @@
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A157" s="1" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="B157" s="2" t="s">
-        <v>586</v>
+        <v>583</v>
       </c>
       <c r="C157" s="2" t="s">
-        <v>587</v>
+        <v>584</v>
       </c>
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A158" s="1" t="s">
-        <v>588</v>
+        <v>585</v>
       </c>
       <c r="B158" s="2" t="s">
-        <v>589</v>
+        <v>586</v>
       </c>
       <c r="C158" s="2" t="s">
-        <v>590</v>
+        <v>587</v>
       </c>
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A159" s="1" t="s">
-        <v>591</v>
+        <v>588</v>
       </c>
       <c r="B159" s="2" t="s">
-        <v>592</v>
+        <v>589</v>
       </c>
       <c r="C159" s="2" t="s">
-        <v>593</v>
+        <v>590</v>
       </c>
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A160" s="1" t="s">
-        <v>594</v>
+        <v>591</v>
       </c>
       <c r="B160" s="2" t="s">
-        <v>595</v>
+        <v>592</v>
       </c>
       <c r="C160" s="2" t="s">
-        <v>596</v>
+        <v>593</v>
       </c>
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A161" s="1" t="s">
-        <v>597</v>
+        <v>594</v>
       </c>
       <c r="B161" s="2" t="s">
-        <v>598</v>
+        <v>595</v>
       </c>
       <c r="C161" s="2" t="s">
-        <v>599</v>
+        <v>596</v>
       </c>
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A162" s="1" t="s">
-        <v>600</v>
+        <v>597</v>
       </c>
       <c r="B162" s="2" t="s">
-        <v>601</v>
+        <v>598</v>
       </c>
       <c r="C162" s="2" t="s">
-        <v>602</v>
+        <v>599</v>
       </c>
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A164" s="1" t="s">
-        <v>603</v>
+        <v>600</v>
       </c>
       <c r="B164" s="1" t="s">
-        <v>604</v>
+        <v>601</v>
       </c>
       <c r="C164" s="1" t="s">
-        <v>605</v>
+        <v>602</v>
       </c>
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A165" s="1" t="s">
-        <v>606</v>
+        <v>603</v>
       </c>
       <c r="B165" s="1" t="s">
-        <v>607</v>
+        <v>604</v>
       </c>
       <c r="C165" s="1" t="s">
-        <v>608</v>
+        <v>605</v>
       </c>
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A166" s="1" t="s">
-        <v>609</v>
+        <v>606</v>
       </c>
       <c r="B166" s="1" t="s">
-        <v>610</v>
+        <v>607</v>
       </c>
       <c r="C166" s="1" t="s">
-        <v>611</v>
+        <v>608</v>
       </c>
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A167" s="1" t="s">
-        <v>612</v>
+        <v>609</v>
       </c>
       <c r="B167" s="1" t="s">
-        <v>613</v>
+        <v>610</v>
       </c>
       <c r="C167" s="1" t="s">
-        <v>614</v>
+        <v>611</v>
       </c>
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A168" s="1" t="s">
-        <v>615</v>
+        <v>612</v>
       </c>
       <c r="B168" s="2" t="s">
-        <v>616</v>
+        <v>613</v>
       </c>
       <c r="C168" s="2" t="s">
-        <v>617</v>
+        <v>614</v>
       </c>
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A169" s="1" t="s">
-        <v>618</v>
+        <v>615</v>
       </c>
       <c r="B169" s="1" t="s">
-        <v>619</v>
+        <v>616</v>
       </c>
       <c r="C169" s="1" t="s">
-        <v>620</v>
+        <v>617</v>
       </c>
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A170" s="1" t="s">
-        <v>621</v>
+        <v>618</v>
       </c>
       <c r="B170" s="1" t="s">
-        <v>622</v>
+        <v>619</v>
       </c>
       <c r="C170" s="1" t="s">
-        <v>623</v>
+        <v>620</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Handle separate tenant names for Cloud and On-Premises Orchestrator instances
</commit_message>
<xml_diff>
--- a/Config.xlsx
+++ b/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mateus.cruz\Documents\GitHub\OrchestratorManager\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{126847A3-A5C0-4FB7-B26E-74DBB35C1CC5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94BA0CD9-66E3-47F9-B8DD-07A58E534400}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="670" uniqueCount="623">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="673" uniqueCount="625">
   <si>
     <t>Name</t>
   </si>
@@ -53,13 +53,28 @@
 Sample value: C:\Users\MyUser\Desktop\Workbooks</t>
   </si>
   <si>
-    <t>TenantName</t>
+    <t>CloudTenantName</t>
+  </si>
+  <si>
+    <t>Name of the tenant to be used in case of Automation Cloud Orchestrator instances. 
+Sample value: Default.</t>
+  </si>
+  <si>
+    <t>CloudAccountName</t>
+  </si>
+  <si>
+    <t>Unique site URL for Automation Cloud organization.
+This parameter is exclusive to Automation Cloud Orchestrator instances.
+Sample value: SampleAccount (assuming the organization account URL is https://cloud.uipath.com/SampleAccount).</t>
+  </si>
+  <si>
+    <t>OnPremisesTenantName</t>
   </si>
   <si>
     <t>Default</t>
   </si>
   <si>
-    <t>Name of the tenant to be used. 
+    <t>Name of the tenant to be used in case of on-premises Orchestrator instances. 
 Sample value: Default.</t>
   </si>
   <si>
@@ -84,14 +99,6 @@
 202004</t>
   </si>
   <si>
-    <t>CloudAccountName</t>
-  </si>
-  <si>
-    <t>Unique site URL for Automation Cloud oganization.
-This parameter is exclusive to Automation Cloud Orchestrator instances.
-Sample value: MyAccount (assuming the organization account URL is https://platform.uipath.com/MyAccount).</t>
-  </si>
-  <si>
     <t>MaximumRequestsThreshold</t>
   </si>
   <si>
@@ -141,7 +148,7 @@
     <t>CloudPlatformURL</t>
   </si>
   <si>
-    <t>https://platform.uipath.com/</t>
+    <t>https://cloud.uipath.com/</t>
   </si>
   <si>
     <t>URL of UiPath Cloud Platform.</t>
@@ -1914,10 +1921,10 @@
     <t>キューアイテム一覧のファイルが見つかりませんでした。</t>
   </si>
   <si>
+    <t>SampleAccount</t>
+  </si>
+  <si>
     <t>https://myOrchestratorURL</t>
-  </si>
-  <si>
-    <t>MyAccount</t>
   </si>
 </sst>
 </file>
@@ -1986,8 +1993,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table14" displayName="Table14" ref="A1:C8" totalsRowShown="0">
-  <autoFilter ref="A1:C8" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table14" displayName="Table14" ref="A1:C7" totalsRowShown="0">
+  <autoFilter ref="A1:C7" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Name"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Value"/>
@@ -2284,7 +2291,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D89C9C48-5454-47C4-AB1D-448E4519251A}">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -2316,48 +2323,59 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="43.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" ht="58" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="2" t="s">
+    </row>
+    <row r="4" spans="1:3" ht="72.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="1" t="s">
         <v>7</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>623</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="58" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>621</v>
+        <v>9</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="159.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="58" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" s="1">
-        <v>202004</v>
+        <v>12</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>624</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="72.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>622</v>
-      </c>
-      <c r="C8" s="2" t="s">
         <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="159.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="1">
+        <v>201804</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -2374,7 +2392,7 @@
   <dimension ref="A1:C63"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2 A2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2397,684 +2415,684 @@
     </row>
     <row r="2" spans="1:3" ht="101.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B2" s="1">
         <v>200</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B3" s="1">
         <v>0</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B4" s="1">
         <v>550</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B5" s="1">
         <v>650</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B6" s="1">
         <v>3</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B7" s="1">
         <v>5000</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A30" s="1" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" s="1" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="1" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A33" s="1" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A34" s="1" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A35" s="1" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A36" s="1" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A37" s="1" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A38" s="1" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A39" s="1" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A40" s="1" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
     </row>
     <row r="41" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A41" s="1" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
     </row>
     <row r="42" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A42" s="1" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
     </row>
     <row r="43" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A43" s="1" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A44" s="1" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
     </row>
     <row r="45" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A45" s="1" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
     </row>
     <row r="46" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A46" s="1" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
     </row>
     <row r="47" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A47" s="1" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
     </row>
     <row r="48" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A48" s="1" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A49" s="1" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
     </row>
     <row r="50" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A50" s="1" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
     </row>
     <row r="51" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A51" s="1" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A52" s="1" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
     </row>
     <row r="53" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A53" s="1" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
     </row>
     <row r="54" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A54" s="1" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A55" s="1" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
     </row>
     <row r="56" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A56" s="1" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
     </row>
     <row r="57" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A57" s="1" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
     </row>
     <row r="58" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A58" s="1" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
     </row>
     <row r="59" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A59" s="1" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
     </row>
     <row r="60" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A60" s="1" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
     </row>
     <row r="61" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A61" s="1" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
     </row>
     <row r="62" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A62" s="1" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
     </row>
     <row r="63" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A63" s="1" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
     </row>
   </sheetData>
@@ -3095,7 +3113,7 @@
   <dimension ref="A1:C170"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2 A2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3110,351 +3128,351 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="43.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A30" s="1" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A31" s="1" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A32" s="1" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.35">
@@ -3463,112 +3481,112 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A34" s="1" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A35" s="1" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A36" s="1" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A37" s="1" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A38" s="1" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A39" s="1" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A40" s="1" t="s">
-        <v>264</v>
+        <v>266</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>265</v>
+        <v>267</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>266</v>
+        <v>268</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A41" s="1" t="s">
-        <v>267</v>
+        <v>269</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>269</v>
+        <v>271</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A42" s="1" t="s">
-        <v>270</v>
+        <v>272</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A43" s="1" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>275</v>
+        <v>277</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.35">
@@ -3577,530 +3595,530 @@
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A45" s="1" t="s">
-        <v>276</v>
+        <v>278</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A46" s="1" t="s">
-        <v>279</v>
+        <v>281</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>280</v>
+        <v>282</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>281</v>
+        <v>283</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A47" s="1" t="s">
-        <v>282</v>
+        <v>284</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>283</v>
+        <v>285</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>284</v>
+        <v>286</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A48" s="1" t="s">
-        <v>285</v>
+        <v>287</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>286</v>
+        <v>288</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>287</v>
+        <v>289</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A49" s="1" t="s">
-        <v>288</v>
+        <v>290</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>289</v>
+        <v>291</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>290</v>
+        <v>292</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A50" s="1" t="s">
-        <v>291</v>
+        <v>293</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>292</v>
+        <v>294</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>293</v>
+        <v>295</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A51" s="1" t="s">
-        <v>294</v>
+        <v>296</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>295</v>
+        <v>297</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A52" s="1" t="s">
-        <v>297</v>
+        <v>299</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>298</v>
+        <v>300</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>299</v>
+        <v>301</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A53" s="1" t="s">
-        <v>300</v>
+        <v>302</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>301</v>
+        <v>303</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A54" s="1" t="s">
-        <v>303</v>
+        <v>305</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>304</v>
+        <v>306</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>305</v>
+        <v>307</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A55" s="1" t="s">
-        <v>306</v>
+        <v>308</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>307</v>
+        <v>309</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>308</v>
+        <v>310</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A56" s="1" t="s">
-        <v>309</v>
+        <v>311</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>310</v>
+        <v>312</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>311</v>
+        <v>313</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A57" s="1" t="s">
-        <v>312</v>
+        <v>314</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>313</v>
+        <v>315</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>314</v>
+        <v>316</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A58" s="1" t="s">
-        <v>315</v>
+        <v>317</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>317</v>
+        <v>319</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A59" s="1" t="s">
-        <v>318</v>
+        <v>320</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>319</v>
+        <v>321</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>320</v>
+        <v>322</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A60" s="1" t="s">
-        <v>321</v>
+        <v>323</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>322</v>
+        <v>324</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>323</v>
+        <v>325</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A61" s="1" t="s">
-        <v>324</v>
+        <v>326</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>325</v>
+        <v>327</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>326</v>
+        <v>328</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A62" s="1" t="s">
-        <v>327</v>
+        <v>329</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>328</v>
+        <v>330</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>329</v>
+        <v>331</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A63" s="1" t="s">
-        <v>330</v>
+        <v>332</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>331</v>
+        <v>333</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>332</v>
+        <v>334</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A64" s="1" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>335</v>
+        <v>337</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A65" s="1" t="s">
-        <v>336</v>
+        <v>338</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>337</v>
+        <v>339</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>338</v>
+        <v>340</v>
       </c>
     </row>
     <row r="66" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A66" s="1" t="s">
-        <v>339</v>
+        <v>341</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>340</v>
+        <v>342</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>341</v>
+        <v>343</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A67" s="1" t="s">
-        <v>342</v>
+        <v>344</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>343</v>
+        <v>345</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>344</v>
+        <v>346</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A68" s="1" t="s">
-        <v>345</v>
+        <v>347</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>346</v>
+        <v>348</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>347</v>
+        <v>349</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A69" s="1" t="s">
-        <v>348</v>
+        <v>350</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>349</v>
+        <v>351</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>350</v>
+        <v>352</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A70" s="1" t="s">
-        <v>351</v>
+        <v>353</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>352</v>
+        <v>354</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>353</v>
+        <v>355</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A71" s="1" t="s">
-        <v>354</v>
+        <v>356</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>355</v>
+        <v>357</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>356</v>
+        <v>358</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A72" s="1" t="s">
-        <v>357</v>
+        <v>359</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>358</v>
+        <v>360</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>359</v>
+        <v>361</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A73" s="1" t="s">
-        <v>360</v>
+        <v>362</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>361</v>
+        <v>363</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>362</v>
+        <v>364</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A74" s="1" t="s">
-        <v>363</v>
+        <v>365</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>364</v>
+        <v>366</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>365</v>
+        <v>367</v>
       </c>
     </row>
     <row r="75" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A75" s="1" t="s">
-        <v>366</v>
+        <v>368</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>367</v>
+        <v>369</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>368</v>
+        <v>370</v>
       </c>
     </row>
     <row r="76" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A76" s="1" t="s">
-        <v>369</v>
+        <v>371</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>370</v>
+        <v>372</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>371</v>
+        <v>373</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A77" s="1" t="s">
-        <v>372</v>
+        <v>374</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>373</v>
+        <v>375</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>374</v>
+        <v>376</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A78" s="1" t="s">
-        <v>375</v>
+        <v>377</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>376</v>
+        <v>378</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>377</v>
+        <v>379</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A79" s="1" t="s">
-        <v>378</v>
+        <v>380</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>379</v>
+        <v>381</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>380</v>
+        <v>382</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A80" s="1" t="s">
-        <v>381</v>
+        <v>383</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>382</v>
+        <v>384</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>383</v>
+        <v>385</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A81" s="1" t="s">
-        <v>384</v>
+        <v>386</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>385</v>
+        <v>387</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>386</v>
+        <v>388</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A82" s="1" t="s">
-        <v>387</v>
+        <v>389</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>388</v>
+        <v>390</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>389</v>
+        <v>391</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A83" s="1" t="s">
-        <v>390</v>
+        <v>392</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>391</v>
+        <v>393</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>392</v>
+        <v>394</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A84" s="1" t="s">
-        <v>393</v>
+        <v>395</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>395</v>
+        <v>397</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A85" s="1" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>397</v>
+        <v>399</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>398</v>
+        <v>400</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A86" s="1" t="s">
-        <v>399</v>
+        <v>401</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>400</v>
+        <v>402</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>401</v>
+        <v>403</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A87" s="1" t="s">
-        <v>402</v>
+        <v>404</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>403</v>
+        <v>405</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>404</v>
+        <v>406</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A88" s="1" t="s">
-        <v>405</v>
+        <v>407</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>406</v>
+        <v>408</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>407</v>
+        <v>409</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A89" s="1" t="s">
-        <v>408</v>
+        <v>410</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>409</v>
+        <v>411</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>410</v>
+        <v>412</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A90" s="1" t="s">
-        <v>411</v>
+        <v>413</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>412</v>
+        <v>414</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>413</v>
+        <v>415</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A91" s="1" t="s">
-        <v>414</v>
+        <v>416</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>415</v>
+        <v>417</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>416</v>
+        <v>418</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A92" s="1" t="s">
-        <v>417</v>
+        <v>419</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>418</v>
+        <v>420</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>419</v>
+        <v>421</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.35">
@@ -4109,90 +4127,90 @@
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A94" s="1" t="s">
-        <v>420</v>
+        <v>422</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>421</v>
+        <v>423</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>422</v>
+        <v>424</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A95" s="1" t="s">
-        <v>423</v>
+        <v>425</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>424</v>
+        <v>426</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>425</v>
+        <v>427</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A96" s="1" t="s">
-        <v>426</v>
+        <v>428</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>427</v>
+        <v>429</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>428</v>
+        <v>430</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A97" s="1" t="s">
-        <v>429</v>
+        <v>431</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>430</v>
+        <v>432</v>
       </c>
       <c r="C97" s="2" t="s">
-        <v>431</v>
+        <v>433</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A98" s="1" t="s">
-        <v>432</v>
+        <v>434</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>433</v>
+        <v>435</v>
       </c>
       <c r="C98" s="2" t="s">
-        <v>434</v>
+        <v>436</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A99" s="1" t="s">
-        <v>435</v>
+        <v>437</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>436</v>
+        <v>438</v>
       </c>
       <c r="C99" s="2" t="s">
-        <v>437</v>
+        <v>439</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A100" s="1" t="s">
-        <v>438</v>
+        <v>440</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>439</v>
+        <v>441</v>
       </c>
       <c r="C100" s="2" t="s">
-        <v>440</v>
+        <v>442</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A101" s="1" t="s">
-        <v>441</v>
+        <v>443</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>442</v>
+        <v>444</v>
       </c>
       <c r="C101" s="2" t="s">
-        <v>443</v>
+        <v>445</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.35">
@@ -4201,101 +4219,101 @@
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A103" s="1" t="s">
-        <v>444</v>
+        <v>446</v>
       </c>
       <c r="B103" s="2" t="s">
-        <v>445</v>
+        <v>447</v>
       </c>
       <c r="C103" s="2" t="s">
-        <v>446</v>
+        <v>448</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A104" s="1" t="s">
-        <v>447</v>
+        <v>449</v>
       </c>
       <c r="B104" s="2" t="s">
-        <v>448</v>
+        <v>450</v>
       </c>
       <c r="C104" s="2" t="s">
-        <v>449</v>
+        <v>451</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A105" s="1" t="s">
-        <v>450</v>
+        <v>452</v>
       </c>
       <c r="B105" s="2" t="s">
-        <v>451</v>
+        <v>453</v>
       </c>
       <c r="C105" s="2" t="s">
-        <v>452</v>
+        <v>454</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A106" s="1" t="s">
-        <v>453</v>
+        <v>455</v>
       </c>
       <c r="B106" s="2" t="s">
-        <v>454</v>
+        <v>456</v>
       </c>
       <c r="C106" s="2" t="s">
-        <v>455</v>
+        <v>457</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A107" s="1" t="s">
-        <v>456</v>
+        <v>458</v>
       </c>
       <c r="B107" s="2" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
       <c r="C107" s="2" t="s">
-        <v>458</v>
+        <v>460</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A108" s="1" t="s">
-        <v>459</v>
+        <v>461</v>
       </c>
       <c r="B108" s="2" t="s">
-        <v>460</v>
+        <v>462</v>
       </c>
       <c r="C108" s="2" t="s">
-        <v>461</v>
+        <v>463</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A109" s="1" t="s">
-        <v>462</v>
+        <v>464</v>
       </c>
       <c r="B109" s="2" t="s">
-        <v>463</v>
+        <v>465</v>
       </c>
       <c r="C109" s="2" t="s">
-        <v>464</v>
+        <v>466</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A110" s="1" t="s">
-        <v>465</v>
+        <v>467</v>
       </c>
       <c r="B110" s="2" t="s">
-        <v>466</v>
+        <v>468</v>
       </c>
       <c r="C110" s="2" t="s">
-        <v>467</v>
+        <v>469</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A111" s="1" t="s">
-        <v>468</v>
+        <v>470</v>
       </c>
       <c r="B111" s="2" t="s">
-        <v>469</v>
+        <v>471</v>
       </c>
       <c r="C111" s="2" t="s">
-        <v>470</v>
+        <v>472</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.35">
@@ -4304,90 +4322,90 @@
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A113" s="1" t="s">
-        <v>471</v>
+        <v>473</v>
       </c>
       <c r="B113" s="2" t="s">
-        <v>472</v>
+        <v>474</v>
       </c>
       <c r="C113" s="2" t="s">
-        <v>473</v>
+        <v>475</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A114" s="1" t="s">
-        <v>474</v>
+        <v>476</v>
       </c>
       <c r="B114" s="2" t="s">
-        <v>475</v>
+        <v>477</v>
       </c>
       <c r="C114" s="2" t="s">
-        <v>476</v>
+        <v>478</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A115" s="1" t="s">
-        <v>477</v>
+        <v>479</v>
       </c>
       <c r="B115" s="2" t="s">
-        <v>478</v>
+        <v>480</v>
       </c>
       <c r="C115" s="2" t="s">
-        <v>479</v>
+        <v>481</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A116" s="1" t="s">
-        <v>480</v>
+        <v>482</v>
       </c>
       <c r="B116" s="2" t="s">
-        <v>481</v>
+        <v>483</v>
       </c>
       <c r="C116" s="2" t="s">
-        <v>482</v>
+        <v>484</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A117" s="1" t="s">
-        <v>483</v>
+        <v>485</v>
       </c>
       <c r="B117" s="2" t="s">
-        <v>484</v>
+        <v>486</v>
       </c>
       <c r="C117" s="2" t="s">
-        <v>485</v>
+        <v>487</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A118" s="1" t="s">
-        <v>486</v>
+        <v>488</v>
       </c>
       <c r="B118" s="2" t="s">
-        <v>487</v>
+        <v>489</v>
       </c>
       <c r="C118" s="2" t="s">
-        <v>488</v>
+        <v>490</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A119" s="1" t="s">
-        <v>489</v>
+        <v>491</v>
       </c>
       <c r="B119" s="2" t="s">
-        <v>490</v>
+        <v>492</v>
       </c>
       <c r="C119" s="2" t="s">
-        <v>491</v>
+        <v>493</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A120" s="1" t="s">
-        <v>492</v>
+        <v>494</v>
       </c>
       <c r="B120" s="2" t="s">
-        <v>493</v>
+        <v>495</v>
       </c>
       <c r="C120" s="2" t="s">
-        <v>494</v>
+        <v>496</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.35">
@@ -4396,266 +4414,266 @@
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A122" s="1" t="s">
-        <v>495</v>
+        <v>497</v>
       </c>
       <c r="B122" s="2" t="s">
-        <v>496</v>
+        <v>498</v>
       </c>
       <c r="C122" s="2" t="s">
-        <v>497</v>
+        <v>499</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A123" s="1" t="s">
-        <v>498</v>
+        <v>500</v>
       </c>
       <c r="B123" s="2" t="s">
-        <v>499</v>
+        <v>501</v>
       </c>
       <c r="C123" s="2" t="s">
-        <v>500</v>
+        <v>502</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A124" s="1" t="s">
-        <v>501</v>
+        <v>503</v>
       </c>
       <c r="B124" s="2" t="s">
-        <v>502</v>
+        <v>504</v>
       </c>
       <c r="C124" s="2" t="s">
-        <v>503</v>
+        <v>505</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A125" s="1" t="s">
-        <v>504</v>
+        <v>506</v>
       </c>
       <c r="B125" s="2" t="s">
-        <v>505</v>
+        <v>507</v>
       </c>
       <c r="C125" s="2" t="s">
-        <v>506</v>
+        <v>508</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A127" s="1" t="s">
-        <v>507</v>
+        <v>509</v>
       </c>
       <c r="B127" s="2" t="s">
-        <v>508</v>
+        <v>510</v>
       </c>
       <c r="C127" s="2" t="s">
-        <v>509</v>
+        <v>511</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A128" s="1" t="s">
-        <v>510</v>
+        <v>512</v>
       </c>
       <c r="B128" s="2" t="s">
-        <v>511</v>
+        <v>513</v>
       </c>
       <c r="C128" s="2" t="s">
-        <v>512</v>
+        <v>514</v>
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A129" s="1" t="s">
-        <v>513</v>
+        <v>515</v>
       </c>
       <c r="B129" s="2" t="s">
-        <v>514</v>
+        <v>516</v>
       </c>
       <c r="C129" s="2" t="s">
-        <v>515</v>
+        <v>517</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A130" s="1" t="s">
-        <v>516</v>
+        <v>518</v>
       </c>
       <c r="B130" s="2" t="s">
-        <v>517</v>
+        <v>519</v>
       </c>
       <c r="C130" s="2" t="s">
-        <v>518</v>
+        <v>520</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A131" s="1" t="s">
-        <v>519</v>
+        <v>521</v>
       </c>
       <c r="B131" s="2" t="s">
-        <v>520</v>
+        <v>522</v>
       </c>
       <c r="C131" s="2" t="s">
-        <v>521</v>
+        <v>523</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A132" s="1" t="s">
-        <v>522</v>
+        <v>524</v>
       </c>
       <c r="B132" s="2" t="s">
-        <v>523</v>
+        <v>525</v>
       </c>
       <c r="C132" s="2" t="s">
-        <v>524</v>
+        <v>526</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A133" s="1" t="s">
-        <v>525</v>
+        <v>527</v>
       </c>
       <c r="B133" s="2" t="s">
-        <v>526</v>
+        <v>528</v>
       </c>
       <c r="C133" s="2" t="s">
-        <v>527</v>
+        <v>529</v>
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A135" s="1" t="s">
-        <v>528</v>
+        <v>530</v>
       </c>
       <c r="B135" s="2" t="s">
-        <v>529</v>
+        <v>531</v>
       </c>
       <c r="C135" s="2" t="s">
-        <v>530</v>
+        <v>532</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A136" s="1" t="s">
-        <v>531</v>
+        <v>533</v>
       </c>
       <c r="B136" s="2" t="s">
-        <v>532</v>
+        <v>534</v>
       </c>
       <c r="C136" s="2" t="s">
-        <v>533</v>
+        <v>535</v>
       </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A137" s="1" t="s">
-        <v>534</v>
+        <v>536</v>
       </c>
       <c r="B137" s="2" t="s">
-        <v>535</v>
+        <v>537</v>
       </c>
       <c r="C137" s="2" t="s">
-        <v>536</v>
+        <v>538</v>
       </c>
     </row>
     <row r="138" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A138" s="1" t="s">
-        <v>537</v>
+        <v>539</v>
       </c>
       <c r="B138" s="2" t="s">
-        <v>538</v>
+        <v>540</v>
       </c>
       <c r="C138" s="2" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A139" s="1" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
       <c r="B139" s="2" t="s">
-        <v>541</v>
+        <v>543</v>
       </c>
       <c r="C139" s="2" t="s">
-        <v>542</v>
+        <v>544</v>
       </c>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A141" s="1" t="s">
-        <v>543</v>
+        <v>545</v>
       </c>
       <c r="B141" s="2" t="s">
-        <v>544</v>
+        <v>546</v>
       </c>
       <c r="C141" s="2" t="s">
-        <v>545</v>
+        <v>547</v>
       </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A142" s="1" t="s">
-        <v>546</v>
+        <v>548</v>
       </c>
       <c r="B142" s="1" t="s">
-        <v>547</v>
+        <v>549</v>
       </c>
       <c r="C142" s="1" t="s">
-        <v>548</v>
+        <v>550</v>
       </c>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A143" s="1" t="s">
-        <v>549</v>
+        <v>551</v>
       </c>
       <c r="B143" s="1" t="s">
-        <v>550</v>
+        <v>552</v>
       </c>
       <c r="C143" s="1" t="s">
-        <v>551</v>
+        <v>553</v>
       </c>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A144" s="1" t="s">
-        <v>552</v>
+        <v>554</v>
       </c>
       <c r="B144" s="2" t="s">
-        <v>553</v>
+        <v>555</v>
       </c>
       <c r="C144" s="1" t="s">
-        <v>554</v>
+        <v>556</v>
       </c>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A145" s="1" t="s">
-        <v>555</v>
+        <v>557</v>
       </c>
       <c r="B145" s="1" t="s">
-        <v>556</v>
+        <v>558</v>
       </c>
       <c r="C145" s="1" t="s">
-        <v>557</v>
+        <v>559</v>
       </c>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A146" s="1" t="s">
-        <v>558</v>
+        <v>560</v>
       </c>
       <c r="B146" s="2" t="s">
-        <v>559</v>
+        <v>561</v>
       </c>
       <c r="C146" s="2" t="s">
-        <v>560</v>
+        <v>562</v>
       </c>
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A148" s="1" t="s">
-        <v>561</v>
+        <v>563</v>
       </c>
       <c r="B148" s="2" t="s">
-        <v>562</v>
+        <v>564</v>
       </c>
       <c r="C148" s="2" t="s">
-        <v>563</v>
+        <v>565</v>
       </c>
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A149" s="1" t="s">
-        <v>564</v>
+        <v>566</v>
       </c>
       <c r="B149" s="2" t="s">
-        <v>565</v>
+        <v>567</v>
       </c>
       <c r="C149" s="2" t="s">
-        <v>566</v>
+        <v>568</v>
       </c>
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.35">
@@ -4664,57 +4682,57 @@
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A151" s="1" t="s">
-        <v>567</v>
+        <v>569</v>
       </c>
       <c r="B151" s="2" t="s">
-        <v>568</v>
+        <v>570</v>
       </c>
       <c r="C151" s="2" t="s">
-        <v>569</v>
+        <v>571</v>
       </c>
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A152" s="1" t="s">
-        <v>570</v>
+        <v>572</v>
       </c>
       <c r="B152" s="2" t="s">
-        <v>571</v>
+        <v>573</v>
       </c>
       <c r="C152" s="2" t="s">
-        <v>572</v>
+        <v>574</v>
       </c>
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A153" s="1" t="s">
-        <v>573</v>
+        <v>575</v>
       </c>
       <c r="B153" s="2" t="s">
-        <v>574</v>
+        <v>576</v>
       </c>
       <c r="C153" s="2" t="s">
-        <v>575</v>
+        <v>577</v>
       </c>
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A154" s="1" t="s">
-        <v>576</v>
+        <v>578</v>
       </c>
       <c r="B154" s="2" t="s">
-        <v>577</v>
+        <v>579</v>
       </c>
       <c r="C154" s="2" t="s">
-        <v>578</v>
+        <v>580</v>
       </c>
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A155" s="1" t="s">
-        <v>579</v>
+        <v>581</v>
       </c>
       <c r="B155" s="2" t="s">
-        <v>580</v>
+        <v>582</v>
       </c>
       <c r="C155" s="2" t="s">
-        <v>581</v>
+        <v>583</v>
       </c>
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.35">
@@ -4723,145 +4741,145 @@
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A157" s="1" t="s">
-        <v>582</v>
+        <v>584</v>
       </c>
       <c r="B157" s="2" t="s">
-        <v>583</v>
+        <v>585</v>
       </c>
       <c r="C157" s="2" t="s">
-        <v>584</v>
+        <v>586</v>
       </c>
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A158" s="1" t="s">
-        <v>585</v>
+        <v>587</v>
       </c>
       <c r="B158" s="2" t="s">
-        <v>586</v>
+        <v>588</v>
       </c>
       <c r="C158" s="2" t="s">
-        <v>587</v>
+        <v>589</v>
       </c>
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A159" s="1" t="s">
-        <v>588</v>
+        <v>590</v>
       </c>
       <c r="B159" s="2" t="s">
-        <v>589</v>
+        <v>591</v>
       </c>
       <c r="C159" s="2" t="s">
-        <v>590</v>
+        <v>592</v>
       </c>
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A160" s="1" t="s">
-        <v>591</v>
+        <v>593</v>
       </c>
       <c r="B160" s="2" t="s">
-        <v>592</v>
+        <v>594</v>
       </c>
       <c r="C160" s="2" t="s">
-        <v>593</v>
+        <v>595</v>
       </c>
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A161" s="1" t="s">
-        <v>594</v>
+        <v>596</v>
       </c>
       <c r="B161" s="2" t="s">
-        <v>595</v>
+        <v>597</v>
       </c>
       <c r="C161" s="2" t="s">
-        <v>596</v>
+        <v>598</v>
       </c>
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A162" s="1" t="s">
-        <v>597</v>
+        <v>599</v>
       </c>
       <c r="B162" s="2" t="s">
-        <v>598</v>
+        <v>600</v>
       </c>
       <c r="C162" s="2" t="s">
-        <v>599</v>
+        <v>601</v>
       </c>
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A164" s="1" t="s">
-        <v>600</v>
+        <v>602</v>
       </c>
       <c r="B164" s="1" t="s">
-        <v>601</v>
+        <v>603</v>
       </c>
       <c r="C164" s="1" t="s">
-        <v>602</v>
+        <v>604</v>
       </c>
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A165" s="1" t="s">
-        <v>603</v>
+        <v>605</v>
       </c>
       <c r="B165" s="1" t="s">
-        <v>604</v>
+        <v>606</v>
       </c>
       <c r="C165" s="1" t="s">
-        <v>605</v>
+        <v>607</v>
       </c>
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A166" s="1" t="s">
-        <v>606</v>
+        <v>608</v>
       </c>
       <c r="B166" s="1" t="s">
-        <v>607</v>
+        <v>609</v>
       </c>
       <c r="C166" s="1" t="s">
-        <v>608</v>
+        <v>610</v>
       </c>
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A167" s="1" t="s">
-        <v>609</v>
+        <v>611</v>
       </c>
       <c r="B167" s="1" t="s">
-        <v>610</v>
+        <v>612</v>
       </c>
       <c r="C167" s="1" t="s">
-        <v>611</v>
+        <v>613</v>
       </c>
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A168" s="1" t="s">
-        <v>612</v>
+        <v>614</v>
       </c>
       <c r="B168" s="2" t="s">
-        <v>613</v>
+        <v>615</v>
       </c>
       <c r="C168" s="2" t="s">
-        <v>614</v>
+        <v>616</v>
       </c>
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A169" s="1" t="s">
-        <v>615</v>
+        <v>617</v>
       </c>
       <c r="B169" s="1" t="s">
-        <v>616</v>
+        <v>618</v>
       </c>
       <c r="C169" s="1" t="s">
-        <v>617</v>
+        <v>619</v>
       </c>
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A170" s="1" t="s">
-        <v>618</v>
+        <v>620</v>
       </c>
       <c r="B170" s="1" t="s">
-        <v>619</v>
+        <v>621</v>
       </c>
       <c r="C170" s="1" t="s">
-        <v>620</v>
+        <v>622</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Change names from Cloud Platform to Automation Cloud
</commit_message>
<xml_diff>
--- a/Config.xlsx
+++ b/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mateus.cruz\Documents\GitHub\OrchestratorManager\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94BA0CD9-66E3-47F9-B8DD-07A58E534400}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91F9BD6B-E550-4B36-8EFC-50F8A07984E6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -136,22 +136,22 @@
     <t>Interval (in milliseconds) between retries of making a HTTP request.</t>
   </si>
   <si>
-    <t>CloudPlatformAuthenticationURL</t>
+    <t>AutomationCloudAuthenticationURL</t>
   </si>
   <si>
     <t>https://account.uipath.com/oauth/token</t>
   </si>
   <si>
-    <t>URL used to authenticate to UiPath Cloud Platform.</t>
-  </si>
-  <si>
-    <t>CloudPlatformURL</t>
+    <t>URL used to authenticate to UiPath Automation Cloud.</t>
+  </si>
+  <si>
+    <t>AutomationCloudURL</t>
   </si>
   <si>
     <t>https://cloud.uipath.com/</t>
   </si>
   <si>
-    <t>URL of UiPath Cloud Platform.</t>
+    <t>URL of UiPath Automation Cloud.</t>
   </si>
   <si>
     <t>ControlPanelTemplatePath</t>
@@ -217,13 +217,13 @@
     <t>Path to the folder containing templates of entities workbooks.</t>
   </si>
   <si>
-    <t>CloudCredentialName</t>
-  </si>
-  <si>
-    <t>OrchestratorManager_CloudCredential</t>
-  </si>
-  <si>
-    <t>Name of credential in Windows Credential Manager to store Cloud Platform Orchestrator administrator's credential (ClientID and UserKey).</t>
+    <t>AutomationCloudCredentialName</t>
+  </si>
+  <si>
+    <t>OrchestratorManager_AutomationCloudCredential</t>
+  </si>
+  <si>
+    <t>Name of credential in Windows Credential Manager to store Automation Cloud Orchestrator administrator's credential (ClientID and UserKey).</t>
   </si>
   <si>
     <t>OnPremisesCredentialName</t>
@@ -2372,7 +2372,7 @@
         <v>14</v>
       </c>
       <c r="B7" s="1">
-        <v>201804</v>
+        <v>202004</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>15</v>

</xml_diff>

<commit_message>
Rename columns according to support in different Orchestrator versions
For example, Robots and Environments can only use Classic Folders
</commit_message>
<xml_diff>
--- a/Config.xlsx
+++ b/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mateus.cruz\Documents\GitHub\OrchestratorManager\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91F9BD6B-E550-4B36-8EFC-50F8A07984E6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9CBADD1-BAEB-4C17-8B05-0313BB49FF69}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="673" uniqueCount="625">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="674" uniqueCount="626">
   <si>
     <t>Name</t>
   </si>
@@ -79,6 +79,9 @@
   </si>
   <si>
     <t>OnPremisesOrchestratorURL</t>
+  </si>
+  <si>
+    <t>https://myOrchestratorURL</t>
   </si>
   <si>
     <t>URL of the Orchestrator instance to be used. 
@@ -1921,10 +1924,10 @@
     <t>キューアイテム一覧のファイルが見つかりませんでした。</t>
   </si>
   <si>
+    <t>C:\Users\MyUser\Desktop\Workbooks</t>
+  </si>
+  <si>
     <t>SampleAccount</t>
-  </si>
-  <si>
-    <t>https://myOrchestratorURL</t>
   </si>
 </sst>
 </file>
@@ -2319,6 +2322,9 @@
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="B2" s="1" t="s">
+        <v>624</v>
+      </c>
       <c r="C2" s="2" t="s">
         <v>4</v>
       </c>
@@ -2339,7 +2345,7 @@
         <v>7</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>623</v>
+        <v>625</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>8</v>
@@ -2361,21 +2367,21 @@
         <v>12</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>624</v>
+        <v>13</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="159.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B7" s="1">
         <v>202004</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -2415,684 +2421,684 @@
     </row>
     <row r="2" spans="1:3" ht="101.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B2" s="1">
         <v>200</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B3" s="1">
         <v>0</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B4" s="1">
         <v>550</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B5" s="1">
         <v>650</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B6" s="1">
         <v>3</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B7" s="1">
         <v>5000</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A30" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="1" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A33" s="1" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A34" s="1" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A35" s="1" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A36" s="1" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A37" s="1" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A38" s="1" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A39" s="1" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A40" s="1" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="41" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A41" s="1" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
     </row>
     <row r="42" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A42" s="1" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="43" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A43" s="1" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A44" s="1" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="45" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A45" s="1" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
     <row r="46" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A46" s="1" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
     </row>
     <row r="47" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A47" s="1" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
     </row>
     <row r="48" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A48" s="1" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A49" s="1" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="50" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A50" s="1" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
     </row>
     <row r="51" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A51" s="1" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A52" s="1" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="53" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A53" s="1" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="54" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A54" s="1" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A55" s="1" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
     </row>
     <row r="56" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A56" s="1" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
     </row>
     <row r="57" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A57" s="1" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
     </row>
     <row r="58" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A58" s="1" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
     </row>
     <row r="59" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A59" s="1" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
     </row>
     <row r="60" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A60" s="1" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
     </row>
     <row r="61" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A61" s="1" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
     </row>
     <row r="62" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A62" s="1" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
     </row>
     <row r="63" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A63" s="1" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
   </sheetData>
@@ -3128,351 +3134,351 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="43.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A30" s="1" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A31" s="1" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A32" s="1" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.35">
@@ -3481,112 +3487,112 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A34" s="1" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A35" s="1" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A36" s="1" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A37" s="1" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A38" s="1" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A39" s="1" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A40" s="1" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A41" s="1" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A42" s="1" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A43" s="1" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.35">
@@ -3595,530 +3601,530 @@
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A45" s="1" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A46" s="1" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A47" s="1" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A48" s="1" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A49" s="1" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A50" s="1" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A51" s="1" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A52" s="1" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A53" s="1" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A54" s="1" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A55" s="1" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A56" s="1" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A57" s="1" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A58" s="1" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A59" s="1" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A60" s="1" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A61" s="1" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A62" s="1" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A63" s="1" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A64" s="1" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A65" s="1" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
     </row>
     <row r="66" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A66" s="1" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A67" s="1" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A68" s="1" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A69" s="1" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A70" s="1" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A71" s="1" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A72" s="1" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A73" s="1" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A74" s="1" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
     </row>
     <row r="75" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A75" s="1" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
     </row>
     <row r="76" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A76" s="1" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A77" s="1" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A78" s="1" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A79" s="1" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A80" s="1" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A81" s="1" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A82" s="1" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A83" s="1" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A84" s="1" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A85" s="1" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A86" s="1" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A87" s="1" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A88" s="1" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A89" s="1" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A90" s="1" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A91" s="1" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A92" s="1" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.35">
@@ -4127,90 +4133,90 @@
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A94" s="1" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>424</v>
+        <v>425</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A95" s="1" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>426</v>
+        <v>427</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A96" s="1" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A97" s="1" t="s">
-        <v>431</v>
+        <v>432</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
       <c r="C97" s="2" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A98" s="1" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="C98" s="2" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A99" s="1" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>438</v>
+        <v>439</v>
       </c>
       <c r="C99" s="2" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A100" s="1" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>441</v>
+        <v>442</v>
       </c>
       <c r="C100" s="2" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A101" s="1" t="s">
-        <v>443</v>
+        <v>444</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>444</v>
+        <v>445</v>
       </c>
       <c r="C101" s="2" t="s">
-        <v>445</v>
+        <v>446</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.35">
@@ -4219,101 +4225,101 @@
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A103" s="1" t="s">
-        <v>446</v>
+        <v>447</v>
       </c>
       <c r="B103" s="2" t="s">
-        <v>447</v>
+        <v>448</v>
       </c>
       <c r="C103" s="2" t="s">
-        <v>448</v>
+        <v>449</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A104" s="1" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
       <c r="B104" s="2" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="C104" s="2" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A105" s="1" t="s">
-        <v>452</v>
+        <v>453</v>
       </c>
       <c r="B105" s="2" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="C105" s="2" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A106" s="1" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
       <c r="B106" s="2" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
       <c r="C106" s="2" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A107" s="1" t="s">
-        <v>458</v>
+        <v>459</v>
       </c>
       <c r="B107" s="2" t="s">
-        <v>459</v>
+        <v>460</v>
       </c>
       <c r="C107" s="2" t="s">
-        <v>460</v>
+        <v>461</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A108" s="1" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="B108" s="2" t="s">
-        <v>462</v>
+        <v>463</v>
       </c>
       <c r="C108" s="2" t="s">
-        <v>463</v>
+        <v>464</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A109" s="1" t="s">
-        <v>464</v>
+        <v>465</v>
       </c>
       <c r="B109" s="2" t="s">
-        <v>465</v>
+        <v>466</v>
       </c>
       <c r="C109" s="2" t="s">
-        <v>466</v>
+        <v>467</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A110" s="1" t="s">
-        <v>467</v>
+        <v>468</v>
       </c>
       <c r="B110" s="2" t="s">
-        <v>468</v>
+        <v>469</v>
       </c>
       <c r="C110" s="2" t="s">
-        <v>469</v>
+        <v>470</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A111" s="1" t="s">
-        <v>470</v>
+        <v>471</v>
       </c>
       <c r="B111" s="2" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="C111" s="2" t="s">
-        <v>472</v>
+        <v>473</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.35">
@@ -4322,90 +4328,90 @@
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A113" s="1" t="s">
-        <v>473</v>
+        <v>474</v>
       </c>
       <c r="B113" s="2" t="s">
-        <v>474</v>
+        <v>475</v>
       </c>
       <c r="C113" s="2" t="s">
-        <v>475</v>
+        <v>476</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A114" s="1" t="s">
-        <v>476</v>
+        <v>477</v>
       </c>
       <c r="B114" s="2" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="C114" s="2" t="s">
-        <v>478</v>
+        <v>479</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A115" s="1" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="B115" s="2" t="s">
-        <v>480</v>
+        <v>481</v>
       </c>
       <c r="C115" s="2" t="s">
-        <v>481</v>
+        <v>482</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A116" s="1" t="s">
-        <v>482</v>
+        <v>483</v>
       </c>
       <c r="B116" s="2" t="s">
-        <v>483</v>
+        <v>484</v>
       </c>
       <c r="C116" s="2" t="s">
-        <v>484</v>
+        <v>485</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A117" s="1" t="s">
-        <v>485</v>
+        <v>486</v>
       </c>
       <c r="B117" s="2" t="s">
-        <v>486</v>
+        <v>487</v>
       </c>
       <c r="C117" s="2" t="s">
-        <v>487</v>
+        <v>488</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A118" s="1" t="s">
-        <v>488</v>
+        <v>489</v>
       </c>
       <c r="B118" s="2" t="s">
-        <v>489</v>
+        <v>490</v>
       </c>
       <c r="C118" s="2" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A119" s="1" t="s">
-        <v>491</v>
+        <v>492</v>
       </c>
       <c r="B119" s="2" t="s">
-        <v>492</v>
+        <v>493</v>
       </c>
       <c r="C119" s="2" t="s">
-        <v>493</v>
+        <v>494</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A120" s="1" t="s">
-        <v>494</v>
+        <v>495</v>
       </c>
       <c r="B120" s="2" t="s">
-        <v>495</v>
+        <v>496</v>
       </c>
       <c r="C120" s="2" t="s">
-        <v>496</v>
+        <v>497</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.35">
@@ -4414,266 +4420,266 @@
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A122" s="1" t="s">
-        <v>497</v>
+        <v>498</v>
       </c>
       <c r="B122" s="2" t="s">
-        <v>498</v>
+        <v>499</v>
       </c>
       <c r="C122" s="2" t="s">
-        <v>499</v>
+        <v>500</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A123" s="1" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="B123" s="2" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C123" s="2" t="s">
-        <v>502</v>
+        <v>503</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A124" s="1" t="s">
-        <v>503</v>
+        <v>504</v>
       </c>
       <c r="B124" s="2" t="s">
-        <v>504</v>
+        <v>505</v>
       </c>
       <c r="C124" s="2" t="s">
-        <v>505</v>
+        <v>506</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A125" s="1" t="s">
-        <v>506</v>
+        <v>507</v>
       </c>
       <c r="B125" s="2" t="s">
-        <v>507</v>
+        <v>508</v>
       </c>
       <c r="C125" s="2" t="s">
-        <v>508</v>
+        <v>509</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A127" s="1" t="s">
-        <v>509</v>
+        <v>510</v>
       </c>
       <c r="B127" s="2" t="s">
-        <v>510</v>
+        <v>511</v>
       </c>
       <c r="C127" s="2" t="s">
-        <v>511</v>
+        <v>512</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A128" s="1" t="s">
-        <v>512</v>
+        <v>513</v>
       </c>
       <c r="B128" s="2" t="s">
-        <v>513</v>
+        <v>514</v>
       </c>
       <c r="C128" s="2" t="s">
-        <v>514</v>
+        <v>515</v>
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A129" s="1" t="s">
-        <v>515</v>
+        <v>516</v>
       </c>
       <c r="B129" s="2" t="s">
-        <v>516</v>
+        <v>517</v>
       </c>
       <c r="C129" s="2" t="s">
-        <v>517</v>
+        <v>518</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A130" s="1" t="s">
-        <v>518</v>
+        <v>519</v>
       </c>
       <c r="B130" s="2" t="s">
-        <v>519</v>
+        <v>520</v>
       </c>
       <c r="C130" s="2" t="s">
-        <v>520</v>
+        <v>521</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A131" s="1" t="s">
-        <v>521</v>
+        <v>522</v>
       </c>
       <c r="B131" s="2" t="s">
-        <v>522</v>
+        <v>523</v>
       </c>
       <c r="C131" s="2" t="s">
-        <v>523</v>
+        <v>524</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A132" s="1" t="s">
-        <v>524</v>
+        <v>525</v>
       </c>
       <c r="B132" s="2" t="s">
-        <v>525</v>
+        <v>526</v>
       </c>
       <c r="C132" s="2" t="s">
-        <v>526</v>
+        <v>527</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A133" s="1" t="s">
-        <v>527</v>
+        <v>528</v>
       </c>
       <c r="B133" s="2" t="s">
-        <v>528</v>
+        <v>529</v>
       </c>
       <c r="C133" s="2" t="s">
-        <v>529</v>
+        <v>530</v>
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A135" s="1" t="s">
-        <v>530</v>
+        <v>531</v>
       </c>
       <c r="B135" s="2" t="s">
-        <v>531</v>
+        <v>532</v>
       </c>
       <c r="C135" s="2" t="s">
-        <v>532</v>
+        <v>533</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A136" s="1" t="s">
-        <v>533</v>
+        <v>534</v>
       </c>
       <c r="B136" s="2" t="s">
-        <v>534</v>
+        <v>535</v>
       </c>
       <c r="C136" s="2" t="s">
-        <v>535</v>
+        <v>536</v>
       </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A137" s="1" t="s">
-        <v>536</v>
+        <v>537</v>
       </c>
       <c r="B137" s="2" t="s">
-        <v>537</v>
+        <v>538</v>
       </c>
       <c r="C137" s="2" t="s">
-        <v>538</v>
+        <v>539</v>
       </c>
     </row>
     <row r="138" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A138" s="1" t="s">
-        <v>539</v>
+        <v>540</v>
       </c>
       <c r="B138" s="2" t="s">
-        <v>540</v>
+        <v>541</v>
       </c>
       <c r="C138" s="2" t="s">
-        <v>541</v>
+        <v>542</v>
       </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A139" s="1" t="s">
-        <v>542</v>
+        <v>543</v>
       </c>
       <c r="B139" s="2" t="s">
-        <v>543</v>
+        <v>544</v>
       </c>
       <c r="C139" s="2" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A141" s="1" t="s">
-        <v>545</v>
+        <v>546</v>
       </c>
       <c r="B141" s="2" t="s">
-        <v>546</v>
+        <v>547</v>
       </c>
       <c r="C141" s="2" t="s">
-        <v>547</v>
+        <v>548</v>
       </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A142" s="1" t="s">
-        <v>548</v>
+        <v>549</v>
       </c>
       <c r="B142" s="1" t="s">
-        <v>549</v>
+        <v>550</v>
       </c>
       <c r="C142" s="1" t="s">
-        <v>550</v>
+        <v>551</v>
       </c>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A143" s="1" t="s">
-        <v>551</v>
+        <v>552</v>
       </c>
       <c r="B143" s="1" t="s">
-        <v>552</v>
+        <v>553</v>
       </c>
       <c r="C143" s="1" t="s">
-        <v>553</v>
+        <v>554</v>
       </c>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A144" s="1" t="s">
-        <v>554</v>
+        <v>555</v>
       </c>
       <c r="B144" s="2" t="s">
-        <v>555</v>
+        <v>556</v>
       </c>
       <c r="C144" s="1" t="s">
-        <v>556</v>
+        <v>557</v>
       </c>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A145" s="1" t="s">
-        <v>557</v>
+        <v>558</v>
       </c>
       <c r="B145" s="1" t="s">
-        <v>558</v>
+        <v>559</v>
       </c>
       <c r="C145" s="1" t="s">
-        <v>559</v>
+        <v>560</v>
       </c>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A146" s="1" t="s">
-        <v>560</v>
+        <v>561</v>
       </c>
       <c r="B146" s="2" t="s">
-        <v>561</v>
+        <v>562</v>
       </c>
       <c r="C146" s="2" t="s">
-        <v>562</v>
+        <v>563</v>
       </c>
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A148" s="1" t="s">
-        <v>563</v>
+        <v>564</v>
       </c>
       <c r="B148" s="2" t="s">
-        <v>564</v>
+        <v>565</v>
       </c>
       <c r="C148" s="2" t="s">
-        <v>565</v>
+        <v>566</v>
       </c>
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A149" s="1" t="s">
-        <v>566</v>
+        <v>567</v>
       </c>
       <c r="B149" s="2" t="s">
-        <v>567</v>
+        <v>568</v>
       </c>
       <c r="C149" s="2" t="s">
-        <v>568</v>
+        <v>569</v>
       </c>
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.35">
@@ -4682,57 +4688,57 @@
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A151" s="1" t="s">
-        <v>569</v>
+        <v>570</v>
       </c>
       <c r="B151" s="2" t="s">
-        <v>570</v>
+        <v>571</v>
       </c>
       <c r="C151" s="2" t="s">
-        <v>571</v>
+        <v>572</v>
       </c>
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A152" s="1" t="s">
-        <v>572</v>
+        <v>573</v>
       </c>
       <c r="B152" s="2" t="s">
-        <v>573</v>
+        <v>574</v>
       </c>
       <c r="C152" s="2" t="s">
-        <v>574</v>
+        <v>575</v>
       </c>
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A153" s="1" t="s">
-        <v>575</v>
+        <v>576</v>
       </c>
       <c r="B153" s="2" t="s">
-        <v>576</v>
+        <v>577</v>
       </c>
       <c r="C153" s="2" t="s">
-        <v>577</v>
+        <v>578</v>
       </c>
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A154" s="1" t="s">
-        <v>578</v>
+        <v>579</v>
       </c>
       <c r="B154" s="2" t="s">
-        <v>579</v>
+        <v>580</v>
       </c>
       <c r="C154" s="2" t="s">
-        <v>580</v>
+        <v>581</v>
       </c>
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A155" s="1" t="s">
-        <v>581</v>
+        <v>582</v>
       </c>
       <c r="B155" s="2" t="s">
-        <v>582</v>
+        <v>583</v>
       </c>
       <c r="C155" s="2" t="s">
-        <v>583</v>
+        <v>584</v>
       </c>
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.35">
@@ -4741,145 +4747,145 @@
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A157" s="1" t="s">
-        <v>584</v>
+        <v>585</v>
       </c>
       <c r="B157" s="2" t="s">
-        <v>585</v>
+        <v>586</v>
       </c>
       <c r="C157" s="2" t="s">
-        <v>586</v>
+        <v>587</v>
       </c>
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A158" s="1" t="s">
-        <v>587</v>
+        <v>588</v>
       </c>
       <c r="B158" s="2" t="s">
-        <v>588</v>
+        <v>589</v>
       </c>
       <c r="C158" s="2" t="s">
-        <v>589</v>
+        <v>590</v>
       </c>
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A159" s="1" t="s">
-        <v>590</v>
+        <v>591</v>
       </c>
       <c r="B159" s="2" t="s">
-        <v>591</v>
+        <v>592</v>
       </c>
       <c r="C159" s="2" t="s">
-        <v>592</v>
+        <v>593</v>
       </c>
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A160" s="1" t="s">
-        <v>593</v>
+        <v>594</v>
       </c>
       <c r="B160" s="2" t="s">
-        <v>594</v>
+        <v>595</v>
       </c>
       <c r="C160" s="2" t="s">
-        <v>595</v>
+        <v>596</v>
       </c>
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A161" s="1" t="s">
-        <v>596</v>
+        <v>597</v>
       </c>
       <c r="B161" s="2" t="s">
-        <v>597</v>
+        <v>598</v>
       </c>
       <c r="C161" s="2" t="s">
-        <v>598</v>
+        <v>599</v>
       </c>
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A162" s="1" t="s">
-        <v>599</v>
+        <v>600</v>
       </c>
       <c r="B162" s="2" t="s">
-        <v>600</v>
+        <v>601</v>
       </c>
       <c r="C162" s="2" t="s">
-        <v>601</v>
+        <v>602</v>
       </c>
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A164" s="1" t="s">
-        <v>602</v>
+        <v>603</v>
       </c>
       <c r="B164" s="1" t="s">
-        <v>603</v>
+        <v>604</v>
       </c>
       <c r="C164" s="1" t="s">
-        <v>604</v>
+        <v>605</v>
       </c>
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A165" s="1" t="s">
-        <v>605</v>
+        <v>606</v>
       </c>
       <c r="B165" s="1" t="s">
-        <v>606</v>
+        <v>607</v>
       </c>
       <c r="C165" s="1" t="s">
-        <v>607</v>
+        <v>608</v>
       </c>
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A166" s="1" t="s">
-        <v>608</v>
+        <v>609</v>
       </c>
       <c r="B166" s="1" t="s">
-        <v>609</v>
+        <v>610</v>
       </c>
       <c r="C166" s="1" t="s">
-        <v>610</v>
+        <v>611</v>
       </c>
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A167" s="1" t="s">
-        <v>611</v>
+        <v>612</v>
       </c>
       <c r="B167" s="1" t="s">
-        <v>612</v>
+        <v>613</v>
       </c>
       <c r="C167" s="1" t="s">
-        <v>613</v>
+        <v>614</v>
       </c>
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A168" s="1" t="s">
-        <v>614</v>
+        <v>615</v>
       </c>
       <c r="B168" s="2" t="s">
-        <v>615</v>
+        <v>616</v>
       </c>
       <c r="C168" s="2" t="s">
-        <v>616</v>
+        <v>617</v>
       </c>
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A169" s="1" t="s">
-        <v>617</v>
+        <v>618</v>
       </c>
       <c r="B169" s="1" t="s">
-        <v>618</v>
+        <v>619</v>
       </c>
       <c r="C169" s="1" t="s">
-        <v>619</v>
+        <v>620</v>
       </c>
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A170" s="1" t="s">
-        <v>620</v>
+        <v>621</v>
       </c>
       <c r="B170" s="1" t="s">
-        <v>621</v>
+        <v>622</v>
       </c>
       <c r="C170" s="1" t="s">
-        <v>622</v>
+        <v>623</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Reflect feedback from reviewers
Remember last chosen entity, add tooltips to authentication panel and fix typos
</commit_message>
<xml_diff>
--- a/Config.xlsx
+++ b/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mateus.cruz\Documents\GitHub\OrchestratorManager\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{197C6E37-B6CD-4DFC-BD80-9FFD7F2BEA43}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BB7985F-3E7E-4681-A511-1567B035D2F5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="679" uniqueCount="631">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="715" uniqueCount="667">
   <si>
     <t>Name</t>
   </si>
@@ -79,6 +79,9 @@
   </si>
   <si>
     <t>OnPremisesOrchestratorURL</t>
+  </si>
+  <si>
+    <t>https://myOrchestratorURL</t>
   </si>
   <si>
     <t>URL of the Orchestrator instance to be used. 
@@ -622,7 +625,7 @@
     <t>Workbooks Path</t>
   </si>
   <si>
-    <t>ワークボックスパス</t>
+    <t>ワークブックフォルダのパス</t>
   </si>
   <si>
     <t>FormUsernameLabel</t>
@@ -796,6 +799,105 @@
     <t>キャンセル</t>
   </si>
   <si>
+    <t>FormOnPremisesOrchestratorTooltip</t>
+  </si>
+  <si>
+    <t>On-premises instance of Orchestrator.</t>
+  </si>
+  <si>
+    <t>オンプレミスのOrchestrator。</t>
+  </si>
+  <si>
+    <t>FormCloudOrchestratorTooltip</t>
+  </si>
+  <si>
+    <t>Orchestrator hosted on UiPath Cloud Automation.</t>
+  </si>
+  <si>
+    <t>UiPath Cloud AutomationのOrchestrator。</t>
+  </si>
+  <si>
+    <t>FormOrchestratorVersionTooltip</t>
+  </si>
+  <si>
+    <t>Version of the on-premises Orchestrator version to be used.</t>
+  </si>
+  <si>
+    <t>オンプレミスのOrchestratorのバージョン。</t>
+  </si>
+  <si>
+    <t>FormUsernameTooltip</t>
+  </si>
+  <si>
+    <t>Username of the user to log into Orchestrator.</t>
+  </si>
+  <si>
+    <t>Orchestratorにログインするユーザーのユーザー名。</t>
+  </si>
+  <si>
+    <t>FormPasswordTooltip</t>
+  </si>
+  <si>
+    <t>Password of the user to log into Orchestrator.</t>
+  </si>
+  <si>
+    <t>Orchestratorにログインするユーザーのパスワード。</t>
+  </si>
+  <si>
+    <t>FormOrchestratorURLTooltip</t>
+  </si>
+  <si>
+    <t xml:space="preserve">URL of the Orchestrator instance to be used. </t>
+  </si>
+  <si>
+    <t>OrchestratorのURL。</t>
+  </si>
+  <si>
+    <t>FormTenantNameTooltip</t>
+  </si>
+  <si>
+    <t>Name of the tenant to be used by Orchestrator Manager.</t>
+  </si>
+  <si>
+    <t>Orchestrator Managerが利用するテナント名。</t>
+  </si>
+  <si>
+    <t>FormUserKeyTooltip</t>
+  </si>
+  <si>
+    <t>Unique login key to be used with UiPath Automation Cloud's API. Consult the UiPath Automation Cloud documentation for more information.</t>
+  </si>
+  <si>
+    <t>代わりにログインしてアクションを実行するためにUiPath Automation Cloud APIで使用する一意のログイン キー。詳細はUiPath Automation Cloudガイドを参考してください。</t>
+  </si>
+  <si>
+    <t>FormClientIDTooltip</t>
+  </si>
+  <si>
+    <t>ID specific to the Orchestrator application itself. Consult the UiPath Automation Cloud documentation for more information.</t>
+  </si>
+  <si>
+    <t>Orchestratorアプリケーション自体のID。詳細はUiPath Autiomation Cloudガイドを参考してください。</t>
+  </si>
+  <si>
+    <t>FormAccountNameTooltip</t>
+  </si>
+  <si>
+    <t>Unique account name for UiPath Automation Cloud organization. For example, assuming that the organization account URL is https://cloud.uipath.com/SampleAccount, the Account Name is SampleAccount.</t>
+  </si>
+  <si>
+    <t>UiPath Automation Cloud上の一意組織ID。例えば、Automation Cloudの組織のURLはhttps://cloud.uipath.com/SampleAccountであれば、アカウントの論理名はSampleAccountです。</t>
+  </si>
+  <si>
+    <t>FormWorkbooksFolderPathTooltip</t>
+  </si>
+  <si>
+    <t>Path to the folder to which entities workbooks should be saved.</t>
+  </si>
+  <si>
+    <t>エンティティワークブックを保存するフォルダーのパス。</t>
+  </si>
+  <si>
     <t>AssetConfigFilePath</t>
   </si>
   <si>
@@ -982,7 +1084,7 @@
     <t>Rollback to Previous Package</t>
   </si>
   <si>
-    <t>以前使用していたバージョンに戻す</t>
+    <t>ひとつ前のバージョンに戻す</t>
   </si>
   <si>
     <t>DownloadQueueItemsOperationName</t>
@@ -1081,7 +1183,7 @@
     <t>Unable to get access token due to failed authentication. Server response: {0}</t>
   </si>
   <si>
-    <t>認証に失敗したため、アクセス トークンを取得できません。サーバーレスポンス：{0}</t>
+    <t>認証に失敗したため、アクセス トークンを取得できません。サーバーレスポンス：{0}。</t>
   </si>
   <si>
     <t>AuthenticationFailed</t>
@@ -1162,7 +1264,8 @@
     <t>HTTP Request failed due to invalid response. Please confirm the specified Orchestrator URL and version.</t>
   </si>
   <si>
-    <t>レスポンスが無効なため、リクエストが失敗しました。指定されたOrchestratorのURLやバージョンなどを確認してください。</t>
+    <t>レスポンスが無効なため、リクエストが失敗しました。
+指定されたOrchestratorのURLやバージョンなどを確認してください。</t>
   </si>
   <si>
     <t>ConfirmNumerousRequests</t>
@@ -1312,10 +1415,21 @@
     <t>FailedToGetDataFromOUFolder</t>
   </si>
   <si>
-    <t>Failed to get data from Folder (Organization Unit) named {0}.</t>
-  </si>
-  <si>
-    <t>{0}というフォルダー（組織単位）からデータを取得することができませんでした。</t>
+    <t>Failed to get data from Folder (Organization Unit) named {0}. Please verify access restrictions.</t>
+  </si>
+  <si>
+    <t>{0}というフォルダー（組織単位）からデータを取得することができませんでした。
+アクセス制限を確認してください。</t>
+  </si>
+  <si>
+    <t>FailedToAccessOUFolder</t>
+  </si>
+  <si>
+    <t>It was not possible to access all Folders (Organization Units). Please check logs for more details.</t>
+  </si>
+  <si>
+    <t>全てのフォルダーをアクセスすることができませんでした。
+詳細はログを確認してください。</t>
   </si>
   <si>
     <t>ErrorMessageBoxTitle</t>
@@ -1940,9 +2054,6 @@
   </si>
   <si>
     <t>SampleAccount</t>
-  </si>
-  <si>
-    <t>https://myOrchestratorURL</t>
   </si>
 </sst>
 </file>
@@ -2035,8 +2146,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table13" displayName="Table13" ref="A1:C172" totalsRowShown="0">
-  <autoFilter ref="A1:C172" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table13" displayName="Table13" ref="A1:C184" totalsRowShown="0">
+  <autoFilter ref="A1:C184" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Name"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="EN"/>
@@ -2357,7 +2468,7 @@
         <v>7</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>629</v>
+        <v>666</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>8</v>
@@ -2379,21 +2490,21 @@
         <v>12</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>630</v>
+        <v>13</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="159.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B7" s="1">
         <v>201804</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -2433,684 +2544,684 @@
     </row>
     <row r="2" spans="1:3" ht="101.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B2" s="1">
         <v>200</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B3" s="1">
         <v>0</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B4" s="1">
         <v>550</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B5" s="1">
         <v>650</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B6" s="1">
         <v>3</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B7" s="1">
         <v>5000</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A30" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="1" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A33" s="1" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A34" s="1" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A35" s="1" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A36" s="1" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A37" s="1" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A38" s="1" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A39" s="1" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A40" s="1" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="41" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A41" s="1" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
     </row>
     <row r="42" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A42" s="1" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="43" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A43" s="1" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A44" s="1" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="45" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A45" s="1" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
     <row r="46" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A46" s="1" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
     </row>
     <row r="47" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A47" s="1" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
     </row>
     <row r="48" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A48" s="1" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A49" s="1" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="50" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A50" s="1" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
     </row>
     <row r="51" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A51" s="1" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A52" s="1" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="53" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A53" s="1" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="54" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A54" s="1" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A55" s="1" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
     </row>
     <row r="56" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A56" s="1" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
     </row>
     <row r="57" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A57" s="1" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
     </row>
     <row r="58" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A58" s="1" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
     </row>
     <row r="59" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A59" s="1" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
     </row>
     <row r="60" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A60" s="1" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
     </row>
     <row r="61" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A61" s="1" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
     </row>
     <row r="62" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A62" s="1" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
     </row>
     <row r="63" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A63" s="1" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
   </sheetData>
@@ -3128,7 +3239,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1927ABA9-1814-4487-9CEC-ABDCAF91481F}">
-  <dimension ref="A1:C172"/>
+  <dimension ref="A1:C184"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -3146,465 +3257,472 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="43.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A30" s="1" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A31" s="1" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A32" s="1" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B33" s="2"/>
-      <c r="C33" s="2"/>
+      <c r="A33" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>251</v>
+      </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A34" s="1" t="s">
-        <v>248</v>
+        <v>252</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>249</v>
+        <v>253</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>250</v>
+        <v>254</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A35" s="1" t="s">
-        <v>251</v>
+        <v>255</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>252</v>
+        <v>256</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>253</v>
+        <v>257</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A36" s="1" t="s">
-        <v>254</v>
+        <v>258</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>255</v>
+        <v>259</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>256</v>
+        <v>260</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A37" s="1" t="s">
-        <v>257</v>
+        <v>261</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>258</v>
+        <v>262</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>259</v>
+        <v>263</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A38" s="1" t="s">
-        <v>260</v>
-      </c>
-      <c r="B38" s="2" t="s">
-        <v>261</v>
-      </c>
-      <c r="C38" s="2" t="s">
-        <v>262</v>
+        <v>264</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>266</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A39" s="1" t="s">
-        <v>263</v>
+        <v>267</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>264</v>
+        <v>268</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" ht="43.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A40" s="1" t="s">
-        <v>266</v>
+        <v>270</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>267</v>
+        <v>271</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A41" s="1" t="s">
-        <v>269</v>
+        <v>273</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>270</v>
+        <v>274</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" ht="58" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A42" s="1" t="s">
-        <v>272</v>
+        <v>276</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>273</v>
+        <v>277</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A43" s="1" t="s">
-        <v>275</v>
+        <v>279</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>276</v>
+        <v>280</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.35">
@@ -3613,1313 +3731,1438 @@
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A45" s="1" t="s">
-        <v>278</v>
+        <v>282</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>279</v>
+        <v>283</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A46" s="1" t="s">
-        <v>281</v>
+        <v>285</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>282</v>
+        <v>286</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>283</v>
+        <v>287</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A47" s="1" t="s">
-        <v>284</v>
+        <v>288</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>285</v>
+        <v>289</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>286</v>
+        <v>290</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A48" s="1" t="s">
-        <v>287</v>
+        <v>291</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>288</v>
+        <v>292</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>289</v>
+        <v>293</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A49" s="1" t="s">
-        <v>290</v>
+        <v>294</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>291</v>
+        <v>295</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>292</v>
+        <v>296</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A50" s="1" t="s">
-        <v>293</v>
+        <v>297</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>294</v>
+        <v>298</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>295</v>
+        <v>299</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A51" s="1" t="s">
-        <v>296</v>
+        <v>300</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>297</v>
+        <v>301</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>298</v>
+        <v>302</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A52" s="1" t="s">
-        <v>299</v>
+        <v>303</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>300</v>
+        <v>304</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>301</v>
+        <v>305</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A53" s="1" t="s">
-        <v>302</v>
+        <v>306</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>303</v>
+        <v>307</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>304</v>
+        <v>308</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A54" s="1" t="s">
-        <v>305</v>
+        <v>309</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>306</v>
+        <v>310</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>307</v>
+        <v>311</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A55" s="1" t="s">
-        <v>308</v>
-      </c>
-      <c r="B55" s="2" t="s">
-        <v>309</v>
-      </c>
-      <c r="C55" s="2" t="s">
-        <v>310</v>
-      </c>
+      <c r="B55" s="2"/>
+      <c r="C55" s="2"/>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A56" s="1" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A57" s="1" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A58" s="1" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A59" s="1" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A60" s="1" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A61" s="1" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A62" s="1" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A63" s="1" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A64" s="1" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A65" s="1" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A66" s="1" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A67" s="1" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A68" s="1" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A69" s="1" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A70" s="1" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A71" s="1" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A72" s="1" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A73" s="1" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="74" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A74" s="1" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>367</v>
-      </c>
-    </row>
-    <row r="75" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A75" s="1" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="76" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A76" s="1" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>373</v>
-      </c>
-    </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.35">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A77" s="1" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A78" s="1" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A79" s="1" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A80" s="1" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A81" s="1" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A82" s="1" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A83" s="1" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A84" s="1" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>397</v>
-      </c>
-    </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.35">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A85" s="1" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.35">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A86" s="1" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.35">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A87" s="1" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A88" s="1" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A89" s="1" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A90" s="1" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A91" s="1" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A92" s="1" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A93" s="1" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>424</v>
+        <v>425</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A94" s="1" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>426</v>
+        <v>427</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B95" s="2"/>
-      <c r="C95" s="2"/>
+      <c r="A95" s="1" t="s">
+        <v>429</v>
+      </c>
+      <c r="B95" s="2" t="s">
+        <v>430</v>
+      </c>
+      <c r="C95" s="2" t="s">
+        <v>431</v>
+      </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A96" s="1" t="s">
-        <v>428</v>
+        <v>432</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>429</v>
+        <v>433</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>430</v>
+        <v>434</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A97" s="1" t="s">
-        <v>431</v>
+        <v>435</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>432</v>
+        <v>436</v>
       </c>
       <c r="C97" s="2" t="s">
-        <v>433</v>
+        <v>437</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A98" s="1" t="s">
-        <v>434</v>
+        <v>438</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>435</v>
+        <v>439</v>
       </c>
       <c r="C98" s="2" t="s">
-        <v>436</v>
+        <v>440</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A99" s="1" t="s">
-        <v>437</v>
+        <v>441</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>438</v>
+        <v>442</v>
       </c>
       <c r="C99" s="2" t="s">
-        <v>439</v>
+        <v>443</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A100" s="1" t="s">
-        <v>440</v>
+        <v>444</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>441</v>
+        <v>445</v>
       </c>
       <c r="C100" s="2" t="s">
-        <v>442</v>
+        <v>446</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A101" s="1" t="s">
-        <v>443</v>
+        <v>447</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>444</v>
+        <v>448</v>
       </c>
       <c r="C101" s="2" t="s">
-        <v>445</v>
+        <v>449</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A102" s="1" t="s">
-        <v>446</v>
+        <v>450</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>447</v>
+        <v>451</v>
       </c>
       <c r="C102" s="2" t="s">
-        <v>448</v>
-      </c>
-    </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.35">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A103" s="1" t="s">
-        <v>449</v>
+        <v>453</v>
       </c>
       <c r="B103" s="2" t="s">
-        <v>450</v>
+        <v>454</v>
       </c>
       <c r="C103" s="2" t="s">
-        <v>451</v>
-      </c>
-    </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B104" s="2"/>
-      <c r="C104" s="2"/>
+        <v>455</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A104" s="1" t="s">
+        <v>456</v>
+      </c>
+      <c r="B104" s="2" t="s">
+        <v>457</v>
+      </c>
+      <c r="C104" s="2" t="s">
+        <v>458</v>
+      </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A105" s="1" t="s">
-        <v>452</v>
+        <v>459</v>
       </c>
       <c r="B105" s="2" t="s">
-        <v>453</v>
+        <v>460</v>
       </c>
       <c r="C105" s="2" t="s">
-        <v>454</v>
+        <v>461</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A106" s="1" t="s">
-        <v>455</v>
+        <v>462</v>
       </c>
       <c r="B106" s="2" t="s">
-        <v>456</v>
+        <v>463</v>
       </c>
       <c r="C106" s="2" t="s">
-        <v>457</v>
+        <v>464</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A107" s="1" t="s">
-        <v>458</v>
-      </c>
-      <c r="B107" s="2" t="s">
-        <v>459</v>
-      </c>
-      <c r="C107" s="2" t="s">
-        <v>460</v>
-      </c>
+      <c r="B107" s="2"/>
+      <c r="C107" s="2"/>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A108" s="1" t="s">
-        <v>461</v>
+        <v>465</v>
       </c>
       <c r="B108" s="2" t="s">
-        <v>462</v>
+        <v>466</v>
       </c>
       <c r="C108" s="2" t="s">
-        <v>463</v>
+        <v>467</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A109" s="1" t="s">
-        <v>464</v>
+        <v>468</v>
       </c>
       <c r="B109" s="2" t="s">
-        <v>465</v>
+        <v>469</v>
       </c>
       <c r="C109" s="2" t="s">
-        <v>466</v>
+        <v>470</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A110" s="1" t="s">
-        <v>467</v>
+        <v>471</v>
       </c>
       <c r="B110" s="2" t="s">
-        <v>468</v>
+        <v>472</v>
       </c>
       <c r="C110" s="2" t="s">
-        <v>469</v>
+        <v>473</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A111" s="1" t="s">
-        <v>470</v>
+        <v>474</v>
       </c>
       <c r="B111" s="2" t="s">
-        <v>471</v>
+        <v>475</v>
       </c>
       <c r="C111" s="2" t="s">
-        <v>472</v>
+        <v>476</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A112" s="1" t="s">
-        <v>473</v>
+        <v>477</v>
       </c>
       <c r="B112" s="2" t="s">
-        <v>474</v>
+        <v>478</v>
       </c>
       <c r="C112" s="2" t="s">
-        <v>475</v>
+        <v>479</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A113" s="1" t="s">
-        <v>476</v>
+        <v>480</v>
       </c>
       <c r="B113" s="2" t="s">
-        <v>477</v>
+        <v>481</v>
       </c>
       <c r="C113" s="2" t="s">
-        <v>478</v>
+        <v>482</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B114" s="2"/>
-      <c r="C114" s="2"/>
+      <c r="A114" s="1" t="s">
+        <v>483</v>
+      </c>
+      <c r="B114" s="2" t="s">
+        <v>484</v>
+      </c>
+      <c r="C114" s="2" t="s">
+        <v>485</v>
+      </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A115" s="1" t="s">
-        <v>479</v>
+        <v>486</v>
       </c>
       <c r="B115" s="2" t="s">
-        <v>480</v>
+        <v>487</v>
       </c>
       <c r="C115" s="2" t="s">
-        <v>481</v>
+        <v>488</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A116" s="1" t="s">
-        <v>482</v>
-      </c>
-      <c r="B116" s="2" t="s">
-        <v>483</v>
-      </c>
-      <c r="C116" s="2" t="s">
-        <v>484</v>
-      </c>
+      <c r="B116" s="2"/>
+      <c r="C116" s="2"/>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A117" s="1" t="s">
-        <v>485</v>
+        <v>489</v>
       </c>
       <c r="B117" s="2" t="s">
-        <v>486</v>
+        <v>490</v>
       </c>
       <c r="C117" s="2" t="s">
-        <v>487</v>
+        <v>491</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A118" s="1" t="s">
-        <v>488</v>
+        <v>492</v>
       </c>
       <c r="B118" s="2" t="s">
-        <v>489</v>
+        <v>493</v>
       </c>
       <c r="C118" s="2" t="s">
-        <v>490</v>
+        <v>494</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A119" s="1" t="s">
-        <v>491</v>
+        <v>495</v>
       </c>
       <c r="B119" s="2" t="s">
-        <v>492</v>
+        <v>496</v>
       </c>
       <c r="C119" s="2" t="s">
-        <v>493</v>
+        <v>497</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A120" s="1" t="s">
-        <v>494</v>
+        <v>498</v>
       </c>
       <c r="B120" s="2" t="s">
-        <v>495</v>
+        <v>499</v>
       </c>
       <c r="C120" s="2" t="s">
-        <v>496</v>
+        <v>500</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A121" s="1" t="s">
-        <v>497</v>
+        <v>501</v>
       </c>
       <c r="B121" s="2" t="s">
-        <v>498</v>
+        <v>502</v>
       </c>
       <c r="C121" s="2" t="s">
-        <v>499</v>
+        <v>503</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A122" s="1" t="s">
-        <v>500</v>
+        <v>504</v>
       </c>
       <c r="B122" s="2" t="s">
-        <v>501</v>
+        <v>505</v>
       </c>
       <c r="C122" s="2" t="s">
-        <v>502</v>
+        <v>506</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B123" s="2"/>
-      <c r="C123" s="2"/>
+      <c r="A123" s="1" t="s">
+        <v>507</v>
+      </c>
+      <c r="B123" s="2" t="s">
+        <v>508</v>
+      </c>
+      <c r="C123" s="2" t="s">
+        <v>509</v>
+      </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A124" s="1" t="s">
-        <v>503</v>
+        <v>510</v>
       </c>
       <c r="B124" s="2" t="s">
-        <v>504</v>
+        <v>511</v>
       </c>
       <c r="C124" s="2" t="s">
-        <v>505</v>
+        <v>512</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A125" s="1" t="s">
-        <v>506</v>
+        <v>513</v>
       </c>
       <c r="B125" s="2" t="s">
-        <v>507</v>
+        <v>514</v>
       </c>
       <c r="C125" s="2" t="s">
-        <v>508</v>
+        <v>515</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A126" s="1" t="s">
-        <v>509</v>
-      </c>
-      <c r="B126" s="2" t="s">
-        <v>510</v>
-      </c>
-      <c r="C126" s="2" t="s">
-        <v>511</v>
-      </c>
+      <c r="B126" s="2"/>
+      <c r="C126" s="2"/>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A127" s="1" t="s">
-        <v>512</v>
+        <v>516</v>
       </c>
       <c r="B127" s="2" t="s">
-        <v>513</v>
+        <v>517</v>
       </c>
       <c r="C127" s="2" t="s">
-        <v>514</v>
+        <v>518</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A128" s="1" t="s">
+        <v>519</v>
+      </c>
+      <c r="B128" s="2" t="s">
+        <v>520</v>
+      </c>
+      <c r="C128" s="2" t="s">
+        <v>521</v>
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A129" s="1" t="s">
-        <v>515</v>
+        <v>522</v>
       </c>
       <c r="B129" s="2" t="s">
-        <v>516</v>
+        <v>523</v>
       </c>
       <c r="C129" s="2" t="s">
-        <v>517</v>
+        <v>524</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A130" s="1" t="s">
-        <v>518</v>
+        <v>525</v>
       </c>
       <c r="B130" s="2" t="s">
-        <v>519</v>
+        <v>526</v>
       </c>
       <c r="C130" s="2" t="s">
-        <v>520</v>
+        <v>527</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A131" s="1" t="s">
-        <v>521</v>
+        <v>528</v>
       </c>
       <c r="B131" s="2" t="s">
-        <v>522</v>
+        <v>529</v>
       </c>
       <c r="C131" s="2" t="s">
-        <v>523</v>
+        <v>530</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A132" s="1" t="s">
-        <v>524</v>
+        <v>531</v>
       </c>
       <c r="B132" s="2" t="s">
-        <v>525</v>
+        <v>532</v>
       </c>
       <c r="C132" s="2" t="s">
-        <v>526</v>
+        <v>533</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A133" s="1" t="s">
-        <v>527</v>
+        <v>534</v>
       </c>
       <c r="B133" s="2" t="s">
-        <v>528</v>
+        <v>535</v>
       </c>
       <c r="C133" s="2" t="s">
-        <v>529</v>
+        <v>536</v>
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A134" s="1" t="s">
-        <v>530</v>
+        <v>537</v>
       </c>
       <c r="B134" s="2" t="s">
-        <v>531</v>
+        <v>538</v>
       </c>
       <c r="C134" s="2" t="s">
-        <v>532</v>
+        <v>539</v>
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A135" s="1" t="s">
-        <v>533</v>
-      </c>
-      <c r="B135" s="2" t="s">
-        <v>534</v>
-      </c>
-      <c r="C135" s="2" t="s">
-        <v>535</v>
+      <c r="B135" s="2"/>
+      <c r="C135" s="2"/>
+    </row>
+    <row r="136" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A136" s="1" t="s">
+        <v>540</v>
+      </c>
+      <c r="B136" s="2" t="s">
+        <v>541</v>
+      </c>
+      <c r="C136" s="2" t="s">
+        <v>542</v>
       </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A137" s="1" t="s">
-        <v>536</v>
+        <v>543</v>
       </c>
       <c r="B137" s="2" t="s">
-        <v>537</v>
+        <v>544</v>
       </c>
       <c r="C137" s="2" t="s">
-        <v>538</v>
+        <v>545</v>
       </c>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A138" s="1" t="s">
-        <v>539</v>
+        <v>546</v>
       </c>
       <c r="B138" s="2" t="s">
-        <v>540</v>
+        <v>547</v>
       </c>
       <c r="C138" s="2" t="s">
-        <v>541</v>
+        <v>548</v>
       </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A139" s="1" t="s">
-        <v>542</v>
+        <v>549</v>
       </c>
       <c r="B139" s="2" t="s">
-        <v>543</v>
+        <v>550</v>
       </c>
       <c r="C139" s="2" t="s">
-        <v>544</v>
-      </c>
-    </row>
-    <row r="140" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A140" s="1" t="s">
-        <v>545</v>
-      </c>
-      <c r="B140" s="2" t="s">
-        <v>546</v>
-      </c>
-      <c r="C140" s="2" t="s">
-        <v>547</v>
+        <v>551</v>
       </c>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A141" s="1" t="s">
-        <v>548</v>
+        <v>552</v>
       </c>
       <c r="B141" s="2" t="s">
-        <v>549</v>
+        <v>553</v>
       </c>
       <c r="C141" s="2" t="s">
-        <v>550</v>
+        <v>554</v>
+      </c>
+    </row>
+    <row r="142" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A142" s="1" t="s">
+        <v>555</v>
+      </c>
+      <c r="B142" s="2" t="s">
+        <v>556</v>
+      </c>
+      <c r="C142" s="2" t="s">
+        <v>557</v>
       </c>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A143" s="1" t="s">
-        <v>551</v>
+        <v>558</v>
       </c>
       <c r="B143" s="2" t="s">
-        <v>552</v>
+        <v>559</v>
       </c>
       <c r="C143" s="2" t="s">
-        <v>553</v>
+        <v>560</v>
       </c>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A144" s="1" t="s">
-        <v>554</v>
-      </c>
-      <c r="B144" s="1" t="s">
-        <v>555</v>
-      </c>
-      <c r="C144" s="1" t="s">
-        <v>556</v>
+        <v>561</v>
+      </c>
+      <c r="B144" s="2" t="s">
+        <v>562</v>
+      </c>
+      <c r="C144" s="2" t="s">
+        <v>563</v>
       </c>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A145" s="1" t="s">
-        <v>557</v>
-      </c>
-      <c r="B145" s="1" t="s">
-        <v>558</v>
-      </c>
-      <c r="C145" s="1" t="s">
-        <v>559</v>
+        <v>564</v>
+      </c>
+      <c r="B145" s="2" t="s">
+        <v>565</v>
+      </c>
+      <c r="C145" s="2" t="s">
+        <v>566</v>
       </c>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A146" s="1" t="s">
-        <v>560</v>
+        <v>567</v>
       </c>
       <c r="B146" s="2" t="s">
-        <v>561</v>
-      </c>
-      <c r="C146" s="1" t="s">
-        <v>562</v>
+        <v>568</v>
+      </c>
+      <c r="C146" s="2" t="s">
+        <v>569</v>
       </c>
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A147" s="1" t="s">
-        <v>563</v>
-      </c>
-      <c r="B147" s="1" t="s">
-        <v>564</v>
-      </c>
-      <c r="C147" s="1" t="s">
-        <v>565</v>
-      </c>
-    </row>
-    <row r="148" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A148" s="1" t="s">
-        <v>566</v>
-      </c>
-      <c r="B148" s="2" t="s">
-        <v>567</v>
-      </c>
-      <c r="C148" s="2" t="s">
-        <v>568</v>
+        <v>570</v>
+      </c>
+      <c r="B147" s="2" t="s">
+        <v>571</v>
+      </c>
+      <c r="C147" s="2" t="s">
+        <v>572</v>
+      </c>
+    </row>
+    <row r="149" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A149" s="1" t="s">
+        <v>573</v>
+      </c>
+      <c r="B149" s="2" t="s">
+        <v>574</v>
+      </c>
+      <c r="C149" s="2" t="s">
+        <v>575</v>
       </c>
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A150" s="1" t="s">
-        <v>569</v>
+        <v>576</v>
       </c>
       <c r="B150" s="2" t="s">
-        <v>570</v>
+        <v>577</v>
       </c>
       <c r="C150" s="2" t="s">
-        <v>571</v>
+        <v>578</v>
       </c>
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A151" s="1" t="s">
-        <v>572</v>
+        <v>579</v>
       </c>
       <c r="B151" s="2" t="s">
-        <v>573</v>
+        <v>580</v>
       </c>
       <c r="C151" s="2" t="s">
-        <v>574</v>
-      </c>
-    </row>
-    <row r="152" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B152" s="2"/>
-      <c r="C152" s="2"/>
+        <v>581</v>
+      </c>
+    </row>
+    <row r="152" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A152" s="1" t="s">
+        <v>582</v>
+      </c>
+      <c r="B152" s="2" t="s">
+        <v>583</v>
+      </c>
+      <c r="C152" s="2" t="s">
+        <v>584</v>
+      </c>
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A153" s="1" t="s">
-        <v>575</v>
+        <v>585</v>
       </c>
       <c r="B153" s="2" t="s">
-        <v>576</v>
+        <v>586</v>
       </c>
       <c r="C153" s="2" t="s">
-        <v>577</v>
-      </c>
-    </row>
-    <row r="154" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A154" s="1" t="s">
-        <v>578</v>
-      </c>
-      <c r="B154" s="2" t="s">
-        <v>579</v>
-      </c>
-      <c r="C154" s="2" t="s">
-        <v>580</v>
+        <v>587</v>
       </c>
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A155" s="1" t="s">
-        <v>581</v>
+        <v>588</v>
       </c>
       <c r="B155" s="2" t="s">
-        <v>582</v>
+        <v>589</v>
       </c>
       <c r="C155" s="2" t="s">
-        <v>583</v>
+        <v>590</v>
       </c>
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A156" s="1" t="s">
-        <v>584</v>
-      </c>
-      <c r="B156" s="2" t="s">
-        <v>585</v>
-      </c>
-      <c r="C156" s="2" t="s">
-        <v>586</v>
+        <v>591</v>
+      </c>
+      <c r="B156" s="1" t="s">
+        <v>592</v>
+      </c>
+      <c r="C156" s="1" t="s">
+        <v>593</v>
       </c>
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A157" s="1" t="s">
-        <v>587</v>
-      </c>
-      <c r="B157" s="2" t="s">
-        <v>588</v>
-      </c>
-      <c r="C157" s="2" t="s">
-        <v>589</v>
+        <v>594</v>
+      </c>
+      <c r="B157" s="1" t="s">
+        <v>595</v>
+      </c>
+      <c r="C157" s="1" t="s">
+        <v>596</v>
       </c>
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B158" s="2"/>
-      <c r="C158" s="2"/>
+      <c r="A158" s="1" t="s">
+        <v>597</v>
+      </c>
+      <c r="B158" s="2" t="s">
+        <v>598</v>
+      </c>
+      <c r="C158" s="1" t="s">
+        <v>599</v>
+      </c>
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A159" s="1" t="s">
-        <v>590</v>
-      </c>
-      <c r="B159" s="2" t="s">
-        <v>591</v>
-      </c>
-      <c r="C159" s="2" t="s">
-        <v>592</v>
+        <v>600</v>
+      </c>
+      <c r="B159" s="1" t="s">
+        <v>601</v>
+      </c>
+      <c r="C159" s="1" t="s">
+        <v>602</v>
       </c>
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A160" s="1" t="s">
-        <v>593</v>
+        <v>603</v>
       </c>
       <c r="B160" s="2" t="s">
-        <v>594</v>
+        <v>604</v>
       </c>
       <c r="C160" s="2" t="s">
-        <v>595</v>
-      </c>
-    </row>
-    <row r="161" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A161" s="1" t="s">
-        <v>596</v>
-      </c>
-      <c r="B161" s="2" t="s">
-        <v>597</v>
-      </c>
-      <c r="C161" s="2" t="s">
-        <v>598</v>
+        <v>605</v>
       </c>
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A162" s="1" t="s">
-        <v>599</v>
+        <v>606</v>
       </c>
       <c r="B162" s="2" t="s">
-        <v>600</v>
+        <v>607</v>
       </c>
       <c r="C162" s="2" t="s">
-        <v>601</v>
+        <v>608</v>
       </c>
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A163" s="1" t="s">
-        <v>602</v>
+        <v>609</v>
       </c>
       <c r="B163" s="2" t="s">
-        <v>603</v>
+        <v>610</v>
       </c>
       <c r="C163" s="2" t="s">
-        <v>604</v>
+        <v>611</v>
       </c>
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A164" s="1" t="s">
-        <v>605</v>
-      </c>
-      <c r="B164" s="2" t="s">
-        <v>606</v>
-      </c>
-      <c r="C164" s="2" t="s">
-        <v>607</v>
+      <c r="B164" s="2"/>
+      <c r="C164" s="2"/>
+    </row>
+    <row r="165" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A165" s="1" t="s">
+        <v>612</v>
+      </c>
+      <c r="B165" s="2" t="s">
+        <v>613</v>
+      </c>
+      <c r="C165" s="2" t="s">
+        <v>614</v>
       </c>
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A166" s="1" t="s">
-        <v>608</v>
-      </c>
-      <c r="B166" s="1" t="s">
-        <v>609</v>
-      </c>
-      <c r="C166" s="1" t="s">
-        <v>610</v>
+        <v>615</v>
+      </c>
+      <c r="B166" s="2" t="s">
+        <v>616</v>
+      </c>
+      <c r="C166" s="2" t="s">
+        <v>617</v>
       </c>
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A167" s="1" t="s">
-        <v>611</v>
-      </c>
-      <c r="B167" s="1" t="s">
-        <v>612</v>
-      </c>
-      <c r="C167" s="1" t="s">
-        <v>613</v>
+        <v>618</v>
+      </c>
+      <c r="B167" s="2" t="s">
+        <v>619</v>
+      </c>
+      <c r="C167" s="2" t="s">
+        <v>620</v>
       </c>
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A168" s="1" t="s">
-        <v>614</v>
-      </c>
-      <c r="B168" s="1" t="s">
-        <v>615</v>
-      </c>
-      <c r="C168" s="1" t="s">
-        <v>616</v>
+        <v>621</v>
+      </c>
+      <c r="B168" s="2" t="s">
+        <v>622</v>
+      </c>
+      <c r="C168" s="2" t="s">
+        <v>623</v>
       </c>
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A169" s="1" t="s">
-        <v>617</v>
-      </c>
-      <c r="B169" s="1" t="s">
-        <v>618</v>
-      </c>
-      <c r="C169" s="1" t="s">
-        <v>619</v>
+        <v>624</v>
+      </c>
+      <c r="B169" s="2" t="s">
+        <v>625</v>
+      </c>
+      <c r="C169" s="2" t="s">
+        <v>626</v>
       </c>
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A170" s="1" t="s">
-        <v>620</v>
-      </c>
-      <c r="B170" s="2" t="s">
-        <v>621</v>
-      </c>
-      <c r="C170" s="2" t="s">
-        <v>622</v>
-      </c>
+      <c r="B170" s="2"/>
+      <c r="C170" s="2"/>
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A171" s="1" t="s">
-        <v>623</v>
-      </c>
-      <c r="B171" s="1" t="s">
-        <v>624</v>
-      </c>
-      <c r="C171" s="1" t="s">
-        <v>625</v>
+        <v>627</v>
+      </c>
+      <c r="B171" s="2" t="s">
+        <v>628</v>
+      </c>
+      <c r="C171" s="2" t="s">
+        <v>629</v>
       </c>
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A172" s="1" t="s">
-        <v>626</v>
-      </c>
-      <c r="B172" s="1" t="s">
-        <v>627</v>
-      </c>
-      <c r="C172" s="1" t="s">
-        <v>628</v>
+        <v>630</v>
+      </c>
+      <c r="B172" s="2" t="s">
+        <v>631</v>
+      </c>
+      <c r="C172" s="2" t="s">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="173" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A173" s="1" t="s">
+        <v>633</v>
+      </c>
+      <c r="B173" s="2" t="s">
+        <v>634</v>
+      </c>
+      <c r="C173" s="2" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="174" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A174" s="1" t="s">
+        <v>636</v>
+      </c>
+      <c r="B174" s="2" t="s">
+        <v>637</v>
+      </c>
+      <c r="C174" s="2" t="s">
+        <v>638</v>
+      </c>
+    </row>
+    <row r="175" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A175" s="1" t="s">
+        <v>639</v>
+      </c>
+      <c r="B175" s="2" t="s">
+        <v>640</v>
+      </c>
+      <c r="C175" s="2" t="s">
+        <v>641</v>
+      </c>
+    </row>
+    <row r="176" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A176" s="1" t="s">
+        <v>642</v>
+      </c>
+      <c r="B176" s="2" t="s">
+        <v>643</v>
+      </c>
+      <c r="C176" s="2" t="s">
+        <v>644</v>
+      </c>
+    </row>
+    <row r="178" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A178" s="1" t="s">
+        <v>645</v>
+      </c>
+      <c r="B178" s="1" t="s">
+        <v>646</v>
+      </c>
+      <c r="C178" s="1" t="s">
+        <v>647</v>
+      </c>
+    </row>
+    <row r="179" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A179" s="1" t="s">
+        <v>648</v>
+      </c>
+      <c r="B179" s="1" t="s">
+        <v>649</v>
+      </c>
+      <c r="C179" s="1" t="s">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="180" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A180" s="1" t="s">
+        <v>651</v>
+      </c>
+      <c r="B180" s="1" t="s">
+        <v>652</v>
+      </c>
+      <c r="C180" s="1" t="s">
+        <v>653</v>
+      </c>
+    </row>
+    <row r="181" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A181" s="1" t="s">
+        <v>654</v>
+      </c>
+      <c r="B181" s="1" t="s">
+        <v>655</v>
+      </c>
+      <c r="C181" s="1" t="s">
+        <v>656</v>
+      </c>
+    </row>
+    <row r="182" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A182" s="1" t="s">
+        <v>657</v>
+      </c>
+      <c r="B182" s="2" t="s">
+        <v>658</v>
+      </c>
+      <c r="C182" s="2" t="s">
+        <v>659</v>
+      </c>
+    </row>
+    <row r="183" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A183" s="1" t="s">
+        <v>660</v>
+      </c>
+      <c r="B183" s="1" t="s">
+        <v>661</v>
+      </c>
+      <c r="C183" s="1" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="184" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A184" s="1" t="s">
+        <v>663</v>
+      </c>
+      <c r="B184" s="1" t="s">
+        <v>664</v>
+      </c>
+      <c r="C184" s="1" t="s">
+        <v>665</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Cache and reuse data about Packages
</commit_message>
<xml_diff>
--- a/Config.xlsx
+++ b/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mateus.cruz\Documents\GitHub\OrchestratorManager\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5E64417-79F2-4780-ADE4-D303AD1CC6C5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5FC3768-9D05-46EE-845B-2D864E50293E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="715" uniqueCount="667">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="721" uniqueCount="673">
   <si>
     <t>Name</t>
   </si>
@@ -547,6 +547,9 @@
     <t>Please mind that many unsuccessful login attempts can temporarily lock the account, as specified in the Security settings of the tenant.</t>
   </si>
   <si>
+    <t>ログイン試行に複数回失敗した場合、テナントのセキュリティ設定で指定した秒数の間、アカウントがロックされることがありますのでご注意ください。</t>
+  </si>
+  <si>
     <t>FormOrchestratorVersionLabel</t>
   </si>
   <si>
@@ -595,6 +598,9 @@
     <t>Account Name</t>
   </si>
   <si>
+    <t>アカウント名</t>
+  </si>
+  <si>
     <t>FormClientIDLabel</t>
   </si>
   <si>
@@ -619,6 +625,9 @@
     <t>Workbooks Path</t>
   </si>
   <si>
+    <t>ブックのパス</t>
+  </si>
+  <si>
     <t>FormUsernameLabel</t>
   </si>
   <si>
@@ -679,12 +688,18 @@
     <t>Use credential stored in Windows's Credential Manager.</t>
   </si>
   <si>
+    <t>Windows の資格情報マネージャーに保存されている資格情報を使用します。</t>
+  </si>
+  <si>
     <t>FormSaveCredentialLabel</t>
   </si>
   <si>
     <t>Save credential in Windows's Credential Manager.</t>
   </si>
   <si>
+    <t>Windows の資格情報マネージャーに資格情報を保存します。</t>
+  </si>
+  <si>
     <t>FormAssetOption</t>
   </si>
   <si>
@@ -727,6 +742,9 @@
     <t>Environment</t>
   </si>
   <si>
+    <t>ロボット グループ</t>
+  </si>
+  <si>
     <t>FormProcessOption</t>
   </si>
   <si>
@@ -787,1029 +805,487 @@
     <t>On-premises instance of Orchestrator.</t>
   </si>
   <si>
+    <t>Orchestrator のオンプレミス インスタンスです。</t>
+  </si>
+  <si>
     <t>FormCloudOrchestratorTooltip</t>
   </si>
   <si>
+    <t>Orchestrator hosted on UiPath Automation Cloud.</t>
+  </si>
+  <si>
+    <t>UiPath Automation Cloud でホストされている Orchestrator です。</t>
+  </si>
+  <si>
     <t>FormOrchestratorVersionTooltip</t>
   </si>
   <si>
     <t>Version of the on-premises Orchestrator version to be used.</t>
   </si>
   <si>
+    <t>使用するオンプレミス版 Orchestrator のバージョンです。</t>
+  </si>
+  <si>
     <t>FormUsernameTooltip</t>
   </si>
   <si>
     <t>Username of the user to log into Orchestrator.</t>
   </si>
   <si>
+    <t>Orchestrator にログインするユーザーのユーザー名です。</t>
+  </si>
+  <si>
     <t>FormPasswordTooltip</t>
   </si>
   <si>
     <t>Password of the user to log into Orchestrator.</t>
   </si>
   <si>
+    <t>Orchestrator にログインするユーザーのパスワードです。</t>
+  </si>
+  <si>
     <t>FormOrchestratorURLTooltip</t>
   </si>
   <si>
     <t xml:space="preserve">URL of the Orchestrator instance to be used. </t>
   </si>
   <si>
+    <t>使用する Orchestrator インスタンスの URL です。</t>
+  </si>
+  <si>
     <t>FormTenantNameTooltip</t>
   </si>
   <si>
     <t>Name of the tenant to be used by Orchestrator Manager.</t>
   </si>
   <si>
+    <t>Orchestrator Manager が使用するテナントの名前です。</t>
+  </si>
+  <si>
     <t>FormUserKeyTooltip</t>
   </si>
   <si>
-    <t>Unique login key to be used with UiPath Automation Cloud's API. Consult the UiPath Automation Cloud documentation for more information.</t>
+    <t>Unique login key to be used with UiPath Automation Cloud's API. 
+Consult the UiPath Automation Cloud documentation for more information.</t>
+  </si>
+  <si>
+    <t>UiPath Automation Cloud の API で使用する一意のログイン キーです。
+詳しくは UiPath Automation Cloud ガイドをご確認ください。</t>
   </si>
   <si>
     <t>FormClientIDTooltip</t>
   </si>
   <si>
-    <t>ID specific to the Orchestrator application itself. Consult the UiPath Automation Cloud documentation for more information.</t>
-  </si>
-  <si>
-    <t>FormAccountNameTooltip</t>
-  </si>
-  <si>
-    <t>Unique account name for UiPath Automation Cloud organization. For example, assuming that the organization account URL is https://cloud.uipath.com/SampleAccount, the Account Name is SampleAccount.</t>
-  </si>
-  <si>
-    <t>FormWorkbooksFolderPathTooltip</t>
-  </si>
-  <si>
-    <t>Path to the folder to which entities workbooks should be saved.</t>
-  </si>
-  <si>
-    <t>AssetConfigFilePath</t>
-  </si>
-  <si>
-    <t>Assets.xlsx</t>
-  </si>
-  <si>
-    <t>アセット.xlsx</t>
-  </si>
-  <si>
-    <t>UserConfigFilePath</t>
-  </si>
-  <si>
-    <t>Users.xlsx</t>
-  </si>
-  <si>
-    <t>ユーザー.xlsx</t>
-  </si>
-  <si>
-    <t>RobotConfigFilePath</t>
-  </si>
-  <si>
-    <t>Robots.xlsx</t>
-  </si>
-  <si>
-    <t>ロボット.xlsx</t>
-  </si>
-  <si>
-    <t>MachineConfigFilePath</t>
-  </si>
-  <si>
-    <t>Machines.xlsx</t>
-  </si>
-  <si>
-    <t>マシン.xlsx</t>
-  </si>
-  <si>
-    <t>EnvironmentConfigFilePath</t>
-  </si>
-  <si>
-    <t>Environments.xlsx</t>
-  </si>
-  <si>
-    <t>ProcessConfigFilePath</t>
-  </si>
-  <si>
-    <t>Processes.xlsx</t>
-  </si>
-  <si>
-    <t>プロセス.xlsx</t>
-  </si>
-  <si>
-    <t>OrganizationUnitConfigFilePath</t>
-  </si>
-  <si>
-    <t>OrganizationUnits.xlsx</t>
-  </si>
-  <si>
-    <t>組織単位.xlsx</t>
-  </si>
-  <si>
-    <t>FolderConfigFilePath</t>
-  </si>
-  <si>
-    <t>Folders.xlsx</t>
-  </si>
-  <si>
-    <t>フォルダー.xlsx</t>
-  </si>
-  <si>
-    <t>QueueConfigFilePath</t>
-  </si>
-  <si>
-    <t>Queues.xlsx</t>
-  </si>
-  <si>
-    <t>キュー.xlsx</t>
-  </si>
-  <si>
-    <t>PackageConfigFilePath</t>
-  </si>
-  <si>
-    <t>Packages.xlsx</t>
-  </si>
-  <si>
-    <t>パッケージ.xlsx</t>
-  </si>
-  <si>
-    <t>GetOperationName</t>
-  </si>
-  <si>
-    <t>Get</t>
-  </si>
-  <si>
-    <t>取得</t>
-  </si>
-  <si>
-    <t>CreateOperationName</t>
-  </si>
-  <si>
-    <t>Create</t>
-  </si>
-  <si>
-    <t>作成</t>
-  </si>
-  <si>
-    <t>EditOperationName</t>
-  </si>
-  <si>
-    <t>Edit</t>
-  </si>
-  <si>
-    <t>編集</t>
-  </si>
-  <si>
-    <t>DeleteOperationName</t>
-  </si>
-  <si>
-    <t>Delete</t>
-  </si>
-  <si>
-    <t>削除</t>
-  </si>
-  <si>
-    <t>CreateCredentialOperationName</t>
-  </si>
-  <si>
-    <t>Create Credential</t>
-  </si>
-  <si>
-    <t>Credential 型を作成</t>
-  </si>
-  <si>
-    <t>EditCredentialOperationName</t>
-  </si>
-  <si>
-    <t>Edit Credential</t>
-  </si>
-  <si>
-    <t>Credential 型を編集</t>
-  </si>
-  <si>
-    <t>AddRemoveEnvironmentRobotsOperationName</t>
-  </si>
-  <si>
-    <t>Add or Remove Robots</t>
-  </si>
-  <si>
-    <t>ロボットを追加または削除</t>
-  </si>
-  <si>
-    <t>AddRemoveUserOrganizationUnitsOperationName</t>
-  </si>
-  <si>
-    <t>Add or Remove OUs</t>
-  </si>
-  <si>
-    <t>組織単位を追加または削除</t>
-  </si>
-  <si>
-    <t>AddRemoveUserRolesOperationName</t>
-  </si>
-  <si>
-    <t>Add or Remove Roles</t>
-  </si>
-  <si>
-    <t>ロールを追加または削除</t>
-  </si>
-  <si>
-    <t>UpdateProcessToLatestPackageVersionOperationName</t>
-  </si>
-  <si>
-    <t>Update to Latest Package</t>
-  </si>
-  <si>
-    <t>RollbackProcessToPreviousPackageVersionOperationName</t>
-  </si>
-  <si>
-    <t>Rollback to Previous Package</t>
-  </si>
-  <si>
-    <t>DownloadQueueItemsOperationName</t>
-  </si>
-  <si>
-    <t>Download Queue Items</t>
-  </si>
-  <si>
-    <t>UploadQueueItemsOperationName</t>
-  </si>
-  <si>
-    <t>Upload Queue Items</t>
-  </si>
-  <si>
-    <t>DownloadPackageOperationName</t>
-  </si>
-  <si>
-    <t>Download</t>
-  </si>
-  <si>
-    <t>ダウンロード</t>
-  </si>
-  <si>
-    <t>UploadPackageOperationName</t>
-  </si>
-  <si>
-    <t>Upload</t>
-  </si>
-  <si>
-    <t>アップロード</t>
-  </si>
-  <si>
-    <t>StoppedExecution</t>
-  </si>
-  <si>
-    <t>The execution has been stopped.</t>
-  </si>
-  <si>
-    <t>実行が停止されました。</t>
-  </si>
-  <si>
-    <t>MandatoryArgumentsNotSpecified</t>
-  </si>
-  <si>
-    <t>Mandatory arguments not specified.</t>
-  </si>
-  <si>
-    <t>UnsupportedEntity</t>
-  </si>
-  <si>
-    <t>Unsupported entity specified.</t>
-  </si>
-  <si>
-    <t>UnsupportedOperation</t>
-  </si>
-  <si>
-    <t>Unsupported operation.</t>
-  </si>
-  <si>
-    <t>操作はサポートされていません。</t>
-  </si>
-  <si>
-    <t>OperationDefaultResult</t>
-  </si>
-  <si>
-    <t>Success</t>
-  </si>
-  <si>
-    <t>成功</t>
-  </si>
-  <si>
-    <t>OnPremisesOrchestratorVersionNotSupported</t>
-  </si>
-  <si>
-    <t>The specified Orchestrator version is not supported.</t>
-  </si>
-  <si>
-    <t>TokenNotRetrieved</t>
-  </si>
-  <si>
-    <t>Unable to get access token due to failed authentication. Server response: {0}</t>
-  </si>
-  <si>
-    <t>AuthenticationFailed</t>
-  </si>
-  <si>
-    <t>Authentication failed. Please check logs for more details.</t>
-  </si>
-  <si>
-    <t>ErrorDuringExecutionLog</t>
-  </si>
-  <si>
-    <t>There was an execution error: {0} at {1}.</t>
-  </si>
-  <si>
-    <t>ErrorDuringExecution</t>
-  </si>
-  <si>
-    <t>There was an execution error. Please check logs for more details.</t>
-  </si>
-  <si>
-    <t>TokenExpired</t>
-  </si>
-  <si>
-    <t>Authentication token expired.</t>
-  </si>
-  <si>
-    <t>認証トークンの期限が切れました。</t>
-  </si>
-  <si>
-    <t>UnsupportedHTTPMethod</t>
-  </si>
-  <si>
-    <t>Unsupported HTTP method specified.</t>
-  </si>
-  <si>
-    <t>ParameterNotFound</t>
-  </si>
-  <si>
-    <t>Parameter not found.</t>
-  </si>
-  <si>
-    <t>ConnectivityIssuesFailure</t>
-  </si>
-  <si>
-    <t>HTTP Request failed due to connectivity issues.</t>
-  </si>
-  <si>
-    <t>ServerErrorFailure</t>
-  </si>
-  <si>
-    <t>HTTP Request failed due to server error issues. Request status: {0} / Response: {1}.</t>
-  </si>
-  <si>
-    <t>InvalidResponseErrorFailure</t>
-  </si>
-  <si>
-    <t>HTTP Request failed due to invalid response. Please confirm the specified Orchestrator URL and version.</t>
-  </si>
-  <si>
-    <t>ConfirmNumerousRequests</t>
-  </si>
-  <si>
-    <t>The selected operation will make a large number of HTTP requests that might impact on Orchestrator's infrastructure. Continue the processing?</t>
-  </si>
-  <si>
-    <t>NumerousRequestsNotConfirmed</t>
-  </si>
-  <si>
-    <t>NumerousRequestsConfirmed</t>
-  </si>
-  <si>
-    <t>ProcessEntityFailure</t>
-  </si>
-  <si>
-    <t>Failed to process entity. Request status: {0} / Response: {1}.</t>
-  </si>
-  <si>
-    <t>ProcessedEntity</t>
-  </si>
-  <si>
-    <t>Already processed.</t>
-  </si>
-  <si>
-    <t>既に処理されています。</t>
-  </si>
-  <si>
-    <t>IDInvalidOrNotSpecified</t>
-  </si>
-  <si>
-    <t>ID invalid or not specified.</t>
-  </si>
-  <si>
-    <t>NameNotSpecified</t>
-  </si>
-  <si>
-    <t>Name not specified.</t>
-  </si>
-  <si>
-    <t>VersionNotSpecified</t>
-  </si>
-  <si>
-    <t>Version not specified.</t>
-  </si>
-  <si>
-    <t>IDAndNameDoNotMatch</t>
-  </si>
-  <si>
-    <t>The specified ID and Name do not match.</t>
-  </si>
-  <si>
-    <t>TypeNotSpecified</t>
-  </si>
-  <si>
-    <t>Type not specified.</t>
-  </si>
-  <si>
-    <t>TypeNotSupported</t>
-  </si>
-  <si>
-    <t>The specified type is not supported.</t>
-  </si>
-  <si>
-    <t>CredentialNotFound</t>
-  </si>
-  <si>
-    <t>The specified credential was not found.</t>
-  </si>
-  <si>
-    <t>OperationCanceledByUser</t>
-  </si>
-  <si>
-    <t>Operation canceled by user.</t>
-  </si>
-  <si>
-    <t>ユーザーが操作をキャンセルしました。</t>
-  </si>
-  <si>
-    <t>OUFolderNameNotSpecified</t>
-  </si>
-  <si>
-    <t>Folder (Organization Unit) name not specified.</t>
-  </si>
-  <si>
-    <t>OUFolderNotFound</t>
-  </si>
-  <si>
-    <t>Folder (Organization Unit) not found.</t>
-  </si>
-  <si>
-    <t>OUFolderIDInvalidOrNotSpecified</t>
-  </si>
-  <si>
-    <t>Folder (Organization Unit) ID invalid or not specified.</t>
-  </si>
-  <si>
-    <t>FailedToGetDataFromOUFolder</t>
-  </si>
-  <si>
-    <t>Failed to get data from Folder (Organization Unit) named {0}. Please verify access restrictions.</t>
-  </si>
-  <si>
-    <t>FailedToAccessOUFolder</t>
-  </si>
-  <si>
-    <t>It was not possible to access all Folders (Organization Units). Please check logs for more details.</t>
-  </si>
-  <si>
-    <t>ErrorMessageBoxTitle</t>
-  </si>
-  <si>
-    <t>Error</t>
-  </si>
-  <si>
-    <t>エラー</t>
-  </si>
-  <si>
-    <t>WarningMessageBoxTitle</t>
-  </si>
-  <si>
-    <t>Warning</t>
-  </si>
-  <si>
-    <t>UnsupportedAssetType</t>
-  </si>
-  <si>
-    <t>The specified asset type is not supported.</t>
-  </si>
-  <si>
-    <t>AssetNotFound</t>
-  </si>
-  <si>
-    <t>Asset not found.</t>
-  </si>
-  <si>
-    <t>AssetIDInvalidOrNotSpecified</t>
-  </si>
-  <si>
-    <t>Asset ID invalid or not specified.</t>
-  </si>
-  <si>
-    <t>AssetNameNotSpecified</t>
-  </si>
-  <si>
-    <t>Asset name not specified.</t>
-  </si>
-  <si>
-    <t>AssetIDAndNameDoNotMatch</t>
-  </si>
-  <si>
-    <t>The specified Asset ID and Asset name do not match.</t>
-  </si>
-  <si>
-    <t>InvalidAssetValue</t>
-  </si>
-  <si>
-    <t>Invalid value.</t>
-  </si>
-  <si>
-    <t>EditCredentialUsernameNewPasswordRequired</t>
-  </si>
-  <si>
-    <t>New Password required when changing Username.</t>
-  </si>
-  <si>
-    <t>ユーザー名の編集に新しいパスワードが必要です。</t>
-  </si>
-  <si>
-    <t>PasswordNotSpecified</t>
-  </si>
-  <si>
-    <t>Password not specified.</t>
-  </si>
-  <si>
-    <t>UserNotFound</t>
-  </si>
-  <si>
-    <t>User not  found.</t>
-  </si>
-  <si>
-    <t>StatusNotSupported</t>
-  </si>
-  <si>
-    <t>Status not supported.</t>
-  </si>
-  <si>
-    <t>ステータスはサポートされていません。</t>
-  </si>
-  <si>
-    <t>UsernameNotSpecified</t>
-  </si>
-  <si>
-    <t>Username not specified.</t>
-  </si>
-  <si>
-    <t>IDAndUsernameDoNotMatch</t>
-  </si>
-  <si>
-    <t>The specified ID and Username do not match.</t>
-  </si>
-  <si>
-    <t>SurnameNotSpecified</t>
-  </si>
-  <si>
-    <t>Surname not specified.</t>
-  </si>
-  <si>
-    <t>EmailNotSpecified</t>
-  </si>
-  <si>
-    <t>Email not specified.</t>
-  </si>
-  <si>
-    <t>OUAddedAndRemoved</t>
-  </si>
-  <si>
-    <t>An Organization Unit is being added and removed at the same time.</t>
-  </si>
-  <si>
-    <t>組織単位が同時に追加および削除されています。</t>
-  </si>
-  <si>
-    <t>RoleAddedAndRemoved</t>
-  </si>
-  <si>
-    <t>A Role is being added and removed at the same time.</t>
-  </si>
-  <si>
-    <t>ロールが同時に追加および削除されています。</t>
-  </si>
-  <si>
-    <t>NamedUserNotFound</t>
-  </si>
-  <si>
-    <t>Username {0} not found.</t>
-  </si>
-  <si>
-    <t>ProcessedRobot</t>
-  </si>
-  <si>
-    <t>Robot already processed. Robot name: {0} / ID: {1}.</t>
-  </si>
-  <si>
-    <t>RobotNotFound</t>
-  </si>
-  <si>
-    <t>Robot not found.</t>
-  </si>
-  <si>
-    <t>HostingTypeNotSpecified</t>
-  </si>
-  <si>
-    <t>Hosting Type not specified.</t>
-  </si>
-  <si>
-    <t>RobotNameNotSpecified</t>
-  </si>
-  <si>
-    <t>Robot Name not specified.</t>
-  </si>
-  <si>
-    <t>RobotTypeNotSpecified</t>
-  </si>
-  <si>
-    <t>Robot Type not specified.</t>
-  </si>
-  <si>
-    <t>RobotIDInvalidOrNotSpecified</t>
-  </si>
-  <si>
-    <t>Robot ID invalid or not specified.</t>
-  </si>
-  <si>
-    <t>RobotIDAndNameDoNotMatch</t>
-  </si>
-  <si>
-    <t>The specified Robot ID and name do not match.</t>
-  </si>
-  <si>
-    <t>NamedRobotNotFound</t>
-  </si>
-  <si>
-    <t>Robot named {0} not found.</t>
-  </si>
-  <si>
-    <t>MachineNotFound</t>
-  </si>
-  <si>
-    <t>Machine not found.</t>
-  </si>
-  <si>
-    <t>GetSingleMachineFailure</t>
-  </si>
-  <si>
-    <t>Failed to get machine with ID: {0}. Request status: {1} / Response: {2}.</t>
-  </si>
-  <si>
-    <t>MachineNameNotSpecified</t>
-  </si>
-  <si>
-    <t>Machine Name not specified.</t>
-  </si>
-  <si>
-    <t>NamedMachineNotFound</t>
-  </si>
-  <si>
-    <t>Machine named {0} not found.</t>
-  </si>
-  <si>
-    <t>FolderNotFound</t>
-  </si>
-  <si>
-    <t>Folder not found.</t>
-  </si>
-  <si>
-    <t>FolderIDInvalidOrNotSpecified</t>
-  </si>
-  <si>
-    <t>Folder ID invalid or not specified.</t>
-  </si>
-  <si>
-    <t>FolderNameNotSpecified</t>
-  </si>
-  <si>
-    <t>Folder name not specified.</t>
-  </si>
-  <si>
-    <t>FolderIDAndNameDoNotMatch</t>
-  </si>
-  <si>
-    <t>The specified Folder ID and Folder name do not match.</t>
-  </si>
-  <si>
-    <t>NamedFolderNotFound</t>
-  </si>
-  <si>
-    <t>Folder named {0} not found.</t>
-  </si>
-  <si>
-    <t>RoleAssignmentModelNotSpecified</t>
-  </si>
-  <si>
-    <t>Role Assignment Model not specified.</t>
-  </si>
-  <si>
-    <t>RoleAssignmentModelNotSupported</t>
-  </si>
-  <si>
-    <t>The specified Role Assignment Model is not supported.</t>
-  </si>
-  <si>
-    <t>OUNotFound</t>
-  </si>
-  <si>
-    <t>Organization Unit not found.</t>
-  </si>
-  <si>
-    <t>OUIDInvalidOrNotSpecified</t>
-  </si>
-  <si>
-    <t>Organization Unit ID invalid or not specified.</t>
-  </si>
-  <si>
-    <t>OUNameNotSpecified</t>
-  </si>
-  <si>
-    <t>Organization Unit name not specified.</t>
-  </si>
-  <si>
-    <t>OUIDAndNameDoNotMatch</t>
-  </si>
-  <si>
-    <t>The specified Organization Unit ID and Organization Unit name do not match.</t>
-  </si>
-  <si>
-    <t>NamedOUNotFound</t>
-  </si>
-  <si>
-    <t>Organization Unit named {0} not found.</t>
-  </si>
-  <si>
-    <t>EnvironmentNotFound</t>
-  </si>
-  <si>
-    <t>Environment not found.</t>
-  </si>
-  <si>
-    <t>RobotEnvironmentAssociationFailure</t>
-  </si>
-  <si>
-    <t>Failed to add robot to environment. Request status: {0} / Response: {1}.</t>
-  </si>
-  <si>
-    <t>EnvironmentIDInvalidOrNotSpecified</t>
-  </si>
-  <si>
-    <t>Environment ID invalid or not specified.</t>
-  </si>
-  <si>
-    <t>EnvironmentNameNotSpecified</t>
-  </si>
-  <si>
-    <t>Environment name not specified.</t>
-  </si>
-  <si>
-    <t>EnvironmentIDAndNameDoNotMatch</t>
-  </si>
-  <si>
-    <t>The specified Environment ID and Environment name do not match.</t>
-  </si>
-  <si>
-    <t>RobotAddedAndRemoved</t>
-  </si>
-  <si>
-    <t>A Robot is being added and removed at the same time.</t>
-  </si>
-  <si>
-    <t>ロボットが同時に追加および削除されています。</t>
-  </si>
-  <si>
-    <t>RoleNotFound</t>
-  </si>
-  <si>
-    <t>Role not found.</t>
-  </si>
-  <si>
-    <t>NamedRoleNotFound</t>
-  </si>
-  <si>
-    <t>Role named {0} not found.</t>
-  </si>
-  <si>
-    <t>ProcessNameNotSpecified</t>
-  </si>
-  <si>
-    <t>Process name not specified.</t>
-  </si>
-  <si>
-    <t>ProcessIDInvalidOrNotSpecified</t>
-  </si>
-  <si>
-    <t>Process ID invalid or not specified.</t>
-  </si>
-  <si>
-    <t>ProcessNotFound</t>
-  </si>
-  <si>
-    <t>Process not found.</t>
-  </si>
-  <si>
-    <t>ProcessIDAndNameDoNotMatch</t>
-  </si>
-  <si>
-    <t>The specified Process ID and Process name do not match.</t>
-  </si>
-  <si>
-    <t>NamedProcessNotFound</t>
-  </si>
-  <si>
-    <t>Process named {0} not found.</t>
-  </si>
-  <si>
-    <t>PackageNameNotSpecified</t>
-  </si>
-  <si>
-    <t>Package name not specified.</t>
-  </si>
-  <si>
-    <t>PackageVersionNotSpecified</t>
-  </si>
-  <si>
-    <t>Package version not specified.</t>
-  </si>
-  <si>
-    <t>PackageFileNotFound</t>
-  </si>
-  <si>
-    <t>Package file not found.</t>
-  </si>
-  <si>
-    <t>PackageNotFound</t>
-  </si>
-  <si>
-    <t>Package not found.</t>
-  </si>
-  <si>
-    <t>PackageVersionNotFound</t>
-  </si>
-  <si>
-    <t>The specified Package version was not found.</t>
-  </si>
-  <si>
-    <t>PackageNameVersionKeyDoNotMatch</t>
-  </si>
-  <si>
-    <t>The specified Package name, version and key do not match.</t>
-  </si>
-  <si>
-    <t>UniqueReferenceInvalidOrNotSpecified</t>
-  </si>
-  <si>
-    <t>Unique Reference invalid or not specified.</t>
-  </si>
-  <si>
-    <t>AutoRetryInvalidOrNotSpecified</t>
-  </si>
-  <si>
-    <t>Auto Retry invalid or not specified.</t>
-  </si>
-  <si>
-    <t>MaxNumberOfRetriesInvalidOrNotSpecified</t>
-  </si>
-  <si>
-    <t>Max Number of Retries invalid or not specified.</t>
-  </si>
-  <si>
-    <t>QueueNotFound</t>
-  </si>
-  <si>
-    <t>Queue not found.</t>
-  </si>
-  <si>
-    <t>NamedQueueNotFound</t>
-  </si>
-  <si>
-    <t>Queue named {0} not found.</t>
-  </si>
-  <si>
-    <t>QueueNameNotSpecified</t>
-  </si>
-  <si>
-    <t>Queue name not specified.</t>
-  </si>
-  <si>
-    <t>QueueItemsFileNotFound</t>
-  </si>
-  <si>
-    <t>SampleAccount</t>
-  </si>
-  <si>
-    <t>ログイン試行に複数回失敗した場合、テナントのセキュリティ設定で指定した秒数の間、アカウントがロックされることがありますのでご注意ください。</t>
-  </si>
-  <si>
-    <t>アカウント名</t>
-  </si>
-  <si>
-    <t>ブックのパス</t>
-  </si>
-  <si>
-    <t>Windows の資格情報マネージャーに保存されている資格情報を使用します。</t>
-  </si>
-  <si>
-    <t>Windows の資格情報マネージャーに資格情報を保存します。</t>
-  </si>
-  <si>
-    <t>ロボット グループ</t>
-  </si>
-  <si>
-    <t>Orchestrator のオンプレミス インスタンスです。</t>
-  </si>
-  <si>
-    <t>UiPath Automation Cloud でホストされている Orchestrator です。</t>
-  </si>
-  <si>
-    <t>Orchestrator hosted on UiPath Automation Cloud.</t>
-  </si>
-  <si>
-    <t>使用するオンプレミス版 Orchestrator のバージョンです。</t>
-  </si>
-  <si>
-    <t>Orchestrator にログインするユーザーのユーザー名です。</t>
-  </si>
-  <si>
-    <t>Orchestrator にログインするユーザーのパスワードです。</t>
-  </si>
-  <si>
-    <t>使用する Orchestrator インスタンスの URL です。</t>
-  </si>
-  <si>
-    <t>Orchestrator Manager が使用するテナントの名前です。</t>
+    <t>ID specific to the Orchestrator application itself. 
+Consult the UiPath Automation Cloud documentation for more information.</t>
   </si>
   <si>
     <t>Orchestrator アプリケーション自体に固有の ID です。
 詳しくは UiPath Automation Cloud ガイドをご確認ください。</t>
   </si>
   <si>
-    <t>UiPath Automation Cloud の API で使用する一意のログイン キーです。
-詳しくは UiPath Automation Cloud ガイドをご確認ください。</t>
+    <t>FormAccountNameTooltip</t>
+  </si>
+  <si>
+    <t>Unique account name for UiPath Automation Cloud organization. 
+For example, assuming that the organization account URL is https://cloud.uipath.com/SampleAccount, the Account Name is SampleAccount.</t>
   </si>
   <si>
     <t>UiPath Automation Cloud 組織の一意のアカウント名です。
 例えば組織アカウントの URL を https://cloud.uipath.com/SampleAccount と仮定すると、アカウント名は SampleAccount になります。</t>
   </si>
   <si>
+    <t>FormWorkbooksFolderPathTooltip</t>
+  </si>
+  <si>
+    <t>Path to the folder to which entities workbooks should be saved.</t>
+  </si>
+  <si>
     <t>エンティティのブックを保存するフォルダーのパスです。</t>
   </si>
   <si>
+    <t>AssetConfigFilePath</t>
+  </si>
+  <si>
+    <t>Assets.xlsx</t>
+  </si>
+  <si>
+    <t>アセット.xlsx</t>
+  </si>
+  <si>
+    <t>UserConfigFilePath</t>
+  </si>
+  <si>
+    <t>Users.xlsx</t>
+  </si>
+  <si>
+    <t>ユーザー.xlsx</t>
+  </si>
+  <si>
+    <t>RobotConfigFilePath</t>
+  </si>
+  <si>
+    <t>Robots.xlsx</t>
+  </si>
+  <si>
+    <t>ロボット.xlsx</t>
+  </si>
+  <si>
+    <t>MachineConfigFilePath</t>
+  </si>
+  <si>
+    <t>Machines.xlsx</t>
+  </si>
+  <si>
+    <t>マシン.xlsx</t>
+  </si>
+  <si>
+    <t>EnvironmentConfigFilePath</t>
+  </si>
+  <si>
+    <t>Environments.xlsx</t>
+  </si>
+  <si>
     <t>ロボット グループ.xlsx</t>
   </si>
   <si>
+    <t>ProcessConfigFilePath</t>
+  </si>
+  <si>
+    <t>Processes.xlsx</t>
+  </si>
+  <si>
+    <t>プロセス.xlsx</t>
+  </si>
+  <si>
+    <t>OrganizationUnitConfigFilePath</t>
+  </si>
+  <si>
+    <t>OrganizationUnits.xlsx</t>
+  </si>
+  <si>
+    <t>組織単位.xlsx</t>
+  </si>
+  <si>
+    <t>FolderConfigFilePath</t>
+  </si>
+  <si>
+    <t>Folders.xlsx</t>
+  </si>
+  <si>
+    <t>フォルダー.xlsx</t>
+  </si>
+  <si>
+    <t>QueueConfigFilePath</t>
+  </si>
+  <si>
+    <t>Queues.xlsx</t>
+  </si>
+  <si>
+    <t>キュー.xlsx</t>
+  </si>
+  <si>
+    <t>PackageConfigFilePath</t>
+  </si>
+  <si>
+    <t>Packages.xlsx</t>
+  </si>
+  <si>
+    <t>パッケージ.xlsx</t>
+  </si>
+  <si>
+    <t>GetOperationName</t>
+  </si>
+  <si>
+    <t>Get</t>
+  </si>
+  <si>
+    <t>取得</t>
+  </si>
+  <si>
+    <t>CreateOperationName</t>
+  </si>
+  <si>
+    <t>Create</t>
+  </si>
+  <si>
+    <t>作成</t>
+  </si>
+  <si>
+    <t>EditOperationName</t>
+  </si>
+  <si>
+    <t>Edit</t>
+  </si>
+  <si>
+    <t>編集</t>
+  </si>
+  <si>
+    <t>DeleteOperationName</t>
+  </si>
+  <si>
+    <t>Delete</t>
+  </si>
+  <si>
+    <t>削除</t>
+  </si>
+  <si>
+    <t>CreateCredentialOperationName</t>
+  </si>
+  <si>
+    <t>Create Credential</t>
+  </si>
+  <si>
+    <t>Credential 型を作成</t>
+  </si>
+  <si>
+    <t>EditCredentialOperationName</t>
+  </si>
+  <si>
+    <t>Edit Credential</t>
+  </si>
+  <si>
+    <t>Credential 型を編集</t>
+  </si>
+  <si>
+    <t>AddRemoveEnvironmentRobotsOperationName</t>
+  </si>
+  <si>
+    <t>Add or Remove Robots</t>
+  </si>
+  <si>
+    <t>ロボットを追加または削除</t>
+  </si>
+  <si>
+    <t>AddRemoveUserOrganizationUnitsOperationName</t>
+  </si>
+  <si>
+    <t>Add or Remove OUs</t>
+  </si>
+  <si>
+    <t>組織単位を追加または削除</t>
+  </si>
+  <si>
+    <t>AddRemoveUserRolesOperationName</t>
+  </si>
+  <si>
+    <t>Add or Remove Roles</t>
+  </si>
+  <si>
+    <t>ロールを追加または削除</t>
+  </si>
+  <si>
+    <t>UpdateProcessToLatestPackageVersionOperationName</t>
+  </si>
+  <si>
+    <t>Update to Latest Package</t>
+  </si>
+  <si>
     <t>最新のパッケージに更新</t>
   </si>
   <si>
+    <t>RollbackProcessToPreviousPackageVersionOperationName</t>
+  </si>
+  <si>
+    <t>Rollback to Previous Package</t>
+  </si>
+  <si>
     <t>以前のパッケージにロールバック</t>
   </si>
   <si>
+    <t>DownloadQueueItemsOperationName</t>
+  </si>
+  <si>
+    <t>Download Queue Items</t>
+  </si>
+  <si>
     <t>キュー アイテムをダウンロード</t>
   </si>
   <si>
+    <t>UploadQueueItemsOperationName</t>
+  </si>
+  <si>
+    <t>Upload Queue Items</t>
+  </si>
+  <si>
     <t>キュー アイテムをアップロード</t>
   </si>
   <si>
+    <t>DownloadPackageOperationName</t>
+  </si>
+  <si>
+    <t>Download</t>
+  </si>
+  <si>
+    <t>ダウンロード</t>
+  </si>
+  <si>
+    <t>UploadPackageOperationName</t>
+  </si>
+  <si>
+    <t>Upload</t>
+  </si>
+  <si>
+    <t>アップロード</t>
+  </si>
+  <si>
+    <t>StoppedExecution</t>
+  </si>
+  <si>
+    <t>The execution has been stopped.</t>
+  </si>
+  <si>
+    <t>実行が停止されました。</t>
+  </si>
+  <si>
+    <t>MandatoryArgumentsNotSpecified</t>
+  </si>
+  <si>
+    <t>Mandatory arguments not specified.</t>
+  </si>
+  <si>
     <t>必須の引数が指定されていません。</t>
   </si>
   <si>
+    <t>UnsupportedEntity</t>
+  </si>
+  <si>
+    <t>Unsupported entity specified.</t>
+  </si>
+  <si>
     <t>指定したエンティティはサポートされていません。</t>
   </si>
   <si>
+    <t>UnsupportedOperation</t>
+  </si>
+  <si>
+    <t>Unsupported operation.</t>
+  </si>
+  <si>
+    <t>操作はサポートされていません。</t>
+  </si>
+  <si>
+    <t>OperationDefaultResult</t>
+  </si>
+  <si>
+    <t>Success</t>
+  </si>
+  <si>
+    <t>成功</t>
+  </si>
+  <si>
+    <t>OnPremisesOrchestratorVersionNotSupported</t>
+  </si>
+  <si>
+    <t>The specified Orchestrator version is not supported.</t>
+  </si>
+  <si>
     <t>指定した Orchestrator のバージョンはサポートされていません。</t>
   </si>
   <si>
-    <t>認証に失敗したため、アクセス トークンを取得できません。サーバーの応答: {0}</t>
+    <t>TokenNotRetrieved</t>
+  </si>
+  <si>
+    <t>Unable to get access token due to failed authentication. 
+Server response: {0}</t>
+  </si>
+  <si>
+    <t>認証に失敗したため、アクセス トークンを取得できません。
+サーバーの応答: {0}</t>
+  </si>
+  <si>
+    <t>AuthenticationFailed</t>
+  </si>
+  <si>
+    <t>Authentication failed. Please check logs for more details.</t>
   </si>
   <si>
     <t>認証に失敗しました。詳細はログをご確認ください。</t>
   </si>
   <si>
+    <t>ErrorDuringExecutionLog</t>
+  </si>
+  <si>
+    <t>There was an execution error: {0} at {1}.</t>
+  </si>
+  <si>
     <t>実行エラーが発生しました: {1} で {0}。</t>
   </si>
   <si>
-    <t>実行エラーが発生しました。詳細はログをご確認ください。</t>
+    <t>ErrorDuringExecution</t>
+  </si>
+  <si>
+    <t>There was an execution error. 
+Please check logs for more details.</t>
+  </si>
+  <si>
+    <t>実行エラーが発生しました。
+詳細はログをご確認ください。</t>
+  </si>
+  <si>
+    <t>TokenExpired</t>
+  </si>
+  <si>
+    <t>Authentication token expired.</t>
+  </si>
+  <si>
+    <t>認証トークンの期限が切れました。</t>
+  </si>
+  <si>
+    <t>UnsupportedHTTPMethod</t>
+  </si>
+  <si>
+    <t>Unsupported HTTP method specified.</t>
   </si>
   <si>
     <t>指定した HTTP メソッドはサポートされていません。</t>
   </si>
   <si>
+    <t>ParameterNotFound</t>
+  </si>
+  <si>
+    <t>Parameter not found.</t>
+  </si>
+  <si>
     <t>パラメーターが見つかりません。</t>
   </si>
   <si>
+    <t>ConnectivityIssuesFailure</t>
+  </si>
+  <si>
+    <t>HTTP Request failed due to connectivity issues.</t>
+  </si>
+  <si>
     <t>接続の問題のため、HTTP 要求に失敗しました。</t>
+  </si>
+  <si>
+    <t>ServerErrorFailure</t>
+  </si>
+  <si>
+    <t>HTTP Request failed due to server error issues. 
+Request status: {0} / Response: {1}.</t>
+  </si>
+  <si>
+    <t>サーバー エラーの問題のため、HTTP 要求に失敗しました。
+要求ステータス: {0} / 応答: {1}。</t>
+  </si>
+  <si>
+    <t>InvalidResponseErrorFailure</t>
+  </si>
+  <si>
+    <t>HTTP Request failed due to invalid response. 
+Please confirm the specified Orchestrator URL and version.</t>
   </si>
   <si>
     <t>応答が無効なため HTTP 要求に失敗しました。
 指定した Orchestrator URL とバージョンを確認してください。</t>
   </si>
   <si>
-    <t>サーバー エラーの問題のため、HTTP 要求に失敗しました。
-要求ステータス: {0} / 応答: {1}。</t>
+    <t>ConfirmNumerousRequests</t>
+  </si>
+  <si>
+    <t>The selected operation will make a large number of HTTP requests that might impact on Orchestrator's infrastructure. 
+Continue the processing?</t>
   </si>
   <si>
     <t>選択した操作により、多数の HTTP 要求が送信されます。
@@ -1817,248 +1293,811 @@
 処理を続行しますか?</t>
   </si>
   <si>
+    <t>NumerousRequestsNotConfirmed</t>
+  </si>
+  <si>
+    <t>User did not confirm proceeding with numerous requests to the API.</t>
+  </si>
+  <si>
     <t>多数の API 要求を伴う操作を、ユーザーが承認しませんでした。</t>
   </si>
   <si>
+    <t>NumerousRequestsConfirmed</t>
+  </si>
+  <si>
+    <t>User confirmed proceeding with numerous requests to the API.</t>
+  </si>
+  <si>
     <t>多数の API 要求を伴う操作を、ユーザーが承認しました。</t>
   </si>
   <si>
-    <t>エンティティの処理に失敗しました。要求ステータス: {0} / 応答: {1}。</t>
-  </si>
-  <si>
-    <t>User did not confirm proceeding with numerous requests to the API.</t>
-  </si>
-  <si>
-    <t>User confirmed proceeding with numerous requests to the API.</t>
+    <t>ProcessEntityFailure</t>
+  </si>
+  <si>
+    <t>Failed to process entity. 
+Request status: {0} / Response: {1}.</t>
+  </si>
+  <si>
+    <t>エンティティの処理に失敗しました。
+要求ステータス: {0} / 応答: {1}。</t>
+  </si>
+  <si>
+    <t>ProcessedEntity</t>
+  </si>
+  <si>
+    <t>Already processed.</t>
+  </si>
+  <si>
+    <t>既に処理されています。</t>
+  </si>
+  <si>
+    <t>IDInvalidOrNotSpecified</t>
+  </si>
+  <si>
+    <t>ID invalid or not specified.</t>
   </si>
   <si>
     <t>ID が無効であるか、指定されていません。</t>
   </si>
   <si>
+    <t>NameNotSpecified</t>
+  </si>
+  <si>
+    <t>Name not specified.</t>
+  </si>
+  <si>
     <t>名前が指定されていません。</t>
   </si>
   <si>
+    <t>VersionNotSpecified</t>
+  </si>
+  <si>
+    <t>Version not specified.</t>
+  </si>
+  <si>
     <t>バージョンが指定されていません。</t>
   </si>
   <si>
+    <t>KeyNotSpecified</t>
+  </si>
+  <si>
+    <t>Key not specified.</t>
+  </si>
+  <si>
+    <t>キーが指定されていません。</t>
+  </si>
+  <si>
+    <t>IDAndNameDoNotMatch</t>
+  </si>
+  <si>
+    <t>The specified ID and Name do not match.</t>
+  </si>
+  <si>
     <t>指定した ID と名前が一致しません。</t>
   </si>
   <si>
+    <t>TypeNotSpecified</t>
+  </si>
+  <si>
+    <t>Type not specified.</t>
+  </si>
+  <si>
     <t>タイプ (種類) が指定されていません。</t>
   </si>
   <si>
+    <t>TypeNotSupported</t>
+  </si>
+  <si>
+    <t>The specified type is not supported.</t>
+  </si>
+  <si>
     <t>指定したタイプ (種類) はサポートされていません。</t>
   </si>
   <si>
+    <t>CredentialNotFound</t>
+  </si>
+  <si>
+    <t>The specified credential was not found.</t>
+  </si>
+  <si>
     <t>指定した資格情報が見つかりませんでした。</t>
   </si>
   <si>
+    <t>OperationCanceledByUser</t>
+  </si>
+  <si>
+    <t>Operation canceled by user.</t>
+  </si>
+  <si>
+    <t>ユーザーが操作をキャンセルしました。</t>
+  </si>
+  <si>
+    <t>OUFolderNameNotSpecified</t>
+  </si>
+  <si>
+    <t>Folder (Organization Unit) name not specified.</t>
+  </si>
+  <si>
     <t>フォルダー (組織単位) の名前が指定されていません。</t>
   </si>
   <si>
+    <t>OUFolderNotFound</t>
+  </si>
+  <si>
+    <t>Folder (Organization Unit) not found.</t>
+  </si>
+  <si>
     <t>フォルダー (組織単位) が見つかりません。</t>
   </si>
   <si>
+    <t>OUFolderIDInvalidOrNotSpecified</t>
+  </si>
+  <si>
+    <t>Folder (Organization Unit) ID invalid or not specified.</t>
+  </si>
+  <si>
     <t>フォルダー (組織単位) ID が無効であるか、指定されていません。</t>
   </si>
   <si>
-    <t>フォルダー (組織単位) {0} からデータを取得できませんでした。アクセス制限を確認してください。</t>
-  </si>
-  <si>
-    <t>全てのフォルダー (組織単位) にアクセスできませんでした。詳細はログをご確認ください。</t>
+    <t>FailedToGetDataFromOUFolder</t>
+  </si>
+  <si>
+    <t>Failed to get data from Folder (Organization Unit) named {0}. 
+Please verify access restrictions.</t>
+  </si>
+  <si>
+    <t>フォルダー (組織単位) {0} からデータを取得できませんでした。
+アクセス制限を確認してください。</t>
+  </si>
+  <si>
+    <t>FailedToAccessOUFolder</t>
+  </si>
+  <si>
+    <t>It was not possible to access all Folders (Organization Units). 
+Please check logs for more details.</t>
+  </si>
+  <si>
+    <t>全てのフォルダー (組織単位) にアクセスできませんでした。
+詳細はログをご確認ください。</t>
+  </si>
+  <si>
+    <t>ErrorMessageBoxTitle</t>
+  </si>
+  <si>
+    <t>Error</t>
+  </si>
+  <si>
+    <t>エラー</t>
+  </si>
+  <si>
+    <t>WarningMessageBoxTitle</t>
+  </si>
+  <si>
+    <t>Warning</t>
   </si>
   <si>
     <t>警告</t>
   </si>
   <si>
+    <t>UnsupportedAssetType</t>
+  </si>
+  <si>
+    <t>The specified asset type is not supported.</t>
+  </si>
+  <si>
     <t>指定したアセット型はサポートされていません。</t>
   </si>
   <si>
+    <t>AssetNotFound</t>
+  </si>
+  <si>
+    <t>Asset not found.</t>
+  </si>
+  <si>
     <t>アセットが見つかりません。</t>
   </si>
   <si>
+    <t>AssetIDInvalidOrNotSpecified</t>
+  </si>
+  <si>
+    <t>Asset ID invalid or not specified.</t>
+  </si>
+  <si>
     <t>アセット ID が無効であるか、指定されていません。</t>
   </si>
   <si>
+    <t>AssetNameNotSpecified</t>
+  </si>
+  <si>
+    <t>Asset name not specified.</t>
+  </si>
+  <si>
     <t>アセット名が指定されていません。</t>
   </si>
   <si>
+    <t>AssetIDAndNameDoNotMatch</t>
+  </si>
+  <si>
+    <t>The specified Asset ID and Asset name do not match.</t>
+  </si>
+  <si>
     <t>指定したアセット ID とアセット名が一致しません。</t>
   </si>
   <si>
+    <t>InvalidAssetValue</t>
+  </si>
+  <si>
+    <t>Invalid value.</t>
+  </si>
+  <si>
     <t>値が無効です。</t>
   </si>
   <si>
+    <t>EditCredentialUsernameNewPasswordRequired</t>
+  </si>
+  <si>
+    <t>New Password required when changing Username.</t>
+  </si>
+  <si>
+    <t>ユーザー名の編集に新しいパスワードが必要です。</t>
+  </si>
+  <si>
+    <t>PasswordNotSpecified</t>
+  </si>
+  <si>
+    <t>Password not specified.</t>
+  </si>
+  <si>
     <t>パスワードが指定されていません。</t>
   </si>
   <si>
+    <t>UserNotFound</t>
+  </si>
+  <si>
+    <t>User not  found.</t>
+  </si>
+  <si>
     <t>ユーザーが見つかりません。</t>
   </si>
   <si>
+    <t>StatusNotSupported</t>
+  </si>
+  <si>
+    <t>Status not supported.</t>
+  </si>
+  <si>
+    <t>ステータスはサポートされていません。</t>
+  </si>
+  <si>
+    <t>UsernameNotSpecified</t>
+  </si>
+  <si>
+    <t>Username not specified.</t>
+  </si>
+  <si>
     <t>ユーザー名が指定されていません。</t>
   </si>
   <si>
+    <t>IDAndUsernameDoNotMatch</t>
+  </si>
+  <si>
+    <t>The specified ID and Username do not match.</t>
+  </si>
+  <si>
     <t>指定した ID とユーザー名が一致しません。</t>
   </si>
   <si>
+    <t>SurnameNotSpecified</t>
+  </si>
+  <si>
+    <t>Surname not specified.</t>
+  </si>
+  <si>
     <t>姓が指定されていません。</t>
   </si>
   <si>
+    <t>EmailNotSpecified</t>
+  </si>
+  <si>
+    <t>Email not specified.</t>
+  </si>
+  <si>
     <t>メール アドレスが指定されていません。</t>
   </si>
   <si>
+    <t>OUAddedAndRemoved</t>
+  </si>
+  <si>
+    <t>An Organization Unit is being added and removed at the same time.</t>
+  </si>
+  <si>
+    <t>組織単位が同時に追加および削除されています。</t>
+  </si>
+  <si>
+    <t>RoleAddedAndRemoved</t>
+  </si>
+  <si>
+    <t>A Role is being added and removed at the same time.</t>
+  </si>
+  <si>
+    <t>ロールが同時に追加および削除されています。</t>
+  </si>
+  <si>
+    <t>NamedUserNotFound</t>
+  </si>
+  <si>
+    <t>Username {0} not found.</t>
+  </si>
+  <si>
     <t>ユーザー名 {0} が見つかりません。</t>
   </si>
   <si>
-    <t>ロボットは既に処理済みです。ロボット名: {0} / ID: {1}。</t>
+    <t>ProcessedRobot</t>
+  </si>
+  <si>
+    <t>Robot already processed. 
+Robot name: {0} / ID: {1}.</t>
+  </si>
+  <si>
+    <t>ロボットは既に処理済みです。
+ロボット名: {0} / ID: {1}。</t>
+  </si>
+  <si>
+    <t>RobotNotFound</t>
+  </si>
+  <si>
+    <t>Robot not found.</t>
   </si>
   <si>
     <t>ロボットが見つかりません。</t>
   </si>
   <si>
+    <t>HostingTypeNotSpecified</t>
+  </si>
+  <si>
+    <t>Hosting Type not specified.</t>
+  </si>
+  <si>
     <t>ホスティングの種類が指定されていません。</t>
   </si>
   <si>
+    <t>RobotNameNotSpecified</t>
+  </si>
+  <si>
+    <t>Robot Name not specified.</t>
+  </si>
+  <si>
     <t>ロボット名が指定されていません。</t>
   </si>
   <si>
+    <t>RobotTypeNotSpecified</t>
+  </si>
+  <si>
+    <t>Robot Type not specified.</t>
+  </si>
+  <si>
     <t>ロボットの種類が指定されていません。</t>
   </si>
   <si>
+    <t>RobotIDInvalidOrNotSpecified</t>
+  </si>
+  <si>
+    <t>Robot ID invalid or not specified.</t>
+  </si>
+  <si>
     <t>ロボット ID が無効であるか、指定されていません。</t>
   </si>
   <si>
+    <t>RobotIDAndNameDoNotMatch</t>
+  </si>
+  <si>
+    <t>The specified Robot ID and name do not match.</t>
+  </si>
+  <si>
     <t>指定したロボット ID とロボット名が一致しません。</t>
   </si>
   <si>
+    <t>NamedRobotNotFound</t>
+  </si>
+  <si>
+    <t>Robot named {0} not found.</t>
+  </si>
+  <si>
     <t>ロボット {0} が見つかりません。</t>
   </si>
   <si>
+    <t>MachineNotFound</t>
+  </si>
+  <si>
+    <t>Machine not found.</t>
+  </si>
+  <si>
     <t>マシンが見つかりません。</t>
+  </si>
+  <si>
+    <t>GetSingleMachineFailure</t>
+  </si>
+  <si>
+    <t>Failed to get machine with ID: {0}. 
+Request status: {1} / Response: {2}.</t>
   </si>
   <si>
     <t>ID {0} のマシンの取得に失敗しました。
 要求ステータス: {1} / 応答: {2}。</t>
   </si>
   <si>
+    <t>MachineNameNotSpecified</t>
+  </si>
+  <si>
+    <t>Machine Name not specified.</t>
+  </si>
+  <si>
     <t>マシン名が指定されていません。</t>
   </si>
   <si>
+    <t>NamedMachineNotFound</t>
+  </si>
+  <si>
+    <t>Machine named {0} not found.</t>
+  </si>
+  <si>
     <t>マシン {0} が見つかりません。</t>
   </si>
   <si>
+    <t>FolderNotFound</t>
+  </si>
+  <si>
+    <t>Folder not found.</t>
+  </si>
+  <si>
     <t>フォルダーが見つかりません。</t>
   </si>
   <si>
+    <t>FolderIDInvalidOrNotSpecified</t>
+  </si>
+  <si>
+    <t>Folder ID invalid or not specified.</t>
+  </si>
+  <si>
     <t>フォルダー ID が無効であるか、指定されていません。</t>
   </si>
   <si>
+    <t>FolderNameNotSpecified</t>
+  </si>
+  <si>
+    <t>Folder name not specified.</t>
+  </si>
+  <si>
     <t>フォルダー名が指定されていません。</t>
   </si>
   <si>
+    <t>FolderIDAndNameDoNotMatch</t>
+  </si>
+  <si>
+    <t>The specified Folder ID and Folder name do not match.</t>
+  </si>
+  <si>
     <t>指定したフォルダー ID とフォルダー名が一致しません。</t>
   </si>
   <si>
+    <t>NamedFolderNotFound</t>
+  </si>
+  <si>
+    <t>Folder named {0} not found.</t>
+  </si>
+  <si>
     <t>フォルダー {0} が見つかりません。</t>
   </si>
   <si>
+    <t>RoleAssignmentModelNotSpecified</t>
+  </si>
+  <si>
+    <t>Role Assignment Model not specified.</t>
+  </si>
+  <si>
     <t>ロール割り当てモデルが指定されていません。</t>
   </si>
   <si>
+    <t>RoleAssignmentModelNotSupported</t>
+  </si>
+  <si>
+    <t>The specified Role Assignment Model is not supported.</t>
+  </si>
+  <si>
     <t>指定したロール割り当てモデルはサポートされていません。</t>
   </si>
   <si>
+    <t>OUNotFound</t>
+  </si>
+  <si>
+    <t>Organization Unit not found.</t>
+  </si>
+  <si>
     <t>組織単位が見つかりません。</t>
   </si>
   <si>
+    <t>OUIDInvalidOrNotSpecified</t>
+  </si>
+  <si>
+    <t>Organization Unit ID invalid or not specified.</t>
+  </si>
+  <si>
     <t>組織単位 ID が無効であるか、指定されていません。</t>
   </si>
   <si>
+    <t>OUNameNotSpecified</t>
+  </si>
+  <si>
+    <t>Organization Unit name not specified.</t>
+  </si>
+  <si>
     <t>組織単位名が指定されていません。</t>
   </si>
   <si>
+    <t>OUIDAndNameDoNotMatch</t>
+  </si>
+  <si>
+    <t>The specified Organization Unit ID and Organization Unit name do not match.</t>
+  </si>
+  <si>
     <t>指定した組織単位 ID と組織単位名が一致しません。</t>
   </si>
   <si>
+    <t>NamedOUNotFound</t>
+  </si>
+  <si>
+    <t>Organization Unit named {0} not found.</t>
+  </si>
+  <si>
     <t>組織単位 {0} が見つかりません。</t>
   </si>
   <si>
+    <t>EnvironmentNotFound</t>
+  </si>
+  <si>
+    <t>Environment not found.</t>
+  </si>
+  <si>
     <t>ロボット グループが見つかりません。</t>
   </si>
   <si>
-    <t>ロボットをロボット グループに追加できませんでした。要求ステータス: {0} / 応答: {1}。</t>
+    <t>RobotEnvironmentAssociationFailure</t>
+  </si>
+  <si>
+    <t>Failed to add robot to environment. 
+Request status: {0} / Response: {1}.</t>
+  </si>
+  <si>
+    <t>ロボットをロボット グループに追加できませんでした。
+要求ステータス: {0} / 応答: {1}。</t>
+  </si>
+  <si>
+    <t>EnvironmentIDInvalidOrNotSpecified</t>
+  </si>
+  <si>
+    <t>Environment ID invalid or not specified.</t>
   </si>
   <si>
     <t>ロボット グループ ID が無効であるか、指定されていません。</t>
   </si>
   <si>
+    <t>EnvironmentNameNotSpecified</t>
+  </si>
+  <si>
+    <t>Environment name not specified.</t>
+  </si>
+  <si>
     <t>ロボット グループ名が指定されていません。</t>
   </si>
   <si>
+    <t>EnvironmentIDAndNameDoNotMatch</t>
+  </si>
+  <si>
+    <t>The specified Environment ID and Environment name do not match.</t>
+  </si>
+  <si>
     <t>指定したロボット グループ ID とロボット グループ名が一致しません。</t>
   </si>
   <si>
+    <t>RobotAddedAndRemoved</t>
+  </si>
+  <si>
+    <t>A Robot is being added and removed at the same time.</t>
+  </si>
+  <si>
+    <t>ロボットが同時に追加および削除されています。</t>
+  </si>
+  <si>
+    <t>RoleNotFound</t>
+  </si>
+  <si>
+    <t>Role not found.</t>
+  </si>
+  <si>
     <t>ロールが見つかりません。</t>
   </si>
   <si>
+    <t>NamedRoleNotFound</t>
+  </si>
+  <si>
+    <t>Role named {0} not found.</t>
+  </si>
+  <si>
     <t>ロール {0} が見つかりません。</t>
   </si>
   <si>
+    <t>ProcessNameNotSpecified</t>
+  </si>
+  <si>
+    <t>Process name not specified.</t>
+  </si>
+  <si>
     <t>プロセス名が指定されていません。</t>
   </si>
   <si>
+    <t>ProcessIDInvalidOrNotSpecified</t>
+  </si>
+  <si>
+    <t>Process ID invalid or not specified.</t>
+  </si>
+  <si>
     <t>プロセス ID が無効であるか、指定されていません。</t>
   </si>
   <si>
+    <t>ProcessNotFound</t>
+  </si>
+  <si>
+    <t>Process not found.</t>
+  </si>
+  <si>
     <t>プロセスが見つかりません。</t>
   </si>
   <si>
+    <t>ProcessIDAndNameDoNotMatch</t>
+  </si>
+  <si>
+    <t>The specified Process ID and Process name do not match.</t>
+  </si>
+  <si>
     <t>指定したプロセス ID とプロセス名が一致しません。</t>
   </si>
   <si>
+    <t>NamedProcessNotFound</t>
+  </si>
+  <si>
+    <t>Process named {0} not found.</t>
+  </si>
+  <si>
     <t>プロセス {0} が見つかりません。</t>
   </si>
   <si>
+    <t>PackageNameNotSpecified</t>
+  </si>
+  <si>
+    <t>Package name not specified.</t>
+  </si>
+  <si>
     <t>パッケージ名が指定されていません。</t>
   </si>
   <si>
+    <t>PackageVersionNotSpecified</t>
+  </si>
+  <si>
+    <t>Package version not specified.</t>
+  </si>
+  <si>
     <t>パッケージ バージョンが指定されていません。</t>
   </si>
   <si>
+    <t>PackageFileNotFound</t>
+  </si>
+  <si>
+    <t>Package file not found.</t>
+  </si>
+  <si>
     <t>パッケージ ファイルが見つかりません。</t>
   </si>
   <si>
+    <t>PackageNotFound</t>
+  </si>
+  <si>
+    <t>Package not found.</t>
+  </si>
+  <si>
     <t>パッケージが見つかりません。</t>
   </si>
   <si>
+    <t>PackageVersionNotFound</t>
+  </si>
+  <si>
+    <t>The specified Package version was not found.</t>
+  </si>
+  <si>
     <t>指定したパッケージ バージョンが見つかりません。</t>
   </si>
   <si>
+    <t>PackageNameVersionKeyDoNotMatch</t>
+  </si>
+  <si>
+    <t>The specified Package name, version and key do not match.</t>
+  </si>
+  <si>
     <t>指定したパッケージ名、バージョン、およびキーが一致しません。</t>
   </si>
   <si>
+    <t>PackageDownloadPathNotSpecified</t>
+  </si>
+  <si>
+    <t>Download Folder Path not specified.</t>
+  </si>
+  <si>
+    <t>保存フォルダーのパスが指定されていません。</t>
+  </si>
+  <si>
+    <t>UniqueReferenceInvalidOrNotSpecified</t>
+  </si>
+  <si>
+    <t>Unique Reference invalid or not specified.</t>
+  </si>
+  <si>
+    <t>一意の参照が無効であるか、指定されていません。</t>
+  </si>
+  <si>
+    <t>AutoRetryInvalidOrNotSpecified</t>
+  </si>
+  <si>
+    <t>Auto Retry invalid or not specified.</t>
+  </si>
+  <si>
+    <t>自動リトライが無効であるか、指定されていません。</t>
+  </si>
+  <si>
+    <t>MaxNumberOfRetriesInvalidOrNotSpecified</t>
+  </si>
+  <si>
+    <t>Max Number of Retries invalid or not specified.</t>
+  </si>
+  <si>
+    <t>最大リトライ回数が無効であるか、指定されていません。</t>
+  </si>
+  <si>
+    <t>QueueNotFound</t>
+  </si>
+  <si>
+    <t>Queue not found.</t>
+  </si>
+  <si>
+    <t>キューが見つかりません。</t>
+  </si>
+  <si>
+    <t>NamedQueueNotFound</t>
+  </si>
+  <si>
+    <t>Queue named {0} not found.</t>
+  </si>
+  <si>
+    <t>キュー {0} が見つかりません。</t>
+  </si>
+  <si>
+    <t>QueueNameNotSpecified</t>
+  </si>
+  <si>
+    <t>Queue name not specified.</t>
+  </si>
+  <si>
+    <t>キュー名が指定されていません。</t>
+  </si>
+  <si>
+    <t>QueueItemsFileNotFound</t>
+  </si>
+  <si>
     <t>The file containing Queue items was not found.</t>
   </si>
   <si>
-    <t>一意の参照が無効であるか、指定されていません。</t>
-  </si>
-  <si>
-    <t>自動リトライが無効であるか、指定されていません。</t>
-  </si>
-  <si>
-    <t>最大リトライ回数が無効であるか、指定されていません。</t>
-  </si>
-  <si>
-    <t>キューが見つかりません。</t>
-  </si>
-  <si>
-    <t>キュー {0} が見つかりません。</t>
-  </si>
-  <si>
-    <t>キュー名が指定されていません。</t>
-  </si>
-  <si>
     <t>キュー アイテムを含むファイルが見つかりませんでした。</t>
+  </si>
+  <si>
+    <t>SampleAccount</t>
   </si>
 </sst>
 </file>
@@ -2151,8 +2190,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table13" displayName="Table13" ref="A1:C184" totalsRowShown="0">
-  <autoFilter ref="A1:C184" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table13" displayName="Table13" ref="A1:C186" totalsRowShown="0">
+  <autoFilter ref="A1:C186" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Name"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="EN"/>
@@ -2473,7 +2512,7 @@
         <v>7</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>549</v>
+        <v>672</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>8</v>
@@ -2526,7 +2565,7 @@
   <dimension ref="A1:C63"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A2" sqref="A2 A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3244,10 +3283,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1927ABA9-1814-4487-9CEC-ABDCAF91481F}">
-  <dimension ref="A1:C184"/>
+  <dimension ref="A1:C186"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A2" sqref="A2 A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3287,447 +3326,447 @@
         <v>164</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>550</v>
+        <v>165</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>551</v>
+        <v>182</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>552</v>
+        <v>191</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
-        <v>192</v>
+        <v>195</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>203</v>
+        <v>206</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>208</v>
+        <v>211</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>553</v>
+        <v>212</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
-        <v>209</v>
+        <v>213</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>210</v>
+        <v>214</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>554</v>
+        <v>215</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>212</v>
+        <v>217</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>213</v>
+        <v>218</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
-        <v>214</v>
+        <v>219</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>215</v>
+        <v>220</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>216</v>
+        <v>221</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
-        <v>217</v>
+        <v>222</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>218</v>
+        <v>223</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>219</v>
+        <v>224</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
-        <v>220</v>
+        <v>225</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>221</v>
+        <v>226</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>222</v>
+        <v>227</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
-        <v>223</v>
+        <v>228</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>224</v>
+        <v>229</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>555</v>
+        <v>230</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
-        <v>225</v>
+        <v>231</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>226</v>
+        <v>232</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>227</v>
+        <v>233</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
-        <v>228</v>
+        <v>234</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>229</v>
+        <v>235</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>203</v>
+        <v>206</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="s">
-        <v>230</v>
+        <v>236</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>231</v>
+        <v>237</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="s">
-        <v>232</v>
+        <v>238</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>233</v>
+        <v>239</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>234</v>
+        <v>240</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A30" s="1" t="s">
-        <v>235</v>
+        <v>241</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>236</v>
+        <v>242</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>237</v>
+        <v>243</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A31" s="1" t="s">
-        <v>238</v>
+        <v>244</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>239</v>
+        <v>245</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>239</v>
+        <v>245</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A32" s="1" t="s">
-        <v>240</v>
+        <v>246</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>241</v>
+        <v>247</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>242</v>
+        <v>248</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A33" s="1" t="s">
-        <v>243</v>
+        <v>249</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>244</v>
+        <v>250</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>556</v>
+        <v>251</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A34" s="1" t="s">
-        <v>245</v>
+        <v>252</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>558</v>
+        <v>253</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>557</v>
+        <v>254</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A35" s="1" t="s">
-        <v>246</v>
+        <v>255</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>247</v>
+        <v>256</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>559</v>
+        <v>257</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A36" s="1" t="s">
-        <v>248</v>
+        <v>258</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>249</v>
+        <v>259</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>560</v>
+        <v>260</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A37" s="1" t="s">
-        <v>250</v>
+        <v>261</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>251</v>
+        <v>262</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>561</v>
+        <v>263</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A38" s="1" t="s">
-        <v>252</v>
+        <v>264</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>253</v>
+        <v>265</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>562</v>
+        <v>266</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A39" s="1" t="s">
-        <v>254</v>
+        <v>267</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>255</v>
+        <v>268</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>563</v>
+        <v>269</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="43.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A40" s="1" t="s">
-        <v>256</v>
+        <v>270</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>257</v>
+        <v>271</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>565</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" ht="43.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A41" s="1" t="s">
-        <v>258</v>
+        <v>273</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>259</v>
+        <v>274</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>564</v>
+        <v>275</v>
       </c>
     </row>
     <row r="42" spans="1:3" ht="58" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A42" s="1" t="s">
-        <v>260</v>
+        <v>276</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>261</v>
+        <v>277</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>566</v>
+        <v>278</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A43" s="1" t="s">
-        <v>262</v>
+        <v>279</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>263</v>
+        <v>280</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>567</v>
+        <v>281</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.35">
@@ -3736,112 +3775,112 @@
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A45" s="1" t="s">
-        <v>264</v>
+        <v>282</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>265</v>
+        <v>283</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>266</v>
+        <v>284</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A46" s="1" t="s">
-        <v>267</v>
+        <v>285</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>268</v>
+        <v>286</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>269</v>
+        <v>287</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A47" s="1" t="s">
-        <v>270</v>
+        <v>288</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>271</v>
+        <v>289</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>272</v>
+        <v>290</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A48" s="1" t="s">
-        <v>273</v>
+        <v>291</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>274</v>
+        <v>292</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>275</v>
+        <v>293</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A49" s="1" t="s">
-        <v>276</v>
+        <v>294</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>277</v>
+        <v>295</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>568</v>
+        <v>296</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A50" s="1" t="s">
-        <v>278</v>
+        <v>297</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>279</v>
+        <v>298</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>280</v>
+        <v>299</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A51" s="1" t="s">
-        <v>281</v>
+        <v>300</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>282</v>
+        <v>301</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>283</v>
+        <v>302</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A52" s="1" t="s">
-        <v>284</v>
+        <v>303</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>285</v>
+        <v>304</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>286</v>
+        <v>305</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A53" s="1" t="s">
-        <v>287</v>
+        <v>306</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>288</v>
+        <v>307</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>289</v>
+        <v>308</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A54" s="1" t="s">
-        <v>290</v>
+        <v>309</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>291</v>
+        <v>310</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>292</v>
+        <v>311</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.35">
@@ -3850,1324 +3889,1346 @@
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A56" s="1" t="s">
-        <v>293</v>
+        <v>312</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>294</v>
+        <v>313</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>295</v>
+        <v>314</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A57" s="1" t="s">
-        <v>296</v>
+        <v>315</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>297</v>
+        <v>316</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>298</v>
+        <v>317</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A58" s="1" t="s">
-        <v>299</v>
+        <v>318</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>300</v>
+        <v>319</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>301</v>
+        <v>320</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A59" s="1" t="s">
-        <v>302</v>
+        <v>321</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>303</v>
+        <v>322</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>304</v>
+        <v>323</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A60" s="1" t="s">
-        <v>305</v>
+        <v>324</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>306</v>
+        <v>325</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>307</v>
+        <v>326</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A61" s="1" t="s">
-        <v>308</v>
+        <v>327</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>309</v>
+        <v>328</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>310</v>
+        <v>329</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A62" s="1" t="s">
-        <v>311</v>
+        <v>330</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>312</v>
+        <v>331</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>313</v>
+        <v>332</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A63" s="1" t="s">
-        <v>314</v>
+        <v>333</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>315</v>
+        <v>334</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>316</v>
+        <v>335</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A64" s="1" t="s">
-        <v>317</v>
+        <v>336</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>318</v>
+        <v>337</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>319</v>
+        <v>338</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A65" s="1" t="s">
-        <v>320</v>
+        <v>339</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>321</v>
+        <v>340</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>569</v>
+        <v>341</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A66" s="1" t="s">
-        <v>322</v>
+        <v>342</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>323</v>
+        <v>343</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>570</v>
+        <v>344</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A67" s="1" t="s">
-        <v>324</v>
+        <v>345</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>325</v>
+        <v>346</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>571</v>
+        <v>347</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A68" s="1" t="s">
-        <v>326</v>
+        <v>348</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>327</v>
+        <v>349</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>572</v>
+        <v>350</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A69" s="1" t="s">
-        <v>328</v>
+        <v>351</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>329</v>
+        <v>352</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>330</v>
+        <v>353</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A70" s="1" t="s">
-        <v>331</v>
+        <v>354</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>332</v>
+        <v>355</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>333</v>
+        <v>356</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A71" s="1" t="s">
-        <v>334</v>
+        <v>357</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>335</v>
+        <v>358</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>336</v>
+        <v>359</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A72" s="1" t="s">
-        <v>337</v>
+        <v>360</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>338</v>
+        <v>361</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>573</v>
+        <v>362</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A73" s="1" t="s">
-        <v>339</v>
+        <v>363</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>340</v>
+        <v>364</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>574</v>
+        <v>365</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A74" s="1" t="s">
-        <v>341</v>
+        <v>366</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>342</v>
+        <v>367</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>343</v>
+        <v>368</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A75" s="1" t="s">
-        <v>344</v>
+        <v>369</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>345</v>
+        <v>370</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>346</v>
+        <v>371</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A76" s="1" t="s">
-        <v>347</v>
+        <v>372</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>348</v>
+        <v>373</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>575</v>
+        <v>374</v>
       </c>
     </row>
     <row r="77" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A77" s="1" t="s">
-        <v>349</v>
+        <v>375</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>350</v>
+        <v>376</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>576</v>
+        <v>377</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A78" s="1" t="s">
-        <v>351</v>
+        <v>378</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>352</v>
+        <v>379</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>577</v>
+        <v>380</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A79" s="1" t="s">
-        <v>353</v>
+        <v>381</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>354</v>
+        <v>382</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>578</v>
-      </c>
-    </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.35">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A80" s="1" t="s">
-        <v>355</v>
+        <v>384</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>356</v>
+        <v>385</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>579</v>
+        <v>386</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A81" s="1" t="s">
-        <v>357</v>
+        <v>387</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>358</v>
+        <v>388</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>359</v>
+        <v>389</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A82" s="1" t="s">
-        <v>360</v>
+        <v>390</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>361</v>
+        <v>391</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>580</v>
+        <v>392</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A83" s="1" t="s">
-        <v>362</v>
+        <v>393</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>363</v>
+        <v>394</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>581</v>
+        <v>395</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A84" s="1" t="s">
-        <v>364</v>
+        <v>396</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>365</v>
+        <v>397</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>582</v>
+        <v>398</v>
       </c>
     </row>
     <row r="85" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A85" s="1" t="s">
-        <v>366</v>
+        <v>399</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>367</v>
+        <v>400</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>584</v>
+        <v>401</v>
       </c>
     </row>
     <row r="86" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A86" s="1" t="s">
-        <v>368</v>
+        <v>402</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>369</v>
+        <v>403</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>583</v>
-      </c>
-    </row>
-    <row r="87" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" ht="43.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A87" s="1" t="s">
-        <v>370</v>
+        <v>405</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>371</v>
+        <v>406</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>585</v>
+        <v>407</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A88" s="1" t="s">
-        <v>372</v>
+        <v>408</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>589</v>
+        <v>409</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>586</v>
+        <v>410</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A89" s="1" t="s">
-        <v>373</v>
+        <v>411</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>590</v>
+        <v>412</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>587</v>
-      </c>
-    </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.35">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A90" s="1" t="s">
-        <v>374</v>
+        <v>414</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>375</v>
+        <v>415</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>588</v>
+        <v>416</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A91" s="1" t="s">
-        <v>376</v>
+        <v>417</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>377</v>
+        <v>418</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>378</v>
+        <v>419</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A92" s="1" t="s">
-        <v>379</v>
+        <v>420</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>380</v>
+        <v>421</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>591</v>
+        <v>422</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A93" s="1" t="s">
-        <v>381</v>
+        <v>423</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>382</v>
+        <v>424</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>592</v>
+        <v>425</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A94" s="1" t="s">
-        <v>383</v>
+        <v>426</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>384</v>
+        <v>427</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>593</v>
+        <v>428</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A95" s="1" t="s">
-        <v>385</v>
+        <v>429</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>386</v>
+        <v>430</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>594</v>
+        <v>431</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A96" s="1" t="s">
-        <v>387</v>
+        <v>432</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>388</v>
+        <v>433</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>595</v>
+        <v>434</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A97" s="1" t="s">
-        <v>389</v>
+        <v>435</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>390</v>
+        <v>436</v>
       </c>
       <c r="C97" s="2" t="s">
-        <v>596</v>
+        <v>437</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A98" s="1" t="s">
-        <v>391</v>
+        <v>438</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>392</v>
+        <v>439</v>
       </c>
       <c r="C98" s="2" t="s">
-        <v>597</v>
+        <v>440</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A99" s="1" t="s">
-        <v>393</v>
+        <v>441</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>394</v>
+        <v>442</v>
       </c>
       <c r="C99" s="2" t="s">
-        <v>395</v>
+        <v>443</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A100" s="1" t="s">
-        <v>396</v>
+        <v>444</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>397</v>
+        <v>445</v>
       </c>
       <c r="C100" s="2" t="s">
-        <v>598</v>
+        <v>446</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A101" s="1" t="s">
-        <v>398</v>
+        <v>447</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>399</v>
+        <v>448</v>
       </c>
       <c r="C101" s="2" t="s">
-        <v>599</v>
+        <v>449</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A102" s="1" t="s">
-        <v>400</v>
+        <v>450</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>401</v>
+        <v>451</v>
       </c>
       <c r="C102" s="2" t="s">
-        <v>600</v>
-      </c>
-    </row>
-    <row r="103" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A103" s="1" t="s">
-        <v>402</v>
+        <v>453</v>
       </c>
       <c r="B103" s="2" t="s">
-        <v>403</v>
+        <v>454</v>
       </c>
       <c r="C103" s="2" t="s">
-        <v>601</v>
+        <v>455</v>
       </c>
     </row>
     <row r="104" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A104" s="1" t="s">
-        <v>404</v>
+        <v>456</v>
       </c>
       <c r="B104" s="2" t="s">
-        <v>405</v>
+        <v>457</v>
       </c>
       <c r="C104" s="2" t="s">
-        <v>602</v>
-      </c>
-    </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.35">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A105" s="1" t="s">
-        <v>406</v>
+        <v>459</v>
       </c>
       <c r="B105" s="2" t="s">
-        <v>407</v>
+        <v>460</v>
       </c>
       <c r="C105" s="2" t="s">
-        <v>408</v>
+        <v>461</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A106" s="1" t="s">
-        <v>409</v>
+        <v>462</v>
       </c>
       <c r="B106" s="2" t="s">
-        <v>410</v>
+        <v>463</v>
       </c>
       <c r="C106" s="2" t="s">
-        <v>603</v>
+        <v>464</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B107" s="2"/>
-      <c r="C107" s="2"/>
+      <c r="A107" s="1" t="s">
+        <v>465</v>
+      </c>
+      <c r="B107" s="2" t="s">
+        <v>466</v>
+      </c>
+      <c r="C107" s="2" t="s">
+        <v>467</v>
+      </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A108" s="1" t="s">
-        <v>411</v>
-      </c>
-      <c r="B108" s="2" t="s">
-        <v>412</v>
-      </c>
-      <c r="C108" s="2" t="s">
-        <v>604</v>
-      </c>
+      <c r="B108" s="2"/>
+      <c r="C108" s="2"/>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A109" s="1" t="s">
-        <v>413</v>
+        <v>468</v>
       </c>
       <c r="B109" s="2" t="s">
-        <v>414</v>
+        <v>469</v>
       </c>
       <c r="C109" s="2" t="s">
-        <v>605</v>
+        <v>470</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A110" s="1" t="s">
-        <v>415</v>
+        <v>471</v>
       </c>
       <c r="B110" s="2" t="s">
-        <v>416</v>
+        <v>472</v>
       </c>
       <c r="C110" s="2" t="s">
-        <v>606</v>
+        <v>473</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A111" s="1" t="s">
-        <v>417</v>
+        <v>474</v>
       </c>
       <c r="B111" s="2" t="s">
-        <v>418</v>
+        <v>475</v>
       </c>
       <c r="C111" s="2" t="s">
-        <v>607</v>
+        <v>476</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A112" s="1" t="s">
-        <v>419</v>
+        <v>477</v>
       </c>
       <c r="B112" s="2" t="s">
-        <v>420</v>
+        <v>478</v>
       </c>
       <c r="C112" s="2" t="s">
-        <v>608</v>
+        <v>479</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A113" s="1" t="s">
-        <v>421</v>
+        <v>480</v>
       </c>
       <c r="B113" s="2" t="s">
-        <v>422</v>
+        <v>481</v>
       </c>
       <c r="C113" s="2" t="s">
-        <v>609</v>
+        <v>482</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A114" s="1" t="s">
-        <v>423</v>
+        <v>483</v>
       </c>
       <c r="B114" s="2" t="s">
-        <v>424</v>
+        <v>484</v>
       </c>
       <c r="C114" s="2" t="s">
-        <v>425</v>
+        <v>485</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A115" s="1" t="s">
-        <v>426</v>
+        <v>486</v>
       </c>
       <c r="B115" s="2" t="s">
-        <v>427</v>
+        <v>487</v>
       </c>
       <c r="C115" s="2" t="s">
-        <v>610</v>
+        <v>488</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B116" s="2"/>
-      <c r="C116" s="2"/>
+      <c r="A116" s="1" t="s">
+        <v>489</v>
+      </c>
+      <c r="B116" s="2" t="s">
+        <v>490</v>
+      </c>
+      <c r="C116" s="2" t="s">
+        <v>491</v>
+      </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A117" s="1" t="s">
-        <v>428</v>
-      </c>
-      <c r="B117" s="2" t="s">
-        <v>429</v>
-      </c>
-      <c r="C117" s="2" t="s">
-        <v>611</v>
-      </c>
+      <c r="B117" s="2"/>
+      <c r="C117" s="2"/>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A118" s="1" t="s">
-        <v>430</v>
+        <v>492</v>
       </c>
       <c r="B118" s="2" t="s">
-        <v>431</v>
+        <v>493</v>
       </c>
       <c r="C118" s="2" t="s">
-        <v>432</v>
+        <v>494</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A119" s="1" t="s">
-        <v>433</v>
+        <v>495</v>
       </c>
       <c r="B119" s="2" t="s">
-        <v>434</v>
+        <v>496</v>
       </c>
       <c r="C119" s="2" t="s">
-        <v>612</v>
+        <v>497</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A120" s="1" t="s">
-        <v>435</v>
+        <v>498</v>
       </c>
       <c r="B120" s="2" t="s">
-        <v>436</v>
+        <v>499</v>
       </c>
       <c r="C120" s="2" t="s">
-        <v>613</v>
+        <v>500</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A121" s="1" t="s">
-        <v>437</v>
+        <v>501</v>
       </c>
       <c r="B121" s="2" t="s">
-        <v>438</v>
+        <v>502</v>
       </c>
       <c r="C121" s="2" t="s">
-        <v>614</v>
+        <v>503</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A122" s="1" t="s">
-        <v>439</v>
+        <v>504</v>
       </c>
       <c r="B122" s="2" t="s">
-        <v>440</v>
+        <v>505</v>
       </c>
       <c r="C122" s="2" t="s">
-        <v>615</v>
+        <v>506</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A123" s="1" t="s">
-        <v>441</v>
+        <v>507</v>
       </c>
       <c r="B123" s="2" t="s">
-        <v>442</v>
+        <v>508</v>
       </c>
       <c r="C123" s="2" t="s">
-        <v>443</v>
+        <v>509</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A124" s="1" t="s">
-        <v>444</v>
+        <v>510</v>
       </c>
       <c r="B124" s="2" t="s">
-        <v>445</v>
+        <v>511</v>
       </c>
       <c r="C124" s="2" t="s">
-        <v>446</v>
+        <v>512</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A125" s="1" t="s">
-        <v>447</v>
+        <v>513</v>
       </c>
       <c r="B125" s="2" t="s">
-        <v>448</v>
+        <v>514</v>
       </c>
       <c r="C125" s="2" t="s">
-        <v>616</v>
+        <v>515</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B126" s="2"/>
-      <c r="C126" s="2"/>
+      <c r="A126" s="1" t="s">
+        <v>516</v>
+      </c>
+      <c r="B126" s="2" t="s">
+        <v>517</v>
+      </c>
+      <c r="C126" s="2" t="s">
+        <v>518</v>
+      </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A127" s="1" t="s">
-        <v>449</v>
-      </c>
-      <c r="B127" s="2" t="s">
-        <v>450</v>
-      </c>
-      <c r="C127" s="2" t="s">
-        <v>617</v>
-      </c>
-    </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B127" s="2"/>
+      <c r="C127" s="2"/>
+    </row>
+    <row r="128" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A128" s="1" t="s">
-        <v>451</v>
+        <v>519</v>
       </c>
       <c r="B128" s="2" t="s">
-        <v>452</v>
+        <v>520</v>
       </c>
       <c r="C128" s="2" t="s">
-        <v>618</v>
+        <v>521</v>
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A129" s="1" t="s">
-        <v>453</v>
+        <v>522</v>
       </c>
       <c r="B129" s="2" t="s">
-        <v>454</v>
+        <v>523</v>
       </c>
       <c r="C129" s="2" t="s">
-        <v>619</v>
+        <v>524</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A130" s="1" t="s">
-        <v>455</v>
+        <v>525</v>
       </c>
       <c r="B130" s="2" t="s">
-        <v>456</v>
+        <v>526</v>
       </c>
       <c r="C130" s="2" t="s">
-        <v>620</v>
+        <v>527</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A131" s="1" t="s">
-        <v>457</v>
+        <v>528</v>
       </c>
       <c r="B131" s="2" t="s">
-        <v>458</v>
+        <v>529</v>
       </c>
       <c r="C131" s="2" t="s">
-        <v>621</v>
+        <v>530</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A132" s="1" t="s">
-        <v>459</v>
+        <v>531</v>
       </c>
       <c r="B132" s="2" t="s">
-        <v>460</v>
+        <v>532</v>
       </c>
       <c r="C132" s="2" t="s">
-        <v>622</v>
+        <v>533</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A133" s="1" t="s">
-        <v>461</v>
+        <v>534</v>
       </c>
       <c r="B133" s="2" t="s">
-        <v>462</v>
+        <v>535</v>
       </c>
       <c r="C133" s="2" t="s">
-        <v>623</v>
+        <v>536</v>
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A134" s="1" t="s">
-        <v>463</v>
+        <v>537</v>
       </c>
       <c r="B134" s="2" t="s">
-        <v>464</v>
+        <v>538</v>
       </c>
       <c r="C134" s="2" t="s">
-        <v>624</v>
+        <v>539</v>
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B135" s="2"/>
-      <c r="C135" s="2"/>
+      <c r="A135" s="1" t="s">
+        <v>540</v>
+      </c>
+      <c r="B135" s="2" t="s">
+        <v>541</v>
+      </c>
+      <c r="C135" s="2" t="s">
+        <v>542</v>
+      </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A136" s="1" t="s">
-        <v>465</v>
-      </c>
-      <c r="B136" s="2" t="s">
-        <v>466</v>
-      </c>
-      <c r="C136" s="2" t="s">
-        <v>625</v>
-      </c>
-    </row>
-    <row r="137" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="B136" s="2"/>
+      <c r="C136" s="2"/>
+    </row>
+    <row r="137" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A137" s="1" t="s">
-        <v>467</v>
+        <v>543</v>
       </c>
       <c r="B137" s="2" t="s">
-        <v>468</v>
+        <v>544</v>
       </c>
       <c r="C137" s="2" t="s">
-        <v>626</v>
-      </c>
-    </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.35">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A138" s="1" t="s">
-        <v>469</v>
+        <v>546</v>
       </c>
       <c r="B138" s="2" t="s">
-        <v>470</v>
+        <v>547</v>
       </c>
       <c r="C138" s="2" t="s">
-        <v>627</v>
+        <v>548</v>
       </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A139" s="1" t="s">
-        <v>471</v>
+        <v>549</v>
       </c>
       <c r="B139" s="2" t="s">
-        <v>472</v>
+        <v>550</v>
       </c>
       <c r="C139" s="2" t="s">
-        <v>628</v>
-      </c>
-    </row>
-    <row r="141" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A141" s="1" t="s">
-        <v>473</v>
-      </c>
-      <c r="B141" s="2" t="s">
-        <v>474</v>
-      </c>
-      <c r="C141" s="2" t="s">
-        <v>629</v>
+        <v>551</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A140" s="1" t="s">
+        <v>552</v>
+      </c>
+      <c r="B140" s="2" t="s">
+        <v>553</v>
+      </c>
+      <c r="C140" s="2" t="s">
+        <v>554</v>
       </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A142" s="1" t="s">
-        <v>475</v>
+        <v>555</v>
       </c>
       <c r="B142" s="2" t="s">
-        <v>476</v>
+        <v>556</v>
       </c>
       <c r="C142" s="2" t="s">
-        <v>630</v>
+        <v>557</v>
       </c>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A143" s="1" t="s">
-        <v>477</v>
+        <v>558</v>
       </c>
       <c r="B143" s="2" t="s">
-        <v>478</v>
+        <v>559</v>
       </c>
       <c r="C143" s="2" t="s">
-        <v>631</v>
+        <v>560</v>
       </c>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A144" s="1" t="s">
-        <v>479</v>
+        <v>561</v>
       </c>
       <c r="B144" s="2" t="s">
-        <v>480</v>
+        <v>562</v>
       </c>
       <c r="C144" s="2" t="s">
-        <v>632</v>
+        <v>563</v>
       </c>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A145" s="1" t="s">
-        <v>481</v>
+        <v>564</v>
       </c>
       <c r="B145" s="2" t="s">
-        <v>482</v>
+        <v>565</v>
       </c>
       <c r="C145" s="2" t="s">
-        <v>633</v>
+        <v>566</v>
       </c>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A146" s="1" t="s">
-        <v>483</v>
+        <v>567</v>
       </c>
       <c r="B146" s="2" t="s">
-        <v>484</v>
+        <v>568</v>
       </c>
       <c r="C146" s="2" t="s">
-        <v>634</v>
+        <v>569</v>
       </c>
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A147" s="1" t="s">
-        <v>485</v>
+        <v>570</v>
       </c>
       <c r="B147" s="2" t="s">
-        <v>486</v>
+        <v>571</v>
       </c>
       <c r="C147" s="2" t="s">
-        <v>635</v>
-      </c>
-    </row>
-    <row r="149" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A149" s="1" t="s">
-        <v>487</v>
-      </c>
-      <c r="B149" s="2" t="s">
-        <v>488</v>
-      </c>
-      <c r="C149" s="2" t="s">
-        <v>636</v>
+        <v>572</v>
+      </c>
+    </row>
+    <row r="148" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A148" s="1" t="s">
+        <v>573</v>
+      </c>
+      <c r="B148" s="2" t="s">
+        <v>574</v>
+      </c>
+      <c r="C148" s="2" t="s">
+        <v>575</v>
       </c>
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A150" s="1" t="s">
-        <v>489</v>
+        <v>576</v>
       </c>
       <c r="B150" s="2" t="s">
-        <v>490</v>
+        <v>577</v>
       </c>
       <c r="C150" s="2" t="s">
-        <v>637</v>
+        <v>578</v>
       </c>
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A151" s="1" t="s">
-        <v>491</v>
+        <v>579</v>
       </c>
       <c r="B151" s="2" t="s">
-        <v>492</v>
+        <v>580</v>
       </c>
       <c r="C151" s="2" t="s">
-        <v>638</v>
-      </c>
-    </row>
-    <row r="152" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
+        <v>581</v>
+      </c>
+    </row>
+    <row r="152" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A152" s="1" t="s">
-        <v>493</v>
+        <v>582</v>
       </c>
       <c r="B152" s="2" t="s">
-        <v>494</v>
+        <v>583</v>
       </c>
       <c r="C152" s="2" t="s">
-        <v>639</v>
-      </c>
-    </row>
-    <row r="153" spans="1:3" x14ac:dyDescent="0.35">
+        <v>584</v>
+      </c>
+    </row>
+    <row r="153" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A153" s="1" t="s">
-        <v>495</v>
+        <v>585</v>
       </c>
       <c r="B153" s="2" t="s">
-        <v>496</v>
+        <v>586</v>
       </c>
       <c r="C153" s="2" t="s">
-        <v>640</v>
-      </c>
-    </row>
-    <row r="155" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A155" s="1" t="s">
-        <v>497</v>
-      </c>
-      <c r="B155" s="2" t="s">
-        <v>498</v>
-      </c>
-      <c r="C155" s="2" t="s">
-        <v>641</v>
+        <v>587</v>
+      </c>
+    </row>
+    <row r="154" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A154" s="1" t="s">
+        <v>588</v>
+      </c>
+      <c r="B154" s="2" t="s">
+        <v>589</v>
+      </c>
+      <c r="C154" s="2" t="s">
+        <v>590</v>
       </c>
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A156" s="1" t="s">
-        <v>499</v>
-      </c>
-      <c r="B156" s="1" t="s">
-        <v>500</v>
-      </c>
-      <c r="C156" s="1" t="s">
-        <v>642</v>
-      </c>
-    </row>
-    <row r="157" spans="1:3" x14ac:dyDescent="0.35">
+        <v>591</v>
+      </c>
+      <c r="B156" s="2" t="s">
+        <v>592</v>
+      </c>
+      <c r="C156" s="2" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="157" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A157" s="1" t="s">
-        <v>501</v>
-      </c>
-      <c r="B157" s="1" t="s">
-        <v>502</v>
-      </c>
-      <c r="C157" s="1" t="s">
-        <v>643</v>
+        <v>594</v>
+      </c>
+      <c r="B157" s="2" t="s">
+        <v>595</v>
+      </c>
+      <c r="C157" s="2" t="s">
+        <v>596</v>
       </c>
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A158" s="1" t="s">
-        <v>503</v>
-      </c>
-      <c r="B158" s="2" t="s">
-        <v>504</v>
+        <v>597</v>
+      </c>
+      <c r="B158" s="1" t="s">
+        <v>598</v>
       </c>
       <c r="C158" s="1" t="s">
-        <v>644</v>
+        <v>599</v>
       </c>
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A159" s="1" t="s">
-        <v>505</v>
-      </c>
-      <c r="B159" s="1" t="s">
-        <v>506</v>
+        <v>600</v>
+      </c>
+      <c r="B159" s="2" t="s">
+        <v>601</v>
       </c>
       <c r="C159" s="1" t="s">
-        <v>645</v>
+        <v>602</v>
       </c>
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A160" s="1" t="s">
-        <v>507</v>
-      </c>
-      <c r="B160" s="2" t="s">
-        <v>508</v>
-      </c>
-      <c r="C160" s="2" t="s">
-        <v>509</v>
-      </c>
-    </row>
-    <row r="162" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A162" s="1" t="s">
-        <v>510</v>
-      </c>
-      <c r="B162" s="2" t="s">
-        <v>511</v>
-      </c>
-      <c r="C162" s="2" t="s">
-        <v>646</v>
+        <v>603</v>
+      </c>
+      <c r="B160" s="1" t="s">
+        <v>604</v>
+      </c>
+      <c r="C160" s="1" t="s">
+        <v>605</v>
+      </c>
+    </row>
+    <row r="161" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A161" s="1" t="s">
+        <v>606</v>
+      </c>
+      <c r="B161" s="2" t="s">
+        <v>607</v>
+      </c>
+      <c r="C161" s="2" t="s">
+        <v>608</v>
       </c>
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A163" s="1" t="s">
-        <v>512</v>
+        <v>609</v>
       </c>
       <c r="B163" s="2" t="s">
-        <v>513</v>
+        <v>610</v>
       </c>
       <c r="C163" s="2" t="s">
-        <v>647</v>
+        <v>611</v>
       </c>
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B164" s="2"/>
-      <c r="C164" s="2"/>
+      <c r="A164" s="1" t="s">
+        <v>612</v>
+      </c>
+      <c r="B164" s="2" t="s">
+        <v>613</v>
+      </c>
+      <c r="C164" s="2" t="s">
+        <v>614</v>
+      </c>
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A165" s="1" t="s">
-        <v>514</v>
-      </c>
-      <c r="B165" s="2" t="s">
-        <v>515</v>
-      </c>
-      <c r="C165" s="2" t="s">
-        <v>648</v>
-      </c>
+      <c r="B165" s="2"/>
+      <c r="C165" s="2"/>
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A166" s="1" t="s">
-        <v>516</v>
+        <v>615</v>
       </c>
       <c r="B166" s="2" t="s">
-        <v>517</v>
+        <v>616</v>
       </c>
       <c r="C166" s="2" t="s">
-        <v>649</v>
+        <v>617</v>
       </c>
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A167" s="1" t="s">
-        <v>518</v>
+        <v>618</v>
       </c>
       <c r="B167" s="2" t="s">
-        <v>519</v>
+        <v>619</v>
       </c>
       <c r="C167" s="2" t="s">
-        <v>650</v>
+        <v>620</v>
       </c>
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A168" s="1" t="s">
-        <v>520</v>
+        <v>621</v>
       </c>
       <c r="B168" s="2" t="s">
-        <v>521</v>
+        <v>622</v>
       </c>
       <c r="C168" s="2" t="s">
-        <v>651</v>
+        <v>623</v>
       </c>
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A169" s="1" t="s">
-        <v>522</v>
+        <v>624</v>
       </c>
       <c r="B169" s="2" t="s">
-        <v>523</v>
+        <v>625</v>
       </c>
       <c r="C169" s="2" t="s">
-        <v>652</v>
+        <v>626</v>
       </c>
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B170" s="2"/>
-      <c r="C170" s="2"/>
+      <c r="A170" s="1" t="s">
+        <v>627</v>
+      </c>
+      <c r="B170" s="2" t="s">
+        <v>628</v>
+      </c>
+      <c r="C170" s="2" t="s">
+        <v>629</v>
+      </c>
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A171" s="1" t="s">
-        <v>524</v>
-      </c>
-      <c r="B171" s="2" t="s">
-        <v>525</v>
-      </c>
-      <c r="C171" s="2" t="s">
-        <v>653</v>
-      </c>
+      <c r="B171" s="2"/>
+      <c r="C171" s="2"/>
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A172" s="1" t="s">
-        <v>526</v>
+        <v>630</v>
       </c>
       <c r="B172" s="2" t="s">
-        <v>527</v>
+        <v>631</v>
       </c>
       <c r="C172" s="2" t="s">
-        <v>654</v>
+        <v>632</v>
       </c>
     </row>
     <row r="173" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A173" s="1" t="s">
-        <v>528</v>
+        <v>633</v>
       </c>
       <c r="B173" s="2" t="s">
-        <v>529</v>
+        <v>634</v>
       </c>
       <c r="C173" s="2" t="s">
-        <v>655</v>
+        <v>635</v>
       </c>
     </row>
     <row r="174" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A174" s="1" t="s">
-        <v>530</v>
+        <v>636</v>
       </c>
       <c r="B174" s="2" t="s">
-        <v>531</v>
+        <v>637</v>
       </c>
       <c r="C174" s="2" t="s">
-        <v>656</v>
+        <v>638</v>
       </c>
     </row>
     <row r="175" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A175" s="1" t="s">
-        <v>532</v>
+        <v>639</v>
       </c>
       <c r="B175" s="2" t="s">
-        <v>533</v>
+        <v>640</v>
       </c>
       <c r="C175" s="2" t="s">
-        <v>657</v>
+        <v>641</v>
       </c>
     </row>
     <row r="176" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A176" s="1" t="s">
-        <v>534</v>
+        <v>642</v>
       </c>
       <c r="B176" s="2" t="s">
-        <v>535</v>
+        <v>643</v>
       </c>
       <c r="C176" s="2" t="s">
-        <v>658</v>
+        <v>644</v>
+      </c>
+    </row>
+    <row r="177" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A177" s="1" t="s">
+        <v>645</v>
+      </c>
+      <c r="B177" s="2" t="s">
+        <v>646</v>
+      </c>
+      <c r="C177" s="2" t="s">
+        <v>647</v>
       </c>
     </row>
     <row r="178" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A178" s="1" t="s">
-        <v>536</v>
-      </c>
-      <c r="B178" s="1" t="s">
-        <v>537</v>
-      </c>
-      <c r="C178" s="1" t="s">
-        <v>660</v>
-      </c>
-    </row>
-    <row r="179" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A179" s="1" t="s">
-        <v>538</v>
-      </c>
-      <c r="B179" s="1" t="s">
-        <v>539</v>
-      </c>
-      <c r="C179" s="1" t="s">
-        <v>661</v>
+        <v>648</v>
+      </c>
+      <c r="B178" s="2" t="s">
+        <v>649</v>
+      </c>
+      <c r="C178" s="2" t="s">
+        <v>650</v>
       </c>
     </row>
     <row r="180" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A180" s="1" t="s">
-        <v>540</v>
+        <v>651</v>
       </c>
       <c r="B180" s="1" t="s">
-        <v>541</v>
+        <v>652</v>
       </c>
       <c r="C180" s="1" t="s">
-        <v>662</v>
+        <v>653</v>
       </c>
     </row>
     <row r="181" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A181" s="1" t="s">
-        <v>542</v>
+        <v>654</v>
       </c>
       <c r="B181" s="1" t="s">
-        <v>543</v>
+        <v>655</v>
       </c>
       <c r="C181" s="1" t="s">
-        <v>663</v>
+        <v>656</v>
       </c>
     </row>
     <row r="182" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A182" s="1" t="s">
-        <v>544</v>
-      </c>
-      <c r="B182" s="2" t="s">
-        <v>545</v>
-      </c>
-      <c r="C182" s="2" t="s">
-        <v>664</v>
+        <v>657</v>
+      </c>
+      <c r="B182" s="1" t="s">
+        <v>658</v>
+      </c>
+      <c r="C182" s="1" t="s">
+        <v>659</v>
       </c>
     </row>
     <row r="183" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A183" s="1" t="s">
-        <v>546</v>
+        <v>660</v>
       </c>
       <c r="B183" s="1" t="s">
-        <v>547</v>
+        <v>661</v>
       </c>
       <c r="C183" s="1" t="s">
-        <v>665</v>
+        <v>662</v>
       </c>
     </row>
     <row r="184" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A184" s="1" t="s">
-        <v>548</v>
-      </c>
-      <c r="B184" s="1" t="s">
-        <v>659</v>
-      </c>
-      <c r="C184" s="1" t="s">
+        <v>663</v>
+      </c>
+      <c r="B184" s="2" t="s">
+        <v>664</v>
+      </c>
+      <c r="C184" s="2" t="s">
+        <v>665</v>
+      </c>
+    </row>
+    <row r="185" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A185" s="1" t="s">
         <v>666</v>
+      </c>
+      <c r="B185" s="1" t="s">
+        <v>667</v>
+      </c>
+      <c r="C185" s="1" t="s">
+        <v>668</v>
+      </c>
+    </row>
+    <row r="186" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A186" s="1" t="s">
+        <v>669</v>
+      </c>
+      <c r="B186" s="1" t="s">
+        <v>670</v>
+      </c>
+      <c r="C186" s="1" t="s">
+        <v>671</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Cache and reuse Folders data
</commit_message>
<xml_diff>
--- a/Config.xlsx
+++ b/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mateus.cruz\Documents\GitHub\OrchestratorManager\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4A4D242-857B-4B82-8949-94B9524037BA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A23C3BF-1052-4556-A937-074ABD8C1624}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="721" uniqueCount="673">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="724" uniqueCount="676">
   <si>
     <t>Name</t>
   </si>
@@ -1347,6 +1347,15 @@
   </si>
   <si>
     <t>名前が指定されていません。</t>
+  </si>
+  <si>
+    <t>NameAlreadyUsed</t>
+  </si>
+  <si>
+    <t>The name {0} is already used.</t>
+  </si>
+  <si>
+    <t>名前 {0} は既に使用されています。</t>
   </si>
   <si>
     <t>VersionNotSpecified</t>
@@ -2190,8 +2199,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table13" displayName="Table13" ref="A1:C186" totalsRowShown="0">
-  <autoFilter ref="A1:C186" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table13" displayName="Table13" ref="A1:C187" totalsRowShown="0">
+  <autoFilter ref="A1:C187" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Name"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="EN"/>
@@ -2512,7 +2521,7 @@
         <v>7</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>672</v>
+        <v>675</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>8</v>
@@ -3283,7 +3292,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1927ABA9-1814-4487-9CEC-ABDCAF91481F}">
-  <dimension ref="A1:C186"/>
+  <dimension ref="A1:C187"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2 A2"/>
@@ -4415,7 +4424,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="104" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A104" s="1" t="s">
         <v>456</v>
       </c>
@@ -4437,7 +4446,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A106" s="1" t="s">
         <v>462</v>
       </c>
@@ -4460,19 +4469,19 @@
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B108" s="2"/>
-      <c r="C108" s="2"/>
+      <c r="A108" s="1" t="s">
+        <v>468</v>
+      </c>
+      <c r="B108" s="2" t="s">
+        <v>469</v>
+      </c>
+      <c r="C108" s="2" t="s">
+        <v>470</v>
+      </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A109" s="1" t="s">
-        <v>468</v>
-      </c>
-      <c r="B109" s="2" t="s">
-        <v>469</v>
-      </c>
-      <c r="C109" s="2" t="s">
-        <v>470</v>
-      </c>
+      <c r="B109" s="2"/>
+      <c r="C109" s="2"/>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A110" s="1" t="s">
@@ -4552,19 +4561,19 @@
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B117" s="2"/>
-      <c r="C117" s="2"/>
+      <c r="A117" s="1" t="s">
+        <v>492</v>
+      </c>
+      <c r="B117" s="2" t="s">
+        <v>493</v>
+      </c>
+      <c r="C117" s="2" t="s">
+        <v>494</v>
+      </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A118" s="1" t="s">
-        <v>492</v>
-      </c>
-      <c r="B118" s="2" t="s">
-        <v>493</v>
-      </c>
-      <c r="C118" s="2" t="s">
-        <v>494</v>
-      </c>
+      <c r="B118" s="2"/>
+      <c r="C118" s="2"/>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A119" s="1" t="s">
@@ -4655,21 +4664,21 @@
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B127" s="2"/>
-      <c r="C127" s="2"/>
-    </row>
-    <row r="128" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A128" s="1" t="s">
+      <c r="A127" s="1" t="s">
         <v>519</v>
       </c>
-      <c r="B128" s="2" t="s">
+      <c r="B127" s="2" t="s">
         <v>520</v>
       </c>
-      <c r="C128" s="2" t="s">
+      <c r="C127" s="2" t="s">
         <v>521</v>
       </c>
     </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B128" s="2"/>
+      <c r="C128" s="2"/>
+    </row>
+    <row r="129" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A129" s="1" t="s">
         <v>522</v>
       </c>
@@ -4747,21 +4756,21 @@
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B136" s="2"/>
-      <c r="C136" s="2"/>
+      <c r="A136" s="1" t="s">
+        <v>543</v>
+      </c>
+      <c r="B136" s="2" t="s">
+        <v>544</v>
+      </c>
+      <c r="C136" s="2" t="s">
+        <v>545</v>
+      </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A137" s="1" t="s">
-        <v>543</v>
-      </c>
-      <c r="B137" s="2" t="s">
-        <v>544</v>
-      </c>
-      <c r="C137" s="2" t="s">
-        <v>545</v>
-      </c>
-    </row>
-    <row r="138" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B137" s="2"/>
+      <c r="C137" s="2"/>
+    </row>
+    <row r="138" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A138" s="1" t="s">
         <v>546</v>
       </c>
@@ -4772,7 +4781,7 @@
         <v>548</v>
       </c>
     </row>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A139" s="1" t="s">
         <v>549</v>
       </c>
@@ -4794,14 +4803,14 @@
         <v>554</v>
       </c>
     </row>
-    <row r="142" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A142" s="1" t="s">
+    <row r="141" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A141" s="1" t="s">
         <v>555</v>
       </c>
-      <c r="B142" s="2" t="s">
+      <c r="B141" s="2" t="s">
         <v>556</v>
       </c>
-      <c r="C142" s="2" t="s">
+      <c r="C141" s="2" t="s">
         <v>557</v>
       </c>
     </row>
@@ -4871,14 +4880,14 @@
         <v>575</v>
       </c>
     </row>
-    <row r="150" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A150" s="1" t="s">
+    <row r="149" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A149" s="1" t="s">
         <v>576</v>
       </c>
-      <c r="B150" s="2" t="s">
+      <c r="B149" s="2" t="s">
         <v>577</v>
       </c>
-      <c r="C150" s="2" t="s">
+      <c r="C149" s="2" t="s">
         <v>578</v>
       </c>
     </row>
@@ -4904,7 +4913,7 @@
         <v>584</v>
       </c>
     </row>
-    <row r="153" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A153" s="1" t="s">
         <v>585</v>
       </c>
@@ -4915,7 +4924,7 @@
         <v>587</v>
       </c>
     </row>
-    <row r="154" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A154" s="1" t="s">
         <v>588</v>
       </c>
@@ -4926,18 +4935,18 @@
         <v>590</v>
       </c>
     </row>
-    <row r="156" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A156" s="1" t="s">
+    <row r="155" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A155" s="1" t="s">
         <v>591</v>
       </c>
-      <c r="B156" s="2" t="s">
+      <c r="B155" s="2" t="s">
         <v>592</v>
       </c>
-      <c r="C156" s="2" t="s">
+      <c r="C155" s="2" t="s">
         <v>593</v>
       </c>
     </row>
-    <row r="157" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A157" s="1" t="s">
         <v>594</v>
       </c>
@@ -4948,14 +4957,14 @@
         <v>596</v>
       </c>
     </row>
-    <row r="158" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A158" s="1" t="s">
         <v>597</v>
       </c>
-      <c r="B158" s="1" t="s">
+      <c r="B158" s="2" t="s">
         <v>598</v>
       </c>
-      <c r="C158" s="1" t="s">
+      <c r="C158" s="2" t="s">
         <v>599</v>
       </c>
     </row>
@@ -4963,7 +4972,7 @@
       <c r="A159" s="1" t="s">
         <v>600</v>
       </c>
-      <c r="B159" s="2" t="s">
+      <c r="B159" s="1" t="s">
         <v>601</v>
       </c>
       <c r="C159" s="1" t="s">
@@ -4974,7 +4983,7 @@
       <c r="A160" s="1" t="s">
         <v>603</v>
       </c>
-      <c r="B160" s="1" t="s">
+      <c r="B160" s="2" t="s">
         <v>604</v>
       </c>
       <c r="C160" s="1" t="s">
@@ -4985,21 +4994,21 @@
       <c r="A161" s="1" t="s">
         <v>606</v>
       </c>
-      <c r="B161" s="2" t="s">
+      <c r="B161" s="1" t="s">
         <v>607</v>
       </c>
-      <c r="C161" s="2" t="s">
+      <c r="C161" s="1" t="s">
         <v>608</v>
       </c>
     </row>
-    <row r="163" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A163" s="1" t="s">
+    <row r="162" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A162" s="1" t="s">
         <v>609</v>
       </c>
-      <c r="B163" s="2" t="s">
+      <c r="B162" s="2" t="s">
         <v>610</v>
       </c>
-      <c r="C163" s="2" t="s">
+      <c r="C162" s="2" t="s">
         <v>611</v>
       </c>
     </row>
@@ -5015,19 +5024,19 @@
       </c>
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B165" s="2"/>
-      <c r="C165" s="2"/>
+      <c r="A165" s="1" t="s">
+        <v>615</v>
+      </c>
+      <c r="B165" s="2" t="s">
+        <v>616</v>
+      </c>
+      <c r="C165" s="2" t="s">
+        <v>617</v>
+      </c>
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A166" s="1" t="s">
-        <v>615</v>
-      </c>
-      <c r="B166" s="2" t="s">
-        <v>616</v>
-      </c>
-      <c r="C166" s="2" t="s">
-        <v>617</v>
-      </c>
+      <c r="B166" s="2"/>
+      <c r="C166" s="2"/>
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A167" s="1" t="s">
@@ -5074,19 +5083,19 @@
       </c>
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B171" s="2"/>
-      <c r="C171" s="2"/>
+      <c r="A171" s="1" t="s">
+        <v>630</v>
+      </c>
+      <c r="B171" s="2" t="s">
+        <v>631</v>
+      </c>
+      <c r="C171" s="2" t="s">
+        <v>632</v>
+      </c>
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A172" s="1" t="s">
-        <v>630</v>
-      </c>
-      <c r="B172" s="2" t="s">
-        <v>631</v>
-      </c>
-      <c r="C172" s="2" t="s">
-        <v>632</v>
-      </c>
+      <c r="B172" s="2"/>
+      <c r="C172" s="2"/>
     </row>
     <row r="173" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A173" s="1" t="s">
@@ -5154,14 +5163,14 @@
         <v>650</v>
       </c>
     </row>
-    <row r="180" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A180" s="1" t="s">
+    <row r="179" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A179" s="1" t="s">
         <v>651</v>
       </c>
-      <c r="B180" s="1" t="s">
+      <c r="B179" s="2" t="s">
         <v>652</v>
       </c>
-      <c r="C180" s="1" t="s">
+      <c r="C179" s="2" t="s">
         <v>653</v>
       </c>
     </row>
@@ -5202,10 +5211,10 @@
       <c r="A184" s="1" t="s">
         <v>663</v>
       </c>
-      <c r="B184" s="2" t="s">
+      <c r="B184" s="1" t="s">
         <v>664</v>
       </c>
-      <c r="C184" s="2" t="s">
+      <c r="C184" s="1" t="s">
         <v>665</v>
       </c>
     </row>
@@ -5213,10 +5222,10 @@
       <c r="A185" s="1" t="s">
         <v>666</v>
       </c>
-      <c r="B185" s="1" t="s">
+      <c r="B185" s="2" t="s">
         <v>667</v>
       </c>
-      <c r="C185" s="1" t="s">
+      <c r="C185" s="2" t="s">
         <v>668</v>
       </c>
     </row>
@@ -5229,6 +5238,17 @@
       </c>
       <c r="C186" s="1" t="s">
         <v>671</v>
+      </c>
+    </row>
+    <row r="187" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A187" s="1" t="s">
+        <v>672</v>
+      </c>
+      <c r="B187" s="1" t="s">
+        <v>673</v>
+      </c>
+      <c r="C187" s="1" t="s">
+        <v>674</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
User field names when updating cached data in Create workflows
</commit_message>
<xml_diff>
--- a/Config.xlsx
+++ b/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mateus.cruz\Documents\GitHub\OrchestratorManager\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A23C3BF-1052-4556-A937-074ABD8C1624}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77FCC7CF-8054-40EE-A670-1EB0403B2115}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -81,9 +81,6 @@
     <t>OnPremisesOrchestratorURL</t>
   </si>
   <si>
-    <t>https://myOrchestratorURL</t>
-  </si>
-  <si>
     <t>URL of the Orchestrator instance to be used. 
 This parameter is exclusive to on-premises Orchestrator instances.
 Sample value: https://myOrchestratorURL</t>
@@ -2107,6 +2104,9 @@
   </si>
   <si>
     <t>SampleAccount</t>
+  </si>
+  <si>
+    <t>https://myOrchestratorURL</t>
   </si>
 </sst>
 </file>
@@ -2521,7 +2521,7 @@
         <v>7</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>8</v>
@@ -2543,21 +2543,21 @@
         <v>12</v>
       </c>
       <c r="B6" s="3" t="s">
+        <v>675</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>13</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="159.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B7" s="1">
         <v>201804</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -2597,684 +2597,684 @@
     </row>
     <row r="2" spans="1:3" ht="101.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B2" s="1">
         <v>200</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B3" s="1">
         <v>0</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B4" s="1">
         <v>550</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B5" s="1">
         <v>650</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B6" s="1">
         <v>3</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B7" s="1">
         <v>5000</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="C8" s="2" t="s">
         <v>30</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B9" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="C9" s="2" t="s">
         <v>33</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="C10" s="2" t="s">
         <v>36</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="C11" s="2" t="s">
         <v>39</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="C12" s="2" t="s">
         <v>42</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="C13" s="2" t="s">
         <v>45</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="C14" s="2" t="s">
         <v>48</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B15" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="C15" s="2" t="s">
         <v>51</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B16" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="C16" s="2" t="s">
         <v>54</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B17" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="C17" s="2" t="s">
         <v>57</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B18" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="C18" s="2" t="s">
         <v>60</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B19" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="C19" s="2" t="s">
         <v>63</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B20" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="C20" s="2" t="s">
         <v>66</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B21" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="C21" s="2" t="s">
         <v>69</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C22" s="2" t="s">
         <v>71</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C23" s="2" t="s">
         <v>73</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B24" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="C24" s="2" t="s">
         <v>76</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C26" s="2" t="s">
         <v>79</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C27" s="2" t="s">
         <v>81</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C28" s="2" t="s">
         <v>83</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C29" s="2" t="s">
         <v>85</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A30" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B30" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="B30" s="1" t="s">
+      <c r="C30" s="2" t="s">
         <v>88</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B31" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="B31" s="1" t="s">
+      <c r="C31" s="2" t="s">
         <v>91</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C32" s="2" t="s">
         <v>93</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="C32" s="2" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A33" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B33" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="B33" s="1" t="s">
+      <c r="C33" s="2" t="s">
         <v>96</v>
-      </c>
-      <c r="C33" s="2" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A34" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C34" s="2" t="s">
         <v>98</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="C34" s="2" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A35" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C35" s="2" t="s">
         <v>100</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="C35" s="2" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A36" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C36" s="2" t="s">
         <v>102</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="C36" s="2" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A37" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C37" s="2" t="s">
         <v>104</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="C37" s="2" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A38" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C38" s="2" t="s">
         <v>106</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="C38" s="2" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A39" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C39" s="2" t="s">
         <v>108</v>
-      </c>
-      <c r="B39" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="C39" s="2" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A40" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C40" s="2" t="s">
         <v>110</v>
-      </c>
-      <c r="B40" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="C40" s="2" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="41" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A41" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C41" s="2" t="s">
         <v>112</v>
-      </c>
-      <c r="B41" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="C41" s="2" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="42" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A42" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C42" s="2" t="s">
         <v>114</v>
-      </c>
-      <c r="B42" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="C42" s="2" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="43" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A43" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C43" s="2" t="s">
         <v>116</v>
-      </c>
-      <c r="B43" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="C43" s="2" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A44" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C44" s="2" t="s">
         <v>118</v>
-      </c>
-      <c r="B44" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="C44" s="2" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="45" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A45" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C45" s="2" t="s">
         <v>120</v>
-      </c>
-      <c r="B45" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="C45" s="2" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="46" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A46" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C46" s="2" t="s">
         <v>122</v>
-      </c>
-      <c r="B46" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="C46" s="2" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="47" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A47" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C47" s="2" t="s">
         <v>124</v>
-      </c>
-      <c r="B47" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="C47" s="2" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="48" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A48" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C48" s="2" t="s">
         <v>126</v>
-      </c>
-      <c r="B48" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="C48" s="2" t="s">
-        <v>127</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A49" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="B49" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="B49" s="1" t="s">
+      <c r="C49" s="2" t="s">
         <v>129</v>
-      </c>
-      <c r="C49" s="2" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="50" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A50" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C50" s="2" t="s">
         <v>131</v>
-      </c>
-      <c r="B50" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="C50" s="2" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="51" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A51" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C51" s="2" t="s">
         <v>133</v>
-      </c>
-      <c r="B51" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="C51" s="2" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A52" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C52" s="2" t="s">
         <v>135</v>
-      </c>
-      <c r="B52" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="C52" s="2" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="53" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A53" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C53" s="2" t="s">
         <v>137</v>
-      </c>
-      <c r="B53" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="C53" s="2" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="54" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A54" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C54" s="2" t="s">
         <v>139</v>
-      </c>
-      <c r="B54" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="C54" s="2" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A55" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="C55" s="2" t="s">
         <v>141</v>
-      </c>
-      <c r="B55" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="C55" s="2" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="56" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A56" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C56" s="2" t="s">
         <v>143</v>
-      </c>
-      <c r="B56" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="C56" s="2" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="57" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A57" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C57" s="2" t="s">
         <v>145</v>
-      </c>
-      <c r="B57" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="C57" s="2" t="s">
-        <v>146</v>
       </c>
     </row>
     <row r="58" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A58" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C58" s="2" t="s">
         <v>147</v>
-      </c>
-      <c r="B58" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="C58" s="2" t="s">
-        <v>148</v>
       </c>
     </row>
     <row r="59" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A59" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C59" s="2" t="s">
         <v>149</v>
-      </c>
-      <c r="B59" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="C59" s="2" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="60" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A60" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C60" s="2" t="s">
         <v>151</v>
-      </c>
-      <c r="B60" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="C60" s="2" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="61" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A61" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C61" s="2" t="s">
         <v>153</v>
-      </c>
-      <c r="B61" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="C61" s="2" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="62" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A62" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C62" s="2" t="s">
         <v>155</v>
-      </c>
-      <c r="B62" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="C62" s="2" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="63" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A63" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="C63" s="2" t="s">
         <v>157</v>
-      </c>
-      <c r="B63" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="C63" s="2" t="s">
-        <v>158</v>
       </c>
     </row>
   </sheetData>
@@ -3310,472 +3310,472 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>159</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>160</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>161</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>162</v>
-      </c>
       <c r="C2" s="2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="43.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>163</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="C3" s="2" t="s">
         <v>164</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>165</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>166</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="C4" s="2" t="s">
         <v>167</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>168</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>170</v>
-      </c>
       <c r="C5" s="2" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="C6" s="2" t="s">
         <v>172</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>173</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="C7" s="2" t="s">
         <v>175</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>176</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>177</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="C8" s="2" t="s">
         <v>178</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>179</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="C9" s="2" t="s">
         <v>181</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>182</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="C10" s="2" t="s">
         <v>184</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>185</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>186</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="C11" s="2" t="s">
         <v>187</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>188</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="B12" s="2" t="s">
         <v>189</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="C12" s="2" t="s">
         <v>190</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>191</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="B13" s="2" t="s">
         <v>192</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="C13" s="2" t="s">
         <v>193</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>194</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="B14" s="2" t="s">
         <v>195</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="C14" s="2" t="s">
         <v>196</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>197</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="B15" s="2" t="s">
         <v>198</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="C15" s="2" t="s">
         <v>199</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>200</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="B16" s="2" t="s">
         <v>201</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="C16" s="2" t="s">
         <v>202</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>203</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="B17" s="2" t="s">
         <v>204</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="C17" s="2" t="s">
         <v>205</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>206</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="B18" s="2" t="s">
         <v>207</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="C18" s="2" t="s">
         <v>208</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>209</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="B19" s="2" t="s">
         <v>210</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="C19" s="2" t="s">
         <v>211</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>212</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="B20" s="2" t="s">
         <v>213</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="C20" s="2" t="s">
         <v>214</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>215</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="B21" s="2" t="s">
         <v>216</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="C21" s="2" t="s">
         <v>217</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>218</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="B22" s="2" t="s">
         <v>219</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="C22" s="2" t="s">
         <v>220</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>221</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="B23" s="2" t="s">
         <v>222</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="C23" s="2" t="s">
         <v>223</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>224</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="B24" s="2" t="s">
         <v>225</v>
       </c>
-      <c r="B24" s="2" t="s">
+      <c r="C24" s="2" t="s">
         <v>226</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>227</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="B25" s="2" t="s">
         <v>228</v>
       </c>
-      <c r="B25" s="2" t="s">
+      <c r="C25" s="2" t="s">
         <v>229</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>230</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="B26" s="2" t="s">
         <v>231</v>
       </c>
-      <c r="B26" s="2" t="s">
+      <c r="C26" s="2" t="s">
         <v>232</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>233</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="B27" s="2" t="s">
         <v>234</v>
       </c>
-      <c r="B27" s="2" t="s">
-        <v>235</v>
-      </c>
       <c r="C27" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="B28" s="2" t="s">
         <v>236</v>
       </c>
-      <c r="B28" s="2" t="s">
-        <v>237</v>
-      </c>
       <c r="C28" s="2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="B29" s="2" t="s">
         <v>238</v>
       </c>
-      <c r="B29" s="2" t="s">
+      <c r="C29" s="2" t="s">
         <v>239</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>240</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A30" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="B30" s="2" t="s">
         <v>241</v>
       </c>
-      <c r="B30" s="2" t="s">
+      <c r="C30" s="2" t="s">
         <v>242</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>243</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A31" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="B31" s="2" t="s">
         <v>244</v>
       </c>
-      <c r="B31" s="2" t="s">
-        <v>245</v>
-      </c>
       <c r="C31" s="2" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A32" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="B32" s="2" t="s">
         <v>246</v>
       </c>
-      <c r="B32" s="2" t="s">
+      <c r="C32" s="2" t="s">
         <v>247</v>
-      </c>
-      <c r="C32" s="2" t="s">
-        <v>248</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A33" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="B33" s="2" t="s">
         <v>249</v>
       </c>
-      <c r="B33" s="2" t="s">
+      <c r="C33" s="2" t="s">
         <v>250</v>
-      </c>
-      <c r="C33" s="2" t="s">
-        <v>251</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A34" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="B34" s="2" t="s">
         <v>252</v>
       </c>
-      <c r="B34" s="2" t="s">
+      <c r="C34" s="2" t="s">
         <v>253</v>
-      </c>
-      <c r="C34" s="2" t="s">
-        <v>254</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A35" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="B35" s="2" t="s">
         <v>255</v>
       </c>
-      <c r="B35" s="2" t="s">
+      <c r="C35" s="2" t="s">
         <v>256</v>
-      </c>
-      <c r="C35" s="2" t="s">
-        <v>257</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A36" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="B36" s="2" t="s">
         <v>258</v>
       </c>
-      <c r="B36" s="2" t="s">
+      <c r="C36" s="2" t="s">
         <v>259</v>
-      </c>
-      <c r="C36" s="2" t="s">
-        <v>260</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A37" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="B37" s="2" t="s">
         <v>261</v>
       </c>
-      <c r="B37" s="2" t="s">
+      <c r="C37" s="2" t="s">
         <v>262</v>
-      </c>
-      <c r="C37" s="2" t="s">
-        <v>263</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A38" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="B38" s="1" t="s">
         <v>264</v>
       </c>
-      <c r="B38" s="1" t="s">
+      <c r="C38" s="1" t="s">
         <v>265</v>
-      </c>
-      <c r="C38" s="1" t="s">
-        <v>266</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A39" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="B39" s="2" t="s">
         <v>267</v>
       </c>
-      <c r="B39" s="2" t="s">
+      <c r="C39" s="2" t="s">
         <v>268</v>
-      </c>
-      <c r="C39" s="2" t="s">
-        <v>269</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="43.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A40" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="B40" s="2" t="s">
         <v>270</v>
       </c>
-      <c r="B40" s="2" t="s">
+      <c r="C40" s="2" t="s">
         <v>271</v>
-      </c>
-      <c r="C40" s="2" t="s">
-        <v>272</v>
       </c>
     </row>
     <row r="41" spans="1:3" ht="43.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A41" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="B41" s="2" t="s">
         <v>273</v>
       </c>
-      <c r="B41" s="2" t="s">
+      <c r="C41" s="2" t="s">
         <v>274</v>
-      </c>
-      <c r="C41" s="2" t="s">
-        <v>275</v>
       </c>
     </row>
     <row r="42" spans="1:3" ht="58" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A42" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="B42" s="2" t="s">
         <v>276</v>
       </c>
-      <c r="B42" s="2" t="s">
+      <c r="C42" s="2" t="s">
         <v>277</v>
-      </c>
-      <c r="C42" s="2" t="s">
-        <v>278</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A43" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="B43" s="2" t="s">
         <v>279</v>
       </c>
-      <c r="B43" s="2" t="s">
+      <c r="C43" s="2" t="s">
         <v>280</v>
-      </c>
-      <c r="C43" s="2" t="s">
-        <v>281</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.35">
@@ -3784,112 +3784,112 @@
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A45" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="B45" s="2" t="s">
         <v>282</v>
       </c>
-      <c r="B45" s="2" t="s">
+      <c r="C45" s="2" t="s">
         <v>283</v>
-      </c>
-      <c r="C45" s="2" t="s">
-        <v>284</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A46" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="B46" s="2" t="s">
         <v>285</v>
       </c>
-      <c r="B46" s="2" t="s">
+      <c r="C46" s="2" t="s">
         <v>286</v>
-      </c>
-      <c r="C46" s="2" t="s">
-        <v>287</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A47" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="B47" s="2" t="s">
         <v>288</v>
       </c>
-      <c r="B47" s="2" t="s">
+      <c r="C47" s="2" t="s">
         <v>289</v>
-      </c>
-      <c r="C47" s="2" t="s">
-        <v>290</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A48" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="B48" s="2" t="s">
         <v>291</v>
       </c>
-      <c r="B48" s="2" t="s">
+      <c r="C48" s="2" t="s">
         <v>292</v>
-      </c>
-      <c r="C48" s="2" t="s">
-        <v>293</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A49" s="1" t="s">
+        <v>293</v>
+      </c>
+      <c r="B49" s="2" t="s">
         <v>294</v>
       </c>
-      <c r="B49" s="2" t="s">
+      <c r="C49" s="2" t="s">
         <v>295</v>
-      </c>
-      <c r="C49" s="2" t="s">
-        <v>296</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A50" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="B50" s="2" t="s">
         <v>297</v>
       </c>
-      <c r="B50" s="2" t="s">
+      <c r="C50" s="2" t="s">
         <v>298</v>
-      </c>
-      <c r="C50" s="2" t="s">
-        <v>299</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A51" s="1" t="s">
+        <v>299</v>
+      </c>
+      <c r="B51" s="2" t="s">
         <v>300</v>
       </c>
-      <c r="B51" s="2" t="s">
+      <c r="C51" s="2" t="s">
         <v>301</v>
-      </c>
-      <c r="C51" s="2" t="s">
-        <v>302</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A52" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="B52" s="2" t="s">
         <v>303</v>
       </c>
-      <c r="B52" s="2" t="s">
+      <c r="C52" s="2" t="s">
         <v>304</v>
-      </c>
-      <c r="C52" s="2" t="s">
-        <v>305</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A53" s="1" t="s">
+        <v>305</v>
+      </c>
+      <c r="B53" s="2" t="s">
         <v>306</v>
       </c>
-      <c r="B53" s="2" t="s">
+      <c r="C53" s="2" t="s">
         <v>307</v>
-      </c>
-      <c r="C53" s="2" t="s">
-        <v>308</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A54" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="B54" s="2" t="s">
         <v>309</v>
       </c>
-      <c r="B54" s="2" t="s">
+      <c r="C54" s="2" t="s">
         <v>310</v>
-      </c>
-      <c r="C54" s="2" t="s">
-        <v>311</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.35">
@@ -3898,585 +3898,585 @@
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A56" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="B56" s="2" t="s">
         <v>312</v>
       </c>
-      <c r="B56" s="2" t="s">
+      <c r="C56" s="2" t="s">
         <v>313</v>
-      </c>
-      <c r="C56" s="2" t="s">
-        <v>314</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A57" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="B57" s="2" t="s">
         <v>315</v>
       </c>
-      <c r="B57" s="2" t="s">
+      <c r="C57" s="2" t="s">
         <v>316</v>
-      </c>
-      <c r="C57" s="2" t="s">
-        <v>317</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A58" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="B58" s="2" t="s">
         <v>318</v>
       </c>
-      <c r="B58" s="2" t="s">
+      <c r="C58" s="2" t="s">
         <v>319</v>
-      </c>
-      <c r="C58" s="2" t="s">
-        <v>320</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A59" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="B59" s="2" t="s">
         <v>321</v>
       </c>
-      <c r="B59" s="2" t="s">
+      <c r="C59" s="2" t="s">
         <v>322</v>
-      </c>
-      <c r="C59" s="2" t="s">
-        <v>323</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A60" s="1" t="s">
+        <v>323</v>
+      </c>
+      <c r="B60" s="2" t="s">
         <v>324</v>
       </c>
-      <c r="B60" s="2" t="s">
+      <c r="C60" s="2" t="s">
         <v>325</v>
-      </c>
-      <c r="C60" s="2" t="s">
-        <v>326</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A61" s="1" t="s">
+        <v>326</v>
+      </c>
+      <c r="B61" s="2" t="s">
         <v>327</v>
       </c>
-      <c r="B61" s="2" t="s">
+      <c r="C61" s="2" t="s">
         <v>328</v>
-      </c>
-      <c r="C61" s="2" t="s">
-        <v>329</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A62" s="1" t="s">
+        <v>329</v>
+      </c>
+      <c r="B62" s="2" t="s">
         <v>330</v>
       </c>
-      <c r="B62" s="2" t="s">
+      <c r="C62" s="2" t="s">
         <v>331</v>
-      </c>
-      <c r="C62" s="2" t="s">
-        <v>332</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A63" s="1" t="s">
+        <v>332</v>
+      </c>
+      <c r="B63" s="2" t="s">
         <v>333</v>
       </c>
-      <c r="B63" s="2" t="s">
+      <c r="C63" s="2" t="s">
         <v>334</v>
-      </c>
-      <c r="C63" s="2" t="s">
-        <v>335</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A64" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="B64" s="2" t="s">
         <v>336</v>
       </c>
-      <c r="B64" s="2" t="s">
+      <c r="C64" s="2" t="s">
         <v>337</v>
-      </c>
-      <c r="C64" s="2" t="s">
-        <v>338</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A65" s="1" t="s">
+        <v>338</v>
+      </c>
+      <c r="B65" s="2" t="s">
         <v>339</v>
       </c>
-      <c r="B65" s="2" t="s">
+      <c r="C65" s="2" t="s">
         <v>340</v>
-      </c>
-      <c r="C65" s="2" t="s">
-        <v>341</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A66" s="1" t="s">
+        <v>341</v>
+      </c>
+      <c r="B66" s="2" t="s">
         <v>342</v>
       </c>
-      <c r="B66" s="2" t="s">
+      <c r="C66" s="2" t="s">
         <v>343</v>
-      </c>
-      <c r="C66" s="2" t="s">
-        <v>344</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A67" s="1" t="s">
+        <v>344</v>
+      </c>
+      <c r="B67" s="2" t="s">
         <v>345</v>
       </c>
-      <c r="B67" s="2" t="s">
+      <c r="C67" s="2" t="s">
         <v>346</v>
-      </c>
-      <c r="C67" s="2" t="s">
-        <v>347</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A68" s="1" t="s">
+        <v>347</v>
+      </c>
+      <c r="B68" s="2" t="s">
         <v>348</v>
       </c>
-      <c r="B68" s="2" t="s">
+      <c r="C68" s="2" t="s">
         <v>349</v>
-      </c>
-      <c r="C68" s="2" t="s">
-        <v>350</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A69" s="1" t="s">
+        <v>350</v>
+      </c>
+      <c r="B69" s="2" t="s">
         <v>351</v>
       </c>
-      <c r="B69" s="2" t="s">
+      <c r="C69" s="2" t="s">
         <v>352</v>
-      </c>
-      <c r="C69" s="2" t="s">
-        <v>353</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A70" s="1" t="s">
+        <v>353</v>
+      </c>
+      <c r="B70" s="2" t="s">
         <v>354</v>
       </c>
-      <c r="B70" s="2" t="s">
+      <c r="C70" s="2" t="s">
         <v>355</v>
-      </c>
-      <c r="C70" s="2" t="s">
-        <v>356</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A71" s="1" t="s">
+        <v>356</v>
+      </c>
+      <c r="B71" s="2" t="s">
         <v>357</v>
       </c>
-      <c r="B71" s="2" t="s">
+      <c r="C71" s="2" t="s">
         <v>358</v>
-      </c>
-      <c r="C71" s="2" t="s">
-        <v>359</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A72" s="1" t="s">
+        <v>359</v>
+      </c>
+      <c r="B72" s="2" t="s">
         <v>360</v>
       </c>
-      <c r="B72" s="2" t="s">
+      <c r="C72" s="2" t="s">
         <v>361</v>
-      </c>
-      <c r="C72" s="2" t="s">
-        <v>362</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A73" s="1" t="s">
+        <v>362</v>
+      </c>
+      <c r="B73" s="2" t="s">
         <v>363</v>
       </c>
-      <c r="B73" s="2" t="s">
+      <c r="C73" s="2" t="s">
         <v>364</v>
-      </c>
-      <c r="C73" s="2" t="s">
-        <v>365</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A74" s="1" t="s">
+        <v>365</v>
+      </c>
+      <c r="B74" s="2" t="s">
         <v>366</v>
       </c>
-      <c r="B74" s="2" t="s">
+      <c r="C74" s="2" t="s">
         <v>367</v>
-      </c>
-      <c r="C74" s="2" t="s">
-        <v>368</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A75" s="1" t="s">
+        <v>368</v>
+      </c>
+      <c r="B75" s="2" t="s">
         <v>369</v>
       </c>
-      <c r="B75" s="2" t="s">
+      <c r="C75" s="2" t="s">
         <v>370</v>
-      </c>
-      <c r="C75" s="2" t="s">
-        <v>371</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A76" s="1" t="s">
+        <v>371</v>
+      </c>
+      <c r="B76" s="2" t="s">
         <v>372</v>
       </c>
-      <c r="B76" s="2" t="s">
+      <c r="C76" s="2" t="s">
         <v>373</v>
-      </c>
-      <c r="C76" s="2" t="s">
-        <v>374</v>
       </c>
     </row>
     <row r="77" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A77" s="1" t="s">
+        <v>374</v>
+      </c>
+      <c r="B77" s="2" t="s">
         <v>375</v>
       </c>
-      <c r="B77" s="2" t="s">
+      <c r="C77" s="2" t="s">
         <v>376</v>
-      </c>
-      <c r="C77" s="2" t="s">
-        <v>377</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A78" s="1" t="s">
+        <v>377</v>
+      </c>
+      <c r="B78" s="2" t="s">
         <v>378</v>
       </c>
-      <c r="B78" s="2" t="s">
+      <c r="C78" s="2" t="s">
         <v>379</v>
-      </c>
-      <c r="C78" s="2" t="s">
-        <v>380</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A79" s="1" t="s">
+        <v>380</v>
+      </c>
+      <c r="B79" s="2" t="s">
         <v>381</v>
       </c>
-      <c r="B79" s="2" t="s">
+      <c r="C79" s="2" t="s">
         <v>382</v>
-      </c>
-      <c r="C79" s="2" t="s">
-        <v>383</v>
       </c>
     </row>
     <row r="80" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A80" s="1" t="s">
+        <v>383</v>
+      </c>
+      <c r="B80" s="2" t="s">
         <v>384</v>
       </c>
-      <c r="B80" s="2" t="s">
+      <c r="C80" s="2" t="s">
         <v>385</v>
-      </c>
-      <c r="C80" s="2" t="s">
-        <v>386</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A81" s="1" t="s">
+        <v>386</v>
+      </c>
+      <c r="B81" s="2" t="s">
         <v>387</v>
       </c>
-      <c r="B81" s="2" t="s">
+      <c r="C81" s="2" t="s">
         <v>388</v>
-      </c>
-      <c r="C81" s="2" t="s">
-        <v>389</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A82" s="1" t="s">
+        <v>389</v>
+      </c>
+      <c r="B82" s="2" t="s">
         <v>390</v>
       </c>
-      <c r="B82" s="2" t="s">
+      <c r="C82" s="2" t="s">
         <v>391</v>
-      </c>
-      <c r="C82" s="2" t="s">
-        <v>392</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A83" s="1" t="s">
+        <v>392</v>
+      </c>
+      <c r="B83" s="2" t="s">
         <v>393</v>
       </c>
-      <c r="B83" s="2" t="s">
+      <c r="C83" s="2" t="s">
         <v>394</v>
-      </c>
-      <c r="C83" s="2" t="s">
-        <v>395</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A84" s="1" t="s">
+        <v>395</v>
+      </c>
+      <c r="B84" s="2" t="s">
         <v>396</v>
       </c>
-      <c r="B84" s="2" t="s">
+      <c r="C84" s="2" t="s">
         <v>397</v>
-      </c>
-      <c r="C84" s="2" t="s">
-        <v>398</v>
       </c>
     </row>
     <row r="85" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A85" s="1" t="s">
+        <v>398</v>
+      </c>
+      <c r="B85" s="2" t="s">
         <v>399</v>
       </c>
-      <c r="B85" s="2" t="s">
+      <c r="C85" s="2" t="s">
         <v>400</v>
-      </c>
-      <c r="C85" s="2" t="s">
-        <v>401</v>
       </c>
     </row>
     <row r="86" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A86" s="1" t="s">
+        <v>401</v>
+      </c>
+      <c r="B86" s="2" t="s">
         <v>402</v>
       </c>
-      <c r="B86" s="2" t="s">
+      <c r="C86" s="2" t="s">
         <v>403</v>
-      </c>
-      <c r="C86" s="2" t="s">
-        <v>404</v>
       </c>
     </row>
     <row r="87" spans="1:3" ht="43.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A87" s="1" t="s">
+        <v>404</v>
+      </c>
+      <c r="B87" s="2" t="s">
         <v>405</v>
       </c>
-      <c r="B87" s="2" t="s">
+      <c r="C87" s="2" t="s">
         <v>406</v>
-      </c>
-      <c r="C87" s="2" t="s">
-        <v>407</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A88" s="1" t="s">
+        <v>407</v>
+      </c>
+      <c r="B88" s="2" t="s">
         <v>408</v>
       </c>
-      <c r="B88" s="2" t="s">
+      <c r="C88" s="2" t="s">
         <v>409</v>
-      </c>
-      <c r="C88" s="2" t="s">
-        <v>410</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A89" s="1" t="s">
+        <v>410</v>
+      </c>
+      <c r="B89" s="2" t="s">
         <v>411</v>
       </c>
-      <c r="B89" s="2" t="s">
+      <c r="C89" s="2" t="s">
         <v>412</v>
-      </c>
-      <c r="C89" s="2" t="s">
-        <v>413</v>
       </c>
     </row>
     <row r="90" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A90" s="1" t="s">
+        <v>413</v>
+      </c>
+      <c r="B90" s="2" t="s">
         <v>414</v>
       </c>
-      <c r="B90" s="2" t="s">
+      <c r="C90" s="2" t="s">
         <v>415</v>
-      </c>
-      <c r="C90" s="2" t="s">
-        <v>416</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A91" s="1" t="s">
+        <v>416</v>
+      </c>
+      <c r="B91" s="2" t="s">
         <v>417</v>
       </c>
-      <c r="B91" s="2" t="s">
+      <c r="C91" s="2" t="s">
         <v>418</v>
-      </c>
-      <c r="C91" s="2" t="s">
-        <v>419</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A92" s="1" t="s">
+        <v>419</v>
+      </c>
+      <c r="B92" s="2" t="s">
         <v>420</v>
       </c>
-      <c r="B92" s="2" t="s">
+      <c r="C92" s="2" t="s">
         <v>421</v>
-      </c>
-      <c r="C92" s="2" t="s">
-        <v>422</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A93" s="1" t="s">
+        <v>422</v>
+      </c>
+      <c r="B93" s="2" t="s">
         <v>423</v>
       </c>
-      <c r="B93" s="2" t="s">
+      <c r="C93" s="2" t="s">
         <v>424</v>
-      </c>
-      <c r="C93" s="2" t="s">
-        <v>425</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A94" s="1" t="s">
+        <v>425</v>
+      </c>
+      <c r="B94" s="2" t="s">
         <v>426</v>
       </c>
-      <c r="B94" s="2" t="s">
+      <c r="C94" s="2" t="s">
         <v>427</v>
-      </c>
-      <c r="C94" s="2" t="s">
-        <v>428</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A95" s="1" t="s">
+        <v>428</v>
+      </c>
+      <c r="B95" s="2" t="s">
         <v>429</v>
       </c>
-      <c r="B95" s="2" t="s">
+      <c r="C95" s="2" t="s">
         <v>430</v>
-      </c>
-      <c r="C95" s="2" t="s">
-        <v>431</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A96" s="1" t="s">
+        <v>431</v>
+      </c>
+      <c r="B96" s="2" t="s">
         <v>432</v>
       </c>
-      <c r="B96" s="2" t="s">
+      <c r="C96" s="2" t="s">
         <v>433</v>
-      </c>
-      <c r="C96" s="2" t="s">
-        <v>434</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A97" s="1" t="s">
+        <v>434</v>
+      </c>
+      <c r="B97" s="2" t="s">
         <v>435</v>
       </c>
-      <c r="B97" s="2" t="s">
+      <c r="C97" s="2" t="s">
         <v>436</v>
-      </c>
-      <c r="C97" s="2" t="s">
-        <v>437</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A98" s="1" t="s">
+        <v>437</v>
+      </c>
+      <c r="B98" s="2" t="s">
         <v>438</v>
       </c>
-      <c r="B98" s="2" t="s">
+      <c r="C98" s="2" t="s">
         <v>439</v>
-      </c>
-      <c r="C98" s="2" t="s">
-        <v>440</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A99" s="1" t="s">
+        <v>440</v>
+      </c>
+      <c r="B99" s="2" t="s">
         <v>441</v>
       </c>
-      <c r="B99" s="2" t="s">
+      <c r="C99" s="2" t="s">
         <v>442</v>
-      </c>
-      <c r="C99" s="2" t="s">
-        <v>443</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A100" s="1" t="s">
+        <v>443</v>
+      </c>
+      <c r="B100" s="2" t="s">
         <v>444</v>
       </c>
-      <c r="B100" s="2" t="s">
+      <c r="C100" s="2" t="s">
         <v>445</v>
-      </c>
-      <c r="C100" s="2" t="s">
-        <v>446</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A101" s="1" t="s">
+        <v>446</v>
+      </c>
+      <c r="B101" s="2" t="s">
         <v>447</v>
       </c>
-      <c r="B101" s="2" t="s">
+      <c r="C101" s="2" t="s">
         <v>448</v>
-      </c>
-      <c r="C101" s="2" t="s">
-        <v>449</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A102" s="1" t="s">
+        <v>449</v>
+      </c>
+      <c r="B102" s="2" t="s">
         <v>450</v>
       </c>
-      <c r="B102" s="2" t="s">
+      <c r="C102" s="2" t="s">
         <v>451</v>
-      </c>
-      <c r="C102" s="2" t="s">
-        <v>452</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A103" s="1" t="s">
+        <v>452</v>
+      </c>
+      <c r="B103" s="2" t="s">
         <v>453</v>
       </c>
-      <c r="B103" s="2" t="s">
+      <c r="C103" s="2" t="s">
         <v>454</v>
-      </c>
-      <c r="C103" s="2" t="s">
-        <v>455</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A104" s="1" t="s">
+        <v>455</v>
+      </c>
+      <c r="B104" s="2" t="s">
         <v>456</v>
       </c>
-      <c r="B104" s="2" t="s">
+      <c r="C104" s="2" t="s">
         <v>457</v>
-      </c>
-      <c r="C104" s="2" t="s">
-        <v>458</v>
       </c>
     </row>
     <row r="105" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A105" s="1" t="s">
+        <v>458</v>
+      </c>
+      <c r="B105" s="2" t="s">
         <v>459</v>
       </c>
-      <c r="B105" s="2" t="s">
+      <c r="C105" s="2" t="s">
         <v>460</v>
-      </c>
-      <c r="C105" s="2" t="s">
-        <v>461</v>
       </c>
     </row>
     <row r="106" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A106" s="1" t="s">
+        <v>461</v>
+      </c>
+      <c r="B106" s="2" t="s">
         <v>462</v>
       </c>
-      <c r="B106" s="2" t="s">
+      <c r="C106" s="2" t="s">
         <v>463</v>
-      </c>
-      <c r="C106" s="2" t="s">
-        <v>464</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A107" s="1" t="s">
+        <v>464</v>
+      </c>
+      <c r="B107" s="2" t="s">
         <v>465</v>
       </c>
-      <c r="B107" s="2" t="s">
+      <c r="C107" s="2" t="s">
         <v>466</v>
-      </c>
-      <c r="C107" s="2" t="s">
-        <v>467</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A108" s="1" t="s">
+        <v>467</v>
+      </c>
+      <c r="B108" s="2" t="s">
         <v>468</v>
       </c>
-      <c r="B108" s="2" t="s">
+      <c r="C108" s="2" t="s">
         <v>469</v>
-      </c>
-      <c r="C108" s="2" t="s">
-        <v>470</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.35">
@@ -4485,90 +4485,90 @@
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A110" s="1" t="s">
+        <v>470</v>
+      </c>
+      <c r="B110" s="2" t="s">
         <v>471</v>
       </c>
-      <c r="B110" s="2" t="s">
+      <c r="C110" s="2" t="s">
         <v>472</v>
-      </c>
-      <c r="C110" s="2" t="s">
-        <v>473</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A111" s="1" t="s">
+        <v>473</v>
+      </c>
+      <c r="B111" s="2" t="s">
         <v>474</v>
       </c>
-      <c r="B111" s="2" t="s">
+      <c r="C111" s="2" t="s">
         <v>475</v>
-      </c>
-      <c r="C111" s="2" t="s">
-        <v>476</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A112" s="1" t="s">
+        <v>476</v>
+      </c>
+      <c r="B112" s="2" t="s">
         <v>477</v>
       </c>
-      <c r="B112" s="2" t="s">
+      <c r="C112" s="2" t="s">
         <v>478</v>
-      </c>
-      <c r="C112" s="2" t="s">
-        <v>479</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A113" s="1" t="s">
+        <v>479</v>
+      </c>
+      <c r="B113" s="2" t="s">
         <v>480</v>
       </c>
-      <c r="B113" s="2" t="s">
+      <c r="C113" s="2" t="s">
         <v>481</v>
-      </c>
-      <c r="C113" s="2" t="s">
-        <v>482</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A114" s="1" t="s">
+        <v>482</v>
+      </c>
+      <c r="B114" s="2" t="s">
         <v>483</v>
       </c>
-      <c r="B114" s="2" t="s">
+      <c r="C114" s="2" t="s">
         <v>484</v>
-      </c>
-      <c r="C114" s="2" t="s">
-        <v>485</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A115" s="1" t="s">
+        <v>485</v>
+      </c>
+      <c r="B115" s="2" t="s">
         <v>486</v>
       </c>
-      <c r="B115" s="2" t="s">
+      <c r="C115" s="2" t="s">
         <v>487</v>
-      </c>
-      <c r="C115" s="2" t="s">
-        <v>488</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A116" s="1" t="s">
+        <v>488</v>
+      </c>
+      <c r="B116" s="2" t="s">
         <v>489</v>
       </c>
-      <c r="B116" s="2" t="s">
+      <c r="C116" s="2" t="s">
         <v>490</v>
-      </c>
-      <c r="C116" s="2" t="s">
-        <v>491</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A117" s="1" t="s">
+        <v>491</v>
+      </c>
+      <c r="B117" s="2" t="s">
         <v>492</v>
       </c>
-      <c r="B117" s="2" t="s">
+      <c r="C117" s="2" t="s">
         <v>493</v>
-      </c>
-      <c r="C117" s="2" t="s">
-        <v>494</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.35">
@@ -4577,101 +4577,101 @@
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A119" s="1" t="s">
+        <v>494</v>
+      </c>
+      <c r="B119" s="2" t="s">
         <v>495</v>
       </c>
-      <c r="B119" s="2" t="s">
+      <c r="C119" s="2" t="s">
         <v>496</v>
-      </c>
-      <c r="C119" s="2" t="s">
-        <v>497</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A120" s="1" t="s">
+        <v>497</v>
+      </c>
+      <c r="B120" s="2" t="s">
         <v>498</v>
       </c>
-      <c r="B120" s="2" t="s">
+      <c r="C120" s="2" t="s">
         <v>499</v>
-      </c>
-      <c r="C120" s="2" t="s">
-        <v>500</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A121" s="1" t="s">
+        <v>500</v>
+      </c>
+      <c r="B121" s="2" t="s">
         <v>501</v>
       </c>
-      <c r="B121" s="2" t="s">
+      <c r="C121" s="2" t="s">
         <v>502</v>
-      </c>
-      <c r="C121" s="2" t="s">
-        <v>503</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A122" s="1" t="s">
+        <v>503</v>
+      </c>
+      <c r="B122" s="2" t="s">
         <v>504</v>
       </c>
-      <c r="B122" s="2" t="s">
+      <c r="C122" s="2" t="s">
         <v>505</v>
-      </c>
-      <c r="C122" s="2" t="s">
-        <v>506</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A123" s="1" t="s">
+        <v>506</v>
+      </c>
+      <c r="B123" s="2" t="s">
         <v>507</v>
       </c>
-      <c r="B123" s="2" t="s">
+      <c r="C123" s="2" t="s">
         <v>508</v>
-      </c>
-      <c r="C123" s="2" t="s">
-        <v>509</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A124" s="1" t="s">
+        <v>509</v>
+      </c>
+      <c r="B124" s="2" t="s">
         <v>510</v>
       </c>
-      <c r="B124" s="2" t="s">
+      <c r="C124" s="2" t="s">
         <v>511</v>
-      </c>
-      <c r="C124" s="2" t="s">
-        <v>512</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A125" s="1" t="s">
+        <v>512</v>
+      </c>
+      <c r="B125" s="2" t="s">
         <v>513</v>
       </c>
-      <c r="B125" s="2" t="s">
+      <c r="C125" s="2" t="s">
         <v>514</v>
-      </c>
-      <c r="C125" s="2" t="s">
-        <v>515</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A126" s="1" t="s">
+        <v>515</v>
+      </c>
+      <c r="B126" s="2" t="s">
         <v>516</v>
       </c>
-      <c r="B126" s="2" t="s">
+      <c r="C126" s="2" t="s">
         <v>517</v>
-      </c>
-      <c r="C126" s="2" t="s">
-        <v>518</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A127" s="1" t="s">
+        <v>518</v>
+      </c>
+      <c r="B127" s="2" t="s">
         <v>519</v>
       </c>
-      <c r="B127" s="2" t="s">
+      <c r="C127" s="2" t="s">
         <v>520</v>
-      </c>
-      <c r="C127" s="2" t="s">
-        <v>521</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.35">
@@ -4680,90 +4680,90 @@
     </row>
     <row r="129" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A129" s="1" t="s">
+        <v>521</v>
+      </c>
+      <c r="B129" s="2" t="s">
         <v>522</v>
       </c>
-      <c r="B129" s="2" t="s">
+      <c r="C129" s="2" t="s">
         <v>523</v>
-      </c>
-      <c r="C129" s="2" t="s">
-        <v>524</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A130" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="B130" s="2" t="s">
         <v>525</v>
       </c>
-      <c r="B130" s="2" t="s">
+      <c r="C130" s="2" t="s">
         <v>526</v>
-      </c>
-      <c r="C130" s="2" t="s">
-        <v>527</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A131" s="1" t="s">
+        <v>527</v>
+      </c>
+      <c r="B131" s="2" t="s">
         <v>528</v>
       </c>
-      <c r="B131" s="2" t="s">
+      <c r="C131" s="2" t="s">
         <v>529</v>
-      </c>
-      <c r="C131" s="2" t="s">
-        <v>530</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A132" s="1" t="s">
+        <v>530</v>
+      </c>
+      <c r="B132" s="2" t="s">
         <v>531</v>
       </c>
-      <c r="B132" s="2" t="s">
+      <c r="C132" s="2" t="s">
         <v>532</v>
-      </c>
-      <c r="C132" s="2" t="s">
-        <v>533</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A133" s="1" t="s">
+        <v>533</v>
+      </c>
+      <c r="B133" s="2" t="s">
         <v>534</v>
       </c>
-      <c r="B133" s="2" t="s">
+      <c r="C133" s="2" t="s">
         <v>535</v>
-      </c>
-      <c r="C133" s="2" t="s">
-        <v>536</v>
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A134" s="1" t="s">
+        <v>536</v>
+      </c>
+      <c r="B134" s="2" t="s">
         <v>537</v>
       </c>
-      <c r="B134" s="2" t="s">
+      <c r="C134" s="2" t="s">
         <v>538</v>
-      </c>
-      <c r="C134" s="2" t="s">
-        <v>539</v>
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A135" s="1" t="s">
+        <v>539</v>
+      </c>
+      <c r="B135" s="2" t="s">
         <v>540</v>
       </c>
-      <c r="B135" s="2" t="s">
+      <c r="C135" s="2" t="s">
         <v>541</v>
-      </c>
-      <c r="C135" s="2" t="s">
-        <v>542</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A136" s="1" t="s">
+        <v>542</v>
+      </c>
+      <c r="B136" s="2" t="s">
         <v>543</v>
       </c>
-      <c r="B136" s="2" t="s">
+      <c r="C136" s="2" t="s">
         <v>544</v>
-      </c>
-      <c r="C136" s="2" t="s">
-        <v>545</v>
       </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.35">
@@ -4772,266 +4772,266 @@
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A138" s="1" t="s">
+        <v>545</v>
+      </c>
+      <c r="B138" s="2" t="s">
         <v>546</v>
       </c>
-      <c r="B138" s="2" t="s">
+      <c r="C138" s="2" t="s">
         <v>547</v>
-      </c>
-      <c r="C138" s="2" t="s">
-        <v>548</v>
       </c>
     </row>
     <row r="139" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A139" s="1" t="s">
+        <v>548</v>
+      </c>
+      <c r="B139" s="2" t="s">
         <v>549</v>
       </c>
-      <c r="B139" s="2" t="s">
+      <c r="C139" s="2" t="s">
         <v>550</v>
-      </c>
-      <c r="C139" s="2" t="s">
-        <v>551</v>
       </c>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A140" s="1" t="s">
+        <v>551</v>
+      </c>
+      <c r="B140" s="2" t="s">
         <v>552</v>
       </c>
-      <c r="B140" s="2" t="s">
+      <c r="C140" s="2" t="s">
         <v>553</v>
-      </c>
-      <c r="C140" s="2" t="s">
-        <v>554</v>
       </c>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A141" s="1" t="s">
+        <v>554</v>
+      </c>
+      <c r="B141" s="2" t="s">
         <v>555</v>
       </c>
-      <c r="B141" s="2" t="s">
+      <c r="C141" s="2" t="s">
         <v>556</v>
-      </c>
-      <c r="C141" s="2" t="s">
-        <v>557</v>
       </c>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A143" s="1" t="s">
+        <v>557</v>
+      </c>
+      <c r="B143" s="2" t="s">
         <v>558</v>
       </c>
-      <c r="B143" s="2" t="s">
+      <c r="C143" s="2" t="s">
         <v>559</v>
-      </c>
-      <c r="C143" s="2" t="s">
-        <v>560</v>
       </c>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A144" s="1" t="s">
+        <v>560</v>
+      </c>
+      <c r="B144" s="2" t="s">
         <v>561</v>
       </c>
-      <c r="B144" s="2" t="s">
+      <c r="C144" s="2" t="s">
         <v>562</v>
-      </c>
-      <c r="C144" s="2" t="s">
-        <v>563</v>
       </c>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A145" s="1" t="s">
+        <v>563</v>
+      </c>
+      <c r="B145" s="2" t="s">
         <v>564</v>
       </c>
-      <c r="B145" s="2" t="s">
+      <c r="C145" s="2" t="s">
         <v>565</v>
-      </c>
-      <c r="C145" s="2" t="s">
-        <v>566</v>
       </c>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A146" s="1" t="s">
+        <v>566</v>
+      </c>
+      <c r="B146" s="2" t="s">
         <v>567</v>
       </c>
-      <c r="B146" s="2" t="s">
+      <c r="C146" s="2" t="s">
         <v>568</v>
-      </c>
-      <c r="C146" s="2" t="s">
-        <v>569</v>
       </c>
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A147" s="1" t="s">
+        <v>569</v>
+      </c>
+      <c r="B147" s="2" t="s">
         <v>570</v>
       </c>
-      <c r="B147" s="2" t="s">
+      <c r="C147" s="2" t="s">
         <v>571</v>
-      </c>
-      <c r="C147" s="2" t="s">
-        <v>572</v>
       </c>
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A148" s="1" t="s">
+        <v>572</v>
+      </c>
+      <c r="B148" s="2" t="s">
         <v>573</v>
       </c>
-      <c r="B148" s="2" t="s">
+      <c r="C148" s="2" t="s">
         <v>574</v>
-      </c>
-      <c r="C148" s="2" t="s">
-        <v>575</v>
       </c>
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A149" s="1" t="s">
+        <v>575</v>
+      </c>
+      <c r="B149" s="2" t="s">
         <v>576</v>
       </c>
-      <c r="B149" s="2" t="s">
+      <c r="C149" s="2" t="s">
         <v>577</v>
-      </c>
-      <c r="C149" s="2" t="s">
-        <v>578</v>
       </c>
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A151" s="1" t="s">
+        <v>578</v>
+      </c>
+      <c r="B151" s="2" t="s">
         <v>579</v>
       </c>
-      <c r="B151" s="2" t="s">
+      <c r="C151" s="2" t="s">
         <v>580</v>
-      </c>
-      <c r="C151" s="2" t="s">
-        <v>581</v>
       </c>
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A152" s="1" t="s">
+        <v>581</v>
+      </c>
+      <c r="B152" s="2" t="s">
         <v>582</v>
       </c>
-      <c r="B152" s="2" t="s">
+      <c r="C152" s="2" t="s">
         <v>583</v>
-      </c>
-      <c r="C152" s="2" t="s">
-        <v>584</v>
       </c>
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A153" s="1" t="s">
+        <v>584</v>
+      </c>
+      <c r="B153" s="2" t="s">
         <v>585</v>
       </c>
-      <c r="B153" s="2" t="s">
+      <c r="C153" s="2" t="s">
         <v>586</v>
-      </c>
-      <c r="C153" s="2" t="s">
-        <v>587</v>
       </c>
     </row>
     <row r="154" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A154" s="1" t="s">
+        <v>587</v>
+      </c>
+      <c r="B154" s="2" t="s">
         <v>588</v>
       </c>
-      <c r="B154" s="2" t="s">
+      <c r="C154" s="2" t="s">
         <v>589</v>
-      </c>
-      <c r="C154" s="2" t="s">
-        <v>590</v>
       </c>
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A155" s="1" t="s">
+        <v>590</v>
+      </c>
+      <c r="B155" s="2" t="s">
         <v>591</v>
       </c>
-      <c r="B155" s="2" t="s">
+      <c r="C155" s="2" t="s">
         <v>592</v>
-      </c>
-      <c r="C155" s="2" t="s">
-        <v>593</v>
       </c>
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A157" s="1" t="s">
+        <v>593</v>
+      </c>
+      <c r="B157" s="2" t="s">
         <v>594</v>
       </c>
-      <c r="B157" s="2" t="s">
+      <c r="C157" s="2" t="s">
         <v>595</v>
-      </c>
-      <c r="C157" s="2" t="s">
-        <v>596</v>
       </c>
     </row>
     <row r="158" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A158" s="1" t="s">
+        <v>596</v>
+      </c>
+      <c r="B158" s="2" t="s">
         <v>597</v>
       </c>
-      <c r="B158" s="2" t="s">
+      <c r="C158" s="2" t="s">
         <v>598</v>
-      </c>
-      <c r="C158" s="2" t="s">
-        <v>599</v>
       </c>
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A159" s="1" t="s">
+        <v>599</v>
+      </c>
+      <c r="B159" s="1" t="s">
         <v>600</v>
       </c>
-      <c r="B159" s="1" t="s">
+      <c r="C159" s="1" t="s">
         <v>601</v>
-      </c>
-      <c r="C159" s="1" t="s">
-        <v>602</v>
       </c>
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A160" s="1" t="s">
+        <v>602</v>
+      </c>
+      <c r="B160" s="2" t="s">
         <v>603</v>
       </c>
-      <c r="B160" s="2" t="s">
+      <c r="C160" s="1" t="s">
         <v>604</v>
-      </c>
-      <c r="C160" s="1" t="s">
-        <v>605</v>
       </c>
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A161" s="1" t="s">
+        <v>605</v>
+      </c>
+      <c r="B161" s="1" t="s">
         <v>606</v>
       </c>
-      <c r="B161" s="1" t="s">
+      <c r="C161" s="1" t="s">
         <v>607</v>
-      </c>
-      <c r="C161" s="1" t="s">
-        <v>608</v>
       </c>
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A162" s="1" t="s">
+        <v>608</v>
+      </c>
+      <c r="B162" s="2" t="s">
         <v>609</v>
       </c>
-      <c r="B162" s="2" t="s">
+      <c r="C162" s="2" t="s">
         <v>610</v>
-      </c>
-      <c r="C162" s="2" t="s">
-        <v>611</v>
       </c>
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A164" s="1" t="s">
+        <v>611</v>
+      </c>
+      <c r="B164" s="2" t="s">
         <v>612</v>
       </c>
-      <c r="B164" s="2" t="s">
+      <c r="C164" s="2" t="s">
         <v>613</v>
-      </c>
-      <c r="C164" s="2" t="s">
-        <v>614</v>
       </c>
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A165" s="1" t="s">
+        <v>614</v>
+      </c>
+      <c r="B165" s="2" t="s">
         <v>615</v>
       </c>
-      <c r="B165" s="2" t="s">
+      <c r="C165" s="2" t="s">
         <v>616</v>
-      </c>
-      <c r="C165" s="2" t="s">
-        <v>617</v>
       </c>
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.35">
@@ -5040,57 +5040,57 @@
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A167" s="1" t="s">
+        <v>617</v>
+      </c>
+      <c r="B167" s="2" t="s">
         <v>618</v>
       </c>
-      <c r="B167" s="2" t="s">
+      <c r="C167" s="2" t="s">
         <v>619</v>
-      </c>
-      <c r="C167" s="2" t="s">
-        <v>620</v>
       </c>
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A168" s="1" t="s">
+        <v>620</v>
+      </c>
+      <c r="B168" s="2" t="s">
         <v>621</v>
       </c>
-      <c r="B168" s="2" t="s">
+      <c r="C168" s="2" t="s">
         <v>622</v>
-      </c>
-      <c r="C168" s="2" t="s">
-        <v>623</v>
       </c>
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A169" s="1" t="s">
+        <v>623</v>
+      </c>
+      <c r="B169" s="2" t="s">
         <v>624</v>
       </c>
-      <c r="B169" s="2" t="s">
+      <c r="C169" s="2" t="s">
         <v>625</v>
-      </c>
-      <c r="C169" s="2" t="s">
-        <v>626</v>
       </c>
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A170" s="1" t="s">
+        <v>626</v>
+      </c>
+      <c r="B170" s="2" t="s">
         <v>627</v>
       </c>
-      <c r="B170" s="2" t="s">
+      <c r="C170" s="2" t="s">
         <v>628</v>
-      </c>
-      <c r="C170" s="2" t="s">
-        <v>629</v>
       </c>
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A171" s="1" t="s">
+        <v>629</v>
+      </c>
+      <c r="B171" s="2" t="s">
         <v>630</v>
       </c>
-      <c r="B171" s="2" t="s">
+      <c r="C171" s="2" t="s">
         <v>631</v>
-      </c>
-      <c r="C171" s="2" t="s">
-        <v>632</v>
       </c>
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.35">
@@ -5099,156 +5099,156 @@
     </row>
     <row r="173" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A173" s="1" t="s">
+        <v>632</v>
+      </c>
+      <c r="B173" s="2" t="s">
         <v>633</v>
       </c>
-      <c r="B173" s="2" t="s">
+      <c r="C173" s="2" t="s">
         <v>634</v>
-      </c>
-      <c r="C173" s="2" t="s">
-        <v>635</v>
       </c>
     </row>
     <row r="174" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A174" s="1" t="s">
+        <v>635</v>
+      </c>
+      <c r="B174" s="2" t="s">
         <v>636</v>
       </c>
-      <c r="B174" s="2" t="s">
+      <c r="C174" s="2" t="s">
         <v>637</v>
-      </c>
-      <c r="C174" s="2" t="s">
-        <v>638</v>
       </c>
     </row>
     <row r="175" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A175" s="1" t="s">
+        <v>638</v>
+      </c>
+      <c r="B175" s="2" t="s">
         <v>639</v>
       </c>
-      <c r="B175" s="2" t="s">
+      <c r="C175" s="2" t="s">
         <v>640</v>
-      </c>
-      <c r="C175" s="2" t="s">
-        <v>641</v>
       </c>
     </row>
     <row r="176" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A176" s="1" t="s">
+        <v>641</v>
+      </c>
+      <c r="B176" s="2" t="s">
         <v>642</v>
       </c>
-      <c r="B176" s="2" t="s">
+      <c r="C176" s="2" t="s">
         <v>643</v>
-      </c>
-      <c r="C176" s="2" t="s">
-        <v>644</v>
       </c>
     </row>
     <row r="177" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A177" s="1" t="s">
+        <v>644</v>
+      </c>
+      <c r="B177" s="2" t="s">
         <v>645</v>
       </c>
-      <c r="B177" s="2" t="s">
+      <c r="C177" s="2" t="s">
         <v>646</v>
-      </c>
-      <c r="C177" s="2" t="s">
-        <v>647</v>
       </c>
     </row>
     <row r="178" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A178" s="1" t="s">
+        <v>647</v>
+      </c>
+      <c r="B178" s="2" t="s">
         <v>648</v>
       </c>
-      <c r="B178" s="2" t="s">
+      <c r="C178" s="2" t="s">
         <v>649</v>
-      </c>
-      <c r="C178" s="2" t="s">
-        <v>650</v>
       </c>
     </row>
     <row r="179" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A179" s="1" t="s">
+        <v>650</v>
+      </c>
+      <c r="B179" s="2" t="s">
         <v>651</v>
       </c>
-      <c r="B179" s="2" t="s">
+      <c r="C179" s="2" t="s">
         <v>652</v>
-      </c>
-      <c r="C179" s="2" t="s">
-        <v>653</v>
       </c>
     </row>
     <row r="181" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A181" s="1" t="s">
+        <v>653</v>
+      </c>
+      <c r="B181" s="1" t="s">
         <v>654</v>
       </c>
-      <c r="B181" s="1" t="s">
+      <c r="C181" s="1" t="s">
         <v>655</v>
-      </c>
-      <c r="C181" s="1" t="s">
-        <v>656</v>
       </c>
     </row>
     <row r="182" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A182" s="1" t="s">
+        <v>656</v>
+      </c>
+      <c r="B182" s="1" t="s">
         <v>657</v>
       </c>
-      <c r="B182" s="1" t="s">
+      <c r="C182" s="1" t="s">
         <v>658</v>
-      </c>
-      <c r="C182" s="1" t="s">
-        <v>659</v>
       </c>
     </row>
     <row r="183" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A183" s="1" t="s">
+        <v>659</v>
+      </c>
+      <c r="B183" s="1" t="s">
         <v>660</v>
       </c>
-      <c r="B183" s="1" t="s">
+      <c r="C183" s="1" t="s">
         <v>661</v>
-      </c>
-      <c r="C183" s="1" t="s">
-        <v>662</v>
       </c>
     </row>
     <row r="184" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A184" s="1" t="s">
+        <v>662</v>
+      </c>
+      <c r="B184" s="1" t="s">
         <v>663</v>
       </c>
-      <c r="B184" s="1" t="s">
+      <c r="C184" s="1" t="s">
         <v>664</v>
-      </c>
-      <c r="C184" s="1" t="s">
-        <v>665</v>
       </c>
     </row>
     <row r="185" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A185" s="1" t="s">
+        <v>665</v>
+      </c>
+      <c r="B185" s="2" t="s">
         <v>666</v>
       </c>
-      <c r="B185" s="2" t="s">
+      <c r="C185" s="2" t="s">
         <v>667</v>
-      </c>
-      <c r="C185" s="2" t="s">
-        <v>668</v>
       </c>
     </row>
     <row r="186" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A186" s="1" t="s">
+        <v>668</v>
+      </c>
+      <c r="B186" s="1" t="s">
         <v>669</v>
       </c>
-      <c r="B186" s="1" t="s">
+      <c r="C186" s="1" t="s">
         <v>670</v>
-      </c>
-      <c r="C186" s="1" t="s">
-        <v>671</v>
       </c>
     </row>
     <row r="187" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A187" s="1" t="s">
+        <v>671</v>
+      </c>
+      <c r="B187" s="1" t="s">
         <v>672</v>
       </c>
-      <c r="B187" s="1" t="s">
+      <c r="C187" s="1" t="s">
         <v>673</v>
-      </c>
-      <c r="C187" s="1" t="s">
-        <v>674</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Cache and reuse data about Users
</commit_message>
<xml_diff>
--- a/Config.xlsx
+++ b/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mateus.cruz\Documents\GitHub\OrchestratorManager\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77FCC7CF-8054-40EE-A670-1EB0403B2115}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44419FD5-3F0B-4E92-BF57-C67BF2F53A38}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="724" uniqueCount="676">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="727" uniqueCount="679">
   <si>
     <t>Name</t>
   </si>
@@ -1636,6 +1636,15 @@
   </si>
   <si>
     <t>ユーザー名 {0} が見つかりません。</t>
+  </si>
+  <si>
+    <t>UsernameAlreadyUsed</t>
+  </si>
+  <si>
+    <t>The Username {0} is already used.</t>
+  </si>
+  <si>
+    <t>ユーザー {0} は既に使用されています。</t>
   </si>
   <si>
     <t>ProcessedRobot</t>
@@ -2199,8 +2208,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table13" displayName="Table13" ref="A1:C187" totalsRowShown="0">
-  <autoFilter ref="A1:C187" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table13" displayName="Table13" ref="A1:C188" totalsRowShown="0">
+  <autoFilter ref="A1:C188" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Name"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="EN"/>
@@ -2521,7 +2530,7 @@
         <v>7</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>674</v>
+        <v>677</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>8</v>
@@ -2543,7 +2552,7 @@
         <v>12</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>675</v>
+        <v>678</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>13</v>
@@ -2574,7 +2583,7 @@
   <dimension ref="A1:C63"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2 A2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3292,10 +3301,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1927ABA9-1814-4487-9CEC-ABDCAF91481F}">
-  <dimension ref="A1:C187"/>
+  <dimension ref="A1:C188"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2 A2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4675,21 +4684,22 @@
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B128" s="2"/>
-      <c r="C128" s="2"/>
+      <c r="A128" s="1" t="s">
+        <v>521</v>
+      </c>
+      <c r="B128" s="2" t="s">
+        <v>522</v>
+      </c>
+      <c r="C128" s="2" t="s">
+        <v>523</v>
+      </c>
     </row>
     <row r="129" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A129" s="1" t="s">
-        <v>521</v>
-      </c>
-      <c r="B129" s="2" t="s">
-        <v>522</v>
-      </c>
-      <c r="C129" s="2" t="s">
-        <v>523</v>
-      </c>
-    </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A129"/>
+      <c r="B129" s="2"/>
+      <c r="C129" s="2"/>
+    </row>
+    <row r="130" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A130" s="1" t="s">
         <v>524</v>
       </c>
@@ -4767,19 +4777,19 @@
       </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B137" s="2"/>
-      <c r="C137" s="2"/>
+      <c r="A137" s="1" t="s">
+        <v>545</v>
+      </c>
+      <c r="B137" s="2" t="s">
+        <v>546</v>
+      </c>
+      <c r="C137" s="2" t="s">
+        <v>547</v>
+      </c>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A138" s="1" t="s">
-        <v>545</v>
-      </c>
-      <c r="B138" s="2" t="s">
-        <v>546</v>
-      </c>
-      <c r="C138" s="2" t="s">
-        <v>547</v>
-      </c>
+      <c r="B138" s="2"/>
+      <c r="C138" s="2"/>
     </row>
     <row r="139" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A139" s="1" t="s">
@@ -4792,7 +4802,7 @@
         <v>550</v>
       </c>
     </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A140" s="1" t="s">
         <v>551</v>
       </c>
@@ -4814,14 +4824,14 @@
         <v>556</v>
       </c>
     </row>
-    <row r="143" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A143" s="1" t="s">
+    <row r="142" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A142" s="1" t="s">
         <v>557</v>
       </c>
-      <c r="B143" s="2" t="s">
+      <c r="B142" s="2" t="s">
         <v>558</v>
       </c>
-      <c r="C143" s="2" t="s">
+      <c r="C142" s="2" t="s">
         <v>559</v>
       </c>
     </row>
@@ -4891,14 +4901,14 @@
         <v>577</v>
       </c>
     </row>
-    <row r="151" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A151" s="1" t="s">
+    <row r="150" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A150" s="1" t="s">
         <v>578</v>
       </c>
-      <c r="B151" s="2" t="s">
+      <c r="B150" s="2" t="s">
         <v>579</v>
       </c>
-      <c r="C151" s="2" t="s">
+      <c r="C150" s="2" t="s">
         <v>580</v>
       </c>
     </row>
@@ -4935,7 +4945,7 @@
         <v>589</v>
       </c>
     </row>
-    <row r="155" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A155" s="1" t="s">
         <v>590</v>
       </c>
@@ -4946,14 +4956,14 @@
         <v>592</v>
       </c>
     </row>
-    <row r="157" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A157" s="1" t="s">
+    <row r="156" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A156" s="1" t="s">
         <v>593</v>
       </c>
-      <c r="B157" s="2" t="s">
+      <c r="B156" s="2" t="s">
         <v>594</v>
       </c>
-      <c r="C157" s="2" t="s">
+      <c r="C156" s="2" t="s">
         <v>595</v>
       </c>
     </row>
@@ -4968,14 +4978,14 @@
         <v>598</v>
       </c>
     </row>
-    <row r="159" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A159" s="1" t="s">
         <v>599</v>
       </c>
-      <c r="B159" s="1" t="s">
+      <c r="B159" s="2" t="s">
         <v>600</v>
       </c>
-      <c r="C159" s="1" t="s">
+      <c r="C159" s="2" t="s">
         <v>601</v>
       </c>
     </row>
@@ -4983,7 +4993,7 @@
       <c r="A160" s="1" t="s">
         <v>602</v>
       </c>
-      <c r="B160" s="2" t="s">
+      <c r="B160" s="1" t="s">
         <v>603</v>
       </c>
       <c r="C160" s="1" t="s">
@@ -4994,7 +5004,7 @@
       <c r="A161" s="1" t="s">
         <v>605</v>
       </c>
-      <c r="B161" s="1" t="s">
+      <c r="B161" s="2" t="s">
         <v>606</v>
       </c>
       <c r="C161" s="1" t="s">
@@ -5005,21 +5015,21 @@
       <c r="A162" s="1" t="s">
         <v>608</v>
       </c>
-      <c r="B162" s="2" t="s">
+      <c r="B162" s="1" t="s">
         <v>609</v>
       </c>
-      <c r="C162" s="2" t="s">
+      <c r="C162" s="1" t="s">
         <v>610</v>
       </c>
     </row>
-    <row r="164" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A164" s="1" t="s">
+    <row r="163" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A163" s="1" t="s">
         <v>611</v>
       </c>
-      <c r="B164" s="2" t="s">
+      <c r="B163" s="2" t="s">
         <v>612</v>
       </c>
-      <c r="C164" s="2" t="s">
+      <c r="C163" s="2" t="s">
         <v>613</v>
       </c>
     </row>
@@ -5035,19 +5045,19 @@
       </c>
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B166" s="2"/>
-      <c r="C166" s="2"/>
+      <c r="A166" s="1" t="s">
+        <v>617</v>
+      </c>
+      <c r="B166" s="2" t="s">
+        <v>618</v>
+      </c>
+      <c r="C166" s="2" t="s">
+        <v>619</v>
+      </c>
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A167" s="1" t="s">
-        <v>617</v>
-      </c>
-      <c r="B167" s="2" t="s">
-        <v>618</v>
-      </c>
-      <c r="C167" s="2" t="s">
-        <v>619</v>
-      </c>
+      <c r="B167" s="2"/>
+      <c r="C167" s="2"/>
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A168" s="1" t="s">
@@ -5094,19 +5104,19 @@
       </c>
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B172" s="2"/>
-      <c r="C172" s="2"/>
+      <c r="A172" s="1" t="s">
+        <v>632</v>
+      </c>
+      <c r="B172" s="2" t="s">
+        <v>633</v>
+      </c>
+      <c r="C172" s="2" t="s">
+        <v>634</v>
+      </c>
     </row>
     <row r="173" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A173" s="1" t="s">
-        <v>632</v>
-      </c>
-      <c r="B173" s="2" t="s">
-        <v>633</v>
-      </c>
-      <c r="C173" s="2" t="s">
-        <v>634</v>
-      </c>
+      <c r="B173" s="2"/>
+      <c r="C173" s="2"/>
     </row>
     <row r="174" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A174" s="1" t="s">
@@ -5174,14 +5184,14 @@
         <v>652</v>
       </c>
     </row>
-    <row r="181" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A181" s="1" t="s">
+    <row r="180" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A180" s="1" t="s">
         <v>653</v>
       </c>
-      <c r="B181" s="1" t="s">
+      <c r="B180" s="2" t="s">
         <v>654</v>
       </c>
-      <c r="C181" s="1" t="s">
+      <c r="C180" s="2" t="s">
         <v>655</v>
       </c>
     </row>
@@ -5222,10 +5232,10 @@
       <c r="A185" s="1" t="s">
         <v>665</v>
       </c>
-      <c r="B185" s="2" t="s">
+      <c r="B185" s="1" t="s">
         <v>666</v>
       </c>
-      <c r="C185" s="2" t="s">
+      <c r="C185" s="1" t="s">
         <v>667</v>
       </c>
     </row>
@@ -5233,10 +5243,10 @@
       <c r="A186" s="1" t="s">
         <v>668</v>
       </c>
-      <c r="B186" s="1" t="s">
+      <c r="B186" s="2" t="s">
         <v>669</v>
       </c>
-      <c r="C186" s="1" t="s">
+      <c r="C186" s="2" t="s">
         <v>670</v>
       </c>
     </row>
@@ -5249,6 +5259,17 @@
       </c>
       <c r="C187" s="1" t="s">
         <v>673</v>
+      </c>
+    </row>
+    <row r="188" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A188" s="1" t="s">
+        <v>674</v>
+      </c>
+      <c r="B188" s="1" t="s">
+        <v>675</v>
+      </c>
+      <c r="C188" s="1" t="s">
+        <v>676</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Cache and reuse data about Environments
</commit_message>
<xml_diff>
--- a/Config.xlsx
+++ b/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mateus.cruz\Documents\GitHub\OrchestratorManager\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44419FD5-3F0B-4E92-BF57-C67BF2F53A38}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C42D761C-7997-4400-BD66-3EB18215FEB4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="727" uniqueCount="679">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="736" uniqueCount="688">
   <si>
     <t>Name</t>
   </si>
@@ -1436,6 +1436,15 @@
     <t>フォルダー (組織単位) が見つかりません。</t>
   </si>
   <si>
+    <t>NamedOUFolderNotFound</t>
+  </si>
+  <si>
+    <t>Folder (Organization Unit) named {0} not found.</t>
+  </si>
+  <si>
+    <t>フォルダー (組織単位)  {0} が見つかりません。</t>
+  </si>
+  <si>
     <t>OUFolderIDInvalidOrNotSpecified</t>
   </si>
   <si>
@@ -1921,6 +1930,24 @@
   </si>
   <si>
     <t>ロボットが同時に追加および削除されています。</t>
+  </si>
+  <si>
+    <t>EnvironmentNameAlreadyUsed</t>
+  </si>
+  <si>
+    <t>The Environment name {0} is already used.</t>
+  </si>
+  <si>
+    <t>ロボット グループ名 {0} は既に使用されています。</t>
+  </si>
+  <si>
+    <t>NamedEnvironmentNotFound</t>
+  </si>
+  <si>
+    <t>Environment named {0} not found.</t>
+  </si>
+  <si>
+    <t>ロボット グループ {0} が見つかりません。</t>
   </si>
   <si>
     <t>RoleNotFound</t>
@@ -2208,8 +2235,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table13" displayName="Table13" ref="A1:C188" totalsRowShown="0">
-  <autoFilter ref="A1:C188" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table13" displayName="Table13" ref="A1:C191" totalsRowShown="0">
+  <autoFilter ref="A1:C191" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Name"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="EN"/>
@@ -2530,7 +2557,7 @@
         <v>7</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>677</v>
+        <v>686</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>8</v>
@@ -2552,7 +2579,7 @@
         <v>12</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>678</v>
+        <v>687</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>13</v>
@@ -3301,7 +3328,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1927ABA9-1814-4487-9CEC-ABDCAF91481F}">
-  <dimension ref="A1:C188"/>
+  <dimension ref="A1:C191"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -4466,7 +4493,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A107" s="1" t="s">
         <v>464</v>
       </c>
@@ -4489,19 +4516,19 @@
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B109" s="2"/>
-      <c r="C109" s="2"/>
+      <c r="A109" s="1" t="s">
+        <v>470</v>
+      </c>
+      <c r="B109" s="2" t="s">
+        <v>471</v>
+      </c>
+      <c r="C109" s="2" t="s">
+        <v>472</v>
+      </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A110" s="1" t="s">
-        <v>470</v>
-      </c>
-      <c r="B110" s="2" t="s">
-        <v>471</v>
-      </c>
-      <c r="C110" s="2" t="s">
-        <v>472</v>
-      </c>
+      <c r="B110" s="2"/>
+      <c r="C110" s="2"/>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A111" s="1" t="s">
@@ -4581,19 +4608,19 @@
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B118" s="2"/>
-      <c r="C118" s="2"/>
+      <c r="A118" s="1" t="s">
+        <v>494</v>
+      </c>
+      <c r="B118" s="2" t="s">
+        <v>495</v>
+      </c>
+      <c r="C118" s="2" t="s">
+        <v>496</v>
+      </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A119" s="1" t="s">
-        <v>494</v>
-      </c>
-      <c r="B119" s="2" t="s">
-        <v>495</v>
-      </c>
-      <c r="C119" s="2" t="s">
-        <v>496</v>
-      </c>
+      <c r="B119" s="2"/>
+      <c r="C119" s="2"/>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A120" s="1" t="s">
@@ -4695,22 +4722,21 @@
       </c>
     </row>
     <row r="129" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A129"/>
-      <c r="B129" s="2"/>
-      <c r="C129" s="2"/>
+      <c r="A129" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="B129" s="2" t="s">
+        <v>525</v>
+      </c>
+      <c r="C129" s="2" t="s">
+        <v>526</v>
+      </c>
     </row>
     <row r="130" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A130" s="1" t="s">
-        <v>524</v>
-      </c>
-      <c r="B130" s="2" t="s">
-        <v>525</v>
-      </c>
-      <c r="C130" s="2" t="s">
-        <v>526</v>
-      </c>
-    </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B130" s="2"/>
+      <c r="C130" s="2"/>
+    </row>
+    <row r="131" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A131" s="1" t="s">
         <v>527</v>
       </c>
@@ -4788,19 +4814,20 @@
       </c>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B138" s="2"/>
-      <c r="C138" s="2"/>
+      <c r="A138" s="1" t="s">
+        <v>548</v>
+      </c>
+      <c r="B138" s="2" t="s">
+        <v>549</v>
+      </c>
+      <c r="C138" s="2" t="s">
+        <v>550</v>
+      </c>
     </row>
     <row r="139" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A139" s="1" t="s">
-        <v>548</v>
-      </c>
-      <c r="B139" s="2" t="s">
-        <v>549</v>
-      </c>
-      <c r="C139" s="2" t="s">
-        <v>550</v>
-      </c>
+      <c r="A139"/>
+      <c r="B139" s="2"/>
+      <c r="C139" s="2"/>
     </row>
     <row r="140" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A140" s="1" t="s">
@@ -4813,7 +4840,7 @@
         <v>553</v>
       </c>
     </row>
-    <row r="141" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A141" s="1" t="s">
         <v>554</v>
       </c>
@@ -4835,14 +4862,14 @@
         <v>559</v>
       </c>
     </row>
-    <row r="144" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A144" s="1" t="s">
+    <row r="143" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A143" s="1" t="s">
         <v>560</v>
       </c>
-      <c r="B144" s="2" t="s">
+      <c r="B143" s="2" t="s">
         <v>561</v>
       </c>
-      <c r="C144" s="2" t="s">
+      <c r="C143" s="2" t="s">
         <v>562</v>
       </c>
     </row>
@@ -4912,14 +4939,14 @@
         <v>580</v>
       </c>
     </row>
-    <row r="152" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A152" s="1" t="s">
+    <row r="151" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A151" s="1" t="s">
         <v>581</v>
       </c>
-      <c r="B152" s="2" t="s">
+      <c r="B151" s="2" t="s">
         <v>582</v>
       </c>
-      <c r="C152" s="2" t="s">
+      <c r="C151" s="2" t="s">
         <v>583</v>
       </c>
     </row>
@@ -4956,7 +4983,7 @@
         <v>592</v>
       </c>
     </row>
-    <row r="156" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A156" s="1" t="s">
         <v>593</v>
       </c>
@@ -4967,16 +4994,21 @@
         <v>595</v>
       </c>
     </row>
+    <row r="157" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A157" s="1" t="s">
+        <v>596</v>
+      </c>
+      <c r="B157" s="2" t="s">
+        <v>597</v>
+      </c>
+      <c r="C157" s="2" t="s">
+        <v>598</v>
+      </c>
+    </row>
     <row r="158" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A158" s="1" t="s">
-        <v>596</v>
-      </c>
-      <c r="B158" s="2" t="s">
-        <v>597</v>
-      </c>
-      <c r="C158" s="2" t="s">
-        <v>598</v>
-      </c>
+      <c r="A158"/>
+      <c r="B158"/>
+      <c r="C158"/>
     </row>
     <row r="159" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A159" s="1" t="s">
@@ -4989,14 +5021,14 @@
         <v>601</v>
       </c>
     </row>
-    <row r="160" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A160" s="1" t="s">
         <v>602</v>
       </c>
-      <c r="B160" s="1" t="s">
+      <c r="B160" s="2" t="s">
         <v>603</v>
       </c>
-      <c r="C160" s="1" t="s">
+      <c r="C160" s="2" t="s">
         <v>604</v>
       </c>
     </row>
@@ -5004,7 +5036,7 @@
       <c r="A161" s="1" t="s">
         <v>605</v>
       </c>
-      <c r="B161" s="2" t="s">
+      <c r="B161" s="1" t="s">
         <v>606</v>
       </c>
       <c r="C161" s="1" t="s">
@@ -5015,7 +5047,7 @@
       <c r="A162" s="1" t="s">
         <v>608</v>
       </c>
-      <c r="B162" s="1" t="s">
+      <c r="B162" s="2" t="s">
         <v>609</v>
       </c>
       <c r="C162" s="1" t="s">
@@ -5026,71 +5058,71 @@
       <c r="A163" s="1" t="s">
         <v>611</v>
       </c>
-      <c r="B163" s="2" t="s">
+      <c r="B163" s="1" t="s">
         <v>612</v>
       </c>
-      <c r="C163" s="2" t="s">
+      <c r="C163" s="1" t="s">
         <v>613</v>
+      </c>
+    </row>
+    <row r="164" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A164" s="1" t="s">
+        <v>614</v>
+      </c>
+      <c r="B164" s="2" t="s">
+        <v>615</v>
+      </c>
+      <c r="C164" s="2" t="s">
+        <v>616</v>
       </c>
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A165" s="1" t="s">
-        <v>614</v>
+        <v>617</v>
       </c>
       <c r="B165" s="2" t="s">
-        <v>615</v>
+        <v>618</v>
       </c>
       <c r="C165" s="2" t="s">
-        <v>616</v>
+        <v>619</v>
       </c>
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A166" s="1" t="s">
-        <v>617</v>
+        <v>620</v>
       </c>
       <c r="B166" s="2" t="s">
-        <v>618</v>
+        <v>621</v>
       </c>
       <c r="C166" s="2" t="s">
-        <v>619</v>
-      </c>
-    </row>
-    <row r="167" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B167" s="2"/>
-      <c r="C167" s="2"/>
+        <v>622</v>
+      </c>
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A168" s="1" t="s">
-        <v>620</v>
+        <v>623</v>
       </c>
       <c r="B168" s="2" t="s">
-        <v>621</v>
+        <v>624</v>
       </c>
       <c r="C168" s="2" t="s">
-        <v>622</v>
+        <v>625</v>
       </c>
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A169" s="1" t="s">
-        <v>623</v>
+        <v>626</v>
       </c>
       <c r="B169" s="2" t="s">
-        <v>624</v>
+        <v>627</v>
       </c>
       <c r="C169" s="2" t="s">
-        <v>625</v>
+        <v>628</v>
       </c>
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A170" s="1" t="s">
-        <v>626</v>
-      </c>
-      <c r="B170" s="2" t="s">
-        <v>627</v>
-      </c>
-      <c r="C170" s="2" t="s">
-        <v>628</v>
-      </c>
+      <c r="B170" s="2"/>
+      <c r="C170" s="2"/>
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A171" s="1" t="s">
@@ -5115,41 +5147,41 @@
       </c>
     </row>
     <row r="173" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B173" s="2"/>
-      <c r="C173" s="2"/>
+      <c r="A173" s="1" t="s">
+        <v>635</v>
+      </c>
+      <c r="B173" s="2" t="s">
+        <v>636</v>
+      </c>
+      <c r="C173" s="2" t="s">
+        <v>637</v>
+      </c>
     </row>
     <row r="174" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A174" s="1" t="s">
-        <v>635</v>
+        <v>638</v>
       </c>
       <c r="B174" s="2" t="s">
-        <v>636</v>
+        <v>639</v>
       </c>
       <c r="C174" s="2" t="s">
-        <v>637</v>
+        <v>640</v>
       </c>
     </row>
     <row r="175" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A175" s="1" t="s">
-        <v>638</v>
+        <v>641</v>
       </c>
       <c r="B175" s="2" t="s">
-        <v>639</v>
+        <v>642</v>
       </c>
       <c r="C175" s="2" t="s">
-        <v>640</v>
+        <v>643</v>
       </c>
     </row>
     <row r="176" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A176" s="1" t="s">
-        <v>641</v>
-      </c>
-      <c r="B176" s="2" t="s">
-        <v>642</v>
-      </c>
-      <c r="C176" s="2" t="s">
-        <v>643</v>
-      </c>
+      <c r="B176" s="2"/>
+      <c r="C176" s="2"/>
     </row>
     <row r="177" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A177" s="1" t="s">
@@ -5195,36 +5227,36 @@
         <v>655</v>
       </c>
     </row>
+    <row r="181" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A181" s="1" t="s">
+        <v>656</v>
+      </c>
+      <c r="B181" s="2" t="s">
+        <v>657</v>
+      </c>
+      <c r="C181" s="2" t="s">
+        <v>658</v>
+      </c>
+    </row>
     <row r="182" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A182" s="1" t="s">
-        <v>656</v>
-      </c>
-      <c r="B182" s="1" t="s">
-        <v>657</v>
-      </c>
-      <c r="C182" s="1" t="s">
-        <v>658</v>
+        <v>659</v>
+      </c>
+      <c r="B182" s="2" t="s">
+        <v>660</v>
+      </c>
+      <c r="C182" s="2" t="s">
+        <v>661</v>
       </c>
     </row>
     <row r="183" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A183" s="1" t="s">
-        <v>659</v>
-      </c>
-      <c r="B183" s="1" t="s">
-        <v>660</v>
-      </c>
-      <c r="C183" s="1" t="s">
-        <v>661</v>
-      </c>
-    </row>
-    <row r="184" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A184" s="1" t="s">
         <v>662</v>
       </c>
-      <c r="B184" s="1" t="s">
+      <c r="B183" s="2" t="s">
         <v>663</v>
       </c>
-      <c r="C184" s="1" t="s">
+      <c r="C183" s="2" t="s">
         <v>664</v>
       </c>
     </row>
@@ -5243,10 +5275,10 @@
       <c r="A186" s="1" t="s">
         <v>668</v>
       </c>
-      <c r="B186" s="2" t="s">
+      <c r="B186" s="1" t="s">
         <v>669</v>
       </c>
-      <c r="C186" s="2" t="s">
+      <c r="C186" s="1" t="s">
         <v>670</v>
       </c>
     </row>
@@ -5270,6 +5302,39 @@
       </c>
       <c r="C188" s="1" t="s">
         <v>676</v>
+      </c>
+    </row>
+    <row r="189" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A189" s="1" t="s">
+        <v>677</v>
+      </c>
+      <c r="B189" s="2" t="s">
+        <v>678</v>
+      </c>
+      <c r="C189" s="2" t="s">
+        <v>679</v>
+      </c>
+    </row>
+    <row r="190" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A190" s="1" t="s">
+        <v>680</v>
+      </c>
+      <c r="B190" s="1" t="s">
+        <v>681</v>
+      </c>
+      <c r="C190" s="1" t="s">
+        <v>682</v>
+      </c>
+    </row>
+    <row r="191" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A191" s="1" t="s">
+        <v>683</v>
+      </c>
+      <c r="B191" s="1" t="s">
+        <v>684</v>
+      </c>
+      <c r="C191" s="1" t="s">
+        <v>685</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Cache and reuse data about Queues
</commit_message>
<xml_diff>
--- a/Config.xlsx
+++ b/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mateus.cruz\Documents\GitHub\OrchestratorManager\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C42D761C-7997-4400-BD66-3EB18215FEB4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72ED7A76-EE4B-46A3-AC4B-1B567F355D83}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="736" uniqueCount="688">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="742" uniqueCount="692">
   <si>
     <t>Name</t>
   </si>
@@ -79,6 +79,9 @@
   </si>
   <si>
     <t>OnPremisesOrchestratorURL</t>
+  </si>
+  <si>
+    <t>https://myOrchestratorURL</t>
   </si>
   <si>
     <t>URL of the Orchestrator instance to be used. 
@@ -2139,10 +2142,19 @@
     <t>キュー アイテムを含むファイルが見つかりませんでした。</t>
   </si>
   <si>
+    <t>QueueNameAlreadyUsed</t>
+  </si>
+  <si>
+    <t>The Queue name {0} is already used.</t>
+  </si>
+  <si>
+    <t>キュー名 {0} は既に使用されています。</t>
+  </si>
+  <si>
+    <t>QueueItemsDownloadPathNotSpecified</t>
+  </si>
+  <si>
     <t>SampleAccount</t>
-  </si>
-  <si>
-    <t>https://myOrchestratorURL</t>
   </si>
 </sst>
 </file>
@@ -2235,8 +2247,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table13" displayName="Table13" ref="A1:C191" totalsRowShown="0">
-  <autoFilter ref="A1:C191" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table13" displayName="Table13" ref="A1:C193" totalsRowShown="0">
+  <autoFilter ref="A1:C193" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Name"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="EN"/>
@@ -2557,7 +2569,7 @@
         <v>7</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>686</v>
+        <v>691</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>8</v>
@@ -2579,21 +2591,21 @@
         <v>12</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>687</v>
+        <v>13</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="159.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B7" s="1">
         <v>201804</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -2633,684 +2645,684 @@
     </row>
     <row r="2" spans="1:3" ht="101.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B2" s="1">
         <v>200</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B3" s="1">
         <v>0</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B4" s="1">
         <v>550</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B5" s="1">
         <v>650</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B6" s="1">
         <v>3</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B7" s="1">
         <v>5000</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A30" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="1" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A33" s="1" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A34" s="1" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A35" s="1" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A36" s="1" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A37" s="1" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A38" s="1" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A39" s="1" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A40" s="1" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="41" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A41" s="1" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
     </row>
     <row r="42" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A42" s="1" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="43" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A43" s="1" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A44" s="1" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="45" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A45" s="1" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
     <row r="46" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A46" s="1" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
     </row>
     <row r="47" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A47" s="1" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
     </row>
     <row r="48" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A48" s="1" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A49" s="1" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="50" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A50" s="1" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
     </row>
     <row r="51" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A51" s="1" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A52" s="1" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="53" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A53" s="1" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="54" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A54" s="1" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A55" s="1" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
     </row>
     <row r="56" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A56" s="1" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
     </row>
     <row r="57" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A57" s="1" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
     </row>
     <row r="58" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A58" s="1" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
     </row>
     <row r="59" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A59" s="1" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
     </row>
     <row r="60" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A60" s="1" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
     </row>
     <row r="61" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A61" s="1" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
     </row>
     <row r="62" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A62" s="1" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
     </row>
     <row r="63" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A63" s="1" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
   </sheetData>
@@ -3328,7 +3340,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1927ABA9-1814-4487-9CEC-ABDCAF91481F}">
-  <dimension ref="A1:C191"/>
+  <dimension ref="A1:C193"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -3346,472 +3358,472 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="43.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A30" s="1" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A31" s="1" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A32" s="1" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A33" s="1" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A34" s="1" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A35" s="1" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A36" s="1" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A37" s="1" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A38" s="1" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A39" s="1" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="43.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A40" s="1" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
     </row>
     <row r="41" spans="1:3" ht="43.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A41" s="1" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
     </row>
     <row r="42" spans="1:3" ht="58" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A42" s="1" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A43" s="1" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.35">
@@ -3820,112 +3832,112 @@
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A45" s="1" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A46" s="1" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A47" s="1" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A48" s="1" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A49" s="1" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A50" s="1" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A51" s="1" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A52" s="1" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A53" s="1" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A54" s="1" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.35">
@@ -3934,596 +3946,596 @@
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A56" s="1" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A57" s="1" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A58" s="1" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A59" s="1" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A60" s="1" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A61" s="1" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A62" s="1" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A63" s="1" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A64" s="1" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A65" s="1" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A66" s="1" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A67" s="1" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A68" s="1" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A69" s="1" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A70" s="1" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A71" s="1" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A72" s="1" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A73" s="1" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A74" s="1" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A75" s="1" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A76" s="1" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
     </row>
     <row r="77" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A77" s="1" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A78" s="1" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A79" s="1" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
     </row>
     <row r="80" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A80" s="1" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A81" s="1" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A82" s="1" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A83" s="1" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A84" s="1" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
     </row>
     <row r="85" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A85" s="1" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
     </row>
     <row r="86" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A86" s="1" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
     </row>
     <row r="87" spans="1:3" ht="43.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A87" s="1" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A88" s="1" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A89" s="1" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
     </row>
     <row r="90" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A90" s="1" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A91" s="1" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A92" s="1" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A93" s="1" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>424</v>
+        <v>425</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A94" s="1" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>426</v>
+        <v>427</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A95" s="1" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A96" s="1" t="s">
-        <v>431</v>
+        <v>432</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A97" s="1" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="C97" s="2" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A98" s="1" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>438</v>
+        <v>439</v>
       </c>
       <c r="C98" s="2" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A99" s="1" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>441</v>
+        <v>442</v>
       </c>
       <c r="C99" s="2" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A100" s="1" t="s">
-        <v>443</v>
+        <v>444</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>444</v>
+        <v>445</v>
       </c>
       <c r="C100" s="2" t="s">
-        <v>445</v>
+        <v>446</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A101" s="1" t="s">
-        <v>446</v>
+        <v>447</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>447</v>
+        <v>448</v>
       </c>
       <c r="C101" s="2" t="s">
-        <v>448</v>
+        <v>449</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A102" s="1" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="C102" s="2" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A103" s="1" t="s">
-        <v>452</v>
+        <v>453</v>
       </c>
       <c r="B103" s="2" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="C103" s="2" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A104" s="1" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
       <c r="B104" s="2" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
       <c r="C104" s="2" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
     </row>
     <row r="105" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A105" s="1" t="s">
-        <v>458</v>
+        <v>459</v>
       </c>
       <c r="B105" s="2" t="s">
-        <v>459</v>
+        <v>460</v>
       </c>
       <c r="C105" s="2" t="s">
-        <v>460</v>
+        <v>461</v>
       </c>
     </row>
     <row r="106" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A106" s="1" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="B106" s="2" t="s">
-        <v>462</v>
+        <v>463</v>
       </c>
       <c r="C106" s="2" t="s">
-        <v>463</v>
+        <v>464</v>
       </c>
     </row>
     <row r="107" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A107" s="1" t="s">
-        <v>464</v>
+        <v>465</v>
       </c>
       <c r="B107" s="2" t="s">
-        <v>465</v>
+        <v>466</v>
       </c>
       <c r="C107" s="2" t="s">
-        <v>466</v>
+        <v>467</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A108" s="1" t="s">
-        <v>467</v>
+        <v>468</v>
       </c>
       <c r="B108" s="2" t="s">
-        <v>468</v>
+        <v>469</v>
       </c>
       <c r="C108" s="2" t="s">
-        <v>469</v>
+        <v>470</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A109" s="1" t="s">
-        <v>470</v>
+        <v>471</v>
       </c>
       <c r="B109" s="2" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="C109" s="2" t="s">
-        <v>472</v>
+        <v>473</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.35">
@@ -4532,90 +4544,90 @@
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A111" s="1" t="s">
-        <v>473</v>
+        <v>474</v>
       </c>
       <c r="B111" s="2" t="s">
-        <v>474</v>
+        <v>475</v>
       </c>
       <c r="C111" s="2" t="s">
-        <v>475</v>
+        <v>476</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A112" s="1" t="s">
-        <v>476</v>
+        <v>477</v>
       </c>
       <c r="B112" s="2" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="C112" s="2" t="s">
-        <v>478</v>
+        <v>479</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A113" s="1" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="B113" s="2" t="s">
-        <v>480</v>
+        <v>481</v>
       </c>
       <c r="C113" s="2" t="s">
-        <v>481</v>
+        <v>482</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A114" s="1" t="s">
-        <v>482</v>
+        <v>483</v>
       </c>
       <c r="B114" s="2" t="s">
-        <v>483</v>
+        <v>484</v>
       </c>
       <c r="C114" s="2" t="s">
-        <v>484</v>
+        <v>485</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A115" s="1" t="s">
-        <v>485</v>
+        <v>486</v>
       </c>
       <c r="B115" s="2" t="s">
-        <v>486</v>
+        <v>487</v>
       </c>
       <c r="C115" s="2" t="s">
-        <v>487</v>
+        <v>488</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A116" s="1" t="s">
-        <v>488</v>
+        <v>489</v>
       </c>
       <c r="B116" s="2" t="s">
-        <v>489</v>
+        <v>490</v>
       </c>
       <c r="C116" s="2" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A117" s="1" t="s">
-        <v>491</v>
+        <v>492</v>
       </c>
       <c r="B117" s="2" t="s">
-        <v>492</v>
+        <v>493</v>
       </c>
       <c r="C117" s="2" t="s">
-        <v>493</v>
+        <v>494</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A118" s="1" t="s">
-        <v>494</v>
+        <v>495</v>
       </c>
       <c r="B118" s="2" t="s">
-        <v>495</v>
+        <v>496</v>
       </c>
       <c r="C118" s="2" t="s">
-        <v>496</v>
+        <v>497</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.35">
@@ -4624,500 +4636,496 @@
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A120" s="1" t="s">
-        <v>497</v>
+        <v>498</v>
       </c>
       <c r="B120" s="2" t="s">
-        <v>498</v>
+        <v>499</v>
       </c>
       <c r="C120" s="2" t="s">
-        <v>499</v>
+        <v>500</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A121" s="1" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="B121" s="2" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C121" s="2" t="s">
-        <v>502</v>
+        <v>503</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A122" s="1" t="s">
-        <v>503</v>
+        <v>504</v>
       </c>
       <c r="B122" s="2" t="s">
-        <v>504</v>
+        <v>505</v>
       </c>
       <c r="C122" s="2" t="s">
-        <v>505</v>
+        <v>506</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A123" s="1" t="s">
-        <v>506</v>
+        <v>507</v>
       </c>
       <c r="B123" s="2" t="s">
-        <v>507</v>
+        <v>508</v>
       </c>
       <c r="C123" s="2" t="s">
-        <v>508</v>
+        <v>509</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A124" s="1" t="s">
-        <v>509</v>
+        <v>510</v>
       </c>
       <c r="B124" s="2" t="s">
-        <v>510</v>
+        <v>511</v>
       </c>
       <c r="C124" s="2" t="s">
-        <v>511</v>
+        <v>512</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A125" s="1" t="s">
-        <v>512</v>
+        <v>513</v>
       </c>
       <c r="B125" s="2" t="s">
-        <v>513</v>
+        <v>514</v>
       </c>
       <c r="C125" s="2" t="s">
-        <v>514</v>
+        <v>515</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A126" s="1" t="s">
-        <v>515</v>
+        <v>516</v>
       </c>
       <c r="B126" s="2" t="s">
-        <v>516</v>
+        <v>517</v>
       </c>
       <c r="C126" s="2" t="s">
-        <v>517</v>
+        <v>518</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A127" s="1" t="s">
-        <v>518</v>
+        <v>519</v>
       </c>
       <c r="B127" s="2" t="s">
-        <v>519</v>
+        <v>520</v>
       </c>
       <c r="C127" s="2" t="s">
-        <v>520</v>
+        <v>521</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A128" s="1" t="s">
-        <v>521</v>
+        <v>522</v>
       </c>
       <c r="B128" s="2" t="s">
-        <v>522</v>
+        <v>523</v>
       </c>
       <c r="C128" s="2" t="s">
-        <v>523</v>
+        <v>524</v>
       </c>
     </row>
     <row r="129" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A129" s="1" t="s">
-        <v>524</v>
+        <v>525</v>
       </c>
       <c r="B129" s="2" t="s">
-        <v>525</v>
+        <v>526</v>
       </c>
       <c r="C129" s="2" t="s">
-        <v>526</v>
+        <v>527</v>
       </c>
     </row>
     <row r="130" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A130"/>
       <c r="B130" s="2"/>
       <c r="C130" s="2"/>
     </row>
     <row r="131" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A131" s="1" t="s">
-        <v>527</v>
+        <v>528</v>
       </c>
       <c r="B131" s="2" t="s">
-        <v>528</v>
+        <v>529</v>
       </c>
       <c r="C131" s="2" t="s">
-        <v>529</v>
+        <v>530</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A132" s="1" t="s">
-        <v>530</v>
+        <v>531</v>
       </c>
       <c r="B132" s="2" t="s">
-        <v>531</v>
+        <v>532</v>
       </c>
       <c r="C132" s="2" t="s">
-        <v>532</v>
+        <v>533</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A133" s="1" t="s">
-        <v>533</v>
+        <v>534</v>
       </c>
       <c r="B133" s="2" t="s">
-        <v>534</v>
+        <v>535</v>
       </c>
       <c r="C133" s="2" t="s">
-        <v>535</v>
+        <v>536</v>
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A134" s="1" t="s">
-        <v>536</v>
+        <v>537</v>
       </c>
       <c r="B134" s="2" t="s">
-        <v>537</v>
+        <v>538</v>
       </c>
       <c r="C134" s="2" t="s">
-        <v>538</v>
+        <v>539</v>
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A135" s="1" t="s">
-        <v>539</v>
+        <v>540</v>
       </c>
       <c r="B135" s="2" t="s">
-        <v>540</v>
+        <v>541</v>
       </c>
       <c r="C135" s="2" t="s">
-        <v>541</v>
+        <v>542</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A136" s="1" t="s">
-        <v>542</v>
+        <v>543</v>
       </c>
       <c r="B136" s="2" t="s">
-        <v>543</v>
+        <v>544</v>
       </c>
       <c r="C136" s="2" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A137" s="1" t="s">
-        <v>545</v>
+        <v>546</v>
       </c>
       <c r="B137" s="2" t="s">
-        <v>546</v>
+        <v>547</v>
       </c>
       <c r="C137" s="2" t="s">
-        <v>547</v>
+        <v>548</v>
       </c>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A138" s="1" t="s">
-        <v>548</v>
+        <v>549</v>
       </c>
       <c r="B138" s="2" t="s">
-        <v>549</v>
+        <v>550</v>
       </c>
       <c r="C138" s="2" t="s">
-        <v>550</v>
+        <v>551</v>
       </c>
     </row>
     <row r="139" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A139"/>
       <c r="B139" s="2"/>
       <c r="C139" s="2"/>
     </row>
     <row r="140" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A140" s="1" t="s">
-        <v>551</v>
+        <v>552</v>
       </c>
       <c r="B140" s="2" t="s">
-        <v>552</v>
+        <v>553</v>
       </c>
       <c r="C140" s="2" t="s">
-        <v>553</v>
+        <v>554</v>
       </c>
     </row>
     <row r="141" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A141" s="1" t="s">
-        <v>554</v>
+        <v>555</v>
       </c>
       <c r="B141" s="2" t="s">
-        <v>555</v>
+        <v>556</v>
       </c>
       <c r="C141" s="2" t="s">
-        <v>556</v>
+        <v>557</v>
       </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A142" s="1" t="s">
-        <v>557</v>
+        <v>558</v>
       </c>
       <c r="B142" s="2" t="s">
-        <v>558</v>
+        <v>559</v>
       </c>
       <c r="C142" s="2" t="s">
-        <v>559</v>
+        <v>560</v>
       </c>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A143" s="1" t="s">
-        <v>560</v>
+        <v>561</v>
       </c>
       <c r="B143" s="2" t="s">
-        <v>561</v>
+        <v>562</v>
       </c>
       <c r="C143" s="2" t="s">
-        <v>562</v>
+        <v>563</v>
       </c>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A145" s="1" t="s">
-        <v>563</v>
+        <v>564</v>
       </c>
       <c r="B145" s="2" t="s">
-        <v>564</v>
+        <v>565</v>
       </c>
       <c r="C145" s="2" t="s">
-        <v>565</v>
+        <v>566</v>
       </c>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A146" s="1" t="s">
-        <v>566</v>
+        <v>567</v>
       </c>
       <c r="B146" s="2" t="s">
-        <v>567</v>
+        <v>568</v>
       </c>
       <c r="C146" s="2" t="s">
-        <v>568</v>
+        <v>569</v>
       </c>
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A147" s="1" t="s">
-        <v>569</v>
+        <v>570</v>
       </c>
       <c r="B147" s="2" t="s">
-        <v>570</v>
+        <v>571</v>
       </c>
       <c r="C147" s="2" t="s">
-        <v>571</v>
+        <v>572</v>
       </c>
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A148" s="1" t="s">
-        <v>572</v>
+        <v>573</v>
       </c>
       <c r="B148" s="2" t="s">
-        <v>573</v>
+        <v>574</v>
       </c>
       <c r="C148" s="2" t="s">
-        <v>574</v>
+        <v>575</v>
       </c>
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A149" s="1" t="s">
-        <v>575</v>
+        <v>576</v>
       </c>
       <c r="B149" s="2" t="s">
-        <v>576</v>
+        <v>577</v>
       </c>
       <c r="C149" s="2" t="s">
-        <v>577</v>
+        <v>578</v>
       </c>
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A150" s="1" t="s">
-        <v>578</v>
+        <v>579</v>
       </c>
       <c r="B150" s="2" t="s">
-        <v>579</v>
+        <v>580</v>
       </c>
       <c r="C150" s="2" t="s">
-        <v>580</v>
+        <v>581</v>
       </c>
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A151" s="1" t="s">
-        <v>581</v>
+        <v>582</v>
       </c>
       <c r="B151" s="2" t="s">
-        <v>582</v>
+        <v>583</v>
       </c>
       <c r="C151" s="2" t="s">
-        <v>583</v>
+        <v>584</v>
       </c>
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A153" s="1" t="s">
-        <v>584</v>
+        <v>585</v>
       </c>
       <c r="B153" s="2" t="s">
-        <v>585</v>
+        <v>586</v>
       </c>
       <c r="C153" s="2" t="s">
-        <v>586</v>
+        <v>587</v>
       </c>
     </row>
     <row r="154" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A154" s="1" t="s">
-        <v>587</v>
+        <v>588</v>
       </c>
       <c r="B154" s="2" t="s">
-        <v>588</v>
+        <v>589</v>
       </c>
       <c r="C154" s="2" t="s">
-        <v>589</v>
+        <v>590</v>
       </c>
     </row>
     <row r="155" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A155" s="1" t="s">
-        <v>590</v>
+        <v>591</v>
       </c>
       <c r="B155" s="2" t="s">
-        <v>591</v>
+        <v>592</v>
       </c>
       <c r="C155" s="2" t="s">
-        <v>592</v>
+        <v>593</v>
       </c>
     </row>
     <row r="156" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A156" s="1" t="s">
-        <v>593</v>
+        <v>594</v>
       </c>
       <c r="B156" s="2" t="s">
-        <v>594</v>
+        <v>595</v>
       </c>
       <c r="C156" s="2" t="s">
-        <v>595</v>
+        <v>596</v>
       </c>
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A157" s="1" t="s">
-        <v>596</v>
+        <v>597</v>
       </c>
       <c r="B157" s="2" t="s">
-        <v>597</v>
+        <v>598</v>
       </c>
       <c r="C157" s="2" t="s">
-        <v>598</v>
-      </c>
-    </row>
-    <row r="158" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A158"/>
-      <c r="B158"/>
-      <c r="C158"/>
-    </row>
+        <v>599</v>
+      </c>
+    </row>
+    <row r="158" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="159" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A159" s="1" t="s">
-        <v>599</v>
+        <v>600</v>
       </c>
       <c r="B159" s="2" t="s">
-        <v>600</v>
+        <v>601</v>
       </c>
       <c r="C159" s="2" t="s">
-        <v>601</v>
+        <v>602</v>
       </c>
     </row>
     <row r="160" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A160" s="1" t="s">
-        <v>602</v>
+        <v>603</v>
       </c>
       <c r="B160" s="2" t="s">
-        <v>603</v>
+        <v>604</v>
       </c>
       <c r="C160" s="2" t="s">
-        <v>604</v>
+        <v>605</v>
       </c>
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A161" s="1" t="s">
-        <v>605</v>
+        <v>606</v>
       </c>
       <c r="B161" s="1" t="s">
-        <v>606</v>
+        <v>607</v>
       </c>
       <c r="C161" s="1" t="s">
-        <v>607</v>
+        <v>608</v>
       </c>
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A162" s="1" t="s">
-        <v>608</v>
+        <v>609</v>
       </c>
       <c r="B162" s="2" t="s">
-        <v>609</v>
+        <v>610</v>
       </c>
       <c r="C162" s="1" t="s">
-        <v>610</v>
+        <v>611</v>
       </c>
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A163" s="1" t="s">
-        <v>611</v>
+        <v>612</v>
       </c>
       <c r="B163" s="1" t="s">
-        <v>612</v>
+        <v>613</v>
       </c>
       <c r="C163" s="1" t="s">
-        <v>613</v>
+        <v>614</v>
       </c>
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A164" s="1" t="s">
-        <v>614</v>
+        <v>615</v>
       </c>
       <c r="B164" s="2" t="s">
-        <v>615</v>
+        <v>616</v>
       </c>
       <c r="C164" s="2" t="s">
-        <v>616</v>
+        <v>617</v>
       </c>
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A165" s="1" t="s">
-        <v>617</v>
+        <v>618</v>
       </c>
       <c r="B165" s="2" t="s">
-        <v>618</v>
+        <v>619</v>
       </c>
       <c r="C165" s="2" t="s">
-        <v>619</v>
+        <v>620</v>
       </c>
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A166" s="1" t="s">
-        <v>620</v>
+        <v>621</v>
       </c>
       <c r="B166" s="2" t="s">
-        <v>621</v>
+        <v>622</v>
       </c>
       <c r="C166" s="2" t="s">
-        <v>622</v>
+        <v>623</v>
       </c>
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A168" s="1" t="s">
-        <v>623</v>
+        <v>624</v>
       </c>
       <c r="B168" s="2" t="s">
-        <v>624</v>
+        <v>625</v>
       </c>
       <c r="C168" s="2" t="s">
-        <v>625</v>
+        <v>626</v>
       </c>
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A169" s="1" t="s">
-        <v>626</v>
+        <v>627</v>
       </c>
       <c r="B169" s="2" t="s">
-        <v>627</v>
+        <v>628</v>
       </c>
       <c r="C169" s="2" t="s">
-        <v>628</v>
+        <v>629</v>
       </c>
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.35">
@@ -5126,57 +5134,57 @@
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A171" s="1" t="s">
-        <v>629</v>
+        <v>630</v>
       </c>
       <c r="B171" s="2" t="s">
-        <v>630</v>
+        <v>631</v>
       </c>
       <c r="C171" s="2" t="s">
-        <v>631</v>
+        <v>632</v>
       </c>
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A172" s="1" t="s">
-        <v>632</v>
+        <v>633</v>
       </c>
       <c r="B172" s="2" t="s">
-        <v>633</v>
+        <v>634</v>
       </c>
       <c r="C172" s="2" t="s">
-        <v>634</v>
+        <v>635</v>
       </c>
     </row>
     <row r="173" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A173" s="1" t="s">
-        <v>635</v>
+        <v>636</v>
       </c>
       <c r="B173" s="2" t="s">
-        <v>636</v>
+        <v>637</v>
       </c>
       <c r="C173" s="2" t="s">
-        <v>637</v>
+        <v>638</v>
       </c>
     </row>
     <row r="174" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A174" s="1" t="s">
-        <v>638</v>
+        <v>639</v>
       </c>
       <c r="B174" s="2" t="s">
-        <v>639</v>
+        <v>640</v>
       </c>
       <c r="C174" s="2" t="s">
-        <v>640</v>
+        <v>641</v>
       </c>
     </row>
     <row r="175" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A175" s="1" t="s">
-        <v>641</v>
+        <v>642</v>
       </c>
       <c r="B175" s="2" t="s">
-        <v>642</v>
+        <v>643</v>
       </c>
       <c r="C175" s="2" t="s">
-        <v>643</v>
+        <v>644</v>
       </c>
     </row>
     <row r="176" spans="1:3" x14ac:dyDescent="0.35">
@@ -5185,156 +5193,178 @@
     </row>
     <row r="177" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A177" s="1" t="s">
-        <v>644</v>
+        <v>645</v>
       </c>
       <c r="B177" s="2" t="s">
-        <v>645</v>
+        <v>646</v>
       </c>
       <c r="C177" s="2" t="s">
-        <v>646</v>
+        <v>647</v>
       </c>
     </row>
     <row r="178" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A178" s="1" t="s">
-        <v>647</v>
+        <v>648</v>
       </c>
       <c r="B178" s="2" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
       <c r="C178" s="2" t="s">
-        <v>649</v>
+        <v>650</v>
       </c>
     </row>
     <row r="179" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A179" s="1" t="s">
-        <v>650</v>
+        <v>651</v>
       </c>
       <c r="B179" s="2" t="s">
-        <v>651</v>
+        <v>652</v>
       </c>
       <c r="C179" s="2" t="s">
-        <v>652</v>
+        <v>653</v>
       </c>
     </row>
     <row r="180" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A180" s="1" t="s">
-        <v>653</v>
+        <v>654</v>
       </c>
       <c r="B180" s="2" t="s">
-        <v>654</v>
+        <v>655</v>
       </c>
       <c r="C180" s="2" t="s">
-        <v>655</v>
+        <v>656</v>
       </c>
     </row>
     <row r="181" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A181" s="1" t="s">
-        <v>656</v>
+        <v>657</v>
       </c>
       <c r="B181" s="2" t="s">
-        <v>657</v>
+        <v>658</v>
       </c>
       <c r="C181" s="2" t="s">
-        <v>658</v>
+        <v>659</v>
       </c>
     </row>
     <row r="182" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A182" s="1" t="s">
-        <v>659</v>
+        <v>660</v>
       </c>
       <c r="B182" s="2" t="s">
-        <v>660</v>
+        <v>661</v>
       </c>
       <c r="C182" s="2" t="s">
-        <v>661</v>
+        <v>662</v>
       </c>
     </row>
     <row r="183" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A183" s="1" t="s">
-        <v>662</v>
+        <v>663</v>
       </c>
       <c r="B183" s="2" t="s">
-        <v>663</v>
+        <v>664</v>
       </c>
       <c r="C183" s="2" t="s">
-        <v>664</v>
+        <v>665</v>
       </c>
     </row>
     <row r="185" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A185" s="1" t="s">
-        <v>665</v>
+        <v>666</v>
       </c>
       <c r="B185" s="1" t="s">
-        <v>666</v>
+        <v>667</v>
       </c>
       <c r="C185" s="1" t="s">
-        <v>667</v>
+        <v>668</v>
       </c>
     </row>
     <row r="186" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A186" s="1" t="s">
-        <v>668</v>
+        <v>669</v>
       </c>
       <c r="B186" s="1" t="s">
-        <v>669</v>
+        <v>670</v>
       </c>
       <c r="C186" s="1" t="s">
-        <v>670</v>
+        <v>671</v>
       </c>
     </row>
     <row r="187" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A187" s="1" t="s">
-        <v>671</v>
+        <v>672</v>
       </c>
       <c r="B187" s="1" t="s">
-        <v>672</v>
+        <v>673</v>
       </c>
       <c r="C187" s="1" t="s">
-        <v>673</v>
+        <v>674</v>
       </c>
     </row>
     <row r="188" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A188" s="1" t="s">
-        <v>674</v>
+        <v>675</v>
       </c>
       <c r="B188" s="1" t="s">
-        <v>675</v>
+        <v>676</v>
       </c>
       <c r="C188" s="1" t="s">
-        <v>676</v>
+        <v>677</v>
       </c>
     </row>
     <row r="189" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A189" s="1" t="s">
-        <v>677</v>
+        <v>678</v>
       </c>
       <c r="B189" s="2" t="s">
-        <v>678</v>
+        <v>679</v>
       </c>
       <c r="C189" s="2" t="s">
-        <v>679</v>
+        <v>680</v>
       </c>
     </row>
     <row r="190" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A190" s="1" t="s">
-        <v>680</v>
+        <v>681</v>
       </c>
       <c r="B190" s="1" t="s">
-        <v>681</v>
+        <v>682</v>
       </c>
       <c r="C190" s="1" t="s">
-        <v>682</v>
+        <v>683</v>
       </c>
     </row>
     <row r="191" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A191" s="1" t="s">
-        <v>683</v>
+        <v>684</v>
       </c>
       <c r="B191" s="1" t="s">
-        <v>684</v>
+        <v>685</v>
       </c>
       <c r="C191" s="1" t="s">
-        <v>685</v>
+        <v>686</v>
+      </c>
+    </row>
+    <row r="192" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A192" s="1" t="s">
+        <v>687</v>
+      </c>
+      <c r="B192" s="2" t="s">
+        <v>688</v>
+      </c>
+      <c r="C192" s="2" t="s">
+        <v>689</v>
+      </c>
+    </row>
+    <row r="193" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A193" s="1" t="s">
+        <v>690</v>
+      </c>
+      <c r="B193" s="2" t="s">
+        <v>664</v>
+      </c>
+      <c r="C193" s="2" t="s">
+        <v>665</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Cache and reuse data about Robots
</commit_message>
<xml_diff>
--- a/Config.xlsx
+++ b/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mateus.cruz\Documents\GitHub\OrchestratorManager\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72ED7A76-EE4B-46A3-AC4B-1B567F355D83}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AA0F309-B94B-4654-8303-E49B6DC0AD33}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="742" uniqueCount="692">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="745" uniqueCount="695">
   <si>
     <t>Name</t>
   </si>
@@ -56,11 +56,17 @@
     <t>CloudTenantName</t>
   </si>
   <si>
+    <t>Default</t>
+  </si>
+  <si>
     <t>Name of the tenant to be used in case of Automation Cloud Orchestrator instances. 
 Sample value: Default.</t>
   </si>
   <si>
     <t>CloudAccountName</t>
+  </si>
+  <si>
+    <t>SampleAccount</t>
   </si>
   <si>
     <t>Unique site URL for Automation Cloud organization.
@@ -71,17 +77,11 @@
     <t>OnPremisesTenantName</t>
   </si>
   <si>
-    <t>Default</t>
-  </si>
-  <si>
     <t>Name of the tenant to be used in case of on-premises Orchestrator instances. 
 Sample value: Default.</t>
   </si>
   <si>
     <t>OnPremisesOrchestratorURL</t>
-  </si>
-  <si>
-    <t>https://myOrchestratorURL</t>
   </si>
   <si>
     <t>URL of the Orchestrator instance to be used. 
@@ -1733,6 +1733,15 @@
     <t>ロボット {0} が見つかりません。</t>
   </si>
   <si>
+    <t>RobotNameAlreadyUsed</t>
+  </si>
+  <si>
+    <t>The Robot name {0} is already used.</t>
+  </si>
+  <si>
+    <t>ロボット名 {0} は既に使用されています。</t>
+  </si>
+  <si>
     <t>MachineNotFound</t>
   </si>
   <si>
@@ -2154,7 +2163,7 @@
     <t>QueueItemsDownloadPathNotSpecified</t>
   </si>
   <si>
-    <t>SampleAccount</t>
+    <t>https://myOrchestratorURL</t>
   </si>
 </sst>
 </file>
@@ -2247,8 +2256,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table13" displayName="Table13" ref="A1:C193" totalsRowShown="0">
-  <autoFilter ref="A1:C193" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table13" displayName="Table13" ref="A1:C194" totalsRowShown="0">
+  <autoFilter ref="A1:C194" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Name"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="EN"/>
@@ -2558,40 +2567,40 @@
         <v>5</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="72.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>691</v>
+        <v>9</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="58" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="58" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>13</v>
+        <v>694</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>14</v>
@@ -2622,7 +2631,7 @@
   <dimension ref="A1:C63"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A2" sqref="A2 A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3340,10 +3349,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1927ABA9-1814-4487-9CEC-ABDCAF91481F}">
-  <dimension ref="A1:C193"/>
+  <dimension ref="A1:C194"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A2" sqref="A2 A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4745,7 +4754,6 @@
       </c>
     </row>
     <row r="130" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A130"/>
       <c r="B130" s="2"/>
       <c r="C130" s="2"/>
     </row>
@@ -4837,20 +4845,20 @@
         <v>551</v>
       </c>
     </row>
-    <row r="139" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B139" s="2"/>
-      <c r="C139" s="2"/>
-    </row>
-    <row r="140" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A140" s="1" t="s">
+    <row r="139" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A139" s="1" t="s">
         <v>552</v>
       </c>
-      <c r="B140" s="2" t="s">
+      <c r="B139" s="2" t="s">
         <v>553</v>
       </c>
-      <c r="C140" s="2" t="s">
+      <c r="C139" s="2" t="s">
         <v>554</v>
       </c>
+    </row>
+    <row r="140" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B140" s="2"/>
+      <c r="C140" s="2"/>
     </row>
     <row r="141" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A141" s="1" t="s">
@@ -4863,7 +4871,7 @@
         <v>557</v>
       </c>
     </row>
-    <row r="142" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A142" s="1" t="s">
         <v>558</v>
       </c>
@@ -4885,14 +4893,14 @@
         <v>563</v>
       </c>
     </row>
-    <row r="145" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A145" s="1" t="s">
+    <row r="144" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A144" s="1" t="s">
         <v>564</v>
       </c>
-      <c r="B145" s="2" t="s">
+      <c r="B144" s="2" t="s">
         <v>565</v>
       </c>
-      <c r="C145" s="2" t="s">
+      <c r="C144" s="2" t="s">
         <v>566</v>
       </c>
     </row>
@@ -4962,18 +4970,18 @@
         <v>584</v>
       </c>
     </row>
-    <row r="153" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A153" s="1" t="s">
+    <row r="152" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A152" s="1" t="s">
         <v>585</v>
       </c>
-      <c r="B153" s="2" t="s">
+      <c r="B152" s="2" t="s">
         <v>586</v>
       </c>
-      <c r="C153" s="2" t="s">
+      <c r="C152" s="2" t="s">
         <v>587</v>
       </c>
     </row>
-    <row r="154" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A154" s="1" t="s">
         <v>588</v>
       </c>
@@ -5006,7 +5014,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="157" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A157" s="1" t="s">
         <v>597</v>
       </c>
@@ -5017,17 +5025,21 @@
         <v>599</v>
       </c>
     </row>
-    <row r="158" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="158" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A158" s="1" t="s">
+        <v>600</v>
+      </c>
+      <c r="B158" s="2" t="s">
+        <v>601</v>
+      </c>
+      <c r="C158" s="2" t="s">
+        <v>602</v>
+      </c>
+    </row>
     <row r="159" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A159" s="1" t="s">
-        <v>600</v>
-      </c>
-      <c r="B159" s="2" t="s">
-        <v>601</v>
-      </c>
-      <c r="C159" s="2" t="s">
-        <v>602</v>
-      </c>
+      <c r="A159"/>
+      <c r="B159"/>
+      <c r="C159"/>
     </row>
     <row r="160" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A160" s="1" t="s">
@@ -5040,14 +5052,14 @@
         <v>605</v>
       </c>
     </row>
-    <row r="161" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A161" s="1" t="s">
         <v>606</v>
       </c>
-      <c r="B161" s="1" t="s">
+      <c r="B161" s="2" t="s">
         <v>607</v>
       </c>
-      <c r="C161" s="1" t="s">
+      <c r="C161" s="2" t="s">
         <v>608</v>
       </c>
     </row>
@@ -5055,7 +5067,7 @@
       <c r="A162" s="1" t="s">
         <v>609</v>
       </c>
-      <c r="B162" s="2" t="s">
+      <c r="B162" s="1" t="s">
         <v>610</v>
       </c>
       <c r="C162" s="1" t="s">
@@ -5066,7 +5078,7 @@
       <c r="A163" s="1" t="s">
         <v>612</v>
       </c>
-      <c r="B163" s="1" t="s">
+      <c r="B163" s="2" t="s">
         <v>613</v>
       </c>
       <c r="C163" s="1" t="s">
@@ -5077,10 +5089,10 @@
       <c r="A164" s="1" t="s">
         <v>615</v>
       </c>
-      <c r="B164" s="2" t="s">
+      <c r="B164" s="1" t="s">
         <v>616</v>
       </c>
-      <c r="C164" s="2" t="s">
+      <c r="C164" s="1" t="s">
         <v>617</v>
       </c>
     </row>
@@ -5106,14 +5118,14 @@
         <v>623</v>
       </c>
     </row>
-    <row r="168" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A168" s="1" t="s">
+    <row r="167" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A167" s="1" t="s">
         <v>624</v>
       </c>
-      <c r="B168" s="2" t="s">
+      <c r="B167" s="2" t="s">
         <v>625</v>
       </c>
-      <c r="C168" s="2" t="s">
+      <c r="C167" s="2" t="s">
         <v>626</v>
       </c>
     </row>
@@ -5129,19 +5141,19 @@
       </c>
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B170" s="2"/>
-      <c r="C170" s="2"/>
+      <c r="A170" s="1" t="s">
+        <v>630</v>
+      </c>
+      <c r="B170" s="2" t="s">
+        <v>631</v>
+      </c>
+      <c r="C170" s="2" t="s">
+        <v>632</v>
+      </c>
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A171" s="1" t="s">
-        <v>630</v>
-      </c>
-      <c r="B171" s="2" t="s">
-        <v>631</v>
-      </c>
-      <c r="C171" s="2" t="s">
-        <v>632</v>
-      </c>
+      <c r="B171" s="2"/>
+      <c r="C171" s="2"/>
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A172" s="1" t="s">
@@ -5188,19 +5200,19 @@
       </c>
     </row>
     <row r="176" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B176" s="2"/>
-      <c r="C176" s="2"/>
+      <c r="A176" s="1" t="s">
+        <v>645</v>
+      </c>
+      <c r="B176" s="2" t="s">
+        <v>646</v>
+      </c>
+      <c r="C176" s="2" t="s">
+        <v>647</v>
+      </c>
     </row>
     <row r="177" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A177" s="1" t="s">
-        <v>645</v>
-      </c>
-      <c r="B177" s="2" t="s">
-        <v>646</v>
-      </c>
-      <c r="C177" s="2" t="s">
-        <v>647</v>
-      </c>
+      <c r="B177" s="2"/>
+      <c r="C177" s="2"/>
     </row>
     <row r="178" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A178" s="1" t="s">
@@ -5268,14 +5280,14 @@
         <v>665</v>
       </c>
     </row>
-    <row r="185" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A185" s="1" t="s">
+    <row r="184" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A184" s="1" t="s">
         <v>666</v>
       </c>
-      <c r="B185" s="1" t="s">
+      <c r="B184" s="2" t="s">
         <v>667</v>
       </c>
-      <c r="C185" s="1" t="s">
+      <c r="C184" s="2" t="s">
         <v>668</v>
       </c>
     </row>
@@ -5316,10 +5328,10 @@
       <c r="A189" s="1" t="s">
         <v>678</v>
       </c>
-      <c r="B189" s="2" t="s">
+      <c r="B189" s="1" t="s">
         <v>679</v>
       </c>
-      <c r="C189" s="2" t="s">
+      <c r="C189" s="1" t="s">
         <v>680</v>
       </c>
     </row>
@@ -5327,10 +5339,10 @@
       <c r="A190" s="1" t="s">
         <v>681</v>
       </c>
-      <c r="B190" s="1" t="s">
+      <c r="B190" s="2" t="s">
         <v>682</v>
       </c>
-      <c r="C190" s="1" t="s">
+      <c r="C190" s="2" t="s">
         <v>683</v>
       </c>
     </row>
@@ -5349,10 +5361,10 @@
       <c r="A192" s="1" t="s">
         <v>687</v>
       </c>
-      <c r="B192" s="2" t="s">
+      <c r="B192" s="1" t="s">
         <v>688</v>
       </c>
-      <c r="C192" s="2" t="s">
+      <c r="C192" s="1" t="s">
         <v>689</v>
       </c>
     </row>
@@ -5361,10 +5373,21 @@
         <v>690</v>
       </c>
       <c r="B193" s="2" t="s">
-        <v>664</v>
+        <v>691</v>
       </c>
       <c r="C193" s="2" t="s">
-        <v>665</v>
+        <v>692</v>
+      </c>
+    </row>
+    <row r="194" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A194" s="1" t="s">
+        <v>693</v>
+      </c>
+      <c r="B194" s="2" t="s">
+        <v>667</v>
+      </c>
+      <c r="C194" s="2" t="s">
+        <v>668</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Cache and reuse data about Processes
</commit_message>
<xml_diff>
--- a/Config.xlsx
+++ b/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mateus.cruz\Documents\GitHub\OrchestratorManager\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AA0F309-B94B-4654-8303-E49B6DC0AD33}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2C34ACB-4CA0-4A00-BF73-EC25349D249B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="745" uniqueCount="695">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="748" uniqueCount="698">
   <si>
     <t>Name</t>
   </si>
@@ -56,17 +56,11 @@
     <t>CloudTenantName</t>
   </si>
   <si>
-    <t>Default</t>
-  </si>
-  <si>
     <t>Name of the tenant to be used in case of Automation Cloud Orchestrator instances. 
 Sample value: Default.</t>
   </si>
   <si>
     <t>CloudAccountName</t>
-  </si>
-  <si>
-    <t>SampleAccount</t>
   </si>
   <si>
     <t>Unique site URL for Automation Cloud organization.
@@ -77,11 +71,17 @@
     <t>OnPremisesTenantName</t>
   </si>
   <si>
+    <t>Default</t>
+  </si>
+  <si>
     <t>Name of the tenant to be used in case of on-premises Orchestrator instances. 
 Sample value: Default.</t>
   </si>
   <si>
     <t>OnPremisesOrchestratorURL</t>
+  </si>
+  <si>
+    <t>https://myOrchestratorURL</t>
   </si>
   <si>
     <t>URL of the Orchestrator instance to be used. 
@@ -2025,6 +2025,15 @@
     <t>プロセス {0} が見つかりません。</t>
   </si>
   <si>
+    <t>ProcessNameAlreadyUsed</t>
+  </si>
+  <si>
+    <t>The Process name {0} is already used.</t>
+  </si>
+  <si>
+    <t>プロセス名 {0} は既に使用されています。</t>
+  </si>
+  <si>
     <t>PackageNameNotSpecified</t>
   </si>
   <si>
@@ -2163,7 +2172,7 @@
     <t>QueueItemsDownloadPathNotSpecified</t>
   </si>
   <si>
-    <t>https://myOrchestratorURL</t>
+    <t>SampleAccount</t>
   </si>
 </sst>
 </file>
@@ -2256,8 +2265,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table13" displayName="Table13" ref="A1:C194" totalsRowShown="0">
-  <autoFilter ref="A1:C194" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table13" displayName="Table13" ref="A1:C195" totalsRowShown="0">
+  <autoFilter ref="A1:C195" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Name"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="EN"/>
@@ -2567,40 +2576,40 @@
         <v>5</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>6</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="72.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>697</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>8</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="58" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>11</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="58" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>13</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>694</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>14</v>
@@ -3119,7 +3128,7 @@
         <v>118</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>63</v>
+        <v>76</v>
       </c>
       <c r="C44" s="2" t="s">
         <v>119</v>
@@ -3130,7 +3139,7 @@
         <v>120</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>76</v>
+        <v>96</v>
       </c>
       <c r="C45" s="2" t="s">
         <v>121</v>
@@ -3349,7 +3358,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1927ABA9-1814-4487-9CEC-ABDCAF91481F}">
-  <dimension ref="A1:C194"/>
+  <dimension ref="A1:C195"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2 A2"/>
@@ -4754,6 +4763,7 @@
       </c>
     </row>
     <row r="130" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A130"/>
       <c r="B130" s="2"/>
       <c r="C130" s="2"/>
     </row>
@@ -5036,11 +5046,7 @@
         <v>602</v>
       </c>
     </row>
-    <row r="159" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A159"/>
-      <c r="B159"/>
-      <c r="C159"/>
-    </row>
+    <row r="159" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="160" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A160" s="1" t="s">
         <v>603</v>
@@ -5211,19 +5217,19 @@
       </c>
     </row>
     <row r="177" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B177" s="2"/>
-      <c r="C177" s="2"/>
+      <c r="A177" s="1" t="s">
+        <v>648</v>
+      </c>
+      <c r="B177" s="2" t="s">
+        <v>649</v>
+      </c>
+      <c r="C177" s="2" t="s">
+        <v>650</v>
+      </c>
     </row>
     <row r="178" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A178" s="1" t="s">
-        <v>648</v>
-      </c>
-      <c r="B178" s="2" t="s">
-        <v>649</v>
-      </c>
-      <c r="C178" s="2" t="s">
-        <v>650</v>
-      </c>
+      <c r="B178" s="2"/>
+      <c r="C178" s="2"/>
     </row>
     <row r="179" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A179" s="1" t="s">
@@ -5291,14 +5297,14 @@
         <v>668</v>
       </c>
     </row>
-    <row r="186" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A186" s="1" t="s">
+    <row r="185" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A185" s="1" t="s">
         <v>669</v>
       </c>
-      <c r="B186" s="1" t="s">
+      <c r="B185" s="2" t="s">
         <v>670</v>
       </c>
-      <c r="C186" s="1" t="s">
+      <c r="C185" s="2" t="s">
         <v>671</v>
       </c>
     </row>
@@ -5339,10 +5345,10 @@
       <c r="A190" s="1" t="s">
         <v>681</v>
       </c>
-      <c r="B190" s="2" t="s">
+      <c r="B190" s="1" t="s">
         <v>682</v>
       </c>
-      <c r="C190" s="2" t="s">
+      <c r="C190" s="1" t="s">
         <v>683</v>
       </c>
     </row>
@@ -5350,10 +5356,10 @@
       <c r="A191" s="1" t="s">
         <v>684</v>
       </c>
-      <c r="B191" s="1" t="s">
+      <c r="B191" s="2" t="s">
         <v>685</v>
       </c>
-      <c r="C191" s="1" t="s">
+      <c r="C191" s="2" t="s">
         <v>686</v>
       </c>
     </row>
@@ -5372,10 +5378,10 @@
       <c r="A193" s="1" t="s">
         <v>690</v>
       </c>
-      <c r="B193" s="2" t="s">
+      <c r="B193" s="1" t="s">
         <v>691</v>
       </c>
-      <c r="C193" s="2" t="s">
+      <c r="C193" s="1" t="s">
         <v>692</v>
       </c>
     </row>
@@ -5384,10 +5390,21 @@
         <v>693</v>
       </c>
       <c r="B194" s="2" t="s">
-        <v>667</v>
+        <v>694</v>
       </c>
       <c r="C194" s="2" t="s">
-        <v>668</v>
+        <v>695</v>
+      </c>
+    </row>
+    <row r="195" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A195" s="1" t="s">
+        <v>696</v>
+      </c>
+      <c r="B195" s="2" t="s">
+        <v>670</v>
+      </c>
+      <c r="C195" s="2" t="s">
+        <v>671</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Cache and reuse data about Assets
</commit_message>
<xml_diff>
--- a/Config.xlsx
+++ b/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mateus.cruz\Documents\GitHub\OrchestratorManager\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2C34ACB-4CA0-4A00-BF73-EC25349D249B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACE6078D-980B-4878-A5F1-3BADD237D72F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="748" uniqueCount="698">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="751" uniqueCount="701">
   <si>
     <t>Name</t>
   </si>
@@ -56,11 +56,17 @@
     <t>CloudTenantName</t>
   </si>
   <si>
+    <t>Default</t>
+  </si>
+  <si>
     <t>Name of the tenant to be used in case of Automation Cloud Orchestrator instances. 
 Sample value: Default.</t>
   </si>
   <si>
     <t>CloudAccountName</t>
+  </si>
+  <si>
+    <t>SampleAccount</t>
   </si>
   <si>
     <t>Unique site URL for Automation Cloud organization.
@@ -71,17 +77,11 @@
     <t>OnPremisesTenantName</t>
   </si>
   <si>
-    <t>Default</t>
-  </si>
-  <si>
     <t>Name of the tenant to be used in case of on-premises Orchestrator instances. 
 Sample value: Default.</t>
   </si>
   <si>
     <t>OnPremisesOrchestratorURL</t>
-  </si>
-  <si>
-    <t>https://myOrchestratorURL</t>
   </si>
   <si>
     <t>URL of the Orchestrator instance to be used. 
@@ -1569,6 +1569,15 @@
     <t>パスワードが指定されていません。</t>
   </si>
   <si>
+    <t>AssetNameAlreadyUsed</t>
+  </si>
+  <si>
+    <t>The Asset name {0} is already used.</t>
+  </si>
+  <si>
+    <t>アセット名 {0} は既に使用されています。</t>
+  </si>
+  <si>
     <t>UserNotFound</t>
   </si>
   <si>
@@ -2172,7 +2181,7 @@
     <t>QueueItemsDownloadPathNotSpecified</t>
   </si>
   <si>
-    <t>SampleAccount</t>
+    <t>https://myOrchestratorURL</t>
   </si>
 </sst>
 </file>
@@ -2265,8 +2274,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table13" displayName="Table13" ref="A1:C195" totalsRowShown="0">
-  <autoFilter ref="A1:C195" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table13" displayName="Table13" ref="A1:C196" totalsRowShown="0">
+  <autoFilter ref="A1:C196" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Name"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="EN"/>
@@ -2576,40 +2585,40 @@
         <v>5</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="72.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>697</v>
+        <v>9</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="58" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="58" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>13</v>
+        <v>700</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>14</v>
@@ -3358,7 +3367,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1927ABA9-1814-4487-9CEC-ABDCAF91481F}">
-  <dimension ref="A1:C195"/>
+  <dimension ref="A1:C196"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2 A2"/>
@@ -4649,19 +4658,19 @@
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B119" s="2"/>
-      <c r="C119" s="2"/>
+      <c r="A119" s="1" t="s">
+        <v>498</v>
+      </c>
+      <c r="B119" s="2" t="s">
+        <v>499</v>
+      </c>
+      <c r="C119" s="2" t="s">
+        <v>500</v>
+      </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A120" s="1" t="s">
-        <v>498</v>
-      </c>
-      <c r="B120" s="2" t="s">
-        <v>499</v>
-      </c>
-      <c r="C120" s="2" t="s">
-        <v>500</v>
-      </c>
+      <c r="B120" s="2"/>
+      <c r="C120" s="2"/>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A121" s="1" t="s">
@@ -4763,22 +4772,21 @@
       </c>
     </row>
     <row r="130" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A130"/>
-      <c r="B130" s="2"/>
-      <c r="C130" s="2"/>
+      <c r="A130" s="1" t="s">
+        <v>528</v>
+      </c>
+      <c r="B130" s="2" t="s">
+        <v>529</v>
+      </c>
+      <c r="C130" s="2" t="s">
+        <v>530</v>
+      </c>
     </row>
     <row r="131" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A131" s="1" t="s">
-        <v>528</v>
-      </c>
-      <c r="B131" s="2" t="s">
-        <v>529</v>
-      </c>
-      <c r="C131" s="2" t="s">
-        <v>530</v>
-      </c>
-    </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B131" s="2"/>
+      <c r="C131" s="2"/>
+    </row>
+    <row r="132" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A132" s="1" t="s">
         <v>531</v>
       </c>
@@ -4867,19 +4875,20 @@
       </c>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B140" s="2"/>
-      <c r="C140" s="2"/>
+      <c r="A140" s="1" t="s">
+        <v>555</v>
+      </c>
+      <c r="B140" s="2" t="s">
+        <v>556</v>
+      </c>
+      <c r="C140" s="2" t="s">
+        <v>557</v>
+      </c>
     </row>
     <row r="141" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A141" s="1" t="s">
-        <v>555</v>
-      </c>
-      <c r="B141" s="2" t="s">
-        <v>556</v>
-      </c>
-      <c r="C141" s="2" t="s">
-        <v>557</v>
-      </c>
+      <c r="A141"/>
+      <c r="B141" s="2"/>
+      <c r="C141" s="2"/>
     </row>
     <row r="142" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A142" s="1" t="s">
@@ -4892,7 +4901,7 @@
         <v>560</v>
       </c>
     </row>
-    <row r="143" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A143" s="1" t="s">
         <v>561</v>
       </c>
@@ -4914,14 +4923,14 @@
         <v>566</v>
       </c>
     </row>
-    <row r="146" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A146" s="1" t="s">
+    <row r="145" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A145" s="1" t="s">
         <v>567</v>
       </c>
-      <c r="B146" s="2" t="s">
+      <c r="B145" s="2" t="s">
         <v>568</v>
       </c>
-      <c r="C146" s="2" t="s">
+      <c r="C145" s="2" t="s">
         <v>569</v>
       </c>
     </row>
@@ -4991,14 +5000,14 @@
         <v>587</v>
       </c>
     </row>
-    <row r="154" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A154" s="1" t="s">
+    <row r="153" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A153" s="1" t="s">
         <v>588</v>
       </c>
-      <c r="B154" s="2" t="s">
+      <c r="B153" s="2" t="s">
         <v>589</v>
       </c>
-      <c r="C154" s="2" t="s">
+      <c r="C153" s="2" t="s">
         <v>590</v>
       </c>
     </row>
@@ -5035,7 +5044,7 @@
         <v>599</v>
       </c>
     </row>
-    <row r="158" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A158" s="1" t="s">
         <v>600</v>
       </c>
@@ -5046,17 +5055,21 @@
         <v>602</v>
       </c>
     </row>
-    <row r="159" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="159" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A159" s="1" t="s">
+        <v>603</v>
+      </c>
+      <c r="B159" s="2" t="s">
+        <v>604</v>
+      </c>
+      <c r="C159" s="2" t="s">
+        <v>605</v>
+      </c>
+    </row>
     <row r="160" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A160" s="1" t="s">
-        <v>603</v>
-      </c>
-      <c r="B160" s="2" t="s">
-        <v>604</v>
-      </c>
-      <c r="C160" s="2" t="s">
-        <v>605</v>
-      </c>
+      <c r="A160"/>
+      <c r="B160"/>
+      <c r="C160"/>
     </row>
     <row r="161" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A161" s="1" t="s">
@@ -5069,14 +5082,14 @@
         <v>608</v>
       </c>
     </row>
-    <row r="162" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A162" s="1" t="s">
         <v>609</v>
       </c>
-      <c r="B162" s="1" t="s">
+      <c r="B162" s="2" t="s">
         <v>610</v>
       </c>
-      <c r="C162" s="1" t="s">
+      <c r="C162" s="2" t="s">
         <v>611</v>
       </c>
     </row>
@@ -5084,7 +5097,7 @@
       <c r="A163" s="1" t="s">
         <v>612</v>
       </c>
-      <c r="B163" s="2" t="s">
+      <c r="B163" s="1" t="s">
         <v>613</v>
       </c>
       <c r="C163" s="1" t="s">
@@ -5095,7 +5108,7 @@
       <c r="A164" s="1" t="s">
         <v>615</v>
       </c>
-      <c r="B164" s="1" t="s">
+      <c r="B164" s="2" t="s">
         <v>616</v>
       </c>
       <c r="C164" s="1" t="s">
@@ -5106,10 +5119,10 @@
       <c r="A165" s="1" t="s">
         <v>618</v>
       </c>
-      <c r="B165" s="2" t="s">
+      <c r="B165" s="1" t="s">
         <v>619</v>
       </c>
-      <c r="C165" s="2" t="s">
+      <c r="C165" s="1" t="s">
         <v>620</v>
       </c>
     </row>
@@ -5135,14 +5148,14 @@
         <v>626</v>
       </c>
     </row>
-    <row r="169" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A169" s="1" t="s">
+    <row r="168" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A168" s="1" t="s">
         <v>627</v>
       </c>
-      <c r="B169" s="2" t="s">
+      <c r="B168" s="2" t="s">
         <v>628</v>
       </c>
-      <c r="C169" s="2" t="s">
+      <c r="C168" s="2" t="s">
         <v>629</v>
       </c>
     </row>
@@ -5158,19 +5171,19 @@
       </c>
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B171" s="2"/>
-      <c r="C171" s="2"/>
+      <c r="A171" s="1" t="s">
+        <v>633</v>
+      </c>
+      <c r="B171" s="2" t="s">
+        <v>634</v>
+      </c>
+      <c r="C171" s="2" t="s">
+        <v>635</v>
+      </c>
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A172" s="1" t="s">
-        <v>633</v>
-      </c>
-      <c r="B172" s="2" t="s">
-        <v>634</v>
-      </c>
-      <c r="C172" s="2" t="s">
-        <v>635</v>
-      </c>
+      <c r="B172" s="2"/>
+      <c r="C172" s="2"/>
     </row>
     <row r="173" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A173" s="1" t="s">
@@ -5228,19 +5241,19 @@
       </c>
     </row>
     <row r="178" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B178" s="2"/>
-      <c r="C178" s="2"/>
+      <c r="A178" s="1" t="s">
+        <v>651</v>
+      </c>
+      <c r="B178" s="2" t="s">
+        <v>652</v>
+      </c>
+      <c r="C178" s="2" t="s">
+        <v>653</v>
+      </c>
     </row>
     <row r="179" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A179" s="1" t="s">
-        <v>651</v>
-      </c>
-      <c r="B179" s="2" t="s">
-        <v>652</v>
-      </c>
-      <c r="C179" s="2" t="s">
-        <v>653</v>
-      </c>
+      <c r="B179" s="2"/>
+      <c r="C179" s="2"/>
     </row>
     <row r="180" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A180" s="1" t="s">
@@ -5308,14 +5321,14 @@
         <v>671</v>
       </c>
     </row>
-    <row r="187" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A187" s="1" t="s">
+    <row r="186" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A186" s="1" t="s">
         <v>672</v>
       </c>
-      <c r="B187" s="1" t="s">
+      <c r="B186" s="2" t="s">
         <v>673</v>
       </c>
-      <c r="C187" s="1" t="s">
+      <c r="C186" s="2" t="s">
         <v>674</v>
       </c>
     </row>
@@ -5356,10 +5369,10 @@
       <c r="A191" s="1" t="s">
         <v>684</v>
       </c>
-      <c r="B191" s="2" t="s">
+      <c r="B191" s="1" t="s">
         <v>685</v>
       </c>
-      <c r="C191" s="2" t="s">
+      <c r="C191" s="1" t="s">
         <v>686</v>
       </c>
     </row>
@@ -5367,10 +5380,10 @@
       <c r="A192" s="1" t="s">
         <v>687</v>
       </c>
-      <c r="B192" s="1" t="s">
+      <c r="B192" s="2" t="s">
         <v>688</v>
       </c>
-      <c r="C192" s="1" t="s">
+      <c r="C192" s="2" t="s">
         <v>689</v>
       </c>
     </row>
@@ -5389,10 +5402,10 @@
       <c r="A194" s="1" t="s">
         <v>693</v>
       </c>
-      <c r="B194" s="2" t="s">
+      <c r="B194" s="1" t="s">
         <v>694</v>
       </c>
-      <c r="C194" s="2" t="s">
+      <c r="C194" s="1" t="s">
         <v>695</v>
       </c>
     </row>
@@ -5401,10 +5414,21 @@
         <v>696</v>
       </c>
       <c r="B195" s="2" t="s">
-        <v>670</v>
+        <v>697</v>
       </c>
       <c r="C195" s="2" t="s">
-        <v>671</v>
+        <v>698</v>
+      </c>
+    </row>
+    <row r="196" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A196" s="1" t="s">
+        <v>699</v>
+      </c>
+      <c r="B196" s="2" t="s">
+        <v>673</v>
+      </c>
+      <c r="C196" s="2" t="s">
+        <v>674</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Standardize workflows according to Workflow Inspector
</commit_message>
<xml_diff>
--- a/Config.xlsx
+++ b/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mateus.cruz\Documents\GitHub\OrchestratorManager\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACE6078D-980B-4878-A5F1-3BADD237D72F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4050A898-B32D-47FA-BB84-80A6E72DE61F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3370,7 +3370,7 @@
   <dimension ref="A1:C196"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2 A2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Refactor workflows to Get entities
</commit_message>
<xml_diff>
--- a/Config.xlsx
+++ b/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mateus.cruz\Documents\GitHub\OrchestratorManager\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4050A898-B32D-47FA-BB84-80A6E72DE61F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F896031D-8DC0-4518-8D6B-3362DA540C32}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -56,17 +56,11 @@
     <t>CloudTenantName</t>
   </si>
   <si>
-    <t>Default</t>
-  </si>
-  <si>
     <t>Name of the tenant to be used in case of Automation Cloud Orchestrator instances. 
 Sample value: Default.</t>
   </si>
   <si>
     <t>CloudAccountName</t>
-  </si>
-  <si>
-    <t>SampleAccount</t>
   </si>
   <si>
     <t>Unique site URL for Automation Cloud organization.
@@ -77,11 +71,17 @@
     <t>OnPremisesTenantName</t>
   </si>
   <si>
+    <t>Default</t>
+  </si>
+  <si>
     <t>Name of the tenant to be used in case of on-premises Orchestrator instances. 
 Sample value: Default.</t>
   </si>
   <si>
     <t>OnPremisesOrchestratorURL</t>
+  </si>
+  <si>
+    <t>https://myOrchestratorURL</t>
   </si>
   <si>
     <t>URL of the Orchestrator instance to be used. 
@@ -2181,7 +2181,7 @@
     <t>QueueItemsDownloadPathNotSpecified</t>
   </si>
   <si>
-    <t>https://myOrchestratorURL</t>
+    <t>SamplesAccount</t>
   </si>
 </sst>
 </file>
@@ -2585,40 +2585,40 @@
         <v>5</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>6</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="72.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>700</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>8</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="58" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>11</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="58" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>13</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>700</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>14</v>
@@ -3370,7 +3370,7 @@
   <dimension ref="A1:C196"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A2" sqref="A2 A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4783,6 +4783,7 @@
       </c>
     </row>
     <row r="131" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A131"/>
       <c r="B131" s="2"/>
       <c r="C131" s="2"/>
     </row>
@@ -4886,7 +4887,6 @@
       </c>
     </row>
     <row r="141" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A141"/>
       <c r="B141" s="2"/>
       <c r="C141" s="2"/>
     </row>
@@ -5066,11 +5066,7 @@
         <v>605</v>
       </c>
     </row>
-    <row r="160" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A160"/>
-      <c r="B160"/>
-      <c r="C160"/>
-    </row>
+    <row r="160" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="161" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A161" s="1" t="s">
         <v>606</v>

</xml_diff>

<commit_message>
Remember last Orchestrator type used
</commit_message>
<xml_diff>
--- a/Config.xlsx
+++ b/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mateus.cruz\Documents\GitHub\OrchestratorManager\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F896031D-8DC0-4518-8D6B-3362DA540C32}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F47919F0-DF24-4102-BECE-A29AFE2B5DE0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="751" uniqueCount="701">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="757" uniqueCount="707">
   <si>
     <t>Name</t>
   </si>
@@ -79,9 +79,6 @@
   </si>
   <si>
     <t>OnPremisesOrchestratorURL</t>
-  </si>
-  <si>
-    <t>https://myOrchestratorURL</t>
   </si>
   <si>
     <t>URL of the Orchestrator instance to be used. 
@@ -238,6 +235,18 @@
     <t>Name of credential in Windows Credential Manager to store on-premises Orchestrator administrator's credential (Username and Password).</t>
   </si>
   <si>
+    <t>OrchestratorType</t>
+  </si>
+  <si>
+    <t>cloud</t>
+  </si>
+  <si>
+    <t>Type of the last used Orchestrator instance. This parameter is used to display the correct Authentication Panel form according to the last used type.
+Possible values:
+cloud
+onPremises</t>
+  </si>
+  <si>
     <t>CreateMachineResultColumn</t>
   </si>
   <si>
@@ -1181,6 +1190,15 @@
   </si>
   <si>
     <t>指定した Orchestrator のバージョンはサポートされていません。</t>
+  </si>
+  <si>
+    <t>OrchestratorTypeNotSupported</t>
+  </si>
+  <si>
+    <t>The specified Orchestrator configuration is not supported.</t>
+  </si>
+  <si>
+    <t>指定した Orchestrator の構成はサポートされていません。</t>
   </si>
   <si>
     <t>TokenNotRetrieved</t>
@@ -2181,7 +2199,10 @@
     <t>QueueItemsDownloadPathNotSpecified</t>
   </si>
   <si>
-    <t>SamplesAccount</t>
+    <t>SampleAccount</t>
+  </si>
+  <si>
+    <t>https://myOrchestratorURL</t>
   </si>
 </sst>
 </file>
@@ -2262,8 +2283,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table1" displayName="Table1" ref="A1:C63" totalsRowShown="0">
-  <autoFilter ref="A1:C63" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table1" displayName="Table1" ref="A1:C64" totalsRowShown="0">
+  <autoFilter ref="A1:C64" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Name"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Value"/>
@@ -2274,8 +2295,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table13" displayName="Table13" ref="A1:C196" totalsRowShown="0">
-  <autoFilter ref="A1:C196" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table13" displayName="Table13" ref="A1:C197" totalsRowShown="0">
+  <autoFilter ref="A1:C197" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Name"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="EN"/>
@@ -2596,7 +2617,7 @@
         <v>7</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>700</v>
+        <v>705</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>8</v>
@@ -2618,21 +2639,21 @@
         <v>12</v>
       </c>
       <c r="B6" s="3" t="s">
+        <v>706</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>13</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="159.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B7" s="1">
         <v>201804</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -2646,10 +2667,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C63"/>
+  <dimension ref="A1:C64"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2 A2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2672,230 +2693,230 @@
     </row>
     <row r="2" spans="1:3" ht="101.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B2" s="1">
         <v>200</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B3" s="1">
         <v>0</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B4" s="1">
         <v>550</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B5" s="1">
         <v>650</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B6" s="1">
         <v>3</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B7" s="1">
         <v>5000</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="C8" s="2" t="s">
         <v>30</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B9" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="C9" s="2" t="s">
         <v>33</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="C10" s="2" t="s">
         <v>36</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="C11" s="2" t="s">
         <v>39</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="C12" s="2" t="s">
         <v>42</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="C13" s="2" t="s">
         <v>45</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="C14" s="2" t="s">
         <v>48</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B15" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="C15" s="2" t="s">
         <v>51</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B16" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="C16" s="2" t="s">
         <v>54</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B17" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="C17" s="2" t="s">
         <v>57</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B18" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="C18" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="C18" s="2" t="s">
+    </row>
+    <row r="19" spans="1:3" ht="87" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="1" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="1" t="s">
+      <c r="B19" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="C19" s="2" t="s">
         <v>63</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B20" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="C20" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="C20" s="2" t="s">
+    </row>
+    <row r="21" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="1" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A21" s="1" t="s">
+      <c r="B21" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="C21" s="2" t="s">
         <v>69</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B22" s="1" t="s">
         <v>71</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>66</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>72</v>
@@ -2906,62 +2927,62 @@
         <v>73</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
         <v>75</v>
       </c>
       <c r="B24" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C24" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="C24" s="2" t="s">
+    </row>
+    <row r="25" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="1" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A25" s="1" t="s">
+      <c r="B25" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="B25" s="1" t="s">
-        <v>63</v>
-      </c>
       <c r="C25" s="2" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B26" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C26" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="C26" s="2" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
+    </row>
+    <row r="27" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
         <v>81</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>63</v>
+        <v>78</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="s">
         <v>83</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>84</v>
@@ -2972,95 +2993,95 @@
         <v>85</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>63</v>
+        <v>78</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="1" t="s">
         <v>87</v>
       </c>
       <c r="B30" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C30" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="C30" s="2" t="s">
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A31" s="1" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="1" t="s">
+      <c r="B31" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="B31" s="1" t="s">
+      <c r="C31" s="2" t="s">
         <v>91</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B32" s="1" t="s">
         <v>93</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>66</v>
       </c>
       <c r="C32" s="2" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" s="1" t="s">
         <v>95</v>
       </c>
       <c r="B33" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C33" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="C33" s="2" t="s">
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A34" s="1" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="1" t="s">
+      <c r="B34" s="1" t="s">
         <v>98</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>63</v>
       </c>
       <c r="C34" s="2" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A35" s="1" t="s">
         <v>100</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>88</v>
+        <v>65</v>
       </c>
       <c r="C35" s="2" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A36" s="1" t="s">
         <v>102</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C36" s="2" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A37" s="1" t="s">
         <v>104</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="C37" s="2" t="s">
         <v>105</v>
@@ -3071,18 +3092,18 @@
         <v>106</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>66</v>
+        <v>90</v>
       </c>
       <c r="C38" s="2" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A39" s="1" t="s">
         <v>108</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C39" s="2" t="s">
         <v>109</v>
@@ -3093,7 +3114,7 @@
         <v>110</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>63</v>
+        <v>71</v>
       </c>
       <c r="C40" s="2" t="s">
         <v>111</v>
@@ -3104,7 +3125,7 @@
         <v>112</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="C41" s="2" t="s">
         <v>113</v>
@@ -3115,7 +3136,7 @@
         <v>114</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="C42" s="2" t="s">
         <v>115</v>
@@ -3126,29 +3147,29 @@
         <v>116</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="C43" s="2" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A44" s="1" t="s">
         <v>118</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="C44" s="2" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="45" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A45" s="1" t="s">
         <v>120</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>96</v>
+        <v>78</v>
       </c>
       <c r="C45" s="2" t="s">
         <v>121</v>
@@ -3159,7 +3180,7 @@
         <v>122</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>63</v>
+        <v>98</v>
       </c>
       <c r="C46" s="2" t="s">
         <v>123</v>
@@ -3170,7 +3191,7 @@
         <v>124</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C47" s="2" t="s">
         <v>125</v>
@@ -3181,29 +3202,29 @@
         <v>126</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="C48" s="2" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A49" s="1" t="s">
         <v>128</v>
       </c>
       <c r="B49" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C49" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="C49" s="2" t="s">
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A50" s="1" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="50" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A50" s="1" t="s">
+      <c r="B50" s="1" t="s">
         <v>131</v>
-      </c>
-      <c r="B50" s="1" t="s">
-        <v>66</v>
       </c>
       <c r="C50" s="2" t="s">
         <v>132</v>
@@ -3214,29 +3235,29 @@
         <v>133</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="C51" s="2" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A52" s="1" t="s">
         <v>135</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="C52" s="2" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="53" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A53" s="1" t="s">
         <v>137</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
       <c r="C53" s="2" t="s">
         <v>138</v>
@@ -3247,29 +3268,29 @@
         <v>139</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>66</v>
+        <v>78</v>
       </c>
       <c r="C54" s="2" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A55" s="1" t="s">
         <v>141</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>96</v>
+        <v>68</v>
       </c>
       <c r="C55" s="2" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="56" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A56" s="1" t="s">
         <v>143</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>88</v>
+        <v>98</v>
       </c>
       <c r="C56" s="2" t="s">
         <v>144</v>
@@ -3280,7 +3301,7 @@
         <v>145</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>63</v>
+        <v>90</v>
       </c>
       <c r="C57" s="2" t="s">
         <v>146</v>
@@ -3291,7 +3312,7 @@
         <v>147</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="C58" s="2" t="s">
         <v>148</v>
@@ -3302,7 +3323,7 @@
         <v>149</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>63</v>
+        <v>71</v>
       </c>
       <c r="C59" s="2" t="s">
         <v>150</v>
@@ -3313,7 +3334,7 @@
         <v>151</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="C60" s="2" t="s">
         <v>152</v>
@@ -3324,7 +3345,7 @@
         <v>153</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="C61" s="2" t="s">
         <v>154</v>
@@ -3335,7 +3356,7 @@
         <v>155</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>63</v>
+        <v>71</v>
       </c>
       <c r="C62" s="2" t="s">
         <v>156</v>
@@ -3346,10 +3367,21 @@
         <v>157</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>129</v>
+        <v>65</v>
       </c>
       <c r="C63" s="2" t="s">
         <v>158</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A64" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="C64" s="2" t="s">
+        <v>160</v>
       </c>
     </row>
   </sheetData>
@@ -3367,10 +3399,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1927ABA9-1814-4487-9CEC-ABDCAF91481F}">
-  <dimension ref="A1:C196"/>
+  <dimension ref="A1:C197"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2 A2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3385,472 +3417,472 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="43.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A30" s="1" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A31" s="1" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A32" s="1" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A33" s="1" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A34" s="1" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A35" s="1" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A36" s="1" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A37" s="1" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A38" s="1" t="s">
-        <v>264</v>
+        <v>266</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>265</v>
+        <v>267</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>266</v>
+        <v>268</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A39" s="1" t="s">
-        <v>267</v>
+        <v>269</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>269</v>
+        <v>271</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="43.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A40" s="1" t="s">
-        <v>270</v>
+        <v>272</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
     </row>
     <row r="41" spans="1:3" ht="43.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A41" s="1" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>275</v>
+        <v>277</v>
       </c>
     </row>
     <row r="42" spans="1:3" ht="58" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A42" s="1" t="s">
-        <v>276</v>
+        <v>278</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A43" s="1" t="s">
-        <v>279</v>
+        <v>281</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>280</v>
+        <v>282</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>281</v>
+        <v>283</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.35">
@@ -3859,112 +3891,112 @@
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A45" s="1" t="s">
-        <v>282</v>
+        <v>284</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>283</v>
+        <v>285</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>284</v>
+        <v>286</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A46" s="1" t="s">
-        <v>285</v>
+        <v>287</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>286</v>
+        <v>288</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>287</v>
+        <v>289</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A47" s="1" t="s">
-        <v>288</v>
+        <v>290</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>289</v>
+        <v>291</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>290</v>
+        <v>292</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A48" s="1" t="s">
-        <v>291</v>
+        <v>293</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>292</v>
+        <v>294</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>293</v>
+        <v>295</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A49" s="1" t="s">
-        <v>294</v>
+        <v>296</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>295</v>
+        <v>297</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A50" s="1" t="s">
-        <v>297</v>
+        <v>299</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>298</v>
+        <v>300</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>299</v>
+        <v>301</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A51" s="1" t="s">
-        <v>300</v>
+        <v>302</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>301</v>
+        <v>303</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A52" s="1" t="s">
-        <v>303</v>
+        <v>305</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>304</v>
+        <v>306</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>305</v>
+        <v>307</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A53" s="1" t="s">
-        <v>306</v>
+        <v>308</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>307</v>
+        <v>309</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>308</v>
+        <v>310</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A54" s="1" t="s">
-        <v>309</v>
+        <v>311</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>310</v>
+        <v>312</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>311</v>
+        <v>313</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.35">
@@ -3973,1458 +4005,1473 @@
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A56" s="1" t="s">
-        <v>312</v>
+        <v>314</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>313</v>
+        <v>315</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>314</v>
+        <v>316</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A57" s="1" t="s">
-        <v>315</v>
+        <v>317</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>317</v>
+        <v>319</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A58" s="1" t="s">
-        <v>318</v>
+        <v>320</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>319</v>
+        <v>321</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>320</v>
+        <v>322</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A59" s="1" t="s">
-        <v>321</v>
+        <v>323</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>322</v>
+        <v>324</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>323</v>
+        <v>325</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A60" s="1" t="s">
-        <v>324</v>
+        <v>326</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>325</v>
+        <v>327</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>326</v>
+        <v>328</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A61" s="1" t="s">
-        <v>327</v>
+        <v>329</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>328</v>
+        <v>330</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>329</v>
+        <v>331</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A62" s="1" t="s">
-        <v>330</v>
+        <v>332</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>331</v>
+        <v>333</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>332</v>
+        <v>334</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A63" s="1" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>335</v>
+        <v>337</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A64" s="1" t="s">
-        <v>336</v>
+        <v>338</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>337</v>
+        <v>339</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>338</v>
+        <v>340</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A65" s="1" t="s">
-        <v>339</v>
+        <v>341</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>340</v>
+        <v>342</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>341</v>
+        <v>343</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A66" s="1" t="s">
-        <v>342</v>
+        <v>344</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>343</v>
+        <v>345</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>344</v>
+        <v>346</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A67" s="1" t="s">
-        <v>345</v>
+        <v>347</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>346</v>
+        <v>348</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>347</v>
+        <v>349</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A68" s="1" t="s">
-        <v>348</v>
+        <v>350</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>349</v>
+        <v>351</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>350</v>
+        <v>352</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A69" s="1" t="s">
-        <v>351</v>
+        <v>353</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>352</v>
+        <v>354</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>353</v>
+        <v>355</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A70" s="1" t="s">
-        <v>354</v>
+        <v>356</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>355</v>
+        <v>357</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>356</v>
+        <v>358</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A71" s="1" t="s">
-        <v>357</v>
+        <v>359</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>358</v>
+        <v>360</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>359</v>
+        <v>361</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A72" s="1" t="s">
-        <v>360</v>
+        <v>362</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>361</v>
+        <v>363</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>362</v>
+        <v>364</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A73" s="1" t="s">
-        <v>363</v>
+        <v>365</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>364</v>
+        <v>366</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>365</v>
+        <v>367</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A74" s="1" t="s">
-        <v>366</v>
+        <v>368</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>367</v>
+        <v>369</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>368</v>
+        <v>370</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A75" s="1" t="s">
-        <v>369</v>
+        <v>371</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>370</v>
+        <v>372</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>371</v>
+        <v>373</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A76" s="1" t="s">
-        <v>372</v>
+        <v>374</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>373</v>
+        <v>375</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>374</v>
-      </c>
-    </row>
-    <row r="77" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A77" s="1" t="s">
-        <v>375</v>
+        <v>377</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>376</v>
+        <v>378</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>377</v>
-      </c>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.35">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A78" s="1" t="s">
-        <v>378</v>
+        <v>380</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>379</v>
+        <v>381</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>380</v>
+        <v>382</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A79" s="1" t="s">
-        <v>381</v>
+        <v>383</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>382</v>
+        <v>384</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>383</v>
-      </c>
-    </row>
-    <row r="80" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A80" s="1" t="s">
-        <v>384</v>
+        <v>386</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>385</v>
+        <v>387</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>386</v>
-      </c>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.35">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A81" s="1" t="s">
-        <v>387</v>
+        <v>389</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>388</v>
+        <v>390</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>389</v>
+        <v>391</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A82" s="1" t="s">
-        <v>390</v>
+        <v>392</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>391</v>
+        <v>393</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>392</v>
+        <v>394</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A83" s="1" t="s">
-        <v>393</v>
+        <v>395</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>395</v>
+        <v>397</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A84" s="1" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>397</v>
+        <v>399</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>398</v>
-      </c>
-    </row>
-    <row r="85" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A85" s="1" t="s">
-        <v>399</v>
+        <v>401</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>400</v>
+        <v>402</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>401</v>
+        <v>403</v>
       </c>
     </row>
     <row r="86" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A86" s="1" t="s">
-        <v>402</v>
+        <v>404</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>403</v>
+        <v>405</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="87" spans="1:3" ht="43.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A87" s="1" t="s">
-        <v>405</v>
+        <v>407</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>406</v>
+        <v>408</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>407</v>
-      </c>
-    </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.35">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" ht="43.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A88" s="1" t="s">
-        <v>408</v>
+        <v>410</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>409</v>
+        <v>411</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>410</v>
+        <v>412</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A89" s="1" t="s">
-        <v>411</v>
+        <v>413</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>412</v>
+        <v>414</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>413</v>
-      </c>
-    </row>
-    <row r="90" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A90" s="1" t="s">
-        <v>414</v>
+        <v>416</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>415</v>
+        <v>417</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.35">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A91" s="1" t="s">
-        <v>417</v>
+        <v>419</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>418</v>
+        <v>420</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>419</v>
+        <v>421</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A92" s="1" t="s">
-        <v>420</v>
+        <v>422</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>421</v>
+        <v>423</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>422</v>
+        <v>424</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A93" s="1" t="s">
-        <v>423</v>
+        <v>425</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>424</v>
+        <v>426</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>425</v>
+        <v>427</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A94" s="1" t="s">
-        <v>426</v>
+        <v>428</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>427</v>
+        <v>429</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>428</v>
+        <v>430</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A95" s="1" t="s">
-        <v>429</v>
+        <v>431</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>430</v>
+        <v>432</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>431</v>
+        <v>433</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A96" s="1" t="s">
-        <v>432</v>
+        <v>434</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>433</v>
+        <v>435</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>434</v>
+        <v>436</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A97" s="1" t="s">
-        <v>435</v>
+        <v>437</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>436</v>
+        <v>438</v>
       </c>
       <c r="C97" s="2" t="s">
-        <v>437</v>
+        <v>439</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A98" s="1" t="s">
-        <v>438</v>
+        <v>440</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>439</v>
+        <v>441</v>
       </c>
       <c r="C98" s="2" t="s">
-        <v>440</v>
+        <v>442</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A99" s="1" t="s">
-        <v>441</v>
+        <v>443</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>442</v>
+        <v>444</v>
       </c>
       <c r="C99" s="2" t="s">
-        <v>443</v>
+        <v>445</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A100" s="1" t="s">
-        <v>444</v>
+        <v>446</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>445</v>
+        <v>447</v>
       </c>
       <c r="C100" s="2" t="s">
-        <v>446</v>
+        <v>448</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A101" s="1" t="s">
-        <v>447</v>
+        <v>449</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>448</v>
+        <v>450</v>
       </c>
       <c r="C101" s="2" t="s">
-        <v>449</v>
+        <v>451</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A102" s="1" t="s">
-        <v>450</v>
+        <v>452</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>451</v>
+        <v>453</v>
       </c>
       <c r="C102" s="2" t="s">
-        <v>452</v>
+        <v>454</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A103" s="1" t="s">
-        <v>453</v>
+        <v>455</v>
       </c>
       <c r="B103" s="2" t="s">
-        <v>454</v>
+        <v>456</v>
       </c>
       <c r="C103" s="2" t="s">
-        <v>455</v>
+        <v>457</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A104" s="1" t="s">
-        <v>456</v>
+        <v>458</v>
       </c>
       <c r="B104" s="2" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
       <c r="C104" s="2" t="s">
-        <v>458</v>
-      </c>
-    </row>
-    <row r="105" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A105" s="1" t="s">
-        <v>459</v>
+        <v>461</v>
       </c>
       <c r="B105" s="2" t="s">
-        <v>460</v>
+        <v>462</v>
       </c>
       <c r="C105" s="2" t="s">
-        <v>461</v>
+        <v>463</v>
       </c>
     </row>
     <row r="106" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A106" s="1" t="s">
-        <v>462</v>
+        <v>464</v>
       </c>
       <c r="B106" s="2" t="s">
-        <v>463</v>
+        <v>465</v>
       </c>
       <c r="C106" s="2" t="s">
-        <v>464</v>
+        <v>466</v>
       </c>
     </row>
     <row r="107" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A107" s="1" t="s">
-        <v>465</v>
+        <v>467</v>
       </c>
       <c r="B107" s="2" t="s">
-        <v>466</v>
+        <v>468</v>
       </c>
       <c r="C107" s="2" t="s">
-        <v>467</v>
-      </c>
-    </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.35">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A108" s="1" t="s">
-        <v>468</v>
+        <v>470</v>
       </c>
       <c r="B108" s="2" t="s">
-        <v>469</v>
+        <v>471</v>
       </c>
       <c r="C108" s="2" t="s">
-        <v>470</v>
+        <v>472</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A109" s="1" t="s">
-        <v>471</v>
+        <v>473</v>
       </c>
       <c r="B109" s="2" t="s">
-        <v>472</v>
+        <v>474</v>
       </c>
       <c r="C109" s="2" t="s">
-        <v>473</v>
+        <v>475</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B110" s="2"/>
-      <c r="C110" s="2"/>
+      <c r="A110" s="1" t="s">
+        <v>476</v>
+      </c>
+      <c r="B110" s="2" t="s">
+        <v>477</v>
+      </c>
+      <c r="C110" s="2" t="s">
+        <v>478</v>
+      </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A111" s="1" t="s">
-        <v>474</v>
-      </c>
-      <c r="B111" s="2" t="s">
-        <v>475</v>
-      </c>
-      <c r="C111" s="2" t="s">
-        <v>476</v>
-      </c>
+      <c r="B111" s="2"/>
+      <c r="C111" s="2"/>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A112" s="1" t="s">
-        <v>477</v>
+        <v>479</v>
       </c>
       <c r="B112" s="2" t="s">
-        <v>478</v>
+        <v>480</v>
       </c>
       <c r="C112" s="2" t="s">
-        <v>479</v>
+        <v>481</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A113" s="1" t="s">
-        <v>480</v>
+        <v>482</v>
       </c>
       <c r="B113" s="2" t="s">
-        <v>481</v>
+        <v>483</v>
       </c>
       <c r="C113" s="2" t="s">
-        <v>482</v>
+        <v>484</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A114" s="1" t="s">
-        <v>483</v>
+        <v>485</v>
       </c>
       <c r="B114" s="2" t="s">
-        <v>484</v>
+        <v>486</v>
       </c>
       <c r="C114" s="2" t="s">
-        <v>485</v>
+        <v>487</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A115" s="1" t="s">
-        <v>486</v>
+        <v>488</v>
       </c>
       <c r="B115" s="2" t="s">
-        <v>487</v>
+        <v>489</v>
       </c>
       <c r="C115" s="2" t="s">
-        <v>488</v>
+        <v>490</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A116" s="1" t="s">
-        <v>489</v>
+        <v>491</v>
       </c>
       <c r="B116" s="2" t="s">
-        <v>490</v>
+        <v>492</v>
       </c>
       <c r="C116" s="2" t="s">
-        <v>491</v>
+        <v>493</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A117" s="1" t="s">
-        <v>492</v>
+        <v>494</v>
       </c>
       <c r="B117" s="2" t="s">
-        <v>493</v>
+        <v>495</v>
       </c>
       <c r="C117" s="2" t="s">
-        <v>494</v>
+        <v>496</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A118" s="1" t="s">
-        <v>495</v>
+        <v>497</v>
       </c>
       <c r="B118" s="2" t="s">
-        <v>496</v>
+        <v>498</v>
       </c>
       <c r="C118" s="2" t="s">
-        <v>497</v>
+        <v>499</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A119" s="1" t="s">
-        <v>498</v>
+        <v>500</v>
       </c>
       <c r="B119" s="2" t="s">
-        <v>499</v>
+        <v>501</v>
       </c>
       <c r="C119" s="2" t="s">
-        <v>500</v>
+        <v>502</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B120" s="2"/>
-      <c r="C120" s="2"/>
+      <c r="A120" s="1" t="s">
+        <v>503</v>
+      </c>
+      <c r="B120" s="2" t="s">
+        <v>504</v>
+      </c>
+      <c r="C120" s="2" t="s">
+        <v>505</v>
+      </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A121" s="1" t="s">
-        <v>501</v>
-      </c>
-      <c r="B121" s="2" t="s">
-        <v>502</v>
-      </c>
-      <c r="C121" s="2" t="s">
-        <v>503</v>
-      </c>
+      <c r="B121" s="2"/>
+      <c r="C121" s="2"/>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A122" s="1" t="s">
-        <v>504</v>
+        <v>506</v>
       </c>
       <c r="B122" s="2" t="s">
-        <v>505</v>
+        <v>507</v>
       </c>
       <c r="C122" s="2" t="s">
-        <v>506</v>
+        <v>508</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A123" s="1" t="s">
-        <v>507</v>
+        <v>509</v>
       </c>
       <c r="B123" s="2" t="s">
-        <v>508</v>
+        <v>510</v>
       </c>
       <c r="C123" s="2" t="s">
-        <v>509</v>
+        <v>511</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A124" s="1" t="s">
-        <v>510</v>
+        <v>512</v>
       </c>
       <c r="B124" s="2" t="s">
-        <v>511</v>
+        <v>513</v>
       </c>
       <c r="C124" s="2" t="s">
-        <v>512</v>
+        <v>514</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A125" s="1" t="s">
-        <v>513</v>
+        <v>515</v>
       </c>
       <c r="B125" s="2" t="s">
-        <v>514</v>
+        <v>516</v>
       </c>
       <c r="C125" s="2" t="s">
-        <v>515</v>
+        <v>517</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A126" s="1" t="s">
-        <v>516</v>
+        <v>518</v>
       </c>
       <c r="B126" s="2" t="s">
-        <v>517</v>
+        <v>519</v>
       </c>
       <c r="C126" s="2" t="s">
-        <v>518</v>
+        <v>520</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A127" s="1" t="s">
-        <v>519</v>
+        <v>521</v>
       </c>
       <c r="B127" s="2" t="s">
-        <v>520</v>
+        <v>522</v>
       </c>
       <c r="C127" s="2" t="s">
-        <v>521</v>
+        <v>523</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A128" s="1" t="s">
-        <v>522</v>
+        <v>524</v>
       </c>
       <c r="B128" s="2" t="s">
-        <v>523</v>
+        <v>525</v>
       </c>
       <c r="C128" s="2" t="s">
-        <v>524</v>
-      </c>
-    </row>
-    <row r="129" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
+        <v>526</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A129" s="1" t="s">
-        <v>525</v>
+        <v>527</v>
       </c>
       <c r="B129" s="2" t="s">
-        <v>526</v>
+        <v>528</v>
       </c>
       <c r="C129" s="2" t="s">
-        <v>527</v>
+        <v>529</v>
       </c>
     </row>
     <row r="130" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A130" s="1" t="s">
-        <v>528</v>
+        <v>530</v>
       </c>
       <c r="B130" s="2" t="s">
-        <v>529</v>
+        <v>531</v>
       </c>
       <c r="C130" s="2" t="s">
-        <v>530</v>
+        <v>532</v>
       </c>
     </row>
     <row r="131" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A131"/>
-      <c r="B131" s="2"/>
-      <c r="C131" s="2"/>
+      <c r="A131" s="1" t="s">
+        <v>533</v>
+      </c>
+      <c r="B131" s="2" t="s">
+        <v>534</v>
+      </c>
+      <c r="C131" s="2" t="s">
+        <v>535</v>
+      </c>
     </row>
     <row r="132" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A132" s="1" t="s">
-        <v>531</v>
-      </c>
-      <c r="B132" s="2" t="s">
-        <v>532</v>
-      </c>
-      <c r="C132" s="2" t="s">
-        <v>533</v>
-      </c>
-    </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B132" s="2"/>
+      <c r="C132" s="2"/>
+    </row>
+    <row r="133" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A133" s="1" t="s">
-        <v>534</v>
+        <v>536</v>
       </c>
       <c r="B133" s="2" t="s">
-        <v>535</v>
+        <v>537</v>
       </c>
       <c r="C133" s="2" t="s">
-        <v>536</v>
+        <v>538</v>
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A134" s="1" t="s">
-        <v>537</v>
+        <v>539</v>
       </c>
       <c r="B134" s="2" t="s">
-        <v>538</v>
+        <v>540</v>
       </c>
       <c r="C134" s="2" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A135" s="1" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
       <c r="B135" s="2" t="s">
-        <v>541</v>
+        <v>543</v>
       </c>
       <c r="C135" s="2" t="s">
-        <v>542</v>
+        <v>544</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A136" s="1" t="s">
-        <v>543</v>
+        <v>545</v>
       </c>
       <c r="B136" s="2" t="s">
-        <v>544</v>
+        <v>546</v>
       </c>
       <c r="C136" s="2" t="s">
-        <v>545</v>
+        <v>547</v>
       </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A137" s="1" t="s">
-        <v>546</v>
+        <v>548</v>
       </c>
       <c r="B137" s="2" t="s">
-        <v>547</v>
+        <v>549</v>
       </c>
       <c r="C137" s="2" t="s">
-        <v>548</v>
+        <v>550</v>
       </c>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A138" s="1" t="s">
-        <v>549</v>
+        <v>551</v>
       </c>
       <c r="B138" s="2" t="s">
-        <v>550</v>
+        <v>552</v>
       </c>
       <c r="C138" s="2" t="s">
-        <v>551</v>
+        <v>553</v>
       </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A139" s="1" t="s">
-        <v>552</v>
+        <v>554</v>
       </c>
       <c r="B139" s="2" t="s">
-        <v>553</v>
+        <v>555</v>
       </c>
       <c r="C139" s="2" t="s">
-        <v>554</v>
+        <v>556</v>
       </c>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A140" s="1" t="s">
-        <v>555</v>
+        <v>557</v>
       </c>
       <c r="B140" s="2" t="s">
-        <v>556</v>
+        <v>558</v>
       </c>
       <c r="C140" s="2" t="s">
-        <v>557</v>
-      </c>
-    </row>
-    <row r="141" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B141" s="2"/>
-      <c r="C141" s="2"/>
+        <v>559</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A141" s="1" t="s">
+        <v>560</v>
+      </c>
+      <c r="B141" s="2" t="s">
+        <v>561</v>
+      </c>
+      <c r="C141" s="2" t="s">
+        <v>562</v>
+      </c>
     </row>
     <row r="142" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A142" s="1" t="s">
-        <v>558</v>
-      </c>
-      <c r="B142" s="2" t="s">
-        <v>559</v>
-      </c>
-      <c r="C142" s="2" t="s">
-        <v>560</v>
-      </c>
+      <c r="A142"/>
+      <c r="B142" s="2"/>
+      <c r="C142" s="2"/>
     </row>
     <row r="143" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A143" s="1" t="s">
-        <v>561</v>
+        <v>563</v>
       </c>
       <c r="B143" s="2" t="s">
-        <v>562</v>
+        <v>564</v>
       </c>
       <c r="C143" s="2" t="s">
-        <v>563</v>
-      </c>
-    </row>
-    <row r="144" spans="1:3" x14ac:dyDescent="0.35">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="144" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A144" s="1" t="s">
-        <v>564</v>
+        <v>566</v>
       </c>
       <c r="B144" s="2" t="s">
-        <v>565</v>
+        <v>567</v>
       </c>
       <c r="C144" s="2" t="s">
-        <v>566</v>
+        <v>568</v>
       </c>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A145" s="1" t="s">
-        <v>567</v>
+        <v>569</v>
       </c>
       <c r="B145" s="2" t="s">
-        <v>568</v>
+        <v>570</v>
       </c>
       <c r="C145" s="2" t="s">
-        <v>569</v>
-      </c>
-    </row>
-    <row r="147" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A147" s="1" t="s">
-        <v>570</v>
-      </c>
-      <c r="B147" s="2" t="s">
         <v>571</v>
       </c>
-      <c r="C147" s="2" t="s">
+    </row>
+    <row r="146" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A146" s="1" t="s">
         <v>572</v>
+      </c>
+      <c r="B146" s="2" t="s">
+        <v>573</v>
+      </c>
+      <c r="C146" s="2" t="s">
+        <v>574</v>
       </c>
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A148" s="1" t="s">
-        <v>573</v>
+        <v>575</v>
       </c>
       <c r="B148" s="2" t="s">
-        <v>574</v>
+        <v>576</v>
       </c>
       <c r="C148" s="2" t="s">
-        <v>575</v>
+        <v>577</v>
       </c>
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A149" s="1" t="s">
-        <v>576</v>
+        <v>578</v>
       </c>
       <c r="B149" s="2" t="s">
-        <v>577</v>
+        <v>579</v>
       </c>
       <c r="C149" s="2" t="s">
-        <v>578</v>
+        <v>580</v>
       </c>
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A150" s="1" t="s">
-        <v>579</v>
+        <v>581</v>
       </c>
       <c r="B150" s="2" t="s">
-        <v>580</v>
+        <v>582</v>
       </c>
       <c r="C150" s="2" t="s">
-        <v>581</v>
+        <v>583</v>
       </c>
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A151" s="1" t="s">
-        <v>582</v>
+        <v>584</v>
       </c>
       <c r="B151" s="2" t="s">
-        <v>583</v>
+        <v>585</v>
       </c>
       <c r="C151" s="2" t="s">
-        <v>584</v>
+        <v>586</v>
       </c>
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A152" s="1" t="s">
-        <v>585</v>
+        <v>587</v>
       </c>
       <c r="B152" s="2" t="s">
-        <v>586</v>
+        <v>588</v>
       </c>
       <c r="C152" s="2" t="s">
-        <v>587</v>
+        <v>589</v>
       </c>
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A153" s="1" t="s">
-        <v>588</v>
+        <v>590</v>
       </c>
       <c r="B153" s="2" t="s">
-        <v>589</v>
+        <v>591</v>
       </c>
       <c r="C153" s="2" t="s">
-        <v>590</v>
-      </c>
-    </row>
-    <row r="155" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A155" s="1" t="s">
-        <v>591</v>
-      </c>
-      <c r="B155" s="2" t="s">
         <v>592</v>
       </c>
-      <c r="C155" s="2" t="s">
+    </row>
+    <row r="154" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A154" s="1" t="s">
         <v>593</v>
+      </c>
+      <c r="B154" s="2" t="s">
+        <v>594</v>
+      </c>
+      <c r="C154" s="2" t="s">
+        <v>595</v>
       </c>
     </row>
     <row r="156" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A156" s="1" t="s">
-        <v>594</v>
+        <v>596</v>
       </c>
       <c r="B156" s="2" t="s">
-        <v>595</v>
+        <v>597</v>
       </c>
       <c r="C156" s="2" t="s">
-        <v>596</v>
+        <v>598</v>
       </c>
     </row>
     <row r="157" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A157" s="1" t="s">
-        <v>597</v>
+        <v>599</v>
       </c>
       <c r="B157" s="2" t="s">
-        <v>598</v>
+        <v>600</v>
       </c>
       <c r="C157" s="2" t="s">
-        <v>599</v>
+        <v>601</v>
       </c>
     </row>
     <row r="158" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A158" s="1" t="s">
-        <v>600</v>
+        <v>602</v>
       </c>
       <c r="B158" s="2" t="s">
-        <v>601</v>
+        <v>603</v>
       </c>
       <c r="C158" s="2" t="s">
-        <v>602</v>
+        <v>604</v>
       </c>
     </row>
     <row r="159" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A159" s="1" t="s">
-        <v>603</v>
+        <v>605</v>
       </c>
       <c r="B159" s="2" t="s">
-        <v>604</v>
+        <v>606</v>
       </c>
       <c r="C159" s="2" t="s">
-        <v>605</v>
-      </c>
-    </row>
-    <row r="160" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35"/>
+        <v>607</v>
+      </c>
+    </row>
+    <row r="160" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A160" s="1" t="s">
+        <v>608</v>
+      </c>
+      <c r="B160" s="2" t="s">
+        <v>609</v>
+      </c>
+      <c r="C160" s="2" t="s">
+        <v>610</v>
+      </c>
+    </row>
     <row r="161" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A161" s="1" t="s">
-        <v>606</v>
-      </c>
-      <c r="B161" s="2" t="s">
-        <v>607</v>
-      </c>
-      <c r="C161" s="2" t="s">
-        <v>608</v>
-      </c>
+      <c r="A161"/>
+      <c r="B161"/>
+      <c r="C161"/>
     </row>
     <row r="162" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A162" s="1" t="s">
-        <v>609</v>
+        <v>611</v>
       </c>
       <c r="B162" s="2" t="s">
-        <v>610</v>
+        <v>612</v>
       </c>
       <c r="C162" s="2" t="s">
-        <v>611</v>
-      </c>
-    </row>
-    <row r="163" spans="1:3" x14ac:dyDescent="0.35">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="163" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A163" s="1" t="s">
-        <v>612</v>
-      </c>
-      <c r="B163" s="1" t="s">
-        <v>613</v>
-      </c>
-      <c r="C163" s="1" t="s">
         <v>614</v>
+      </c>
+      <c r="B163" s="2" t="s">
+        <v>615</v>
+      </c>
+      <c r="C163" s="2" t="s">
+        <v>616</v>
       </c>
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A164" s="1" t="s">
-        <v>615</v>
-      </c>
-      <c r="B164" s="2" t="s">
-        <v>616</v>
+        <v>617</v>
+      </c>
+      <c r="B164" s="1" t="s">
+        <v>618</v>
       </c>
       <c r="C164" s="1" t="s">
-        <v>617</v>
+        <v>619</v>
       </c>
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A165" s="1" t="s">
-        <v>618</v>
-      </c>
-      <c r="B165" s="1" t="s">
-        <v>619</v>
+        <v>620</v>
+      </c>
+      <c r="B165" s="2" t="s">
+        <v>621</v>
       </c>
       <c r="C165" s="1" t="s">
-        <v>620</v>
+        <v>622</v>
       </c>
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A166" s="1" t="s">
-        <v>621</v>
-      </c>
-      <c r="B166" s="2" t="s">
-        <v>622</v>
-      </c>
-      <c r="C166" s="2" t="s">
         <v>623</v>
+      </c>
+      <c r="B166" s="1" t="s">
+        <v>624</v>
+      </c>
+      <c r="C166" s="1" t="s">
+        <v>625</v>
       </c>
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A167" s="1" t="s">
-        <v>624</v>
+        <v>626</v>
       </c>
       <c r="B167" s="2" t="s">
-        <v>625</v>
+        <v>627</v>
       </c>
       <c r="C167" s="2" t="s">
-        <v>626</v>
+        <v>628</v>
       </c>
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A168" s="1" t="s">
-        <v>627</v>
+        <v>629</v>
       </c>
       <c r="B168" s="2" t="s">
-        <v>628</v>
+        <v>630</v>
       </c>
       <c r="C168" s="2" t="s">
-        <v>629</v>
-      </c>
-    </row>
-    <row r="170" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A170" s="1" t="s">
-        <v>630</v>
-      </c>
-      <c r="B170" s="2" t="s">
         <v>631</v>
       </c>
-      <c r="C170" s="2" t="s">
+    </row>
+    <row r="169" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A169" s="1" t="s">
         <v>632</v>
+      </c>
+      <c r="B169" s="2" t="s">
+        <v>633</v>
+      </c>
+      <c r="C169" s="2" t="s">
+        <v>634</v>
       </c>
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A171" s="1" t="s">
-        <v>633</v>
+        <v>635</v>
       </c>
       <c r="B171" s="2" t="s">
-        <v>634</v>
+        <v>636</v>
       </c>
       <c r="C171" s="2" t="s">
-        <v>635</v>
+        <v>637</v>
       </c>
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B172" s="2"/>
-      <c r="C172" s="2"/>
+      <c r="A172" s="1" t="s">
+        <v>638</v>
+      </c>
+      <c r="B172" s="2" t="s">
+        <v>639</v>
+      </c>
+      <c r="C172" s="2" t="s">
+        <v>640</v>
+      </c>
     </row>
     <row r="173" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A173" s="1" t="s">
-        <v>636</v>
-      </c>
-      <c r="B173" s="2" t="s">
-        <v>637</v>
-      </c>
-      <c r="C173" s="2" t="s">
-        <v>638</v>
-      </c>
+      <c r="B173" s="2"/>
+      <c r="C173" s="2"/>
     </row>
     <row r="174" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A174" s="1" t="s">
-        <v>639</v>
+        <v>641</v>
       </c>
       <c r="B174" s="2" t="s">
-        <v>640</v>
+        <v>642</v>
       </c>
       <c r="C174" s="2" t="s">
-        <v>641</v>
+        <v>643</v>
       </c>
     </row>
     <row r="175" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A175" s="1" t="s">
-        <v>642</v>
+        <v>644</v>
       </c>
       <c r="B175" s="2" t="s">
-        <v>643</v>
+        <v>645</v>
       </c>
       <c r="C175" s="2" t="s">
-        <v>644</v>
+        <v>646</v>
       </c>
     </row>
     <row r="176" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A176" s="1" t="s">
-        <v>645</v>
+        <v>647</v>
       </c>
       <c r="B176" s="2" t="s">
-        <v>646</v>
+        <v>648</v>
       </c>
       <c r="C176" s="2" t="s">
-        <v>647</v>
+        <v>649</v>
       </c>
     </row>
     <row r="177" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A177" s="1" t="s">
-        <v>648</v>
+        <v>650</v>
       </c>
       <c r="B177" s="2" t="s">
-        <v>649</v>
+        <v>651</v>
       </c>
       <c r="C177" s="2" t="s">
-        <v>650</v>
+        <v>652</v>
       </c>
     </row>
     <row r="178" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A178" s="1" t="s">
-        <v>651</v>
+        <v>653</v>
       </c>
       <c r="B178" s="2" t="s">
-        <v>652</v>
+        <v>654</v>
       </c>
       <c r="C178" s="2" t="s">
-        <v>653</v>
+        <v>655</v>
       </c>
     </row>
     <row r="179" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B179" s="2"/>
-      <c r="C179" s="2"/>
+      <c r="A179" s="1" t="s">
+        <v>656</v>
+      </c>
+      <c r="B179" s="2" t="s">
+        <v>657</v>
+      </c>
+      <c r="C179" s="2" t="s">
+        <v>658</v>
+      </c>
     </row>
     <row r="180" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A180" s="1" t="s">
-        <v>654</v>
-      </c>
-      <c r="B180" s="2" t="s">
-        <v>655</v>
-      </c>
-      <c r="C180" s="2" t="s">
-        <v>656</v>
-      </c>
+      <c r="B180" s="2"/>
+      <c r="C180" s="2"/>
     </row>
     <row r="181" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A181" s="1" t="s">
-        <v>657</v>
+        <v>659</v>
       </c>
       <c r="B181" s="2" t="s">
-        <v>658</v>
+        <v>660</v>
       </c>
       <c r="C181" s="2" t="s">
-        <v>659</v>
+        <v>661</v>
       </c>
     </row>
     <row r="182" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A182" s="1" t="s">
-        <v>660</v>
+        <v>662</v>
       </c>
       <c r="B182" s="2" t="s">
-        <v>661</v>
+        <v>663</v>
       </c>
       <c r="C182" s="2" t="s">
-        <v>662</v>
+        <v>664</v>
       </c>
     </row>
     <row r="183" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A183" s="1" t="s">
-        <v>663</v>
+        <v>665</v>
       </c>
       <c r="B183" s="2" t="s">
-        <v>664</v>
+        <v>666</v>
       </c>
       <c r="C183" s="2" t="s">
-        <v>665</v>
+        <v>667</v>
       </c>
     </row>
     <row r="184" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A184" s="1" t="s">
-        <v>666</v>
+        <v>668</v>
       </c>
       <c r="B184" s="2" t="s">
-        <v>667</v>
+        <v>669</v>
       </c>
       <c r="C184" s="2" t="s">
-        <v>668</v>
+        <v>670</v>
       </c>
     </row>
     <row r="185" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A185" s="1" t="s">
-        <v>669</v>
+        <v>671</v>
       </c>
       <c r="B185" s="2" t="s">
-        <v>670</v>
+        <v>672</v>
       </c>
       <c r="C185" s="2" t="s">
-        <v>671</v>
+        <v>673</v>
       </c>
     </row>
     <row r="186" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A186" s="1" t="s">
-        <v>672</v>
+        <v>674</v>
       </c>
       <c r="B186" s="2" t="s">
-        <v>673</v>
+        <v>675</v>
       </c>
       <c r="C186" s="2" t="s">
-        <v>674</v>
-      </c>
-    </row>
-    <row r="188" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A188" s="1" t="s">
-        <v>675</v>
-      </c>
-      <c r="B188" s="1" t="s">
         <v>676</v>
       </c>
-      <c r="C188" s="1" t="s">
+    </row>
+    <row r="187" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A187" s="1" t="s">
         <v>677</v>
+      </c>
+      <c r="B187" s="2" t="s">
+        <v>678</v>
+      </c>
+      <c r="C187" s="2" t="s">
+        <v>679</v>
       </c>
     </row>
     <row r="189" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A189" s="1" t="s">
-        <v>678</v>
+        <v>680</v>
       </c>
       <c r="B189" s="1" t="s">
-        <v>679</v>
+        <v>681</v>
       </c>
       <c r="C189" s="1" t="s">
-        <v>680</v>
+        <v>682</v>
       </c>
     </row>
     <row r="190" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A190" s="1" t="s">
-        <v>681</v>
+        <v>683</v>
       </c>
       <c r="B190" s="1" t="s">
-        <v>682</v>
+        <v>684</v>
       </c>
       <c r="C190" s="1" t="s">
-        <v>683</v>
+        <v>685</v>
       </c>
     </row>
     <row r="191" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A191" s="1" t="s">
-        <v>684</v>
+        <v>686</v>
       </c>
       <c r="B191" s="1" t="s">
-        <v>685</v>
+        <v>687</v>
       </c>
       <c r="C191" s="1" t="s">
-        <v>686</v>
+        <v>688</v>
       </c>
     </row>
     <row r="192" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A192" s="1" t="s">
-        <v>687</v>
-      </c>
-      <c r="B192" s="2" t="s">
-        <v>688</v>
-      </c>
-      <c r="C192" s="2" t="s">
         <v>689</v>
+      </c>
+      <c r="B192" s="1" t="s">
+        <v>690</v>
+      </c>
+      <c r="C192" s="1" t="s">
+        <v>691</v>
       </c>
     </row>
     <row r="193" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A193" s="1" t="s">
-        <v>690</v>
-      </c>
-      <c r="B193" s="1" t="s">
-        <v>691</v>
-      </c>
-      <c r="C193" s="1" t="s">
         <v>692</v>
+      </c>
+      <c r="B193" s="2" t="s">
+        <v>693</v>
+      </c>
+      <c r="C193" s="2" t="s">
+        <v>694</v>
       </c>
     </row>
     <row r="194" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A194" s="1" t="s">
-        <v>693</v>
+        <v>695</v>
       </c>
       <c r="B194" s="1" t="s">
-        <v>694</v>
+        <v>696</v>
       </c>
       <c r="C194" s="1" t="s">
-        <v>695</v>
+        <v>697</v>
       </c>
     </row>
     <row r="195" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A195" s="1" t="s">
-        <v>696</v>
-      </c>
-      <c r="B195" s="2" t="s">
-        <v>697</v>
-      </c>
-      <c r="C195" s="2" t="s">
         <v>698</v>
+      </c>
+      <c r="B195" s="1" t="s">
+        <v>699</v>
+      </c>
+      <c r="C195" s="1" t="s">
+        <v>700</v>
       </c>
     </row>
     <row r="196" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A196" s="1" t="s">
-        <v>699</v>
+        <v>701</v>
       </c>
       <c r="B196" s="2" t="s">
-        <v>673</v>
+        <v>702</v>
       </c>
       <c r="C196" s="2" t="s">
-        <v>674</v>
+        <v>703</v>
+      </c>
+    </row>
+    <row r="197" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A197" s="1" t="s">
+        <v>704</v>
+      </c>
+      <c r="B197" s="2" t="s">
+        <v>678</v>
+      </c>
+      <c r="C197" s="2" t="s">
+        <v>679</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Implement migration of Queues with associated Processes
</commit_message>
<xml_diff>
--- a/Config.xlsx
+++ b/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mateus.cruz\Documents\GitHub\OrchestratorManager\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6BA9CAB-437B-4969-A81C-FAF4984201D4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{959E27CA-7E87-4D1C-A226-0861FB74AB63}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="3" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="886" uniqueCount="814">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="904" uniqueCount="832">
   <si>
     <t>Name</t>
   </si>
@@ -1718,6 +1718,15 @@
     <t>アセット名 {0} は既に使用されています。</t>
   </si>
   <si>
+    <t>MigrateAsset</t>
+  </si>
+  <si>
+    <t>Migrating Asset {0}.</t>
+  </si>
+  <si>
+    <t>アセット {0} を移行中。</t>
+  </si>
+  <si>
     <t>UserNotFound</t>
   </si>
   <si>
@@ -2019,6 +2028,15 @@
     <t>Credential 型のアセット {0} の移行をスキップしました。</t>
   </si>
   <si>
+    <t>MigrateFolder</t>
+  </si>
+  <si>
+    <t>Migrating Classic Folder {0}.</t>
+  </si>
+  <si>
+    <t>クラッシックフォルダー {0} を移行中。</t>
+  </si>
+  <si>
     <t>MigrateAssetFailure</t>
   </si>
   <si>
@@ -2372,6 +2390,15 @@
     <t>プロセス名 {0} は既に使用されています。</t>
   </si>
   <si>
+    <t>MigrateProcess</t>
+  </si>
+  <si>
+    <t>Migrating Process {0}.</t>
+  </si>
+  <si>
+    <t>プロセス {0} を移行中。</t>
+  </si>
+  <si>
     <t>PackageNameNotSpecified</t>
   </si>
   <si>
@@ -2535,6 +2562,33 @@
   </si>
   <si>
     <t>キュー {0} に関するプロセスが見つかりませんでした。</t>
+  </si>
+  <si>
+    <t>QueueTriggerNotFound</t>
+  </si>
+  <si>
+    <t>Trigger associated with Queue {0} not found.</t>
+  </si>
+  <si>
+    <t>キュー {0} に関するトリガーが見つかりませんでした。</t>
+  </si>
+  <si>
+    <t>MigrateQueue</t>
+  </si>
+  <si>
+    <t>Migrating Queue {0}.</t>
+  </si>
+  <si>
+    <t>キュー {0} を移行中。</t>
+  </si>
+  <si>
+    <t>TriggerIDInvalidOrNotSpecified</t>
+  </si>
+  <si>
+    <t>Trigger ID invalid or not specified.</t>
+  </si>
+  <si>
+    <t>トリガー ID が無効であるか、指定されていません。</t>
   </si>
   <si>
     <t>SampleAccount</t>
@@ -2636,8 +2690,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table13" displayName="Table13" ref="A1:C235" totalsRowShown="0">
-  <autoFilter ref="A1:C235" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table13" displayName="Table13" ref="A1:C243" totalsRowShown="0">
+  <autoFilter ref="A1:C243" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Name"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="EN"/>
@@ -2916,14 +2970,14 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="39.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="57.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="62.42578125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="39.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="57.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="62.453125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2934,7 +2988,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" ht="43.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -2942,7 +2996,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="57.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" ht="58" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
@@ -2953,18 +3007,18 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="90" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" ht="90" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>813</v>
+        <v>831</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="57.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" ht="58" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>9</v>
       </c>
@@ -2975,7 +3029,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="57.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" ht="58" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>12</v>
       </c>
@@ -2986,7 +3040,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="159.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" ht="159.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>15</v>
       </c>
@@ -3014,14 +3068,14 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="48.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="43.140625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="63.85546875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="48.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="43.1796875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="63.81640625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3032,7 +3086,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="101.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" ht="101.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>17</v>
       </c>
@@ -3043,7 +3097,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" ht="29.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>19</v>
       </c>
@@ -3054,7 +3108,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>21</v>
       </c>
@@ -3065,7 +3119,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>23</v>
       </c>
@@ -3076,7 +3130,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" ht="29.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>25</v>
       </c>
@@ -3087,7 +3141,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>27</v>
       </c>
@@ -3098,7 +3152,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>29</v>
       </c>
@@ -3109,7 +3163,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>32</v>
       </c>
@@ -3120,7 +3174,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>35</v>
       </c>
@@ -3131,7 +3185,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>38</v>
       </c>
@@ -3142,7 +3196,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" ht="29.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>41</v>
       </c>
@@ -3153,7 +3207,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>44</v>
       </c>
@@ -3164,7 +3218,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" ht="29.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>47</v>
       </c>
@@ -3175,7 +3229,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>50</v>
       </c>
@@ -3186,7 +3240,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>53</v>
       </c>
@@ -3197,7 +3251,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>56</v>
       </c>
@@ -3208,7 +3262,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
         <v>59</v>
       </c>
@@ -3219,7 +3273,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
         <v>62</v>
       </c>
@@ -3230,7 +3284,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
         <v>65</v>
       </c>
@@ -3241,7 +3295,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" ht="45" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
         <v>68</v>
       </c>
@@ -3252,7 +3306,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" ht="29.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
         <v>71</v>
       </c>
@@ -3263,7 +3317,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" ht="29.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
         <v>74</v>
       </c>
@@ -3274,7 +3328,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="87" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" ht="87" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
         <v>77</v>
       </c>
@@ -3285,7 +3339,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" ht="29.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
         <v>80</v>
       </c>
@@ -3296,7 +3350,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" ht="29.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
         <v>83</v>
       </c>
@@ -3307,7 +3361,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
         <v>86</v>
       </c>
@@ -3318,7 +3372,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="s">
         <v>89</v>
       </c>
@@ -3329,7 +3383,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="s">
         <v>91</v>
       </c>
@@ -3340,7 +3394,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" ht="29.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="1" t="s">
         <v>93</v>
       </c>
@@ -3351,7 +3405,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A31" s="1" t="s">
         <v>96</v>
       </c>
@@ -3362,7 +3416,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" ht="29.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="1" t="s">
         <v>97</v>
       </c>
@@ -3373,7 +3427,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" s="1" t="s">
         <v>99</v>
       </c>
@@ -3384,7 +3438,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" ht="29.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A34" s="1" t="s">
         <v>101</v>
       </c>
@@ -3395,7 +3449,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" ht="29.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A35" s="1" t="s">
         <v>103</v>
       </c>
@@ -3406,7 +3460,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A36" s="1" t="s">
         <v>105</v>
       </c>
@@ -3417,7 +3471,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" ht="29.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A37" s="1" t="s">
         <v>108</v>
       </c>
@@ -3428,7 +3482,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" ht="29.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A38" s="1" t="s">
         <v>111</v>
       </c>
@@ -3439,7 +3493,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A39" s="1" t="s">
         <v>113</v>
       </c>
@@ -3450,7 +3504,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" ht="29.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A40" s="1" t="s">
         <v>116</v>
       </c>
@@ -3461,7 +3515,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A41" s="1" t="s">
         <v>118</v>
       </c>
@@ -3472,7 +3526,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" ht="29.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A42" s="1" t="s">
         <v>120</v>
       </c>
@@ -3483,7 +3537,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A43" s="1" t="s">
         <v>122</v>
       </c>
@@ -3494,7 +3548,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="44" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A44" s="1" t="s">
         <v>124</v>
       </c>
@@ -3505,7 +3559,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="45" spans="1:3" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3" ht="29.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A45" s="1" t="s">
         <v>126</v>
       </c>
@@ -3516,7 +3570,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="46" spans="1:3" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3" ht="29.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A46" s="1" t="s">
         <v>128</v>
       </c>
@@ -3527,7 +3581,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="47" spans="1:3" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3" ht="29.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A47" s="1" t="s">
         <v>130</v>
       </c>
@@ -3538,7 +3592,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="48" spans="1:3" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:3" ht="29.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A48" s="1" t="s">
         <v>132</v>
       </c>
@@ -3549,7 +3603,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="49" spans="1:3" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3" ht="29.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A49" s="1" t="s">
         <v>134</v>
       </c>
@@ -3560,7 +3614,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A50" s="1" t="s">
         <v>136</v>
       </c>
@@ -3571,7 +3625,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="51" spans="1:3" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:3" ht="29.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A51" s="1" t="s">
         <v>138</v>
       </c>
@@ -3582,7 +3636,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="52" spans="1:3" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:3" ht="29.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A52" s="1" t="s">
         <v>140</v>
       </c>
@@ -3593,7 +3647,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="53" spans="1:3" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:3" ht="29.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A53" s="1" t="s">
         <v>142</v>
       </c>
@@ -3604,7 +3658,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="54" spans="1:3" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:3" ht="29.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A54" s="1" t="s">
         <v>144</v>
       </c>
@@ -3615,7 +3669,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="55" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A55" s="1" t="s">
         <v>146</v>
       </c>
@@ -3626,7 +3680,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="56" spans="1:3" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:3" ht="29.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A56" s="1" t="s">
         <v>149</v>
       </c>
@@ -3637,7 +3691,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="57" spans="1:3" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:3" ht="29.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A57" s="1" t="s">
         <v>151</v>
       </c>
@@ -3648,7 +3702,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A58" s="1" t="s">
         <v>153</v>
       </c>
@@ -3659,7 +3713,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="59" spans="1:3" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:3" ht="29.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A59" s="1" t="s">
         <v>155</v>
       </c>
@@ -3670,7 +3724,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="60" spans="1:3" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:3" ht="29.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A60" s="1" t="s">
         <v>157</v>
       </c>
@@ -3681,7 +3735,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="61" spans="1:3" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:3" ht="29.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A61" s="1" t="s">
         <v>159</v>
       </c>
@@ -3692,7 +3746,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A62" s="1" t="s">
         <v>161</v>
       </c>
@@ -3703,7 +3757,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="63" spans="1:3" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:3" ht="29.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A63" s="1" t="s">
         <v>163</v>
       </c>
@@ -3714,7 +3768,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="64" spans="1:3" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:3" ht="29.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A64" s="1" t="s">
         <v>165</v>
       </c>
@@ -3725,7 +3779,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="65" spans="1:3" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:3" ht="29.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A65" s="1" t="s">
         <v>167</v>
       </c>
@@ -3736,7 +3790,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="66" spans="1:3" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:3" ht="29.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A66" s="1" t="s">
         <v>169</v>
       </c>
@@ -3747,7 +3801,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="67" spans="1:3" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:3" ht="29.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A67" s="1" t="s">
         <v>171</v>
       </c>
@@ -3758,7 +3812,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="68" spans="1:3" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:3" ht="29.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A68" s="1" t="s">
         <v>173</v>
       </c>
@@ -3769,7 +3823,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="69" spans="1:3" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:3" ht="29.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A69" s="1" t="s">
         <v>175</v>
       </c>
@@ -3780,7 +3834,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="70" spans="1:3" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:3" ht="29.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A70" s="1" t="s">
         <v>177</v>
       </c>
@@ -3806,20 +3860,20 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1927ABA9-1814-4487-9CEC-ABDCAF91481F}">
-  <dimension ref="A1:C235"/>
+  <dimension ref="A1:C243"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="50.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="61.85546875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="74.42578125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="50.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="61.81640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="74.453125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3830,7 +3884,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>181</v>
       </c>
@@ -3841,7 +3895,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" ht="43.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>183</v>
       </c>
@@ -3852,7 +3906,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>186</v>
       </c>
@@ -3863,7 +3917,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>189</v>
       </c>
@@ -3874,7 +3928,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>191</v>
       </c>
@@ -3885,7 +3939,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>194</v>
       </c>
@@ -3896,7 +3950,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>197</v>
       </c>
@@ -3907,7 +3961,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>200</v>
       </c>
@@ -3918,7 +3972,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>203</v>
       </c>
@@ -3929,7 +3983,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>206</v>
       </c>
@@ -3940,7 +3994,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>209</v>
       </c>
@@ -3951,7 +4005,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>212</v>
       </c>
@@ -3962,7 +4016,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>215</v>
       </c>
@@ -3973,7 +4027,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>218</v>
       </c>
@@ -3984,7 +4038,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>221</v>
       </c>
@@ -3995,7 +4049,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>224</v>
       </c>
@@ -